<commit_message>
Release 0.3.2 CW3M_Installer_McKenzie_0.3.2.exe  Add the Clackamas basin.  Get the McKenzie working with future climates.  Add a Required Input page to the Data Dictionary.  Add more to the McKenzie section of the Handbook.
</commit_message>
<xml_diff>
--- a/DataCW3M/CW3MdigitalHandbook/CW3MdataDictionary.xlsx
+++ b/DataCW3M/CW3MdigitalHandbook/CW3MdataDictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CW3M.git\trunk\DataCW3M\CW3MdigitalHandbook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A10E80DE-4DFF-45AE-9F9E-C98256D2B1C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4543FF54-8C20-4798-9E79-674439B6BC9E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-2295" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-2295" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Necessary input data" sheetId="7" r:id="rId1"/>
@@ -75,7 +75,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H249" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+    <comment ref="H252" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -94,7 +94,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2670" uniqueCount="846">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2689" uniqueCount="856">
   <si>
     <t>LULC_A</t>
   </si>
@@ -2633,6 +2633,36 @@
   </si>
   <si>
     <t>this is LULC_C, the most detailed land-use-land-cover class</t>
+  </si>
+  <si>
+    <t>WETL_PCT</t>
+  </si>
+  <si>
+    <t>wetlands model</t>
+  </si>
+  <si>
+    <t>the % of this IDU's area which is wetland</t>
+  </si>
+  <si>
+    <t>calculated in wetlands model</t>
+  </si>
+  <si>
+    <t>WETL_CAP</t>
+  </si>
+  <si>
+    <t>constant?</t>
+  </si>
+  <si>
+    <t>storage capacity of wetland</t>
+  </si>
+  <si>
+    <t>WETL_VOL</t>
+  </si>
+  <si>
+    <t>current volume of water stored in the wetland</t>
+  </si>
+  <si>
+    <t>calculated in Flow?</t>
   </si>
 </sst>
 </file>
@@ -3294,9 +3324,9 @@
   </sheetPr>
   <dimension ref="A1:Z781"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A84" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A102" sqref="A102:XFD109"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C60" sqref="C60:I60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -4991,73 +5021,66 @@
       <c r="U48" s="7"/>
     </row>
     <row r="49" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A49" s="41" t="s">
-        <v>236</v>
-      </c>
-      <c r="B49" s="41"/>
-      <c r="C49" s="42" t="s">
-        <v>606</v>
-      </c>
-      <c r="D49" s="43" t="s">
+      <c r="A49" s="33" t="s">
+        <v>328</v>
+      </c>
+      <c r="B49" s="33" t="s">
+        <v>24</v>
+      </c>
+      <c r="C49" s="7" t="s">
+        <v>609</v>
+      </c>
+      <c r="D49" s="10"/>
+      <c r="E49" s="10" t="s">
+        <v>610</v>
+      </c>
+      <c r="F49" s="10"/>
+      <c r="G49" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="H49" s="30" t="s">
+        <v>611</v>
+      </c>
+      <c r="I49" s="32" t="s">
+        <v>276</v>
+      </c>
+      <c r="J49" s="3"/>
+      <c r="K49" s="7"/>
+      <c r="L49" s="7"/>
+      <c r="M49" s="7"/>
+      <c r="N49" s="7"/>
+      <c r="O49" s="7"/>
+      <c r="P49" s="7"/>
+      <c r="Q49" s="7"/>
+      <c r="R49" s="7"/>
+      <c r="S49" s="7"/>
+      <c r="T49" s="7"/>
+      <c r="U49" s="7"/>
+    </row>
+    <row r="50" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A50" s="33"/>
+      <c r="B50" s="33" t="s">
+        <v>178</v>
+      </c>
+      <c r="C50" s="7" t="s">
+        <v>643</v>
+      </c>
+      <c r="D50" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="E49" s="43" t="s">
-        <v>607</v>
-      </c>
-      <c r="F49" s="43" t="s">
-        <v>28</v>
-      </c>
-      <c r="G49" s="43" t="s">
-        <v>29</v>
-      </c>
-      <c r="H49" s="44" t="s">
-        <v>608</v>
-      </c>
-      <c r="I49" s="45" t="s">
-        <v>132</v>
-      </c>
-      <c r="J49" s="39"/>
-      <c r="K49" s="35"/>
-      <c r="L49" s="35"/>
-      <c r="M49" s="35"/>
-      <c r="N49" s="35"/>
-      <c r="O49" s="35"/>
-      <c r="P49" s="35"/>
-      <c r="Q49" s="35"/>
-      <c r="R49" s="35"/>
-      <c r="S49" s="35"/>
-      <c r="T49" s="35"/>
-      <c r="U49" s="35"/>
-      <c r="V49" s="40"/>
-      <c r="W49" s="40"/>
-      <c r="X49" s="40"/>
-      <c r="Y49" s="40"/>
-      <c r="Z49" s="40"/>
-    </row>
-    <row r="50" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A50" s="33" t="s">
-        <v>328</v>
-      </c>
-      <c r="B50" s="33" t="s">
-        <v>24</v>
-      </c>
-      <c r="C50" s="7" t="s">
-        <v>609</v>
-      </c>
-      <c r="D50" s="10"/>
       <c r="E50" s="10" t="s">
-        <v>610</v>
-      </c>
-      <c r="F50" s="10"/>
+        <v>644</v>
+      </c>
+      <c r="F50" s="10" t="s">
+        <v>40</v>
+      </c>
       <c r="G50" s="10" t="s">
         <v>34</v>
       </c>
       <c r="H50" s="30" t="s">
-        <v>611</v>
-      </c>
-      <c r="I50" s="32" t="s">
-        <v>276</v>
-      </c>
+        <v>645</v>
+      </c>
+      <c r="I50" s="32"/>
       <c r="J50" s="3"/>
       <c r="K50" s="7"/>
       <c r="L50" s="7"/>
@@ -5070,33 +5093,36 @@
       <c r="S50" s="7"/>
       <c r="T50" s="7"/>
       <c r="U50" s="7"/>
+      <c r="V50" s="7"/>
+      <c r="W50" s="7"/>
+      <c r="X50" s="7"/>
+      <c r="Y50" s="7"/>
+      <c r="Z50" s="7"/>
     </row>
     <row r="51" spans="1:26" ht="14.25" customHeight="1">
       <c r="A51" s="33"/>
       <c r="B51" s="33" t="s">
-        <v>178</v>
+        <v>24</v>
       </c>
       <c r="C51" s="7" t="s">
-        <v>643</v>
-      </c>
-      <c r="D51" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="E51" s="10" t="s">
-        <v>644</v>
-      </c>
-      <c r="F51" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="G51" s="10" t="s">
-        <v>34</v>
+        <v>650</v>
+      </c>
+      <c r="D51" s="32"/>
+      <c r="E51" s="32" t="s">
+        <v>497</v>
+      </c>
+      <c r="F51" s="32"/>
+      <c r="G51" s="32" t="s">
+        <v>651</v>
       </c>
       <c r="H51" s="30" t="s">
-        <v>645</v>
-      </c>
-      <c r="I51" s="32"/>
+        <v>652</v>
+      </c>
+      <c r="I51" s="10"/>
       <c r="J51" s="3"/>
-      <c r="K51" s="7"/>
+      <c r="K51" s="7" t="s">
+        <v>653</v>
+      </c>
       <c r="L51" s="7"/>
       <c r="M51" s="7"/>
       <c r="N51" s="7"/>
@@ -5107,11 +5133,6 @@
       <c r="S51" s="7"/>
       <c r="T51" s="7"/>
       <c r="U51" s="7"/>
-      <c r="V51" s="7"/>
-      <c r="W51" s="7"/>
-      <c r="X51" s="7"/>
-      <c r="Y51" s="7"/>
-      <c r="Z51" s="7"/>
     </row>
     <row r="52" spans="1:26" ht="14.25" customHeight="1">
       <c r="A52" s="33"/>
@@ -5119,24 +5140,18 @@
         <v>24</v>
       </c>
       <c r="C52" s="7" t="s">
-        <v>650</v>
-      </c>
-      <c r="D52" s="32"/>
-      <c r="E52" s="32" t="s">
-        <v>497</v>
-      </c>
-      <c r="F52" s="32"/>
-      <c r="G52" s="32" t="s">
-        <v>651</v>
-      </c>
+        <v>662</v>
+      </c>
+      <c r="D52" s="10"/>
+      <c r="E52" s="10"/>
+      <c r="F52" s="10"/>
+      <c r="G52" s="10"/>
       <c r="H52" s="30" t="s">
-        <v>652</v>
+        <v>663</v>
       </c>
       <c r="I52" s="10"/>
       <c r="J52" s="3"/>
-      <c r="K52" s="7" t="s">
-        <v>653</v>
-      </c>
+      <c r="K52" s="7"/>
       <c r="L52" s="7"/>
       <c r="M52" s="7"/>
       <c r="N52" s="7"/>
@@ -5154,18 +5169,24 @@
         <v>24</v>
       </c>
       <c r="C53" s="7" t="s">
-        <v>662</v>
+        <v>138</v>
       </c>
       <c r="D53" s="10"/>
-      <c r="E53" s="10"/>
+      <c r="E53" s="10" t="s">
+        <v>667</v>
+      </c>
       <c r="F53" s="10"/>
-      <c r="G53" s="10"/>
+      <c r="G53" s="10" t="s">
+        <v>34</v>
+      </c>
       <c r="H53" s="30" t="s">
-        <v>663</v>
+        <v>668</v>
       </c>
       <c r="I53" s="10"/>
       <c r="J53" s="3"/>
-      <c r="K53" s="7"/>
+      <c r="K53" s="7" t="s">
+        <v>208</v>
+      </c>
       <c r="L53" s="7"/>
       <c r="M53" s="7"/>
       <c r="N53" s="7"/>
@@ -5183,18 +5204,18 @@
         <v>24</v>
       </c>
       <c r="C54" s="7" t="s">
-        <v>138</v>
+        <v>669</v>
       </c>
       <c r="D54" s="10"/>
       <c r="E54" s="10" t="s">
-        <v>667</v>
+        <v>670</v>
       </c>
       <c r="F54" s="10"/>
       <c r="G54" s="10" t="s">
         <v>34</v>
       </c>
       <c r="H54" s="30" t="s">
-        <v>668</v>
+        <v>671</v>
       </c>
       <c r="I54" s="10"/>
       <c r="J54" s="3"/>
@@ -5218,24 +5239,16 @@
         <v>24</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>669</v>
+        <v>672</v>
       </c>
       <c r="D55" s="10"/>
-      <c r="E55" s="10" t="s">
-        <v>670</v>
-      </c>
+      <c r="E55" s="10"/>
       <c r="F55" s="10"/>
-      <c r="G55" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="H55" s="30" t="s">
-        <v>671</v>
-      </c>
+      <c r="G55" s="10"/>
+      <c r="H55" s="30"/>
       <c r="I55" s="10"/>
       <c r="J55" s="3"/>
-      <c r="K55" s="7" t="s">
-        <v>208</v>
-      </c>
+      <c r="K55" s="7"/>
       <c r="L55" s="7"/>
       <c r="M55" s="7"/>
       <c r="N55" s="7"/>
@@ -5253,16 +5266,24 @@
         <v>24</v>
       </c>
       <c r="C56" s="7" t="s">
-        <v>672</v>
+        <v>218</v>
       </c>
       <c r="D56" s="10"/>
-      <c r="E56" s="10"/>
+      <c r="E56" s="10" t="s">
+        <v>501</v>
+      </c>
       <c r="F56" s="10"/>
-      <c r="G56" s="10"/>
-      <c r="H56" s="30"/>
-      <c r="I56" s="10"/>
+      <c r="G56" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="H56" s="30" t="s">
+        <v>712</v>
+      </c>
+      <c r="I56" s="32"/>
       <c r="J56" s="3"/>
-      <c r="K56" s="7"/>
+      <c r="K56" s="3" t="s">
+        <v>208</v>
+      </c>
       <c r="L56" s="7"/>
       <c r="M56" s="7"/>
       <c r="N56" s="7"/>
@@ -5280,24 +5301,22 @@
         <v>24</v>
       </c>
       <c r="C57" s="7" t="s">
-        <v>218</v>
+        <v>714</v>
       </c>
       <c r="D57" s="10"/>
       <c r="E57" s="10" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
       <c r="F57" s="10"/>
       <c r="G57" s="10" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="H57" s="30" t="s">
-        <v>712</v>
+        <v>715</v>
       </c>
       <c r="I57" s="32"/>
       <c r="J57" s="3"/>
-      <c r="K57" s="3" t="s">
-        <v>208</v>
-      </c>
+      <c r="K57" s="7"/>
       <c r="L57" s="7"/>
       <c r="M57" s="7"/>
       <c r="N57" s="7"/>
@@ -5315,18 +5334,16 @@
         <v>24</v>
       </c>
       <c r="C58" s="7" t="s">
-        <v>714</v>
+        <v>716</v>
       </c>
       <c r="D58" s="10"/>
       <c r="E58" s="10" t="s">
         <v>497</v>
       </c>
       <c r="F58" s="10"/>
-      <c r="G58" s="10" t="s">
-        <v>34</v>
-      </c>
+      <c r="G58" s="10"/>
       <c r="H58" s="30" t="s">
-        <v>715</v>
+        <v>717</v>
       </c>
       <c r="I58" s="32"/>
       <c r="J58" s="3"/>
@@ -5348,20 +5365,26 @@
         <v>24</v>
       </c>
       <c r="C59" s="7" t="s">
-        <v>716</v>
+        <v>14</v>
       </c>
       <c r="D59" s="10"/>
       <c r="E59" s="10" t="s">
-        <v>497</v>
+        <v>215</v>
       </c>
       <c r="F59" s="10"/>
-      <c r="G59" s="10"/>
-      <c r="H59" s="30" t="s">
-        <v>717</v>
-      </c>
-      <c r="I59" s="32"/>
+      <c r="G59" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="H59" s="87" t="s">
+        <v>845</v>
+      </c>
+      <c r="I59" s="32" t="s">
+        <v>132</v>
+      </c>
       <c r="J59" s="3"/>
-      <c r="K59" s="7"/>
+      <c r="K59" s="3" t="s">
+        <v>208</v>
+      </c>
       <c r="L59" s="7"/>
       <c r="M59" s="7"/>
       <c r="N59" s="7"/>
@@ -5375,30 +5398,30 @@
     </row>
     <row r="60" spans="1:26" ht="14.25" customHeight="1">
       <c r="A60" s="33"/>
-      <c r="B60" s="33" t="s">
-        <v>24</v>
-      </c>
+      <c r="B60" s="33"/>
       <c r="C60" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D60" s="10"/>
+        <v>846</v>
+      </c>
+      <c r="D60" s="10" t="s">
+        <v>32</v>
+      </c>
       <c r="E60" s="10" t="s">
-        <v>215</v>
-      </c>
-      <c r="F60" s="10"/>
+        <v>245</v>
+      </c>
+      <c r="F60" s="10" t="s">
+        <v>847</v>
+      </c>
       <c r="G60" s="10" t="s">
         <v>29</v>
       </c>
       <c r="H60" s="87" t="s">
-        <v>845</v>
+        <v>848</v>
       </c>
       <c r="I60" s="32" t="s">
-        <v>132</v>
+        <v>849</v>
       </c>
       <c r="J60" s="3"/>
-      <c r="K60" s="3" t="s">
-        <v>208</v>
-      </c>
+      <c r="K60" s="3"/>
       <c r="L60" s="7"/>
       <c r="M60" s="7"/>
       <c r="N60" s="7"/>
@@ -8595,11 +8618,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Z1033"/>
+  <dimension ref="A1:Z1036"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K63" sqref="K63"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A181" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C216" sqref="C216"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -15841,7 +15864,7 @@
       <c r="T208" s="7"/>
       <c r="U208" s="7"/>
     </row>
-    <row r="209" spans="1:26" ht="14.25" customHeight="1">
+    <row r="209" spans="1:21" ht="14.25" customHeight="1">
       <c r="A209" s="6"/>
       <c r="B209" s="6" t="s">
         <v>24</v>
@@ -15878,7 +15901,7 @@
       <c r="T209" s="7"/>
       <c r="U209" s="7"/>
     </row>
-    <row r="210" spans="1:26" ht="14.25" customHeight="1">
+    <row r="210" spans="1:21" ht="14.25" customHeight="1">
       <c r="A210" s="6"/>
       <c r="B210" s="6" t="s">
         <v>178</v>
@@ -15905,7 +15928,7 @@
       <c r="T210" s="7"/>
       <c r="U210" s="7"/>
     </row>
-    <row r="211" spans="1:26" ht="14.25" customHeight="1">
+    <row r="211" spans="1:21" ht="14.25" customHeight="1">
       <c r="A211" s="6"/>
       <c r="B211" s="6" t="s">
         <v>178</v>
@@ -15932,7 +15955,7 @@
       <c r="T211" s="7"/>
       <c r="U211" s="7"/>
     </row>
-    <row r="212" spans="1:26" ht="14.25" customHeight="1">
+    <row r="212" spans="1:21" ht="14.25" customHeight="1">
       <c r="A212" s="6"/>
       <c r="B212" s="6" t="s">
         <v>178</v>
@@ -15967,29 +15990,27 @@
       <c r="T212" s="7"/>
       <c r="U212" s="7"/>
     </row>
-    <row r="213" spans="1:26" ht="42.75" customHeight="1">
-      <c r="A213" s="6"/>
-      <c r="B213" s="6"/>
-      <c r="C213" s="20" t="s">
-        <v>528</v>
+    <row r="213" spans="1:21" s="24" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A213" s="33"/>
+      <c r="B213" s="33"/>
+      <c r="C213" s="7" t="s">
+        <v>850</v>
       </c>
       <c r="D213" s="10" t="s">
         <v>32</v>
       </c>
       <c r="E213" s="10" t="s">
-        <v>529</v>
-      </c>
-      <c r="F213" s="10" t="s">
-        <v>40</v>
-      </c>
+        <v>113</v>
+      </c>
+      <c r="F213" s="10"/>
       <c r="G213" s="10" t="s">
-        <v>29</v>
+        <v>851</v>
       </c>
       <c r="H213" s="30" t="s">
-        <v>747</v>
-      </c>
-      <c r="I213" s="31" t="s">
-        <v>836</v>
+        <v>852</v>
+      </c>
+      <c r="I213" s="32" t="s">
+        <v>548</v>
       </c>
       <c r="J213" s="3"/>
       <c r="K213" s="7"/>
@@ -16004,27 +16025,29 @@
       <c r="T213" s="7"/>
       <c r="U213" s="7"/>
     </row>
-    <row r="214" spans="1:26" ht="42.75" customHeight="1">
-      <c r="A214" s="6"/>
-      <c r="B214" s="6" t="s">
-        <v>178</v>
-      </c>
+    <row r="214" spans="1:21" s="24" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A214" s="33"/>
+      <c r="B214" s="33"/>
       <c r="C214" s="7" t="s">
-        <v>748</v>
-      </c>
-      <c r="D214" s="8"/>
-      <c r="E214" s="8" t="s">
-        <v>749</v>
-      </c>
-      <c r="F214" s="10"/>
-      <c r="G214" s="8" t="s">
+        <v>846</v>
+      </c>
+      <c r="D214" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E214" s="10" t="s">
+        <v>245</v>
+      </c>
+      <c r="F214" s="10" t="s">
+        <v>847</v>
+      </c>
+      <c r="G214" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="H214" s="15" t="s">
-        <v>750</v>
+      <c r="H214" s="87" t="s">
+        <v>848</v>
       </c>
       <c r="I214" s="32" t="s">
-        <v>746</v>
+        <v>849</v>
       </c>
       <c r="J214" s="3"/>
       <c r="K214" s="7"/>
@@ -16039,27 +16062,29 @@
       <c r="T214" s="7"/>
       <c r="U214" s="7"/>
     </row>
-    <row r="215" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A215" s="6"/>
-      <c r="B215" s="6" t="s">
-        <v>178</v>
-      </c>
+    <row r="215" spans="1:21" s="24" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A215" s="33"/>
+      <c r="B215" s="33"/>
       <c r="C215" s="7" t="s">
-        <v>751</v>
-      </c>
-      <c r="D215" s="8"/>
-      <c r="E215" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="F215" s="10"/>
-      <c r="G215" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="H215" s="15" t="s">
-        <v>752</v>
+        <v>853</v>
+      </c>
+      <c r="D215" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E215" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="F215" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="G215" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="H215" s="30" t="s">
+        <v>854</v>
       </c>
       <c r="I215" s="32" t="s">
-        <v>746</v>
+        <v>855</v>
       </c>
       <c r="J215" s="3"/>
       <c r="K215" s="7"/>
@@ -16074,27 +16099,29 @@
       <c r="T215" s="7"/>
       <c r="U215" s="7"/>
     </row>
-    <row r="216" spans="1:26" ht="14.25" customHeight="1">
+    <row r="216" spans="1:21" ht="42.75" customHeight="1">
       <c r="A216" s="6"/>
-      <c r="B216" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C216" s="7" t="s">
-        <v>753</v>
-      </c>
-      <c r="D216" s="8"/>
-      <c r="E216" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="F216" s="10"/>
-      <c r="G216" s="8" t="s">
+      <c r="B216" s="6"/>
+      <c r="C216" s="20" t="s">
+        <v>528</v>
+      </c>
+      <c r="D216" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E216" s="10" t="s">
+        <v>529</v>
+      </c>
+      <c r="F216" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="G216" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="H216" s="15" t="s">
-        <v>754</v>
-      </c>
-      <c r="I216" s="32" t="s">
-        <v>746</v>
+      <c r="H216" s="30" t="s">
+        <v>747</v>
+      </c>
+      <c r="I216" s="31" t="s">
+        <v>836</v>
       </c>
       <c r="J216" s="3"/>
       <c r="K216" s="7"/>
@@ -16109,26 +16136,28 @@
       <c r="T216" s="7"/>
       <c r="U216" s="7"/>
     </row>
-    <row r="217" spans="1:26" ht="14.25" customHeight="1">
+    <row r="217" spans="1:21" ht="42.75" customHeight="1">
       <c r="A217" s="6"/>
       <c r="B217" s="6" t="s">
         <v>178</v>
       </c>
       <c r="C217" s="7" t="s">
-        <v>755</v>
+        <v>748</v>
       </c>
       <c r="D217" s="8"/>
       <c r="E217" s="8" t="s">
-        <v>82</v>
+        <v>749</v>
       </c>
       <c r="F217" s="10"/>
       <c r="G217" s="8" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="H217" s="15" t="s">
-        <v>756</v>
-      </c>
-      <c r="I217" s="32"/>
+        <v>750</v>
+      </c>
+      <c r="I217" s="32" t="s">
+        <v>746</v>
+      </c>
       <c r="J217" s="3"/>
       <c r="K217" s="7"/>
       <c r="L217" s="7"/>
@@ -16142,24 +16171,24 @@
       <c r="T217" s="7"/>
       <c r="U217" s="7"/>
     </row>
-    <row r="218" spans="1:26" ht="14.25" customHeight="1">
+    <row r="218" spans="1:21" ht="14.25" customHeight="1">
       <c r="A218" s="6"/>
       <c r="B218" s="6" t="s">
         <v>178</v>
       </c>
       <c r="C218" s="7" t="s">
-        <v>757</v>
+        <v>751</v>
       </c>
       <c r="D218" s="8"/>
       <c r="E218" s="8" t="s">
-        <v>245</v>
+        <v>82</v>
       </c>
       <c r="F218" s="10"/>
       <c r="G218" s="8" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="H218" s="15" t="s">
-        <v>758</v>
+        <v>752</v>
       </c>
       <c r="I218" s="32" t="s">
         <v>746</v>
@@ -16177,24 +16206,24 @@
       <c r="T218" s="7"/>
       <c r="U218" s="7"/>
     </row>
-    <row r="219" spans="1:26" ht="14.25" customHeight="1">
+    <row r="219" spans="1:21" ht="14.25" customHeight="1">
       <c r="A219" s="6"/>
       <c r="B219" s="6" t="s">
-        <v>178</v>
+        <v>24</v>
       </c>
       <c r="C219" s="7" t="s">
-        <v>759</v>
+        <v>753</v>
       </c>
       <c r="D219" s="8"/>
       <c r="E219" s="8" t="s">
-        <v>245</v>
+        <v>82</v>
       </c>
       <c r="F219" s="10"/>
       <c r="G219" s="8" t="s">
         <v>29</v>
       </c>
       <c r="H219" s="15" t="s">
-        <v>760</v>
+        <v>754</v>
       </c>
       <c r="I219" s="32" t="s">
         <v>746</v>
@@ -16212,26 +16241,26 @@
       <c r="T219" s="7"/>
       <c r="U219" s="7"/>
     </row>
-    <row r="220" spans="1:26" ht="14.25" customHeight="1">
+    <row r="220" spans="1:21" ht="14.25" customHeight="1">
       <c r="A220" s="6"/>
       <c r="B220" s="6" t="s">
-        <v>24</v>
+        <v>178</v>
       </c>
       <c r="C220" s="7" t="s">
-        <v>761</v>
+        <v>755</v>
       </c>
       <c r="D220" s="8"/>
-      <c r="E220" s="8"/>
+      <c r="E220" s="8" t="s">
+        <v>82</v>
+      </c>
       <c r="F220" s="10"/>
       <c r="G220" s="8" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="H220" s="15" t="s">
-        <v>762</v>
-      </c>
-      <c r="I220" s="32" t="s">
-        <v>132</v>
-      </c>
+        <v>756</v>
+      </c>
+      <c r="I220" s="32"/>
       <c r="J220" s="3"/>
       <c r="K220" s="7"/>
       <c r="L220" s="7"/>
@@ -16245,27 +16274,27 @@
       <c r="T220" s="7"/>
       <c r="U220" s="7"/>
     </row>
-    <row r="221" spans="1:26" ht="14.25" customHeight="1">
+    <row r="221" spans="1:21" ht="14.25" customHeight="1">
       <c r="A221" s="6"/>
       <c r="B221" s="6" t="s">
         <v>178</v>
       </c>
       <c r="C221" s="7" t="s">
-        <v>763</v>
+        <v>757</v>
       </c>
       <c r="D221" s="8"/>
       <c r="E221" s="8" t="s">
-        <v>764</v>
+        <v>245</v>
       </c>
       <c r="F221" s="10"/>
       <c r="G221" s="8" t="s">
         <v>29</v>
       </c>
       <c r="H221" s="15" t="s">
-        <v>765</v>
+        <v>758</v>
       </c>
       <c r="I221" s="32" t="s">
-        <v>132</v>
+        <v>746</v>
       </c>
       <c r="J221" s="3"/>
       <c r="K221" s="7"/>
@@ -16280,29 +16309,27 @@
       <c r="T221" s="7"/>
       <c r="U221" s="7"/>
     </row>
-    <row r="222" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A222" s="6" t="s">
-        <v>328</v>
-      </c>
+    <row r="222" spans="1:21" ht="14.25" customHeight="1">
+      <c r="A222" s="6"/>
       <c r="B222" s="6" t="s">
-        <v>24</v>
+        <v>178</v>
       </c>
       <c r="C222" s="7" t="s">
-        <v>766</v>
+        <v>759</v>
       </c>
       <c r="D222" s="8"/>
       <c r="E222" s="8" t="s">
-        <v>767</v>
+        <v>245</v>
       </c>
       <c r="F222" s="10"/>
       <c r="G222" s="8" t="s">
         <v>29</v>
       </c>
       <c r="H222" s="15" t="s">
-        <v>768</v>
+        <v>760</v>
       </c>
       <c r="I222" s="32" t="s">
-        <v>132</v>
+        <v>746</v>
       </c>
       <c r="J222" s="3"/>
       <c r="K222" s="7"/>
@@ -16317,32 +16344,28 @@
       <c r="T222" s="7"/>
       <c r="U222" s="7"/>
     </row>
-    <row r="223" spans="1:26" ht="14.25" customHeight="1">
+    <row r="223" spans="1:21" ht="14.25" customHeight="1">
       <c r="A223" s="6"/>
       <c r="B223" s="6" t="s">
-        <v>178</v>
+        <v>24</v>
       </c>
       <c r="C223" s="7" t="s">
-        <v>399</v>
+        <v>761</v>
       </c>
       <c r="D223" s="8"/>
-      <c r="E223" s="8" t="s">
-        <v>215</v>
-      </c>
+      <c r="E223" s="8"/>
       <c r="F223" s="10"/>
       <c r="G223" s="8" t="s">
         <v>29</v>
       </c>
       <c r="H223" s="15" t="s">
-        <v>769</v>
+        <v>762</v>
       </c>
       <c r="I223" s="32" t="s">
         <v>132</v>
       </c>
       <c r="J223" s="3"/>
-      <c r="K223" s="3" t="s">
-        <v>208</v>
-      </c>
+      <c r="K223" s="7"/>
       <c r="L223" s="7"/>
       <c r="M223" s="7"/>
       <c r="N223" s="7"/>
@@ -16353,32 +16376,25 @@
       <c r="S223" s="7"/>
       <c r="T223" s="7"/>
       <c r="U223" s="7"/>
-      <c r="V223" s="7"/>
-      <c r="W223" s="7"/>
-      <c r="X223" s="7"/>
-      <c r="Y223" s="7"/>
-      <c r="Z223" s="7"/>
-    </row>
-    <row r="224" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A224" s="6" t="s">
-        <v>770</v>
-      </c>
+    </row>
+    <row r="224" spans="1:21" ht="14.25" customHeight="1">
+      <c r="A224" s="6"/>
       <c r="B224" s="6" t="s">
-        <v>24</v>
+        <v>178</v>
       </c>
       <c r="C224" s="7" t="s">
-        <v>771</v>
+        <v>763</v>
       </c>
       <c r="D224" s="8"/>
       <c r="E224" s="8" t="s">
-        <v>82</v>
+        <v>764</v>
       </c>
       <c r="F224" s="10"/>
       <c r="G224" s="8" t="s">
         <v>29</v>
       </c>
       <c r="H224" s="15" t="s">
-        <v>772</v>
+        <v>765</v>
       </c>
       <c r="I224" s="32" t="s">
         <v>132</v>
@@ -16396,24 +16412,26 @@
       <c r="T224" s="7"/>
       <c r="U224" s="7"/>
     </row>
-    <row r="225" spans="1:21" ht="14.25" customHeight="1">
-      <c r="A225" s="6"/>
+    <row r="225" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A225" s="6" t="s">
+        <v>328</v>
+      </c>
       <c r="B225" s="6" t="s">
         <v>24</v>
       </c>
       <c r="C225" s="7" t="s">
-        <v>773</v>
+        <v>766</v>
       </c>
       <c r="D225" s="8"/>
       <c r="E225" s="8" t="s">
-        <v>774</v>
+        <v>767</v>
       </c>
       <c r="F225" s="10"/>
       <c r="G225" s="8" t="s">
         <v>29</v>
       </c>
       <c r="H225" s="15" t="s">
-        <v>775</v>
+        <v>768</v>
       </c>
       <c r="I225" s="32" t="s">
         <v>132</v>
@@ -16431,30 +16449,32 @@
       <c r="T225" s="7"/>
       <c r="U225" s="7"/>
     </row>
-    <row r="226" spans="1:21" ht="14.25" customHeight="1">
+    <row r="226" spans="1:26" ht="14.25" customHeight="1">
       <c r="A226" s="6"/>
       <c r="B226" s="6" t="s">
-        <v>24</v>
+        <v>178</v>
       </c>
       <c r="C226" s="7" t="s">
-        <v>776</v>
+        <v>399</v>
       </c>
       <c r="D226" s="8"/>
       <c r="E226" s="8" t="s">
-        <v>777</v>
+        <v>215</v>
       </c>
       <c r="F226" s="10"/>
       <c r="G226" s="8" t="s">
         <v>29</v>
       </c>
       <c r="H226" s="15" t="s">
-        <v>778</v>
+        <v>769</v>
       </c>
       <c r="I226" s="32" t="s">
         <v>132</v>
       </c>
       <c r="J226" s="3"/>
-      <c r="K226" s="7"/>
+      <c r="K226" s="3" t="s">
+        <v>208</v>
+      </c>
       <c r="L226" s="7"/>
       <c r="M226" s="7"/>
       <c r="N226" s="7"/>
@@ -16465,25 +16485,32 @@
       <c r="S226" s="7"/>
       <c r="T226" s="7"/>
       <c r="U226" s="7"/>
-    </row>
-    <row r="227" spans="1:21" ht="14.25" customHeight="1">
+      <c r="V226" s="7"/>
+      <c r="W226" s="7"/>
+      <c r="X226" s="7"/>
+      <c r="Y226" s="7"/>
+      <c r="Z226" s="7"/>
+    </row>
+    <row r="227" spans="1:26" ht="14.25" customHeight="1">
       <c r="A227" s="6" t="s">
-        <v>328</v>
+        <v>770</v>
       </c>
       <c r="B227" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C227" s="8" t="s">
-        <v>779</v>
+      <c r="C227" s="7" t="s">
+        <v>771</v>
       </c>
       <c r="D227" s="8"/>
-      <c r="E227" s="8"/>
+      <c r="E227" s="8" t="s">
+        <v>82</v>
+      </c>
       <c r="F227" s="10"/>
       <c r="G227" s="8" t="s">
         <v>29</v>
       </c>
       <c r="H227" s="15" t="s">
-        <v>780</v>
+        <v>772</v>
       </c>
       <c r="I227" s="32" t="s">
         <v>132</v>
@@ -16501,24 +16528,24 @@
       <c r="T227" s="7"/>
       <c r="U227" s="7"/>
     </row>
-    <row r="228" spans="1:21" ht="14.25" customHeight="1">
-      <c r="A228" s="6" t="s">
-        <v>328</v>
-      </c>
+    <row r="228" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A228" s="6"/>
       <c r="B228" s="6" t="s">
         <v>24</v>
       </c>
       <c r="C228" s="7" t="s">
-        <v>781</v>
+        <v>773</v>
       </c>
       <c r="D228" s="8"/>
-      <c r="E228" s="8"/>
+      <c r="E228" s="8" t="s">
+        <v>774</v>
+      </c>
       <c r="F228" s="10"/>
       <c r="G228" s="8" t="s">
         <v>29</v>
       </c>
       <c r="H228" s="15" t="s">
-        <v>780</v>
+        <v>775</v>
       </c>
       <c r="I228" s="32" t="s">
         <v>132</v>
@@ -16536,24 +16563,24 @@
       <c r="T228" s="7"/>
       <c r="U228" s="7"/>
     </row>
-    <row r="229" spans="1:21" ht="14.25" customHeight="1">
-      <c r="A229" s="6" t="s">
-        <v>328</v>
-      </c>
+    <row r="229" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A229" s="6"/>
       <c r="B229" s="6" t="s">
         <v>24</v>
       </c>
       <c r="C229" s="7" t="s">
-        <v>782</v>
+        <v>776</v>
       </c>
       <c r="D229" s="8"/>
-      <c r="E229" s="8"/>
+      <c r="E229" s="8" t="s">
+        <v>777</v>
+      </c>
       <c r="F229" s="10"/>
       <c r="G229" s="8" t="s">
         <v>29</v>
       </c>
       <c r="H229" s="15" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="I229" s="32" t="s">
         <v>132</v>
@@ -16571,15 +16598,15 @@
       <c r="T229" s="7"/>
       <c r="U229" s="7"/>
     </row>
-    <row r="230" spans="1:21" ht="14.25" customHeight="1">
+    <row r="230" spans="1:26" ht="14.25" customHeight="1">
       <c r="A230" s="6" t="s">
         <v>328</v>
       </c>
       <c r="B230" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C230" s="7" t="s">
-        <v>783</v>
+      <c r="C230" s="8" t="s">
+        <v>779</v>
       </c>
       <c r="D230" s="8"/>
       <c r="E230" s="8"/>
@@ -16606,7 +16633,7 @@
       <c r="T230" s="7"/>
       <c r="U230" s="7"/>
     </row>
-    <row r="231" spans="1:21" ht="14.25" customHeight="1">
+    <row r="231" spans="1:26" ht="14.25" customHeight="1">
       <c r="A231" s="6" t="s">
         <v>328</v>
       </c>
@@ -16614,7 +16641,7 @@
         <v>24</v>
       </c>
       <c r="C231" s="7" t="s">
-        <v>784</v>
+        <v>781</v>
       </c>
       <c r="D231" s="8"/>
       <c r="E231" s="8"/>
@@ -16641,7 +16668,7 @@
       <c r="T231" s="7"/>
       <c r="U231" s="7"/>
     </row>
-    <row r="232" spans="1:21" ht="14.25" customHeight="1">
+    <row r="232" spans="1:26" ht="14.25" customHeight="1">
       <c r="A232" s="6" t="s">
         <v>328</v>
       </c>
@@ -16649,7 +16676,7 @@
         <v>24</v>
       </c>
       <c r="C232" s="7" t="s">
-        <v>785</v>
+        <v>782</v>
       </c>
       <c r="D232" s="8"/>
       <c r="E232" s="8"/>
@@ -16676,7 +16703,7 @@
       <c r="T232" s="7"/>
       <c r="U232" s="7"/>
     </row>
-    <row r="233" spans="1:21" ht="14.25" customHeight="1">
+    <row r="233" spans="1:26" ht="14.25" customHeight="1">
       <c r="A233" s="6" t="s">
         <v>328</v>
       </c>
@@ -16684,7 +16711,7 @@
         <v>24</v>
       </c>
       <c r="C233" s="7" t="s">
-        <v>786</v>
+        <v>783</v>
       </c>
       <c r="D233" s="8"/>
       <c r="E233" s="8"/>
@@ -16711,7 +16738,7 @@
       <c r="T233" s="7"/>
       <c r="U233" s="7"/>
     </row>
-    <row r="234" spans="1:21" ht="14.25" customHeight="1">
+    <row r="234" spans="1:26" ht="14.25" customHeight="1">
       <c r="A234" s="6" t="s">
         <v>328</v>
       </c>
@@ -16719,7 +16746,7 @@
         <v>24</v>
       </c>
       <c r="C234" s="7" t="s">
-        <v>787</v>
+        <v>784</v>
       </c>
       <c r="D234" s="8"/>
       <c r="E234" s="8"/>
@@ -16746,7 +16773,7 @@
       <c r="T234" s="7"/>
       <c r="U234" s="7"/>
     </row>
-    <row r="235" spans="1:21" ht="14.25" customHeight="1">
+    <row r="235" spans="1:26" ht="14.25" customHeight="1">
       <c r="A235" s="6" t="s">
         <v>328</v>
       </c>
@@ -16754,7 +16781,7 @@
         <v>24</v>
       </c>
       <c r="C235" s="7" t="s">
-        <v>788</v>
+        <v>785</v>
       </c>
       <c r="D235" s="8"/>
       <c r="E235" s="8"/>
@@ -16781,7 +16808,7 @@
       <c r="T235" s="7"/>
       <c r="U235" s="7"/>
     </row>
-    <row r="236" spans="1:21" ht="14.25" customHeight="1">
+    <row r="236" spans="1:26" ht="14.25" customHeight="1">
       <c r="A236" s="6" t="s">
         <v>328</v>
       </c>
@@ -16789,7 +16816,7 @@
         <v>24</v>
       </c>
       <c r="C236" s="7" t="s">
-        <v>789</v>
+        <v>786</v>
       </c>
       <c r="D236" s="8"/>
       <c r="E236" s="8"/>
@@ -16816,7 +16843,7 @@
       <c r="T236" s="7"/>
       <c r="U236" s="7"/>
     </row>
-    <row r="237" spans="1:21" ht="14.25" customHeight="1">
+    <row r="237" spans="1:26" ht="14.25" customHeight="1">
       <c r="A237" s="6" t="s">
         <v>328</v>
       </c>
@@ -16824,7 +16851,7 @@
         <v>24</v>
       </c>
       <c r="C237" s="7" t="s">
-        <v>790</v>
+        <v>787</v>
       </c>
       <c r="D237" s="8"/>
       <c r="E237" s="8"/>
@@ -16851,7 +16878,7 @@
       <c r="T237" s="7"/>
       <c r="U237" s="7"/>
     </row>
-    <row r="238" spans="1:21" ht="14.25" customHeight="1">
+    <row r="238" spans="1:26" ht="14.25" customHeight="1">
       <c r="A238" s="6" t="s">
         <v>328</v>
       </c>
@@ -16859,7 +16886,7 @@
         <v>24</v>
       </c>
       <c r="C238" s="7" t="s">
-        <v>791</v>
+        <v>788</v>
       </c>
       <c r="D238" s="8"/>
       <c r="E238" s="8"/>
@@ -16886,7 +16913,7 @@
       <c r="T238" s="7"/>
       <c r="U238" s="7"/>
     </row>
-    <row r="239" spans="1:21" ht="14.25" customHeight="1">
+    <row r="239" spans="1:26" ht="14.25" customHeight="1">
       <c r="A239" s="6" t="s">
         <v>328</v>
       </c>
@@ -16894,7 +16921,7 @@
         <v>24</v>
       </c>
       <c r="C239" s="7" t="s">
-        <v>792</v>
+        <v>789</v>
       </c>
       <c r="D239" s="8"/>
       <c r="E239" s="8"/>
@@ -16921,7 +16948,7 @@
       <c r="T239" s="7"/>
       <c r="U239" s="7"/>
     </row>
-    <row r="240" spans="1:21" ht="14.25" customHeight="1">
+    <row r="240" spans="1:26" ht="14.25" customHeight="1">
       <c r="A240" s="6" t="s">
         <v>328</v>
       </c>
@@ -16929,7 +16956,7 @@
         <v>24</v>
       </c>
       <c r="C240" s="7" t="s">
-        <v>793</v>
+        <v>790</v>
       </c>
       <c r="D240" s="8"/>
       <c r="E240" s="8"/>
@@ -16964,7 +16991,7 @@
         <v>24</v>
       </c>
       <c r="C241" s="7" t="s">
-        <v>794</v>
+        <v>791</v>
       </c>
       <c r="D241" s="8"/>
       <c r="E241" s="8"/>
@@ -16999,7 +17026,7 @@
         <v>24</v>
       </c>
       <c r="C242" s="7" t="s">
-        <v>795</v>
+        <v>792</v>
       </c>
       <c r="D242" s="8"/>
       <c r="E242" s="8"/>
@@ -17034,7 +17061,7 @@
         <v>24</v>
       </c>
       <c r="C243" s="7" t="s">
-        <v>796</v>
+        <v>793</v>
       </c>
       <c r="D243" s="8"/>
       <c r="E243" s="8"/>
@@ -17062,19 +17089,27 @@
       <c r="U243" s="7"/>
     </row>
     <row r="244" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A244" s="6"/>
+      <c r="A244" s="6" t="s">
+        <v>328</v>
+      </c>
       <c r="B244" s="6" t="s">
         <v>24</v>
       </c>
       <c r="C244" s="7" t="s">
-        <v>797</v>
+        <v>794</v>
       </c>
       <c r="D244" s="8"/>
       <c r="E244" s="8"/>
       <c r="F244" s="10"/>
-      <c r="G244" s="8"/>
-      <c r="H244" s="15"/>
-      <c r="I244" s="32"/>
+      <c r="G244" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H244" s="15" t="s">
+        <v>780</v>
+      </c>
+      <c r="I244" s="32" t="s">
+        <v>132</v>
+      </c>
       <c r="J244" s="3"/>
       <c r="K244" s="7"/>
       <c r="L244" s="7"/>
@@ -17089,25 +17124,27 @@
       <c r="U244" s="7"/>
     </row>
     <row r="245" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A245" s="6"/>
+      <c r="A245" s="6" t="s">
+        <v>328</v>
+      </c>
       <c r="B245" s="6" t="s">
-        <v>178</v>
+        <v>24</v>
       </c>
       <c r="C245" s="7" t="s">
-        <v>798</v>
+        <v>795</v>
       </c>
       <c r="D245" s="8"/>
-      <c r="E245" s="8" t="s">
-        <v>176</v>
-      </c>
+      <c r="E245" s="8"/>
       <c r="F245" s="10"/>
       <c r="G245" s="8" t="s">
-        <v>799</v>
+        <v>29</v>
       </c>
       <c r="H245" s="15" t="s">
-        <v>800</v>
-      </c>
-      <c r="I245" s="32"/>
+        <v>780</v>
+      </c>
+      <c r="I245" s="32" t="s">
+        <v>132</v>
+      </c>
       <c r="J245" s="3"/>
       <c r="K245" s="7"/>
       <c r="L245" s="7"/>
@@ -17122,25 +17159,27 @@
       <c r="U245" s="7"/>
     </row>
     <row r="246" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A246" s="6"/>
+      <c r="A246" s="6" t="s">
+        <v>328</v>
+      </c>
       <c r="B246" s="6" t="s">
-        <v>178</v>
+        <v>24</v>
       </c>
       <c r="C246" s="7" t="s">
-        <v>801</v>
+        <v>796</v>
       </c>
       <c r="D246" s="8"/>
-      <c r="E246" s="8" t="s">
-        <v>176</v>
-      </c>
+      <c r="E246" s="8"/>
       <c r="F246" s="10"/>
       <c r="G246" s="8" t="s">
-        <v>799</v>
+        <v>29</v>
       </c>
       <c r="H246" s="15" t="s">
-        <v>802</v>
-      </c>
-      <c r="I246" s="32"/>
+        <v>780</v>
+      </c>
+      <c r="I246" s="32" t="s">
+        <v>132</v>
+      </c>
       <c r="J246" s="3"/>
       <c r="K246" s="7"/>
       <c r="L246" s="7"/>
@@ -17160,19 +17199,13 @@
         <v>24</v>
       </c>
       <c r="C247" s="7" t="s">
-        <v>803</v>
+        <v>797</v>
       </c>
       <c r="D247" s="8"/>
-      <c r="E247" s="8" t="s">
-        <v>176</v>
-      </c>
+      <c r="E247" s="8"/>
       <c r="F247" s="10"/>
-      <c r="G247" s="8" t="s">
-        <v>799</v>
-      </c>
-      <c r="H247" s="15" t="s">
-        <v>804</v>
-      </c>
+      <c r="G247" s="8"/>
+      <c r="H247" s="15"/>
       <c r="I247" s="32"/>
       <c r="J247" s="3"/>
       <c r="K247" s="7"/>
@@ -17188,73 +17221,60 @@
       <c r="U247" s="7"/>
     </row>
     <row r="248" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A248" s="41" t="s">
-        <v>236</v>
-      </c>
-      <c r="B248" s="34"/>
-      <c r="C248" s="42" t="s">
-        <v>805</v>
-      </c>
-      <c r="D248" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="E248" s="43" t="s">
-        <v>806</v>
-      </c>
-      <c r="F248" s="43" t="s">
-        <v>28</v>
-      </c>
-      <c r="G248" s="43" t="s">
-        <v>29</v>
-      </c>
-      <c r="H248" s="44" t="s">
-        <v>807</v>
-      </c>
-      <c r="I248" s="36"/>
-      <c r="J248" s="39"/>
-      <c r="K248" s="39"/>
-      <c r="L248" s="35"/>
-      <c r="M248" s="35"/>
-      <c r="N248" s="35"/>
-      <c r="O248" s="35"/>
-      <c r="P248" s="35"/>
-      <c r="Q248" s="35"/>
-      <c r="R248" s="35"/>
-      <c r="S248" s="35"/>
-      <c r="T248" s="35"/>
-      <c r="U248" s="35"/>
-      <c r="V248" s="40"/>
-      <c r="W248" s="40"/>
-      <c r="X248" s="40"/>
-      <c r="Y248" s="40"/>
-      <c r="Z248" s="40"/>
+      <c r="A248" s="6"/>
+      <c r="B248" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="C248" s="7" t="s">
+        <v>798</v>
+      </c>
+      <c r="D248" s="8"/>
+      <c r="E248" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="F248" s="10"/>
+      <c r="G248" s="8" t="s">
+        <v>799</v>
+      </c>
+      <c r="H248" s="15" t="s">
+        <v>800</v>
+      </c>
+      <c r="I248" s="32"/>
+      <c r="J248" s="3"/>
+      <c r="K248" s="7"/>
+      <c r="L248" s="7"/>
+      <c r="M248" s="7"/>
+      <c r="N248" s="7"/>
+      <c r="O248" s="7"/>
+      <c r="P248" s="7"/>
+      <c r="Q248" s="7"/>
+      <c r="R248" s="7"/>
+      <c r="S248" s="7"/>
+      <c r="T248" s="7"/>
+      <c r="U248" s="7"/>
     </row>
     <row r="249" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A249" s="6" t="s">
-        <v>808</v>
-      </c>
+      <c r="A249" s="6"/>
       <c r="B249" s="6" t="s">
-        <v>24</v>
+        <v>178</v>
       </c>
       <c r="C249" s="7" t="s">
-        <v>247</v>
+        <v>801</v>
       </c>
       <c r="D249" s="8"/>
       <c r="E249" s="8" t="s">
-        <v>215</v>
+        <v>176</v>
       </c>
       <c r="F249" s="10"/>
       <c r="G249" s="8" t="s">
-        <v>34</v>
+        <v>799</v>
       </c>
       <c r="H249" s="15" t="s">
-        <v>809</v>
-      </c>
-      <c r="I249" s="8"/>
+        <v>802</v>
+      </c>
+      <c r="I249" s="32"/>
       <c r="J249" s="3"/>
-      <c r="K249" s="3" t="s">
-        <v>208</v>
-      </c>
+      <c r="K249" s="7"/>
       <c r="L249" s="7"/>
       <c r="M249" s="7"/>
       <c r="N249" s="7"/>
@@ -17268,13 +17288,23 @@
     </row>
     <row r="250" spans="1:26" ht="14.25" customHeight="1">
       <c r="A250" s="6"/>
-      <c r="B250" s="6"/>
-      <c r="C250" s="7"/>
+      <c r="B250" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C250" s="7" t="s">
+        <v>803</v>
+      </c>
       <c r="D250" s="8"/>
-      <c r="E250" s="8"/>
+      <c r="E250" s="8" t="s">
+        <v>176</v>
+      </c>
       <c r="F250" s="10"/>
-      <c r="G250" s="8"/>
-      <c r="H250" s="15"/>
+      <c r="G250" s="8" t="s">
+        <v>799</v>
+      </c>
+      <c r="H250" s="15" t="s">
+        <v>804</v>
+      </c>
       <c r="I250" s="32"/>
       <c r="J250" s="3"/>
       <c r="K250" s="7"/>
@@ -17290,40 +17320,73 @@
       <c r="U250" s="7"/>
     </row>
     <row r="251" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A251" s="6"/>
-      <c r="B251" s="6"/>
-      <c r="C251" s="7"/>
-      <c r="D251" s="8"/>
-      <c r="E251" s="8"/>
-      <c r="F251" s="10"/>
-      <c r="G251" s="8"/>
-      <c r="H251" s="15"/>
-      <c r="I251" s="8"/>
-      <c r="J251" s="7"/>
-      <c r="K251" s="7"/>
-      <c r="L251" s="7"/>
-      <c r="M251" s="7"/>
-      <c r="N251" s="7"/>
-      <c r="O251" s="7"/>
-      <c r="P251" s="7"/>
-      <c r="Q251" s="7"/>
-      <c r="R251" s="7"/>
-      <c r="S251" s="7"/>
-      <c r="T251" s="7"/>
-      <c r="U251" s="7"/>
+      <c r="A251" s="41" t="s">
+        <v>236</v>
+      </c>
+      <c r="B251" s="34"/>
+      <c r="C251" s="42" t="s">
+        <v>805</v>
+      </c>
+      <c r="D251" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="E251" s="43" t="s">
+        <v>806</v>
+      </c>
+      <c r="F251" s="43" t="s">
+        <v>28</v>
+      </c>
+      <c r="G251" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="H251" s="44" t="s">
+        <v>807</v>
+      </c>
+      <c r="I251" s="36"/>
+      <c r="J251" s="39"/>
+      <c r="K251" s="39"/>
+      <c r="L251" s="35"/>
+      <c r="M251" s="35"/>
+      <c r="N251" s="35"/>
+      <c r="O251" s="35"/>
+      <c r="P251" s="35"/>
+      <c r="Q251" s="35"/>
+      <c r="R251" s="35"/>
+      <c r="S251" s="35"/>
+      <c r="T251" s="35"/>
+      <c r="U251" s="35"/>
+      <c r="V251" s="40"/>
+      <c r="W251" s="40"/>
+      <c r="X251" s="40"/>
+      <c r="Y251" s="40"/>
+      <c r="Z251" s="40"/>
     </row>
     <row r="252" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A252" s="6"/>
-      <c r="B252" s="6"/>
-      <c r="C252" s="7"/>
+      <c r="A252" s="6" t="s">
+        <v>808</v>
+      </c>
+      <c r="B252" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C252" s="7" t="s">
+        <v>247</v>
+      </c>
       <c r="D252" s="8"/>
-      <c r="E252" s="8"/>
+      <c r="E252" s="8" t="s">
+        <v>215</v>
+      </c>
       <c r="F252" s="10"/>
-      <c r="G252" s="8"/>
-      <c r="H252" s="15"/>
+      <c r="G252" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="H252" s="15" t="s">
+        <v>809</v>
+      </c>
       <c r="I252" s="8"/>
-      <c r="J252" s="7"/>
-      <c r="K252" s="7"/>
+      <c r="J252" s="3"/>
+      <c r="K252" s="3" t="s">
+        <v>208</v>
+      </c>
       <c r="L252" s="7"/>
       <c r="M252" s="7"/>
       <c r="N252" s="7"/>
@@ -17344,8 +17407,8 @@
       <c r="F253" s="10"/>
       <c r="G253" s="8"/>
       <c r="H253" s="15"/>
-      <c r="I253" s="8"/>
-      <c r="J253" s="7"/>
+      <c r="I253" s="32"/>
+      <c r="J253" s="3"/>
       <c r="K253" s="7"/>
       <c r="L253" s="7"/>
       <c r="M253" s="7"/>
@@ -17526,8 +17589,8 @@
       <c r="D261" s="8"/>
       <c r="E261" s="8"/>
       <c r="F261" s="10"/>
-      <c r="G261" s="9"/>
-      <c r="H261" s="7"/>
+      <c r="G261" s="8"/>
+      <c r="H261" s="15"/>
       <c r="I261" s="8"/>
       <c r="J261" s="7"/>
       <c r="K261" s="7"/>
@@ -17542,7 +17605,7 @@
       <c r="T261" s="7"/>
       <c r="U261" s="7"/>
     </row>
-    <row r="262" spans="1:21">
+    <row r="262" spans="1:21" ht="14.25" customHeight="1">
       <c r="A262" s="6"/>
       <c r="B262" s="6"/>
       <c r="C262" s="7"/>
@@ -17550,7 +17613,7 @@
       <c r="E262" s="8"/>
       <c r="F262" s="10"/>
       <c r="G262" s="8"/>
-      <c r="H262" s="7"/>
+      <c r="H262" s="15"/>
       <c r="I262" s="8"/>
       <c r="J262" s="7"/>
       <c r="K262" s="7"/>
@@ -17565,14 +17628,74 @@
       <c r="T262" s="7"/>
       <c r="U262" s="7"/>
     </row>
-    <row r="263" spans="1:21">
-      <c r="B263" s="7"/>
-    </row>
-    <row r="264" spans="1:21">
-      <c r="B264" s="7"/>
+    <row r="263" spans="1:21" ht="14.25" customHeight="1">
+      <c r="A263" s="6"/>
+      <c r="B263" s="6"/>
+      <c r="C263" s="7"/>
+      <c r="D263" s="8"/>
+      <c r="E263" s="8"/>
+      <c r="F263" s="10"/>
+      <c r="G263" s="8"/>
+      <c r="H263" s="15"/>
+      <c r="I263" s="8"/>
+      <c r="J263" s="7"/>
+      <c r="K263" s="7"/>
+      <c r="L263" s="7"/>
+      <c r="M263" s="7"/>
+      <c r="N263" s="7"/>
+      <c r="O263" s="7"/>
+      <c r="P263" s="7"/>
+      <c r="Q263" s="7"/>
+      <c r="R263" s="7"/>
+      <c r="S263" s="7"/>
+      <c r="T263" s="7"/>
+      <c r="U263" s="7"/>
+    </row>
+    <row r="264" spans="1:21" ht="14.25" customHeight="1">
+      <c r="A264" s="6"/>
+      <c r="B264" s="6"/>
+      <c r="C264" s="7"/>
+      <c r="D264" s="8"/>
+      <c r="E264" s="8"/>
+      <c r="F264" s="10"/>
+      <c r="G264" s="9"/>
+      <c r="H264" s="7"/>
+      <c r="I264" s="8"/>
+      <c r="J264" s="7"/>
+      <c r="K264" s="7"/>
+      <c r="L264" s="7"/>
+      <c r="M264" s="7"/>
+      <c r="N264" s="7"/>
+      <c r="O264" s="7"/>
+      <c r="P264" s="7"/>
+      <c r="Q264" s="7"/>
+      <c r="R264" s="7"/>
+      <c r="S264" s="7"/>
+      <c r="T264" s="7"/>
+      <c r="U264" s="7"/>
     </row>
     <row r="265" spans="1:21">
-      <c r="B265" s="7"/>
+      <c r="A265" s="6"/>
+      <c r="B265" s="6"/>
+      <c r="C265" s="7"/>
+      <c r="D265" s="8"/>
+      <c r="E265" s="8"/>
+      <c r="F265" s="10"/>
+      <c r="G265" s="8"/>
+      <c r="H265" s="7"/>
+      <c r="I265" s="8"/>
+      <c r="J265" s="7"/>
+      <c r="K265" s="7"/>
+      <c r="L265" s="7"/>
+      <c r="M265" s="7"/>
+      <c r="N265" s="7"/>
+      <c r="O265" s="7"/>
+      <c r="P265" s="7"/>
+      <c r="Q265" s="7"/>
+      <c r="R265" s="7"/>
+      <c r="S265" s="7"/>
+      <c r="T265" s="7"/>
+      <c r="U265" s="7"/>
     </row>
     <row r="266" spans="1:21">
       <c r="B266" s="7"/>
@@ -19877,6 +20000,15 @@
     </row>
     <row r="1033" spans="2:2">
       <c r="B1033" s="7"/>
+    </row>
+    <row r="1034" spans="2:2">
+      <c r="B1034" s="7"/>
+    </row>
+    <row r="1035" spans="2:2">
+      <c r="B1035" s="7"/>
+    </row>
+    <row r="1036" spans="2:2">
+      <c r="B1036" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add and populate the WETL_ID attribute to the McKenzie and Clackamas basin IDU layers.
</commit_message>
<xml_diff>
--- a/DataCW3M/CW3MdigitalHandbook/CW3MdataDictionary.xlsx
+++ b/DataCW3M/CW3MdigitalHandbook/CW3MdataDictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CW3M.git\trunk\DataCW3M\CW3MdigitalHandbook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4543FF54-8C20-4798-9E79-674439B6BC9E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D6E1212-2101-4FC9-BF85-8EE21C533EE3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-2295" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="-24390" yWindow="585" windowWidth="24030" windowHeight="13050" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Necessary input data" sheetId="7" r:id="rId1"/>
@@ -24,7 +24,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -8620,7 +8622,7 @@
   </sheetPr>
   <dimension ref="A1:Z1036"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="3" topLeftCell="A181" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C216" sqref="C216"/>
     </sheetView>
@@ -20024,8 +20026,8 @@
   <dimension ref="A1:Z67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4:XFD67"/>
+      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -20531,7 +20533,7 @@
         <v>24</v>
       </c>
       <c r="B21" s="17"/>
-      <c r="E21" s="7" t="s">
+      <c r="E21" s="63" t="s">
         <v>61</v>
       </c>
       <c r="F21" s="7" t="s">
@@ -21756,9 +21758,9 @@
   </sheetPr>
   <dimension ref="A1:Z41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>

<commit_message>
CW3MdataDictionary.xlsx, Reach_McKenzie.dbf - Add Reach attribute REACH_EVAP. Specification for Thermal Loading Estimator.docx - Start changes to combine Segment layer with Reach layer. Flow_McKenzie.xml - Add REACH_EVAP to the thermal energy reports. Flow.cpp, .h - Remove member m_volume from class ReachSubnode. Add Reach attribute REACH_EVAP. ReachRouting.cpp - Remove member m_volume from class ReachSubnode.
</commit_message>
<xml_diff>
--- a/DataCW3M/CW3MdigitalHandbook/CW3MdataDictionary.xlsx
+++ b/DataCW3M/CW3MdigitalHandbook/CW3MdataDictionary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\CW3MdigitalHandbook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23B780A7-7392-4370-B582-E3052141F473}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C4A4E76-1D46-4837-B8F1-73D1EF8AD65B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-7425" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Necessary input data" sheetId="7" r:id="rId1"/>
@@ -96,7 +96,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2732" uniqueCount="872">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2738" uniqueCount="874">
   <si>
     <t>LULC_A</t>
   </si>
@@ -2713,6 +2713,12 @@
   </si>
   <si>
     <t>AREA_H2O</t>
+  </si>
+  <si>
+    <t>REACH_EVAP</t>
+  </si>
+  <si>
+    <t>daily evaporation from reach</t>
   </si>
 </sst>
 </file>
@@ -8671,7 +8677,7 @@
   <dimension ref="A1:Z1036"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A147" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="3" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="H167" sqref="H167"/>
     </sheetView>
   </sheetViews>
@@ -20071,11 +20077,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Z74"/>
+  <dimension ref="A1:Z75"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
+      <pane ySplit="4" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K50" sqref="K50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -21256,70 +21262,71 @@
         <v>861</v>
       </c>
     </row>
-    <row r="50" spans="1:26">
-      <c r="A50" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="B50" s="29" t="s">
+    <row r="50" spans="1:26" s="24" customFormat="1">
+      <c r="A50" s="22"/>
+      <c r="B50" s="22"/>
+      <c r="E50" s="7" t="s">
+        <v>872</v>
+      </c>
+      <c r="F50" s="7"/>
+      <c r="G50" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="H50" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="I50" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="J50" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="K50" s="28" t="s">
+        <v>873</v>
+      </c>
+    </row>
+    <row r="51" spans="1:26">
+      <c r="A51" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="B51" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="C50" s="19" t="s">
+      <c r="C51" s="19" t="s">
         <v>109</v>
       </c>
-      <c r="D50" s="19" t="s">
+      <c r="D51" s="19" t="s">
         <v>110</v>
       </c>
-      <c r="E50" s="20" t="s">
+      <c r="E51" s="20" t="s">
         <v>111</v>
       </c>
-      <c r="F50" s="7"/>
-      <c r="G50" s="20" t="s">
+      <c r="F51" s="7"/>
+      <c r="G51" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="H50" s="20" t="s">
+      <c r="H51" s="20" t="s">
         <v>112</v>
       </c>
-      <c r="I50" s="19" t="s">
+      <c r="I51" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="J50" s="19" t="s">
+      <c r="J51" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="K50" s="19" t="s">
+      <c r="K51" s="19" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="51" spans="1:26">
-      <c r="A51" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="B51" s="17" t="s">
+    <row r="52" spans="1:26">
+      <c r="A52" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B52" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="E51" s="7" t="s">
+      <c r="E52" s="7" t="s">
         <v>114</v>
-      </c>
-      <c r="F51" s="20">
-        <v>1</v>
-      </c>
-      <c r="G51" s="20" t="s">
-        <v>115</v>
-      </c>
-      <c r="H51" s="20" t="s">
-        <v>116</v>
-      </c>
-      <c r="J51" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="K51" s="19" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="52" spans="1:26">
-      <c r="A52" s="17"/>
-      <c r="B52" s="17"/>
-      <c r="E52" s="20" t="s">
-        <v>118</v>
       </c>
       <c r="F52" s="20">
         <v>1</v>
@@ -21330,167 +21337,157 @@
       <c r="H52" s="20" t="s">
         <v>116</v>
       </c>
-      <c r="I52" s="19" t="s">
-        <v>28</v>
-      </c>
       <c r="J52" s="19" t="s">
         <v>34</v>
       </c>
       <c r="K52" s="19" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="53" spans="1:26">
+      <c r="A53" s="17"/>
+      <c r="B53" s="17"/>
+      <c r="E53" s="20" t="s">
+        <v>118</v>
+      </c>
+      <c r="F53" s="20">
+        <v>1</v>
+      </c>
+      <c r="G53" s="20" t="s">
+        <v>115</v>
+      </c>
+      <c r="H53" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="I53" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="J53" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="K53" s="19" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="53" spans="1:26" s="24" customFormat="1" ht="14.25" customHeight="1">
-      <c r="C53" s="33"/>
-      <c r="D53" s="33"/>
-      <c r="E53" s="7" t="s">
+    <row r="54" spans="1:26" s="24" customFormat="1" ht="14.25" customHeight="1">
+      <c r="C54" s="33"/>
+      <c r="D54" s="33"/>
+      <c r="E54" s="7" t="s">
         <v>832</v>
       </c>
-      <c r="F53" s="7"/>
-      <c r="G53" s="85" t="s">
+      <c r="F54" s="7"/>
+      <c r="G54" s="85" t="s">
         <v>32</v>
       </c>
-      <c r="H53" s="85" t="s">
+      <c r="H54" s="85" t="s">
         <v>244</v>
       </c>
-      <c r="I53" s="85" t="s">
+      <c r="I54" s="85" t="s">
         <v>40</v>
       </c>
-      <c r="J53" s="85" t="s">
+      <c r="J54" s="85" t="s">
         <v>29</v>
       </c>
-      <c r="K53" s="62" t="s">
+      <c r="K54" s="62" t="s">
         <v>833</v>
       </c>
-      <c r="L53" s="85" t="s">
+      <c r="L54" s="85" t="s">
         <v>834</v>
       </c>
-      <c r="M53" s="3"/>
-      <c r="N53" s="7"/>
-      <c r="O53" s="7"/>
-      <c r="P53" s="7"/>
-      <c r="Q53" s="7"/>
-      <c r="R53" s="7"/>
-      <c r="S53" s="7"/>
-      <c r="T53" s="7"/>
-      <c r="U53" s="7"/>
-      <c r="V53" s="7"/>
-      <c r="W53" s="7"/>
-      <c r="X53" s="7"/>
-    </row>
-    <row r="54" spans="1:26">
-      <c r="A54" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="B54" s="17" t="s">
+      <c r="M54" s="3"/>
+      <c r="N54" s="7"/>
+      <c r="O54" s="7"/>
+      <c r="P54" s="7"/>
+      <c r="Q54" s="7"/>
+      <c r="R54" s="7"/>
+      <c r="S54" s="7"/>
+      <c r="T54" s="7"/>
+      <c r="U54" s="7"/>
+      <c r="V54" s="7"/>
+      <c r="W54" s="7"/>
+      <c r="X54" s="7"/>
+    </row>
+    <row r="55" spans="1:26">
+      <c r="A55" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B55" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="E54" s="7" t="s">
+      <c r="E55" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="F54" s="7">
+      <c r="F55" s="7">
         <v>-1</v>
       </c>
-      <c r="G54" s="7"/>
-      <c r="H54" s="7"/>
-    </row>
-    <row r="55" spans="1:26">
-      <c r="A55" s="17"/>
-      <c r="B55" s="17"/>
-      <c r="C55" s="7" t="s">
+      <c r="G55" s="7"/>
+      <c r="H55" s="7"/>
+    </row>
+    <row r="56" spans="1:26">
+      <c r="A56" s="17"/>
+      <c r="B56" s="17"/>
+      <c r="C56" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="D55" s="7" t="s">
+      <c r="D56" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="E55" s="7" t="s">
+      <c r="E56" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="F55" s="7">
+      <c r="F56" s="7">
         <v>0.6</v>
       </c>
-      <c r="G55" s="7" t="s">
+      <c r="G56" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="H55" s="7" t="s">
+      <c r="H56" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="I55" s="7" t="s">
+      <c r="I56" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="J55" s="7" t="s">
+      <c r="J56" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="K55" s="7" t="s">
+      <c r="K56" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="L55" s="7"/>
-      <c r="M55" s="7"/>
-      <c r="N55" s="7"/>
-      <c r="O55" s="7"/>
-      <c r="P55" s="7"/>
-      <c r="Q55" s="7"/>
-      <c r="R55" s="7"/>
-      <c r="S55" s="7"/>
-      <c r="T55" s="7"/>
-      <c r="U55" s="7"/>
-      <c r="V55" s="7"/>
-      <c r="W55" s="7"/>
-      <c r="X55" s="7"/>
-      <c r="Y55" s="7"/>
-      <c r="Z55" s="7"/>
-    </row>
-    <row r="56" spans="1:26">
-      <c r="A56" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="B56" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="E56" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="F56" s="7">
-        <v>1739.927555</v>
-      </c>
-      <c r="G56" s="7"/>
-      <c r="H56" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="K56" s="3" t="s">
-        <v>130</v>
-      </c>
+      <c r="L56" s="7"/>
+      <c r="M56" s="7"/>
+      <c r="N56" s="7"/>
+      <c r="O56" s="7"/>
+      <c r="P56" s="7"/>
+      <c r="Q56" s="7"/>
+      <c r="R56" s="7"/>
+      <c r="S56" s="7"/>
+      <c r="T56" s="7"/>
+      <c r="U56" s="7"/>
+      <c r="V56" s="7"/>
+      <c r="W56" s="7"/>
+      <c r="X56" s="7"/>
+      <c r="Y56" s="7"/>
+      <c r="Z56" s="7"/>
     </row>
     <row r="57" spans="1:26">
       <c r="A57" s="17" t="s">
         <v>24</v>
       </c>
       <c r="B57" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="C57" s="3" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="E57" s="7" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="F57" s="7">
-        <v>1</v>
-      </c>
-      <c r="G57" s="7" t="s">
-        <v>53</v>
-      </c>
+        <v>1739.927555</v>
+      </c>
+      <c r="G57" s="7"/>
       <c r="H57" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="I57" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="J57" s="3" t="s">
-        <v>34</v>
+        <v>96</v>
       </c>
       <c r="K57" s="3" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="58" spans="1:26">
@@ -21500,14 +21497,30 @@
       <c r="B58" s="17" t="s">
         <v>25</v>
       </c>
+      <c r="C58" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="E58" s="7" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="F58" s="7">
-        <v>553659</v>
-      </c>
-      <c r="G58" s="7"/>
-      <c r="H58" s="7"/>
+        <v>1</v>
+      </c>
+      <c r="G58" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="H58" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="I58" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="J58" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="K58" s="3" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="59" spans="1:26">
       <c r="A59" s="17" t="s">
@@ -21517,10 +21530,10 @@
         <v>25</v>
       </c>
       <c r="E59" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F59" s="7">
-        <v>4891208</v>
+        <v>553659</v>
       </c>
       <c r="G59" s="7"/>
       <c r="H59" s="7"/>
@@ -21532,30 +21545,14 @@
       <c r="B60" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="C60" s="3" t="s">
-        <v>25</v>
-      </c>
       <c r="E60" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F60" s="7">
-        <v>1</v>
-      </c>
-      <c r="G60" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="H60" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="I60" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="J60" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="K60" s="3" t="s">
-        <v>140</v>
-      </c>
+        <v>4891208</v>
+      </c>
+      <c r="G60" s="7"/>
+      <c r="H60" s="7"/>
     </row>
     <row r="61" spans="1:26">
       <c r="A61" s="17" t="s">
@@ -21568,10 +21565,10 @@
         <v>25</v>
       </c>
       <c r="E61" s="7" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="F61" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G61" s="7" t="s">
         <v>53</v>
@@ -21586,64 +21583,63 @@
         <v>34</v>
       </c>
       <c r="K61" s="3" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="62" spans="1:26">
+      <c r="A62" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B62" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E62" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="F62" s="7">
+        <v>0</v>
+      </c>
+      <c r="G62" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="H62" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="I62" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="J62" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="K62" s="3" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="62" spans="1:26" s="24" customFormat="1">
-      <c r="A62" s="22" t="s">
+    <row r="63" spans="1:26" s="24" customFormat="1">
+      <c r="A63" s="22" t="s">
         <v>857</v>
       </c>
-      <c r="B62" s="22" t="s">
+      <c r="B63" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="C62" s="3" t="s">
+      <c r="C63" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="D62" s="24" t="s">
+      <c r="D63" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="E62" s="7" t="s">
+      <c r="E63" s="7" t="s">
         <v>856</v>
       </c>
-      <c r="F62" s="7">
+      <c r="F63" s="7">
         <v>5</v>
       </c>
-      <c r="G62" s="7" t="s">
+      <c r="G63" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="H62" s="7" t="s">
-        <v>146</v>
-      </c>
-      <c r="I62" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="J62" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="K62" s="3" t="s">
-        <v>858</v>
-      </c>
-      <c r="L62" s="28" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="63" spans="1:26">
-      <c r="A63" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="B63" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="D63" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="E63" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="F63" s="7">
-        <v>0</v>
-      </c>
-      <c r="G63" s="7"/>
       <c r="H63" s="7" t="s">
         <v>146</v>
       </c>
@@ -21654,85 +21650,92 @@
         <v>29</v>
       </c>
       <c r="K63" s="3" t="s">
-        <v>147</v>
+        <v>858</v>
+      </c>
+      <c r="L63" s="28" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="64" spans="1:26">
       <c r="A64" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="B64" s="17"/>
+      <c r="B64" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="D64" s="3" t="s">
+        <v>144</v>
+      </c>
       <c r="E64" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="F64" s="7">
+        <v>0</v>
+      </c>
+      <c r="G64" s="7"/>
+      <c r="H64" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="I64" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="J64" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="K64" s="3" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11">
+      <c r="A65" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B65" s="17"/>
+      <c r="E65" s="7" t="s">
         <v>148</v>
       </c>
-      <c r="F64" s="7">
+      <c r="F65" s="7">
         <v>6772</v>
       </c>
-      <c r="G64" s="7"/>
-      <c r="H64" s="7"/>
-    </row>
-    <row r="65" spans="1:11" s="24" customFormat="1">
-      <c r="A65" s="22"/>
-      <c r="B65" s="22"/>
-      <c r="E65" s="7" t="s">
-        <v>864</v>
-      </c>
-      <c r="F65" s="7">
-        <v>1</v>
-      </c>
-      <c r="G65" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="H65" s="7" t="s">
-        <v>865</v>
-      </c>
-      <c r="I65" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="J65" s="28" t="s">
-        <v>866</v>
-      </c>
+      <c r="G65" s="7"/>
+      <c r="H65" s="7"/>
     </row>
     <row r="66" spans="1:11" s="24" customFormat="1">
       <c r="A66" s="22"/>
       <c r="B66" s="22"/>
       <c r="E66" s="7" t="s">
-        <v>863</v>
+        <v>864</v>
       </c>
       <c r="F66" s="7">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="G66" s="7" t="s">
         <v>126</v>
       </c>
       <c r="H66" s="7" t="s">
-        <v>643</v>
+        <v>865</v>
       </c>
       <c r="I66" s="28" t="s">
         <v>28</v>
       </c>
       <c r="J66" s="28" t="s">
-        <v>29</v>
-      </c>
-      <c r="K66" s="28" t="s">
-        <v>869</v>
+        <v>866</v>
       </c>
     </row>
     <row r="67" spans="1:11" s="24" customFormat="1">
       <c r="A67" s="22"/>
       <c r="B67" s="22"/>
-      <c r="D67" s="62" t="s">
-        <v>26</v>
-      </c>
       <c r="E67" s="7" t="s">
-        <v>813</v>
-      </c>
-      <c r="F67" s="7"/>
-      <c r="G67" s="63" t="s">
-        <v>32</v>
+        <v>863</v>
+      </c>
+      <c r="F67" s="7">
+        <v>10</v>
+      </c>
+      <c r="G67" s="7" t="s">
+        <v>126</v>
       </c>
       <c r="H67" s="7" t="s">
-        <v>84</v>
+        <v>643</v>
       </c>
       <c r="I67" s="28" t="s">
         <v>28</v>
@@ -21741,19 +21744,17 @@
         <v>29</v>
       </c>
       <c r="K67" s="28" t="s">
-        <v>814</v>
+        <v>869</v>
       </c>
     </row>
     <row r="68" spans="1:11" s="24" customFormat="1">
-      <c r="A68" s="22" t="s">
-        <v>24</v>
-      </c>
+      <c r="A68" s="22"/>
       <c r="B68" s="22"/>
       <c r="D68" s="62" t="s">
         <v>26</v>
       </c>
       <c r="E68" s="7" t="s">
-        <v>815</v>
+        <v>813</v>
       </c>
       <c r="F68" s="7"/>
       <c r="G68" s="63" t="s">
@@ -21769,39 +21770,35 @@
         <v>29</v>
       </c>
       <c r="K68" s="28" t="s">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" s="24" customFormat="1">
+      <c r="A69" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="B69" s="22"/>
+      <c r="D69" s="62" t="s">
+        <v>26</v>
+      </c>
+      <c r="E69" s="7" t="s">
+        <v>815</v>
+      </c>
+      <c r="F69" s="7"/>
+      <c r="G69" s="63" t="s">
+        <v>32</v>
+      </c>
+      <c r="H69" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="I69" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="J69" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="K69" s="28" t="s">
         <v>816</v>
-      </c>
-    </row>
-    <row r="69" spans="1:11">
-      <c r="A69" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="B69" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="D69" s="19" t="s">
-        <v>150</v>
-      </c>
-      <c r="E69" s="20" t="s">
-        <v>152</v>
-      </c>
-      <c r="F69" s="20">
-        <v>1500</v>
-      </c>
-      <c r="G69" s="20" t="s">
-        <v>126</v>
-      </c>
-      <c r="H69" s="20" t="s">
-        <v>96</v>
-      </c>
-      <c r="I69" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="J69" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="K69" s="19" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="70" spans="1:11">
@@ -21814,16 +21811,16 @@
       <c r="D70" s="19" t="s">
         <v>150</v>
       </c>
-      <c r="E70" s="19" t="s">
-        <v>157</v>
-      </c>
-      <c r="F70" s="19">
+      <c r="E70" s="20" t="s">
+        <v>152</v>
+      </c>
+      <c r="F70" s="20">
         <v>1500</v>
       </c>
       <c r="G70" s="20" t="s">
         <v>126</v>
       </c>
-      <c r="H70" s="19" t="s">
+      <c r="H70" s="20" t="s">
         <v>96</v>
       </c>
       <c r="I70" s="19" t="s">
@@ -21833,7 +21830,7 @@
         <v>34</v>
       </c>
       <c r="K70" s="19" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="71" spans="1:11">
@@ -21847,7 +21844,7 @@
         <v>150</v>
       </c>
       <c r="E71" s="19" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="F71" s="19">
         <v>1500</v>
@@ -21865,7 +21862,7 @@
         <v>34</v>
       </c>
       <c r="K71" s="19" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="72" spans="1:11">
@@ -21873,16 +21870,16 @@
         <v>24</v>
       </c>
       <c r="B72" s="18" t="s">
-        <v>162</v>
+        <v>25</v>
       </c>
       <c r="D72" s="19" t="s">
         <v>150</v>
       </c>
       <c r="E72" s="19" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="F72" s="19">
-        <v>1000</v>
+        <v>1500</v>
       </c>
       <c r="G72" s="20" t="s">
         <v>126</v>
@@ -21897,7 +21894,7 @@
         <v>34</v>
       </c>
       <c r="K72" s="19" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="73" spans="1:11">
@@ -21911,7 +21908,7 @@
         <v>150</v>
       </c>
       <c r="E73" s="19" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="F73" s="19">
         <v>1000</v>
@@ -21920,7 +21917,7 @@
         <v>126</v>
       </c>
       <c r="H73" s="19" t="s">
-        <v>123</v>
+        <v>96</v>
       </c>
       <c r="I73" s="19" t="s">
         <v>40</v>
@@ -21929,7 +21926,7 @@
         <v>34</v>
       </c>
       <c r="K73" s="19" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="74" spans="1:11">
@@ -21943,7 +21940,7 @@
         <v>150</v>
       </c>
       <c r="E74" s="19" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="F74" s="19">
         <v>1000</v>
@@ -21961,13 +21958,45 @@
         <v>34</v>
       </c>
       <c r="K74" s="19" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11">
+      <c r="A75" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B75" s="18" t="s">
+        <v>162</v>
+      </c>
+      <c r="D75" s="19" t="s">
+        <v>150</v>
+      </c>
+      <c r="E75" s="19" t="s">
+        <v>167</v>
+      </c>
+      <c r="F75" s="19">
+        <v>1000</v>
+      </c>
+      <c r="G75" s="20" t="s">
+        <v>126</v>
+      </c>
+      <c r="H75" s="19" t="s">
+        <v>123</v>
+      </c>
+      <c r="I75" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="J75" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="K75" s="19" t="s">
         <v>168</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B50">
+  <conditionalFormatting sqref="B51">
     <cfRule type="notContainsBlanks" dxfId="0" priority="1">
-      <formula>LEN(TRIM(B50))&gt;0</formula>
+      <formula>LEN(TRIM(B51))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
WORK-IN-PROGRESS. Begin to replace m_discharge with m_dischargeWP.
</commit_message>
<xml_diff>
--- a/DataCW3M/CW3MdigitalHandbook/CW3MdataDictionary.xlsx
+++ b/DataCW3M/CW3MdigitalHandbook/CW3MdataDictionary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\CW3MdigitalHandbook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C4A4E76-1D46-4837-B8F1-73D1EF8AD65B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF104903-FA85-4134-8C96-09E3B4306CCD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-7425" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -96,7 +96,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2738" uniqueCount="874">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2744" uniqueCount="875">
   <si>
     <t>LULC_A</t>
   </si>
@@ -2685,9 +2685,6 @@
     <t xml:space="preserve"> net longwave radiation out of the stream to the atmosphere; positive values for energy going from the stream to the atmosphere</t>
   </si>
   <si>
-    <t>insolation flux; positive for energy going into the stream</t>
-  </si>
-  <si>
     <t>WIDTH</t>
   </si>
   <si>
@@ -2719,6 +2716,12 @@
   </si>
   <si>
     <t>daily evaporation from reach</t>
+  </si>
+  <si>
+    <t>EVAP_MM</t>
+  </si>
+  <si>
+    <t>net insolation flux after taking shading and cloudiness into account; positive for energy going into the stream</t>
   </si>
 </sst>
 </file>
@@ -20077,10 +20080,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Z75"/>
+  <dimension ref="A1:Z76"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="4" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="K50" sqref="K50"/>
     </sheetView>
   </sheetViews>
@@ -20276,7 +20279,7 @@
       <c r="B6" s="64"/>
       <c r="D6" s="66"/>
       <c r="E6" s="66" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="F6" s="66">
         <v>5.2</v>
@@ -20292,7 +20295,7 @@
         <v>29</v>
       </c>
       <c r="K6" s="65" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="30">
@@ -20483,7 +20486,7 @@
       <c r="B16" s="22"/>
       <c r="D16" s="3"/>
       <c r="E16" s="7" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="F16" s="7">
         <v>1</v>
@@ -20501,7 +20504,7 @@
         <v>29</v>
       </c>
       <c r="K16" s="24" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
     </row>
     <row r="17" spans="1:26">
@@ -20590,32 +20593,46 @@
         <v>57</v>
       </c>
     </row>
-    <row r="20" spans="1:26">
-      <c r="A20" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="B20" s="17" t="s">
-        <v>30</v>
-      </c>
+    <row r="20" spans="1:26" s="24" customFormat="1">
+      <c r="A20" s="22"/>
+      <c r="B20" s="22"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
       <c r="E20" s="7" t="s">
-        <v>58</v>
+        <v>873</v>
       </c>
       <c r="F20" s="7">
-        <v>0</v>
-      </c>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
+        <v>4.2</v>
+      </c>
+      <c r="G20" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="H20" s="7" t="s">
+        <v>424</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="J20" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="K20" s="3" t="s">
+        <v>872</v>
+      </c>
+      <c r="N20" s="3"/>
     </row>
     <row r="21" spans="1:26">
       <c r="A21" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="B21" s="17"/>
+      <c r="B21" s="17" t="s">
+        <v>30</v>
+      </c>
       <c r="E21" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F21" s="7">
-        <v>6713</v>
+        <v>0</v>
       </c>
       <c r="G21" s="7"/>
       <c r="H21" s="7"/>
@@ -20626,9 +20643,11 @@
       </c>
       <c r="B22" s="17"/>
       <c r="E22" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="F22" s="7"/>
+        <v>59</v>
+      </c>
+      <c r="F22" s="7">
+        <v>6713</v>
+      </c>
       <c r="G22" s="7"/>
       <c r="H22" s="7"/>
     </row>
@@ -20637,12 +20656,10 @@
         <v>24</v>
       </c>
       <c r="B23" s="17"/>
-      <c r="E23" s="63" t="s">
-        <v>61</v>
-      </c>
-      <c r="F23" s="7" t="s">
-        <v>62</v>
-      </c>
+      <c r="E23" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="F23" s="7"/>
       <c r="G23" s="7"/>
       <c r="H23" s="7"/>
     </row>
@@ -20650,110 +20667,108 @@
       <c r="A24" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="B24" s="17" t="s">
+      <c r="B24" s="17"/>
+      <c r="E24" s="63" t="s">
+        <v>61</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="G24" s="7"/>
+      <c r="H24" s="7"/>
+    </row>
+    <row r="25" spans="1:26">
+      <c r="A25" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C25" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="E24" s="7" t="s">
+      <c r="E25" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="F24" s="7">
+      <c r="F25" s="7">
         <v>34</v>
       </c>
-      <c r="G24" s="7" t="s">
+      <c r="G25" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="H24" s="7" t="s">
+      <c r="H25" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="K24" s="3" t="s">
+      <c r="K25" s="3" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="25" spans="1:26" ht="18.75" customHeight="1">
-      <c r="A25" s="22"/>
-      <c r="B25" s="22"/>
-      <c r="C25" s="23"/>
-      <c r="D25" s="21" t="s">
+    <row r="26" spans="1:26" ht="18.75" customHeight="1">
+      <c r="A26" s="22"/>
+      <c r="B26" s="22"/>
+      <c r="C26" s="23"/>
+      <c r="D26" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="E25" s="24" t="s">
+      <c r="E26" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="F25" s="25">
+      <c r="F26" s="25">
         <v>6737</v>
       </c>
-      <c r="G25" s="24" t="s">
+      <c r="G26" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="H25" s="26" t="s">
+      <c r="H26" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="I25" s="23"/>
-      <c r="J25" s="27" t="s">
+      <c r="I26" s="23"/>
+      <c r="J26" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="K25" s="28" t="s">
+      <c r="K26" s="28" t="s">
         <v>855</v>
       </c>
-      <c r="L25" s="23"/>
-      <c r="M25" s="23"/>
-      <c r="N25" s="23"/>
-      <c r="O25" s="23"/>
-      <c r="P25" s="23"/>
-      <c r="Q25" s="23"/>
-      <c r="R25" s="23"/>
-      <c r="S25" s="23"/>
-      <c r="T25" s="23"/>
-      <c r="U25" s="23"/>
-      <c r="V25" s="23"/>
-      <c r="W25" s="23"/>
-      <c r="X25" s="23"/>
-      <c r="Y25" s="23"/>
-      <c r="Z25" s="23"/>
-    </row>
-    <row r="26" spans="1:26">
-      <c r="A26" s="17"/>
-      <c r="B26" s="17"/>
-      <c r="D26" s="19" t="s">
+      <c r="L26" s="23"/>
+      <c r="M26" s="23"/>
+      <c r="N26" s="23"/>
+      <c r="O26" s="23"/>
+      <c r="P26" s="23"/>
+      <c r="Q26" s="23"/>
+      <c r="R26" s="23"/>
+      <c r="S26" s="23"/>
+      <c r="T26" s="23"/>
+      <c r="U26" s="23"/>
+      <c r="V26" s="23"/>
+      <c r="W26" s="23"/>
+      <c r="X26" s="23"/>
+      <c r="Y26" s="23"/>
+      <c r="Z26" s="23"/>
+    </row>
+    <row r="27" spans="1:26">
+      <c r="A27" s="17"/>
+      <c r="B27" s="17"/>
+      <c r="D27" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="E26" s="20" t="s">
+      <c r="E27" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="F26" s="20">
+      <c r="F27" s="20">
         <v>1</v>
       </c>
-      <c r="G26" s="20" t="s">
+      <c r="G27" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="H26" s="20" t="s">
+      <c r="H27" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="J26" s="19" t="s">
+      <c r="J27" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="K26" s="19" t="s">
+      <c r="K27" s="19" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="27" spans="1:26">
-      <c r="A27" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="B27" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="E27" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="F27" s="7">
-        <v>104</v>
-      </c>
-      <c r="G27" s="7"/>
-      <c r="H27" s="7"/>
     </row>
     <row r="28" spans="1:26">
       <c r="A28" s="17" t="s">
@@ -20763,10 +20778,10 @@
         <v>30</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F28" s="7">
-        <v>589</v>
+        <v>104</v>
       </c>
       <c r="G28" s="7"/>
       <c r="H28" s="7"/>
@@ -20779,89 +20794,84 @@
         <v>30</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F29" s="7">
-        <v>0</v>
+        <v>589</v>
       </c>
       <c r="G29" s="7"/>
       <c r="H29" s="7"/>
     </row>
     <row r="30" spans="1:26">
-      <c r="A30" s="17"/>
-      <c r="B30" s="18" t="s">
+      <c r="A30" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B30" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="E30" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="F30" s="7">
+        <v>0</v>
+      </c>
+      <c r="G30" s="7"/>
+      <c r="H30" s="7"/>
+    </row>
+    <row r="31" spans="1:26">
+      <c r="A31" s="17"/>
+      <c r="B31" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="D30" s="19" t="s">
+      <c r="D31" s="19" t="s">
         <v>76</v>
       </c>
-      <c r="E30" s="20" t="s">
+      <c r="E31" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="F30" s="7"/>
-      <c r="G30" s="20" t="s">
+      <c r="F31" s="7"/>
+      <c r="G31" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="H30" s="20" t="s">
+      <c r="H31" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="I30" s="19" t="s">
+      <c r="I31" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="J30" s="19" t="s">
+      <c r="J31" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="K30" s="28" t="s">
+      <c r="K31" s="28" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="31" spans="1:26" s="24" customFormat="1">
-      <c r="A31" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="B31" s="22" t="s">
+    <row r="32" spans="1:26" s="24" customFormat="1">
+      <c r="A32" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="B32" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="D31" s="27"/>
-      <c r="E31" s="24" t="s">
+      <c r="D32" s="27"/>
+      <c r="E32" s="24" t="s">
         <v>827</v>
       </c>
-      <c r="F31" s="7"/>
-      <c r="G31" s="62" t="s">
+      <c r="F32" s="7"/>
+      <c r="G32" s="62" t="s">
         <v>32</v>
       </c>
-      <c r="H31" s="62" t="s">
+      <c r="H32" s="62" t="s">
         <v>84</v>
       </c>
-      <c r="I31" s="28" t="s">
+      <c r="I32" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="J31" s="28" t="s">
+      <c r="J32" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="K31" s="28" t="s">
+      <c r="K32" s="28" t="s">
         <v>828</v>
-      </c>
-    </row>
-    <row r="32" spans="1:26">
-      <c r="A32" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="B32" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="E32" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="F32" s="7">
-        <v>0</v>
-      </c>
-      <c r="G32" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="H32" s="7"/>
-      <c r="K32" s="3" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="33" spans="1:11">
@@ -20871,23 +20881,18 @@
       <c r="B33" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="D33" s="3" t="s">
-        <v>45</v>
-      </c>
       <c r="E33" s="7" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F33" s="7">
         <v>0</v>
       </c>
-      <c r="G33" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="H33" s="20" t="s">
-        <v>84</v>
-      </c>
-      <c r="K33" s="19" t="s">
-        <v>85</v>
+      <c r="G33" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="H33" s="7"/>
+      <c r="K33" s="3" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="34" spans="1:11">
@@ -20897,20 +20902,23 @@
       <c r="B34" s="17" t="s">
         <v>25</v>
       </c>
+      <c r="D34" s="3" t="s">
+        <v>45</v>
+      </c>
       <c r="E34" s="7" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F34" s="7">
         <v>0</v>
       </c>
       <c r="G34" s="20" t="s">
-        <v>53</v>
+        <v>32</v>
       </c>
       <c r="H34" s="20" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="K34" s="19" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="35" spans="1:11">
@@ -20921,19 +20929,19 @@
         <v>25</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="F35" s="7">
         <v>0</v>
       </c>
       <c r="G35" s="20" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
       <c r="H35" s="20" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="K35" s="19" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="36" spans="1:11">
@@ -20944,79 +20952,72 @@
         <v>25</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F36" s="7">
         <v>0</v>
       </c>
       <c r="G36" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="H36" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="K36" s="19" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11">
+      <c r="A37" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B37" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="E37" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="F37" s="7">
+        <v>0</v>
+      </c>
+      <c r="G37" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="H36" s="20" t="s">
+      <c r="H37" s="20" t="s">
         <v>92</v>
       </c>
-      <c r="K36" s="19" t="s">
+      <c r="K37" s="19" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="37" spans="1:11" s="67" customFormat="1">
-      <c r="A37" s="64" t="s">
-        <v>24</v>
-      </c>
-      <c r="B37" s="64" t="s">
+    <row r="38" spans="1:11" s="67" customFormat="1">
+      <c r="A38" s="64" t="s">
+        <v>24</v>
+      </c>
+      <c r="B38" s="64" t="s">
         <v>25</v>
       </c>
-      <c r="D37" s="68" t="s">
+      <c r="D38" s="68" t="s">
         <v>26</v>
       </c>
-      <c r="E37" s="69" t="s">
+      <c r="E38" s="69" t="s">
         <v>94</v>
       </c>
-      <c r="F37" s="69">
+      <c r="F38" s="69">
         <v>0</v>
       </c>
-      <c r="G37" s="69"/>
-      <c r="H37" s="68" t="s">
+      <c r="G38" s="69"/>
+      <c r="H38" s="68" t="s">
         <v>112</v>
       </c>
-      <c r="I37" s="68" t="s">
+      <c r="I38" s="68" t="s">
         <v>28</v>
       </c>
-      <c r="J37" s="68" t="s">
+      <c r="J38" s="68" t="s">
         <v>29</v>
       </c>
-      <c r="K37" s="65" t="s">
+      <c r="K38" s="65" t="s">
         <v>818</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11">
-      <c r="A38" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="B38" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E38" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="F38" s="7">
-        <v>1739.9274680000001</v>
-      </c>
-      <c r="G38" s="7"/>
-      <c r="H38" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="I38" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="J38" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="K38" s="3" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="39" spans="1:11">
@@ -21026,30 +21027,44 @@
       <c r="B39" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="D39" s="3" t="s">
-        <v>50</v>
+      <c r="C39" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="F39" s="7">
-        <v>6699</v>
+        <v>1739.9274680000001</v>
       </c>
       <c r="G39" s="7"/>
-      <c r="H39" s="7"/>
+      <c r="H39" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="I39" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="J39" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="K39" s="3" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="40" spans="1:11">
       <c r="A40" s="17" t="s">
         <v>24</v>
       </c>
       <c r="B40" s="17" t="s">
-        <v>30</v>
+        <v>25</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>50</v>
       </c>
       <c r="E40" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F40" s="7">
-        <v>0</v>
+        <v>6699</v>
       </c>
       <c r="G40" s="7"/>
       <c r="H40" s="7"/>
@@ -21059,13 +21074,10 @@
         <v>24</v>
       </c>
       <c r="B41" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="D41" s="3" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="E41" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F41" s="7">
         <v>0</v>
@@ -21073,7 +21085,7 @@
       <c r="G41" s="7"/>
       <c r="H41" s="7"/>
     </row>
-    <row r="42" spans="1:11" ht="60">
+    <row r="42" spans="1:11">
       <c r="A42" s="17" t="s">
         <v>24</v>
       </c>
@@ -21081,27 +21093,18 @@
         <v>25</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>101</v>
+        <v>45</v>
       </c>
       <c r="E42" s="7" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F42" s="7">
         <v>0</v>
       </c>
       <c r="G42" s="7"/>
-      <c r="H42" s="15" t="s">
-        <v>103</v>
-      </c>
-      <c r="I42" s="7"/>
-      <c r="J42" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="K42" s="7" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11">
+      <c r="H42" s="7"/>
+    </row>
+    <row r="43" spans="1:11" ht="60">
       <c r="A43" s="17" t="s">
         <v>24</v>
       </c>
@@ -21109,46 +21112,44 @@
         <v>25</v>
       </c>
       <c r="D43" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="E43" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="F43" s="7">
+        <v>0</v>
+      </c>
+      <c r="G43" s="7"/>
+      <c r="H43" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="I43" s="7"/>
+      <c r="J43" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="K43" s="7" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11">
+      <c r="A44" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B44" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="D44" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="E43" s="7" t="s">
+      <c r="E44" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="F43" s="7">
+      <c r="F44" s="7">
         <v>6758</v>
       </c>
-      <c r="G43" s="7"/>
-      <c r="H43" s="7"/>
-    </row>
-    <row r="44" spans="1:11" s="24" customFormat="1">
-      <c r="A44" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="B44" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="D44" s="3" t="s">
-        <v>824</v>
-      </c>
-      <c r="E44" s="7" t="s">
-        <v>821</v>
-      </c>
-      <c r="F44" s="7"/>
-      <c r="G44" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="H44" s="63" t="s">
-        <v>84</v>
-      </c>
-      <c r="I44" s="62" t="s">
-        <v>28</v>
-      </c>
-      <c r="J44" s="62" t="s">
-        <v>29</v>
-      </c>
-      <c r="K44" s="62" t="s">
-        <v>823</v>
-      </c>
+      <c r="G44" s="7"/>
+      <c r="H44" s="7"/>
     </row>
     <row r="45" spans="1:11" s="24" customFormat="1">
       <c r="A45" s="22" t="s">
@@ -21158,10 +21159,10 @@
         <v>25</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>825</v>
-      </c>
-      <c r="E45" s="63" t="s">
-        <v>822</v>
+        <v>824</v>
+      </c>
+      <c r="E45" s="7" t="s">
+        <v>821</v>
       </c>
       <c r="F45" s="7"/>
       <c r="G45" s="7" t="s">
@@ -21177,30 +21178,37 @@
         <v>29</v>
       </c>
       <c r="K45" s="62" t="s">
+        <v>823</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" s="24" customFormat="1">
+      <c r="A46" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="B46" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>825</v>
+      </c>
+      <c r="E46" s="63" t="s">
+        <v>822</v>
+      </c>
+      <c r="F46" s="7"/>
+      <c r="G46" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="H46" s="63" t="s">
+        <v>84</v>
+      </c>
+      <c r="I46" s="62" t="s">
+        <v>28</v>
+      </c>
+      <c r="J46" s="62" t="s">
+        <v>29</v>
+      </c>
+      <c r="K46" s="62" t="s">
         <v>826</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11">
-      <c r="A46" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="B46" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="E46" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="F46" s="7">
-        <v>0</v>
-      </c>
-      <c r="G46" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="H46" s="62" t="s">
-        <v>84</v>
-      </c>
-      <c r="I46" s="19" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="47" spans="1:11">
@@ -21211,41 +21219,44 @@
         <v>25</v>
       </c>
       <c r="E47" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F47" s="7">
         <v>0</v>
       </c>
-      <c r="G47" s="7"/>
-      <c r="H47" s="7"/>
-      <c r="K47" s="19" t="s">
+      <c r="G47" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="H47" s="62" t="s">
+        <v>84</v>
+      </c>
+      <c r="I47" s="19" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11">
+      <c r="A48" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B48" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="E48" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="F48" s="7">
+        <v>0</v>
+      </c>
+      <c r="G48" s="7"/>
+      <c r="H48" s="7"/>
+      <c r="K48" s="19" t="s">
         <v>108</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" s="24" customFormat="1">
-      <c r="A48" s="22"/>
-      <c r="B48" s="22"/>
-      <c r="E48" s="7" t="s">
-        <v>859</v>
-      </c>
-      <c r="F48" s="7"/>
-      <c r="G48" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="H48" s="7" t="s">
-        <v>492</v>
-      </c>
-      <c r="I48" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="K48" s="28" t="s">
-        <v>862</v>
       </c>
     </row>
     <row r="49" spans="1:26" s="24" customFormat="1">
       <c r="A49" s="22"/>
       <c r="B49" s="22"/>
-      <c r="E49" s="7" t="s">
+      <c r="E49" s="63" t="s">
         <v>860</v>
       </c>
       <c r="F49" s="7"/>
@@ -21266,89 +21277,87 @@
       <c r="A50" s="22"/>
       <c r="B50" s="22"/>
       <c r="E50" s="7" t="s">
-        <v>872</v>
+        <v>859</v>
       </c>
       <c r="F50" s="7"/>
       <c r="G50" s="7" t="s">
         <v>126</v>
       </c>
       <c r="H50" s="7" t="s">
-        <v>112</v>
+        <v>492</v>
       </c>
       <c r="I50" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="J50" s="24" t="s">
+      <c r="K50" s="28" t="s">
+        <v>874</v>
+      </c>
+    </row>
+    <row r="51" spans="1:26" s="67" customFormat="1">
+      <c r="A51" s="64"/>
+      <c r="B51" s="64"/>
+      <c r="E51" s="69" t="s">
+        <v>871</v>
+      </c>
+      <c r="F51" s="69"/>
+      <c r="G51" s="69" t="s">
+        <v>126</v>
+      </c>
+      <c r="H51" s="69" t="s">
+        <v>112</v>
+      </c>
+      <c r="I51" s="67" t="s">
+        <v>28</v>
+      </c>
+      <c r="J51" s="67" t="s">
         <v>29</v>
       </c>
-      <c r="K50" s="28" t="s">
-        <v>873</v>
-      </c>
-    </row>
-    <row r="51" spans="1:26">
-      <c r="A51" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="B51" s="29" t="s">
+      <c r="K51" s="65" t="s">
+        <v>872</v>
+      </c>
+    </row>
+    <row r="52" spans="1:26">
+      <c r="A52" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="B52" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="C51" s="19" t="s">
+      <c r="C52" s="19" t="s">
         <v>109</v>
       </c>
-      <c r="D51" s="19" t="s">
+      <c r="D52" s="19" t="s">
         <v>110</v>
       </c>
-      <c r="E51" s="20" t="s">
+      <c r="E52" s="20" t="s">
         <v>111</v>
       </c>
-      <c r="F51" s="7"/>
-      <c r="G51" s="20" t="s">
+      <c r="F52" s="7"/>
+      <c r="G52" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="H51" s="20" t="s">
+      <c r="H52" s="20" t="s">
         <v>112</v>
       </c>
-      <c r="I51" s="19" t="s">
+      <c r="I52" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="J51" s="19" t="s">
+      <c r="J52" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="K51" s="19" t="s">
+      <c r="K52" s="19" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="52" spans="1:26">
-      <c r="A52" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="B52" s="17" t="s">
+    <row r="53" spans="1:26">
+      <c r="A53" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B53" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="E52" s="7" t="s">
+      <c r="E53" s="7" t="s">
         <v>114</v>
-      </c>
-      <c r="F52" s="20">
-        <v>1</v>
-      </c>
-      <c r="G52" s="20" t="s">
-        <v>115</v>
-      </c>
-      <c r="H52" s="20" t="s">
-        <v>116</v>
-      </c>
-      <c r="J52" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="K52" s="19" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="53" spans="1:26">
-      <c r="A53" s="17"/>
-      <c r="B53" s="17"/>
-      <c r="E53" s="20" t="s">
-        <v>118</v>
       </c>
       <c r="F53" s="20">
         <v>1</v>
@@ -21359,167 +21368,157 @@
       <c r="H53" s="20" t="s">
         <v>116</v>
       </c>
-      <c r="I53" s="19" t="s">
-        <v>28</v>
-      </c>
       <c r="J53" s="19" t="s">
         <v>34</v>
       </c>
       <c r="K53" s="19" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="54" spans="1:26">
+      <c r="A54" s="17"/>
+      <c r="B54" s="17"/>
+      <c r="E54" s="20" t="s">
+        <v>118</v>
+      </c>
+      <c r="F54" s="20">
+        <v>1</v>
+      </c>
+      <c r="G54" s="20" t="s">
+        <v>115</v>
+      </c>
+      <c r="H54" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="I54" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="J54" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="K54" s="19" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="54" spans="1:26" s="24" customFormat="1" ht="14.25" customHeight="1">
-      <c r="C54" s="33"/>
-      <c r="D54" s="33"/>
-      <c r="E54" s="7" t="s">
+    <row r="55" spans="1:26" s="24" customFormat="1" ht="14.25" customHeight="1">
+      <c r="C55" s="33"/>
+      <c r="D55" s="33"/>
+      <c r="E55" s="7" t="s">
         <v>832</v>
       </c>
-      <c r="F54" s="7"/>
-      <c r="G54" s="85" t="s">
+      <c r="F55" s="7"/>
+      <c r="G55" s="85" t="s">
         <v>32</v>
       </c>
-      <c r="H54" s="85" t="s">
+      <c r="H55" s="85" t="s">
         <v>244</v>
       </c>
-      <c r="I54" s="85" t="s">
+      <c r="I55" s="85" t="s">
         <v>40</v>
       </c>
-      <c r="J54" s="85" t="s">
+      <c r="J55" s="85" t="s">
         <v>29</v>
       </c>
-      <c r="K54" s="62" t="s">
+      <c r="K55" s="62" t="s">
         <v>833</v>
       </c>
-      <c r="L54" s="85" t="s">
+      <c r="L55" s="85" t="s">
         <v>834</v>
       </c>
-      <c r="M54" s="3"/>
-      <c r="N54" s="7"/>
-      <c r="O54" s="7"/>
-      <c r="P54" s="7"/>
-      <c r="Q54" s="7"/>
-      <c r="R54" s="7"/>
-      <c r="S54" s="7"/>
-      <c r="T54" s="7"/>
-      <c r="U54" s="7"/>
-      <c r="V54" s="7"/>
-      <c r="W54" s="7"/>
-      <c r="X54" s="7"/>
-    </row>
-    <row r="55" spans="1:26">
-      <c r="A55" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="B55" s="17" t="s">
+      <c r="M55" s="3"/>
+      <c r="N55" s="7"/>
+      <c r="O55" s="7"/>
+      <c r="P55" s="7"/>
+      <c r="Q55" s="7"/>
+      <c r="R55" s="7"/>
+      <c r="S55" s="7"/>
+      <c r="T55" s="7"/>
+      <c r="U55" s="7"/>
+      <c r="V55" s="7"/>
+      <c r="W55" s="7"/>
+      <c r="X55" s="7"/>
+    </row>
+    <row r="56" spans="1:26">
+      <c r="A56" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B56" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="E55" s="7" t="s">
+      <c r="E56" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="F55" s="7">
+      <c r="F56" s="7">
         <v>-1</v>
       </c>
-      <c r="G55" s="7"/>
-      <c r="H55" s="7"/>
-    </row>
-    <row r="56" spans="1:26">
-      <c r="A56" s="17"/>
-      <c r="B56" s="17"/>
-      <c r="C56" s="7" t="s">
+      <c r="G56" s="7"/>
+      <c r="H56" s="7"/>
+    </row>
+    <row r="57" spans="1:26">
+      <c r="A57" s="17"/>
+      <c r="B57" s="17"/>
+      <c r="C57" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="D56" s="7" t="s">
+      <c r="D57" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="E56" s="7" t="s">
+      <c r="E57" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="F56" s="7">
+      <c r="F57" s="7">
         <v>0.6</v>
       </c>
-      <c r="G56" s="7" t="s">
+      <c r="G57" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="H56" s="7" t="s">
+      <c r="H57" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="I56" s="7" t="s">
+      <c r="I57" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="J56" s="7" t="s">
+      <c r="J57" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="K56" s="7" t="s">
+      <c r="K57" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="L56" s="7"/>
-      <c r="M56" s="7"/>
-      <c r="N56" s="7"/>
-      <c r="O56" s="7"/>
-      <c r="P56" s="7"/>
-      <c r="Q56" s="7"/>
-      <c r="R56" s="7"/>
-      <c r="S56" s="7"/>
-      <c r="T56" s="7"/>
-      <c r="U56" s="7"/>
-      <c r="V56" s="7"/>
-      <c r="W56" s="7"/>
-      <c r="X56" s="7"/>
-      <c r="Y56" s="7"/>
-      <c r="Z56" s="7"/>
-    </row>
-    <row r="57" spans="1:26">
-      <c r="A57" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="B57" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="E57" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="F57" s="7">
-        <v>1739.927555</v>
-      </c>
-      <c r="G57" s="7"/>
-      <c r="H57" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="K57" s="3" t="s">
-        <v>130</v>
-      </c>
+      <c r="L57" s="7"/>
+      <c r="M57" s="7"/>
+      <c r="N57" s="7"/>
+      <c r="O57" s="7"/>
+      <c r="P57" s="7"/>
+      <c r="Q57" s="7"/>
+      <c r="R57" s="7"/>
+      <c r="S57" s="7"/>
+      <c r="T57" s="7"/>
+      <c r="U57" s="7"/>
+      <c r="V57" s="7"/>
+      <c r="W57" s="7"/>
+      <c r="X57" s="7"/>
+      <c r="Y57" s="7"/>
+      <c r="Z57" s="7"/>
     </row>
     <row r="58" spans="1:26">
       <c r="A58" s="17" t="s">
         <v>24</v>
       </c>
       <c r="B58" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="C58" s="3" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="E58" s="7" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="F58" s="7">
-        <v>1</v>
-      </c>
-      <c r="G58" s="7" t="s">
-        <v>53</v>
-      </c>
+        <v>1739.927555</v>
+      </c>
+      <c r="G58" s="7"/>
       <c r="H58" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="I58" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="J58" s="3" t="s">
-        <v>34</v>
+        <v>96</v>
       </c>
       <c r="K58" s="3" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="59" spans="1:26">
@@ -21529,14 +21528,30 @@
       <c r="B59" s="17" t="s">
         <v>25</v>
       </c>
+      <c r="C59" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="E59" s="7" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="F59" s="7">
-        <v>553659</v>
-      </c>
-      <c r="G59" s="7"/>
-      <c r="H59" s="7"/>
+        <v>1</v>
+      </c>
+      <c r="G59" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="H59" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="I59" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="J59" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="K59" s="3" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="60" spans="1:26">
       <c r="A60" s="17" t="s">
@@ -21546,10 +21561,10 @@
         <v>25</v>
       </c>
       <c r="E60" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F60" s="7">
-        <v>4891208</v>
+        <v>553659</v>
       </c>
       <c r="G60" s="7"/>
       <c r="H60" s="7"/>
@@ -21561,30 +21576,14 @@
       <c r="B61" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="C61" s="3" t="s">
-        <v>25</v>
-      </c>
       <c r="E61" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F61" s="7">
-        <v>1</v>
-      </c>
-      <c r="G61" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="H61" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="I61" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="J61" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="K61" s="3" t="s">
-        <v>140</v>
-      </c>
+        <v>4891208</v>
+      </c>
+      <c r="G61" s="7"/>
+      <c r="H61" s="7"/>
     </row>
     <row r="62" spans="1:26">
       <c r="A62" s="17" t="s">
@@ -21597,10 +21596,10 @@
         <v>25</v>
       </c>
       <c r="E62" s="7" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="F62" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G62" s="7" t="s">
         <v>53</v>
@@ -21615,64 +21614,63 @@
         <v>34</v>
       </c>
       <c r="K62" s="3" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="63" spans="1:26">
+      <c r="A63" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B63" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E63" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="F63" s="7">
+        <v>0</v>
+      </c>
+      <c r="G63" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="H63" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="I63" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="J63" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="K63" s="3" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="63" spans="1:26" s="24" customFormat="1">
-      <c r="A63" s="22" t="s">
+    <row r="64" spans="1:26" s="24" customFormat="1">
+      <c r="A64" s="22" t="s">
         <v>857</v>
       </c>
-      <c r="B63" s="22" t="s">
+      <c r="B64" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="C63" s="3" t="s">
+      <c r="C64" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="D63" s="24" t="s">
+      <c r="D64" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="E63" s="7" t="s">
+      <c r="E64" s="7" t="s">
         <v>856</v>
       </c>
-      <c r="F63" s="7">
+      <c r="F64" s="7">
         <v>5</v>
       </c>
-      <c r="G63" s="7" t="s">
+      <c r="G64" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="H63" s="7" t="s">
-        <v>146</v>
-      </c>
-      <c r="I63" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="J63" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="K63" s="3" t="s">
-        <v>858</v>
-      </c>
-      <c r="L63" s="28" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="64" spans="1:26">
-      <c r="A64" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="B64" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="D64" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="E64" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="F64" s="7">
-        <v>0</v>
-      </c>
-      <c r="G64" s="7"/>
       <c r="H64" s="7" t="s">
         <v>146</v>
       </c>
@@ -21683,44 +21681,55 @@
         <v>29</v>
       </c>
       <c r="K64" s="3" t="s">
-        <v>147</v>
+        <v>858</v>
+      </c>
+      <c r="L64" s="28" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="65" spans="1:11">
       <c r="A65" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="B65" s="17"/>
+      <c r="B65" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="D65" s="3" t="s">
+        <v>144</v>
+      </c>
       <c r="E65" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="F65" s="7">
+        <v>0</v>
+      </c>
+      <c r="G65" s="7"/>
+      <c r="H65" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="I65" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="J65" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="K65" s="3" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11">
+      <c r="A66" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B66" s="17"/>
+      <c r="E66" s="7" t="s">
         <v>148</v>
       </c>
-      <c r="F65" s="7">
+      <c r="F66" s="7">
         <v>6772</v>
       </c>
-      <c r="G65" s="7"/>
-      <c r="H65" s="7"/>
-    </row>
-    <row r="66" spans="1:11" s="24" customFormat="1">
-      <c r="A66" s="22"/>
-      <c r="B66" s="22"/>
-      <c r="E66" s="7" t="s">
-        <v>864</v>
-      </c>
-      <c r="F66" s="7">
-        <v>1</v>
-      </c>
-      <c r="G66" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="H66" s="7" t="s">
-        <v>865</v>
-      </c>
-      <c r="I66" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="J66" s="28" t="s">
-        <v>866</v>
-      </c>
+      <c r="G66" s="7"/>
+      <c r="H66" s="7"/>
     </row>
     <row r="67" spans="1:11" s="24" customFormat="1">
       <c r="A67" s="22"/>
@@ -21729,39 +21738,35 @@
         <v>863</v>
       </c>
       <c r="F67" s="7">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="G67" s="7" t="s">
         <v>126</v>
       </c>
       <c r="H67" s="7" t="s">
-        <v>643</v>
+        <v>864</v>
       </c>
       <c r="I67" s="28" t="s">
         <v>28</v>
       </c>
       <c r="J67" s="28" t="s">
-        <v>29</v>
-      </c>
-      <c r="K67" s="28" t="s">
-        <v>869</v>
+        <v>865</v>
       </c>
     </row>
     <row r="68" spans="1:11" s="24" customFormat="1">
       <c r="A68" s="22"/>
       <c r="B68" s="22"/>
-      <c r="D68" s="62" t="s">
-        <v>26</v>
-      </c>
       <c r="E68" s="7" t="s">
-        <v>813</v>
-      </c>
-      <c r="F68" s="7"/>
-      <c r="G68" s="63" t="s">
-        <v>32</v>
+        <v>862</v>
+      </c>
+      <c r="F68" s="7">
+        <v>10</v>
+      </c>
+      <c r="G68" s="7" t="s">
+        <v>126</v>
       </c>
       <c r="H68" s="7" t="s">
-        <v>84</v>
+        <v>643</v>
       </c>
       <c r="I68" s="28" t="s">
         <v>28</v>
@@ -21770,19 +21775,17 @@
         <v>29</v>
       </c>
       <c r="K68" s="28" t="s">
-        <v>814</v>
+        <v>868</v>
       </c>
     </row>
     <row r="69" spans="1:11" s="24" customFormat="1">
-      <c r="A69" s="22" t="s">
-        <v>24</v>
-      </c>
+      <c r="A69" s="22"/>
       <c r="B69" s="22"/>
       <c r="D69" s="62" t="s">
         <v>26</v>
       </c>
       <c r="E69" s="7" t="s">
-        <v>815</v>
+        <v>813</v>
       </c>
       <c r="F69" s="7"/>
       <c r="G69" s="63" t="s">
@@ -21798,39 +21801,35 @@
         <v>29</v>
       </c>
       <c r="K69" s="28" t="s">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" s="24" customFormat="1">
+      <c r="A70" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="B70" s="22"/>
+      <c r="D70" s="62" t="s">
+        <v>26</v>
+      </c>
+      <c r="E70" s="7" t="s">
+        <v>815</v>
+      </c>
+      <c r="F70" s="7"/>
+      <c r="G70" s="63" t="s">
+        <v>32</v>
+      </c>
+      <c r="H70" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="I70" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="J70" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="K70" s="28" t="s">
         <v>816</v>
-      </c>
-    </row>
-    <row r="70" spans="1:11">
-      <c r="A70" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="B70" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="D70" s="19" t="s">
-        <v>150</v>
-      </c>
-      <c r="E70" s="20" t="s">
-        <v>152</v>
-      </c>
-      <c r="F70" s="20">
-        <v>1500</v>
-      </c>
-      <c r="G70" s="20" t="s">
-        <v>126</v>
-      </c>
-      <c r="H70" s="20" t="s">
-        <v>96</v>
-      </c>
-      <c r="I70" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="J70" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="K70" s="19" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="71" spans="1:11">
@@ -21843,16 +21842,16 @@
       <c r="D71" s="19" t="s">
         <v>150</v>
       </c>
-      <c r="E71" s="19" t="s">
-        <v>157</v>
-      </c>
-      <c r="F71" s="19">
+      <c r="E71" s="20" t="s">
+        <v>152</v>
+      </c>
+      <c r="F71" s="20">
         <v>1500</v>
       </c>
       <c r="G71" s="20" t="s">
         <v>126</v>
       </c>
-      <c r="H71" s="19" t="s">
+      <c r="H71" s="20" t="s">
         <v>96</v>
       </c>
       <c r="I71" s="19" t="s">
@@ -21862,7 +21861,7 @@
         <v>34</v>
       </c>
       <c r="K71" s="19" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="72" spans="1:11">
@@ -21876,7 +21875,7 @@
         <v>150</v>
       </c>
       <c r="E72" s="19" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="F72" s="19">
         <v>1500</v>
@@ -21894,7 +21893,7 @@
         <v>34</v>
       </c>
       <c r="K72" s="19" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="73" spans="1:11">
@@ -21902,16 +21901,16 @@
         <v>24</v>
       </c>
       <c r="B73" s="18" t="s">
-        <v>162</v>
+        <v>25</v>
       </c>
       <c r="D73" s="19" t="s">
         <v>150</v>
       </c>
       <c r="E73" s="19" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="F73" s="19">
-        <v>1000</v>
+        <v>1500</v>
       </c>
       <c r="G73" s="20" t="s">
         <v>126</v>
@@ -21926,7 +21925,7 @@
         <v>34</v>
       </c>
       <c r="K73" s="19" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="74" spans="1:11">
@@ -21940,7 +21939,7 @@
         <v>150</v>
       </c>
       <c r="E74" s="19" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="F74" s="19">
         <v>1000</v>
@@ -21949,7 +21948,7 @@
         <v>126</v>
       </c>
       <c r="H74" s="19" t="s">
-        <v>123</v>
+        <v>96</v>
       </c>
       <c r="I74" s="19" t="s">
         <v>40</v>
@@ -21958,7 +21957,7 @@
         <v>34</v>
       </c>
       <c r="K74" s="19" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="75" spans="1:11">
@@ -21972,7 +21971,7 @@
         <v>150</v>
       </c>
       <c r="E75" s="19" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="F75" s="19">
         <v>1000</v>
@@ -21990,13 +21989,45 @@
         <v>34</v>
       </c>
       <c r="K75" s="19" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11">
+      <c r="A76" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B76" s="18" t="s">
+        <v>162</v>
+      </c>
+      <c r="D76" s="19" t="s">
+        <v>150</v>
+      </c>
+      <c r="E76" s="19" t="s">
+        <v>167</v>
+      </c>
+      <c r="F76" s="19">
+        <v>1000</v>
+      </c>
+      <c r="G76" s="20" t="s">
+        <v>126</v>
+      </c>
+      <c r="H76" s="19" t="s">
+        <v>123</v>
+      </c>
+      <c r="I76" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="J76" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="K76" s="19" t="s">
         <v>168</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B51">
+  <conditionalFormatting sqref="B52">
     <cfRule type="notContainsBlanks" dxfId="0" priority="1">
-      <formula>LEN(TRIM(B51))&gt;0</formula>
+      <formula>LEN(TRIM(B52))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
WORK-IN-PROGRESS. Continuing application of water parcel logic to reservoirs. Add Reach attribute Q_UPSTREAM. Add FLOW BLU analysis report. Flow.cpp, .h - Add Reach attribute Q_UPSTREAM. ReachRouting.cpp - Add Reach attribute Q_UPSTREAM.
</commit_message>
<xml_diff>
--- a/DataCW3M/CW3MdigitalHandbook/CW3MdataDictionary.xlsx
+++ b/DataCW3M/CW3MdigitalHandbook/CW3MdataDictionary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\CW3MdigitalHandbook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8857B367-538E-4106-9982-93434C3F898F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B67ADA0-3474-48DA-86DA-5634FB26D9D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -96,7 +96,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2763" uniqueCount="882">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2763" uniqueCount="883">
   <si>
     <t>LULC_A</t>
   </si>
@@ -2743,6 +2743,9 @@
   </si>
   <si>
     <t>nominal low flow</t>
+  </si>
+  <si>
+    <t>if this reach is the outfall of a reservoir, then RES_OUT = the reservoir ID for that reservoir, else RES_OUT = 0. Note that when RESOUTFALL is nonzero, RES_ID will usually be 0, i.e. the outfall reach is not in the reservoir itself.</t>
   </si>
 </sst>
 </file>
@@ -2865,7 +2868,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -3075,6 +3078,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -20104,8 +20110,8 @@
   <dimension ref="A1:Z79"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F51" sqref="F51"/>
+      <pane ySplit="4" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K56" sqref="K56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -20114,8 +20120,9 @@
     <col min="4" max="4" width="22.44140625" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
     <col min="6" max="8" width="11.5546875" customWidth="1"/>
-    <col min="9" max="10" width="7.5546875" customWidth="1"/>
-    <col min="11" max="11" width="17.5546875" customWidth="1"/>
+    <col min="9" max="9" width="7.5546875" customWidth="1"/>
+    <col min="10" max="10" width="11.5546875" customWidth="1"/>
+    <col min="11" max="11" width="39.88671875" customWidth="1"/>
     <col min="12" max="12" width="64" customWidth="1"/>
     <col min="13" max="24" width="7.5546875" customWidth="1"/>
     <col min="25" max="26" width="12.5546875" customWidth="1"/>
@@ -21419,7 +21426,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="55" spans="1:26" ht="14.4">
+    <row r="55" spans="1:26" ht="43.2">
       <c r="A55" s="17" t="s">
         <v>24</v>
       </c>
@@ -21441,33 +21448,33 @@
       <c r="J55" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="K55" s="19" t="s">
+      <c r="K55" s="21" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="56" spans="1:26" ht="14.4">
-      <c r="A56" s="17"/>
-      <c r="B56" s="17"/>
-      <c r="E56" s="20" t="s">
+    <row r="56" spans="1:26" s="30" customFormat="1" ht="86.4">
+      <c r="A56" s="96"/>
+      <c r="B56" s="96"/>
+      <c r="E56" s="30" t="s">
         <v>118</v>
       </c>
-      <c r="F56" s="20">
+      <c r="F56" s="30">
         <v>1</v>
       </c>
-      <c r="G56" s="20" t="s">
+      <c r="G56" s="30" t="s">
         <v>115</v>
       </c>
-      <c r="H56" s="20" t="s">
+      <c r="H56" s="30" t="s">
         <v>116</v>
       </c>
-      <c r="I56" s="19" t="s">
+      <c r="I56" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="J56" s="19" t="s">
+      <c r="J56" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="K56" s="19" t="s">
-        <v>119</v>
+      <c r="K56" s="95" t="s">
+        <v>882</v>
       </c>
     </row>
     <row r="57" spans="1:26" s="24" customFormat="1" ht="14.25" customHeight="1">

</xml_diff>

<commit_message>
Add McKenzie basin thermal energy budget report, and switch to new 2010-19 actual weather data. Flow_McKenzie.xml - Switch to new 2010-19 actual weather climate files for the BaselineGridMultiyearFiles climate scenario. Add "FLOW Daily Thermal Energy Budget for McKenzie basin streams" report. Reach_McKenzie.dbf - Add DIRECTION, IN_RUNOF_C, SPRINGTEMP, RESAREA_HA, RES_TEMP. Removed HUC_5, HUC6, and DS_Res as obsolete. Flow.cpp, .h - Added Reach attributes RES_H2O, RES_TEMP, RESAREA_HA, SPRINGTEMP, and IN_RUNOF_C. FluxExpr.cpp, GlobalMethods.h - Add Reach attribute SPRINGTEMP. WaterRights.h, .cpp - Delete unused Reach attribute DS_Res.
</commit_message>
<xml_diff>
--- a/DataCW3M/CW3MdigitalHandbook/CW3MdataDictionary.xlsx
+++ b/DataCW3M/CW3MdigitalHandbook/CW3MdataDictionary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\CW3MdigitalHandbook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{609E827C-4FF5-4A99-9880-86C802BBDEEB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC9706D9-25A4-49D1-8C58-4C901B2D46E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -96,7 +96,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2834" uniqueCount="922">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2873" uniqueCount="938">
   <si>
     <t>LULC_A</t>
   </si>
@@ -2853,9 +2853,6 @@
     <t>IDU INDEX of representative IDU on rightt bank of reach looking downstream</t>
   </si>
   <si>
-    <t>12/15/20 Changed BANK_L_IDU and BANK_R_IDU from IDU IDs to IDU indices. Added DIRECTION.</t>
-  </si>
-  <si>
     <t>DIRECTION</t>
   </si>
   <si>
@@ -2863,6 +2860,57 @@
   </si>
   <si>
     <t>net direction of flow in reach, from upstream end to downstream end</t>
+  </si>
+  <si>
+    <t>temperature of inflow from springs</t>
+  </si>
+  <si>
+    <t>IN_RUNOF_C</t>
+  </si>
+  <si>
+    <t>temperature of IN_RUNOFF</t>
+  </si>
+  <si>
+    <t>long</t>
+  </si>
+  <si>
+    <t>"Exotic" is a species group in APs.xml</t>
+  </si>
+  <si>
+    <t>FishModel</t>
+  </si>
+  <si>
+    <t>Long</t>
+  </si>
+  <si>
+    <t>"Native" is a species group in APs.xml</t>
+  </si>
+  <si>
+    <t>area of reservoir water surface, updated daily</t>
+  </si>
+  <si>
+    <t>RES_H2O</t>
+  </si>
+  <si>
+    <t>volume of water in the reservoir, updated daily</t>
+  </si>
+  <si>
+    <t>RES_TEMP</t>
+  </si>
+  <si>
+    <t>temperature of water in the reservoir, updated daily</t>
+  </si>
+  <si>
+    <t>RESAREA_HA</t>
+  </si>
+  <si>
+    <t>ha</t>
+  </si>
+  <si>
+    <t>SPRINGTEMP</t>
+  </si>
+  <si>
+    <t>12/16/20 Changed BANK_L_IDU and BANK_R_IDU from IDU IDs to IDU indices. Added DIRECTION, IN_RUNOF_C, SPRINGTEMP, RESAREA_HA, RES_H2O, RES_TEMP. Removed HUC_5, HUC6, and DS_Res as obsolete.</t>
   </si>
 </sst>
 </file>
@@ -8830,7 +8878,7 @@
   <dimension ref="A1:Z1047"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="3" topLeftCell="A128" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="H199" sqref="H199"/>
     </sheetView>
   </sheetViews>
@@ -20550,11 +20598,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Z80"/>
+  <dimension ref="A1:Z86"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K18" sqref="K18"/>
+      <pane ySplit="4" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -20631,7 +20679,7 @@
     </row>
     <row r="3" spans="1:26" s="63" customFormat="1" ht="12.75" customHeight="1">
       <c r="A3" s="68" t="s">
-        <v>918</v>
+        <v>937</v>
       </c>
       <c r="B3" s="66"/>
       <c r="C3" s="65"/>
@@ -20995,7 +21043,7 @@
       <c r="B18" s="22"/>
       <c r="D18" s="3"/>
       <c r="E18" s="7" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="F18" s="7">
         <v>90</v>
@@ -21004,13 +21052,13 @@
         <v>124</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="J18" s="23" t="s">
         <v>33</v>
       </c>
       <c r="K18" s="23" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
     </row>
     <row r="19" spans="1:26" ht="14.4">
@@ -21132,7 +21180,10 @@
         <v>24</v>
       </c>
       <c r="B23" s="17" t="s">
-        <v>29</v>
+        <v>25</v>
+      </c>
+      <c r="D23" t="s">
+        <v>926</v>
       </c>
       <c r="E23" s="7" t="s">
         <v>57</v>
@@ -21140,8 +21191,13 @@
       <c r="F23" s="7">
         <v>0</v>
       </c>
-      <c r="G23" s="7"/>
+      <c r="G23" s="7" t="s">
+        <v>924</v>
+      </c>
       <c r="H23" s="7"/>
+      <c r="K23" s="25" t="s">
+        <v>925</v>
+      </c>
     </row>
     <row r="24" spans="1:26" ht="14.4">
       <c r="A24" s="17" t="s">
@@ -21404,25 +21460,28 @@
         <v>874</v>
       </c>
     </row>
-    <row r="36" spans="1:11" ht="14.4">
-      <c r="A36" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="B36" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="E36" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="F36" s="7">
-        <v>0</v>
-      </c>
-      <c r="G36" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="H36" s="7"/>
-      <c r="K36" s="3" t="s">
-        <v>81</v>
+    <row r="36" spans="1:11" s="23" customFormat="1" ht="14.4">
+      <c r="A36" s="22"/>
+      <c r="B36" s="22"/>
+      <c r="D36" s="24"/>
+      <c r="E36" s="23" t="s">
+        <v>922</v>
+      </c>
+      <c r="F36" s="7"/>
+      <c r="G36" s="59" t="s">
+        <v>124</v>
+      </c>
+      <c r="H36" s="59" t="s">
+        <v>144</v>
+      </c>
+      <c r="I36" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="J36" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="K36" s="25" t="s">
+        <v>923</v>
       </c>
     </row>
     <row r="37" spans="1:11" ht="14.4">
@@ -21432,23 +21491,18 @@
       <c r="B37" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="D37" s="3" t="s">
-        <v>44</v>
-      </c>
       <c r="E37" s="7" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F37" s="7">
         <v>0</v>
       </c>
-      <c r="G37" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="H37" s="20" t="s">
-        <v>83</v>
-      </c>
-      <c r="K37" s="19" t="s">
-        <v>84</v>
+      <c r="G37" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="H37" s="7"/>
+      <c r="K37" s="3" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="38" spans="1:11" ht="14.4">
@@ -21458,20 +21512,23 @@
       <c r="B38" s="17" t="s">
         <v>25</v>
       </c>
+      <c r="D38" s="3" t="s">
+        <v>44</v>
+      </c>
       <c r="E38" s="7" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="F38" s="7">
         <v>0</v>
       </c>
       <c r="G38" s="20" t="s">
-        <v>52</v>
+        <v>31</v>
       </c>
       <c r="H38" s="20" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="K38" s="19" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="39" spans="1:11" ht="14.4">
@@ -21482,19 +21539,19 @@
         <v>25</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="F39" s="7">
         <v>0</v>
       </c>
       <c r="G39" s="20" t="s">
-        <v>31</v>
+        <v>52</v>
       </c>
       <c r="H39" s="20" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="K39" s="19" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="40" spans="1:11" ht="14.4">
@@ -21505,19 +21562,19 @@
         <v>25</v>
       </c>
       <c r="E40" s="7" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F40" s="7">
         <v>0</v>
       </c>
       <c r="G40" s="20" t="s">
-        <v>52</v>
+        <v>31</v>
       </c>
       <c r="H40" s="20" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="K40" s="19" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="41" spans="1:11" ht="14.4">
@@ -21527,27 +21584,20 @@
       <c r="B41" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="C41" s="3" t="s">
-        <v>25</v>
-      </c>
       <c r="E41" s="7" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F41" s="7">
-        <v>1739.9274680000001</v>
-      </c>
-      <c r="G41" s="7"/>
-      <c r="H41" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="I41" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="J41" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="K41" s="3" t="s">
-        <v>95</v>
+        <v>0</v>
+      </c>
+      <c r="G41" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="H41" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="K41" s="19" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="42" spans="1:11" ht="14.4">
@@ -21557,30 +21607,44 @@
       <c r="B42" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="D42" s="3" t="s">
-        <v>49</v>
+      <c r="C42" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="E42" s="7" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="F42" s="7">
-        <v>6699</v>
+        <v>1739.9274680000001</v>
       </c>
       <c r="G42" s="7"/>
-      <c r="H42" s="7"/>
+      <c r="H42" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="I42" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="J42" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="K42" s="3" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="43" spans="1:11" ht="14.4">
       <c r="A43" s="17" t="s">
         <v>24</v>
       </c>
       <c r="B43" s="17" t="s">
-        <v>29</v>
+        <v>25</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>49</v>
       </c>
       <c r="E43" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F43" s="7">
-        <v>0</v>
+        <v>6699</v>
       </c>
       <c r="G43" s="7"/>
       <c r="H43" s="7"/>
@@ -21592,19 +21656,24 @@
       <c r="B44" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="D44" s="3" t="s">
-        <v>44</v>
+      <c r="D44" t="s">
+        <v>926</v>
       </c>
       <c r="E44" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F44" s="7">
         <v>0</v>
       </c>
-      <c r="G44" s="7"/>
+      <c r="G44" s="7" t="s">
+        <v>927</v>
+      </c>
       <c r="H44" s="7"/>
-    </row>
-    <row r="45" spans="1:11" ht="57.6">
+      <c r="K44" s="25" t="s">
+        <v>928</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" ht="14.4">
       <c r="A45" s="17" t="s">
         <v>24</v>
       </c>
@@ -21612,27 +21681,18 @@
         <v>25</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>99</v>
+        <v>44</v>
       </c>
       <c r="E45" s="7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F45" s="7">
         <v>0</v>
       </c>
       <c r="G45" s="7"/>
-      <c r="H45" s="15" t="s">
-        <v>101</v>
-      </c>
-      <c r="I45" s="7"/>
-      <c r="J45" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="K45" s="7" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" ht="14.4">
+      <c r="H45" s="7"/>
+    </row>
+    <row r="46" spans="1:11" ht="57.6">
       <c r="A46" s="17" t="s">
         <v>24</v>
       </c>
@@ -21640,46 +21700,44 @@
         <v>25</v>
       </c>
       <c r="D46" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="E46" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="F46" s="7">
+        <v>0</v>
+      </c>
+      <c r="G46" s="7"/>
+      <c r="H46" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="I46" s="7"/>
+      <c r="J46" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="K46" s="7" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" ht="14.4">
+      <c r="A47" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B47" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="D47" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="E46" s="7" t="s">
+      <c r="E47" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="F46" s="7">
+      <c r="F47" s="7">
         <v>6758</v>
       </c>
-      <c r="G46" s="7"/>
-      <c r="H46" s="7"/>
-    </row>
-    <row r="47" spans="1:11" s="23" customFormat="1" ht="14.4">
-      <c r="A47" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="B47" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="D47" s="3" t="s">
-        <v>819</v>
-      </c>
-      <c r="E47" s="7" t="s">
-        <v>816</v>
-      </c>
-      <c r="F47" s="7"/>
-      <c r="G47" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="H47" s="60" t="s">
-        <v>83</v>
-      </c>
-      <c r="I47" s="59" t="s">
-        <v>27</v>
-      </c>
-      <c r="J47" s="59" t="s">
-        <v>28</v>
-      </c>
-      <c r="K47" s="59" t="s">
-        <v>818</v>
-      </c>
+      <c r="G47" s="7"/>
+      <c r="H47" s="7"/>
     </row>
     <row r="48" spans="1:11" s="23" customFormat="1" ht="14.4">
       <c r="A48" s="22" t="s">
@@ -21689,10 +21747,10 @@
         <v>25</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>820</v>
-      </c>
-      <c r="E48" s="60" t="s">
-        <v>817</v>
+        <v>819</v>
+      </c>
+      <c r="E48" s="7" t="s">
+        <v>816</v>
       </c>
       <c r="F48" s="7"/>
       <c r="G48" s="7" t="s">
@@ -21708,33 +21766,40 @@
         <v>28</v>
       </c>
       <c r="K48" s="59" t="s">
+        <v>818</v>
+      </c>
+    </row>
+    <row r="49" spans="1:24" s="23" customFormat="1" ht="14.4">
+      <c r="A49" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="B49" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>820</v>
+      </c>
+      <c r="E49" s="60" t="s">
+        <v>817</v>
+      </c>
+      <c r="F49" s="7"/>
+      <c r="G49" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="H49" s="60" t="s">
+        <v>83</v>
+      </c>
+      <c r="I49" s="59" t="s">
+        <v>27</v>
+      </c>
+      <c r="J49" s="59" t="s">
+        <v>28</v>
+      </c>
+      <c r="K49" s="59" t="s">
         <v>821</v>
       </c>
     </row>
-    <row r="49" spans="1:26" ht="14.4">
-      <c r="A49" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="B49" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="E49" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="F49" s="7">
-        <v>0</v>
-      </c>
-      <c r="G49" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="H49" s="59" t="s">
-        <v>83</v>
-      </c>
-      <c r="I49" s="19" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="50" spans="1:26" ht="14.4">
+    <row r="50" spans="1:24" ht="14.4">
       <c r="A50" s="17" t="s">
         <v>24</v>
       </c>
@@ -21742,67 +21807,70 @@
         <v>25</v>
       </c>
       <c r="E50" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F50" s="7">
         <v>0</v>
       </c>
-      <c r="G50" s="7"/>
-      <c r="H50" s="7"/>
-      <c r="K50" s="19" t="s">
+      <c r="G50" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="H50" s="59" t="s">
+        <v>83</v>
+      </c>
+      <c r="I50" s="19" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="51" spans="1:24" ht="14.4">
+      <c r="A51" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B51" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="E51" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="F51" s="7">
+        <v>0</v>
+      </c>
+      <c r="G51" s="7"/>
+      <c r="H51" s="7"/>
+      <c r="K51" s="19" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="51" spans="1:26" s="23" customFormat="1" ht="14.4">
-      <c r="A51" s="22"/>
-      <c r="B51" s="22"/>
-      <c r="E51" s="7" t="s">
-        <v>875</v>
-      </c>
-      <c r="F51" s="7">
-        <v>0.08</v>
-      </c>
-      <c r="G51" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="H51" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="I51" s="23" t="s">
-        <v>39</v>
-      </c>
-      <c r="J51" s="23" t="s">
-        <v>33</v>
-      </c>
-      <c r="K51" s="25" t="s">
-        <v>876</v>
-      </c>
-    </row>
-    <row r="52" spans="1:26" s="23" customFormat="1" ht="14.4">
+    <row r="52" spans="1:24" s="23" customFormat="1" ht="14.4">
       <c r="A52" s="22"/>
       <c r="B52" s="22"/>
-      <c r="E52" s="60" t="s">
-        <v>855</v>
-      </c>
-      <c r="F52" s="7"/>
+      <c r="E52" s="7" t="s">
+        <v>875</v>
+      </c>
+      <c r="F52" s="7">
+        <v>0.08</v>
+      </c>
       <c r="G52" s="7" t="s">
         <v>124</v>
       </c>
       <c r="H52" s="7" t="s">
-        <v>490</v>
+        <v>83</v>
       </c>
       <c r="I52" s="23" t="s">
-        <v>27</v>
+        <v>39</v>
+      </c>
+      <c r="J52" s="23" t="s">
+        <v>33</v>
       </c>
       <c r="K52" s="25" t="s">
-        <v>856</v>
-      </c>
-    </row>
-    <row r="53" spans="1:26" s="23" customFormat="1" ht="14.4">
+        <v>876</v>
+      </c>
+    </row>
+    <row r="53" spans="1:24" s="23" customFormat="1" ht="14.4">
       <c r="A53" s="22"/>
       <c r="B53" s="22"/>
-      <c r="E53" s="7" t="s">
-        <v>854</v>
+      <c r="E53" s="60" t="s">
+        <v>855</v>
       </c>
       <c r="F53" s="7"/>
       <c r="G53" s="7" t="s">
@@ -21815,155 +21883,140 @@
         <v>27</v>
       </c>
       <c r="K53" s="25" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="54" spans="1:24" s="23" customFormat="1" ht="14.4">
+      <c r="A54" s="22"/>
+      <c r="B54" s="22"/>
+      <c r="E54" s="7" t="s">
+        <v>854</v>
+      </c>
+      <c r="F54" s="7"/>
+      <c r="G54" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="H54" s="7" t="s">
+        <v>490</v>
+      </c>
+      <c r="I54" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="K54" s="25" t="s">
         <v>869</v>
       </c>
     </row>
-    <row r="54" spans="1:26" s="63" customFormat="1" ht="14.4">
-      <c r="A54" s="61"/>
-      <c r="B54" s="61"/>
-      <c r="E54" s="64" t="s">
+    <row r="55" spans="1:24" s="63" customFormat="1" ht="14.4">
+      <c r="A55" s="61"/>
+      <c r="B55" s="61"/>
+      <c r="E55" s="64" t="s">
         <v>866</v>
       </c>
-      <c r="F54" s="64"/>
-      <c r="G54" s="64" t="s">
+      <c r="F55" s="64"/>
+      <c r="G55" s="64" t="s">
         <v>124</v>
       </c>
-      <c r="H54" s="64" t="s">
+      <c r="H55" s="64" t="s">
         <v>110</v>
       </c>
-      <c r="I54" s="63" t="s">
+      <c r="I55" s="63" t="s">
         <v>27</v>
       </c>
-      <c r="J54" s="63" t="s">
+      <c r="J55" s="63" t="s">
         <v>28</v>
       </c>
-      <c r="K54" s="62" t="s">
+      <c r="K55" s="62" t="s">
         <v>867</v>
       </c>
     </row>
-    <row r="55" spans="1:26" ht="14.4">
-      <c r="A55" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="B55" s="26" t="s">
+    <row r="56" spans="1:24" ht="14.4">
+      <c r="A56" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="B56" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="C55" s="19" t="s">
+      <c r="C56" s="19" t="s">
         <v>107</v>
       </c>
-      <c r="D55" s="19" t="s">
+      <c r="D56" s="19" t="s">
         <v>108</v>
       </c>
-      <c r="E55" s="20" t="s">
+      <c r="E56" s="20" t="s">
         <v>109</v>
       </c>
-      <c r="F55" s="7"/>
-      <c r="G55" s="20" t="s">
+      <c r="F56" s="7"/>
+      <c r="G56" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="H55" s="20" t="s">
+      <c r="H56" s="20" t="s">
         <v>110</v>
       </c>
-      <c r="I55" s="19" t="s">
+      <c r="I56" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="J55" s="19" t="s">
+      <c r="J56" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="K55" s="19" t="s">
+      <c r="K56" s="19" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="56" spans="1:26" ht="43.2">
-      <c r="A56" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="B56" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="E56" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F56" s="20">
-        <v>1</v>
-      </c>
-      <c r="G56" s="20" t="s">
-        <v>113</v>
-      </c>
-      <c r="H56" s="20" t="s">
-        <v>114</v>
-      </c>
-      <c r="J56" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="K56" s="21" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="57" spans="1:26" s="27" customFormat="1" ht="86.4">
-      <c r="A57" s="91"/>
-      <c r="B57" s="91"/>
-      <c r="E57" s="27" t="s">
-        <v>116</v>
-      </c>
-      <c r="F57" s="27">
-        <v>1</v>
-      </c>
-      <c r="G57" s="27" t="s">
-        <v>113</v>
-      </c>
-      <c r="H57" s="27" t="s">
-        <v>114</v>
-      </c>
-      <c r="I57" s="21" t="s">
+    <row r="57" spans="1:24" s="23" customFormat="1" ht="14.4">
+      <c r="A57" s="22"/>
+      <c r="B57" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="C57" s="24"/>
+      <c r="D57" s="24"/>
+      <c r="E57" s="23" t="s">
+        <v>934</v>
+      </c>
+      <c r="F57" s="7"/>
+      <c r="G57" s="23" t="s">
+        <v>124</v>
+      </c>
+      <c r="H57" s="23" t="s">
+        <v>935</v>
+      </c>
+      <c r="I57" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="J57" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="K57" s="90" t="s">
-        <v>877</v>
-      </c>
-    </row>
-    <row r="58" spans="1:26" s="23" customFormat="1" ht="14.25" customHeight="1">
-      <c r="C58" s="30"/>
-      <c r="D58" s="30"/>
-      <c r="E58" s="7" t="s">
-        <v>827</v>
+      <c r="J57" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="K57" s="25" t="s">
+        <v>929</v>
+      </c>
+    </row>
+    <row r="58" spans="1:24" s="23" customFormat="1" ht="14.4">
+      <c r="A58" s="22"/>
+      <c r="B58" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="C58" s="24"/>
+      <c r="D58" s="24"/>
+      <c r="E58" s="23" t="s">
+        <v>930</v>
       </c>
       <c r="F58" s="7"/>
-      <c r="G58" s="80" t="s">
-        <v>31</v>
-      </c>
-      <c r="H58" s="80" t="s">
-        <v>242</v>
-      </c>
-      <c r="I58" s="80" t="s">
-        <v>39</v>
-      </c>
-      <c r="J58" s="80" t="s">
+      <c r="G58" s="23" t="s">
+        <v>124</v>
+      </c>
+      <c r="H58" s="23" t="s">
+        <v>110</v>
+      </c>
+      <c r="I58" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="J58" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="K58" s="59" t="s">
-        <v>828</v>
-      </c>
-      <c r="L58" s="80" t="s">
-        <v>829</v>
-      </c>
-      <c r="M58" s="3"/>
-      <c r="N58" s="7"/>
-      <c r="O58" s="7"/>
-      <c r="P58" s="7"/>
-      <c r="Q58" s="7"/>
-      <c r="R58" s="7"/>
-      <c r="S58" s="7"/>
-      <c r="T58" s="7"/>
-      <c r="U58" s="7"/>
-      <c r="V58" s="7"/>
-      <c r="W58" s="7"/>
-      <c r="X58" s="7"/>
-    </row>
-    <row r="59" spans="1:26" ht="14.4">
+      <c r="K58" s="25" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="59" spans="1:24" ht="43.2">
       <c r="A59" s="17" t="s">
         <v>24</v>
       </c>
@@ -21971,614 +22024,759 @@
         <v>25</v>
       </c>
       <c r="E59" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="F59" s="7">
-        <v>-1</v>
-      </c>
-      <c r="G59" s="7"/>
-      <c r="H59" s="7"/>
-    </row>
-    <row r="60" spans="1:26" ht="14.4">
-      <c r="A60" s="17"/>
-      <c r="B60" s="17"/>
-      <c r="C60" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="D60" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="E60" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="F60" s="7">
-        <v>0.6</v>
-      </c>
-      <c r="G60" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="F59" s="20">
+        <v>1</v>
+      </c>
+      <c r="G59" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="H59" s="20" t="s">
+        <v>114</v>
+      </c>
+      <c r="J59" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="K59" s="21" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="60" spans="1:24" s="27" customFormat="1" ht="86.4">
+      <c r="A60" s="91"/>
+      <c r="B60" s="91"/>
+      <c r="E60" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="F60" s="27">
+        <v>1</v>
+      </c>
+      <c r="G60" s="27" t="s">
+        <v>113</v>
+      </c>
+      <c r="H60" s="27" t="s">
+        <v>114</v>
+      </c>
+      <c r="I60" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="J60" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="K60" s="90" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="61" spans="1:24" s="27" customFormat="1" ht="28.8">
+      <c r="A61" s="91"/>
+      <c r="B61" s="91" t="s">
+        <v>24</v>
+      </c>
+      <c r="E61" s="27" t="s">
+        <v>932</v>
+      </c>
+      <c r="G61" s="27" t="s">
+        <v>124</v>
+      </c>
+      <c r="H61" s="27" t="s">
+        <v>144</v>
+      </c>
+      <c r="I61" s="90" t="s">
+        <v>27</v>
+      </c>
+      <c r="J61" s="21"/>
+      <c r="K61" s="90" t="s">
+        <v>933</v>
+      </c>
+    </row>
+    <row r="62" spans="1:24" s="23" customFormat="1" ht="14.25" customHeight="1">
+      <c r="C62" s="30"/>
+      <c r="D62" s="30"/>
+      <c r="E62" s="7" t="s">
+        <v>827</v>
+      </c>
+      <c r="F62" s="7"/>
+      <c r="G62" s="80" t="s">
         <v>31</v>
       </c>
-      <c r="H60" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="I60" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="J60" s="7" t="s">
+      <c r="H62" s="80" t="s">
+        <v>242</v>
+      </c>
+      <c r="I62" s="80" t="s">
+        <v>39</v>
+      </c>
+      <c r="J62" s="80" t="s">
         <v>28</v>
       </c>
-      <c r="K60" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="L60" s="7"/>
-      <c r="M60" s="7"/>
-      <c r="N60" s="7"/>
-      <c r="O60" s="7"/>
-      <c r="P60" s="7"/>
-      <c r="Q60" s="7"/>
-      <c r="R60" s="7"/>
-      <c r="S60" s="7"/>
-      <c r="T60" s="7"/>
-      <c r="U60" s="7"/>
-      <c r="V60" s="7"/>
-      <c r="W60" s="7"/>
-      <c r="X60" s="7"/>
-      <c r="Y60" s="7"/>
-      <c r="Z60" s="7"/>
-    </row>
-    <row r="61" spans="1:26" ht="14.4">
-      <c r="A61" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="B61" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="E61" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="F61" s="7">
-        <v>1739.927555</v>
-      </c>
-      <c r="G61" s="7"/>
-      <c r="H61" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="K61" s="3" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="62" spans="1:26" s="23" customFormat="1" ht="14.4">
-      <c r="A62" s="22"/>
-      <c r="B62" s="22"/>
-      <c r="E62" s="7" t="s">
-        <v>870</v>
-      </c>
-      <c r="F62" s="7"/>
-      <c r="G62" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="H62" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="I62" s="23" t="s">
-        <v>39</v>
-      </c>
-      <c r="J62" s="23" t="s">
-        <v>33</v>
-      </c>
-      <c r="K62" s="23" t="s">
-        <v>872</v>
-      </c>
-      <c r="L62" s="3" t="s">
-        <v>871</v>
-      </c>
-    </row>
-    <row r="63" spans="1:26" ht="14.4">
+      <c r="K62" s="59" t="s">
+        <v>828</v>
+      </c>
+      <c r="L62" s="80" t="s">
+        <v>829</v>
+      </c>
+      <c r="M62" s="3"/>
+      <c r="N62" s="7"/>
+      <c r="O62" s="7"/>
+      <c r="P62" s="7"/>
+      <c r="Q62" s="7"/>
+      <c r="R62" s="7"/>
+      <c r="S62" s="7"/>
+      <c r="T62" s="7"/>
+      <c r="U62" s="7"/>
+      <c r="V62" s="7"/>
+      <c r="W62" s="7"/>
+      <c r="X62" s="7"/>
+    </row>
+    <row r="63" spans="1:24" ht="14.4">
       <c r="A63" s="17" t="s">
         <v>24</v>
       </c>
       <c r="B63" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="C63" s="3" t="s">
-        <v>25</v>
-      </c>
       <c r="E63" s="7" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
       <c r="F63" s="7">
-        <v>1</v>
-      </c>
-      <c r="G63" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="H63" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="I63" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="J63" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="K63" s="3" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="64" spans="1:26" ht="14.4">
-      <c r="A64" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="B64" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="E64" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="F64" s="7">
-        <v>553659</v>
-      </c>
+        <v>-1</v>
+      </c>
+      <c r="G63" s="7"/>
+      <c r="H63" s="7"/>
+    </row>
+    <row r="64" spans="1:24" s="23" customFormat="1" ht="14.4">
+      <c r="A64" s="22"/>
+      <c r="B64" s="22"/>
+      <c r="E64" s="7"/>
+      <c r="F64" s="7"/>
       <c r="G64" s="7"/>
       <c r="H64" s="7"/>
     </row>
-    <row r="65" spans="1:12" ht="14.4">
-      <c r="A65" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="B65" s="17" t="s">
-        <v>25</v>
+    <row r="65" spans="1:26" ht="14.4">
+      <c r="A65" s="17"/>
+      <c r="B65" s="17"/>
+      <c r="C65" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="D65" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="E65" s="7" t="s">
-        <v>134</v>
+        <v>120</v>
       </c>
       <c r="F65" s="7">
-        <v>4891208</v>
-      </c>
-      <c r="G65" s="7"/>
-      <c r="H65" s="7"/>
-    </row>
-    <row r="66" spans="1:12" ht="14.4">
+        <v>0.6</v>
+      </c>
+      <c r="G65" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="H65" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="I65" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="J65" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="K65" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="L65" s="7"/>
+      <c r="M65" s="7"/>
+      <c r="N65" s="7"/>
+      <c r="O65" s="7"/>
+      <c r="P65" s="7"/>
+      <c r="Q65" s="7"/>
+      <c r="R65" s="7"/>
+      <c r="S65" s="7"/>
+      <c r="T65" s="7"/>
+      <c r="U65" s="7"/>
+      <c r="V65" s="7"/>
+      <c r="W65" s="7"/>
+      <c r="X65" s="7"/>
+      <c r="Y65" s="7"/>
+      <c r="Z65" s="7"/>
+    </row>
+    <row r="66" spans="1:26" ht="14.4">
       <c r="A66" s="17" t="s">
         <v>24</v>
       </c>
       <c r="B66" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="C66" s="3" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="E66" s="7" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="F66" s="7">
-        <v>1</v>
-      </c>
-      <c r="G66" s="7" t="s">
-        <v>52</v>
-      </c>
+        <v>1739.927555</v>
+      </c>
+      <c r="G66" s="7"/>
       <c r="H66" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="I66" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="K66" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="67" spans="1:26" s="23" customFormat="1" ht="14.4">
+      <c r="A67" s="22"/>
+      <c r="B67" s="22"/>
+      <c r="E67" s="7" t="s">
+        <v>870</v>
+      </c>
+      <c r="F67" s="7"/>
+      <c r="G67" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="H67" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="I67" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="J66" s="3" t="s">
+      <c r="J67" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="K66" s="3" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="67" spans="1:12" ht="14.4">
-      <c r="A67" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="B67" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="C67" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E67" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="F67" s="7">
-        <v>0</v>
-      </c>
-      <c r="G67" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="H67" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="I67" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="J67" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="K67" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="68" spans="1:12" s="23" customFormat="1" ht="14.4">
-      <c r="A68" s="22" t="s">
-        <v>852</v>
-      </c>
-      <c r="B68" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="C68" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="D68" s="23" t="s">
-        <v>75</v>
-      </c>
+      <c r="K67" s="23" t="s">
+        <v>872</v>
+      </c>
+      <c r="L67" s="3" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="68" spans="1:26" s="23" customFormat="1" ht="14.4">
+      <c r="A68" s="22"/>
+      <c r="B68" s="22"/>
       <c r="E68" s="7" t="s">
-        <v>851</v>
-      </c>
-      <c r="F68" s="7">
-        <v>5</v>
-      </c>
+        <v>936</v>
+      </c>
+      <c r="F68" s="7"/>
       <c r="G68" s="7" t="s">
-        <v>124</v>
+        <v>31</v>
       </c>
       <c r="H68" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="I68" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="J68" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="K68" s="3" t="s">
-        <v>853</v>
-      </c>
-      <c r="L68" s="25" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="69" spans="1:12" ht="14.4">
+      <c r="I68" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="J68" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="K68" s="23" t="s">
+        <v>921</v>
+      </c>
+      <c r="L68" s="3" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="69" spans="1:26" ht="14.4">
       <c r="A69" s="17" t="s">
         <v>24</v>
       </c>
       <c r="B69" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="D69" s="3" t="s">
-        <v>142</v>
+      <c r="C69" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="E69" s="7" t="s">
-        <v>143</v>
+        <v>130</v>
       </c>
       <c r="F69" s="7">
-        <v>0</v>
-      </c>
-      <c r="G69" s="7"/>
+        <v>1</v>
+      </c>
+      <c r="G69" s="7" t="s">
+        <v>52</v>
+      </c>
       <c r="H69" s="7" t="s">
-        <v>144</v>
+        <v>131</v>
       </c>
       <c r="I69" s="3" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="J69" s="3" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="K69" s="3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="70" spans="1:12" ht="14.4">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="70" spans="1:26" ht="14.4">
       <c r="A70" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="B70" s="17"/>
+      <c r="B70" s="17" t="s">
+        <v>25</v>
+      </c>
       <c r="E70" s="7" t="s">
-        <v>146</v>
+        <v>133</v>
       </c>
       <c r="F70" s="7">
-        <v>6772</v>
+        <v>553659</v>
       </c>
       <c r="G70" s="7"/>
       <c r="H70" s="7"/>
     </row>
-    <row r="71" spans="1:12" s="23" customFormat="1" ht="14.4">
-      <c r="A71" s="22"/>
-      <c r="B71" s="22"/>
+    <row r="71" spans="1:26" ht="14.4">
+      <c r="A71" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B71" s="17" t="s">
+        <v>25</v>
+      </c>
       <c r="E71" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="F71" s="7">
+        <v>4891208</v>
+      </c>
+      <c r="G71" s="7"/>
+      <c r="H71" s="7"/>
+    </row>
+    <row r="72" spans="1:26" ht="14.4">
+      <c r="A72" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B72" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="C72" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E72" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="F72" s="7">
+        <v>1</v>
+      </c>
+      <c r="G72" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="H72" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="I72" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="J72" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="K72" s="3" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="73" spans="1:26" ht="14.4">
+      <c r="A73" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B73" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="C73" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E73" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="F73" s="7">
+        <v>0</v>
+      </c>
+      <c r="G73" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="H73" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="I73" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="J73" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="K73" s="3" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="74" spans="1:26" s="23" customFormat="1" ht="14.4">
+      <c r="A74" s="22" t="s">
+        <v>852</v>
+      </c>
+      <c r="B74" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="C74" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="D74" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="E74" s="7" t="s">
+        <v>851</v>
+      </c>
+      <c r="F74" s="7">
+        <v>5</v>
+      </c>
+      <c r="G74" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="H74" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="I74" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="J74" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="K74" s="3" t="s">
+        <v>853</v>
+      </c>
+      <c r="L74" s="25" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="75" spans="1:26" ht="14.4">
+      <c r="A75" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B75" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="D75" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="E75" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="F75" s="7">
+        <v>0</v>
+      </c>
+      <c r="G75" s="7"/>
+      <c r="H75" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="I75" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="J75" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="K75" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="76" spans="1:26" ht="14.4">
+      <c r="A76" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B76" s="17"/>
+      <c r="E76" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="F76" s="7">
+        <v>6772</v>
+      </c>
+      <c r="G76" s="7"/>
+      <c r="H76" s="7"/>
+    </row>
+    <row r="77" spans="1:26" s="23" customFormat="1" ht="14.4">
+      <c r="A77" s="22"/>
+      <c r="B77" s="22"/>
+      <c r="E77" s="7" t="s">
         <v>858</v>
       </c>
-      <c r="F71" s="7">
+      <c r="F77" s="7">
         <v>1</v>
       </c>
-      <c r="G71" s="7" t="s">
+      <c r="G77" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="H71" s="7" t="s">
+      <c r="H77" s="7" t="s">
         <v>859</v>
       </c>
-      <c r="I71" s="25" t="s">
+      <c r="I77" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="J71" s="25" t="s">
+      <c r="J77" s="25" t="s">
         <v>860</v>
       </c>
     </row>
-    <row r="72" spans="1:12" s="23" customFormat="1" ht="14.4">
-      <c r="A72" s="22"/>
-      <c r="B72" s="22"/>
-      <c r="E72" s="7" t="s">
+    <row r="78" spans="1:26" s="23" customFormat="1" ht="14.4">
+      <c r="A78" s="22"/>
+      <c r="B78" s="22"/>
+      <c r="E78" s="7" t="s">
         <v>857</v>
       </c>
-      <c r="F72" s="7">
+      <c r="F78" s="7">
         <v>10</v>
       </c>
-      <c r="G72" s="7" t="s">
+      <c r="G78" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="H72" s="7" t="s">
+      <c r="H78" s="7" t="s">
         <v>641</v>
       </c>
-      <c r="I72" s="25" t="s">
+      <c r="I78" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="J72" s="25" t="s">
+      <c r="J78" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="K72" s="25" t="s">
+      <c r="K78" s="25" t="s">
         <v>863</v>
       </c>
     </row>
-    <row r="73" spans="1:12" s="23" customFormat="1" ht="14.4">
-      <c r="A73" s="22"/>
-      <c r="B73" s="22"/>
-      <c r="D73" s="59" t="s">
+    <row r="79" spans="1:26" s="23" customFormat="1" ht="14.4">
+      <c r="A79" s="22"/>
+      <c r="B79" s="22"/>
+      <c r="D79" s="59" t="s">
         <v>26</v>
       </c>
-      <c r="E73" s="7" t="s">
+      <c r="E79" s="7" t="s">
         <v>811</v>
       </c>
-      <c r="F73" s="7"/>
-      <c r="G73" s="60" t="s">
+      <c r="F79" s="7"/>
+      <c r="G79" s="60" t="s">
         <v>31</v>
       </c>
-      <c r="H73" s="7" t="s">
+      <c r="H79" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="I73" s="25" t="s">
+      <c r="I79" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="J73" s="25" t="s">
+      <c r="J79" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="K73" s="25" t="s">
+      <c r="K79" s="25" t="s">
         <v>812</v>
       </c>
     </row>
-    <row r="74" spans="1:12" s="23" customFormat="1" ht="14.4">
-      <c r="A74" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="B74" s="22"/>
-      <c r="D74" s="59" t="s">
+    <row r="80" spans="1:26" s="23" customFormat="1" ht="14.4">
+      <c r="A80" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="B80" s="22"/>
+      <c r="D80" s="59" t="s">
         <v>26</v>
       </c>
-      <c r="E74" s="7" t="s">
+      <c r="E80" s="7" t="s">
         <v>813</v>
       </c>
-      <c r="F74" s="7"/>
-      <c r="G74" s="60" t="s">
+      <c r="F80" s="7"/>
+      <c r="G80" s="60" t="s">
         <v>31</v>
       </c>
-      <c r="H74" s="7" t="s">
+      <c r="H80" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="I74" s="25" t="s">
+      <c r="I80" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="J74" s="25" t="s">
+      <c r="J80" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="K74" s="25" t="s">
+      <c r="K80" s="25" t="s">
         <v>814</v>
       </c>
     </row>
-    <row r="75" spans="1:12" ht="14.4">
-      <c r="A75" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="B75" s="18" t="s">
+    <row r="81" spans="1:11" ht="14.4">
+      <c r="A81" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B81" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="D75" s="19" t="s">
+      <c r="D81" s="19" t="s">
         <v>148</v>
       </c>
-      <c r="E75" s="20" t="s">
+      <c r="E81" s="20" t="s">
         <v>150</v>
       </c>
-      <c r="F75" s="20">
+      <c r="F81" s="20">
         <v>1500</v>
       </c>
-      <c r="G75" s="20" t="s">
+      <c r="G81" s="20" t="s">
         <v>124</v>
       </c>
-      <c r="H75" s="20" t="s">
+      <c r="H81" s="20" t="s">
         <v>94</v>
       </c>
-      <c r="I75" s="19" t="s">
+      <c r="I81" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="J75" s="19" t="s">
+      <c r="J81" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="K75" s="19" t="s">
+      <c r="K81" s="19" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="76" spans="1:12" ht="14.4">
-      <c r="A76" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="B76" s="18" t="s">
+    <row r="82" spans="1:11" ht="14.4">
+      <c r="A82" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B82" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="D76" s="19" t="s">
+      <c r="D82" s="19" t="s">
         <v>148</v>
       </c>
-      <c r="E76" s="19" t="s">
+      <c r="E82" s="19" t="s">
         <v>155</v>
       </c>
-      <c r="F76" s="19">
+      <c r="F82" s="19">
         <v>1500</v>
       </c>
-      <c r="G76" s="20" t="s">
+      <c r="G82" s="20" t="s">
         <v>124</v>
       </c>
-      <c r="H76" s="19" t="s">
+      <c r="H82" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="I76" s="19" t="s">
+      <c r="I82" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="J76" s="19" t="s">
+      <c r="J82" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="K76" s="19" t="s">
+      <c r="K82" s="19" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="77" spans="1:12" ht="14.4">
-      <c r="A77" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="B77" s="18" t="s">
+    <row r="83" spans="1:11" ht="14.4">
+      <c r="A83" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B83" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="D77" s="19" t="s">
+      <c r="D83" s="19" t="s">
         <v>148</v>
       </c>
-      <c r="E77" s="19" t="s">
+      <c r="E83" s="19" t="s">
         <v>158</v>
       </c>
-      <c r="F77" s="19">
+      <c r="F83" s="19">
         <v>1500</v>
       </c>
-      <c r="G77" s="20" t="s">
+      <c r="G83" s="20" t="s">
         <v>124</v>
       </c>
-      <c r="H77" s="19" t="s">
+      <c r="H83" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="I77" s="19" t="s">
+      <c r="I83" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="J77" s="19" t="s">
+      <c r="J83" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="K77" s="19" t="s">
+      <c r="K83" s="19" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="78" spans="1:12" ht="14.4">
-      <c r="A78" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="B78" s="18" t="s">
+    <row r="84" spans="1:11" ht="14.4">
+      <c r="A84" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B84" s="18" t="s">
         <v>160</v>
       </c>
-      <c r="D78" s="19" t="s">
+      <c r="D84" s="19" t="s">
         <v>148</v>
       </c>
-      <c r="E78" s="19" t="s">
+      <c r="E84" s="19" t="s">
         <v>161</v>
       </c>
-      <c r="F78" s="19">
+      <c r="F84" s="19">
         <v>1000</v>
       </c>
-      <c r="G78" s="20" t="s">
+      <c r="G84" s="20" t="s">
         <v>124</v>
       </c>
-      <c r="H78" s="19" t="s">
+      <c r="H84" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="I78" s="19" t="s">
+      <c r="I84" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="J78" s="19" t="s">
+      <c r="J84" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="K78" s="19" t="s">
+      <c r="K84" s="19" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="79" spans="1:12" ht="14.4">
-      <c r="A79" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="B79" s="18" t="s">
+    <row r="85" spans="1:11" ht="14.4">
+      <c r="A85" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B85" s="18" t="s">
         <v>160</v>
       </c>
-      <c r="D79" s="19" t="s">
+      <c r="D85" s="19" t="s">
         <v>148</v>
       </c>
-      <c r="E79" s="19" t="s">
+      <c r="E85" s="19" t="s">
         <v>163</v>
       </c>
-      <c r="F79" s="19">
+      <c r="F85" s="19">
         <v>1000</v>
       </c>
-      <c r="G79" s="20" t="s">
+      <c r="G85" s="20" t="s">
         <v>124</v>
       </c>
-      <c r="H79" s="19" t="s">
+      <c r="H85" s="19" t="s">
         <v>121</v>
       </c>
-      <c r="I79" s="19" t="s">
+      <c r="I85" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="J79" s="19" t="s">
+      <c r="J85" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="K79" s="19" t="s">
+      <c r="K85" s="19" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="80" spans="1:12" ht="14.4">
-      <c r="A80" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="B80" s="18" t="s">
+    <row r="86" spans="1:11" ht="14.4">
+      <c r="A86" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B86" s="18" t="s">
         <v>160</v>
       </c>
-      <c r="D80" s="19" t="s">
+      <c r="D86" s="19" t="s">
         <v>148</v>
       </c>
-      <c r="E80" s="19" t="s">
+      <c r="E86" s="19" t="s">
         <v>165</v>
       </c>
-      <c r="F80" s="19">
+      <c r="F86" s="19">
         <v>1000</v>
       </c>
-      <c r="G80" s="20" t="s">
+      <c r="G86" s="20" t="s">
         <v>124</v>
       </c>
-      <c r="H80" s="19" t="s">
+      <c r="H86" s="19" t="s">
         <v>121</v>
       </c>
-      <c r="I80" s="19" t="s">
+      <c r="I86" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="J80" s="19" t="s">
+      <c r="J86" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="K80" s="19" t="s">
+      <c r="K86" s="19" t="s">
         <v>166</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B55">
+  <conditionalFormatting sqref="B56:B58">
     <cfRule type="notContainsBlanks" dxfId="0" priority="1">
-      <formula>LEN(TRIM(B55))&gt;0</formula>
+      <formula>LEN(TRIM(B56))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
HBV.csv - Change W2A_SLP and W2A_INT for CGR to improve the temperature calibration. Further reduce ET_MULT for Mohawk.
</commit_message>
<xml_diff>
--- a/DataCW3M/CW3MdigitalHandbook/CW3MdataDictionary.xlsx
+++ b/DataCW3M/CW3MdigitalHandbook/CW3MdataDictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\CW3MdigitalHandbook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC9706D9-25A4-49D1-8C58-4C901B2D46E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2548E4B-8C32-4EED-8590-031825A60714}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-7425" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Necessary input data" sheetId="7" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="Conventions" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>

</xml_diff>

<commit_message>
CW3MdataDictionary.xlsx, Reach_McKenzie.dbf - Add Reach attributes ADDEDVOL_C and OUTIRRIG_C. Flow_McKenzie.xml - Refine the "FLOW McKenzie Thermal Energy Budget for streams" reports. Flow.cpp, .h - Add Reach attributes ADDEDVOL_C and OUTIRRIG_C. ReachRouting.cpp - In ReachRouting::Step() and in ApplyReachOutflowWP() add logic for tracking the temperature of added water. WaterRights.cpp, .h - Add Reach attribute OUTIRRIG_C. In AllocateSurfaceWR(), add logic to track the thermal energy in irrigation withdrawals.
</commit_message>
<xml_diff>
--- a/DataCW3M/CW3MdigitalHandbook/CW3MdataDictionary.xlsx
+++ b/DataCW3M/CW3MdigitalHandbook/CW3MdataDictionary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\CW3MdigitalHandbook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C44E9B8F-D9CD-46F6-94B6-EAF871F96510}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E8FFFD8-F074-45BA-A229-807BDBDE7C18}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-7425" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -96,7 +96,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2868" uniqueCount="936">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2883" uniqueCount="940">
   <si>
     <t>LULC_A</t>
   </si>
@@ -2898,13 +2898,25 @@
     <t>ADDED_VOL</t>
   </si>
   <si>
-    <t>1/1/21 Added ADDED_Q and ADDEDVOL. Removed AVEGAGECFS, HUC_4, HUC_5, HUC6, NODE_ID, and SUB_AREA_C as obsolete.</t>
-  </si>
-  <si>
     <t>updated daily: amount added so far this year by the model to the volume of water in the reach by to avoid math problems (e.g. to prevent reaches from going dry)</t>
   </si>
   <si>
     <t>updated daily: the amount added so far this year to the reach discharge by the model to ensure that the discharge is &gt;= NOMINAL_LOW_FLOW_CMS</t>
+  </si>
+  <si>
+    <t>ADDEDVOL_C</t>
+  </si>
+  <si>
+    <t>temperature of ADDED_VOL</t>
+  </si>
+  <si>
+    <t>OUTIRRIG_C</t>
+  </si>
+  <si>
+    <t>temperature of daily withdrawal from reach for irrigation</t>
+  </si>
+  <si>
+    <t>1/5/21, 1/5 Added ADDED_Q,  ADDED_VOL, ADDEDVOL_C, and OUTIRRIG_C. Removed AVEGAGECFS, HUC_4, HUC_5, HUC6, NODE_ID, and SUB_AREA_C as obsolete.</t>
   </si>
 </sst>
 </file>
@@ -20581,11 +20593,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Z84"/>
+  <dimension ref="A1:Z86"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K5" sqref="K5"/>
+      <pane ySplit="3" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -20632,7 +20644,7 @@
     </row>
     <row r="2" spans="1:26" s="95" customFormat="1" ht="12.75" customHeight="1">
       <c r="A2" s="91" t="s">
-        <v>933</v>
+        <v>939</v>
       </c>
       <c r="B2" s="92"/>
       <c r="C2" s="93"/>
@@ -20736,7 +20748,7 @@
         <v>27</v>
       </c>
       <c r="K4" s="57" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="L4" s="9"/>
       <c r="M4" s="25"/>
@@ -20774,7 +20786,7 @@
         <v>27</v>
       </c>
       <c r="K5" s="57" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="L5" s="9"/>
       <c r="M5" s="25"/>
@@ -20790,59 +20802,76 @@
       <c r="W5" s="25"/>
       <c r="X5" s="25"/>
     </row>
-    <row r="6" spans="1:26" s="87" customFormat="1" ht="14.4">
-      <c r="A6" s="86"/>
-      <c r="B6" s="86"/>
-      <c r="D6" s="88" t="s">
+    <row r="6" spans="1:26" s="21" customFormat="1" ht="14.4">
+      <c r="A6" s="13"/>
+      <c r="B6" s="13"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="76" t="s">
+        <v>935</v>
+      </c>
+      <c r="F6" s="10"/>
+      <c r="G6" s="74" t="s">
+        <v>112</v>
+      </c>
+      <c r="H6" s="74" t="s">
+        <v>132</v>
+      </c>
+      <c r="I6" s="83" t="s">
+        <v>26</v>
+      </c>
+      <c r="J6" s="83" t="s">
+        <v>27</v>
+      </c>
+      <c r="K6" s="74" t="s">
+        <v>936</v>
+      </c>
+      <c r="L6" s="9"/>
+      <c r="M6" s="25"/>
+      <c r="N6" s="7"/>
+      <c r="O6" s="25"/>
+      <c r="P6" s="25"/>
+      <c r="Q6" s="25"/>
+      <c r="R6" s="25"/>
+      <c r="S6" s="25"/>
+      <c r="T6" s="25"/>
+      <c r="U6" s="25"/>
+      <c r="V6" s="25"/>
+      <c r="W6" s="25"/>
+      <c r="X6" s="25"/>
+    </row>
+    <row r="7" spans="1:26" s="87" customFormat="1" ht="14.4">
+      <c r="A7" s="86"/>
+      <c r="B7" s="86"/>
+      <c r="D7" s="88" t="s">
         <v>902</v>
       </c>
-      <c r="E6" s="88" t="s">
+      <c r="E7" s="88" t="s">
         <v>853</v>
       </c>
-      <c r="F6" s="88">
+      <c r="F7" s="88">
         <v>5.2</v>
       </c>
-      <c r="G6" s="88"/>
-      <c r="H6" s="88" t="s">
+      <c r="G7" s="88"/>
+      <c r="H7" s="88" t="s">
         <v>112</v>
       </c>
-      <c r="I6" s="88" t="s">
+      <c r="I7" s="88" t="s">
         <v>26</v>
       </c>
-      <c r="J6" s="88" t="s">
+      <c r="J7" s="88" t="s">
         <v>27</v>
       </c>
-      <c r="K6" s="87" t="s">
+      <c r="K7" s="87" t="s">
         <v>852</v>
       </c>
-    </row>
-    <row r="7" spans="1:26" s="21" customFormat="1" ht="28.8">
-      <c r="A7" s="20"/>
-      <c r="B7" s="20"/>
-      <c r="C7" s="22"/>
-      <c r="E7" s="21" t="s">
-        <v>900</v>
-      </c>
-      <c r="G7" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="H7" s="21" t="s">
-        <v>903</v>
-      </c>
-      <c r="J7" s="23" t="s">
-        <v>30</v>
-      </c>
-      <c r="K7" s="84" t="s">
-        <v>904</v>
-      </c>
-      <c r="L7" s="22"/>
     </row>
     <row r="8" spans="1:26" s="21" customFormat="1" ht="28.8">
       <c r="A8" s="20"/>
       <c r="B8" s="20"/>
       <c r="C8" s="22"/>
       <c r="E8" s="21" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="G8" s="21" t="s">
         <v>47</v>
@@ -20854,25 +20883,30 @@
         <v>30</v>
       </c>
       <c r="K8" s="84" t="s">
+        <v>904</v>
+      </c>
+      <c r="L8" s="22"/>
+    </row>
+    <row r="9" spans="1:26" s="21" customFormat="1" ht="28.8">
+      <c r="A9" s="20"/>
+      <c r="B9" s="20"/>
+      <c r="C9" s="22"/>
+      <c r="E9" s="21" t="s">
+        <v>901</v>
+      </c>
+      <c r="G9" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="H9" s="21" t="s">
+        <v>903</v>
+      </c>
+      <c r="J9" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="K9" s="84" t="s">
         <v>905</v>
       </c>
-      <c r="L8" s="22"/>
-    </row>
-    <row r="9" spans="1:26" ht="14.4">
-      <c r="A9" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="F9" s="7">
-        <v>3220</v>
-      </c>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
+      <c r="L9" s="22"/>
     </row>
     <row r="10" spans="1:26" ht="14.4">
       <c r="A10" s="15" t="s">
@@ -20881,28 +20915,14 @@
       <c r="B10" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>24</v>
-      </c>
       <c r="E10" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F10" s="7">
-        <v>23773405</v>
+        <v>3220</v>
       </c>
       <c r="G10" s="7"/>
-      <c r="H10" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="I10" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="J10" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="K10" s="7" t="s">
-        <v>35</v>
-      </c>
+      <c r="H10" s="7"/>
     </row>
     <row r="11" spans="1:26" ht="14.4">
       <c r="A11" s="15" t="s">
@@ -20911,14 +20931,28 @@
       <c r="B11" s="15" t="s">
         <v>24</v>
       </c>
+      <c r="C11" s="3" t="s">
+        <v>24</v>
+      </c>
       <c r="E11" s="7" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="F11" s="7">
-        <v>23773403</v>
+        <v>23773405</v>
       </c>
       <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
+      <c r="H11" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="I11" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="J11" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="K11" s="7" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="12" spans="1:26" ht="14.4">
       <c r="A12" s="15" t="s">
@@ -20928,10 +20962,10 @@
         <v>24</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F12" s="7">
-        <v>23773407</v>
+        <v>23773403</v>
       </c>
       <c r="G12" s="7"/>
       <c r="H12" s="7"/>
@@ -20944,10 +20978,10 @@
         <v>24</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F13" s="7">
-        <v>0</v>
+        <v>23773407</v>
       </c>
       <c r="G13" s="7"/>
       <c r="H13" s="7"/>
@@ -20959,11 +20993,8 @@
       <c r="B14" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="D14" s="3" t="s">
-        <v>39</v>
-      </c>
       <c r="E14" s="7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F14" s="7">
         <v>0</v>
@@ -20982,7 +21013,7 @@
         <v>39</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F15" s="7">
         <v>0</v>
@@ -20998,10 +21029,10 @@
         <v>24</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F16" s="7">
         <v>0</v>
@@ -21009,121 +21040,108 @@
       <c r="G16" s="7"/>
       <c r="H16" s="7"/>
     </row>
-    <row r="17" spans="1:26" s="21" customFormat="1" ht="14.4">
-      <c r="A17" s="20"/>
-      <c r="B17" s="20"/>
-      <c r="D17" s="3"/>
+    <row r="17" spans="1:26" ht="14.4">
+      <c r="A17" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>42</v>
+      </c>
       <c r="E17" s="7" t="s">
-        <v>849</v>
+        <v>43</v>
       </c>
       <c r="F17" s="7">
-        <v>1</v>
-      </c>
-      <c r="G17" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="H17" s="7" t="s">
-        <v>629</v>
-      </c>
-      <c r="I17" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="J17" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="K17" s="21" t="s">
-        <v>850</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
     </row>
     <row r="18" spans="1:26" s="21" customFormat="1" ht="14.4">
       <c r="A18" s="20"/>
       <c r="B18" s="20"/>
       <c r="D18" s="3"/>
       <c r="E18" s="7" t="s">
-        <v>906</v>
+        <v>849</v>
       </c>
       <c r="F18" s="7">
-        <v>90</v>
+        <v>1</v>
       </c>
       <c r="G18" s="7" t="s">
         <v>112</v>
       </c>
       <c r="H18" s="7" t="s">
+        <v>629</v>
+      </c>
+      <c r="I18" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="J18" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="K18" s="21" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="19" spans="1:26" s="21" customFormat="1" ht="14.4">
+      <c r="A19" s="20"/>
+      <c r="B19" s="20"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="7" t="s">
+        <v>906</v>
+      </c>
+      <c r="F19" s="7">
+        <v>90</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="H19" s="7" t="s">
         <v>907</v>
       </c>
-      <c r="J18" s="21" t="s">
+      <c r="J19" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="K18" s="21" t="s">
+      <c r="K19" s="21" t="s">
         <v>908</v>
       </c>
-    </row>
-    <row r="19" spans="1:26" ht="14.4">
-      <c r="A19" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B19" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E19" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="F19" s="7">
-        <v>6772</v>
-      </c>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
     </row>
     <row r="20" spans="1:26" ht="14.4">
       <c r="A20" s="15" t="s">
         <v>23</v>
       </c>
       <c r="B20" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="C20" s="3" t="s">
         <v>24</v>
       </c>
+      <c r="D20" s="3" t="s">
+        <v>44</v>
+      </c>
       <c r="E20" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F20" s="7">
-        <v>0</v>
-      </c>
-      <c r="G20" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="H20" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="J20" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="K20" s="3" t="s">
-        <v>48</v>
-      </c>
+        <v>6772</v>
+      </c>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
     </row>
     <row r="21" spans="1:26" ht="14.4">
       <c r="A21" s="15" t="s">
         <v>23</v>
       </c>
       <c r="B21" s="15" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D21" s="3" t="s">
-        <v>39</v>
-      </c>
       <c r="E21" s="7" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F21" s="7">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="G21" s="7" t="s">
         <v>47</v>
@@ -21131,84 +21149,102 @@
       <c r="H21" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="I21" s="3" t="s">
-        <v>34</v>
-      </c>
       <c r="J21" s="3" t="s">
         <v>30</v>
       </c>
       <c r="K21" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="22" spans="1:26" ht="14.4">
+      <c r="A22" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="F22" s="7">
+        <v>7</v>
+      </c>
+      <c r="G22" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="H22" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="I22" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="J22" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="K22" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="N21" s="3" t="s">
+      <c r="N22" s="3" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="22" spans="1:26" s="21" customFormat="1" ht="14.4">
-      <c r="A22" s="20"/>
-      <c r="B22" s="20"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="7" t="s">
+    <row r="23" spans="1:26" s="21" customFormat="1" ht="14.4">
+      <c r="A23" s="20"/>
+      <c r="B23" s="20"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="7" t="s">
         <v>856</v>
       </c>
-      <c r="F22" s="7">
+      <c r="F23" s="7">
         <v>4.2</v>
       </c>
-      <c r="G22" s="7" t="s">
+      <c r="G23" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="H22" s="7" t="s">
+      <c r="H23" s="7" t="s">
         <v>410</v>
       </c>
-      <c r="I22" s="3" t="s">
+      <c r="I23" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="J22" s="3" t="s">
+      <c r="J23" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="K22" s="3" t="s">
+      <c r="K23" s="3" t="s">
         <v>855</v>
       </c>
-      <c r="N22" s="3"/>
-    </row>
-    <row r="23" spans="1:26" ht="14.4">
-      <c r="A23" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B23" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="D23" t="s">
-        <v>914</v>
-      </c>
-      <c r="E23" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="F23" s="7">
-        <v>0</v>
-      </c>
-      <c r="G23" s="7" t="s">
-        <v>912</v>
-      </c>
-      <c r="H23" s="7"/>
-      <c r="K23" s="23" t="s">
-        <v>913</v>
-      </c>
+      <c r="N23" s="3"/>
     </row>
     <row r="24" spans="1:26" ht="14.4">
       <c r="A24" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="B24" s="15"/>
+      <c r="B24" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D24" t="s">
+        <v>914</v>
+      </c>
       <c r="E24" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F24" s="7">
-        <v>6713</v>
-      </c>
-      <c r="G24" s="7"/>
+        <v>0</v>
+      </c>
+      <c r="G24" s="7" t="s">
+        <v>912</v>
+      </c>
       <c r="H24" s="7"/>
+      <c r="K24" s="23" t="s">
+        <v>913</v>
+      </c>
     </row>
     <row r="25" spans="1:26" ht="14.4">
       <c r="A25" s="15" t="s">
@@ -21216,9 +21252,11 @@
       </c>
       <c r="B25" s="15"/>
       <c r="E25" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="F25" s="7"/>
+        <v>53</v>
+      </c>
+      <c r="F25" s="7">
+        <v>6713</v>
+      </c>
       <c r="G25" s="7"/>
       <c r="H25" s="7"/>
     </row>
@@ -21227,174 +21265,162 @@
         <v>23</v>
       </c>
       <c r="B26" s="15"/>
-      <c r="E26" s="58" t="s">
-        <v>55</v>
-      </c>
-      <c r="F26" s="7" t="s">
-        <v>56</v>
-      </c>
+      <c r="E26" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="F26" s="7"/>
       <c r="G26" s="7"/>
       <c r="H26" s="7"/>
     </row>
-    <row r="27" spans="1:26" ht="25.2" customHeight="1">
+    <row r="27" spans="1:26" ht="14.4">
       <c r="A27" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="B27" s="15" t="s">
+      <c r="B27" s="15"/>
+      <c r="E27" s="58" t="s">
+        <v>55</v>
+      </c>
+      <c r="F27" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G27" s="7"/>
+      <c r="H27" s="7"/>
+    </row>
+    <row r="28" spans="1:26" ht="25.2" customHeight="1">
+      <c r="A28" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B28" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="C28" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="E27" s="7" t="s">
+      <c r="E28" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="F27" s="7">
+      <c r="F28" s="7">
         <v>34</v>
       </c>
-      <c r="G27" s="7" t="s">
+      <c r="G28" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="H27" s="7" t="s">
+      <c r="H28" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="K27" s="3" t="s">
+      <c r="K28" s="3" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="28" spans="1:26" s="25" customFormat="1" ht="72">
-      <c r="A28" s="85"/>
-      <c r="B28" s="85"/>
-      <c r="C28" s="19"/>
-      <c r="D28" s="19" t="s">
+    <row r="29" spans="1:26" s="25" customFormat="1" ht="72">
+      <c r="A29" s="85"/>
+      <c r="B29" s="85"/>
+      <c r="C29" s="19"/>
+      <c r="D29" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="E28" s="25" t="s">
+      <c r="E29" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="F28" s="89">
+      <c r="F29" s="89">
         <v>6737</v>
       </c>
-      <c r="G28" s="25" t="s">
+      <c r="G29" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="H28" s="90" t="s">
+      <c r="H29" s="90" t="s">
         <v>33</v>
       </c>
-      <c r="I28" s="19"/>
-      <c r="J28" s="19" t="s">
+      <c r="I29" s="19"/>
+      <c r="J29" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="K28" s="84" t="s">
+      <c r="K29" s="84" t="s">
         <v>838</v>
       </c>
-      <c r="L28" s="19"/>
-      <c r="M28" s="19"/>
-      <c r="N28" s="19"/>
-      <c r="O28" s="19"/>
-      <c r="P28" s="19"/>
-      <c r="Q28" s="19"/>
-      <c r="R28" s="19"/>
-      <c r="S28" s="19"/>
-      <c r="T28" s="19"/>
-      <c r="U28" s="19"/>
-      <c r="V28" s="19"/>
-      <c r="W28" s="19"/>
-      <c r="X28" s="19"/>
-      <c r="Y28" s="19"/>
-      <c r="Z28" s="19"/>
-    </row>
-    <row r="29" spans="1:26" ht="14.4">
-      <c r="A29" s="15"/>
-      <c r="B29" s="15"/>
-      <c r="D29" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="E29" s="18" t="s">
-        <v>64</v>
-      </c>
-      <c r="F29" s="18">
-        <v>1</v>
-      </c>
-      <c r="G29" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="H29" s="18" t="s">
-        <v>65</v>
-      </c>
-      <c r="J29" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="K29" s="17" t="s">
-        <v>66</v>
-      </c>
+      <c r="L29" s="19"/>
+      <c r="M29" s="19"/>
+      <c r="N29" s="19"/>
+      <c r="O29" s="19"/>
+      <c r="P29" s="19"/>
+      <c r="Q29" s="19"/>
+      <c r="R29" s="19"/>
+      <c r="S29" s="19"/>
+      <c r="T29" s="19"/>
+      <c r="U29" s="19"/>
+      <c r="V29" s="19"/>
+      <c r="W29" s="19"/>
+      <c r="X29" s="19"/>
+      <c r="Y29" s="19"/>
+      <c r="Z29" s="19"/>
     </row>
     <row r="30" spans="1:26" ht="14.4">
       <c r="A30" s="15"/>
-      <c r="B30" s="16" t="s">
-        <v>24</v>
-      </c>
+      <c r="B30" s="15"/>
       <c r="D30" s="17" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="E30" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="F30" s="7"/>
+        <v>64</v>
+      </c>
+      <c r="F30" s="18">
+        <v>1</v>
+      </c>
       <c r="G30" s="18" t="s">
         <v>29</v>
       </c>
       <c r="H30" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="J30" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="K30" s="17" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="31" spans="1:26" ht="14.4">
+      <c r="A31" s="15"/>
+      <c r="B31" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="D31" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="E31" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="F31" s="7"/>
+      <c r="G31" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="H31" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="I30" s="17" t="s">
+      <c r="I31" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="J30" s="17" t="s">
+      <c r="J31" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="K30" s="23" t="s">
+      <c r="K31" s="23" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="31" spans="1:26" s="21" customFormat="1" ht="14.4">
-      <c r="A31" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="B31" s="20" t="s">
+    <row r="32" spans="1:26" s="21" customFormat="1" ht="14.4">
+      <c r="A32" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="B32" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="D31" s="22"/>
-      <c r="E31" s="21" t="s">
-        <v>810</v>
-      </c>
-      <c r="F31" s="7"/>
-      <c r="G31" s="57" t="s">
-        <v>29</v>
-      </c>
-      <c r="H31" s="57" t="s">
-        <v>75</v>
-      </c>
-      <c r="I31" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="J31" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="K31" s="23" t="s">
-        <v>811</v>
-      </c>
-    </row>
-    <row r="32" spans="1:26" s="21" customFormat="1" ht="14.4">
-      <c r="A32" s="20"/>
-      <c r="B32" s="20"/>
       <c r="D32" s="22"/>
       <c r="E32" s="21" t="s">
-        <v>861</v>
+        <v>810</v>
       </c>
       <c r="F32" s="7"/>
       <c r="G32" s="57" t="s">
-        <v>112</v>
+        <v>29</v>
       </c>
       <c r="H32" s="57" t="s">
         <v>75</v>
@@ -21406,7 +21432,7 @@
         <v>27</v>
       </c>
       <c r="K32" s="23" t="s">
-        <v>862</v>
+        <v>811</v>
       </c>
     </row>
     <row r="33" spans="1:11" s="21" customFormat="1" ht="14.4">
@@ -21414,14 +21440,14 @@
       <c r="B33" s="20"/>
       <c r="D33" s="22"/>
       <c r="E33" s="21" t="s">
-        <v>910</v>
+        <v>861</v>
       </c>
       <c r="F33" s="7"/>
       <c r="G33" s="57" t="s">
         <v>112</v>
       </c>
       <c r="H33" s="57" t="s">
-        <v>132</v>
+        <v>75</v>
       </c>
       <c r="I33" s="23" t="s">
         <v>26</v>
@@ -21430,28 +21456,31 @@
         <v>27</v>
       </c>
       <c r="K33" s="23" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" s="21" customFormat="1" ht="14.4">
+      <c r="A34" s="20"/>
+      <c r="B34" s="20"/>
+      <c r="D34" s="22"/>
+      <c r="E34" s="21" t="s">
+        <v>910</v>
+      </c>
+      <c r="F34" s="7"/>
+      <c r="G34" s="57" t="s">
+        <v>112</v>
+      </c>
+      <c r="H34" s="57" t="s">
+        <v>132</v>
+      </c>
+      <c r="I34" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="J34" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="K34" s="23" t="s">
         <v>911</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" ht="14.4">
-      <c r="A34" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B34" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="E34" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="F34" s="7">
-        <v>0</v>
-      </c>
-      <c r="G34" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="H34" s="7"/>
-      <c r="K34" s="3" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="14.4">
@@ -21461,23 +21490,18 @@
       <c r="B35" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="D35" s="3" t="s">
-        <v>39</v>
-      </c>
       <c r="E35" s="7" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F35" s="7">
         <v>0</v>
       </c>
-      <c r="G35" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="H35" s="18" t="s">
-        <v>75</v>
-      </c>
-      <c r="K35" s="17" t="s">
-        <v>76</v>
+      <c r="G35" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="H35" s="7"/>
+      <c r="K35" s="3" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="36" spans="1:11" ht="14.4">
@@ -21487,20 +21511,23 @@
       <c r="B36" s="15" t="s">
         <v>24</v>
       </c>
+      <c r="D36" s="3" t="s">
+        <v>39</v>
+      </c>
       <c r="E36" s="7" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F36" s="7">
         <v>0</v>
       </c>
       <c r="G36" s="18" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="H36" s="18" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="K36" s="17" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="37" spans="1:11" ht="14.4">
@@ -21511,19 +21538,19 @@
         <v>24</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="F37" s="7">
         <v>0</v>
       </c>
       <c r="G37" s="18" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="H37" s="18" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="K37" s="17" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="38" spans="1:11" ht="14.4">
@@ -21534,19 +21561,19 @@
         <v>24</v>
       </c>
       <c r="E38" s="7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F38" s="7">
         <v>0</v>
       </c>
       <c r="G38" s="18" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="H38" s="18" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="K38" s="17" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="39" spans="1:11" ht="14.4">
@@ -21556,27 +21583,20 @@
       <c r="B39" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="C39" s="3" t="s">
-        <v>24</v>
-      </c>
       <c r="E39" s="7" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="F39" s="7">
-        <v>1739.9274680000001</v>
-      </c>
-      <c r="G39" s="7"/>
-      <c r="H39" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="I39" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="J39" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="K39" s="3" t="s">
-        <v>87</v>
+        <v>0</v>
+      </c>
+      <c r="G39" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="H39" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="K39" s="17" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="40" spans="1:11" ht="14.4">
@@ -21586,17 +21606,28 @@
       <c r="B40" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="D40" s="3" t="s">
-        <v>44</v>
+      <c r="C40" s="3" t="s">
+        <v>24</v>
       </c>
       <c r="E40" s="7" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="F40" s="7">
-        <v>6699</v>
+        <v>1739.9274680000001</v>
       </c>
       <c r="G40" s="7"/>
-      <c r="H40" s="7"/>
+      <c r="H40" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="I40" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="J40" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="K40" s="3" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="41" spans="1:11" ht="14.4">
       <c r="A41" s="15" t="s">
@@ -21605,22 +21636,17 @@
       <c r="B41" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="D41" t="s">
-        <v>914</v>
+      <c r="D41" s="3" t="s">
+        <v>44</v>
       </c>
       <c r="E41" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F41" s="7">
-        <v>0</v>
-      </c>
-      <c r="G41" s="7" t="s">
-        <v>915</v>
-      </c>
+        <v>6699</v>
+      </c>
+      <c r="G41" s="7"/>
       <c r="H41" s="7"/>
-      <c r="K41" s="23" t="s">
-        <v>916</v>
-      </c>
     </row>
     <row r="42" spans="1:11" ht="14.4">
       <c r="A42" s="15" t="s">
@@ -21629,17 +21655,22 @@
       <c r="B42" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="D42" s="3" t="s">
-        <v>39</v>
+      <c r="D42" t="s">
+        <v>914</v>
       </c>
       <c r="E42" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F42" s="7">
         <v>0</v>
       </c>
-      <c r="G42" s="7"/>
+      <c r="G42" s="7" t="s">
+        <v>915</v>
+      </c>
       <c r="H42" s="7"/>
+      <c r="K42" s="23" t="s">
+        <v>916</v>
+      </c>
     </row>
     <row r="43" spans="1:11" ht="14.4">
       <c r="A43" s="15" t="s">
@@ -21649,46 +21680,35 @@
         <v>24</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="E43" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F43" s="7">
-        <v>6758</v>
+        <v>0</v>
       </c>
       <c r="G43" s="7"/>
       <c r="H43" s="7"/>
     </row>
-    <row r="44" spans="1:11" s="21" customFormat="1" ht="14.4">
-      <c r="A44" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="B44" s="20" t="s">
+    <row r="44" spans="1:11" ht="14.4">
+      <c r="A44" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B44" s="15" t="s">
         <v>24</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>807</v>
+        <v>44</v>
       </c>
       <c r="E44" s="7" t="s">
-        <v>804</v>
-      </c>
-      <c r="F44" s="7"/>
-      <c r="G44" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="H44" s="58" t="s">
-        <v>75</v>
-      </c>
-      <c r="I44" s="57" t="s">
-        <v>26</v>
-      </c>
-      <c r="J44" s="57" t="s">
-        <v>27</v>
-      </c>
-      <c r="K44" s="57" t="s">
-        <v>806</v>
-      </c>
+        <v>91</v>
+      </c>
+      <c r="F44" s="7">
+        <v>6758</v>
+      </c>
+      <c r="G44" s="7"/>
+      <c r="H44" s="7"/>
     </row>
     <row r="45" spans="1:11" s="21" customFormat="1" ht="14.4">
       <c r="A45" s="20" t="s">
@@ -21698,10 +21718,10 @@
         <v>24</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>808</v>
-      </c>
-      <c r="E45" s="58" t="s">
-        <v>805</v>
+        <v>807</v>
+      </c>
+      <c r="E45" s="7" t="s">
+        <v>804</v>
       </c>
       <c r="F45" s="7"/>
       <c r="G45" s="7" t="s">
@@ -21717,225 +21737,233 @@
         <v>27</v>
       </c>
       <c r="K45" s="57" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" s="21" customFormat="1" ht="14.4">
+      <c r="A46" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="B46" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>807</v>
+      </c>
+      <c r="E46" s="7" t="s">
+        <v>937</v>
+      </c>
+      <c r="F46" s="7"/>
+      <c r="G46" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="H46" s="58" t="s">
+        <v>132</v>
+      </c>
+      <c r="I46" s="57" t="s">
+        <v>26</v>
+      </c>
+      <c r="J46" s="57" t="s">
+        <v>27</v>
+      </c>
+      <c r="K46" s="57" t="s">
+        <v>938</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" s="21" customFormat="1" ht="14.4">
+      <c r="A47" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="B47" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>808</v>
+      </c>
+      <c r="E47" s="58" t="s">
+        <v>805</v>
+      </c>
+      <c r="F47" s="7"/>
+      <c r="G47" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H47" s="58" t="s">
+        <v>75</v>
+      </c>
+      <c r="I47" s="57" t="s">
+        <v>26</v>
+      </c>
+      <c r="J47" s="57" t="s">
+        <v>27</v>
+      </c>
+      <c r="K47" s="57" t="s">
         <v>809</v>
       </c>
     </row>
-    <row r="46" spans="1:11" ht="14.4">
-      <c r="A46" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B46" s="15" t="s">
+    <row r="48" spans="1:11" ht="14.4">
+      <c r="A48" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B48" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="E46" s="7" t="s">
+      <c r="E48" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="F46" s="7">
+      <c r="F48" s="7">
         <v>0</v>
       </c>
-      <c r="G46" s="18" t="s">
+      <c r="G48" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="H46" s="57" t="s">
+      <c r="H48" s="57" t="s">
         <v>75</v>
       </c>
-      <c r="I46" s="17" t="s">
+      <c r="I48" s="17" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="47" spans="1:11" ht="14.4">
-      <c r="A47" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B47" s="15" t="s">
+    <row r="49" spans="1:24" ht="14.4">
+      <c r="A49" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B49" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="E47" s="7" t="s">
+      <c r="E49" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="F47" s="7">
+      <c r="F49" s="7">
         <v>0</v>
       </c>
-      <c r="G47" s="7"/>
-      <c r="H47" s="7"/>
-      <c r="K47" s="17" t="s">
+      <c r="G49" s="7"/>
+      <c r="H49" s="7"/>
+      <c r="K49" s="17" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="48" spans="1:11" s="21" customFormat="1" ht="14.4">
-      <c r="A48" s="20"/>
-      <c r="B48" s="20"/>
-      <c r="E48" s="7" t="s">
-        <v>863</v>
-      </c>
-      <c r="F48" s="7">
-        <v>0.08</v>
-      </c>
-      <c r="G48" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="H48" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="I48" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="J48" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="K48" s="23" t="s">
-        <v>864</v>
-      </c>
-    </row>
-    <row r="49" spans="1:26" s="21" customFormat="1" ht="14.4">
-      <c r="A49" s="20"/>
-      <c r="B49" s="20"/>
-      <c r="E49" s="58" t="s">
-        <v>843</v>
-      </c>
-      <c r="F49" s="7"/>
-      <c r="G49" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="H49" s="7" t="s">
-        <v>478</v>
-      </c>
-      <c r="I49" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="K49" s="23" t="s">
-        <v>844</v>
-      </c>
-    </row>
-    <row r="50" spans="1:26" s="21" customFormat="1" ht="14.4">
+    <row r="50" spans="1:24" s="21" customFormat="1" ht="14.4">
       <c r="A50" s="20"/>
       <c r="B50" s="20"/>
       <c r="E50" s="7" t="s">
-        <v>842</v>
-      </c>
-      <c r="F50" s="7"/>
+        <v>863</v>
+      </c>
+      <c r="F50" s="7">
+        <v>0.08</v>
+      </c>
       <c r="G50" s="7" t="s">
         <v>112</v>
       </c>
       <c r="H50" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="I50" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="J50" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="K50" s="23" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="51" spans="1:24" s="21" customFormat="1" ht="14.4">
+      <c r="A51" s="20"/>
+      <c r="B51" s="20"/>
+      <c r="E51" s="58" t="s">
+        <v>843</v>
+      </c>
+      <c r="F51" s="7"/>
+      <c r="G51" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="H51" s="7" t="s">
         <v>478</v>
       </c>
-      <c r="I50" s="21" t="s">
+      <c r="I51" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="K50" s="23" t="s">
+      <c r="K51" s="23" t="s">
+        <v>844</v>
+      </c>
+    </row>
+    <row r="52" spans="1:24" s="21" customFormat="1" ht="14.4">
+      <c r="A52" s="20"/>
+      <c r="B52" s="20"/>
+      <c r="E52" s="7" t="s">
+        <v>842</v>
+      </c>
+      <c r="F52" s="7"/>
+      <c r="G52" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="H52" s="7" t="s">
+        <v>478</v>
+      </c>
+      <c r="I52" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="K52" s="23" t="s">
         <v>857</v>
       </c>
     </row>
-    <row r="51" spans="1:26" s="61" customFormat="1" ht="14.4">
-      <c r="A51" s="59"/>
-      <c r="B51" s="59"/>
-      <c r="E51" s="62" t="s">
+    <row r="53" spans="1:24" s="61" customFormat="1" ht="14.4">
+      <c r="A53" s="59"/>
+      <c r="B53" s="59"/>
+      <c r="E53" s="62" t="s">
         <v>854</v>
       </c>
-      <c r="F51" s="62"/>
-      <c r="G51" s="62" t="s">
+      <c r="F53" s="62"/>
+      <c r="G53" s="62" t="s">
         <v>112</v>
       </c>
-      <c r="H51" s="62" t="s">
+      <c r="H53" s="62" t="s">
         <v>98</v>
       </c>
-      <c r="I51" s="61" t="s">
+      <c r="I53" s="61" t="s">
         <v>26</v>
       </c>
-      <c r="J51" s="61" t="s">
+      <c r="J53" s="61" t="s">
         <v>27</v>
       </c>
-      <c r="K51" s="60" t="s">
+      <c r="K53" s="60" t="s">
         <v>855</v>
       </c>
     </row>
-    <row r="52" spans="1:26" ht="14.4">
-      <c r="A52" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="B52" s="24" t="s">
+    <row r="54" spans="1:24" ht="14.4">
+      <c r="A54" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B54" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="C52" s="17" t="s">
+      <c r="C54" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="D52" s="17" t="s">
+      <c r="D54" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="E52" s="18" t="s">
+      <c r="E54" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="F52" s="7"/>
-      <c r="G52" s="18" t="s">
+      <c r="F54" s="7"/>
+      <c r="G54" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="H52" s="18" t="s">
+      <c r="H54" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="I52" s="17" t="s">
+      <c r="I54" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="J52" s="17" t="s">
+      <c r="J54" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="K52" s="17" t="s">
+      <c r="K54" s="17" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="53" spans="1:26" s="21" customFormat="1" ht="14.4">
-      <c r="A53" s="20"/>
-      <c r="B53" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="C53" s="22"/>
-      <c r="D53" s="22"/>
-      <c r="E53" s="21" t="s">
-        <v>922</v>
-      </c>
-      <c r="F53" s="7"/>
-      <c r="G53" s="21" t="s">
-        <v>112</v>
-      </c>
-      <c r="H53" s="21" t="s">
-        <v>923</v>
-      </c>
-      <c r="I53" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="J53" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="K53" s="23" t="s">
-        <v>917</v>
-      </c>
-    </row>
-    <row r="54" spans="1:26" s="21" customFormat="1" ht="14.4">
-      <c r="A54" s="20"/>
-      <c r="B54" s="24"/>
-      <c r="C54" s="22"/>
-      <c r="D54" s="22"/>
-      <c r="E54" s="21" t="s">
-        <v>925</v>
-      </c>
-      <c r="F54" s="7"/>
-      <c r="G54" s="21" t="s">
-        <v>112</v>
-      </c>
-      <c r="H54" s="21" t="s">
-        <v>410</v>
-      </c>
-      <c r="I54" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="J54" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="K54" s="23" t="s">
-        <v>926</v>
-      </c>
-    </row>
-    <row r="55" spans="1:26" s="21" customFormat="1" ht="14.4">
+    <row r="55" spans="1:24" s="21" customFormat="1" ht="14.4">
       <c r="A55" s="20"/>
       <c r="B55" s="24" t="s">
         <v>23</v>
@@ -21943,14 +21971,14 @@
       <c r="C55" s="22"/>
       <c r="D55" s="22"/>
       <c r="E55" s="21" t="s">
-        <v>918</v>
+        <v>922</v>
       </c>
       <c r="F55" s="7"/>
       <c r="G55" s="21" t="s">
         <v>112</v>
       </c>
       <c r="H55" s="21" t="s">
-        <v>98</v>
+        <v>923</v>
       </c>
       <c r="I55" s="23" t="s">
         <v>26</v>
@@ -21959,575 +21987,573 @@
         <v>27</v>
       </c>
       <c r="K55" s="23" t="s">
-        <v>919</v>
-      </c>
-    </row>
-    <row r="56" spans="1:26" ht="43.2">
-      <c r="A56" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B56" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="E56" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="F56" s="18">
-        <v>1</v>
-      </c>
-      <c r="G56" s="18" t="s">
-        <v>101</v>
-      </c>
-      <c r="H56" s="18" t="s">
-        <v>102</v>
-      </c>
-      <c r="J56" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="K56" s="19" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="57" spans="1:26" s="21" customFormat="1" ht="14.4">
+        <v>917</v>
+      </c>
+    </row>
+    <row r="56" spans="1:24" s="21" customFormat="1" ht="14.4">
+      <c r="A56" s="20"/>
+      <c r="B56" s="24"/>
+      <c r="C56" s="22"/>
+      <c r="D56" s="22"/>
+      <c r="E56" s="21" t="s">
+        <v>925</v>
+      </c>
+      <c r="F56" s="7"/>
+      <c r="G56" s="21" t="s">
+        <v>112</v>
+      </c>
+      <c r="H56" s="21" t="s">
+        <v>410</v>
+      </c>
+      <c r="I56" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="J56" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="K56" s="23" t="s">
+        <v>926</v>
+      </c>
+    </row>
+    <row r="57" spans="1:24" s="21" customFormat="1" ht="14.4">
       <c r="A57" s="20"/>
-      <c r="B57" s="20"/>
-      <c r="E57" s="7" t="s">
-        <v>927</v>
-      </c>
+      <c r="B57" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="C57" s="22"/>
+      <c r="D57" s="22"/>
+      <c r="E57" s="21" t="s">
+        <v>918</v>
+      </c>
+      <c r="F57" s="7"/>
       <c r="G57" s="21" t="s">
         <v>112</v>
       </c>
       <c r="H57" s="21" t="s">
-        <v>478</v>
+        <v>98</v>
       </c>
       <c r="I57" s="23" t="s">
         <v>26</v>
       </c>
       <c r="J57" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="K57" s="23" t="s">
+        <v>919</v>
+      </c>
+    </row>
+    <row r="58" spans="1:24" ht="43.2">
+      <c r="A58" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B58" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="E58" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="F58" s="18">
+        <v>1</v>
+      </c>
+      <c r="G58" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="H58" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="J58" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="K57" s="23" t="s">
+      <c r="K58" s="19" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="59" spans="1:24" s="21" customFormat="1" ht="14.4">
+      <c r="A59" s="20"/>
+      <c r="B59" s="20"/>
+      <c r="E59" s="7" t="s">
+        <v>927</v>
+      </c>
+      <c r="G59" s="21" t="s">
+        <v>112</v>
+      </c>
+      <c r="H59" s="21" t="s">
+        <v>478</v>
+      </c>
+      <c r="I59" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="J59" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="K59" s="23" t="s">
         <v>928</v>
       </c>
     </row>
-    <row r="58" spans="1:26" s="25" customFormat="1" ht="86.4">
-      <c r="A58" s="85"/>
-      <c r="B58" s="85"/>
-      <c r="E58" s="25" t="s">
+    <row r="60" spans="1:24" s="25" customFormat="1" ht="86.4">
+      <c r="A60" s="85"/>
+      <c r="B60" s="85"/>
+      <c r="E60" s="25" t="s">
         <v>104</v>
       </c>
-      <c r="F58" s="25">
+      <c r="F60" s="25">
         <v>1</v>
       </c>
-      <c r="G58" s="25" t="s">
+      <c r="G60" s="25" t="s">
         <v>101</v>
       </c>
-      <c r="H58" s="25" t="s">
+      <c r="H60" s="25" t="s">
         <v>102</v>
       </c>
-      <c r="I58" s="19" t="s">
+      <c r="I60" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="J58" s="19" t="s">
+      <c r="J60" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="K58" s="84" t="s">
+      <c r="K60" s="84" t="s">
         <v>865</v>
       </c>
     </row>
-    <row r="59" spans="1:26" s="25" customFormat="1" ht="14.4">
-      <c r="A59" s="85"/>
-      <c r="B59" s="85"/>
-      <c r="E59" s="76" t="s">
+    <row r="61" spans="1:24" s="25" customFormat="1" ht="14.4">
+      <c r="A61" s="85"/>
+      <c r="B61" s="85"/>
+      <c r="E61" s="76" t="s">
         <v>929</v>
       </c>
-      <c r="G59" s="76" t="s">
+      <c r="G61" s="76" t="s">
         <v>112</v>
       </c>
-      <c r="H59" s="76" t="s">
+      <c r="H61" s="76" t="s">
         <v>478</v>
       </c>
-      <c r="I59" s="84" t="s">
+      <c r="I61" s="84" t="s">
         <v>26</v>
       </c>
-      <c r="J59" s="84" t="s">
+      <c r="J61" s="84" t="s">
         <v>27</v>
       </c>
-      <c r="K59" s="23" t="s">
+      <c r="K61" s="23" t="s">
         <v>930</v>
       </c>
     </row>
-    <row r="60" spans="1:26" s="25" customFormat="1" ht="28.8">
-      <c r="A60" s="85"/>
-      <c r="B60" s="85" t="s">
-        <v>23</v>
-      </c>
-      <c r="E60" s="25" t="s">
+    <row r="62" spans="1:24" s="25" customFormat="1" ht="28.8">
+      <c r="A62" s="85"/>
+      <c r="B62" s="85" t="s">
+        <v>23</v>
+      </c>
+      <c r="E62" s="25" t="s">
         <v>920</v>
       </c>
-      <c r="G60" s="25" t="s">
+      <c r="G62" s="25" t="s">
         <v>112</v>
       </c>
-      <c r="H60" s="25" t="s">
+      <c r="H62" s="25" t="s">
         <v>132</v>
       </c>
-      <c r="I60" s="84" t="s">
+      <c r="I62" s="84" t="s">
         <v>26</v>
       </c>
-      <c r="J60" s="19"/>
-      <c r="K60" s="84" t="s">
+      <c r="J62" s="19"/>
+      <c r="K62" s="84" t="s">
         <v>921</v>
       </c>
     </row>
-    <row r="61" spans="1:26" s="21" customFormat="1" ht="14.25" customHeight="1">
-      <c r="C61" s="28"/>
-      <c r="D61" s="28"/>
-      <c r="E61" s="7" t="s">
+    <row r="63" spans="1:24" s="21" customFormat="1" ht="14.25" customHeight="1">
+      <c r="C63" s="28"/>
+      <c r="D63" s="28"/>
+      <c r="E63" s="7" t="s">
         <v>815</v>
       </c>
-      <c r="F61" s="7"/>
-      <c r="G61" s="74" t="s">
+      <c r="F63" s="7"/>
+      <c r="G63" s="74" t="s">
         <v>29</v>
       </c>
-      <c r="H61" s="74" t="s">
+      <c r="H63" s="74" t="s">
         <v>230</v>
       </c>
-      <c r="I61" s="74" t="s">
+      <c r="I63" s="74" t="s">
         <v>34</v>
       </c>
-      <c r="J61" s="74" t="s">
+      <c r="J63" s="74" t="s">
         <v>27</v>
       </c>
-      <c r="K61" s="57" t="s">
+      <c r="K63" s="57" t="s">
         <v>816</v>
       </c>
-      <c r="L61" s="74" t="s">
+      <c r="L63" s="74" t="s">
         <v>817</v>
       </c>
-      <c r="M61" s="3"/>
-      <c r="N61" s="7"/>
-      <c r="O61" s="7"/>
-      <c r="P61" s="7"/>
-      <c r="Q61" s="7"/>
-      <c r="R61" s="7"/>
-      <c r="S61" s="7"/>
-      <c r="T61" s="7"/>
-      <c r="U61" s="7"/>
-      <c r="V61" s="7"/>
-      <c r="W61" s="7"/>
-      <c r="X61" s="7"/>
-    </row>
-    <row r="62" spans="1:26" ht="14.4">
-      <c r="A62" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B62" s="15" t="s">
+      <c r="M63" s="3"/>
+      <c r="N63" s="7"/>
+      <c r="O63" s="7"/>
+      <c r="P63" s="7"/>
+      <c r="Q63" s="7"/>
+      <c r="R63" s="7"/>
+      <c r="S63" s="7"/>
+      <c r="T63" s="7"/>
+      <c r="U63" s="7"/>
+      <c r="V63" s="7"/>
+      <c r="W63" s="7"/>
+      <c r="X63" s="7"/>
+    </row>
+    <row r="64" spans="1:24" ht="14.4">
+      <c r="A64" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B64" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="E62" s="7" t="s">
+      <c r="E64" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="F62" s="7">
+      <c r="F64" s="7">
         <v>-1</v>
       </c>
-      <c r="G62" s="7"/>
-      <c r="H62" s="7"/>
-    </row>
-    <row r="63" spans="1:26" s="21" customFormat="1" ht="14.4">
-      <c r="A63" s="20"/>
-      <c r="B63" s="20"/>
-      <c r="E63" s="7"/>
-      <c r="F63" s="7"/>
-      <c r="G63" s="7"/>
-      <c r="H63" s="7"/>
-    </row>
-    <row r="64" spans="1:26" ht="14.4">
-      <c r="A64" s="15"/>
-      <c r="B64" s="15"/>
-      <c r="C64" s="7" t="s">
+      <c r="G64" s="7"/>
+      <c r="H64" s="7"/>
+    </row>
+    <row r="65" spans="1:26" s="21" customFormat="1" ht="14.4">
+      <c r="A65" s="20"/>
+      <c r="B65" s="20"/>
+      <c r="E65" s="7"/>
+      <c r="F65" s="7"/>
+      <c r="G65" s="7"/>
+      <c r="H65" s="7"/>
+    </row>
+    <row r="66" spans="1:26" ht="14.4">
+      <c r="A66" s="15"/>
+      <c r="B66" s="15"/>
+      <c r="C66" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="D64" s="7" t="s">
+      <c r="D66" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="E64" s="7" t="s">
+      <c r="E66" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="F64" s="7">
+      <c r="F66" s="7">
         <v>0.6</v>
       </c>
-      <c r="G64" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="H64" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="I64" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="J64" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="K64" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="L64" s="7"/>
-      <c r="M64" s="7"/>
-      <c r="N64" s="7"/>
-      <c r="O64" s="7"/>
-      <c r="P64" s="7"/>
-      <c r="Q64" s="7"/>
-      <c r="R64" s="7"/>
-      <c r="S64" s="7"/>
-      <c r="T64" s="7"/>
-      <c r="U64" s="7"/>
-      <c r="V64" s="7"/>
-      <c r="W64" s="7"/>
-      <c r="X64" s="7"/>
-      <c r="Y64" s="7"/>
-      <c r="Z64" s="7"/>
-    </row>
-    <row r="65" spans="1:12" ht="14.4">
-      <c r="A65" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B65" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="E65" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="F65" s="7">
-        <v>1739.927555</v>
-      </c>
-      <c r="G65" s="7"/>
-      <c r="H65" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="K65" s="3" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="66" spans="1:12" s="21" customFormat="1" ht="14.4">
-      <c r="A66" s="20"/>
-      <c r="B66" s="20"/>
-      <c r="E66" s="7" t="s">
-        <v>858</v>
-      </c>
-      <c r="F66" s="7"/>
       <c r="G66" s="7" t="s">
         <v>29</v>
       </c>
       <c r="H66" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="I66" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="J66" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="K66" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="L66" s="7"/>
+      <c r="M66" s="7"/>
+      <c r="N66" s="7"/>
+      <c r="O66" s="7"/>
+      <c r="P66" s="7"/>
+      <c r="Q66" s="7"/>
+      <c r="R66" s="7"/>
+      <c r="S66" s="7"/>
+      <c r="T66" s="7"/>
+      <c r="U66" s="7"/>
+      <c r="V66" s="7"/>
+      <c r="W66" s="7"/>
+      <c r="X66" s="7"/>
+      <c r="Y66" s="7"/>
+      <c r="Z66" s="7"/>
+    </row>
+    <row r="67" spans="1:26" ht="14.4">
+      <c r="A67" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B67" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="E67" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="F67" s="7">
+        <v>1739.927555</v>
+      </c>
+      <c r="G67" s="7"/>
+      <c r="H67" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="K67" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="68" spans="1:26" s="21" customFormat="1" ht="14.4">
+      <c r="A68" s="20"/>
+      <c r="B68" s="20"/>
+      <c r="E68" s="7" t="s">
+        <v>858</v>
+      </c>
+      <c r="F68" s="7"/>
+      <c r="G68" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H68" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="I66" s="21" t="s">
+      <c r="I68" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="J66" s="21" t="s">
+      <c r="J68" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="K66" s="21" t="s">
+      <c r="K68" s="21" t="s">
         <v>860</v>
       </c>
-      <c r="L66" s="3" t="s">
+      <c r="L68" s="3" t="s">
         <v>859</v>
       </c>
     </row>
-    <row r="67" spans="1:12" s="21" customFormat="1" ht="14.4">
-      <c r="A67" s="20"/>
-      <c r="B67" s="20"/>
-      <c r="E67" s="7" t="s">
+    <row r="69" spans="1:26" s="21" customFormat="1" ht="14.4">
+      <c r="A69" s="20"/>
+      <c r="B69" s="20"/>
+      <c r="E69" s="7" t="s">
         <v>924</v>
       </c>
-      <c r="F67" s="7"/>
-      <c r="G67" s="7" t="s">
+      <c r="F69" s="7"/>
+      <c r="G69" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="H67" s="7" t="s">
+      <c r="H69" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="I67" s="21" t="s">
+      <c r="I69" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="J67" s="21" t="s">
+      <c r="J69" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="K67" s="21" t="s">
+      <c r="K69" s="21" t="s">
         <v>909</v>
       </c>
-      <c r="L67" s="3" t="s">
+      <c r="L69" s="3" t="s">
         <v>859</v>
       </c>
     </row>
-    <row r="68" spans="1:12" ht="14.4">
-      <c r="A68" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B68" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="C68" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E68" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="F68" s="7">
-        <v>1</v>
-      </c>
-      <c r="G68" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="H68" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="I68" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="J68" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="K68" s="3" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="69" spans="1:12" ht="14.4">
-      <c r="A69" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B69" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="E69" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="F69" s="7">
-        <v>553659</v>
-      </c>
-      <c r="G69" s="7"/>
-      <c r="H69" s="7"/>
-    </row>
-    <row r="70" spans="1:12" ht="14.4">
+    <row r="70" spans="1:26" ht="14.4">
       <c r="A70" s="15" t="s">
         <v>23</v>
       </c>
       <c r="B70" s="15" t="s">
         <v>24</v>
       </c>
+      <c r="C70" s="3" t="s">
+        <v>24</v>
+      </c>
       <c r="E70" s="7" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="F70" s="7">
-        <v>4891208</v>
-      </c>
-      <c r="G70" s="7"/>
-      <c r="H70" s="7"/>
-    </row>
-    <row r="71" spans="1:12" ht="14.4">
+        <v>1</v>
+      </c>
+      <c r="G70" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="H70" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="I70" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="J70" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="K70" s="3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="71" spans="1:26" ht="14.4">
       <c r="A71" s="15" t="s">
         <v>23</v>
       </c>
       <c r="B71" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="C71" s="3" t="s">
+      <c r="E71" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="F71" s="7">
+        <v>553659</v>
+      </c>
+      <c r="G71" s="7"/>
+      <c r="H71" s="7"/>
+    </row>
+    <row r="72" spans="1:26" ht="14.4">
+      <c r="A72" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B72" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="E71" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="F71" s="7">
-        <v>1</v>
-      </c>
-      <c r="G71" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="H71" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="I71" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="J71" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="K71" s="3" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="72" spans="1:12" s="21" customFormat="1" ht="14.4">
-      <c r="A72" s="20" t="s">
-        <v>840</v>
-      </c>
-      <c r="B72" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="C72" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="D72" s="21" t="s">
-        <v>67</v>
-      </c>
       <c r="E72" s="7" t="s">
-        <v>839</v>
+        <v>122</v>
       </c>
       <c r="F72" s="7">
-        <v>5</v>
-      </c>
-      <c r="G72" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="H72" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="I72" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="J72" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="K72" s="3" t="s">
-        <v>841</v>
-      </c>
-      <c r="L72" s="23" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="73" spans="1:12" ht="14.4">
+        <v>4891208</v>
+      </c>
+      <c r="G72" s="7"/>
+      <c r="H72" s="7"/>
+    </row>
+    <row r="73" spans="1:26" ht="14.4">
       <c r="A73" s="15" t="s">
         <v>23</v>
       </c>
       <c r="B73" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="D73" s="3" t="s">
+      <c r="C73" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E73" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="F73" s="7">
+        <v>1</v>
+      </c>
+      <c r="G73" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="H73" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="I73" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="J73" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="K73" s="3" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="74" spans="1:26" s="21" customFormat="1" ht="14.4">
+      <c r="A74" s="20" t="s">
+        <v>840</v>
+      </c>
+      <c r="B74" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="C74" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D74" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="E74" s="7" t="s">
+        <v>839</v>
+      </c>
+      <c r="F74" s="7">
+        <v>5</v>
+      </c>
+      <c r="G74" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="H74" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="I74" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J74" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K74" s="3" t="s">
+        <v>841</v>
+      </c>
+      <c r="L74" s="23" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="75" spans="1:26" ht="14.4">
+      <c r="A75" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B75" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D75" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="E73" s="7" t="s">
+      <c r="E75" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="F73" s="7">
+      <c r="F75" s="7">
         <v>0</v>
       </c>
-      <c r="G73" s="7"/>
-      <c r="H73" s="7" t="s">
+      <c r="G75" s="7"/>
+      <c r="H75" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="I73" s="3" t="s">
+      <c r="I75" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="J73" s="3" t="s">
+      <c r="J75" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="K73" s="3" t="s">
+      <c r="K75" s="3" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="74" spans="1:12" ht="14.4">
-      <c r="A74" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B74" s="15"/>
-      <c r="E74" s="7" t="s">
+    <row r="76" spans="1:26" ht="14.4">
+      <c r="A76" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B76" s="15"/>
+      <c r="E76" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="F74" s="7">
+      <c r="F76" s="7">
         <v>6772</v>
       </c>
-      <c r="G74" s="7"/>
-      <c r="H74" s="7"/>
-    </row>
-    <row r="75" spans="1:12" s="21" customFormat="1" ht="14.4">
-      <c r="A75" s="20"/>
-      <c r="B75" s="20"/>
-      <c r="E75" s="7" t="s">
-        <v>846</v>
-      </c>
-      <c r="F75" s="7">
-        <v>1</v>
-      </c>
-      <c r="G75" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="H75" s="7" t="s">
-        <v>847</v>
-      </c>
-      <c r="I75" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="J75" s="23" t="s">
-        <v>848</v>
-      </c>
-    </row>
-    <row r="76" spans="1:12" s="21" customFormat="1" ht="14.4">
-      <c r="A76" s="20"/>
-      <c r="B76" s="20"/>
-      <c r="E76" s="7" t="s">
-        <v>845</v>
-      </c>
-      <c r="F76" s="7">
-        <v>10</v>
-      </c>
-      <c r="G76" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="H76" s="7" t="s">
-        <v>629</v>
-      </c>
-      <c r="I76" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="J76" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="K76" s="23" t="s">
-        <v>851</v>
-      </c>
-    </row>
-    <row r="77" spans="1:12" s="21" customFormat="1" ht="14.4">
+      <c r="G76" s="7"/>
+      <c r="H76" s="7"/>
+    </row>
+    <row r="77" spans="1:26" s="21" customFormat="1" ht="14.4">
       <c r="A77" s="20"/>
       <c r="B77" s="20"/>
-      <c r="D77" s="57" t="s">
-        <v>25</v>
-      </c>
       <c r="E77" s="7" t="s">
-        <v>799</v>
-      </c>
-      <c r="F77" s="7"/>
-      <c r="G77" s="58" t="s">
-        <v>29</v>
+        <v>846</v>
+      </c>
+      <c r="F77" s="7">
+        <v>1</v>
+      </c>
+      <c r="G77" s="7" t="s">
+        <v>112</v>
       </c>
       <c r="H77" s="7" t="s">
-        <v>75</v>
+        <v>847</v>
       </c>
       <c r="I77" s="23" t="s">
         <v>26</v>
       </c>
       <c r="J77" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="K77" s="23" t="s">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="78" spans="1:12" s="21" customFormat="1" ht="14.4">
-      <c r="A78" s="20" t="s">
-        <v>23</v>
-      </c>
+        <v>848</v>
+      </c>
+    </row>
+    <row r="78" spans="1:26" s="21" customFormat="1" ht="14.4">
+      <c r="A78" s="20"/>
       <c r="B78" s="20"/>
-      <c r="D78" s="57" t="s">
-        <v>25</v>
-      </c>
       <c r="E78" s="7" t="s">
-        <v>801</v>
-      </c>
-      <c r="F78" s="7"/>
-      <c r="G78" s="58" t="s">
-        <v>29</v>
+        <v>845</v>
+      </c>
+      <c r="F78" s="7">
+        <v>10</v>
+      </c>
+      <c r="G78" s="7" t="s">
+        <v>112</v>
       </c>
       <c r="H78" s="7" t="s">
-        <v>75</v>
+        <v>629</v>
       </c>
       <c r="I78" s="23" t="s">
         <v>26</v>
@@ -22536,71 +22562,61 @@
         <v>27</v>
       </c>
       <c r="K78" s="23" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="79" spans="1:26" s="21" customFormat="1" ht="14.4">
+      <c r="A79" s="20"/>
+      <c r="B79" s="20"/>
+      <c r="D79" s="57" t="s">
+        <v>25</v>
+      </c>
+      <c r="E79" s="7" t="s">
+        <v>799</v>
+      </c>
+      <c r="F79" s="7"/>
+      <c r="G79" s="58" t="s">
+        <v>29</v>
+      </c>
+      <c r="H79" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="I79" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="J79" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="K79" s="23" t="s">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="80" spans="1:26" s="21" customFormat="1" ht="14.4">
+      <c r="A80" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="B80" s="20"/>
+      <c r="D80" s="57" t="s">
+        <v>25</v>
+      </c>
+      <c r="E80" s="7" t="s">
+        <v>801</v>
+      </c>
+      <c r="F80" s="7"/>
+      <c r="G80" s="58" t="s">
+        <v>29</v>
+      </c>
+      <c r="H80" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="I80" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="J80" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="K80" s="23" t="s">
         <v>802</v>
-      </c>
-    </row>
-    <row r="79" spans="1:12" ht="14.4">
-      <c r="A79" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B79" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="D79" s="17" t="s">
-        <v>136</v>
-      </c>
-      <c r="E79" s="18" t="s">
-        <v>138</v>
-      </c>
-      <c r="F79" s="18">
-        <v>1500</v>
-      </c>
-      <c r="G79" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="H79" s="18" t="s">
-        <v>86</v>
-      </c>
-      <c r="I79" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="J79" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="K79" s="17" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="80" spans="1:12" ht="14.4">
-      <c r="A80" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B80" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="D80" s="17" t="s">
-        <v>136</v>
-      </c>
-      <c r="E80" s="17" t="s">
-        <v>143</v>
-      </c>
-      <c r="F80" s="17">
-        <v>1500</v>
-      </c>
-      <c r="G80" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="H80" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="I80" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="J80" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="K80" s="17" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="81" spans="1:11" ht="14.4">
@@ -22613,16 +22629,16 @@
       <c r="D81" s="17" t="s">
         <v>136</v>
       </c>
-      <c r="E81" s="17" t="s">
-        <v>146</v>
-      </c>
-      <c r="F81" s="17">
+      <c r="E81" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="F81" s="18">
         <v>1500</v>
       </c>
       <c r="G81" s="18" t="s">
         <v>112</v>
       </c>
-      <c r="H81" s="17" t="s">
+      <c r="H81" s="18" t="s">
         <v>86</v>
       </c>
       <c r="I81" s="17" t="s">
@@ -22632,7 +22648,7 @@
         <v>30</v>
       </c>
       <c r="K81" s="17" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
     </row>
     <row r="82" spans="1:11" ht="14.4">
@@ -22640,16 +22656,16 @@
         <v>23</v>
       </c>
       <c r="B82" s="16" t="s">
-        <v>148</v>
+        <v>24</v>
       </c>
       <c r="D82" s="17" t="s">
         <v>136</v>
       </c>
       <c r="E82" s="17" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="F82" s="17">
-        <v>1000</v>
+        <v>1500</v>
       </c>
       <c r="G82" s="18" t="s">
         <v>112</v>
@@ -22664,7 +22680,7 @@
         <v>30</v>
       </c>
       <c r="K82" s="17" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
     </row>
     <row r="83" spans="1:11" ht="14.4">
@@ -22672,22 +22688,22 @@
         <v>23</v>
       </c>
       <c r="B83" s="16" t="s">
-        <v>148</v>
+        <v>24</v>
       </c>
       <c r="D83" s="17" t="s">
         <v>136</v>
       </c>
       <c r="E83" s="17" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="F83" s="17">
-        <v>1000</v>
+        <v>1500</v>
       </c>
       <c r="G83" s="18" t="s">
         <v>112</v>
       </c>
       <c r="H83" s="17" t="s">
-        <v>109</v>
+        <v>86</v>
       </c>
       <c r="I83" s="17" t="s">
         <v>34</v>
@@ -22696,7 +22712,7 @@
         <v>30</v>
       </c>
       <c r="K83" s="17" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
     </row>
     <row r="84" spans="1:11" ht="14.4">
@@ -22710,7 +22726,7 @@
         <v>136</v>
       </c>
       <c r="E84" s="17" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="F84" s="17">
         <v>1000</v>
@@ -22719,7 +22735,7 @@
         <v>112</v>
       </c>
       <c r="H84" s="17" t="s">
-        <v>109</v>
+        <v>86</v>
       </c>
       <c r="I84" s="17" t="s">
         <v>34</v>
@@ -22728,13 +22744,77 @@
         <v>30</v>
       </c>
       <c r="K84" s="17" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" ht="14.4">
+      <c r="A85" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B85" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="D85" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="E85" s="17" t="s">
+        <v>151</v>
+      </c>
+      <c r="F85" s="17">
+        <v>1000</v>
+      </c>
+      <c r="G85" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="H85" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="I85" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="J85" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="K85" s="17" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" ht="14.4">
+      <c r="A86" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B86" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="D86" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="E86" s="17" t="s">
+        <v>153</v>
+      </c>
+      <c r="F86" s="17">
+        <v>1000</v>
+      </c>
+      <c r="G86" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="H86" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="I86" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="J86" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="K86" s="17" t="s">
         <v>154</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B52:B55">
+  <conditionalFormatting sqref="B54:B57">
     <cfRule type="notContainsBlanks" dxfId="0" priority="1">
-      <formula>LEN(TRIM(B52))&gt;0</formula>
+      <formula>LEN(TRIM(B54))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Tune up the flows for better agreement with gage records. HBV.csv - Increase ET_MULT for BLU9 and Lookout49 from 0.355 to 1.5. Increase ET_MULT for ClearLake46 from 0.5 to 1.0. Add PEST_ClearLake46/flow2010.ic. Flow_PEST_ClearLake46.xml - Increase spring feeding Clear Lake from 5.7 cms to 6.6 cms, the literature value. In the FLOW Q at gage reports, apply the 2.716 multiplier, for the ratio of the gage drainage to the simulated drainage, only to the runoff, not to the spring water. Flow_PEST_SFork48.xml - Decrease the spring flow above CGR from 6.06 cms (214 cfs) to 139 cfs. Flow_PEST_Smith47.xml - Decrease the spring flow from 0.76 cms (27 cfs) to 4 cfs.
</commit_message>
<xml_diff>
--- a/DataCW3M/CW3MdigitalHandbook/CW3MdataDictionary.xlsx
+++ b/DataCW3M/CW3MdigitalHandbook/CW3MdataDictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\CW3MdigitalHandbook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1189A22-7583-4551-8960-5A40066148B9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{474C6D33-3CF7-4DC9-B20D-6EC65F576C90}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2652" yWindow="156" windowWidth="18900" windowHeight="11388" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Necessary input data" sheetId="7" r:id="rId1"/>
@@ -20590,7 +20590,7 @@
   <dimension ref="A1:Z85"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="3" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A21" sqref="A21:XFD21"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Flow.cpp, .h - Code changes in the DumpReachInsolationData() logic.
</commit_message>
<xml_diff>
--- a/DataCW3M/CW3MdigitalHandbook/CW3MdataDictionary.xlsx
+++ b/DataCW3M/CW3MdigitalHandbook/CW3MdataDictionary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\CW3MdigitalHandbook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{474C6D33-3CF7-4DC9-B20D-6EC65F576C90}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3F4E6F2-94A5-4B4C-A12B-8421F37927C0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -96,7 +96,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2875" uniqueCount="938">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2896" uniqueCount="948">
   <si>
     <t>LULC_A</t>
   </si>
@@ -2911,6 +2911,36 @@
   </si>
   <si>
     <t>if this reach is the outfall of a reservoir, then RESOUTFALL = the reservoir ID for that reservoir, else RESOUTFALL = 0. Note that when RESOUTFALL is nonzero, RES_ID will usually be 0, i.e. the outfall reach is not in the reservoir itself.</t>
+  </si>
+  <si>
+    <t>TEMP_AIR</t>
+  </si>
+  <si>
+    <t>TMAX_AIR</t>
+  </si>
+  <si>
+    <t>average air temperature for the current day</t>
+  </si>
+  <si>
+    <t>maximum air temperature for the current day</t>
+  </si>
+  <si>
+    <t>TMIN_AIR</t>
+  </si>
+  <si>
+    <t>minimum air temperature for the current day</t>
+  </si>
+  <si>
+    <t>precip in the current day</t>
+  </si>
+  <si>
+    <t>average specific humidity for the current day</t>
+  </si>
+  <si>
+    <t>unshaded shortwave energy at the surface from climate models, takes cloudiness into account</t>
+  </si>
+  <si>
+    <t>average windspeed for the current day</t>
   </si>
 </sst>
 </file>
@@ -20587,11 +20617,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Z85"/>
+  <dimension ref="A1:Z92"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A21" sqref="A21:XFD21"/>
+      <pane ySplit="3" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K84" sqref="K84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -21765,27 +21795,22 @@
         <v>807</v>
       </c>
     </row>
-    <row r="47" spans="1:11" ht="14.4">
-      <c r="A47" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B47" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="E47" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="F47" s="7">
-        <v>0</v>
-      </c>
-      <c r="G47" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="H47" s="57" t="s">
-        <v>73</v>
-      </c>
-      <c r="I47" s="17" t="s">
-        <v>26</v>
+    <row r="47" spans="1:11" s="21" customFormat="1" ht="14.4">
+      <c r="A47" s="20"/>
+      <c r="B47" s="20"/>
+      <c r="D47" s="3"/>
+      <c r="E47" s="58" t="s">
+        <v>421</v>
+      </c>
+      <c r="F47" s="7"/>
+      <c r="G47" s="7"/>
+      <c r="H47" s="58" t="s">
+        <v>174</v>
+      </c>
+      <c r="I47" s="57"/>
+      <c r="J47" s="57"/>
+      <c r="K47" s="57" t="s">
+        <v>944</v>
       </c>
     </row>
     <row r="48" spans="1:11" ht="14.4">
@@ -21796,67 +21821,70 @@
         <v>24</v>
       </c>
       <c r="E48" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F48" s="7">
         <v>0</v>
       </c>
-      <c r="G48" s="7"/>
-      <c r="H48" s="7"/>
-      <c r="K48" s="17" t="s">
+      <c r="G48" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="H48" s="57" t="s">
+        <v>73</v>
+      </c>
+      <c r="I48" s="17" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="49" spans="1:24" ht="14.4">
+      <c r="A49" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B49" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="E49" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="F49" s="7">
+        <v>0</v>
+      </c>
+      <c r="G49" s="7"/>
+      <c r="H49" s="7"/>
+      <c r="K49" s="17" t="s">
         <v>92</v>
-      </c>
-    </row>
-    <row r="49" spans="1:24" s="21" customFormat="1" ht="14.4">
-      <c r="A49" s="20"/>
-      <c r="B49" s="20"/>
-      <c r="E49" s="7" t="s">
-        <v>861</v>
-      </c>
-      <c r="F49" s="7">
-        <v>0.08</v>
-      </c>
-      <c r="G49" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="H49" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="I49" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="J49" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="K49" s="23" t="s">
-        <v>862</v>
       </c>
     </row>
     <row r="50" spans="1:24" s="21" customFormat="1" ht="14.4">
       <c r="A50" s="20"/>
       <c r="B50" s="20"/>
-      <c r="E50" s="58" t="s">
-        <v>841</v>
-      </c>
-      <c r="F50" s="7"/>
+      <c r="E50" s="7" t="s">
+        <v>861</v>
+      </c>
+      <c r="F50" s="7">
+        <v>0.08</v>
+      </c>
       <c r="G50" s="7" t="s">
         <v>110</v>
       </c>
       <c r="H50" s="7" t="s">
-        <v>476</v>
+        <v>73</v>
       </c>
       <c r="I50" s="21" t="s">
-        <v>26</v>
+        <v>34</v>
+      </c>
+      <c r="J50" s="21" t="s">
+        <v>30</v>
       </c>
       <c r="K50" s="23" t="s">
-        <v>842</v>
+        <v>862</v>
       </c>
     </row>
     <row r="51" spans="1:24" s="21" customFormat="1" ht="14.4">
       <c r="A51" s="20"/>
       <c r="B51" s="20"/>
-      <c r="E51" s="7" t="s">
-        <v>840</v>
+      <c r="E51" s="58" t="s">
+        <v>841</v>
       </c>
       <c r="F51" s="7"/>
       <c r="G51" s="7" t="s">
@@ -21869,115 +21897,98 @@
         <v>26</v>
       </c>
       <c r="K51" s="23" t="s">
+        <v>842</v>
+      </c>
+    </row>
+    <row r="52" spans="1:24" s="21" customFormat="1" ht="14.4">
+      <c r="A52" s="20"/>
+      <c r="B52" s="20"/>
+      <c r="E52" s="58" t="s">
+        <v>474</v>
+      </c>
+      <c r="F52" s="7"/>
+      <c r="G52" s="7"/>
+      <c r="H52" s="7" t="s">
+        <v>476</v>
+      </c>
+      <c r="K52" s="23" t="s">
+        <v>946</v>
+      </c>
+    </row>
+    <row r="53" spans="1:24" s="21" customFormat="1" ht="14.4">
+      <c r="A53" s="20"/>
+      <c r="B53" s="20"/>
+      <c r="E53" s="7" t="s">
+        <v>840</v>
+      </c>
+      <c r="F53" s="7"/>
+      <c r="G53" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="H53" s="7" t="s">
+        <v>476</v>
+      </c>
+      <c r="I53" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="K53" s="23" t="s">
         <v>855</v>
       </c>
     </row>
-    <row r="52" spans="1:24" s="61" customFormat="1" ht="14.4">
-      <c r="A52" s="59"/>
-      <c r="B52" s="59"/>
-      <c r="E52" s="62" t="s">
+    <row r="54" spans="1:24" s="61" customFormat="1" ht="14.4">
+      <c r="A54" s="59"/>
+      <c r="B54" s="59"/>
+      <c r="E54" s="62" t="s">
         <v>852</v>
       </c>
-      <c r="F52" s="62"/>
-      <c r="G52" s="62" t="s">
+      <c r="F54" s="62"/>
+      <c r="G54" s="62" t="s">
         <v>110</v>
       </c>
-      <c r="H52" s="62" t="s">
+      <c r="H54" s="62" t="s">
         <v>96</v>
       </c>
-      <c r="I52" s="61" t="s">
+      <c r="I54" s="61" t="s">
         <v>26</v>
       </c>
-      <c r="J52" s="61" t="s">
+      <c r="J54" s="61" t="s">
         <v>27</v>
       </c>
-      <c r="K52" s="60" t="s">
+      <c r="K54" s="60" t="s">
         <v>853</v>
       </c>
     </row>
-    <row r="53" spans="1:24" ht="14.4">
-      <c r="A53" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="B53" s="24" t="s">
+    <row r="55" spans="1:24" ht="14.4">
+      <c r="A55" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B55" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="C53" s="17" t="s">
+      <c r="C55" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="D53" s="17" t="s">
+      <c r="D55" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="E53" s="18" t="s">
+      <c r="E55" s="18" t="s">
         <v>95</v>
       </c>
-      <c r="F53" s="7"/>
-      <c r="G53" s="18" t="s">
+      <c r="F55" s="7"/>
+      <c r="G55" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="H53" s="18" t="s">
+      <c r="H55" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="I53" s="17" t="s">
+      <c r="I55" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="J53" s="17" t="s">
+      <c r="J55" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="K53" s="17" t="s">
+      <c r="K55" s="17" t="s">
         <v>97</v>
-      </c>
-    </row>
-    <row r="54" spans="1:24" s="21" customFormat="1" ht="14.4">
-      <c r="A54" s="20"/>
-      <c r="B54" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="C54" s="22"/>
-      <c r="D54" s="22"/>
-      <c r="E54" s="21" t="s">
-        <v>919</v>
-      </c>
-      <c r="F54" s="7"/>
-      <c r="G54" s="21" t="s">
-        <v>110</v>
-      </c>
-      <c r="H54" s="21" t="s">
-        <v>920</v>
-      </c>
-      <c r="I54" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="J54" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="K54" s="23" t="s">
-        <v>914</v>
-      </c>
-    </row>
-    <row r="55" spans="1:24" s="21" customFormat="1" ht="14.4">
-      <c r="A55" s="20"/>
-      <c r="B55" s="24"/>
-      <c r="C55" s="22"/>
-      <c r="D55" s="22"/>
-      <c r="E55" s="21" t="s">
-        <v>922</v>
-      </c>
-      <c r="F55" s="7"/>
-      <c r="G55" s="21" t="s">
-        <v>110</v>
-      </c>
-      <c r="H55" s="21" t="s">
-        <v>408</v>
-      </c>
-      <c r="I55" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="J55" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="K55" s="23" t="s">
-        <v>923</v>
       </c>
     </row>
     <row r="56" spans="1:24" s="21" customFormat="1" ht="14.4">
@@ -21988,14 +21999,14 @@
       <c r="C56" s="22"/>
       <c r="D56" s="22"/>
       <c r="E56" s="21" t="s">
-        <v>915</v>
+        <v>919</v>
       </c>
       <c r="F56" s="7"/>
       <c r="G56" s="21" t="s">
         <v>110</v>
       </c>
       <c r="H56" s="21" t="s">
-        <v>96</v>
+        <v>920</v>
       </c>
       <c r="I56" s="23" t="s">
         <v>26</v>
@@ -22004,370 +22015,371 @@
         <v>27</v>
       </c>
       <c r="K56" s="23" t="s">
-        <v>916</v>
-      </c>
-    </row>
-    <row r="57" spans="1:24" ht="43.2">
-      <c r="A57" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B57" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="E57" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="F57" s="18">
-        <v>1</v>
-      </c>
-      <c r="G57" s="18" t="s">
-        <v>99</v>
-      </c>
-      <c r="H57" s="18" t="s">
-        <v>100</v>
-      </c>
-      <c r="J57" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="K57" s="19" t="s">
-        <v>101</v>
+        <v>914</v>
+      </c>
+    </row>
+    <row r="57" spans="1:24" s="21" customFormat="1" ht="14.4">
+      <c r="A57" s="20"/>
+      <c r="B57" s="24"/>
+      <c r="C57" s="22"/>
+      <c r="D57" s="22"/>
+      <c r="E57" s="21" t="s">
+        <v>922</v>
+      </c>
+      <c r="F57" s="7"/>
+      <c r="G57" s="21" t="s">
+        <v>110</v>
+      </c>
+      <c r="H57" s="21" t="s">
+        <v>408</v>
+      </c>
+      <c r="I57" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="J57" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="K57" s="23" t="s">
+        <v>923</v>
       </c>
     </row>
     <row r="58" spans="1:24" s="21" customFormat="1" ht="14.4">
       <c r="A58" s="20"/>
-      <c r="B58" s="20"/>
-      <c r="E58" s="7" t="s">
-        <v>924</v>
-      </c>
+      <c r="B58" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="C58" s="22"/>
+      <c r="D58" s="22"/>
+      <c r="E58" s="21" t="s">
+        <v>915</v>
+      </c>
+      <c r="F58" s="7"/>
       <c r="G58" s="21" t="s">
         <v>110</v>
       </c>
       <c r="H58" s="21" t="s">
-        <v>476</v>
+        <v>96</v>
       </c>
       <c r="I58" s="23" t="s">
         <v>26</v>
       </c>
       <c r="J58" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="K58" s="23" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="59" spans="1:24" ht="43.2">
+      <c r="A59" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B59" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="E59" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="F59" s="18">
+        <v>1</v>
+      </c>
+      <c r="G59" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="H59" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="J59" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="K58" s="23" t="s">
+      <c r="K59" s="19" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="60" spans="1:24" s="21" customFormat="1" ht="14.4">
+      <c r="A60" s="20"/>
+      <c r="B60" s="20"/>
+      <c r="E60" s="7" t="s">
+        <v>924</v>
+      </c>
+      <c r="G60" s="21" t="s">
+        <v>110</v>
+      </c>
+      <c r="H60" s="21" t="s">
+        <v>476</v>
+      </c>
+      <c r="I60" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="J60" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="K60" s="23" t="s">
         <v>925</v>
       </c>
     </row>
-    <row r="59" spans="1:24" s="25" customFormat="1" ht="86.4">
-      <c r="A59" s="85"/>
-      <c r="B59" s="85"/>
-      <c r="E59" s="25" t="s">
+    <row r="61" spans="1:24" s="25" customFormat="1" ht="86.4">
+      <c r="A61" s="85"/>
+      <c r="B61" s="85"/>
+      <c r="E61" s="25" t="s">
         <v>102</v>
       </c>
-      <c r="F59" s="25">
+      <c r="F61" s="25">
         <v>1</v>
       </c>
-      <c r="G59" s="25" t="s">
+      <c r="G61" s="25" t="s">
         <v>99</v>
       </c>
-      <c r="H59" s="25" t="s">
+      <c r="H61" s="25" t="s">
         <v>100</v>
       </c>
-      <c r="I59" s="19" t="s">
+      <c r="I61" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="J59" s="19" t="s">
+      <c r="J61" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="K59" s="84" t="s">
+      <c r="K61" s="84" t="s">
         <v>937</v>
       </c>
     </row>
-    <row r="60" spans="1:24" s="25" customFormat="1" ht="14.4">
-      <c r="A60" s="85"/>
-      <c r="B60" s="85"/>
-      <c r="E60" s="76" t="s">
+    <row r="62" spans="1:24" s="25" customFormat="1" ht="14.4">
+      <c r="A62" s="85"/>
+      <c r="B62" s="85"/>
+      <c r="E62" s="76" t="s">
         <v>926</v>
       </c>
-      <c r="G60" s="76" t="s">
+      <c r="G62" s="76" t="s">
         <v>110</v>
       </c>
-      <c r="H60" s="76" t="s">
+      <c r="H62" s="76" t="s">
         <v>476</v>
       </c>
-      <c r="I60" s="84" t="s">
+      <c r="I62" s="84" t="s">
         <v>26</v>
       </c>
-      <c r="J60" s="84" t="s">
+      <c r="J62" s="84" t="s">
         <v>27</v>
       </c>
-      <c r="K60" s="23" t="s">
+      <c r="K62" s="23" t="s">
         <v>927</v>
       </c>
     </row>
-    <row r="61" spans="1:24" s="25" customFormat="1" ht="28.8">
-      <c r="A61" s="85"/>
-      <c r="B61" s="85" t="s">
-        <v>23</v>
-      </c>
-      <c r="E61" s="25" t="s">
+    <row r="63" spans="1:24" s="25" customFormat="1" ht="28.8">
+      <c r="A63" s="85"/>
+      <c r="B63" s="85" t="s">
+        <v>23</v>
+      </c>
+      <c r="E63" s="25" t="s">
         <v>917</v>
       </c>
-      <c r="G61" s="25" t="s">
+      <c r="G63" s="25" t="s">
         <v>110</v>
       </c>
-      <c r="H61" s="25" t="s">
+      <c r="H63" s="25" t="s">
         <v>130</v>
       </c>
-      <c r="I61" s="84" t="s">
+      <c r="I63" s="84" t="s">
         <v>26</v>
       </c>
-      <c r="J61" s="19"/>
-      <c r="K61" s="84" t="s">
+      <c r="J63" s="19"/>
+      <c r="K63" s="84" t="s">
         <v>918</v>
       </c>
     </row>
-    <row r="62" spans="1:24" s="21" customFormat="1" ht="14.25" customHeight="1">
-      <c r="C62" s="28"/>
-      <c r="D62" s="28"/>
-      <c r="E62" s="7" t="s">
+    <row r="64" spans="1:24" s="21" customFormat="1" ht="14.25" customHeight="1">
+      <c r="C64" s="28"/>
+      <c r="D64" s="28"/>
+      <c r="E64" s="7" t="s">
         <v>813</v>
       </c>
-      <c r="F62" s="7"/>
-      <c r="G62" s="74" t="s">
+      <c r="F64" s="7"/>
+      <c r="G64" s="74" t="s">
         <v>29</v>
       </c>
-      <c r="H62" s="74" t="s">
+      <c r="H64" s="74" t="s">
         <v>228</v>
       </c>
-      <c r="I62" s="74" t="s">
+      <c r="I64" s="74" t="s">
         <v>34</v>
       </c>
-      <c r="J62" s="74" t="s">
+      <c r="J64" s="74" t="s">
         <v>27</v>
       </c>
-      <c r="K62" s="57" t="s">
+      <c r="K64" s="57" t="s">
         <v>814</v>
       </c>
-      <c r="L62" s="74" t="s">
+      <c r="L64" s="74" t="s">
         <v>815</v>
       </c>
-      <c r="M62" s="3"/>
-      <c r="N62" s="7"/>
-      <c r="O62" s="7"/>
-      <c r="P62" s="7"/>
-      <c r="Q62" s="7"/>
-      <c r="R62" s="7"/>
-      <c r="S62" s="7"/>
-      <c r="T62" s="7"/>
-      <c r="U62" s="7"/>
-      <c r="V62" s="7"/>
-      <c r="W62" s="7"/>
-      <c r="X62" s="7"/>
-    </row>
-    <row r="63" spans="1:24" ht="14.4">
-      <c r="A63" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B63" s="15" t="s">
+      <c r="M64" s="3"/>
+      <c r="N64" s="7"/>
+      <c r="O64" s="7"/>
+      <c r="P64" s="7"/>
+      <c r="Q64" s="7"/>
+      <c r="R64" s="7"/>
+      <c r="S64" s="7"/>
+      <c r="T64" s="7"/>
+      <c r="U64" s="7"/>
+      <c r="V64" s="7"/>
+      <c r="W64" s="7"/>
+      <c r="X64" s="7"/>
+    </row>
+    <row r="65" spans="1:26" ht="14.4">
+      <c r="A65" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B65" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="E63" s="7" t="s">
+      <c r="E65" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="F63" s="7">
+      <c r="F65" s="7">
         <v>-1</v>
       </c>
-      <c r="G63" s="7"/>
-      <c r="H63" s="7"/>
-    </row>
-    <row r="64" spans="1:24" s="21" customFormat="1" ht="14.4">
-      <c r="A64" s="20"/>
-      <c r="B64" s="20"/>
-      <c r="E64" s="7"/>
-      <c r="F64" s="7"/>
-      <c r="G64" s="7"/>
-      <c r="H64" s="7"/>
-    </row>
-    <row r="65" spans="1:26" ht="14.4">
-      <c r="A65" s="15"/>
-      <c r="B65" s="15"/>
-      <c r="C65" s="7" t="s">
+      <c r="G65" s="7"/>
+      <c r="H65" s="7"/>
+    </row>
+    <row r="66" spans="1:26" s="21" customFormat="1" ht="14.4">
+      <c r="A66" s="20"/>
+      <c r="B66" s="20"/>
+      <c r="E66" s="7"/>
+      <c r="F66" s="7"/>
+      <c r="G66" s="7"/>
+      <c r="H66" s="7"/>
+    </row>
+    <row r="67" spans="1:26" ht="14.4">
+      <c r="A67" s="15"/>
+      <c r="B67" s="15"/>
+      <c r="C67" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="D65" s="7" t="s">
+      <c r="D67" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="E65" s="7" t="s">
+      <c r="E67" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="F65" s="7">
+      <c r="F67" s="7">
         <v>0.6</v>
       </c>
-      <c r="G65" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="H65" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="I65" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="J65" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="K65" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="L65" s="7"/>
-      <c r="M65" s="7"/>
-      <c r="N65" s="7"/>
-      <c r="O65" s="7"/>
-      <c r="P65" s="7"/>
-      <c r="Q65" s="7"/>
-      <c r="R65" s="7"/>
-      <c r="S65" s="7"/>
-      <c r="T65" s="7"/>
-      <c r="U65" s="7"/>
-      <c r="V65" s="7"/>
-      <c r="W65" s="7"/>
-      <c r="X65" s="7"/>
-      <c r="Y65" s="7"/>
-      <c r="Z65" s="7"/>
-    </row>
-    <row r="66" spans="1:26" ht="14.4">
-      <c r="A66" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B66" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="E66" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="F66" s="7">
-        <v>1739.927555</v>
-      </c>
-      <c r="G66" s="7"/>
-      <c r="H66" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="K66" s="3" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="67" spans="1:26" s="21" customFormat="1" ht="14.4">
-      <c r="A67" s="20"/>
-      <c r="B67" s="20"/>
-      <c r="E67" s="7" t="s">
-        <v>856</v>
-      </c>
-      <c r="F67" s="7"/>
       <c r="G67" s="7" t="s">
         <v>29</v>
       </c>
       <c r="H67" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="I67" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="J67" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="K67" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="L67" s="7"/>
+      <c r="M67" s="7"/>
+      <c r="N67" s="7"/>
+      <c r="O67" s="7"/>
+      <c r="P67" s="7"/>
+      <c r="Q67" s="7"/>
+      <c r="R67" s="7"/>
+      <c r="S67" s="7"/>
+      <c r="T67" s="7"/>
+      <c r="U67" s="7"/>
+      <c r="V67" s="7"/>
+      <c r="W67" s="7"/>
+      <c r="X67" s="7"/>
+      <c r="Y67" s="7"/>
+      <c r="Z67" s="7"/>
+    </row>
+    <row r="68" spans="1:26" ht="14.4">
+      <c r="A68" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B68" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="E68" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="F68" s="7">
+        <v>1739.927555</v>
+      </c>
+      <c r="G68" s="7"/>
+      <c r="H68" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="K68" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="69" spans="1:26" s="21" customFormat="1" ht="14.4">
+      <c r="A69" s="20"/>
+      <c r="B69" s="20"/>
+      <c r="E69" s="7" t="s">
+        <v>498</v>
+      </c>
+      <c r="F69" s="7"/>
+      <c r="G69" s="7"/>
+      <c r="H69" s="7"/>
+      <c r="K69" s="3" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="70" spans="1:26" s="21" customFormat="1" ht="14.4">
+      <c r="A70" s="20"/>
+      <c r="B70" s="20"/>
+      <c r="E70" s="7" t="s">
+        <v>856</v>
+      </c>
+      <c r="F70" s="7"/>
+      <c r="G70" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H70" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="I67" s="21" t="s">
+      <c r="I70" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="J67" s="21" t="s">
+      <c r="J70" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="K67" s="21" t="s">
+      <c r="K70" s="21" t="s">
         <v>858</v>
       </c>
-      <c r="L67" s="3" t="s">
+      <c r="L70" s="3" t="s">
         <v>857</v>
       </c>
     </row>
-    <row r="68" spans="1:26" s="21" customFormat="1" ht="14.4">
-      <c r="A68" s="20"/>
-      <c r="B68" s="20"/>
-      <c r="E68" s="7" t="s">
+    <row r="71" spans="1:26" s="21" customFormat="1" ht="14.4">
+      <c r="A71" s="20"/>
+      <c r="B71" s="20"/>
+      <c r="E71" s="7" t="s">
         <v>921</v>
       </c>
-      <c r="F68" s="7"/>
-      <c r="G68" s="7" t="s">
+      <c r="F71" s="7"/>
+      <c r="G71" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="H68" s="7" t="s">
+      <c r="H71" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="I68" s="21" t="s">
+      <c r="I71" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="J68" s="21" t="s">
+      <c r="J71" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="K68" s="21" t="s">
+      <c r="K71" s="21" t="s">
         <v>906</v>
       </c>
-      <c r="L68" s="3" t="s">
+      <c r="L71" s="3" t="s">
         <v>857</v>
       </c>
-    </row>
-    <row r="69" spans="1:26" ht="14.4">
-      <c r="A69" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B69" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="C69" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E69" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="F69" s="7">
-        <v>1</v>
-      </c>
-      <c r="G69" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="H69" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="I69" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="J69" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="K69" s="3" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="70" spans="1:26" ht="14.4">
-      <c r="A70" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B70" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="E70" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="F70" s="7">
-        <v>553659</v>
-      </c>
-      <c r="G70" s="7"/>
-      <c r="H70" s="7"/>
-    </row>
-    <row r="71" spans="1:26" ht="14.4">
-      <c r="A71" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B71" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="E71" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="F71" s="7">
-        <v>4891208</v>
-      </c>
-      <c r="G71" s="7"/>
-      <c r="H71" s="7"/>
     </row>
     <row r="72" spans="1:26" ht="14.4">
       <c r="A72" s="15" t="s">
@@ -22380,7 +22392,7 @@
         <v>24</v>
       </c>
       <c r="E72" s="7" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="F72" s="7">
         <v>1</v>
@@ -22389,7 +22401,7 @@
         <v>46</v>
       </c>
       <c r="H72" s="7" t="s">
-        <v>33</v>
+        <v>117</v>
       </c>
       <c r="I72" s="3" t="s">
         <v>34</v>
@@ -22398,46 +22410,24 @@
         <v>30</v>
       </c>
       <c r="K72" s="3" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="73" spans="1:26" s="21" customFormat="1" ht="14.4">
-      <c r="A73" s="20" t="s">
-        <v>838</v>
-      </c>
-      <c r="B73" s="20" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="73" spans="1:26" ht="14.4">
+      <c r="A73" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B73" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="C73" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="D73" s="21" t="s">
-        <v>65</v>
-      </c>
       <c r="E73" s="7" t="s">
-        <v>837</v>
+        <v>119</v>
       </c>
       <c r="F73" s="7">
-        <v>5</v>
-      </c>
-      <c r="G73" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="H73" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="I73" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="J73" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="K73" s="3" t="s">
-        <v>839</v>
-      </c>
-      <c r="L73" s="23" t="s">
-        <v>65</v>
-      </c>
+        <v>553659</v>
+      </c>
+      <c r="G73" s="7"/>
+      <c r="H73" s="7"/>
     </row>
     <row r="74" spans="1:26" ht="14.4">
       <c r="A74" s="15" t="s">
@@ -22446,340 +22436,499 @@
       <c r="B74" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="D74" s="3" t="s">
-        <v>128</v>
-      </c>
       <c r="E74" s="7" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="F74" s="7">
-        <v>0</v>
+        <v>4891208</v>
       </c>
       <c r="G74" s="7"/>
-      <c r="H74" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="I74" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="J74" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="K74" s="3" t="s">
-        <v>131</v>
-      </c>
+      <c r="H74" s="7"/>
     </row>
     <row r="75" spans="1:26" ht="14.4">
       <c r="A75" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="B75" s="15"/>
+      <c r="B75" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C75" s="3" t="s">
+        <v>24</v>
+      </c>
       <c r="E75" s="7" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="F75" s="7">
-        <v>6772</v>
-      </c>
-      <c r="G75" s="7"/>
-      <c r="H75" s="7"/>
+        <v>1</v>
+      </c>
+      <c r="G75" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="H75" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="I75" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="J75" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="K75" s="3" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="76" spans="1:26" s="21" customFormat="1" ht="14.4">
       <c r="A76" s="20"/>
       <c r="B76" s="20"/>
+      <c r="C76" s="3"/>
       <c r="E76" s="7" t="s">
-        <v>844</v>
-      </c>
-      <c r="F76" s="7">
-        <v>1</v>
-      </c>
-      <c r="G76" s="7" t="s">
-        <v>110</v>
-      </c>
+        <v>938</v>
+      </c>
+      <c r="F76" s="7"/>
+      <c r="G76" s="7"/>
       <c r="H76" s="7" t="s">
-        <v>845</v>
-      </c>
-      <c r="I76" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="J76" s="23" t="s">
-        <v>846</v>
+        <v>130</v>
+      </c>
+      <c r="I76" s="3"/>
+      <c r="J76" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K76" s="3" t="s">
+        <v>940</v>
       </c>
     </row>
     <row r="77" spans="1:26" s="21" customFormat="1" ht="14.4">
-      <c r="A77" s="20"/>
-      <c r="B77" s="20"/>
+      <c r="A77" s="20" t="s">
+        <v>838</v>
+      </c>
+      <c r="B77" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="C77" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="D77" s="21" t="s">
+        <v>65</v>
+      </c>
       <c r="E77" s="7" t="s">
-        <v>843</v>
+        <v>837</v>
       </c>
       <c r="F77" s="7">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G77" s="7" t="s">
         <v>110</v>
       </c>
       <c r="H77" s="7" t="s">
-        <v>627</v>
-      </c>
-      <c r="I77" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="I77" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="J77" s="23" t="s">
+      <c r="J77" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="K77" s="23" t="s">
-        <v>849</v>
-      </c>
-    </row>
-    <row r="78" spans="1:26" s="21" customFormat="1" ht="14.4">
-      <c r="A78" s="20"/>
-      <c r="B78" s="20"/>
-      <c r="D78" s="57" t="s">
-        <v>25</v>
+      <c r="K77" s="3" t="s">
+        <v>839</v>
+      </c>
+      <c r="L77" s="23" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="78" spans="1:26" ht="14.4">
+      <c r="A78" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B78" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D78" s="3" t="s">
+        <v>128</v>
       </c>
       <c r="E78" s="7" t="s">
-        <v>797</v>
-      </c>
-      <c r="F78" s="7"/>
-      <c r="G78" s="58" t="s">
-        <v>29</v>
-      </c>
+        <v>129</v>
+      </c>
+      <c r="F78" s="7">
+        <v>0</v>
+      </c>
+      <c r="G78" s="7"/>
       <c r="H78" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="I78" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="I78" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="J78" s="23" t="s">
+      <c r="J78" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="K78" s="23" t="s">
-        <v>798</v>
+      <c r="K78" s="3" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="79" spans="1:26" s="21" customFormat="1" ht="14.4">
-      <c r="A79" s="20" t="s">
-        <v>23</v>
-      </c>
+      <c r="A79" s="20"/>
       <c r="B79" s="20"/>
-      <c r="D79" s="57" t="s">
-        <v>25</v>
-      </c>
+      <c r="D79" s="3"/>
       <c r="E79" s="7" t="s">
-        <v>799</v>
+        <v>939</v>
       </c>
       <c r="F79" s="7"/>
-      <c r="G79" s="58" t="s">
-        <v>29</v>
-      </c>
+      <c r="G79" s="7"/>
       <c r="H79" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="I79" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="J79" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="K79" s="23" t="s">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="80" spans="1:26" ht="14.4">
-      <c r="A80" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B80" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="D80" s="17" t="s">
-        <v>134</v>
-      </c>
-      <c r="E80" s="18" t="s">
-        <v>136</v>
-      </c>
-      <c r="F80" s="18">
-        <v>1500</v>
-      </c>
-      <c r="G80" s="18" t="s">
-        <v>110</v>
-      </c>
-      <c r="H80" s="18" t="s">
-        <v>84</v>
-      </c>
-      <c r="I80" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="J80" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="K80" s="17" t="s">
-        <v>139</v>
+        <v>130</v>
+      </c>
+      <c r="I79" s="3"/>
+      <c r="J79" s="3"/>
+      <c r="K79" s="3" t="s">
+        <v>941</v>
+      </c>
+    </row>
+    <row r="80" spans="1:26" s="21" customFormat="1" ht="14.4">
+      <c r="A80" s="20"/>
+      <c r="B80" s="20"/>
+      <c r="D80" s="3"/>
+      <c r="E80" s="7" t="s">
+        <v>942</v>
+      </c>
+      <c r="F80" s="7"/>
+      <c r="G80" s="7"/>
+      <c r="H80" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="I80" s="3"/>
+      <c r="J80" s="3"/>
+      <c r="K80" s="3" t="s">
+        <v>943</v>
       </c>
     </row>
     <row r="81" spans="1:11" ht="14.4">
       <c r="A81" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="B81" s="16" t="s">
+      <c r="B81" s="15"/>
+      <c r="E81" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="F81" s="7">
+        <v>6772</v>
+      </c>
+      <c r="G81" s="7"/>
+      <c r="H81" s="7"/>
+    </row>
+    <row r="82" spans="1:11" s="21" customFormat="1" ht="14.4">
+      <c r="A82" s="20"/>
+      <c r="B82" s="20"/>
+      <c r="E82" s="7" t="s">
+        <v>844</v>
+      </c>
+      <c r="F82" s="7">
+        <v>1</v>
+      </c>
+      <c r="G82" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="H82" s="7" t="s">
+        <v>845</v>
+      </c>
+      <c r="I82" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="J82" s="23" t="s">
+        <v>846</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" s="21" customFormat="1" ht="14.4">
+      <c r="A83" s="20"/>
+      <c r="B83" s="20"/>
+      <c r="E83" s="7" t="s">
+        <v>843</v>
+      </c>
+      <c r="F83" s="7">
+        <v>10</v>
+      </c>
+      <c r="G83" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="H83" s="7" t="s">
+        <v>627</v>
+      </c>
+      <c r="I83" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="J83" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="K83" s="23" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" s="21" customFormat="1" ht="14.4">
+      <c r="A84" s="20"/>
+      <c r="B84" s="20"/>
+      <c r="E84" s="7" t="s">
+        <v>511</v>
+      </c>
+      <c r="F84" s="7"/>
+      <c r="G84" s="7"/>
+      <c r="H84" s="7" t="s">
+        <v>512</v>
+      </c>
+      <c r="I84" s="23"/>
+      <c r="J84" s="23"/>
+      <c r="K84" s="23" t="s">
+        <v>947</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" s="21" customFormat="1" ht="14.4">
+      <c r="A85" s="20"/>
+      <c r="B85" s="20"/>
+      <c r="D85" s="57" t="s">
+        <v>25</v>
+      </c>
+      <c r="E85" s="7" t="s">
+        <v>797</v>
+      </c>
+      <c r="F85" s="7"/>
+      <c r="G85" s="58" t="s">
+        <v>29</v>
+      </c>
+      <c r="H85" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="I85" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="J85" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="K85" s="23" t="s">
+        <v>798</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" s="21" customFormat="1" ht="14.4">
+      <c r="A86" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="B86" s="20"/>
+      <c r="D86" s="57" t="s">
+        <v>25</v>
+      </c>
+      <c r="E86" s="7" t="s">
+        <v>799</v>
+      </c>
+      <c r="F86" s="7"/>
+      <c r="G86" s="58" t="s">
+        <v>29</v>
+      </c>
+      <c r="H86" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="I86" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="J86" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="K86" s="23" t="s">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11" ht="14.4">
+      <c r="A87" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B87" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="D81" s="17" t="s">
+      <c r="D87" s="17" t="s">
         <v>134</v>
       </c>
-      <c r="E81" s="17" t="s">
+      <c r="E87" s="18" t="s">
+        <v>136</v>
+      </c>
+      <c r="F87" s="18">
+        <v>1500</v>
+      </c>
+      <c r="G87" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="H87" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="I87" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="J87" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="K87" s="17" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11" ht="14.4">
+      <c r="A88" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B88" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="D88" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="E88" s="17" t="s">
         <v>141</v>
       </c>
-      <c r="F81" s="17">
+      <c r="F88" s="17">
         <v>1500</v>
       </c>
-      <c r="G81" s="18" t="s">
+      <c r="G88" s="18" t="s">
         <v>110</v>
       </c>
-      <c r="H81" s="17" t="s">
+      <c r="H88" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="I81" s="17" t="s">
+      <c r="I88" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="J81" s="17" t="s">
+      <c r="J88" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="K81" s="17" t="s">
+      <c r="K88" s="17" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="82" spans="1:11" ht="14.4">
-      <c r="A82" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B82" s="16" t="s">
+    <row r="89" spans="1:11" ht="14.4">
+      <c r="A89" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B89" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="D82" s="17" t="s">
+      <c r="D89" s="17" t="s">
         <v>134</v>
       </c>
-      <c r="E82" s="17" t="s">
+      <c r="E89" s="17" t="s">
         <v>144</v>
       </c>
-      <c r="F82" s="17">
+      <c r="F89" s="17">
         <v>1500</v>
       </c>
-      <c r="G82" s="18" t="s">
+      <c r="G89" s="18" t="s">
         <v>110</v>
       </c>
-      <c r="H82" s="17" t="s">
+      <c r="H89" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="I82" s="17" t="s">
+      <c r="I89" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="J82" s="17" t="s">
+      <c r="J89" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="K82" s="17" t="s">
+      <c r="K89" s="17" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="83" spans="1:11" ht="14.4">
-      <c r="A83" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B83" s="16" t="s">
+    <row r="90" spans="1:11" ht="14.4">
+      <c r="A90" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B90" s="16" t="s">
         <v>146</v>
       </c>
-      <c r="D83" s="17" t="s">
+      <c r="D90" s="17" t="s">
         <v>134</v>
       </c>
-      <c r="E83" s="17" t="s">
+      <c r="E90" s="17" t="s">
         <v>147</v>
       </c>
-      <c r="F83" s="17">
+      <c r="F90" s="17">
         <v>1000</v>
       </c>
-      <c r="G83" s="18" t="s">
+      <c r="G90" s="18" t="s">
         <v>110</v>
       </c>
-      <c r="H83" s="17" t="s">
+      <c r="H90" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="I83" s="17" t="s">
+      <c r="I90" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="J83" s="17" t="s">
+      <c r="J90" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="K83" s="17" t="s">
+      <c r="K90" s="17" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="84" spans="1:11" ht="14.4">
-      <c r="A84" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B84" s="16" t="s">
+    <row r="91" spans="1:11" ht="14.4">
+      <c r="A91" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B91" s="16" t="s">
         <v>146</v>
       </c>
-      <c r="D84" s="17" t="s">
+      <c r="D91" s="17" t="s">
         <v>134</v>
       </c>
-      <c r="E84" s="17" t="s">
+      <c r="E91" s="17" t="s">
         <v>149</v>
       </c>
-      <c r="F84" s="17">
+      <c r="F91" s="17">
         <v>1000</v>
       </c>
-      <c r="G84" s="18" t="s">
+      <c r="G91" s="18" t="s">
         <v>110</v>
       </c>
-      <c r="H84" s="17" t="s">
+      <c r="H91" s="17" t="s">
         <v>107</v>
       </c>
-      <c r="I84" s="17" t="s">
+      <c r="I91" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="J84" s="17" t="s">
+      <c r="J91" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="K84" s="17" t="s">
+      <c r="K91" s="17" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="85" spans="1:11" ht="14.4">
-      <c r="A85" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B85" s="16" t="s">
+    <row r="92" spans="1:11" ht="14.4">
+      <c r="A92" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B92" s="16" t="s">
         <v>146</v>
       </c>
-      <c r="D85" s="17" t="s">
+      <c r="D92" s="17" t="s">
         <v>134</v>
       </c>
-      <c r="E85" s="17" t="s">
+      <c r="E92" s="17" t="s">
         <v>151</v>
       </c>
-      <c r="F85" s="17">
+      <c r="F92" s="17">
         <v>1000</v>
       </c>
-      <c r="G85" s="18" t="s">
+      <c r="G92" s="18" t="s">
         <v>110</v>
       </c>
-      <c r="H85" s="17" t="s">
+      <c r="H92" s="17" t="s">
         <v>107</v>
       </c>
-      <c r="I85" s="17" t="s">
+      <c r="I92" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="J85" s="17" t="s">
+      <c r="J92" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="K85" s="17" t="s">
+      <c r="K92" s="17" t="s">
         <v>152</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B53:B56">
+  <conditionalFormatting sqref="B55:B58">
     <cfRule type="notContainsBlanks" dxfId="0" priority="1">
-      <formula>LEN(TRIM(B53))&gt;0</formula>
+      <formula>LEN(TRIM(B55))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Continue to add logic for Shade-a-lator testing. CW3MdataDictionary.xlsx - Add Reach attribute WIDTHGIVEN. Reach_McKenzie.dbf - Add Reach attributes  WIDTHGIVEN, TOPOELEV_E, S, W, and VEG_HT_R and L. Flow.cpp, .h - Add code to read the Shade-a-lator input data file and populate WIDTHGIVEN, TOPOELEV_E, S, W, and VEG_HT_R and L.
</commit_message>
<xml_diff>
--- a/DataCW3M/CW3MdigitalHandbook/CW3MdataDictionary.xlsx
+++ b/DataCW3M/CW3MdigitalHandbook/CW3MdataDictionary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\CW3MdigitalHandbook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4CCAA7E-877A-4680-99CD-40447C08EFDB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABAC855E-C17E-4B2D-9B3C-02EDC60D5FEB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -96,7 +96,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2902" uniqueCount="963">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2909" uniqueCount="966">
   <si>
     <t>LULC_A</t>
   </si>
@@ -2986,6 +2986,15 @@
   </si>
   <si>
     <t>Slength</t>
+  </si>
+  <si>
+    <t>WIDTHGIVEN</t>
+  </si>
+  <si>
+    <t>prescribed stream width, may be calculated from Shade-a-lator input data</t>
+  </si>
+  <si>
+    <t>1/27/21 - Added WIDTHGIVEN.</t>
   </si>
 </sst>
 </file>
@@ -20650,11 +20659,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Z92"/>
+  <dimension ref="A1:Z94"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K66" sqref="K66"/>
+      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -20699,127 +20708,117 @@
       <c r="W1" s="7"/>
       <c r="X1" s="7"/>
     </row>
-    <row r="2" spans="1:26" s="91" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A2" s="87" t="s">
+    <row r="2" spans="1:26" s="57" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A2" s="70" t="s">
+        <v>965</v>
+      </c>
+      <c r="B2" s="69"/>
+      <c r="C2" s="69"/>
+      <c r="D2" s="69"/>
+      <c r="E2" s="58"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="70"/>
+      <c r="H2" s="70"/>
+      <c r="I2" s="79"/>
+      <c r="J2" s="79"/>
+      <c r="K2" s="58"/>
+      <c r="L2" s="70"/>
+      <c r="M2" s="58"/>
+      <c r="N2" s="58"/>
+      <c r="O2" s="58"/>
+      <c r="P2" s="58"/>
+      <c r="Q2" s="58"/>
+      <c r="R2" s="58"/>
+      <c r="S2" s="58"/>
+      <c r="T2" s="58"/>
+      <c r="U2" s="58"/>
+      <c r="V2" s="58"/>
+      <c r="W2" s="58"/>
+      <c r="X2" s="58"/>
+    </row>
+    <row r="3" spans="1:26" s="91" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A3" s="87" t="s">
         <v>961</v>
       </c>
-      <c r="B2" s="88"/>
-      <c r="C2" s="89"/>
-      <c r="D2" s="89"/>
-      <c r="E2" s="89"/>
-      <c r="F2" s="89"/>
-      <c r="G2" s="89"/>
-      <c r="H2" s="89"/>
-      <c r="I2" s="90"/>
-      <c r="J2" s="90"/>
-      <c r="K2" s="89"/>
-      <c r="L2" s="89"/>
-      <c r="M2" s="89"/>
-      <c r="N2" s="89"/>
-      <c r="O2" s="89"/>
-      <c r="P2" s="89"/>
-      <c r="Q2" s="89"/>
-      <c r="R2" s="89"/>
-      <c r="S2" s="89"/>
-      <c r="T2" s="89"/>
-      <c r="U2" s="89"/>
-      <c r="V2" s="89"/>
-      <c r="W2" s="89"/>
-      <c r="X2" s="89"/>
-      <c r="Y2" s="89"/>
-      <c r="Z2" s="89"/>
-    </row>
-    <row r="3" spans="1:26" ht="59.25" customHeight="1">
-      <c r="A3" s="13" t="s">
+      <c r="B3" s="88"/>
+      <c r="C3" s="89"/>
+      <c r="D3" s="89"/>
+      <c r="E3" s="89"/>
+      <c r="F3" s="89"/>
+      <c r="G3" s="89"/>
+      <c r="H3" s="89"/>
+      <c r="I3" s="90"/>
+      <c r="J3" s="90"/>
+      <c r="K3" s="89"/>
+      <c r="L3" s="89"/>
+      <c r="M3" s="89"/>
+      <c r="N3" s="89"/>
+      <c r="O3" s="89"/>
+      <c r="P3" s="89"/>
+      <c r="Q3" s="89"/>
+      <c r="R3" s="89"/>
+      <c r="S3" s="89"/>
+      <c r="T3" s="89"/>
+      <c r="U3" s="89"/>
+      <c r="V3" s="89"/>
+      <c r="W3" s="89"/>
+      <c r="X3" s="89"/>
+      <c r="Y3" s="89"/>
+      <c r="Z3" s="89"/>
+    </row>
+    <row r="4" spans="1:26" ht="59.25" customHeight="1">
+      <c r="A4" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B4" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C4" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D4" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="E4" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F4" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G4" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="H4" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="9" t="s">
+      <c r="I4" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="J3" s="9" t="s">
+      <c r="J4" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="K3" s="14" t="s">
+      <c r="K4" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="L3" s="9" t="s">
+      <c r="L4" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="M3" s="14" t="s">
+      <c r="M4" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="N3" s="7" t="s">
+      <c r="N4" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="O3" s="14"/>
-      <c r="P3" s="14"/>
-      <c r="Q3" s="14"/>
-      <c r="R3" s="14"/>
-      <c r="S3" s="14"/>
-      <c r="T3" s="14"/>
-      <c r="U3" s="14"/>
-      <c r="V3" s="14"/>
-      <c r="W3" s="14"/>
-      <c r="X3" s="14"/>
-    </row>
-    <row r="4" spans="1:26" s="21" customFormat="1" ht="14.4">
-      <c r="A4" s="13"/>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="72" t="s">
-        <v>926</v>
-      </c>
-      <c r="F4" s="10"/>
-      <c r="G4" s="70" t="s">
-        <v>109</v>
-      </c>
-      <c r="H4" s="70" t="s">
-        <v>73</v>
-      </c>
-      <c r="I4" s="79" t="s">
-        <v>26</v>
-      </c>
-      <c r="J4" s="79" t="s">
-        <v>27</v>
-      </c>
-      <c r="K4" s="57" t="s">
-        <v>929</v>
-      </c>
-      <c r="L4" s="9"/>
-      <c r="M4" s="25"/>
-      <c r="N4" s="7"/>
-      <c r="O4" s="25"/>
-      <c r="P4" s="25"/>
-      <c r="Q4" s="25"/>
-      <c r="R4" s="25"/>
-      <c r="S4" s="25"/>
-      <c r="T4" s="25"/>
-      <c r="U4" s="25"/>
-      <c r="V4" s="25"/>
-      <c r="W4" s="25"/>
-      <c r="X4" s="25"/>
+      <c r="O4" s="14"/>
+      <c r="P4" s="14"/>
+      <c r="Q4" s="14"/>
+      <c r="R4" s="14"/>
+      <c r="S4" s="14"/>
+      <c r="T4" s="14"/>
+      <c r="U4" s="14"/>
+      <c r="V4" s="14"/>
+      <c r="W4" s="14"/>
+      <c r="X4" s="14"/>
     </row>
     <row r="5" spans="1:26" s="21" customFormat="1" ht="14.4">
       <c r="A5" s="13"/>
@@ -20827,14 +20826,14 @@
       <c r="C5" s="13"/>
       <c r="D5" s="13"/>
       <c r="E5" s="72" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F5" s="10"/>
       <c r="G5" s="70" t="s">
         <v>109</v>
       </c>
       <c r="H5" s="70" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="I5" s="79" t="s">
         <v>26</v>
@@ -20843,7 +20842,7 @@
         <v>27</v>
       </c>
       <c r="K5" s="57" t="s">
-        <v>928</v>
+        <v>929</v>
       </c>
       <c r="L5" s="9"/>
       <c r="M5" s="25"/>
@@ -20865,14 +20864,14 @@
       <c r="C6" s="13"/>
       <c r="D6" s="13"/>
       <c r="E6" s="72" t="s">
-        <v>930</v>
+        <v>927</v>
       </c>
       <c r="F6" s="10"/>
       <c r="G6" s="70" t="s">
         <v>109</v>
       </c>
       <c r="H6" s="70" t="s">
-        <v>129</v>
+        <v>95</v>
       </c>
       <c r="I6" s="79" t="s">
         <v>26</v>
@@ -20880,8 +20879,8 @@
       <c r="J6" s="79" t="s">
         <v>27</v>
       </c>
-      <c r="K6" s="70" t="s">
-        <v>931</v>
+      <c r="K6" s="57" t="s">
+        <v>928</v>
       </c>
       <c r="L6" s="9"/>
       <c r="M6" s="25"/>
@@ -20897,59 +20896,76 @@
       <c r="W6" s="25"/>
       <c r="X6" s="25"/>
     </row>
-    <row r="7" spans="1:26" s="83" customFormat="1" ht="14.4">
-      <c r="A7" s="82"/>
-      <c r="B7" s="82"/>
-      <c r="D7" s="84" t="s">
+    <row r="7" spans="1:26" s="21" customFormat="1" ht="14.4">
+      <c r="A7" s="13"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="72" t="s">
+        <v>930</v>
+      </c>
+      <c r="F7" s="10"/>
+      <c r="G7" s="70" t="s">
+        <v>109</v>
+      </c>
+      <c r="H7" s="70" t="s">
+        <v>129</v>
+      </c>
+      <c r="I7" s="79" t="s">
+        <v>26</v>
+      </c>
+      <c r="J7" s="79" t="s">
+        <v>27</v>
+      </c>
+      <c r="K7" s="70" t="s">
+        <v>931</v>
+      </c>
+      <c r="L7" s="9"/>
+      <c r="M7" s="25"/>
+      <c r="N7" s="7"/>
+      <c r="O7" s="25"/>
+      <c r="P7" s="25"/>
+      <c r="Q7" s="25"/>
+      <c r="R7" s="25"/>
+      <c r="S7" s="25"/>
+      <c r="T7" s="25"/>
+      <c r="U7" s="25"/>
+      <c r="V7" s="25"/>
+      <c r="W7" s="25"/>
+      <c r="X7" s="25"/>
+    </row>
+    <row r="8" spans="1:26" s="83" customFormat="1" ht="14.4">
+      <c r="A8" s="82"/>
+      <c r="B8" s="82"/>
+      <c r="D8" s="84" t="s">
         <v>897</v>
       </c>
-      <c r="E7" s="84" t="s">
+      <c r="E8" s="84" t="s">
         <v>850</v>
       </c>
-      <c r="F7" s="84">
+      <c r="F8" s="84">
         <v>5.2</v>
       </c>
-      <c r="G7" s="84"/>
-      <c r="H7" s="84" t="s">
+      <c r="G8" s="84"/>
+      <c r="H8" s="84" t="s">
         <v>109</v>
       </c>
-      <c r="I7" s="84" t="s">
+      <c r="I8" s="84" t="s">
         <v>26</v>
       </c>
-      <c r="J7" s="84" t="s">
+      <c r="J8" s="84" t="s">
         <v>27</v>
       </c>
-      <c r="K7" s="83" t="s">
+      <c r="K8" s="83" t="s">
         <v>849</v>
       </c>
-    </row>
-    <row r="8" spans="1:26" s="21" customFormat="1" ht="28.8">
-      <c r="A8" s="20"/>
-      <c r="B8" s="20"/>
-      <c r="C8" s="22"/>
-      <c r="E8" s="21" t="s">
-        <v>895</v>
-      </c>
-      <c r="G8" s="21" t="s">
-        <v>46</v>
-      </c>
-      <c r="H8" s="21" t="s">
-        <v>898</v>
-      </c>
-      <c r="J8" s="23" t="s">
-        <v>30</v>
-      </c>
-      <c r="K8" s="80" t="s">
-        <v>899</v>
-      </c>
-      <c r="L8" s="22"/>
     </row>
     <row r="9" spans="1:26" s="21" customFormat="1" ht="28.8">
       <c r="A9" s="20"/>
       <c r="B9" s="20"/>
       <c r="C9" s="22"/>
       <c r="E9" s="21" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="G9" s="21" t="s">
         <v>46</v>
@@ -20961,7 +20977,7 @@
         <v>30</v>
       </c>
       <c r="K9" s="80" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="L9" s="22"/>
     </row>
@@ -20969,49 +20985,54 @@
       <c r="A10" s="20"/>
       <c r="B10" s="20"/>
       <c r="C10" s="22"/>
-      <c r="D10" s="57" t="s">
+      <c r="E10" s="21" t="s">
+        <v>896</v>
+      </c>
+      <c r="G10" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="H10" s="21" t="s">
+        <v>898</v>
+      </c>
+      <c r="J10" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="K10" s="80" t="s">
+        <v>900</v>
+      </c>
+      <c r="L10" s="22"/>
+    </row>
+    <row r="11" spans="1:26" s="21" customFormat="1" ht="28.8">
+      <c r="A11" s="20"/>
+      <c r="B11" s="20"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="57" t="s">
         <v>945</v>
       </c>
-      <c r="E10" s="57" t="s">
+      <c r="E11" s="57" t="s">
         <v>946</v>
       </c>
-      <c r="F10" s="21">
+      <c r="F11" s="21">
         <v>36</v>
       </c>
-      <c r="G10" s="57" t="s">
+      <c r="G11" s="57" t="s">
         <v>109</v>
       </c>
-      <c r="H10" s="57" t="s">
+      <c r="H11" s="57" t="s">
         <v>227</v>
       </c>
-      <c r="I10" s="57" t="s">
+      <c r="I11" s="57" t="s">
         <v>948</v>
       </c>
-      <c r="J10" s="23" t="s">
+      <c r="J11" s="23" t="s">
         <v>947</v>
       </c>
-      <c r="K10" s="80" t="s">
+      <c r="K11" s="80" t="s">
         <v>949</v>
       </c>
-      <c r="L10" s="23" t="s">
+      <c r="L11" s="23" t="s">
         <v>950</v>
       </c>
-    </row>
-    <row r="11" spans="1:26" ht="14.4">
-      <c r="A11" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B11" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="F11" s="7">
-        <v>3220</v>
-      </c>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
     </row>
     <row r="12" spans="1:26" ht="14.4">
       <c r="A12" s="15" t="s">
@@ -21020,28 +21041,14 @@
       <c r="B12" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>24</v>
-      </c>
       <c r="E12" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F12" s="7">
-        <v>23773405</v>
+        <v>3220</v>
       </c>
       <c r="G12" s="7"/>
-      <c r="H12" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="I12" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="J12" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="K12" s="7" t="s">
-        <v>35</v>
-      </c>
+      <c r="H12" s="7"/>
     </row>
     <row r="13" spans="1:26" ht="14.4">
       <c r="A13" s="15" t="s">
@@ -21050,14 +21057,28 @@
       <c r="B13" s="15" t="s">
         <v>24</v>
       </c>
+      <c r="C13" s="3" t="s">
+        <v>24</v>
+      </c>
       <c r="E13" s="7" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="F13" s="7">
-        <v>23773403</v>
+        <v>23773405</v>
       </c>
       <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
+      <c r="H13" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="I13" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="J13" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="K13" s="7" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="14" spans="1:26" ht="14.4">
       <c r="A14" s="15" t="s">
@@ -21067,10 +21088,10 @@
         <v>24</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F14" s="7">
-        <v>23773407</v>
+        <v>23773403</v>
       </c>
       <c r="G14" s="7"/>
       <c r="H14" s="7"/>
@@ -21083,10 +21104,10 @@
         <v>24</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F15" s="7">
-        <v>0</v>
+        <v>23773407</v>
       </c>
       <c r="G15" s="7"/>
       <c r="H15" s="7"/>
@@ -21098,11 +21119,8 @@
       <c r="B16" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="D16" s="3" t="s">
-        <v>39</v>
-      </c>
       <c r="E16" s="7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F16" s="7">
         <v>0</v>
@@ -21121,7 +21139,7 @@
         <v>39</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F17" s="7">
         <v>0</v>
@@ -21137,10 +21155,10 @@
         <v>24</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F18" s="7">
         <v>0</v>
@@ -21148,73 +21166,73 @@
       <c r="G18" s="7"/>
       <c r="H18" s="7"/>
     </row>
-    <row r="19" spans="1:26" s="21" customFormat="1" ht="14.4">
-      <c r="A19" s="20"/>
-      <c r="B19" s="20"/>
-      <c r="D19" s="3"/>
+    <row r="19" spans="1:26" ht="14.4">
+      <c r="A19" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>42</v>
+      </c>
       <c r="E19" s="7" t="s">
-        <v>846</v>
+        <v>43</v>
       </c>
       <c r="F19" s="7">
-        <v>1</v>
-      </c>
-      <c r="G19" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="H19" s="7" t="s">
-        <v>626</v>
-      </c>
-      <c r="I19" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="J19" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="K19" s="21" t="s">
-        <v>847</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
     </row>
     <row r="20" spans="1:26" s="21" customFormat="1" ht="14.4">
       <c r="A20" s="20"/>
       <c r="B20" s="20"/>
       <c r="D20" s="3"/>
       <c r="E20" s="7" t="s">
-        <v>901</v>
+        <v>846</v>
       </c>
       <c r="F20" s="7">
-        <v>90</v>
+        <v>1</v>
       </c>
       <c r="G20" s="7" t="s">
         <v>109</v>
       </c>
       <c r="H20" s="7" t="s">
+        <v>626</v>
+      </c>
+      <c r="I20" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="J20" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="K20" s="21" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="21" spans="1:26" s="21" customFormat="1" ht="14.4">
+      <c r="A21" s="20"/>
+      <c r="B21" s="20"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="7" t="s">
+        <v>901</v>
+      </c>
+      <c r="F21" s="7">
+        <v>90</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="H21" s="7" t="s">
         <v>902</v>
       </c>
-      <c r="J20" s="21" t="s">
+      <c r="J21" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="K20" s="21" t="s">
+      <c r="K21" s="21" t="s">
         <v>903</v>
       </c>
-    </row>
-    <row r="21" spans="1:26" ht="14.4">
-      <c r="A21" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B21" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E21" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="F21" s="7">
-        <v>6772</v>
-      </c>
-      <c r="G21" s="7"/>
-      <c r="H21" s="7"/>
     </row>
     <row r="22" spans="1:26" ht="14.4">
       <c r="A22" s="15" t="s">
@@ -21223,276 +21241,271 @@
       <c r="B22" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="D22" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="F22" s="7">
+        <v>6772</v>
+      </c>
+      <c r="G22" s="7"/>
+      <c r="H22" s="7"/>
+    </row>
+    <row r="23" spans="1:26" ht="14.4">
+      <c r="A23" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="C23" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D23" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="E22" s="7" t="s">
+      <c r="E23" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="F22" s="7">
+      <c r="F23" s="7">
         <v>7</v>
       </c>
-      <c r="G22" s="7" t="s">
+      <c r="G23" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="H22" s="7" t="s">
+      <c r="H23" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="I22" s="3" t="s">
+      <c r="I23" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="J22" s="3" t="s">
+      <c r="J23" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="K22" s="3" t="s">
+      <c r="K23" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="N22" s="3" t="s">
+      <c r="N23" s="3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="23" spans="1:26" s="21" customFormat="1" ht="14.4">
-      <c r="A23" s="20"/>
-      <c r="B23" s="20"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="7" t="s">
+    <row r="24" spans="1:26" s="21" customFormat="1" ht="14.4">
+      <c r="A24" s="20"/>
+      <c r="B24" s="20"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="7" t="s">
         <v>852</v>
       </c>
-      <c r="F23" s="7">
+      <c r="F24" s="7">
         <v>4.2</v>
       </c>
-      <c r="G23" s="7" t="s">
+      <c r="G24" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="H23" s="7" t="s">
+      <c r="H24" s="7" t="s">
         <v>407</v>
       </c>
-      <c r="I23" s="3" t="s">
+      <c r="I24" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="J23" s="3" t="s">
+      <c r="J24" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="K23" s="3" t="s">
+      <c r="K24" s="3" t="s">
         <v>851</v>
       </c>
-      <c r="N23" s="3"/>
-    </row>
-    <row r="24" spans="1:26" ht="14.4">
-      <c r="A24" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B24" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="D24" t="s">
-        <v>909</v>
-      </c>
-      <c r="E24" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="F24" s="7">
-        <v>0</v>
-      </c>
-      <c r="G24" s="7" t="s">
-        <v>907</v>
-      </c>
-      <c r="H24" s="7"/>
-      <c r="K24" s="23" t="s">
-        <v>908</v>
-      </c>
+      <c r="N24" s="3"/>
     </row>
     <row r="25" spans="1:26" ht="14.4">
       <c r="A25" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="15"/>
+      <c r="B25" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D25" t="s">
+        <v>909</v>
+      </c>
       <c r="E25" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F25" s="7">
-        <v>6713</v>
-      </c>
-      <c r="G25" s="7"/>
+        <v>0</v>
+      </c>
+      <c r="G25" s="7" t="s">
+        <v>907</v>
+      </c>
       <c r="H25" s="7"/>
+      <c r="K25" s="23" t="s">
+        <v>908</v>
+      </c>
     </row>
     <row r="26" spans="1:26" ht="14.4">
       <c r="A26" s="15" t="s">
         <v>23</v>
       </c>
       <c r="B26" s="15"/>
-      <c r="E26" s="58" t="s">
-        <v>53</v>
-      </c>
-      <c r="F26" s="7" t="s">
-        <v>54</v>
+      <c r="E26" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="F26" s="7">
+        <v>6713</v>
       </c>
       <c r="G26" s="7"/>
       <c r="H26" s="7"/>
     </row>
-    <row r="27" spans="1:26" ht="25.2" customHeight="1">
+    <row r="27" spans="1:26" ht="14.4">
       <c r="A27" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="B27" s="15" t="s">
+      <c r="B27" s="15"/>
+      <c r="E27" s="58" t="s">
+        <v>53</v>
+      </c>
+      <c r="F27" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="G27" s="7"/>
+      <c r="H27" s="7"/>
+    </row>
+    <row r="28" spans="1:26" ht="25.2" customHeight="1">
+      <c r="A28" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B28" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="C28" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="E27" s="7" t="s">
+      <c r="E28" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="F27" s="7">
+      <c r="F28" s="7">
         <v>34</v>
       </c>
-      <c r="G27" s="7" t="s">
+      <c r="G28" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="H27" s="7" t="s">
+      <c r="H28" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="K27" s="3" t="s">
+      <c r="K28" s="3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="28" spans="1:26" s="25" customFormat="1" ht="72">
-      <c r="A28" s="81"/>
-      <c r="B28" s="81"/>
-      <c r="C28" s="19"/>
-      <c r="D28" s="19" t="s">
+    <row r="29" spans="1:26" s="25" customFormat="1" ht="72">
+      <c r="A29" s="81"/>
+      <c r="B29" s="81"/>
+      <c r="C29" s="19"/>
+      <c r="D29" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="E28" s="25" t="s">
+      <c r="E29" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="F28" s="85">
+      <c r="F29" s="85">
         <v>6737</v>
       </c>
-      <c r="G28" s="25" t="s">
+      <c r="G29" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="H28" s="86" t="s">
+      <c r="H29" s="86" t="s">
         <v>33</v>
       </c>
-      <c r="I28" s="19"/>
-      <c r="J28" s="19" t="s">
+      <c r="I29" s="19"/>
+      <c r="J29" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="K28" s="80" t="s">
+      <c r="K29" s="80" t="s">
         <v>835</v>
       </c>
-      <c r="L28" s="19"/>
-      <c r="M28" s="19"/>
-      <c r="N28" s="19"/>
-      <c r="O28" s="19"/>
-      <c r="P28" s="19"/>
-      <c r="Q28" s="19"/>
-      <c r="R28" s="19"/>
-      <c r="S28" s="19"/>
-      <c r="T28" s="19"/>
-      <c r="U28" s="19"/>
-      <c r="V28" s="19"/>
-      <c r="W28" s="19"/>
-      <c r="X28" s="19"/>
-      <c r="Y28" s="19"/>
-      <c r="Z28" s="19"/>
-    </row>
-    <row r="29" spans="1:26" ht="14.4">
-      <c r="A29" s="15"/>
-      <c r="B29" s="15"/>
-      <c r="D29" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="E29" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="F29" s="18">
-        <v>1</v>
-      </c>
-      <c r="G29" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="H29" s="18" t="s">
-        <v>63</v>
-      </c>
-      <c r="J29" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="K29" s="17" t="s">
-        <v>64</v>
-      </c>
+      <c r="L29" s="19"/>
+      <c r="M29" s="19"/>
+      <c r="N29" s="19"/>
+      <c r="O29" s="19"/>
+      <c r="P29" s="19"/>
+      <c r="Q29" s="19"/>
+      <c r="R29" s="19"/>
+      <c r="S29" s="19"/>
+      <c r="T29" s="19"/>
+      <c r="U29" s="19"/>
+      <c r="V29" s="19"/>
+      <c r="W29" s="19"/>
+      <c r="X29" s="19"/>
+      <c r="Y29" s="19"/>
+      <c r="Z29" s="19"/>
     </row>
     <row r="30" spans="1:26" ht="14.4">
       <c r="A30" s="15"/>
-      <c r="B30" s="16" t="s">
-        <v>24</v>
-      </c>
+      <c r="B30" s="15"/>
       <c r="D30" s="17" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E30" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="F30" s="7"/>
+        <v>62</v>
+      </c>
+      <c r="F30" s="18">
+        <v>1</v>
+      </c>
       <c r="G30" s="18" t="s">
         <v>29</v>
       </c>
       <c r="H30" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="J30" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="K30" s="17" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="31" spans="1:26" ht="14.4">
+      <c r="A31" s="15"/>
+      <c r="B31" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="D31" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="E31" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="F31" s="7"/>
+      <c r="G31" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="H31" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="I30" s="17" t="s">
+      <c r="I31" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="J30" s="17" t="s">
+      <c r="J31" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="K30" s="23" t="s">
+      <c r="K31" s="23" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="31" spans="1:26" s="21" customFormat="1" ht="14.4">
-      <c r="A31" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="B31" s="20" t="s">
+    <row r="32" spans="1:26" s="21" customFormat="1" ht="14.4">
+      <c r="A32" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="B32" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="D31" s="22"/>
-      <c r="E31" s="21" t="s">
-        <v>807</v>
-      </c>
-      <c r="F31" s="7"/>
-      <c r="G31" s="57" t="s">
-        <v>29</v>
-      </c>
-      <c r="H31" s="57" t="s">
-        <v>73</v>
-      </c>
-      <c r="I31" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="J31" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="K31" s="23" t="s">
-        <v>808</v>
-      </c>
-    </row>
-    <row r="32" spans="1:26" s="21" customFormat="1" ht="14.4">
-      <c r="A32" s="20"/>
-      <c r="B32" s="20"/>
       <c r="D32" s="22"/>
       <c r="E32" s="21" t="s">
-        <v>857</v>
+        <v>807</v>
       </c>
       <c r="F32" s="7"/>
       <c r="G32" s="57" t="s">
-        <v>109</v>
+        <v>29</v>
       </c>
       <c r="H32" s="57" t="s">
         <v>73</v>
@@ -21504,7 +21517,7 @@
         <v>27</v>
       </c>
       <c r="K32" s="23" t="s">
-        <v>858</v>
+        <v>808</v>
       </c>
     </row>
     <row r="33" spans="1:11" s="21" customFormat="1" ht="14.4">
@@ -21512,14 +21525,14 @@
       <c r="B33" s="20"/>
       <c r="D33" s="22"/>
       <c r="E33" s="21" t="s">
-        <v>905</v>
+        <v>857</v>
       </c>
       <c r="F33" s="7"/>
       <c r="G33" s="57" t="s">
         <v>109</v>
       </c>
       <c r="H33" s="57" t="s">
-        <v>129</v>
+        <v>73</v>
       </c>
       <c r="I33" s="23" t="s">
         <v>26</v>
@@ -21528,28 +21541,31 @@
         <v>27</v>
       </c>
       <c r="K33" s="23" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" s="21" customFormat="1" ht="14.4">
+      <c r="A34" s="20"/>
+      <c r="B34" s="20"/>
+      <c r="D34" s="22"/>
+      <c r="E34" s="21" t="s">
+        <v>905</v>
+      </c>
+      <c r="F34" s="7"/>
+      <c r="G34" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="H34" s="57" t="s">
+        <v>129</v>
+      </c>
+      <c r="I34" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="J34" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="K34" s="23" t="s">
         <v>906</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" ht="14.4">
-      <c r="A34" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B34" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="E34" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="F34" s="7">
-        <v>0</v>
-      </c>
-      <c r="G34" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="H34" s="7"/>
-      <c r="K34" s="3" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="14.4">
@@ -21559,23 +21575,18 @@
       <c r="B35" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="D35" s="3" t="s">
-        <v>39</v>
-      </c>
       <c r="E35" s="7" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F35" s="7">
         <v>0</v>
       </c>
-      <c r="G35" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="H35" s="18" t="s">
-        <v>73</v>
-      </c>
-      <c r="K35" s="17" t="s">
-        <v>74</v>
+      <c r="G35" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="H35" s="7"/>
+      <c r="K35" s="3" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="36" spans="1:11" ht="14.4">
@@ -21585,20 +21596,23 @@
       <c r="B36" s="15" t="s">
         <v>24</v>
       </c>
+      <c r="D36" s="3" t="s">
+        <v>39</v>
+      </c>
       <c r="E36" s="7" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F36" s="7">
         <v>0</v>
       </c>
       <c r="G36" s="18" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="H36" s="18" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="K36" s="17" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="37" spans="1:11" ht="14.4">
@@ -21609,19 +21623,19 @@
         <v>24</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F37" s="7">
         <v>0</v>
       </c>
       <c r="G37" s="18" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
       <c r="H37" s="18" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="K37" s="17" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="38" spans="1:11" ht="14.4">
@@ -21632,19 +21646,19 @@
         <v>24</v>
       </c>
       <c r="E38" s="7" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F38" s="7">
         <v>0</v>
       </c>
       <c r="G38" s="18" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="H38" s="18" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="K38" s="17" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="39" spans="1:11" ht="14.4">
@@ -21654,27 +21668,20 @@
       <c r="B39" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="C39" s="3" t="s">
-        <v>24</v>
-      </c>
       <c r="E39" s="7" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F39" s="7">
-        <v>1739.9274680000001</v>
-      </c>
-      <c r="G39" s="7"/>
-      <c r="H39" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="I39" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="J39" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="K39" s="3" t="s">
-        <v>85</v>
+        <v>0</v>
+      </c>
+      <c r="G39" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="H39" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="K39" s="17" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="40" spans="1:11" ht="14.4">
@@ -21684,17 +21691,28 @@
       <c r="B40" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="D40" s="3" t="s">
-        <v>44</v>
+      <c r="C40" s="3" t="s">
+        <v>24</v>
       </c>
       <c r="E40" s="7" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F40" s="7">
-        <v>6699</v>
+        <v>1739.9274680000001</v>
       </c>
       <c r="G40" s="7"/>
-      <c r="H40" s="7"/>
+      <c r="H40" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="I40" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="J40" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="K40" s="3" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="41" spans="1:11" ht="14.4">
       <c r="A41" s="15" t="s">
@@ -21703,22 +21721,17 @@
       <c r="B41" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="D41" t="s">
-        <v>909</v>
+      <c r="D41" s="3" t="s">
+        <v>44</v>
       </c>
       <c r="E41" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F41" s="7">
-        <v>0</v>
-      </c>
-      <c r="G41" s="7" t="s">
-        <v>910</v>
-      </c>
+        <v>6699</v>
+      </c>
+      <c r="G41" s="7"/>
       <c r="H41" s="7"/>
-      <c r="K41" s="23" t="s">
-        <v>911</v>
-      </c>
     </row>
     <row r="42" spans="1:11" ht="14.4">
       <c r="A42" s="15" t="s">
@@ -21727,47 +21740,41 @@
       <c r="B42" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="D42" s="3" t="s">
+      <c r="D42" t="s">
+        <v>909</v>
+      </c>
+      <c r="E42" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="F42" s="7">
+        <v>0</v>
+      </c>
+      <c r="G42" s="7" t="s">
+        <v>910</v>
+      </c>
+      <c r="H42" s="7"/>
+      <c r="K42" s="23" t="s">
+        <v>911</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" ht="14.4">
+      <c r="A43" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B43" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D43" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="E42" s="7" t="s">
+      <c r="E43" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="F42" s="7">
+      <c r="F43" s="7">
         <v>6758</v>
       </c>
-      <c r="G42" s="7"/>
-      <c r="H42" s="7"/>
-    </row>
-    <row r="43" spans="1:11" s="21" customFormat="1" ht="14.4">
-      <c r="A43" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="B43" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="D43" s="3" t="s">
-        <v>804</v>
-      </c>
-      <c r="E43" s="7" t="s">
-        <v>801</v>
-      </c>
-      <c r="F43" s="7"/>
-      <c r="G43" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="H43" s="58" t="s">
-        <v>73</v>
-      </c>
-      <c r="I43" s="57" t="s">
-        <v>26</v>
-      </c>
-      <c r="J43" s="57" t="s">
-        <v>27</v>
-      </c>
-      <c r="K43" s="57" t="s">
-        <v>803</v>
-      </c>
+      <c r="G43" s="7"/>
+      <c r="H43" s="7"/>
     </row>
     <row r="44" spans="1:11" s="21" customFormat="1" ht="14.4">
       <c r="A44" s="20" t="s">
@@ -21780,14 +21787,14 @@
         <v>804</v>
       </c>
       <c r="E44" s="7" t="s">
-        <v>932</v>
+        <v>801</v>
       </c>
       <c r="F44" s="7"/>
       <c r="G44" s="7" t="s">
-        <v>109</v>
+        <v>29</v>
       </c>
       <c r="H44" s="58" t="s">
-        <v>129</v>
+        <v>73</v>
       </c>
       <c r="I44" s="57" t="s">
         <v>26</v>
@@ -21796,7 +21803,7 @@
         <v>27</v>
       </c>
       <c r="K44" s="57" t="s">
-        <v>933</v>
+        <v>803</v>
       </c>
     </row>
     <row r="45" spans="1:11" s="21" customFormat="1" ht="14.4">
@@ -21807,17 +21814,17 @@
         <v>24</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>805</v>
-      </c>
-      <c r="E45" s="58" t="s">
-        <v>802</v>
+        <v>804</v>
+      </c>
+      <c r="E45" s="7" t="s">
+        <v>932</v>
       </c>
       <c r="F45" s="7"/>
       <c r="G45" s="7" t="s">
-        <v>29</v>
+        <v>109</v>
       </c>
       <c r="H45" s="58" t="s">
-        <v>73</v>
+        <v>129</v>
       </c>
       <c r="I45" s="57" t="s">
         <v>26</v>
@@ -21826,48 +21833,55 @@
         <v>27</v>
       </c>
       <c r="K45" s="57" t="s">
+        <v>933</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" s="21" customFormat="1" ht="14.4">
+      <c r="A46" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="B46" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>805</v>
+      </c>
+      <c r="E46" s="58" t="s">
+        <v>802</v>
+      </c>
+      <c r="F46" s="7"/>
+      <c r="G46" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H46" s="58" t="s">
+        <v>73</v>
+      </c>
+      <c r="I46" s="57" t="s">
+        <v>26</v>
+      </c>
+      <c r="J46" s="57" t="s">
+        <v>27</v>
+      </c>
+      <c r="K46" s="57" t="s">
         <v>806</v>
       </c>
     </row>
-    <row r="46" spans="1:11" s="21" customFormat="1" ht="14.4">
-      <c r="A46" s="20"/>
-      <c r="B46" s="20"/>
-      <c r="D46" s="3"/>
-      <c r="E46" s="58" t="s">
+    <row r="47" spans="1:11" s="21" customFormat="1" ht="14.4">
+      <c r="A47" s="20"/>
+      <c r="B47" s="20"/>
+      <c r="D47" s="3"/>
+      <c r="E47" s="58" t="s">
         <v>420</v>
       </c>
-      <c r="F46" s="7"/>
-      <c r="G46" s="7"/>
-      <c r="H46" s="58" t="s">
+      <c r="F47" s="7"/>
+      <c r="G47" s="7"/>
+      <c r="H47" s="58" t="s">
         <v>173</v>
       </c>
-      <c r="I46" s="57"/>
-      <c r="J46" s="57"/>
-      <c r="K46" s="57" t="s">
+      <c r="I47" s="57"/>
+      <c r="J47" s="57"/>
+      <c r="K47" s="57" t="s">
         <v>941</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" ht="14.4">
-      <c r="A47" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B47" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="E47" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="F47" s="7">
-        <v>0</v>
-      </c>
-      <c r="G47" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="H47" s="57" t="s">
-        <v>73</v>
-      </c>
-      <c r="I47" s="17" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="48" spans="1:11" ht="14.4">
@@ -21878,171 +21892,169 @@
         <v>24</v>
       </c>
       <c r="E48" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F48" s="7">
         <v>0</v>
       </c>
-      <c r="G48" s="7"/>
-      <c r="H48" s="7"/>
-      <c r="K48" s="17" t="s">
+      <c r="G48" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="H48" s="57" t="s">
+        <v>73</v>
+      </c>
+      <c r="I48" s="17" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="49" spans="1:24" ht="14.4">
+      <c r="A49" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B49" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="E49" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="F49" s="7">
+        <v>0</v>
+      </c>
+      <c r="G49" s="7"/>
+      <c r="H49" s="7"/>
+      <c r="K49" s="17" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="49" spans="1:26" s="21" customFormat="1" ht="14.4">
-      <c r="A49" s="20"/>
-      <c r="B49" s="20"/>
-      <c r="E49" s="7" t="s">
-        <v>859</v>
-      </c>
-      <c r="F49" s="7">
-        <v>0.08</v>
-      </c>
-      <c r="G49" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="H49" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="I49" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="J49" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="K49" s="23" t="s">
-        <v>860</v>
-      </c>
-    </row>
-    <row r="50" spans="1:26" s="21" customFormat="1" ht="14.4">
+    <row r="50" spans="1:24" s="21" customFormat="1" ht="14.4">
       <c r="A50" s="20"/>
       <c r="B50" s="20"/>
-      <c r="E50" s="58" t="s">
-        <v>840</v>
-      </c>
-      <c r="F50" s="7"/>
+      <c r="E50" s="7" t="s">
+        <v>859</v>
+      </c>
+      <c r="F50" s="7">
+        <v>0.08</v>
+      </c>
       <c r="G50" s="7" t="s">
         <v>109</v>
       </c>
       <c r="H50" s="7" t="s">
-        <v>475</v>
+        <v>73</v>
       </c>
       <c r="I50" s="21" t="s">
-        <v>26</v>
+        <v>34</v>
+      </c>
+      <c r="J50" s="21" t="s">
+        <v>30</v>
       </c>
       <c r="K50" s="23" t="s">
-        <v>841</v>
-      </c>
-    </row>
-    <row r="51" spans="1:26" s="21" customFormat="1" ht="14.4">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="51" spans="1:24" s="21" customFormat="1" ht="14.4">
       <c r="A51" s="20"/>
       <c r="B51" s="20"/>
       <c r="E51" s="58" t="s">
-        <v>473</v>
+        <v>840</v>
       </c>
       <c r="F51" s="7"/>
-      <c r="G51" s="7"/>
+      <c r="G51" s="7" t="s">
+        <v>109</v>
+      </c>
       <c r="H51" s="7" t="s">
         <v>475</v>
       </c>
+      <c r="I51" s="21" t="s">
+        <v>26</v>
+      </c>
       <c r="K51" s="23" t="s">
-        <v>943</v>
-      </c>
-    </row>
-    <row r="52" spans="1:26" s="21" customFormat="1" ht="14.4">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="52" spans="1:24" s="21" customFormat="1" ht="14.4">
       <c r="A52" s="20"/>
       <c r="B52" s="20"/>
-      <c r="E52" s="7" t="s">
-        <v>839</v>
+      <c r="E52" s="58" t="s">
+        <v>473</v>
       </c>
       <c r="F52" s="7"/>
-      <c r="G52" s="7" t="s">
-        <v>109</v>
-      </c>
+      <c r="G52" s="7"/>
       <c r="H52" s="7" t="s">
         <v>475</v>
       </c>
-      <c r="I52" s="21" t="s">
+      <c r="K52" s="23" t="s">
+        <v>943</v>
+      </c>
+    </row>
+    <row r="53" spans="1:24" s="21" customFormat="1" ht="14.4">
+      <c r="A53" s="20"/>
+      <c r="B53" s="20"/>
+      <c r="E53" s="7" t="s">
+        <v>839</v>
+      </c>
+      <c r="F53" s="7"/>
+      <c r="G53" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="H53" s="7" t="s">
+        <v>475</v>
+      </c>
+      <c r="I53" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="K52" s="23" t="s">
+      <c r="K53" s="23" t="s">
         <v>853</v>
       </c>
     </row>
-    <row r="53" spans="1:26" ht="14.4">
-      <c r="A53" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="B53" s="24" t="s">
+    <row r="54" spans="1:24" ht="14.4">
+      <c r="A54" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B54" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="C53" s="17" t="s">
+      <c r="C54" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="D53" s="17" t="s">
+      <c r="D54" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="E53" s="18" t="s">
+      <c r="E54" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="F53" s="7"/>
-      <c r="G53" s="18" t="s">
+      <c r="F54" s="7"/>
+      <c r="G54" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="H53" s="18" t="s">
+      <c r="H54" s="18" t="s">
         <v>95</v>
       </c>
-      <c r="I53" s="17" t="s">
+      <c r="I54" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="J53" s="17" t="s">
+      <c r="J54" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="K53" s="17" t="s">
+      <c r="K54" s="17" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="54" spans="1:26" s="21" customFormat="1" ht="14.4">
-      <c r="A54" s="20"/>
-      <c r="B54" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="C54" s="22"/>
-      <c r="D54" s="22"/>
-      <c r="E54" s="21" t="s">
-        <v>917</v>
-      </c>
-      <c r="F54" s="7"/>
-      <c r="G54" s="21" t="s">
-        <v>109</v>
-      </c>
-      <c r="H54" s="21" t="s">
-        <v>918</v>
-      </c>
-      <c r="I54" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="J54" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="K54" s="23" t="s">
-        <v>912</v>
-      </c>
-    </row>
-    <row r="55" spans="1:26" s="21" customFormat="1" ht="14.4">
+    <row r="55" spans="1:24" s="21" customFormat="1" ht="14.4">
       <c r="A55" s="20"/>
-      <c r="B55" s="24"/>
+      <c r="B55" s="24" t="s">
+        <v>23</v>
+      </c>
       <c r="C55" s="22"/>
       <c r="D55" s="22"/>
       <c r="E55" s="21" t="s">
-        <v>920</v>
+        <v>917</v>
       </c>
       <c r="F55" s="7"/>
       <c r="G55" s="21" t="s">
         <v>109</v>
       </c>
       <c r="H55" s="21" t="s">
-        <v>407</v>
+        <v>918</v>
       </c>
       <c r="I55" s="23" t="s">
         <v>26</v>
@@ -22051,25 +22063,23 @@
         <v>27</v>
       </c>
       <c r="K55" s="23" t="s">
-        <v>921</v>
-      </c>
-    </row>
-    <row r="56" spans="1:26" s="21" customFormat="1" ht="14.4">
+        <v>912</v>
+      </c>
+    </row>
+    <row r="56" spans="1:24" s="21" customFormat="1" ht="14.4">
       <c r="A56" s="20"/>
-      <c r="B56" s="24" t="s">
-        <v>23</v>
-      </c>
+      <c r="B56" s="24"/>
       <c r="C56" s="22"/>
       <c r="D56" s="22"/>
       <c r="E56" s="21" t="s">
-        <v>913</v>
+        <v>920</v>
       </c>
       <c r="F56" s="7"/>
       <c r="G56" s="21" t="s">
         <v>109</v>
       </c>
       <c r="H56" s="21" t="s">
-        <v>95</v>
+        <v>407</v>
       </c>
       <c r="I56" s="23" t="s">
         <v>26</v>
@@ -22078,319 +22088,320 @@
         <v>27</v>
       </c>
       <c r="K56" s="23" t="s">
+        <v>921</v>
+      </c>
+    </row>
+    <row r="57" spans="1:24" s="21" customFormat="1" ht="14.4">
+      <c r="A57" s="20"/>
+      <c r="B57" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="C57" s="22"/>
+      <c r="D57" s="22"/>
+      <c r="E57" s="21" t="s">
+        <v>913</v>
+      </c>
+      <c r="F57" s="7"/>
+      <c r="G57" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="H57" s="21" t="s">
+        <v>95</v>
+      </c>
+      <c r="I57" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="J57" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="K57" s="23" t="s">
         <v>914</v>
       </c>
     </row>
-    <row r="57" spans="1:26" ht="43.2">
-      <c r="A57" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B57" s="15" t="s">
+    <row r="58" spans="1:24" ht="43.2">
+      <c r="A58" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B58" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="E57" s="7" t="s">
+      <c r="E58" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="F57" s="18">
+      <c r="F58" s="18">
         <v>1</v>
       </c>
-      <c r="G57" s="18" t="s">
+      <c r="G58" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="H57" s="18" t="s">
+      <c r="H58" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="J57" s="17" t="s">
+      <c r="J58" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="K57" s="19" t="s">
+      <c r="K58" s="19" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="58" spans="1:26" s="21" customFormat="1" ht="14.4">
-      <c r="A58" s="20"/>
-      <c r="B58" s="20"/>
-      <c r="E58" s="7" t="s">
+    <row r="59" spans="1:24" s="21" customFormat="1" ht="14.4">
+      <c r="A59" s="20"/>
+      <c r="B59" s="20"/>
+      <c r="E59" s="7" t="s">
         <v>922</v>
       </c>
-      <c r="G58" s="21" t="s">
+      <c r="G59" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="H58" s="21" t="s">
+      <c r="H59" s="21" t="s">
         <v>475</v>
       </c>
-      <c r="I58" s="23" t="s">
+      <c r="I59" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="J58" s="23" t="s">
+      <c r="J59" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="K58" s="23" t="s">
+      <c r="K59" s="23" t="s">
         <v>923</v>
       </c>
     </row>
-    <row r="59" spans="1:26" s="25" customFormat="1" ht="86.4">
-      <c r="A59" s="81"/>
-      <c r="B59" s="81"/>
-      <c r="E59" s="25" t="s">
-        <v>101</v>
-      </c>
-      <c r="F59" s="25">
-        <v>1</v>
-      </c>
-      <c r="G59" s="25" t="s">
-        <v>98</v>
-      </c>
-      <c r="H59" s="25" t="s">
-        <v>99</v>
-      </c>
-      <c r="I59" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="J59" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="K59" s="80" t="s">
-        <v>934</v>
-      </c>
-    </row>
-    <row r="60" spans="1:26" s="25" customFormat="1" ht="14.4">
+    <row r="60" spans="1:24" s="25" customFormat="1" ht="86.4">
       <c r="A60" s="81"/>
       <c r="B60" s="81"/>
-      <c r="E60" s="72" t="s">
+      <c r="E60" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="F60" s="25">
+        <v>1</v>
+      </c>
+      <c r="G60" s="25" t="s">
+        <v>98</v>
+      </c>
+      <c r="H60" s="25" t="s">
+        <v>99</v>
+      </c>
+      <c r="I60" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="J60" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="K60" s="80" t="s">
+        <v>934</v>
+      </c>
+    </row>
+    <row r="61" spans="1:24" s="25" customFormat="1" ht="14.4">
+      <c r="A61" s="81"/>
+      <c r="B61" s="81"/>
+      <c r="E61" s="72" t="s">
         <v>924</v>
       </c>
-      <c r="G60" s="72" t="s">
+      <c r="G61" s="72" t="s">
         <v>109</v>
       </c>
-      <c r="H60" s="72" t="s">
+      <c r="H61" s="72" t="s">
         <v>475</v>
-      </c>
-      <c r="I60" s="80" t="s">
-        <v>26</v>
-      </c>
-      <c r="J60" s="80" t="s">
-        <v>27</v>
-      </c>
-      <c r="K60" s="23" t="s">
-        <v>925</v>
-      </c>
-    </row>
-    <row r="61" spans="1:26" s="25" customFormat="1" ht="28.8">
-      <c r="A61" s="81"/>
-      <c r="B61" s="81" t="s">
-        <v>23</v>
-      </c>
-      <c r="E61" s="25" t="s">
-        <v>915</v>
-      </c>
-      <c r="G61" s="25" t="s">
-        <v>109</v>
-      </c>
-      <c r="H61" s="25" t="s">
-        <v>129</v>
       </c>
       <c r="I61" s="80" t="s">
         <v>26</v>
       </c>
-      <c r="J61" s="19"/>
-      <c r="K61" s="80" t="s">
+      <c r="J61" s="80" t="s">
+        <v>27</v>
+      </c>
+      <c r="K61" s="23" t="s">
+        <v>925</v>
+      </c>
+    </row>
+    <row r="62" spans="1:24" s="25" customFormat="1" ht="28.8">
+      <c r="A62" s="81"/>
+      <c r="B62" s="81" t="s">
+        <v>23</v>
+      </c>
+      <c r="E62" s="25" t="s">
+        <v>915</v>
+      </c>
+      <c r="G62" s="25" t="s">
+        <v>109</v>
+      </c>
+      <c r="H62" s="25" t="s">
+        <v>129</v>
+      </c>
+      <c r="I62" s="80" t="s">
+        <v>26</v>
+      </c>
+      <c r="J62" s="19"/>
+      <c r="K62" s="80" t="s">
         <v>916</v>
       </c>
     </row>
-    <row r="62" spans="1:26" s="21" customFormat="1" ht="14.25" customHeight="1">
-      <c r="C62" s="28"/>
-      <c r="D62" s="28"/>
-      <c r="E62" s="7" t="s">
+    <row r="63" spans="1:24" s="21" customFormat="1" ht="14.25" customHeight="1">
+      <c r="C63" s="28"/>
+      <c r="D63" s="28"/>
+      <c r="E63" s="7" t="s">
         <v>812</v>
       </c>
-      <c r="F62" s="7"/>
-      <c r="G62" s="70" t="s">
+      <c r="F63" s="7"/>
+      <c r="G63" s="70" t="s">
         <v>29</v>
       </c>
-      <c r="H62" s="70" t="s">
+      <c r="H63" s="70" t="s">
         <v>227</v>
       </c>
-      <c r="I62" s="70" t="s">
+      <c r="I63" s="70" t="s">
         <v>34</v>
       </c>
-      <c r="J62" s="70" t="s">
+      <c r="J63" s="70" t="s">
         <v>27</v>
       </c>
-      <c r="K62" s="57" t="s">
+      <c r="K63" s="57" t="s">
         <v>813</v>
       </c>
-      <c r="L62" s="70" t="s">
+      <c r="L63" s="70" t="s">
         <v>814</v>
       </c>
-      <c r="M62" s="3"/>
-      <c r="N62" s="7"/>
-      <c r="O62" s="7"/>
-      <c r="P62" s="7"/>
-      <c r="Q62" s="7"/>
-      <c r="R62" s="7"/>
-      <c r="S62" s="7"/>
-      <c r="T62" s="7"/>
-      <c r="U62" s="7"/>
-      <c r="V62" s="7"/>
-      <c r="W62" s="7"/>
-      <c r="X62" s="7"/>
-    </row>
-    <row r="63" spans="1:26" ht="14.4">
-      <c r="A63" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B63" s="15" t="s">
+      <c r="M63" s="3"/>
+      <c r="N63" s="7"/>
+      <c r="O63" s="7"/>
+      <c r="P63" s="7"/>
+      <c r="Q63" s="7"/>
+      <c r="R63" s="7"/>
+      <c r="S63" s="7"/>
+      <c r="T63" s="7"/>
+      <c r="U63" s="7"/>
+      <c r="V63" s="7"/>
+      <c r="W63" s="7"/>
+      <c r="X63" s="7"/>
+    </row>
+    <row r="64" spans="1:24" ht="14.4">
+      <c r="A64" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B64" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="E63" s="7" t="s">
+      <c r="E64" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="F63" s="7">
+      <c r="F64" s="7">
         <v>-1</v>
       </c>
-      <c r="G63" s="7"/>
-      <c r="H63" s="7"/>
-    </row>
-    <row r="64" spans="1:26" ht="14.4">
-      <c r="A64" s="15"/>
-      <c r="B64" s="15"/>
-      <c r="C64" s="7" t="s">
+      <c r="G64" s="7"/>
+      <c r="H64" s="7"/>
+    </row>
+    <row r="65" spans="1:26" ht="14.4">
+      <c r="A65" s="15"/>
+      <c r="B65" s="15"/>
+      <c r="C65" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="D64" s="7" t="s">
+      <c r="D65" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="E64" s="7" t="s">
+      <c r="E65" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="F64" s="7">
+      <c r="F65" s="7">
         <v>0.6</v>
       </c>
-      <c r="G64" s="7" t="s">
+      <c r="G65" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="H64" s="7" t="s">
+      <c r="H65" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="I64" s="7" t="s">
+      <c r="I65" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="J64" s="7" t="s">
+      <c r="J65" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="K64" s="7" t="s">
+      <c r="K65" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="L64" s="7"/>
-      <c r="M64" s="7"/>
-      <c r="N64" s="7"/>
-      <c r="O64" s="7"/>
-      <c r="P64" s="7"/>
-      <c r="Q64" s="7"/>
-      <c r="R64" s="7"/>
-      <c r="S64" s="7"/>
-      <c r="T64" s="7"/>
-      <c r="U64" s="7"/>
-      <c r="V64" s="7"/>
-      <c r="W64" s="7"/>
-      <c r="X64" s="7"/>
-      <c r="Y64" s="7"/>
-      <c r="Z64" s="7"/>
-    </row>
-    <row r="65" spans="1:12" ht="14.4">
-      <c r="A65" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B65" s="15" t="s">
+      <c r="L65" s="7"/>
+      <c r="M65" s="7"/>
+      <c r="N65" s="7"/>
+      <c r="O65" s="7"/>
+      <c r="P65" s="7"/>
+      <c r="Q65" s="7"/>
+      <c r="R65" s="7"/>
+      <c r="S65" s="7"/>
+      <c r="T65" s="7"/>
+      <c r="U65" s="7"/>
+      <c r="V65" s="7"/>
+      <c r="W65" s="7"/>
+      <c r="X65" s="7"/>
+      <c r="Y65" s="7"/>
+      <c r="Z65" s="7"/>
+    </row>
+    <row r="66" spans="1:26" ht="14.4">
+      <c r="A66" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B66" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="E65" s="7" t="s">
+      <c r="E66" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="F65" s="7">
+      <c r="F66" s="7">
         <v>1739.927555</v>
       </c>
-      <c r="G65" s="7"/>
-      <c r="H65" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="K65" s="3" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="66" spans="1:12" s="21" customFormat="1" ht="14.4">
-      <c r="A66" s="20"/>
-      <c r="B66" s="20"/>
-      <c r="E66" s="7" t="s">
-        <v>962</v>
-      </c>
-      <c r="F66" s="7"/>
-      <c r="G66" s="7" t="s">
-        <v>109</v>
-      </c>
+      <c r="G66" s="7"/>
       <c r="H66" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="I66" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="J66" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="K66" s="3"/>
-    </row>
-    <row r="67" spans="1:12" s="21" customFormat="1" ht="14.4">
+      <c r="K66" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="67" spans="1:26" s="21" customFormat="1" ht="14.4">
       <c r="A67" s="20"/>
       <c r="B67" s="20"/>
       <c r="E67" s="7" t="s">
-        <v>497</v>
+        <v>962</v>
       </c>
       <c r="F67" s="7"/>
-      <c r="G67" s="7"/>
-      <c r="H67" s="7"/>
-      <c r="K67" s="3" t="s">
-        <v>942</v>
-      </c>
-    </row>
-    <row r="68" spans="1:12" s="21" customFormat="1" ht="14.4">
+      <c r="G67" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="H67" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="I67" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="J67" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="K67" s="3"/>
+    </row>
+    <row r="68" spans="1:26" s="21" customFormat="1" ht="14.4">
       <c r="A68" s="20"/>
       <c r="B68" s="20"/>
       <c r="E68" s="7" t="s">
-        <v>854</v>
+        <v>497</v>
       </c>
       <c r="F68" s="7"/>
-      <c r="G68" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="H68" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="I68" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="J68" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="K68" s="21" t="s">
-        <v>856</v>
-      </c>
-      <c r="L68" s="3" t="s">
-        <v>855</v>
-      </c>
-    </row>
-    <row r="69" spans="1:12" s="21" customFormat="1" ht="14.4">
+      <c r="G68" s="7"/>
+      <c r="H68" s="7"/>
+      <c r="K68" s="3" t="s">
+        <v>942</v>
+      </c>
+    </row>
+    <row r="69" spans="1:26" s="21" customFormat="1" ht="14.4">
       <c r="A69" s="20"/>
       <c r="B69" s="20"/>
       <c r="E69" s="7" t="s">
-        <v>919</v>
+        <v>854</v>
       </c>
       <c r="F69" s="7"/>
       <c r="G69" s="7" t="s">
         <v>29</v>
       </c>
       <c r="H69" s="7" t="s">
-        <v>129</v>
+        <v>73</v>
       </c>
       <c r="I69" s="21" t="s">
         <v>34</v>
@@ -22399,61 +22410,71 @@
         <v>30</v>
       </c>
       <c r="K69" s="21" t="s">
-        <v>904</v>
+        <v>856</v>
       </c>
       <c r="L69" s="3" t="s">
         <v>855</v>
       </c>
     </row>
-    <row r="70" spans="1:12" ht="14.4">
-      <c r="A70" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B70" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="C70" s="3" t="s">
-        <v>24</v>
-      </c>
+    <row r="70" spans="1:26" s="21" customFormat="1" ht="14.4">
+      <c r="A70" s="20"/>
+      <c r="B70" s="20"/>
       <c r="E70" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="F70" s="7">
-        <v>1</v>
-      </c>
+        <v>919</v>
+      </c>
+      <c r="F70" s="7"/>
       <c r="G70" s="7" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="H70" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="I70" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="I70" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="J70" s="3" t="s">
+      <c r="J70" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="K70" s="3" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="71" spans="1:12" ht="14.4">
+      <c r="K70" s="21" t="s">
+        <v>904</v>
+      </c>
+      <c r="L70" s="3" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="71" spans="1:26" ht="14.4">
       <c r="A71" s="15" t="s">
         <v>23</v>
       </c>
       <c r="B71" s="15" t="s">
         <v>24</v>
       </c>
+      <c r="C71" s="3" t="s">
+        <v>24</v>
+      </c>
       <c r="E71" s="7" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="F71" s="7">
-        <v>553659</v>
-      </c>
-      <c r="G71" s="7"/>
-      <c r="H71" s="7"/>
-    </row>
-    <row r="72" spans="1:12" ht="14.4">
+        <v>1</v>
+      </c>
+      <c r="G71" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="H71" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="I71" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="J71" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="K71" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="72" spans="1:26" ht="14.4">
       <c r="A72" s="15" t="s">
         <v>23</v>
       </c>
@@ -22461,121 +22482,104 @@
         <v>24</v>
       </c>
       <c r="E72" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F72" s="7">
-        <v>4891208</v>
+        <v>553659</v>
       </c>
       <c r="G72" s="7"/>
       <c r="H72" s="7"/>
     </row>
-    <row r="73" spans="1:12" ht="14.4">
+    <row r="73" spans="1:26" ht="14.4">
       <c r="A73" s="15" t="s">
         <v>23</v>
       </c>
       <c r="B73" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="C73" s="3" t="s">
+      <c r="E73" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="F73" s="7">
+        <v>4891208</v>
+      </c>
+      <c r="G73" s="7"/>
+      <c r="H73" s="7"/>
+    </row>
+    <row r="74" spans="1:26" ht="14.4">
+      <c r="A74" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B74" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="E73" s="7" t="s">
+      <c r="C74" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E74" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="F73" s="7">
+      <c r="F74" s="7">
         <v>1</v>
       </c>
-      <c r="G73" s="7" t="s">
+      <c r="G74" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="H73" s="7" t="s">
+      <c r="H74" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="I73" s="3" t="s">
+      <c r="I74" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="J73" s="3" t="s">
+      <c r="J74" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="K73" s="3" t="s">
+      <c r="K74" s="3" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="74" spans="1:12" s="21" customFormat="1" ht="14.4">
-      <c r="A74" s="20"/>
-      <c r="B74" s="20"/>
-      <c r="C74" s="3"/>
-      <c r="E74" s="7" t="s">
+    <row r="75" spans="1:26" s="21" customFormat="1" ht="14.4">
+      <c r="A75" s="20"/>
+      <c r="B75" s="20"/>
+      <c r="C75" s="3"/>
+      <c r="E75" s="7" t="s">
         <v>935</v>
       </c>
-      <c r="F74" s="7"/>
-      <c r="G74" s="7"/>
-      <c r="H74" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="I74" s="3"/>
-      <c r="J74" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="K74" s="3" t="s">
-        <v>937</v>
-      </c>
-    </row>
-    <row r="75" spans="1:12" s="21" customFormat="1" ht="14.4">
-      <c r="A75" s="20" t="s">
-        <v>837</v>
-      </c>
-      <c r="B75" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="C75" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="D75" s="21" t="s">
-        <v>65</v>
-      </c>
-      <c r="E75" s="7" t="s">
-        <v>836</v>
-      </c>
-      <c r="F75" s="7">
-        <v>5</v>
-      </c>
-      <c r="G75" s="7" t="s">
-        <v>109</v>
-      </c>
+      <c r="F75" s="7"/>
+      <c r="G75" s="7"/>
       <c r="H75" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="I75" s="3" t="s">
-        <v>26</v>
-      </c>
+      <c r="I75" s="3"/>
       <c r="J75" s="3" t="s">
         <v>27</v>
       </c>
       <c r="K75" s="3" t="s">
-        <v>838</v>
-      </c>
-      <c r="L75" s="23" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="76" spans="1:26" s="21" customFormat="1" ht="14.4">
+      <c r="A76" s="20" t="s">
+        <v>837</v>
+      </c>
+      <c r="B76" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="C76" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D76" s="21" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="76" spans="1:12" ht="14.4">
-      <c r="A76" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B76" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="D76" s="3" t="s">
-        <v>127</v>
-      </c>
       <c r="E76" s="7" t="s">
-        <v>128</v>
+        <v>836</v>
       </c>
       <c r="F76" s="7">
-        <v>0</v>
-      </c>
-      <c r="G76" s="7"/>
+        <v>5</v>
+      </c>
+      <c r="G76" s="7" t="s">
+        <v>109</v>
+      </c>
       <c r="H76" s="7" t="s">
         <v>129</v>
       </c>
@@ -22586,33 +22590,48 @@
         <v>27</v>
       </c>
       <c r="K76" s="3" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="77" spans="1:12" s="21" customFormat="1" ht="14.4">
-      <c r="A77" s="20"/>
-      <c r="B77" s="20"/>
-      <c r="D77" s="3"/>
+        <v>838</v>
+      </c>
+      <c r="L76" s="23" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="77" spans="1:26" ht="14.4">
+      <c r="A77" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B77" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D77" s="3" t="s">
+        <v>127</v>
+      </c>
       <c r="E77" s="7" t="s">
-        <v>936</v>
-      </c>
-      <c r="F77" s="7"/>
+        <v>128</v>
+      </c>
+      <c r="F77" s="7">
+        <v>0</v>
+      </c>
       <c r="G77" s="7"/>
       <c r="H77" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="I77" s="3"/>
-      <c r="J77" s="3"/>
+      <c r="I77" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J77" s="3" t="s">
+        <v>27</v>
+      </c>
       <c r="K77" s="3" t="s">
-        <v>938</v>
-      </c>
-    </row>
-    <row r="78" spans="1:12" s="21" customFormat="1" ht="14.4">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="78" spans="1:26" s="21" customFormat="1" ht="14.4">
       <c r="A78" s="20"/>
       <c r="B78" s="20"/>
       <c r="D78" s="3"/>
       <c r="E78" s="7" t="s">
-        <v>939</v>
+        <v>936</v>
       </c>
       <c r="F78" s="7"/>
       <c r="G78" s="7"/>
@@ -22622,53 +22641,46 @@
       <c r="I78" s="3"/>
       <c r="J78" s="3"/>
       <c r="K78" s="3" t="s">
+        <v>938</v>
+      </c>
+    </row>
+    <row r="79" spans="1:26" s="21" customFormat="1" ht="14.4">
+      <c r="A79" s="20"/>
+      <c r="B79" s="20"/>
+      <c r="D79" s="3"/>
+      <c r="E79" s="7" t="s">
+        <v>939</v>
+      </c>
+      <c r="F79" s="7"/>
+      <c r="G79" s="7"/>
+      <c r="H79" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="I79" s="3"/>
+      <c r="J79" s="3"/>
+      <c r="K79" s="3" t="s">
         <v>940</v>
       </c>
     </row>
-    <row r="79" spans="1:12" ht="14.4">
-      <c r="A79" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B79" s="15"/>
-      <c r="E79" s="7" t="s">
+    <row r="80" spans="1:26" ht="14.4">
+      <c r="A80" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B80" s="15"/>
+      <c r="E80" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="F79" s="7">
+      <c r="F80" s="7">
         <v>6772</v>
       </c>
-      <c r="G79" s="7"/>
-      <c r="H79" s="7"/>
-    </row>
-    <row r="80" spans="1:12" s="21" customFormat="1" ht="14.4">
-      <c r="A80" s="20"/>
-      <c r="B80" s="20"/>
-      <c r="E80" s="7" t="s">
-        <v>955</v>
-      </c>
-      <c r="F80" s="7">
-        <v>5</v>
-      </c>
-      <c r="G80" s="58" t="s">
-        <v>109</v>
-      </c>
-      <c r="H80" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="I80" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="J80" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="K80" s="23" t="s">
-        <v>956</v>
-      </c>
+      <c r="G80" s="7"/>
+      <c r="H80" s="7"/>
     </row>
     <row r="81" spans="1:12" s="21" customFormat="1" ht="14.4">
       <c r="A81" s="20"/>
       <c r="B81" s="20"/>
-      <c r="E81" s="58" t="s">
-        <v>957</v>
+      <c r="E81" s="7" t="s">
+        <v>955</v>
       </c>
       <c r="F81" s="7">
         <v>5</v>
@@ -22686,14 +22698,14 @@
         <v>30</v>
       </c>
       <c r="K81" s="23" t="s">
-        <v>958</v>
+        <v>956</v>
       </c>
     </row>
     <row r="82" spans="1:12" s="21" customFormat="1" ht="14.4">
       <c r="A82" s="20"/>
       <c r="B82" s="20"/>
       <c r="E82" s="58" t="s">
-        <v>959</v>
+        <v>957</v>
       </c>
       <c r="F82" s="7">
         <v>5</v>
@@ -22711,57 +22723,55 @@
         <v>30</v>
       </c>
       <c r="K82" s="23" t="s">
-        <v>960</v>
+        <v>958</v>
       </c>
     </row>
     <row r="83" spans="1:12" s="21" customFormat="1" ht="14.4">
       <c r="A83" s="20"/>
       <c r="B83" s="20"/>
-      <c r="E83" s="7" t="s">
-        <v>843</v>
+      <c r="E83" s="58" t="s">
+        <v>959</v>
       </c>
       <c r="F83" s="7">
-        <v>1</v>
-      </c>
-      <c r="G83" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G83" s="58" t="s">
         <v>109</v>
       </c>
       <c r="H83" s="7" t="s">
-        <v>844</v>
-      </c>
-      <c r="I83" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="J83" s="23" t="s">
-        <v>845</v>
+        <v>129</v>
+      </c>
+      <c r="I83" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="J83" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="K83" s="23" t="s">
+        <v>960</v>
       </c>
     </row>
     <row r="84" spans="1:12" s="21" customFormat="1" ht="14.4">
       <c r="A84" s="20"/>
       <c r="B84" s="20"/>
-      <c r="D84" s="57" t="s">
-        <v>945</v>
-      </c>
       <c r="E84" s="7" t="s">
-        <v>951</v>
-      </c>
-      <c r="F84" s="7"/>
-      <c r="G84" s="58" t="s">
+        <v>843</v>
+      </c>
+      <c r="F84" s="7">
+        <v>1</v>
+      </c>
+      <c r="G84" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="H84" s="58" t="s">
-        <v>84</v>
+      <c r="H84" s="7" t="s">
+        <v>844</v>
       </c>
       <c r="I84" s="23" t="s">
-        <v>948</v>
+        <v>26</v>
       </c>
       <c r="J84" s="23" t="s">
-        <v>948</v>
-      </c>
-      <c r="K84" s="23" t="s">
-        <v>953</v>
-      </c>
-      <c r="L84" s="23"/>
+        <v>845</v>
+      </c>
     </row>
     <row r="85" spans="1:12" s="21" customFormat="1" ht="14.4">
       <c r="A85" s="20"/>
@@ -22770,7 +22780,7 @@
         <v>945</v>
       </c>
       <c r="E85" s="7" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="F85" s="7"/>
       <c r="G85" s="58" t="s">
@@ -22785,168 +22795,154 @@
       <c r="J85" s="23" t="s">
         <v>948</v>
       </c>
-      <c r="K85" s="57" t="s">
-        <v>954</v>
-      </c>
+      <c r="K85" s="23" t="s">
+        <v>953</v>
+      </c>
+      <c r="L85" s="23"/>
     </row>
     <row r="86" spans="1:12" s="21" customFormat="1" ht="14.4">
       <c r="A86" s="20"/>
       <c r="B86" s="20"/>
+      <c r="D86" s="57" t="s">
+        <v>945</v>
+      </c>
       <c r="E86" s="7" t="s">
-        <v>842</v>
-      </c>
-      <c r="F86" s="7">
-        <v>10</v>
-      </c>
-      <c r="G86" s="7" t="s">
+        <v>952</v>
+      </c>
+      <c r="F86" s="7"/>
+      <c r="G86" s="58" t="s">
         <v>109</v>
       </c>
-      <c r="H86" s="7" t="s">
-        <v>626</v>
+      <c r="H86" s="58" t="s">
+        <v>84</v>
       </c>
       <c r="I86" s="23" t="s">
-        <v>26</v>
+        <v>948</v>
       </c>
       <c r="J86" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="K86" s="23" t="s">
-        <v>848</v>
+        <v>948</v>
+      </c>
+      <c r="K86" s="57" t="s">
+        <v>954</v>
       </c>
     </row>
     <row r="87" spans="1:12" s="21" customFormat="1" ht="14.4">
       <c r="A87" s="20"/>
       <c r="B87" s="20"/>
       <c r="E87" s="7" t="s">
-        <v>510</v>
-      </c>
-      <c r="F87" s="7"/>
-      <c r="G87" s="7"/>
+        <v>842</v>
+      </c>
+      <c r="F87" s="7">
+        <v>10</v>
+      </c>
+      <c r="G87" s="7" t="s">
+        <v>109</v>
+      </c>
       <c r="H87" s="7" t="s">
-        <v>511</v>
-      </c>
-      <c r="I87" s="23"/>
-      <c r="J87" s="23"/>
+        <v>626</v>
+      </c>
+      <c r="I87" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="J87" s="23" t="s">
+        <v>27</v>
+      </c>
       <c r="K87" s="23" t="s">
-        <v>944</v>
+        <v>848</v>
       </c>
     </row>
     <row r="88" spans="1:12" s="21" customFormat="1" ht="14.4">
       <c r="A88" s="20"/>
       <c r="B88" s="20"/>
-      <c r="D88" s="57" t="s">
+      <c r="E88" s="7" t="s">
+        <v>963</v>
+      </c>
+      <c r="F88" s="7"/>
+      <c r="G88" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="H88" s="7" t="s">
+        <v>626</v>
+      </c>
+      <c r="I88" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="J88" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="K88" s="23" t="s">
+        <v>964</v>
+      </c>
+    </row>
+    <row r="89" spans="1:12" s="21" customFormat="1" ht="14.4">
+      <c r="A89" s="20"/>
+      <c r="B89" s="20"/>
+      <c r="E89" s="7" t="s">
+        <v>510</v>
+      </c>
+      <c r="F89" s="7"/>
+      <c r="G89" s="7"/>
+      <c r="H89" s="7" t="s">
+        <v>511</v>
+      </c>
+      <c r="I89" s="23"/>
+      <c r="J89" s="23"/>
+      <c r="K89" s="23" t="s">
+        <v>944</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12" s="21" customFormat="1" ht="14.4">
+      <c r="A90" s="20"/>
+      <c r="B90" s="20"/>
+      <c r="D90" s="57" t="s">
         <v>25</v>
       </c>
-      <c r="E88" s="7" t="s">
+      <c r="E90" s="7" t="s">
         <v>796</v>
       </c>
-      <c r="F88" s="7"/>
-      <c r="G88" s="58" t="s">
+      <c r="F90" s="7"/>
+      <c r="G90" s="58" t="s">
         <v>29</v>
       </c>
-      <c r="H88" s="7" t="s">
+      <c r="H90" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="I88" s="23" t="s">
+      <c r="I90" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="J88" s="23" t="s">
+      <c r="J90" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="K88" s="23" t="s">
+      <c r="K90" s="23" t="s">
         <v>797</v>
       </c>
     </row>
-    <row r="89" spans="1:12" s="21" customFormat="1" ht="14.4">
-      <c r="A89" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="B89" s="20"/>
-      <c r="D89" s="57" t="s">
+    <row r="91" spans="1:12" s="21" customFormat="1" ht="14.4">
+      <c r="A91" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="B91" s="20"/>
+      <c r="D91" s="57" t="s">
         <v>25</v>
       </c>
-      <c r="E89" s="7" t="s">
+      <c r="E91" s="7" t="s">
         <v>798</v>
       </c>
-      <c r="F89" s="7"/>
-      <c r="G89" s="58" t="s">
+      <c r="F91" s="7"/>
+      <c r="G91" s="58" t="s">
         <v>29</v>
       </c>
-      <c r="H89" s="7" t="s">
+      <c r="H91" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="I89" s="23" t="s">
+      <c r="I91" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="J89" s="23" t="s">
+      <c r="J91" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="K89" s="23" t="s">
+      <c r="K91" s="23" t="s">
         <v>799</v>
-      </c>
-    </row>
-    <row r="90" spans="1:12" ht="14.4">
-      <c r="A90" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B90" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="D90" s="17" t="s">
-        <v>133</v>
-      </c>
-      <c r="E90" s="18" t="s">
-        <v>135</v>
-      </c>
-      <c r="F90" s="18">
-        <v>1500</v>
-      </c>
-      <c r="G90" s="18" t="s">
-        <v>109</v>
-      </c>
-      <c r="H90" s="18" t="s">
-        <v>84</v>
-      </c>
-      <c r="I90" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="J90" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="K90" s="17" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="91" spans="1:12" ht="14.4">
-      <c r="A91" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B91" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="D91" s="17" t="s">
-        <v>133</v>
-      </c>
-      <c r="E91" s="17" t="s">
-        <v>140</v>
-      </c>
-      <c r="F91" s="17">
-        <v>1500</v>
-      </c>
-      <c r="G91" s="18" t="s">
-        <v>109</v>
-      </c>
-      <c r="H91" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="I91" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="J91" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="K91" s="17" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="92" spans="1:12" ht="14.4">
@@ -22959,16 +22955,16 @@
       <c r="D92" s="17" t="s">
         <v>133</v>
       </c>
-      <c r="E92" s="17" t="s">
-        <v>143</v>
-      </c>
-      <c r="F92" s="17">
+      <c r="E92" s="18" t="s">
+        <v>135</v>
+      </c>
+      <c r="F92" s="18">
         <v>1500</v>
       </c>
       <c r="G92" s="18" t="s">
         <v>109</v>
       </c>
-      <c r="H92" s="17" t="s">
+      <c r="H92" s="18" t="s">
         <v>84</v>
       </c>
       <c r="I92" s="17" t="s">
@@ -22978,13 +22974,77 @@
         <v>30</v>
       </c>
       <c r="K92" s="17" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="93" spans="1:12" ht="14.4">
+      <c r="A93" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B93" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="D93" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="E93" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="F93" s="17">
+        <v>1500</v>
+      </c>
+      <c r="G93" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="H93" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="I93" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="J93" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="K93" s="17" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="94" spans="1:12" ht="14.4">
+      <c r="A94" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B94" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="D94" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="E94" s="17" t="s">
+        <v>143</v>
+      </c>
+      <c r="F94" s="17">
+        <v>1500</v>
+      </c>
+      <c r="G94" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="H94" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="I94" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="J94" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="K94" s="17" t="s">
         <v>144</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B53:B56">
+  <conditionalFormatting sqref="B54:B57">
     <cfRule type="notContainsBlanks" dxfId="0" priority="1">
-      <formula>LEN(TRIM(B53))&gt;0</formula>
+      <formula>LEN(TRIM(B54))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
More preparations for 0.4.6.  Restore the spring flows and HBV.csv values to what they were in C242.
</commit_message>
<xml_diff>
--- a/DataCW3M/CW3MdigitalHandbook/CW3MdataDictionary.xlsx
+++ b/DataCW3M/CW3MdigitalHandbook/CW3MdataDictionary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\CW3MdigitalHandbook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABAC855E-C17E-4B2D-9B3C-02EDC60D5FEB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41BAA624-171E-44ED-87EA-10575033CE97}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20662,7 +20662,7 @@
   <dimension ref="A1:Z94"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="4" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
More changes to get the Shade-a-lator logic working. CW3MdataDictionary.xlsx, Reach_McKenzie.dbf - Add Reach attribute SAL_REACH. Add McKenzie/Shade_a_latorData/75FC_kcal_transposed.csv. Add folders ScenarioData/SAL75CC_Test/ and .../SAL75FC_Test/. Scenario.cpp - Correct the name of the canopy density field as "SAL_canopy_density_pct". Flow.cpp, .h - Add Reach attribute SAL_REACH. Use SAL_REACH instead of RADSWGIVEN to flag a reach as included in the Shade-a-lator study. Fix some logic problems in CalcReachVegParamsIfNecessary(). ReachRouting.cpp - Use SAL_REACH instead of RADSWGIVEN to flag a reach as included in the Shade-a-lator study.
</commit_message>
<xml_diff>
--- a/DataCW3M/CW3MdigitalHandbook/CW3MdataDictionary.xlsx
+++ b/DataCW3M/CW3MdigitalHandbook/CW3MdataDictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\CW3MdigitalHandbook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{040BAB22-1BA5-43C3-AC4D-D89461AFE430}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B9DD3A8-80AA-4275-B7AB-12B63BE2FD42}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-7425" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Necessary input data" sheetId="7" r:id="rId1"/>
@@ -96,7 +96,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2947" uniqueCount="982">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2951" uniqueCount="985">
   <si>
     <t>LULC_A</t>
   </si>
@@ -3043,6 +3043,15 @@
   </si>
   <si>
     <t>vegetation height on right bank of stream from Shade-a-lator data</t>
+  </si>
+  <si>
+    <t>SAL_REACH</t>
+  </si>
+  <si>
+    <t>1 or 0</t>
+  </si>
+  <si>
+    <t>1 =&gt; this reach is completely covered by  the Shade-a-lator data</t>
   </si>
 </sst>
 </file>
@@ -20715,11 +20724,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Z101"/>
+  <dimension ref="A1:Z102"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A81" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K91" sqref="K91"/>
+      <pane ySplit="4" topLeftCell="A57" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K70" sqref="K70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -22440,145 +22449,136 @@
       <c r="G68" s="7"/>
       <c r="H68" s="7"/>
     </row>
-    <row r="69" spans="1:26" ht="14.4">
-      <c r="A69" s="15"/>
-      <c r="B69" s="15"/>
-      <c r="C69" s="7" t="s">
+    <row r="69" spans="1:26" s="21" customFormat="1" ht="14.4">
+      <c r="A69" s="20"/>
+      <c r="B69" s="20"/>
+      <c r="E69" s="25" t="s">
+        <v>982</v>
+      </c>
+      <c r="F69" s="7" t="s">
+        <v>983</v>
+      </c>
+      <c r="G69" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="H69" s="7"/>
+      <c r="K69" s="21" t="s">
+        <v>984</v>
+      </c>
+    </row>
+    <row r="70" spans="1:26" ht="14.4">
+      <c r="A70" s="15"/>
+      <c r="B70" s="15"/>
+      <c r="C70" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="D69" s="7" t="s">
+      <c r="D70" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="E69" s="7" t="s">
+      <c r="E70" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="F69" s="7">
+      <c r="F70" s="7">
         <v>0.6</v>
       </c>
-      <c r="G69" s="7" t="s">
+      <c r="G70" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="H69" s="7" t="s">
+      <c r="H70" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="I69" s="7" t="s">
+      <c r="I70" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="J69" s="7" t="s">
+      <c r="J70" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="K69" s="7" t="s">
+      <c r="K70" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="L69" s="7"/>
-      <c r="M69" s="7"/>
-      <c r="N69" s="7"/>
-      <c r="O69" s="7"/>
-      <c r="P69" s="7"/>
-      <c r="Q69" s="7"/>
-      <c r="R69" s="7"/>
-      <c r="S69" s="7"/>
-      <c r="T69" s="7"/>
-      <c r="U69" s="7"/>
-      <c r="V69" s="7"/>
-      <c r="W69" s="7"/>
-      <c r="X69" s="7"/>
-      <c r="Y69" s="7"/>
-      <c r="Z69" s="7"/>
-    </row>
-    <row r="70" spans="1:26" ht="14.4">
-      <c r="A70" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B70" s="15" t="s">
+      <c r="L70" s="7"/>
+      <c r="M70" s="7"/>
+      <c r="N70" s="7"/>
+      <c r="O70" s="7"/>
+      <c r="P70" s="7"/>
+      <c r="Q70" s="7"/>
+      <c r="R70" s="7"/>
+      <c r="S70" s="7"/>
+      <c r="T70" s="7"/>
+      <c r="U70" s="7"/>
+      <c r="V70" s="7"/>
+      <c r="W70" s="7"/>
+      <c r="X70" s="7"/>
+      <c r="Y70" s="7"/>
+      <c r="Z70" s="7"/>
+    </row>
+    <row r="71" spans="1:26" ht="14.4">
+      <c r="A71" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B71" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="E70" s="7" t="s">
+      <c r="E71" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="F70" s="7">
+      <c r="F71" s="7">
         <v>1739.927555</v>
       </c>
-      <c r="G70" s="7"/>
-      <c r="H70" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="K70" s="3" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="71" spans="1:26" s="21" customFormat="1" ht="14.4">
-      <c r="A71" s="20"/>
-      <c r="B71" s="20"/>
-      <c r="E71" s="7" t="s">
-        <v>959</v>
-      </c>
-      <c r="F71" s="7"/>
-      <c r="G71" s="7" t="s">
-        <v>109</v>
-      </c>
+      <c r="G71" s="7"/>
       <c r="H71" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="I71" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="J71" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="K71" s="3"/>
+      <c r="K71" s="3" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="72" spans="1:26" s="21" customFormat="1" ht="14.4">
       <c r="A72" s="20"/>
       <c r="B72" s="20"/>
       <c r="E72" s="7" t="s">
-        <v>497</v>
+        <v>959</v>
       </c>
       <c r="F72" s="7"/>
-      <c r="G72" s="7"/>
-      <c r="H72" s="7"/>
-      <c r="K72" s="3" t="s">
-        <v>941</v>
-      </c>
+      <c r="G72" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="H72" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="I72" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="J72" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="K72" s="3"/>
     </row>
     <row r="73" spans="1:26" s="21" customFormat="1" ht="14.4">
       <c r="A73" s="20"/>
       <c r="B73" s="20"/>
       <c r="E73" s="7" t="s">
-        <v>854</v>
+        <v>497</v>
       </c>
       <c r="F73" s="7"/>
-      <c r="G73" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="H73" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="I73" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="J73" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="K73" s="21" t="s">
-        <v>856</v>
-      </c>
-      <c r="L73" s="3" t="s">
-        <v>855</v>
+      <c r="G73" s="7"/>
+      <c r="H73" s="7"/>
+      <c r="K73" s="3" t="s">
+        <v>941</v>
       </c>
     </row>
     <row r="74" spans="1:26" s="21" customFormat="1" ht="14.4">
       <c r="A74" s="20"/>
       <c r="B74" s="20"/>
       <c r="E74" s="7" t="s">
-        <v>918</v>
+        <v>854</v>
       </c>
       <c r="F74" s="7"/>
       <c r="G74" s="7" t="s">
         <v>29</v>
       </c>
       <c r="H74" s="7" t="s">
-        <v>129</v>
+        <v>73</v>
       </c>
       <c r="I74" s="21" t="s">
         <v>34</v>
@@ -22587,42 +22587,36 @@
         <v>30</v>
       </c>
       <c r="K74" s="21" t="s">
-        <v>903</v>
+        <v>856</v>
       </c>
       <c r="L74" s="3" t="s">
         <v>855</v>
       </c>
     </row>
-    <row r="75" spans="1:26" ht="14.4">
-      <c r="A75" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B75" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="C75" s="3" t="s">
-        <v>24</v>
-      </c>
+    <row r="75" spans="1:26" s="21" customFormat="1" ht="14.4">
+      <c r="A75" s="20"/>
+      <c r="B75" s="20"/>
       <c r="E75" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="F75" s="7">
-        <v>1</v>
-      </c>
+        <v>918</v>
+      </c>
+      <c r="F75" s="7"/>
       <c r="G75" s="7" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="H75" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="I75" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="I75" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="J75" s="3" t="s">
+      <c r="J75" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="K75" s="3" t="s">
-        <v>117</v>
+      <c r="K75" s="21" t="s">
+        <v>903</v>
+      </c>
+      <c r="L75" s="3" t="s">
+        <v>855</v>
       </c>
     </row>
     <row r="76" spans="1:26" ht="14.4">
@@ -22632,14 +22626,30 @@
       <c r="B76" s="15" t="s">
         <v>24</v>
       </c>
+      <c r="C76" s="3" t="s">
+        <v>24</v>
+      </c>
       <c r="E76" s="7" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="F76" s="7">
-        <v>553659</v>
-      </c>
-      <c r="G76" s="7"/>
-      <c r="H76" s="7"/>
+        <v>1</v>
+      </c>
+      <c r="G76" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="H76" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="I76" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="J76" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="K76" s="3" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="77" spans="1:26" ht="14.4">
       <c r="A77" s="15" t="s">
@@ -22649,10 +22659,10 @@
         <v>24</v>
       </c>
       <c r="E77" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F77" s="7">
-        <v>4891208</v>
+        <v>553659</v>
       </c>
       <c r="G77" s="7"/>
       <c r="H77" s="7"/>
@@ -22664,106 +22674,89 @@
       <c r="B78" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="C78" s="3" t="s">
+      <c r="E78" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="F78" s="7">
+        <v>4891208</v>
+      </c>
+      <c r="G78" s="7"/>
+      <c r="H78" s="7"/>
+    </row>
+    <row r="79" spans="1:26" ht="14.4">
+      <c r="A79" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B79" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="E78" s="7" t="s">
+      <c r="C79" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E79" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="F78" s="7">
+      <c r="F79" s="7">
         <v>1</v>
       </c>
-      <c r="G78" s="7" t="s">
+      <c r="G79" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="H78" s="7" t="s">
+      <c r="H79" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="I78" s="3" t="s">
+      <c r="I79" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="J78" s="3" t="s">
+      <c r="J79" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="K78" s="3" t="s">
+      <c r="K79" s="3" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="79" spans="1:26" s="21" customFormat="1" ht="14.4">
-      <c r="A79" s="20"/>
-      <c r="B79" s="20"/>
-      <c r="C79" s="3"/>
-      <c r="E79" s="7" t="s">
+    <row r="80" spans="1:26" s="21" customFormat="1" ht="14.4">
+      <c r="A80" s="20"/>
+      <c r="B80" s="20"/>
+      <c r="C80" s="3"/>
+      <c r="E80" s="7" t="s">
         <v>934</v>
       </c>
-      <c r="F79" s="7"/>
-      <c r="G79" s="7"/>
-      <c r="H79" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="I79" s="3"/>
-      <c r="J79" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="K79" s="3" t="s">
-        <v>936</v>
-      </c>
-    </row>
-    <row r="80" spans="1:26" s="21" customFormat="1" ht="14.4">
-      <c r="A80" s="20" t="s">
-        <v>837</v>
-      </c>
-      <c r="B80" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="C80" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="D80" s="21" t="s">
-        <v>65</v>
-      </c>
-      <c r="E80" s="7" t="s">
-        <v>836</v>
-      </c>
-      <c r="F80" s="7">
-        <v>5</v>
-      </c>
-      <c r="G80" s="7" t="s">
-        <v>109</v>
-      </c>
+      <c r="F80" s="7"/>
+      <c r="G80" s="7"/>
       <c r="H80" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="I80" s="3" t="s">
-        <v>26</v>
-      </c>
+      <c r="I80" s="3"/>
       <c r="J80" s="3" t="s">
         <v>27</v>
       </c>
       <c r="K80" s="3" t="s">
-        <v>838</v>
-      </c>
-      <c r="L80" s="23" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12" s="21" customFormat="1" ht="14.4">
+      <c r="A81" s="20" t="s">
+        <v>837</v>
+      </c>
+      <c r="B81" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="C81" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D81" s="21" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="81" spans="1:12" ht="14.4">
-      <c r="A81" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B81" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="D81" s="3" t="s">
-        <v>127</v>
-      </c>
       <c r="E81" s="7" t="s">
-        <v>128</v>
+        <v>836</v>
       </c>
       <c r="F81" s="7">
-        <v>0</v>
-      </c>
-      <c r="G81" s="7"/>
+        <v>5</v>
+      </c>
+      <c r="G81" s="7" t="s">
+        <v>109</v>
+      </c>
       <c r="H81" s="7" t="s">
         <v>129</v>
       </c>
@@ -22774,25 +22767,40 @@
         <v>27</v>
       </c>
       <c r="K81" s="3" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="82" spans="1:12" s="21" customFormat="1" ht="14.4">
-      <c r="A82" s="20"/>
-      <c r="B82" s="20"/>
-      <c r="D82" s="3"/>
+        <v>838</v>
+      </c>
+      <c r="L81" s="23" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12" ht="14.4">
+      <c r="A82" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B82" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D82" s="3" t="s">
+        <v>127</v>
+      </c>
       <c r="E82" s="7" t="s">
-        <v>935</v>
-      </c>
-      <c r="F82" s="7"/>
+        <v>128</v>
+      </c>
+      <c r="F82" s="7">
+        <v>0</v>
+      </c>
       <c r="G82" s="7"/>
       <c r="H82" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="I82" s="3"/>
-      <c r="J82" s="3"/>
+      <c r="I82" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J82" s="3" t="s">
+        <v>27</v>
+      </c>
       <c r="K82" s="3" t="s">
-        <v>937</v>
+        <v>130</v>
       </c>
     </row>
     <row r="83" spans="1:12" s="21" customFormat="1" ht="14.4">
@@ -22800,7 +22808,7 @@
       <c r="B83" s="20"/>
       <c r="D83" s="3"/>
       <c r="E83" s="7" t="s">
-        <v>938</v>
+        <v>935</v>
       </c>
       <c r="F83" s="7"/>
       <c r="G83" s="7"/>
@@ -22810,53 +22818,46 @@
       <c r="I83" s="3"/>
       <c r="J83" s="3"/>
       <c r="K83" s="3" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12" s="21" customFormat="1" ht="14.4">
+      <c r="A84" s="20"/>
+      <c r="B84" s="20"/>
+      <c r="D84" s="3"/>
+      <c r="E84" s="7" t="s">
+        <v>938</v>
+      </c>
+      <c r="F84" s="7"/>
+      <c r="G84" s="7"/>
+      <c r="H84" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="I84" s="3"/>
+      <c r="J84" s="3"/>
+      <c r="K84" s="3" t="s">
         <v>939</v>
       </c>
     </row>
-    <row r="84" spans="1:12" ht="14.4">
-      <c r="A84" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B84" s="15"/>
-      <c r="E84" s="7" t="s">
+    <row r="85" spans="1:12" ht="14.4">
+      <c r="A85" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B85" s="15"/>
+      <c r="E85" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="F84" s="7">
+      <c r="F85" s="7">
         <v>6772</v>
       </c>
-      <c r="G84" s="7"/>
-      <c r="H84" s="7"/>
-    </row>
-    <row r="85" spans="1:12" s="21" customFormat="1" ht="14.4">
-      <c r="A85" s="20"/>
-      <c r="B85" s="20"/>
-      <c r="E85" s="7" t="s">
-        <v>952</v>
-      </c>
-      <c r="F85" s="7">
-        <v>5</v>
-      </c>
-      <c r="G85" s="58" t="s">
-        <v>109</v>
-      </c>
-      <c r="H85" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="I85" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="J85" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="K85" s="23" t="s">
-        <v>953</v>
-      </c>
+      <c r="G85" s="7"/>
+      <c r="H85" s="7"/>
     </row>
     <row r="86" spans="1:12" s="21" customFormat="1" ht="14.4">
       <c r="A86" s="20"/>
       <c r="B86" s="20"/>
-      <c r="E86" s="58" t="s">
-        <v>954</v>
+      <c r="E86" s="7" t="s">
+        <v>952</v>
       </c>
       <c r="F86" s="7">
         <v>5</v>
@@ -22874,14 +22875,14 @@
         <v>30</v>
       </c>
       <c r="K86" s="23" t="s">
-        <v>955</v>
+        <v>953</v>
       </c>
     </row>
     <row r="87" spans="1:12" s="21" customFormat="1" ht="14.4">
       <c r="A87" s="20"/>
       <c r="B87" s="20"/>
       <c r="E87" s="58" t="s">
-        <v>956</v>
+        <v>954</v>
       </c>
       <c r="F87" s="7">
         <v>5</v>
@@ -22899,82 +22900,87 @@
         <v>30</v>
       </c>
       <c r="K87" s="23" t="s">
-        <v>957</v>
+        <v>955</v>
       </c>
     </row>
     <row r="88" spans="1:12" s="21" customFormat="1" ht="14.4">
       <c r="A88" s="20"/>
       <c r="B88" s="20"/>
-      <c r="E88" s="7" t="s">
-        <v>843</v>
+      <c r="E88" s="58" t="s">
+        <v>956</v>
       </c>
       <c r="F88" s="7">
-        <v>1</v>
-      </c>
-      <c r="G88" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G88" s="58" t="s">
         <v>109</v>
       </c>
       <c r="H88" s="7" t="s">
-        <v>844</v>
-      </c>
-      <c r="I88" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="J88" s="23" t="s">
-        <v>845</v>
+        <v>129</v>
+      </c>
+      <c r="I88" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="J88" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="K88" s="23" t="s">
+        <v>957</v>
       </c>
     </row>
     <row r="89" spans="1:12" s="21" customFormat="1" ht="14.4">
       <c r="A89" s="20"/>
       <c r="B89" s="20"/>
       <c r="E89" s="7" t="s">
-        <v>978</v>
-      </c>
-      <c r="F89" s="7"/>
+        <v>843</v>
+      </c>
+      <c r="F89" s="7">
+        <v>1</v>
+      </c>
       <c r="G89" s="7" t="s">
         <v>109</v>
       </c>
       <c r="H89" s="7" t="s">
-        <v>63</v>
+        <v>844</v>
       </c>
       <c r="I89" s="23" t="s">
         <v>26</v>
       </c>
       <c r="J89" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="K89" s="23" t="s">
-        <v>979</v>
-      </c>
-      <c r="L89" s="23" t="s">
-        <v>977</v>
+        <v>845</v>
       </c>
     </row>
     <row r="90" spans="1:12" s="21" customFormat="1" ht="14.4">
       <c r="A90" s="20"/>
       <c r="B90" s="20"/>
       <c r="E90" s="7" t="s">
-        <v>950</v>
+        <v>978</v>
       </c>
       <c r="F90" s="7"/>
       <c r="G90" s="7" t="s">
         <v>109</v>
       </c>
       <c r="H90" s="7" t="s">
-        <v>626</v>
-      </c>
-      <c r="I90" s="23"/>
-      <c r="J90" s="23"/>
+        <v>63</v>
+      </c>
+      <c r="I90" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="J90" s="23" t="s">
+        <v>27</v>
+      </c>
       <c r="K90" s="23" t="s">
-        <v>980</v>
-      </c>
-      <c r="L90" s="23"/>
+        <v>979</v>
+      </c>
+      <c r="L90" s="23" t="s">
+        <v>977</v>
+      </c>
     </row>
     <row r="91" spans="1:12" s="21" customFormat="1" ht="14.4">
       <c r="A91" s="20"/>
       <c r="B91" s="20"/>
       <c r="E91" s="7" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="F91" s="7"/>
       <c r="G91" s="7" t="s">
@@ -22986,69 +22992,66 @@
       <c r="I91" s="23"/>
       <c r="J91" s="23"/>
       <c r="K91" s="23" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
       <c r="L91" s="23"/>
     </row>
     <row r="92" spans="1:12" s="21" customFormat="1" ht="14.4">
       <c r="A92" s="20"/>
       <c r="B92" s="20"/>
-      <c r="D92" s="57" t="s">
-        <v>944</v>
-      </c>
       <c r="E92" s="7" t="s">
-        <v>970</v>
+        <v>951</v>
       </c>
       <c r="F92" s="7"/>
-      <c r="G92" s="58" t="s">
+      <c r="G92" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="H92" s="58" t="s">
-        <v>84</v>
-      </c>
-      <c r="I92" s="23" t="s">
-        <v>947</v>
-      </c>
-      <c r="J92" s="23" t="s">
-        <v>947</v>
-      </c>
+      <c r="H92" s="7" t="s">
+        <v>626</v>
+      </c>
+      <c r="I92" s="23"/>
+      <c r="J92" s="23"/>
       <c r="K92" s="23" t="s">
-        <v>971</v>
+        <v>981</v>
       </c>
       <c r="L92" s="23"/>
     </row>
     <row r="93" spans="1:12" s="21" customFormat="1" ht="14.4">
       <c r="A93" s="20"/>
       <c r="B93" s="20"/>
+      <c r="D93" s="57" t="s">
+        <v>944</v>
+      </c>
       <c r="E93" s="7" t="s">
-        <v>842</v>
-      </c>
-      <c r="F93" s="7">
-        <v>10</v>
-      </c>
-      <c r="G93" s="7" t="s">
+        <v>970</v>
+      </c>
+      <c r="F93" s="7"/>
+      <c r="G93" s="58" t="s">
         <v>109</v>
       </c>
-      <c r="H93" s="7" t="s">
-        <v>626</v>
+      <c r="H93" s="58" t="s">
+        <v>84</v>
       </c>
       <c r="I93" s="23" t="s">
-        <v>26</v>
+        <v>947</v>
       </c>
       <c r="J93" s="23" t="s">
-        <v>27</v>
+        <v>947</v>
       </c>
       <c r="K93" s="23" t="s">
-        <v>848</v>
-      </c>
+        <v>971</v>
+      </c>
+      <c r="L93" s="23"/>
     </row>
     <row r="94" spans="1:12" s="21" customFormat="1" ht="14.4">
       <c r="A94" s="20"/>
       <c r="B94" s="20"/>
       <c r="E94" s="7" t="s">
-        <v>960</v>
-      </c>
-      <c r="F94" s="7"/>
+        <v>842</v>
+      </c>
+      <c r="F94" s="7">
+        <v>10</v>
+      </c>
       <c r="G94" s="7" t="s">
         <v>109</v>
       </c>
@@ -23056,20 +23059,20 @@
         <v>626</v>
       </c>
       <c r="I94" s="23" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="J94" s="23" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="K94" s="23" t="s">
-        <v>961</v>
+        <v>848</v>
       </c>
     </row>
     <row r="95" spans="1:12" s="21" customFormat="1" ht="14.4">
       <c r="A95" s="20"/>
       <c r="B95" s="20"/>
       <c r="E95" s="7" t="s">
-        <v>974</v>
+        <v>960</v>
       </c>
       <c r="F95" s="7"/>
       <c r="G95" s="7" t="s">
@@ -23078,70 +23081,65 @@
       <c r="H95" s="7" t="s">
         <v>626</v>
       </c>
-      <c r="I95" s="23"/>
+      <c r="I95" s="23" t="s">
+        <v>34</v>
+      </c>
       <c r="J95" s="23" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="K95" s="23" t="s">
-        <v>975</v>
-      </c>
-      <c r="L95" s="23" t="s">
-        <v>976</v>
+        <v>961</v>
       </c>
     </row>
     <row r="96" spans="1:12" s="21" customFormat="1" ht="14.4">
       <c r="A96" s="20"/>
       <c r="B96" s="20"/>
       <c r="E96" s="7" t="s">
-        <v>510</v>
+        <v>974</v>
       </c>
       <c r="F96" s="7"/>
-      <c r="G96" s="7"/>
+      <c r="G96" s="7" t="s">
+        <v>109</v>
+      </c>
       <c r="H96" s="7" t="s">
-        <v>511</v>
+        <v>626</v>
       </c>
       <c r="I96" s="23"/>
-      <c r="J96" s="23"/>
+      <c r="J96" s="23" t="s">
+        <v>27</v>
+      </c>
       <c r="K96" s="23" t="s">
-        <v>943</v>
+        <v>975</v>
+      </c>
+      <c r="L96" s="23" t="s">
+        <v>976</v>
       </c>
     </row>
     <row r="97" spans="1:11" s="21" customFormat="1" ht="14.4">
       <c r="A97" s="20"/>
       <c r="B97" s="20"/>
-      <c r="D97" s="57" t="s">
-        <v>25</v>
-      </c>
       <c r="E97" s="7" t="s">
-        <v>796</v>
+        <v>510</v>
       </c>
       <c r="F97" s="7"/>
-      <c r="G97" s="58" t="s">
-        <v>29</v>
-      </c>
+      <c r="G97" s="7"/>
       <c r="H97" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="I97" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="J97" s="23" t="s">
-        <v>27</v>
-      </c>
+        <v>511</v>
+      </c>
+      <c r="I97" s="23"/>
+      <c r="J97" s="23"/>
       <c r="K97" s="23" t="s">
-        <v>797</v>
+        <v>943</v>
       </c>
     </row>
     <row r="98" spans="1:11" s="21" customFormat="1" ht="14.4">
-      <c r="A98" s="20" t="s">
-        <v>23</v>
-      </c>
+      <c r="A98" s="20"/>
       <c r="B98" s="20"/>
       <c r="D98" s="57" t="s">
         <v>25</v>
       </c>
       <c r="E98" s="7" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
       <c r="F98" s="7"/>
       <c r="G98" s="58" t="s">
@@ -23157,39 +23155,35 @@
         <v>27</v>
       </c>
       <c r="K98" s="23" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11" s="21" customFormat="1" ht="14.4">
+      <c r="A99" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="B99" s="20"/>
+      <c r="D99" s="57" t="s">
+        <v>25</v>
+      </c>
+      <c r="E99" s="7" t="s">
+        <v>798</v>
+      </c>
+      <c r="F99" s="7"/>
+      <c r="G99" s="58" t="s">
+        <v>29</v>
+      </c>
+      <c r="H99" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="I99" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="J99" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="K99" s="23" t="s">
         <v>799</v>
-      </c>
-    </row>
-    <row r="99" spans="1:11" ht="14.4">
-      <c r="A99" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B99" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="D99" s="17" t="s">
-        <v>133</v>
-      </c>
-      <c r="E99" s="18" t="s">
-        <v>135</v>
-      </c>
-      <c r="F99" s="18">
-        <v>1500</v>
-      </c>
-      <c r="G99" s="18" t="s">
-        <v>109</v>
-      </c>
-      <c r="H99" s="18" t="s">
-        <v>84</v>
-      </c>
-      <c r="I99" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="J99" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="K99" s="17" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="100" spans="1:11" ht="14.4">
@@ -23202,16 +23196,16 @@
       <c r="D100" s="17" t="s">
         <v>133</v>
       </c>
-      <c r="E100" s="17" t="s">
-        <v>140</v>
-      </c>
-      <c r="F100" s="17">
+      <c r="E100" s="18" t="s">
+        <v>135</v>
+      </c>
+      <c r="F100" s="18">
         <v>1500</v>
       </c>
       <c r="G100" s="18" t="s">
         <v>109</v>
       </c>
-      <c r="H100" s="17" t="s">
+      <c r="H100" s="18" t="s">
         <v>84</v>
       </c>
       <c r="I100" s="17" t="s">
@@ -23221,7 +23215,7 @@
         <v>30</v>
       </c>
       <c r="K100" s="17" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="101" spans="1:11" ht="14.4">
@@ -23235,7 +23229,7 @@
         <v>133</v>
       </c>
       <c r="E101" s="17" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="F101" s="17">
         <v>1500</v>
@@ -23253,6 +23247,38 @@
         <v>30</v>
       </c>
       <c r="K101" s="17" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11" ht="14.4">
+      <c r="A102" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B102" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="D102" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="E102" s="17" t="s">
+        <v>143</v>
+      </c>
+      <c r="F102" s="17">
+        <v>1500</v>
+      </c>
+      <c r="G102" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="H102" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="I102" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="J102" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="K102" s="17" t="s">
         <v>144</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Flow.cpp - Correct the logic error in the code which reads the SAL input file which was causing all the widths to be the same.
</commit_message>
<xml_diff>
--- a/DataCW3M/CW3MdigitalHandbook/CW3MdataDictionary.xlsx
+++ b/DataCW3M/CW3MdigitalHandbook/CW3MdataDictionary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\CW3MdigitalHandbook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B9DD3A8-80AA-4275-B7AB-12B63BE2FD42}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3845F36-93BD-4809-A3D5-9DFE7D07D509}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-7425" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -96,7 +96,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2951" uniqueCount="985">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2957" uniqueCount="988">
   <si>
     <t>LULC_A</t>
   </si>
@@ -3052,6 +3052,15 @@
   </si>
   <si>
     <t>1 =&gt; this reach is completely covered by  the Shade-a-lator data</t>
+  </si>
+  <si>
+    <t>KCAL_REACH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">today's kcal from RAD_SW_IN </t>
+  </si>
+  <si>
+    <t>kcal</t>
   </si>
 </sst>
 </file>
@@ -20724,11 +20733,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Z102"/>
+  <dimension ref="A1:Z103"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A57" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K70" sqref="K70"/>
+      <pane ySplit="4" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J41" sqref="J41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -21777,16 +21786,14 @@
       <c r="A41" s="20"/>
       <c r="B41" s="20"/>
       <c r="E41" s="7" t="s">
-        <v>431</v>
-      </c>
-      <c r="F41" s="7">
-        <v>1.3</v>
-      </c>
+        <v>985</v>
+      </c>
+      <c r="F41" s="7"/>
       <c r="G41" s="21" t="s">
         <v>109</v>
       </c>
       <c r="H41" s="21" t="s">
-        <v>969</v>
+        <v>987</v>
       </c>
       <c r="I41" s="21" t="s">
         <v>26</v>
@@ -21795,16 +21802,18 @@
         <v>27</v>
       </c>
       <c r="K41" s="23" t="s">
-        <v>968</v>
+        <v>986</v>
       </c>
     </row>
     <row r="42" spans="1:12" s="21" customFormat="1" ht="14.4">
       <c r="A42" s="20"/>
       <c r="B42" s="20"/>
       <c r="E42" s="7" t="s">
-        <v>972</v>
-      </c>
-      <c r="F42" s="7"/>
+        <v>431</v>
+      </c>
+      <c r="F42" s="7">
+        <v>1.3</v>
+      </c>
       <c r="G42" s="21" t="s">
         <v>109</v>
       </c>
@@ -21820,38 +21829,31 @@
       <c r="K42" s="23" t="s">
         <v>968</v>
       </c>
-      <c r="L42" s="21" t="s">
+    </row>
+    <row r="43" spans="1:12" s="21" customFormat="1" ht="14.4">
+      <c r="A43" s="20"/>
+      <c r="B43" s="20"/>
+      <c r="E43" s="7" t="s">
+        <v>972</v>
+      </c>
+      <c r="F43" s="7"/>
+      <c r="G43" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="H43" s="21" t="s">
+        <v>969</v>
+      </c>
+      <c r="I43" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="J43" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="K43" s="23" t="s">
+        <v>968</v>
+      </c>
+      <c r="L43" s="21" t="s">
         <v>973</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" ht="14.4">
-      <c r="A43" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B43" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E43" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="F43" s="7">
-        <v>1739.9274680000001</v>
-      </c>
-      <c r="G43" s="7"/>
-      <c r="H43" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="I43" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="J43" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="K43" s="3" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="44" spans="1:12" ht="14.4">
@@ -21861,17 +21863,28 @@
       <c r="B44" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="D44" s="3" t="s">
-        <v>44</v>
+      <c r="C44" s="3" t="s">
+        <v>24</v>
       </c>
       <c r="E44" s="7" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F44" s="7">
-        <v>6699</v>
+        <v>1739.9274680000001</v>
       </c>
       <c r="G44" s="7"/>
-      <c r="H44" s="7"/>
+      <c r="H44" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="I44" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="J44" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="K44" s="3" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="45" spans="1:12" ht="14.4">
       <c r="A45" s="15" t="s">
@@ -21880,22 +21893,17 @@
       <c r="B45" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="D45" t="s">
-        <v>908</v>
+      <c r="D45" s="3" t="s">
+        <v>44</v>
       </c>
       <c r="E45" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F45" s="7">
-        <v>0</v>
-      </c>
-      <c r="G45" s="7" t="s">
-        <v>909</v>
-      </c>
+        <v>6699</v>
+      </c>
+      <c r="G45" s="7"/>
       <c r="H45" s="7"/>
-      <c r="K45" s="23" t="s">
-        <v>910</v>
-      </c>
     </row>
     <row r="46" spans="1:12" ht="14.4">
       <c r="A46" s="15" t="s">
@@ -21904,47 +21912,41 @@
       <c r="B46" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="D46" s="3" t="s">
+      <c r="D46" t="s">
+        <v>908</v>
+      </c>
+      <c r="E46" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="F46" s="7">
+        <v>0</v>
+      </c>
+      <c r="G46" s="7" t="s">
+        <v>909</v>
+      </c>
+      <c r="H46" s="7"/>
+      <c r="K46" s="23" t="s">
+        <v>910</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" ht="14.4">
+      <c r="A47" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B47" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D47" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="E46" s="7" t="s">
+      <c r="E47" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="F46" s="7">
+      <c r="F47" s="7">
         <v>6758</v>
       </c>
-      <c r="G46" s="7"/>
-      <c r="H46" s="7"/>
-    </row>
-    <row r="47" spans="1:12" s="21" customFormat="1" ht="14.4">
-      <c r="A47" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="B47" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="D47" s="3" t="s">
-        <v>804</v>
-      </c>
-      <c r="E47" s="7" t="s">
-        <v>801</v>
-      </c>
-      <c r="F47" s="7"/>
-      <c r="G47" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="H47" s="58" t="s">
-        <v>73</v>
-      </c>
-      <c r="I47" s="57" t="s">
-        <v>26</v>
-      </c>
-      <c r="J47" s="57" t="s">
-        <v>27</v>
-      </c>
-      <c r="K47" s="57" t="s">
-        <v>803</v>
-      </c>
+      <c r="G47" s="7"/>
+      <c r="H47" s="7"/>
     </row>
     <row r="48" spans="1:12" s="21" customFormat="1" ht="14.4">
       <c r="A48" s="20" t="s">
@@ -21957,14 +21959,14 @@
         <v>804</v>
       </c>
       <c r="E48" s="7" t="s">
-        <v>931</v>
+        <v>801</v>
       </c>
       <c r="F48" s="7"/>
       <c r="G48" s="7" t="s">
-        <v>109</v>
+        <v>29</v>
       </c>
       <c r="H48" s="58" t="s">
-        <v>129</v>
+        <v>73</v>
       </c>
       <c r="I48" s="57" t="s">
         <v>26</v>
@@ -21973,7 +21975,7 @@
         <v>27</v>
       </c>
       <c r="K48" s="57" t="s">
-        <v>932</v>
+        <v>803</v>
       </c>
     </row>
     <row r="49" spans="1:11" s="21" customFormat="1" ht="14.4">
@@ -21984,17 +21986,17 @@
         <v>24</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>805</v>
-      </c>
-      <c r="E49" s="58" t="s">
-        <v>802</v>
+        <v>804</v>
+      </c>
+      <c r="E49" s="7" t="s">
+        <v>931</v>
       </c>
       <c r="F49" s="7"/>
       <c r="G49" s="7" t="s">
-        <v>29</v>
+        <v>109</v>
       </c>
       <c r="H49" s="58" t="s">
-        <v>73</v>
+        <v>129</v>
       </c>
       <c r="I49" s="57" t="s">
         <v>26</v>
@@ -22003,48 +22005,55 @@
         <v>27</v>
       </c>
       <c r="K49" s="57" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" s="21" customFormat="1" ht="14.4">
+      <c r="A50" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="B50" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>805</v>
+      </c>
+      <c r="E50" s="58" t="s">
+        <v>802</v>
+      </c>
+      <c r="F50" s="7"/>
+      <c r="G50" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H50" s="58" t="s">
+        <v>73</v>
+      </c>
+      <c r="I50" s="57" t="s">
+        <v>26</v>
+      </c>
+      <c r="J50" s="57" t="s">
+        <v>27</v>
+      </c>
+      <c r="K50" s="57" t="s">
         <v>806</v>
       </c>
     </row>
-    <row r="50" spans="1:11" s="21" customFormat="1" ht="14.4">
-      <c r="A50" s="20"/>
-      <c r="B50" s="20"/>
-      <c r="D50" s="3"/>
-      <c r="E50" s="58" t="s">
+    <row r="51" spans="1:11" s="21" customFormat="1" ht="14.4">
+      <c r="A51" s="20"/>
+      <c r="B51" s="20"/>
+      <c r="D51" s="3"/>
+      <c r="E51" s="58" t="s">
         <v>420</v>
       </c>
-      <c r="F50" s="7"/>
-      <c r="G50" s="7"/>
-      <c r="H50" s="58" t="s">
+      <c r="F51" s="7"/>
+      <c r="G51" s="7"/>
+      <c r="H51" s="58" t="s">
         <v>173</v>
       </c>
-      <c r="I50" s="57"/>
-      <c r="J50" s="57"/>
-      <c r="K50" s="57" t="s">
+      <c r="I51" s="57"/>
+      <c r="J51" s="57"/>
+      <c r="K51" s="57" t="s">
         <v>940</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11" ht="14.4">
-      <c r="A51" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B51" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="E51" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="F51" s="7">
-        <v>0</v>
-      </c>
-      <c r="G51" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="H51" s="57" t="s">
-        <v>73</v>
-      </c>
-      <c r="I51" s="17" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="52" spans="1:11" ht="14.4">
@@ -22055,102 +22064,105 @@
         <v>24</v>
       </c>
       <c r="E52" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F52" s="7">
         <v>0</v>
       </c>
-      <c r="G52" s="7"/>
-      <c r="H52" s="7"/>
-      <c r="K52" s="17" t="s">
+      <c r="G52" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="H52" s="57" t="s">
+        <v>73</v>
+      </c>
+      <c r="I52" s="17" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" ht="14.4">
+      <c r="A53" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B53" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="E53" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="F53" s="7">
+        <v>0</v>
+      </c>
+      <c r="G53" s="7"/>
+      <c r="H53" s="7"/>
+      <c r="K53" s="17" t="s">
         <v>91</v>
-      </c>
-    </row>
-    <row r="53" spans="1:11" s="21" customFormat="1" ht="14.4">
-      <c r="A53" s="20"/>
-      <c r="B53" s="20"/>
-      <c r="E53" s="7" t="s">
-        <v>859</v>
-      </c>
-      <c r="F53" s="7">
-        <v>0.08</v>
-      </c>
-      <c r="G53" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="H53" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="I53" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="J53" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="K53" s="23" t="s">
-        <v>860</v>
       </c>
     </row>
     <row r="54" spans="1:11" s="21" customFormat="1" ht="14.4">
       <c r="A54" s="20"/>
       <c r="B54" s="20"/>
-      <c r="E54" s="58" t="s">
-        <v>840</v>
-      </c>
-      <c r="F54" s="7"/>
+      <c r="E54" s="7" t="s">
+        <v>859</v>
+      </c>
+      <c r="F54" s="7">
+        <v>0.08</v>
+      </c>
       <c r="G54" s="7" t="s">
         <v>109</v>
       </c>
       <c r="H54" s="7" t="s">
-        <v>475</v>
+        <v>73</v>
       </c>
       <c r="I54" s="21" t="s">
-        <v>26</v>
+        <v>34</v>
+      </c>
+      <c r="J54" s="21" t="s">
+        <v>30</v>
       </c>
       <c r="K54" s="23" t="s">
-        <v>841</v>
+        <v>860</v>
       </c>
     </row>
     <row r="55" spans="1:11" s="21" customFormat="1" ht="14.4">
       <c r="A55" s="20"/>
       <c r="B55" s="20"/>
       <c r="E55" s="58" t="s">
-        <v>473</v>
+        <v>840</v>
       </c>
       <c r="F55" s="7"/>
-      <c r="G55" s="7"/>
+      <c r="G55" s="7" t="s">
+        <v>109</v>
+      </c>
       <c r="H55" s="7" t="s">
         <v>475</v>
       </c>
+      <c r="I55" s="21" t="s">
+        <v>26</v>
+      </c>
       <c r="K55" s="23" t="s">
-        <v>942</v>
+        <v>841</v>
       </c>
     </row>
     <row r="56" spans="1:11" s="21" customFormat="1" ht="14.4">
       <c r="A56" s="20"/>
       <c r="B56" s="20"/>
-      <c r="E56" s="7" t="s">
-        <v>839</v>
+      <c r="E56" s="58" t="s">
+        <v>473</v>
       </c>
       <c r="F56" s="7"/>
-      <c r="G56" s="7" t="s">
-        <v>109</v>
-      </c>
+      <c r="G56" s="7"/>
       <c r="H56" s="7" t="s">
         <v>475</v>
       </c>
-      <c r="I56" s="21" t="s">
-        <v>26</v>
-      </c>
       <c r="K56" s="23" t="s">
-        <v>853</v>
+        <v>942</v>
       </c>
     </row>
     <row r="57" spans="1:11" s="21" customFormat="1" ht="14.4">
       <c r="A57" s="20"/>
       <c r="B57" s="20"/>
       <c r="E57" s="7" t="s">
-        <v>962</v>
+        <v>839</v>
       </c>
       <c r="F57" s="7"/>
       <c r="G57" s="7" t="s">
@@ -22160,86 +22172,81 @@
         <v>475</v>
       </c>
       <c r="I57" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="K57" s="23" t="s">
+        <v>853</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" s="21" customFormat="1" ht="14.4">
+      <c r="A58" s="20"/>
+      <c r="B58" s="20"/>
+      <c r="E58" s="7" t="s">
+        <v>962</v>
+      </c>
+      <c r="F58" s="7"/>
+      <c r="G58" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="H58" s="7" t="s">
+        <v>475</v>
+      </c>
+      <c r="I58" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="K57" s="23" t="s">
+      <c r="K58" s="23" t="s">
         <v>963</v>
       </c>
     </row>
-    <row r="58" spans="1:11" ht="14.4">
-      <c r="A58" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="B58" s="24" t="s">
+    <row r="59" spans="1:11" ht="14.4">
+      <c r="A59" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B59" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="C58" s="17" t="s">
+      <c r="C59" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="D58" s="17" t="s">
+      <c r="D59" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="E58" s="18" t="s">
+      <c r="E59" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="F58" s="7"/>
-      <c r="G58" s="18" t="s">
+      <c r="F59" s="7"/>
+      <c r="G59" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="H58" s="18" t="s">
+      <c r="H59" s="18" t="s">
         <v>95</v>
       </c>
-      <c r="I58" s="17" t="s">
+      <c r="I59" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="J58" s="17" t="s">
+      <c r="J59" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="K58" s="17" t="s">
+      <c r="K59" s="17" t="s">
         <v>96</v>
-      </c>
-    </row>
-    <row r="59" spans="1:11" s="21" customFormat="1" ht="14.4">
-      <c r="A59" s="20"/>
-      <c r="B59" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="C59" s="22"/>
-      <c r="D59" s="22"/>
-      <c r="E59" s="21" t="s">
-        <v>916</v>
-      </c>
-      <c r="F59" s="7"/>
-      <c r="G59" s="21" t="s">
-        <v>109</v>
-      </c>
-      <c r="H59" s="21" t="s">
-        <v>917</v>
-      </c>
-      <c r="I59" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="J59" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="K59" s="23" t="s">
-        <v>911</v>
       </c>
     </row>
     <row r="60" spans="1:11" s="21" customFormat="1" ht="14.4">
       <c r="A60" s="20"/>
-      <c r="B60" s="24"/>
+      <c r="B60" s="24" t="s">
+        <v>23</v>
+      </c>
       <c r="C60" s="22"/>
       <c r="D60" s="22"/>
       <c r="E60" s="21" t="s">
-        <v>919</v>
+        <v>916</v>
       </c>
       <c r="F60" s="7"/>
       <c r="G60" s="21" t="s">
         <v>109</v>
       </c>
       <c r="H60" s="21" t="s">
-        <v>407</v>
+        <v>917</v>
       </c>
       <c r="I60" s="23" t="s">
         <v>26</v>
@@ -22248,25 +22255,23 @@
         <v>27</v>
       </c>
       <c r="K60" s="23" t="s">
-        <v>920</v>
+        <v>911</v>
       </c>
     </row>
     <row r="61" spans="1:11" s="21" customFormat="1" ht="14.4">
       <c r="A61" s="20"/>
-      <c r="B61" s="24" t="s">
-        <v>23</v>
-      </c>
+      <c r="B61" s="24"/>
       <c r="C61" s="22"/>
       <c r="D61" s="22"/>
       <c r="E61" s="21" t="s">
-        <v>912</v>
+        <v>919</v>
       </c>
       <c r="F61" s="7"/>
       <c r="G61" s="21" t="s">
         <v>109</v>
       </c>
       <c r="H61" s="21" t="s">
-        <v>95</v>
+        <v>407</v>
       </c>
       <c r="I61" s="23" t="s">
         <v>26</v>
@@ -22275,336 +22280,337 @@
         <v>27</v>
       </c>
       <c r="K61" s="23" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" s="21" customFormat="1" ht="14.4">
+      <c r="A62" s="20"/>
+      <c r="B62" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="C62" s="22"/>
+      <c r="D62" s="22"/>
+      <c r="E62" s="21" t="s">
+        <v>912</v>
+      </c>
+      <c r="F62" s="7"/>
+      <c r="G62" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="H62" s="21" t="s">
+        <v>95</v>
+      </c>
+      <c r="I62" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="J62" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="K62" s="23" t="s">
         <v>913</v>
       </c>
     </row>
-    <row r="62" spans="1:11" ht="43.2">
-      <c r="A62" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B62" s="15" t="s">
+    <row r="63" spans="1:11" ht="43.2">
+      <c r="A63" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B63" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="E62" s="7" t="s">
+      <c r="E63" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="F62" s="18">
+      <c r="F63" s="18">
         <v>1</v>
       </c>
-      <c r="G62" s="18" t="s">
+      <c r="G63" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="H62" s="18" t="s">
+      <c r="H63" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="J62" s="17" t="s">
+      <c r="J63" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="K62" s="19" t="s">
+      <c r="K63" s="19" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="63" spans="1:11" s="21" customFormat="1" ht="14.4">
-      <c r="A63" s="20"/>
-      <c r="B63" s="20"/>
-      <c r="E63" s="7" t="s">
+    <row r="64" spans="1:11" s="21" customFormat="1" ht="14.4">
+      <c r="A64" s="20"/>
+      <c r="B64" s="20"/>
+      <c r="E64" s="7" t="s">
         <v>921</v>
       </c>
-      <c r="G63" s="21" t="s">
+      <c r="G64" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="H63" s="21" t="s">
+      <c r="H64" s="21" t="s">
         <v>475</v>
       </c>
-      <c r="I63" s="23" t="s">
+      <c r="I64" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="J63" s="23" t="s">
+      <c r="J64" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="K63" s="23" t="s">
+      <c r="K64" s="23" t="s">
         <v>922</v>
       </c>
     </row>
-    <row r="64" spans="1:11" s="25" customFormat="1" ht="86.4">
-      <c r="A64" s="81"/>
-      <c r="B64" s="81"/>
-      <c r="E64" s="25" t="s">
-        <v>101</v>
-      </c>
-      <c r="F64" s="25">
-        <v>1</v>
-      </c>
-      <c r="G64" s="25" t="s">
-        <v>98</v>
-      </c>
-      <c r="H64" s="25" t="s">
-        <v>99</v>
-      </c>
-      <c r="I64" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="J64" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="K64" s="80" t="s">
-        <v>933</v>
-      </c>
-    </row>
-    <row r="65" spans="1:26" s="25" customFormat="1" ht="14.4">
+    <row r="65" spans="1:26" s="25" customFormat="1" ht="86.4">
       <c r="A65" s="81"/>
       <c r="B65" s="81"/>
-      <c r="E65" s="72" t="s">
+      <c r="E65" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="F65" s="25">
+        <v>1</v>
+      </c>
+      <c r="G65" s="25" t="s">
+        <v>98</v>
+      </c>
+      <c r="H65" s="25" t="s">
+        <v>99</v>
+      </c>
+      <c r="I65" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="J65" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="K65" s="80" t="s">
+        <v>933</v>
+      </c>
+    </row>
+    <row r="66" spans="1:26" s="25" customFormat="1" ht="14.4">
+      <c r="A66" s="81"/>
+      <c r="B66" s="81"/>
+      <c r="E66" s="72" t="s">
         <v>923</v>
       </c>
-      <c r="G65" s="72" t="s">
+      <c r="G66" s="72" t="s">
         <v>109</v>
       </c>
-      <c r="H65" s="72" t="s">
+      <c r="H66" s="72" t="s">
         <v>475</v>
-      </c>
-      <c r="I65" s="80" t="s">
-        <v>26</v>
-      </c>
-      <c r="J65" s="80" t="s">
-        <v>27</v>
-      </c>
-      <c r="K65" s="23" t="s">
-        <v>924</v>
-      </c>
-    </row>
-    <row r="66" spans="1:26" s="25" customFormat="1" ht="28.8">
-      <c r="A66" s="81"/>
-      <c r="B66" s="81" t="s">
-        <v>23</v>
-      </c>
-      <c r="E66" s="25" t="s">
-        <v>914</v>
-      </c>
-      <c r="G66" s="25" t="s">
-        <v>109</v>
-      </c>
-      <c r="H66" s="25" t="s">
-        <v>129</v>
       </c>
       <c r="I66" s="80" t="s">
         <v>26</v>
       </c>
-      <c r="J66" s="19"/>
-      <c r="K66" s="80" t="s">
+      <c r="J66" s="80" t="s">
+        <v>27</v>
+      </c>
+      <c r="K66" s="23" t="s">
+        <v>924</v>
+      </c>
+    </row>
+    <row r="67" spans="1:26" s="25" customFormat="1" ht="28.8">
+      <c r="A67" s="81"/>
+      <c r="B67" s="81" t="s">
+        <v>23</v>
+      </c>
+      <c r="E67" s="25" t="s">
+        <v>914</v>
+      </c>
+      <c r="G67" s="25" t="s">
+        <v>109</v>
+      </c>
+      <c r="H67" s="25" t="s">
+        <v>129</v>
+      </c>
+      <c r="I67" s="80" t="s">
+        <v>26</v>
+      </c>
+      <c r="J67" s="19"/>
+      <c r="K67" s="80" t="s">
         <v>915</v>
       </c>
     </row>
-    <row r="67" spans="1:26" s="21" customFormat="1" ht="14.25" customHeight="1">
-      <c r="C67" s="28"/>
-      <c r="D67" s="28"/>
-      <c r="E67" s="7" t="s">
+    <row r="68" spans="1:26" s="21" customFormat="1" ht="14.25" customHeight="1">
+      <c r="C68" s="28"/>
+      <c r="D68" s="28"/>
+      <c r="E68" s="7" t="s">
         <v>812</v>
       </c>
-      <c r="F67" s="7"/>
-      <c r="G67" s="70" t="s">
+      <c r="F68" s="7"/>
+      <c r="G68" s="70" t="s">
         <v>29</v>
       </c>
-      <c r="H67" s="70" t="s">
+      <c r="H68" s="70" t="s">
         <v>227</v>
       </c>
-      <c r="I67" s="70" t="s">
+      <c r="I68" s="70" t="s">
         <v>34</v>
       </c>
-      <c r="J67" s="70" t="s">
+      <c r="J68" s="70" t="s">
         <v>27</v>
       </c>
-      <c r="K67" s="57" t="s">
+      <c r="K68" s="57" t="s">
         <v>813</v>
       </c>
-      <c r="L67" s="70" t="s">
+      <c r="L68" s="70" t="s">
         <v>814</v>
       </c>
-      <c r="M67" s="3"/>
-      <c r="N67" s="7"/>
-      <c r="O67" s="7"/>
-      <c r="P67" s="7"/>
-      <c r="Q67" s="7"/>
-      <c r="R67" s="7"/>
-      <c r="S67" s="7"/>
-      <c r="T67" s="7"/>
-      <c r="U67" s="7"/>
-      <c r="V67" s="7"/>
-      <c r="W67" s="7"/>
-      <c r="X67" s="7"/>
-    </row>
-    <row r="68" spans="1:26" ht="14.4">
-      <c r="A68" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B68" s="15" t="s">
+      <c r="M68" s="3"/>
+      <c r="N68" s="7"/>
+      <c r="O68" s="7"/>
+      <c r="P68" s="7"/>
+      <c r="Q68" s="7"/>
+      <c r="R68" s="7"/>
+      <c r="S68" s="7"/>
+      <c r="T68" s="7"/>
+      <c r="U68" s="7"/>
+      <c r="V68" s="7"/>
+      <c r="W68" s="7"/>
+      <c r="X68" s="7"/>
+    </row>
+    <row r="69" spans="1:26" ht="14.4">
+      <c r="A69" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B69" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="E68" s="7" t="s">
+      <c r="E69" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="F68" s="7">
+      <c r="F69" s="7">
         <v>-1</v>
       </c>
-      <c r="G68" s="7"/>
-      <c r="H68" s="7"/>
-    </row>
-    <row r="69" spans="1:26" s="21" customFormat="1" ht="14.4">
-      <c r="A69" s="20"/>
-      <c r="B69" s="20"/>
-      <c r="E69" s="25" t="s">
+      <c r="G69" s="7"/>
+      <c r="H69" s="7"/>
+    </row>
+    <row r="70" spans="1:26" s="21" customFormat="1" ht="14.4">
+      <c r="A70" s="20"/>
+      <c r="B70" s="20"/>
+      <c r="E70" s="25" t="s">
         <v>982</v>
       </c>
-      <c r="F69" s="7" t="s">
+      <c r="F70" s="7" t="s">
         <v>983</v>
       </c>
-      <c r="G69" s="25" t="s">
+      <c r="G70" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="H69" s="7"/>
-      <c r="K69" s="21" t="s">
+      <c r="H70" s="7"/>
+      <c r="K70" s="21" t="s">
         <v>984</v>
       </c>
     </row>
-    <row r="70" spans="1:26" ht="14.4">
-      <c r="A70" s="15"/>
-      <c r="B70" s="15"/>
-      <c r="C70" s="7" t="s">
+    <row r="71" spans="1:26" ht="14.4">
+      <c r="A71" s="15"/>
+      <c r="B71" s="15"/>
+      <c r="C71" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="D70" s="7" t="s">
+      <c r="D71" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="E70" s="7" t="s">
+      <c r="E71" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="F70" s="7">
+      <c r="F71" s="7">
         <v>0.6</v>
       </c>
-      <c r="G70" s="7" t="s">
+      <c r="G71" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="H70" s="7" t="s">
+      <c r="H71" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="I70" s="7" t="s">
+      <c r="I71" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="J70" s="7" t="s">
+      <c r="J71" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="K70" s="7" t="s">
+      <c r="K71" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="L70" s="7"/>
-      <c r="M70" s="7"/>
-      <c r="N70" s="7"/>
-      <c r="O70" s="7"/>
-      <c r="P70" s="7"/>
-      <c r="Q70" s="7"/>
-      <c r="R70" s="7"/>
-      <c r="S70" s="7"/>
-      <c r="T70" s="7"/>
-      <c r="U70" s="7"/>
-      <c r="V70" s="7"/>
-      <c r="W70" s="7"/>
-      <c r="X70" s="7"/>
-      <c r="Y70" s="7"/>
-      <c r="Z70" s="7"/>
-    </row>
-    <row r="71" spans="1:26" ht="14.4">
-      <c r="A71" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B71" s="15" t="s">
+      <c r="L71" s="7"/>
+      <c r="M71" s="7"/>
+      <c r="N71" s="7"/>
+      <c r="O71" s="7"/>
+      <c r="P71" s="7"/>
+      <c r="Q71" s="7"/>
+      <c r="R71" s="7"/>
+      <c r="S71" s="7"/>
+      <c r="T71" s="7"/>
+      <c r="U71" s="7"/>
+      <c r="V71" s="7"/>
+      <c r="W71" s="7"/>
+      <c r="X71" s="7"/>
+      <c r="Y71" s="7"/>
+      <c r="Z71" s="7"/>
+    </row>
+    <row r="72" spans="1:26" ht="14.4">
+      <c r="A72" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B72" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="E71" s="7" t="s">
+      <c r="E72" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="F71" s="7">
+      <c r="F72" s="7">
         <v>1739.927555</v>
       </c>
-      <c r="G71" s="7"/>
-      <c r="H71" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="K71" s="3" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="72" spans="1:26" s="21" customFormat="1" ht="14.4">
-      <c r="A72" s="20"/>
-      <c r="B72" s="20"/>
-      <c r="E72" s="7" t="s">
-        <v>959</v>
-      </c>
-      <c r="F72" s="7"/>
-      <c r="G72" s="7" t="s">
-        <v>109</v>
-      </c>
+      <c r="G72" s="7"/>
       <c r="H72" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="I72" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="J72" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="K72" s="3"/>
+      <c r="K72" s="3" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="73" spans="1:26" s="21" customFormat="1" ht="14.4">
       <c r="A73" s="20"/>
       <c r="B73" s="20"/>
       <c r="E73" s="7" t="s">
-        <v>497</v>
+        <v>959</v>
       </c>
       <c r="F73" s="7"/>
-      <c r="G73" s="7"/>
-      <c r="H73" s="7"/>
-      <c r="K73" s="3" t="s">
-        <v>941</v>
-      </c>
+      <c r="G73" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="H73" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="I73" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="J73" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="K73" s="3"/>
     </row>
     <row r="74" spans="1:26" s="21" customFormat="1" ht="14.4">
       <c r="A74" s="20"/>
       <c r="B74" s="20"/>
       <c r="E74" s="7" t="s">
-        <v>854</v>
+        <v>497</v>
       </c>
       <c r="F74" s="7"/>
-      <c r="G74" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="H74" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="I74" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="J74" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="K74" s="21" t="s">
-        <v>856</v>
-      </c>
-      <c r="L74" s="3" t="s">
-        <v>855</v>
+      <c r="G74" s="7"/>
+      <c r="H74" s="7"/>
+      <c r="K74" s="3" t="s">
+        <v>941</v>
       </c>
     </row>
     <row r="75" spans="1:26" s="21" customFormat="1" ht="14.4">
       <c r="A75" s="20"/>
       <c r="B75" s="20"/>
       <c r="E75" s="7" t="s">
-        <v>918</v>
+        <v>854</v>
       </c>
       <c r="F75" s="7"/>
       <c r="G75" s="7" t="s">
         <v>29</v>
       </c>
       <c r="H75" s="7" t="s">
-        <v>129</v>
+        <v>73</v>
       </c>
       <c r="I75" s="21" t="s">
         <v>34</v>
@@ -22613,42 +22619,36 @@
         <v>30</v>
       </c>
       <c r="K75" s="21" t="s">
-        <v>903</v>
+        <v>856</v>
       </c>
       <c r="L75" s="3" t="s">
         <v>855</v>
       </c>
     </row>
-    <row r="76" spans="1:26" ht="14.4">
-      <c r="A76" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B76" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="C76" s="3" t="s">
-        <v>24</v>
-      </c>
+    <row r="76" spans="1:26" s="21" customFormat="1" ht="14.4">
+      <c r="A76" s="20"/>
+      <c r="B76" s="20"/>
       <c r="E76" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="F76" s="7">
-        <v>1</v>
-      </c>
+        <v>918</v>
+      </c>
+      <c r="F76" s="7"/>
       <c r="G76" s="7" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="H76" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="I76" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="I76" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="J76" s="3" t="s">
+      <c r="J76" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="K76" s="3" t="s">
-        <v>117</v>
+      <c r="K76" s="21" t="s">
+        <v>903</v>
+      </c>
+      <c r="L76" s="3" t="s">
+        <v>855</v>
       </c>
     </row>
     <row r="77" spans="1:26" ht="14.4">
@@ -22658,14 +22658,30 @@
       <c r="B77" s="15" t="s">
         <v>24</v>
       </c>
+      <c r="C77" s="3" t="s">
+        <v>24</v>
+      </c>
       <c r="E77" s="7" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="F77" s="7">
-        <v>553659</v>
-      </c>
-      <c r="G77" s="7"/>
-      <c r="H77" s="7"/>
+        <v>1</v>
+      </c>
+      <c r="G77" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="H77" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="I77" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="J77" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="K77" s="3" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="78" spans="1:26" ht="14.4">
       <c r="A78" s="15" t="s">
@@ -22675,10 +22691,10 @@
         <v>24</v>
       </c>
       <c r="E78" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F78" s="7">
-        <v>4891208</v>
+        <v>553659</v>
       </c>
       <c r="G78" s="7"/>
       <c r="H78" s="7"/>
@@ -22690,106 +22706,89 @@
       <c r="B79" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="C79" s="3" t="s">
+      <c r="E79" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="F79" s="7">
+        <v>4891208</v>
+      </c>
+      <c r="G79" s="7"/>
+      <c r="H79" s="7"/>
+    </row>
+    <row r="80" spans="1:26" ht="14.4">
+      <c r="A80" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B80" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="E79" s="7" t="s">
+      <c r="C80" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E80" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="F79" s="7">
+      <c r="F80" s="7">
         <v>1</v>
       </c>
-      <c r="G79" s="7" t="s">
+      <c r="G80" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="H79" s="7" t="s">
+      <c r="H80" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="I79" s="3" t="s">
+      <c r="I80" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="J79" s="3" t="s">
+      <c r="J80" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="K79" s="3" t="s">
+      <c r="K80" s="3" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="80" spans="1:26" s="21" customFormat="1" ht="14.4">
-      <c r="A80" s="20"/>
-      <c r="B80" s="20"/>
-      <c r="C80" s="3"/>
-      <c r="E80" s="7" t="s">
+    <row r="81" spans="1:12" s="21" customFormat="1" ht="14.4">
+      <c r="A81" s="20"/>
+      <c r="B81" s="20"/>
+      <c r="C81" s="3"/>
+      <c r="E81" s="7" t="s">
         <v>934</v>
       </c>
-      <c r="F80" s="7"/>
-      <c r="G80" s="7"/>
-      <c r="H80" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="I80" s="3"/>
-      <c r="J80" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="K80" s="3" t="s">
-        <v>936</v>
-      </c>
-    </row>
-    <row r="81" spans="1:12" s="21" customFormat="1" ht="14.4">
-      <c r="A81" s="20" t="s">
-        <v>837</v>
-      </c>
-      <c r="B81" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="C81" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="D81" s="21" t="s">
-        <v>65</v>
-      </c>
-      <c r="E81" s="7" t="s">
-        <v>836</v>
-      </c>
-      <c r="F81" s="7">
-        <v>5</v>
-      </c>
-      <c r="G81" s="7" t="s">
-        <v>109</v>
-      </c>
+      <c r="F81" s="7"/>
+      <c r="G81" s="7"/>
       <c r="H81" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="I81" s="3" t="s">
-        <v>26</v>
-      </c>
+      <c r="I81" s="3"/>
       <c r="J81" s="3" t="s">
         <v>27</v>
       </c>
       <c r="K81" s="3" t="s">
-        <v>838</v>
-      </c>
-      <c r="L81" s="23" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12" s="21" customFormat="1" ht="14.4">
+      <c r="A82" s="20" t="s">
+        <v>837</v>
+      </c>
+      <c r="B82" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="C82" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D82" s="21" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="82" spans="1:12" ht="14.4">
-      <c r="A82" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B82" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="D82" s="3" t="s">
-        <v>127</v>
-      </c>
       <c r="E82" s="7" t="s">
-        <v>128</v>
+        <v>836</v>
       </c>
       <c r="F82" s="7">
-        <v>0</v>
-      </c>
-      <c r="G82" s="7"/>
+        <v>5</v>
+      </c>
+      <c r="G82" s="7" t="s">
+        <v>109</v>
+      </c>
       <c r="H82" s="7" t="s">
         <v>129</v>
       </c>
@@ -22800,25 +22799,40 @@
         <v>27</v>
       </c>
       <c r="K82" s="3" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="83" spans="1:12" s="21" customFormat="1" ht="14.4">
-      <c r="A83" s="20"/>
-      <c r="B83" s="20"/>
-      <c r="D83" s="3"/>
+        <v>838</v>
+      </c>
+      <c r="L82" s="23" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12" ht="14.4">
+      <c r="A83" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B83" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D83" s="3" t="s">
+        <v>127</v>
+      </c>
       <c r="E83" s="7" t="s">
-        <v>935</v>
-      </c>
-      <c r="F83" s="7"/>
+        <v>128</v>
+      </c>
+      <c r="F83" s="7">
+        <v>0</v>
+      </c>
       <c r="G83" s="7"/>
       <c r="H83" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="I83" s="3"/>
-      <c r="J83" s="3"/>
+      <c r="I83" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J83" s="3" t="s">
+        <v>27</v>
+      </c>
       <c r="K83" s="3" t="s">
-        <v>937</v>
+        <v>130</v>
       </c>
     </row>
     <row r="84" spans="1:12" s="21" customFormat="1" ht="14.4">
@@ -22826,7 +22840,7 @@
       <c r="B84" s="20"/>
       <c r="D84" s="3"/>
       <c r="E84" s="7" t="s">
-        <v>938</v>
+        <v>935</v>
       </c>
       <c r="F84" s="7"/>
       <c r="G84" s="7"/>
@@ -22836,53 +22850,46 @@
       <c r="I84" s="3"/>
       <c r="J84" s="3"/>
       <c r="K84" s="3" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12" s="21" customFormat="1" ht="14.4">
+      <c r="A85" s="20"/>
+      <c r="B85" s="20"/>
+      <c r="D85" s="3"/>
+      <c r="E85" s="7" t="s">
+        <v>938</v>
+      </c>
+      <c r="F85" s="7"/>
+      <c r="G85" s="7"/>
+      <c r="H85" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="I85" s="3"/>
+      <c r="J85" s="3"/>
+      <c r="K85" s="3" t="s">
         <v>939</v>
       </c>
     </row>
-    <row r="85" spans="1:12" ht="14.4">
-      <c r="A85" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B85" s="15"/>
-      <c r="E85" s="7" t="s">
+    <row r="86" spans="1:12" ht="14.4">
+      <c r="A86" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B86" s="15"/>
+      <c r="E86" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="F85" s="7">
+      <c r="F86" s="7">
         <v>6772</v>
       </c>
-      <c r="G85" s="7"/>
-      <c r="H85" s="7"/>
-    </row>
-    <row r="86" spans="1:12" s="21" customFormat="1" ht="14.4">
-      <c r="A86" s="20"/>
-      <c r="B86" s="20"/>
-      <c r="E86" s="7" t="s">
-        <v>952</v>
-      </c>
-      <c r="F86" s="7">
-        <v>5</v>
-      </c>
-      <c r="G86" s="58" t="s">
-        <v>109</v>
-      </c>
-      <c r="H86" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="I86" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="J86" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="K86" s="23" t="s">
-        <v>953</v>
-      </c>
+      <c r="G86" s="7"/>
+      <c r="H86" s="7"/>
     </row>
     <row r="87" spans="1:12" s="21" customFormat="1" ht="14.4">
       <c r="A87" s="20"/>
       <c r="B87" s="20"/>
-      <c r="E87" s="58" t="s">
-        <v>954</v>
+      <c r="E87" s="7" t="s">
+        <v>952</v>
       </c>
       <c r="F87" s="7">
         <v>5</v>
@@ -22900,14 +22907,14 @@
         <v>30</v>
       </c>
       <c r="K87" s="23" t="s">
-        <v>955</v>
+        <v>953</v>
       </c>
     </row>
     <row r="88" spans="1:12" s="21" customFormat="1" ht="14.4">
       <c r="A88" s="20"/>
       <c r="B88" s="20"/>
       <c r="E88" s="58" t="s">
-        <v>956</v>
+        <v>954</v>
       </c>
       <c r="F88" s="7">
         <v>5</v>
@@ -22925,82 +22932,87 @@
         <v>30</v>
       </c>
       <c r="K88" s="23" t="s">
-        <v>957</v>
+        <v>955</v>
       </c>
     </row>
     <row r="89" spans="1:12" s="21" customFormat="1" ht="14.4">
       <c r="A89" s="20"/>
       <c r="B89" s="20"/>
-      <c r="E89" s="7" t="s">
-        <v>843</v>
+      <c r="E89" s="58" t="s">
+        <v>956</v>
       </c>
       <c r="F89" s="7">
-        <v>1</v>
-      </c>
-      <c r="G89" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G89" s="58" t="s">
         <v>109</v>
       </c>
       <c r="H89" s="7" t="s">
-        <v>844</v>
-      </c>
-      <c r="I89" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="J89" s="23" t="s">
-        <v>845</v>
+        <v>129</v>
+      </c>
+      <c r="I89" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="J89" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="K89" s="23" t="s">
+        <v>957</v>
       </c>
     </row>
     <row r="90" spans="1:12" s="21" customFormat="1" ht="14.4">
       <c r="A90" s="20"/>
       <c r="B90" s="20"/>
       <c r="E90" s="7" t="s">
-        <v>978</v>
-      </c>
-      <c r="F90" s="7"/>
+        <v>843</v>
+      </c>
+      <c r="F90" s="7">
+        <v>1</v>
+      </c>
       <c r="G90" s="7" t="s">
         <v>109</v>
       </c>
       <c r="H90" s="7" t="s">
-        <v>63</v>
+        <v>844</v>
       </c>
       <c r="I90" s="23" t="s">
         <v>26</v>
       </c>
       <c r="J90" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="K90" s="23" t="s">
-        <v>979</v>
-      </c>
-      <c r="L90" s="23" t="s">
-        <v>977</v>
+        <v>845</v>
       </c>
     </row>
     <row r="91" spans="1:12" s="21" customFormat="1" ht="14.4">
       <c r="A91" s="20"/>
       <c r="B91" s="20"/>
       <c r="E91" s="7" t="s">
-        <v>950</v>
+        <v>978</v>
       </c>
       <c r="F91" s="7"/>
       <c r="G91" s="7" t="s">
         <v>109</v>
       </c>
       <c r="H91" s="7" t="s">
-        <v>626</v>
-      </c>
-      <c r="I91" s="23"/>
-      <c r="J91" s="23"/>
+        <v>63</v>
+      </c>
+      <c r="I91" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="J91" s="23" t="s">
+        <v>27</v>
+      </c>
       <c r="K91" s="23" t="s">
-        <v>980</v>
-      </c>
-      <c r="L91" s="23"/>
+        <v>979</v>
+      </c>
+      <c r="L91" s="23" t="s">
+        <v>977</v>
+      </c>
     </row>
     <row r="92" spans="1:12" s="21" customFormat="1" ht="14.4">
       <c r="A92" s="20"/>
       <c r="B92" s="20"/>
       <c r="E92" s="7" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="F92" s="7"/>
       <c r="G92" s="7" t="s">
@@ -23012,69 +23024,66 @@
       <c r="I92" s="23"/>
       <c r="J92" s="23"/>
       <c r="K92" s="23" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
       <c r="L92" s="23"/>
     </row>
     <row r="93" spans="1:12" s="21" customFormat="1" ht="14.4">
       <c r="A93" s="20"/>
       <c r="B93" s="20"/>
-      <c r="D93" s="57" t="s">
-        <v>944</v>
-      </c>
       <c r="E93" s="7" t="s">
-        <v>970</v>
+        <v>951</v>
       </c>
       <c r="F93" s="7"/>
-      <c r="G93" s="58" t="s">
+      <c r="G93" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="H93" s="58" t="s">
-        <v>84</v>
-      </c>
-      <c r="I93" s="23" t="s">
-        <v>947</v>
-      </c>
-      <c r="J93" s="23" t="s">
-        <v>947</v>
-      </c>
+      <c r="H93" s="7" t="s">
+        <v>626</v>
+      </c>
+      <c r="I93" s="23"/>
+      <c r="J93" s="23"/>
       <c r="K93" s="23" t="s">
-        <v>971</v>
+        <v>981</v>
       </c>
       <c r="L93" s="23"/>
     </row>
     <row r="94" spans="1:12" s="21" customFormat="1" ht="14.4">
       <c r="A94" s="20"/>
       <c r="B94" s="20"/>
+      <c r="D94" s="57" t="s">
+        <v>944</v>
+      </c>
       <c r="E94" s="7" t="s">
-        <v>842</v>
-      </c>
-      <c r="F94" s="7">
-        <v>10</v>
-      </c>
-      <c r="G94" s="7" t="s">
+        <v>970</v>
+      </c>
+      <c r="F94" s="7"/>
+      <c r="G94" s="58" t="s">
         <v>109</v>
       </c>
-      <c r="H94" s="7" t="s">
-        <v>626</v>
+      <c r="H94" s="58" t="s">
+        <v>84</v>
       </c>
       <c r="I94" s="23" t="s">
-        <v>26</v>
+        <v>947</v>
       </c>
       <c r="J94" s="23" t="s">
-        <v>27</v>
+        <v>947</v>
       </c>
       <c r="K94" s="23" t="s">
-        <v>848</v>
-      </c>
+        <v>971</v>
+      </c>
+      <c r="L94" s="23"/>
     </row>
     <row r="95" spans="1:12" s="21" customFormat="1" ht="14.4">
       <c r="A95" s="20"/>
       <c r="B95" s="20"/>
       <c r="E95" s="7" t="s">
-        <v>960</v>
-      </c>
-      <c r="F95" s="7"/>
+        <v>842</v>
+      </c>
+      <c r="F95" s="7">
+        <v>10</v>
+      </c>
       <c r="G95" s="7" t="s">
         <v>109</v>
       </c>
@@ -23082,20 +23091,20 @@
         <v>626</v>
       </c>
       <c r="I95" s="23" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="J95" s="23" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="K95" s="23" t="s">
-        <v>961</v>
+        <v>848</v>
       </c>
     </row>
     <row r="96" spans="1:12" s="21" customFormat="1" ht="14.4">
       <c r="A96" s="20"/>
       <c r="B96" s="20"/>
       <c r="E96" s="7" t="s">
-        <v>974</v>
+        <v>960</v>
       </c>
       <c r="F96" s="7"/>
       <c r="G96" s="7" t="s">
@@ -23104,70 +23113,65 @@
       <c r="H96" s="7" t="s">
         <v>626</v>
       </c>
-      <c r="I96" s="23"/>
+      <c r="I96" s="23" t="s">
+        <v>34</v>
+      </c>
       <c r="J96" s="23" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="K96" s="23" t="s">
-        <v>975</v>
-      </c>
-      <c r="L96" s="23" t="s">
-        <v>976</v>
-      </c>
-    </row>
-    <row r="97" spans="1:11" s="21" customFormat="1" ht="14.4">
+        <v>961</v>
+      </c>
+    </row>
+    <row r="97" spans="1:12" s="21" customFormat="1" ht="14.4">
       <c r="A97" s="20"/>
       <c r="B97" s="20"/>
       <c r="E97" s="7" t="s">
-        <v>510</v>
+        <v>974</v>
       </c>
       <c r="F97" s="7"/>
-      <c r="G97" s="7"/>
+      <c r="G97" s="7" t="s">
+        <v>109</v>
+      </c>
       <c r="H97" s="7" t="s">
-        <v>511</v>
+        <v>626</v>
       </c>
       <c r="I97" s="23"/>
-      <c r="J97" s="23"/>
+      <c r="J97" s="23" t="s">
+        <v>27</v>
+      </c>
       <c r="K97" s="23" t="s">
-        <v>943</v>
-      </c>
-    </row>
-    <row r="98" spans="1:11" s="21" customFormat="1" ht="14.4">
+        <v>975</v>
+      </c>
+      <c r="L97" s="23" t="s">
+        <v>976</v>
+      </c>
+    </row>
+    <row r="98" spans="1:12" s="21" customFormat="1" ht="14.4">
       <c r="A98" s="20"/>
       <c r="B98" s="20"/>
-      <c r="D98" s="57" t="s">
-        <v>25</v>
-      </c>
       <c r="E98" s="7" t="s">
-        <v>796</v>
+        <v>510</v>
       </c>
       <c r="F98" s="7"/>
-      <c r="G98" s="58" t="s">
-        <v>29</v>
-      </c>
+      <c r="G98" s="7"/>
       <c r="H98" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="I98" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="J98" s="23" t="s">
-        <v>27</v>
-      </c>
+        <v>511</v>
+      </c>
+      <c r="I98" s="23"/>
+      <c r="J98" s="23"/>
       <c r="K98" s="23" t="s">
-        <v>797</v>
-      </c>
-    </row>
-    <row r="99" spans="1:11" s="21" customFormat="1" ht="14.4">
-      <c r="A99" s="20" t="s">
-        <v>23</v>
-      </c>
+        <v>943</v>
+      </c>
+    </row>
+    <row r="99" spans="1:12" s="21" customFormat="1" ht="14.4">
+      <c r="A99" s="20"/>
       <c r="B99" s="20"/>
       <c r="D99" s="57" t="s">
         <v>25</v>
       </c>
       <c r="E99" s="7" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
       <c r="F99" s="7"/>
       <c r="G99" s="58" t="s">
@@ -23183,42 +23187,38 @@
         <v>27</v>
       </c>
       <c r="K99" s="23" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="100" spans="1:12" s="21" customFormat="1" ht="14.4">
+      <c r="A100" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="B100" s="20"/>
+      <c r="D100" s="57" t="s">
+        <v>25</v>
+      </c>
+      <c r="E100" s="7" t="s">
+        <v>798</v>
+      </c>
+      <c r="F100" s="7"/>
+      <c r="G100" s="58" t="s">
+        <v>29</v>
+      </c>
+      <c r="H100" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="I100" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="J100" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="K100" s="23" t="s">
         <v>799</v>
       </c>
     </row>
-    <row r="100" spans="1:11" ht="14.4">
-      <c r="A100" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B100" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="D100" s="17" t="s">
-        <v>133</v>
-      </c>
-      <c r="E100" s="18" t="s">
-        <v>135</v>
-      </c>
-      <c r="F100" s="18">
-        <v>1500</v>
-      </c>
-      <c r="G100" s="18" t="s">
-        <v>109</v>
-      </c>
-      <c r="H100" s="18" t="s">
-        <v>84</v>
-      </c>
-      <c r="I100" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="J100" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="K100" s="17" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="101" spans="1:11" ht="14.4">
+    <row r="101" spans="1:12" ht="14.4">
       <c r="A101" s="15" t="s">
         <v>23</v>
       </c>
@@ -23228,16 +23228,16 @@
       <c r="D101" s="17" t="s">
         <v>133</v>
       </c>
-      <c r="E101" s="17" t="s">
-        <v>140</v>
-      </c>
-      <c r="F101" s="17">
+      <c r="E101" s="18" t="s">
+        <v>135</v>
+      </c>
+      <c r="F101" s="18">
         <v>1500</v>
       </c>
       <c r="G101" s="18" t="s">
         <v>109</v>
       </c>
-      <c r="H101" s="17" t="s">
+      <c r="H101" s="18" t="s">
         <v>84</v>
       </c>
       <c r="I101" s="17" t="s">
@@ -23247,10 +23247,10 @@
         <v>30</v>
       </c>
       <c r="K101" s="17" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="102" spans="1:11" ht="14.4">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="102" spans="1:12" ht="14.4">
       <c r="A102" s="15" t="s">
         <v>23</v>
       </c>
@@ -23261,7 +23261,7 @@
         <v>133</v>
       </c>
       <c r="E102" s="17" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="F102" s="17">
         <v>1500</v>
@@ -23279,13 +23279,45 @@
         <v>30</v>
       </c>
       <c r="K102" s="17" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="103" spans="1:12" ht="14.4">
+      <c r="A103" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B103" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="D103" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="E103" s="17" t="s">
+        <v>143</v>
+      </c>
+      <c r="F103" s="17">
+        <v>1500</v>
+      </c>
+      <c r="G103" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="H103" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="I103" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="J103" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="K103" s="17" t="s">
         <v>144</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B58:B61">
+  <conditionalFormatting sqref="B59:B62">
     <cfRule type="notContainsBlanks" dxfId="0" priority="1">
-      <formula>LEN(TRIM(B58))&gt;0</formula>
+      <formula>LEN(TRIM(B59))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Work on reconciling CW3M output with Shade-a-lator output. FLOWreports_McKenzie.xml - Delete some obsolete reports. Reporter_McKenzie.xml - Add REP Forest Disturbance Report. SimulationScenarios.xml - Add Clearcut_above_1000m scenario. Flow.cpp, .h - Add TopoSetting::VegShade_pct(). Make TopoSetting::SolarDeclination_deg() static. Add a static version of TopoSetting::SolarElev_deg(). Add extensive comments to VegElevNS_deg(). Add four columns to the ReachInsolationData.csv file: KCAL_GIVEN, KCAL_CALCULATED, KCAL_DIFF_PCT, and RAD_SW_EST. Correct bugs in the calculation of effective reach lengths related to negative values of overlap_m.
</commit_message>
<xml_diff>
--- a/DataCW3M/CW3MdigitalHandbook/CW3MdataDictionary.xlsx
+++ b/DataCW3M/CW3MdigitalHandbook/CW3MdataDictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\CW3MdigitalHandbook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3845F36-93BD-4809-A3D5-9DFE7D07D509}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AB58806-7FC8-49D7-ADD0-C16DE25831D8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-7425" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Necessary input data" sheetId="7" r:id="rId1"/>
@@ -96,7 +96,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2957" uniqueCount="988">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2963" uniqueCount="990">
   <si>
     <t>LULC_A</t>
   </si>
@@ -3061,6 +3061,12 @@
   </si>
   <si>
     <t>kcal</t>
+  </si>
+  <si>
+    <t>RAD_SW_EST</t>
+  </si>
+  <si>
+    <t>estimate of daily average surface insolation flux based on geographical location and date, for comparison to Shade-a-lator output</t>
   </si>
 </sst>
 </file>
@@ -9013,7 +9019,7 @@
   <dimension ref="A1:Z1047"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A76" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="3" topLeftCell="A128" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="H199" sqref="H199"/>
     </sheetView>
   </sheetViews>
@@ -20733,11 +20739,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Z103"/>
+  <dimension ref="A1:Z104"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J41" sqref="J41"/>
+      <pane ySplit="4" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K57" sqref="K57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -22161,8 +22167,8 @@
     <row r="57" spans="1:11" s="21" customFormat="1" ht="14.4">
       <c r="A57" s="20"/>
       <c r="B57" s="20"/>
-      <c r="E57" s="7" t="s">
-        <v>839</v>
+      <c r="E57" s="58" t="s">
+        <v>988</v>
       </c>
       <c r="F57" s="7"/>
       <c r="G57" s="7" t="s">
@@ -22174,15 +22180,18 @@
       <c r="I57" s="21" t="s">
         <v>26</v>
       </c>
+      <c r="J57" s="21" t="s">
+        <v>27</v>
+      </c>
       <c r="K57" s="23" t="s">
-        <v>853</v>
+        <v>989</v>
       </c>
     </row>
     <row r="58" spans="1:11" s="21" customFormat="1" ht="14.4">
       <c r="A58" s="20"/>
       <c r="B58" s="20"/>
       <c r="E58" s="7" t="s">
-        <v>962</v>
+        <v>839</v>
       </c>
       <c r="F58" s="7"/>
       <c r="G58" s="7" t="s">
@@ -22192,86 +22201,81 @@
         <v>475</v>
       </c>
       <c r="I58" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="K58" s="23" t="s">
+        <v>853</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" s="21" customFormat="1" ht="14.4">
+      <c r="A59" s="20"/>
+      <c r="B59" s="20"/>
+      <c r="E59" s="7" t="s">
+        <v>962</v>
+      </c>
+      <c r="F59" s="7"/>
+      <c r="G59" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="H59" s="7" t="s">
+        <v>475</v>
+      </c>
+      <c r="I59" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="K58" s="23" t="s">
+      <c r="K59" s="23" t="s">
         <v>963</v>
       </c>
     </row>
-    <row r="59" spans="1:11" ht="14.4">
-      <c r="A59" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="B59" s="24" t="s">
+    <row r="60" spans="1:11" ht="14.4">
+      <c r="A60" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B60" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="C59" s="17" t="s">
+      <c r="C60" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="D59" s="17" t="s">
+      <c r="D60" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="E59" s="18" t="s">
+      <c r="E60" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="F59" s="7"/>
-      <c r="G59" s="18" t="s">
+      <c r="F60" s="7"/>
+      <c r="G60" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="H59" s="18" t="s">
+      <c r="H60" s="18" t="s">
         <v>95</v>
       </c>
-      <c r="I59" s="17" t="s">
+      <c r="I60" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="J59" s="17" t="s">
+      <c r="J60" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="K59" s="17" t="s">
+      <c r="K60" s="17" t="s">
         <v>96</v>
-      </c>
-    </row>
-    <row r="60" spans="1:11" s="21" customFormat="1" ht="14.4">
-      <c r="A60" s="20"/>
-      <c r="B60" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="C60" s="22"/>
-      <c r="D60" s="22"/>
-      <c r="E60" s="21" t="s">
-        <v>916</v>
-      </c>
-      <c r="F60" s="7"/>
-      <c r="G60" s="21" t="s">
-        <v>109</v>
-      </c>
-      <c r="H60" s="21" t="s">
-        <v>917</v>
-      </c>
-      <c r="I60" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="J60" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="K60" s="23" t="s">
-        <v>911</v>
       </c>
     </row>
     <row r="61" spans="1:11" s="21" customFormat="1" ht="14.4">
       <c r="A61" s="20"/>
-      <c r="B61" s="24"/>
+      <c r="B61" s="24" t="s">
+        <v>23</v>
+      </c>
       <c r="C61" s="22"/>
       <c r="D61" s="22"/>
       <c r="E61" s="21" t="s">
-        <v>919</v>
+        <v>916</v>
       </c>
       <c r="F61" s="7"/>
       <c r="G61" s="21" t="s">
         <v>109</v>
       </c>
       <c r="H61" s="21" t="s">
-        <v>407</v>
+        <v>917</v>
       </c>
       <c r="I61" s="23" t="s">
         <v>26</v>
@@ -22280,25 +22284,23 @@
         <v>27</v>
       </c>
       <c r="K61" s="23" t="s">
-        <v>920</v>
+        <v>911</v>
       </c>
     </row>
     <row r="62" spans="1:11" s="21" customFormat="1" ht="14.4">
       <c r="A62" s="20"/>
-      <c r="B62" s="24" t="s">
-        <v>23</v>
-      </c>
+      <c r="B62" s="24"/>
       <c r="C62" s="22"/>
       <c r="D62" s="22"/>
       <c r="E62" s="21" t="s">
-        <v>912</v>
+        <v>919</v>
       </c>
       <c r="F62" s="7"/>
       <c r="G62" s="21" t="s">
         <v>109</v>
       </c>
       <c r="H62" s="21" t="s">
-        <v>95</v>
+        <v>407</v>
       </c>
       <c r="I62" s="23" t="s">
         <v>26</v>
@@ -22307,336 +22309,337 @@
         <v>27</v>
       </c>
       <c r="K62" s="23" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" s="21" customFormat="1" ht="14.4">
+      <c r="A63" s="20"/>
+      <c r="B63" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="C63" s="22"/>
+      <c r="D63" s="22"/>
+      <c r="E63" s="21" t="s">
+        <v>912</v>
+      </c>
+      <c r="F63" s="7"/>
+      <c r="G63" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="H63" s="21" t="s">
+        <v>95</v>
+      </c>
+      <c r="I63" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="J63" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="K63" s="23" t="s">
         <v>913</v>
       </c>
     </row>
-    <row r="63" spans="1:11" ht="43.2">
-      <c r="A63" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B63" s="15" t="s">
+    <row r="64" spans="1:11" ht="43.2">
+      <c r="A64" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B64" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="E63" s="7" t="s">
+      <c r="E64" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="F63" s="18">
+      <c r="F64" s="18">
         <v>1</v>
       </c>
-      <c r="G63" s="18" t="s">
+      <c r="G64" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="H63" s="18" t="s">
+      <c r="H64" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="J63" s="17" t="s">
+      <c r="J64" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="K63" s="19" t="s">
+      <c r="K64" s="19" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="64" spans="1:11" s="21" customFormat="1" ht="14.4">
-      <c r="A64" s="20"/>
-      <c r="B64" s="20"/>
-      <c r="E64" s="7" t="s">
+    <row r="65" spans="1:26" s="21" customFormat="1" ht="14.4">
+      <c r="A65" s="20"/>
+      <c r="B65" s="20"/>
+      <c r="E65" s="7" t="s">
         <v>921</v>
       </c>
-      <c r="G64" s="21" t="s">
+      <c r="G65" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="H64" s="21" t="s">
+      <c r="H65" s="21" t="s">
         <v>475</v>
       </c>
-      <c r="I64" s="23" t="s">
+      <c r="I65" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="J64" s="23" t="s">
+      <c r="J65" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="K64" s="23" t="s">
+      <c r="K65" s="23" t="s">
         <v>922</v>
       </c>
     </row>
-    <row r="65" spans="1:26" s="25" customFormat="1" ht="86.4">
-      <c r="A65" s="81"/>
-      <c r="B65" s="81"/>
-      <c r="E65" s="25" t="s">
-        <v>101</v>
-      </c>
-      <c r="F65" s="25">
-        <v>1</v>
-      </c>
-      <c r="G65" s="25" t="s">
-        <v>98</v>
-      </c>
-      <c r="H65" s="25" t="s">
-        <v>99</v>
-      </c>
-      <c r="I65" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="J65" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="K65" s="80" t="s">
-        <v>933</v>
-      </c>
-    </row>
-    <row r="66" spans="1:26" s="25" customFormat="1" ht="14.4">
+    <row r="66" spans="1:26" s="25" customFormat="1" ht="86.4">
       <c r="A66" s="81"/>
       <c r="B66" s="81"/>
-      <c r="E66" s="72" t="s">
+      <c r="E66" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="F66" s="25">
+        <v>1</v>
+      </c>
+      <c r="G66" s="25" t="s">
+        <v>98</v>
+      </c>
+      <c r="H66" s="25" t="s">
+        <v>99</v>
+      </c>
+      <c r="I66" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="J66" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="K66" s="80" t="s">
+        <v>933</v>
+      </c>
+    </row>
+    <row r="67" spans="1:26" s="25" customFormat="1" ht="14.4">
+      <c r="A67" s="81"/>
+      <c r="B67" s="81"/>
+      <c r="E67" s="72" t="s">
         <v>923</v>
       </c>
-      <c r="G66" s="72" t="s">
+      <c r="G67" s="72" t="s">
         <v>109</v>
       </c>
-      <c r="H66" s="72" t="s">
+      <c r="H67" s="72" t="s">
         <v>475</v>
-      </c>
-      <c r="I66" s="80" t="s">
-        <v>26</v>
-      </c>
-      <c r="J66" s="80" t="s">
-        <v>27</v>
-      </c>
-      <c r="K66" s="23" t="s">
-        <v>924</v>
-      </c>
-    </row>
-    <row r="67" spans="1:26" s="25" customFormat="1" ht="28.8">
-      <c r="A67" s="81"/>
-      <c r="B67" s="81" t="s">
-        <v>23</v>
-      </c>
-      <c r="E67" s="25" t="s">
-        <v>914</v>
-      </c>
-      <c r="G67" s="25" t="s">
-        <v>109</v>
-      </c>
-      <c r="H67" s="25" t="s">
-        <v>129</v>
       </c>
       <c r="I67" s="80" t="s">
         <v>26</v>
       </c>
-      <c r="J67" s="19"/>
-      <c r="K67" s="80" t="s">
+      <c r="J67" s="80" t="s">
+        <v>27</v>
+      </c>
+      <c r="K67" s="23" t="s">
+        <v>924</v>
+      </c>
+    </row>
+    <row r="68" spans="1:26" s="25" customFormat="1" ht="28.8">
+      <c r="A68" s="81"/>
+      <c r="B68" s="81" t="s">
+        <v>23</v>
+      </c>
+      <c r="E68" s="25" t="s">
+        <v>914</v>
+      </c>
+      <c r="G68" s="25" t="s">
+        <v>109</v>
+      </c>
+      <c r="H68" s="25" t="s">
+        <v>129</v>
+      </c>
+      <c r="I68" s="80" t="s">
+        <v>26</v>
+      </c>
+      <c r="J68" s="19"/>
+      <c r="K68" s="80" t="s">
         <v>915</v>
       </c>
     </row>
-    <row r="68" spans="1:26" s="21" customFormat="1" ht="14.25" customHeight="1">
-      <c r="C68" s="28"/>
-      <c r="D68" s="28"/>
-      <c r="E68" s="7" t="s">
+    <row r="69" spans="1:26" s="21" customFormat="1" ht="14.25" customHeight="1">
+      <c r="C69" s="28"/>
+      <c r="D69" s="28"/>
+      <c r="E69" s="7" t="s">
         <v>812</v>
       </c>
-      <c r="F68" s="7"/>
-      <c r="G68" s="70" t="s">
+      <c r="F69" s="7"/>
+      <c r="G69" s="70" t="s">
         <v>29</v>
       </c>
-      <c r="H68" s="70" t="s">
+      <c r="H69" s="70" t="s">
         <v>227</v>
       </c>
-      <c r="I68" s="70" t="s">
+      <c r="I69" s="70" t="s">
         <v>34</v>
       </c>
-      <c r="J68" s="70" t="s">
+      <c r="J69" s="70" t="s">
         <v>27</v>
       </c>
-      <c r="K68" s="57" t="s">
+      <c r="K69" s="57" t="s">
         <v>813</v>
       </c>
-      <c r="L68" s="70" t="s">
+      <c r="L69" s="70" t="s">
         <v>814</v>
       </c>
-      <c r="M68" s="3"/>
-      <c r="N68" s="7"/>
-      <c r="O68" s="7"/>
-      <c r="P68" s="7"/>
-      <c r="Q68" s="7"/>
-      <c r="R68" s="7"/>
-      <c r="S68" s="7"/>
-      <c r="T68" s="7"/>
-      <c r="U68" s="7"/>
-      <c r="V68" s="7"/>
-      <c r="W68" s="7"/>
-      <c r="X68" s="7"/>
-    </row>
-    <row r="69" spans="1:26" ht="14.4">
-      <c r="A69" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B69" s="15" t="s">
+      <c r="M69" s="3"/>
+      <c r="N69" s="7"/>
+      <c r="O69" s="7"/>
+      <c r="P69" s="7"/>
+      <c r="Q69" s="7"/>
+      <c r="R69" s="7"/>
+      <c r="S69" s="7"/>
+      <c r="T69" s="7"/>
+      <c r="U69" s="7"/>
+      <c r="V69" s="7"/>
+      <c r="W69" s="7"/>
+      <c r="X69" s="7"/>
+    </row>
+    <row r="70" spans="1:26" ht="14.4">
+      <c r="A70" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B70" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="E69" s="7" t="s">
+      <c r="E70" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="F69" s="7">
+      <c r="F70" s="7">
         <v>-1</v>
       </c>
-      <c r="G69" s="7"/>
-      <c r="H69" s="7"/>
-    </row>
-    <row r="70" spans="1:26" s="21" customFormat="1" ht="14.4">
-      <c r="A70" s="20"/>
-      <c r="B70" s="20"/>
-      <c r="E70" s="25" t="s">
+      <c r="G70" s="7"/>
+      <c r="H70" s="7"/>
+    </row>
+    <row r="71" spans="1:26" s="21" customFormat="1" ht="14.4">
+      <c r="A71" s="20"/>
+      <c r="B71" s="20"/>
+      <c r="E71" s="25" t="s">
         <v>982</v>
       </c>
-      <c r="F70" s="7" t="s">
+      <c r="F71" s="7" t="s">
         <v>983</v>
       </c>
-      <c r="G70" s="25" t="s">
+      <c r="G71" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="H70" s="7"/>
-      <c r="K70" s="21" t="s">
+      <c r="H71" s="7"/>
+      <c r="K71" s="21" t="s">
         <v>984</v>
       </c>
     </row>
-    <row r="71" spans="1:26" ht="14.4">
-      <c r="A71" s="15"/>
-      <c r="B71" s="15"/>
-      <c r="C71" s="7" t="s">
+    <row r="72" spans="1:26" ht="14.4">
+      <c r="A72" s="15"/>
+      <c r="B72" s="15"/>
+      <c r="C72" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="D71" s="7" t="s">
+      <c r="D72" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="E71" s="7" t="s">
+      <c r="E72" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="F71" s="7">
+      <c r="F72" s="7">
         <v>0.6</v>
       </c>
-      <c r="G71" s="7" t="s">
+      <c r="G72" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="H71" s="7" t="s">
+      <c r="H72" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="I71" s="7" t="s">
+      <c r="I72" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="J71" s="7" t="s">
+      <c r="J72" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="K71" s="7" t="s">
+      <c r="K72" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="L71" s="7"/>
-      <c r="M71" s="7"/>
-      <c r="N71" s="7"/>
-      <c r="O71" s="7"/>
-      <c r="P71" s="7"/>
-      <c r="Q71" s="7"/>
-      <c r="R71" s="7"/>
-      <c r="S71" s="7"/>
-      <c r="T71" s="7"/>
-      <c r="U71" s="7"/>
-      <c r="V71" s="7"/>
-      <c r="W71" s="7"/>
-      <c r="X71" s="7"/>
-      <c r="Y71" s="7"/>
-      <c r="Z71" s="7"/>
-    </row>
-    <row r="72" spans="1:26" ht="14.4">
-      <c r="A72" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B72" s="15" t="s">
+      <c r="L72" s="7"/>
+      <c r="M72" s="7"/>
+      <c r="N72" s="7"/>
+      <c r="O72" s="7"/>
+      <c r="P72" s="7"/>
+      <c r="Q72" s="7"/>
+      <c r="R72" s="7"/>
+      <c r="S72" s="7"/>
+      <c r="T72" s="7"/>
+      <c r="U72" s="7"/>
+      <c r="V72" s="7"/>
+      <c r="W72" s="7"/>
+      <c r="X72" s="7"/>
+      <c r="Y72" s="7"/>
+      <c r="Z72" s="7"/>
+    </row>
+    <row r="73" spans="1:26" ht="14.4">
+      <c r="A73" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B73" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="E72" s="7" t="s">
+      <c r="E73" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="F72" s="7">
+      <c r="F73" s="7">
         <v>1739.927555</v>
       </c>
-      <c r="G72" s="7"/>
-      <c r="H72" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="K72" s="3" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="73" spans="1:26" s="21" customFormat="1" ht="14.4">
-      <c r="A73" s="20"/>
-      <c r="B73" s="20"/>
-      <c r="E73" s="7" t="s">
-        <v>959</v>
-      </c>
-      <c r="F73" s="7"/>
-      <c r="G73" s="7" t="s">
-        <v>109</v>
-      </c>
+      <c r="G73" s="7"/>
       <c r="H73" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="I73" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="J73" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="K73" s="3"/>
+      <c r="K73" s="3" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="74" spans="1:26" s="21" customFormat="1" ht="14.4">
       <c r="A74" s="20"/>
       <c r="B74" s="20"/>
       <c r="E74" s="7" t="s">
-        <v>497</v>
+        <v>959</v>
       </c>
       <c r="F74" s="7"/>
-      <c r="G74" s="7"/>
-      <c r="H74" s="7"/>
-      <c r="K74" s="3" t="s">
-        <v>941</v>
-      </c>
+      <c r="G74" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="H74" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="I74" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="J74" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="K74" s="3"/>
     </row>
     <row r="75" spans="1:26" s="21" customFormat="1" ht="14.4">
       <c r="A75" s="20"/>
       <c r="B75" s="20"/>
       <c r="E75" s="7" t="s">
-        <v>854</v>
+        <v>497</v>
       </c>
       <c r="F75" s="7"/>
-      <c r="G75" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="H75" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="I75" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="J75" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="K75" s="21" t="s">
-        <v>856</v>
-      </c>
-      <c r="L75" s="3" t="s">
-        <v>855</v>
+      <c r="G75" s="7"/>
+      <c r="H75" s="7"/>
+      <c r="K75" s="3" t="s">
+        <v>941</v>
       </c>
     </row>
     <row r="76" spans="1:26" s="21" customFormat="1" ht="14.4">
       <c r="A76" s="20"/>
       <c r="B76" s="20"/>
       <c r="E76" s="7" t="s">
-        <v>918</v>
+        <v>854</v>
       </c>
       <c r="F76" s="7"/>
       <c r="G76" s="7" t="s">
         <v>29</v>
       </c>
       <c r="H76" s="7" t="s">
-        <v>129</v>
+        <v>73</v>
       </c>
       <c r="I76" s="21" t="s">
         <v>34</v>
@@ -22645,42 +22648,36 @@
         <v>30</v>
       </c>
       <c r="K76" s="21" t="s">
-        <v>903</v>
+        <v>856</v>
       </c>
       <c r="L76" s="3" t="s">
         <v>855</v>
       </c>
     </row>
-    <row r="77" spans="1:26" ht="14.4">
-      <c r="A77" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B77" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="C77" s="3" t="s">
-        <v>24</v>
-      </c>
+    <row r="77" spans="1:26" s="21" customFormat="1" ht="14.4">
+      <c r="A77" s="20"/>
+      <c r="B77" s="20"/>
       <c r="E77" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="F77" s="7">
-        <v>1</v>
-      </c>
+        <v>918</v>
+      </c>
+      <c r="F77" s="7"/>
       <c r="G77" s="7" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="H77" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="I77" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="I77" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="J77" s="3" t="s">
+      <c r="J77" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="K77" s="3" t="s">
-        <v>117</v>
+      <c r="K77" s="21" t="s">
+        <v>903</v>
+      </c>
+      <c r="L77" s="3" t="s">
+        <v>855</v>
       </c>
     </row>
     <row r="78" spans="1:26" ht="14.4">
@@ -22690,14 +22687,30 @@
       <c r="B78" s="15" t="s">
         <v>24</v>
       </c>
+      <c r="C78" s="3" t="s">
+        <v>24</v>
+      </c>
       <c r="E78" s="7" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="F78" s="7">
-        <v>553659</v>
-      </c>
-      <c r="G78" s="7"/>
-      <c r="H78" s="7"/>
+        <v>1</v>
+      </c>
+      <c r="G78" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="H78" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="I78" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="J78" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="K78" s="3" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="79" spans="1:26" ht="14.4">
       <c r="A79" s="15" t="s">
@@ -22707,10 +22720,10 @@
         <v>24</v>
       </c>
       <c r="E79" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F79" s="7">
-        <v>4891208</v>
+        <v>553659</v>
       </c>
       <c r="G79" s="7"/>
       <c r="H79" s="7"/>
@@ -22722,106 +22735,89 @@
       <c r="B80" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="C80" s="3" t="s">
+      <c r="E80" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="F80" s="7">
+        <v>4891208</v>
+      </c>
+      <c r="G80" s="7"/>
+      <c r="H80" s="7"/>
+    </row>
+    <row r="81" spans="1:12" ht="14.4">
+      <c r="A81" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B81" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="E80" s="7" t="s">
+      <c r="C81" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E81" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="F80" s="7">
+      <c r="F81" s="7">
         <v>1</v>
       </c>
-      <c r="G80" s="7" t="s">
+      <c r="G81" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="H80" s="7" t="s">
+      <c r="H81" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="I80" s="3" t="s">
+      <c r="I81" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="J80" s="3" t="s">
+      <c r="J81" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="K80" s="3" t="s">
+      <c r="K81" s="3" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="81" spans="1:12" s="21" customFormat="1" ht="14.4">
-      <c r="A81" s="20"/>
-      <c r="B81" s="20"/>
-      <c r="C81" s="3"/>
-      <c r="E81" s="7" t="s">
+    <row r="82" spans="1:12" s="21" customFormat="1" ht="14.4">
+      <c r="A82" s="20"/>
+      <c r="B82" s="20"/>
+      <c r="C82" s="3"/>
+      <c r="E82" s="7" t="s">
         <v>934</v>
       </c>
-      <c r="F81" s="7"/>
-      <c r="G81" s="7"/>
-      <c r="H81" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="I81" s="3"/>
-      <c r="J81" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="K81" s="3" t="s">
-        <v>936</v>
-      </c>
-    </row>
-    <row r="82" spans="1:12" s="21" customFormat="1" ht="14.4">
-      <c r="A82" s="20" t="s">
-        <v>837</v>
-      </c>
-      <c r="B82" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="C82" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="D82" s="21" t="s">
-        <v>65</v>
-      </c>
-      <c r="E82" s="7" t="s">
-        <v>836</v>
-      </c>
-      <c r="F82" s="7">
-        <v>5</v>
-      </c>
-      <c r="G82" s="7" t="s">
-        <v>109</v>
-      </c>
+      <c r="F82" s="7"/>
+      <c r="G82" s="7"/>
       <c r="H82" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="I82" s="3" t="s">
-        <v>26</v>
-      </c>
+      <c r="I82" s="3"/>
       <c r="J82" s="3" t="s">
         <v>27</v>
       </c>
       <c r="K82" s="3" t="s">
-        <v>838</v>
-      </c>
-      <c r="L82" s="23" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12" s="21" customFormat="1" ht="14.4">
+      <c r="A83" s="20" t="s">
+        <v>837</v>
+      </c>
+      <c r="B83" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="C83" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D83" s="21" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="83" spans="1:12" ht="14.4">
-      <c r="A83" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B83" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="D83" s="3" t="s">
-        <v>127</v>
-      </c>
       <c r="E83" s="7" t="s">
-        <v>128</v>
+        <v>836</v>
       </c>
       <c r="F83" s="7">
-        <v>0</v>
-      </c>
-      <c r="G83" s="7"/>
+        <v>5</v>
+      </c>
+      <c r="G83" s="7" t="s">
+        <v>109</v>
+      </c>
       <c r="H83" s="7" t="s">
         <v>129</v>
       </c>
@@ -22832,25 +22828,40 @@
         <v>27</v>
       </c>
       <c r="K83" s="3" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="84" spans="1:12" s="21" customFormat="1" ht="14.4">
-      <c r="A84" s="20"/>
-      <c r="B84" s="20"/>
-      <c r="D84" s="3"/>
+        <v>838</v>
+      </c>
+      <c r="L83" s="23" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12" ht="14.4">
+      <c r="A84" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B84" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D84" s="3" t="s">
+        <v>127</v>
+      </c>
       <c r="E84" s="7" t="s">
-        <v>935</v>
-      </c>
-      <c r="F84" s="7"/>
+        <v>128</v>
+      </c>
+      <c r="F84" s="7">
+        <v>0</v>
+      </c>
       <c r="G84" s="7"/>
       <c r="H84" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="I84" s="3"/>
-      <c r="J84" s="3"/>
+      <c r="I84" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J84" s="3" t="s">
+        <v>27</v>
+      </c>
       <c r="K84" s="3" t="s">
-        <v>937</v>
+        <v>130</v>
       </c>
     </row>
     <row r="85" spans="1:12" s="21" customFormat="1" ht="14.4">
@@ -22858,7 +22869,7 @@
       <c r="B85" s="20"/>
       <c r="D85" s="3"/>
       <c r="E85" s="7" t="s">
-        <v>938</v>
+        <v>935</v>
       </c>
       <c r="F85" s="7"/>
       <c r="G85" s="7"/>
@@ -22868,53 +22879,46 @@
       <c r="I85" s="3"/>
       <c r="J85" s="3"/>
       <c r="K85" s="3" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12" s="21" customFormat="1" ht="14.4">
+      <c r="A86" s="20"/>
+      <c r="B86" s="20"/>
+      <c r="D86" s="3"/>
+      <c r="E86" s="7" t="s">
+        <v>938</v>
+      </c>
+      <c r="F86" s="7"/>
+      <c r="G86" s="7"/>
+      <c r="H86" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="I86" s="3"/>
+      <c r="J86" s="3"/>
+      <c r="K86" s="3" t="s">
         <v>939</v>
       </c>
     </row>
-    <row r="86" spans="1:12" ht="14.4">
-      <c r="A86" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B86" s="15"/>
-      <c r="E86" s="7" t="s">
+    <row r="87" spans="1:12" ht="14.4">
+      <c r="A87" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B87" s="15"/>
+      <c r="E87" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="F86" s="7">
+      <c r="F87" s="7">
         <v>6772</v>
       </c>
-      <c r="G86" s="7"/>
-      <c r="H86" s="7"/>
-    </row>
-    <row r="87" spans="1:12" s="21" customFormat="1" ht="14.4">
-      <c r="A87" s="20"/>
-      <c r="B87" s="20"/>
-      <c r="E87" s="7" t="s">
-        <v>952</v>
-      </c>
-      <c r="F87" s="7">
-        <v>5</v>
-      </c>
-      <c r="G87" s="58" t="s">
-        <v>109</v>
-      </c>
-      <c r="H87" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="I87" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="J87" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="K87" s="23" t="s">
-        <v>953</v>
-      </c>
+      <c r="G87" s="7"/>
+      <c r="H87" s="7"/>
     </row>
     <row r="88" spans="1:12" s="21" customFormat="1" ht="14.4">
       <c r="A88" s="20"/>
       <c r="B88" s="20"/>
-      <c r="E88" s="58" t="s">
-        <v>954</v>
+      <c r="E88" s="7" t="s">
+        <v>952</v>
       </c>
       <c r="F88" s="7">
         <v>5</v>
@@ -22932,14 +22936,14 @@
         <v>30</v>
       </c>
       <c r="K88" s="23" t="s">
-        <v>955</v>
+        <v>953</v>
       </c>
     </row>
     <row r="89" spans="1:12" s="21" customFormat="1" ht="14.4">
       <c r="A89" s="20"/>
       <c r="B89" s="20"/>
       <c r="E89" s="58" t="s">
-        <v>956</v>
+        <v>954</v>
       </c>
       <c r="F89" s="7">
         <v>5</v>
@@ -22957,82 +22961,87 @@
         <v>30</v>
       </c>
       <c r="K89" s="23" t="s">
-        <v>957</v>
+        <v>955</v>
       </c>
     </row>
     <row r="90" spans="1:12" s="21" customFormat="1" ht="14.4">
       <c r="A90" s="20"/>
       <c r="B90" s="20"/>
-      <c r="E90" s="7" t="s">
-        <v>843</v>
+      <c r="E90" s="58" t="s">
+        <v>956</v>
       </c>
       <c r="F90" s="7">
-        <v>1</v>
-      </c>
-      <c r="G90" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G90" s="58" t="s">
         <v>109</v>
       </c>
       <c r="H90" s="7" t="s">
-        <v>844</v>
-      </c>
-      <c r="I90" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="J90" s="23" t="s">
-        <v>845</v>
+        <v>129</v>
+      </c>
+      <c r="I90" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="J90" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="K90" s="23" t="s">
+        <v>957</v>
       </c>
     </row>
     <row r="91" spans="1:12" s="21" customFormat="1" ht="14.4">
       <c r="A91" s="20"/>
       <c r="B91" s="20"/>
       <c r="E91" s="7" t="s">
-        <v>978</v>
-      </c>
-      <c r="F91" s="7"/>
+        <v>843</v>
+      </c>
+      <c r="F91" s="7">
+        <v>1</v>
+      </c>
       <c r="G91" s="7" t="s">
         <v>109</v>
       </c>
       <c r="H91" s="7" t="s">
-        <v>63</v>
+        <v>844</v>
       </c>
       <c r="I91" s="23" t="s">
         <v>26</v>
       </c>
       <c r="J91" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="K91" s="23" t="s">
-        <v>979</v>
-      </c>
-      <c r="L91" s="23" t="s">
-        <v>977</v>
+        <v>845</v>
       </c>
     </row>
     <row r="92" spans="1:12" s="21" customFormat="1" ht="14.4">
       <c r="A92" s="20"/>
       <c r="B92" s="20"/>
       <c r="E92" s="7" t="s">
-        <v>950</v>
+        <v>978</v>
       </c>
       <c r="F92" s="7"/>
       <c r="G92" s="7" t="s">
         <v>109</v>
       </c>
       <c r="H92" s="7" t="s">
-        <v>626</v>
-      </c>
-      <c r="I92" s="23"/>
-      <c r="J92" s="23"/>
+        <v>63</v>
+      </c>
+      <c r="I92" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="J92" s="23" t="s">
+        <v>27</v>
+      </c>
       <c r="K92" s="23" t="s">
-        <v>980</v>
-      </c>
-      <c r="L92" s="23"/>
+        <v>979</v>
+      </c>
+      <c r="L92" s="23" t="s">
+        <v>977</v>
+      </c>
     </row>
     <row r="93" spans="1:12" s="21" customFormat="1" ht="14.4">
       <c r="A93" s="20"/>
       <c r="B93" s="20"/>
       <c r="E93" s="7" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="F93" s="7"/>
       <c r="G93" s="7" t="s">
@@ -23044,69 +23053,66 @@
       <c r="I93" s="23"/>
       <c r="J93" s="23"/>
       <c r="K93" s="23" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
       <c r="L93" s="23"/>
     </row>
     <row r="94" spans="1:12" s="21" customFormat="1" ht="14.4">
       <c r="A94" s="20"/>
       <c r="B94" s="20"/>
-      <c r="D94" s="57" t="s">
-        <v>944</v>
-      </c>
       <c r="E94" s="7" t="s">
-        <v>970</v>
+        <v>951</v>
       </c>
       <c r="F94" s="7"/>
-      <c r="G94" s="58" t="s">
+      <c r="G94" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="H94" s="58" t="s">
-        <v>84</v>
-      </c>
-      <c r="I94" s="23" t="s">
-        <v>947</v>
-      </c>
-      <c r="J94" s="23" t="s">
-        <v>947</v>
-      </c>
+      <c r="H94" s="7" t="s">
+        <v>626</v>
+      </c>
+      <c r="I94" s="23"/>
+      <c r="J94" s="23"/>
       <c r="K94" s="23" t="s">
-        <v>971</v>
+        <v>981</v>
       </c>
       <c r="L94" s="23"/>
     </row>
     <row r="95" spans="1:12" s="21" customFormat="1" ht="14.4">
       <c r="A95" s="20"/>
       <c r="B95" s="20"/>
+      <c r="D95" s="57" t="s">
+        <v>944</v>
+      </c>
       <c r="E95" s="7" t="s">
-        <v>842</v>
-      </c>
-      <c r="F95" s="7">
-        <v>10</v>
-      </c>
-      <c r="G95" s="7" t="s">
+        <v>970</v>
+      </c>
+      <c r="F95" s="7"/>
+      <c r="G95" s="58" t="s">
         <v>109</v>
       </c>
-      <c r="H95" s="7" t="s">
-        <v>626</v>
+      <c r="H95" s="58" t="s">
+        <v>84</v>
       </c>
       <c r="I95" s="23" t="s">
-        <v>26</v>
+        <v>947</v>
       </c>
       <c r="J95" s="23" t="s">
-        <v>27</v>
+        <v>947</v>
       </c>
       <c r="K95" s="23" t="s">
-        <v>848</v>
-      </c>
+        <v>971</v>
+      </c>
+      <c r="L95" s="23"/>
     </row>
     <row r="96" spans="1:12" s="21" customFormat="1" ht="14.4">
       <c r="A96" s="20"/>
       <c r="B96" s="20"/>
       <c r="E96" s="7" t="s">
-        <v>960</v>
-      </c>
-      <c r="F96" s="7"/>
+        <v>842</v>
+      </c>
+      <c r="F96" s="7">
+        <v>10</v>
+      </c>
       <c r="G96" s="7" t="s">
         <v>109</v>
       </c>
@@ -23114,20 +23120,20 @@
         <v>626</v>
       </c>
       <c r="I96" s="23" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="J96" s="23" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="K96" s="23" t="s">
-        <v>961</v>
+        <v>848</v>
       </c>
     </row>
     <row r="97" spans="1:12" s="21" customFormat="1" ht="14.4">
       <c r="A97" s="20"/>
       <c r="B97" s="20"/>
       <c r="E97" s="7" t="s">
-        <v>974</v>
+        <v>960</v>
       </c>
       <c r="F97" s="7"/>
       <c r="G97" s="7" t="s">
@@ -23136,70 +23142,65 @@
       <c r="H97" s="7" t="s">
         <v>626</v>
       </c>
-      <c r="I97" s="23"/>
+      <c r="I97" s="23" t="s">
+        <v>34</v>
+      </c>
       <c r="J97" s="23" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="K97" s="23" t="s">
-        <v>975</v>
-      </c>
-      <c r="L97" s="23" t="s">
-        <v>976</v>
+        <v>961</v>
       </c>
     </row>
     <row r="98" spans="1:12" s="21" customFormat="1" ht="14.4">
       <c r="A98" s="20"/>
       <c r="B98" s="20"/>
       <c r="E98" s="7" t="s">
-        <v>510</v>
+        <v>974</v>
       </c>
       <c r="F98" s="7"/>
-      <c r="G98" s="7"/>
+      <c r="G98" s="7" t="s">
+        <v>109</v>
+      </c>
       <c r="H98" s="7" t="s">
-        <v>511</v>
+        <v>626</v>
       </c>
       <c r="I98" s="23"/>
-      <c r="J98" s="23"/>
+      <c r="J98" s="23" t="s">
+        <v>27</v>
+      </c>
       <c r="K98" s="23" t="s">
-        <v>943</v>
+        <v>975</v>
+      </c>
+      <c r="L98" s="23" t="s">
+        <v>976</v>
       </c>
     </row>
     <row r="99" spans="1:12" s="21" customFormat="1" ht="14.4">
       <c r="A99" s="20"/>
       <c r="B99" s="20"/>
-      <c r="D99" s="57" t="s">
-        <v>25</v>
-      </c>
       <c r="E99" s="7" t="s">
-        <v>796</v>
+        <v>510</v>
       </c>
       <c r="F99" s="7"/>
-      <c r="G99" s="58" t="s">
-        <v>29</v>
-      </c>
+      <c r="G99" s="7"/>
       <c r="H99" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="I99" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="J99" s="23" t="s">
-        <v>27</v>
-      </c>
+        <v>511</v>
+      </c>
+      <c r="I99" s="23"/>
+      <c r="J99" s="23"/>
       <c r="K99" s="23" t="s">
-        <v>797</v>
+        <v>943</v>
       </c>
     </row>
     <row r="100" spans="1:12" s="21" customFormat="1" ht="14.4">
-      <c r="A100" s="20" t="s">
-        <v>23</v>
-      </c>
+      <c r="A100" s="20"/>
       <c r="B100" s="20"/>
       <c r="D100" s="57" t="s">
         <v>25</v>
       </c>
       <c r="E100" s="7" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
       <c r="F100" s="7"/>
       <c r="G100" s="58" t="s">
@@ -23215,39 +23216,35 @@
         <v>27</v>
       </c>
       <c r="K100" s="23" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="101" spans="1:12" s="21" customFormat="1" ht="14.4">
+      <c r="A101" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="B101" s="20"/>
+      <c r="D101" s="57" t="s">
+        <v>25</v>
+      </c>
+      <c r="E101" s="7" t="s">
+        <v>798</v>
+      </c>
+      <c r="F101" s="7"/>
+      <c r="G101" s="58" t="s">
+        <v>29</v>
+      </c>
+      <c r="H101" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="I101" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="J101" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="K101" s="23" t="s">
         <v>799</v>
-      </c>
-    </row>
-    <row r="101" spans="1:12" ht="14.4">
-      <c r="A101" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B101" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="D101" s="17" t="s">
-        <v>133</v>
-      </c>
-      <c r="E101" s="18" t="s">
-        <v>135</v>
-      </c>
-      <c r="F101" s="18">
-        <v>1500</v>
-      </c>
-      <c r="G101" s="18" t="s">
-        <v>109</v>
-      </c>
-      <c r="H101" s="18" t="s">
-        <v>84</v>
-      </c>
-      <c r="I101" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="J101" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="K101" s="17" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="102" spans="1:12" ht="14.4">
@@ -23260,16 +23257,16 @@
       <c r="D102" s="17" t="s">
         <v>133</v>
       </c>
-      <c r="E102" s="17" t="s">
-        <v>140</v>
-      </c>
-      <c r="F102" s="17">
+      <c r="E102" s="18" t="s">
+        <v>135</v>
+      </c>
+      <c r="F102" s="18">
         <v>1500</v>
       </c>
       <c r="G102" s="18" t="s">
         <v>109</v>
       </c>
-      <c r="H102" s="17" t="s">
+      <c r="H102" s="18" t="s">
         <v>84</v>
       </c>
       <c r="I102" s="17" t="s">
@@ -23279,7 +23276,7 @@
         <v>30</v>
       </c>
       <c r="K102" s="17" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="103" spans="1:12" ht="14.4">
@@ -23293,7 +23290,7 @@
         <v>133</v>
       </c>
       <c r="E103" s="17" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="F103" s="17">
         <v>1500</v>
@@ -23311,13 +23308,45 @@
         <v>30</v>
       </c>
       <c r="K103" s="17" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="104" spans="1:12" ht="14.4">
+      <c r="A104" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B104" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="D104" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="E104" s="17" t="s">
+        <v>143</v>
+      </c>
+      <c r="F104" s="17">
+        <v>1500</v>
+      </c>
+      <c r="G104" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="H104" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="I104" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="J104" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="K104" s="17" t="s">
         <v>144</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B59:B62">
+  <conditionalFormatting sqref="B60:B63">
     <cfRule type="notContainsBlanks" dxfId="0" priority="1">
-      <formula>LEN(TRIM(B59))&gt;0</formula>
+      <formula>LEN(TRIM(B60))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add CW3M_LULC_NWI_crosswalk.xlsx to the repository. CW3MdataDictionary.xlsx, IDU_McKenzie.dbf, Reach_McKenzie.dbf - Add IDU attributes WETNESS, WETL_CAP; and Reach attributes Q_CAP, QSPILL_FRC, and RIVER_KM. Flow.cpp, .h - Begin to add code to populate RIVER_KM. Add and then comment out code in FlowModel::Init() to read a Shade-a-lator data file and populate CW3M data. Add more columns to the ReachInsolationData.csv file.
</commit_message>
<xml_diff>
--- a/DataCW3M/CW3MdigitalHandbook/CW3MdataDictionary.xlsx
+++ b/DataCW3M/CW3MdigitalHandbook/CW3MdataDictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\CW3MdigitalHandbook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AB58806-7FC8-49D7-ADD0-C16DE25831D8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A47A7341-D7B1-428D-9D91-D618D815EAD7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-7425" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Necessary input data" sheetId="7" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="Conventions" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -77,7 +78,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H263" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+    <comment ref="H264" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -96,7 +97,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2963" uniqueCount="990">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2987" uniqueCount="1001">
   <si>
     <t>LULC_A</t>
   </si>
@@ -3067,6 +3068,39 @@
   </si>
   <si>
     <t>estimate of daily average surface insolation flux based on geographical location and date, for comparison to Shade-a-lator output</t>
+  </si>
+  <si>
+    <t>WETNESS</t>
+  </si>
+  <si>
+    <t>&gt;0 =&gt; depth of inundation; &lt;0 =&gt; depth of water required to reach saturation</t>
+  </si>
+  <si>
+    <t>m3 H2O or maybe mm H2O</t>
+  </si>
+  <si>
+    <t>Q_CAP</t>
+  </si>
+  <si>
+    <t>how much flow there can be before some of it spills over into adjacent wetlands</t>
+  </si>
+  <si>
+    <t>fraction of 1</t>
+  </si>
+  <si>
+    <t>when Q overflows the channel, this is the fraction which diverts to the adjacent wetlands</t>
+  </si>
+  <si>
+    <t>QSPILL_FRC</t>
+  </si>
+  <si>
+    <t>RIVER_KM</t>
+  </si>
+  <si>
+    <t>km</t>
+  </si>
+  <si>
+    <t>distance from the downstream end of the reach to the outlet; "river mile" only in metric</t>
   </si>
 </sst>
 </file>
@@ -3177,7 +3211,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="100">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -3393,6 +3427,16 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -9016,11 +9060,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Z1047"/>
+  <dimension ref="A1:Z1048"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A128" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H199" sqref="H199"/>
+      <pane ySplit="3" topLeftCell="A200" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E225" sqref="E225"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -16717,8 +16761,8 @@
       <c r="D224" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="E224" s="10" t="s">
-        <v>95</v>
+      <c r="E224" s="70" t="s">
+        <v>992</v>
       </c>
       <c r="F224" s="10"/>
       <c r="G224" s="10" t="s">
@@ -16743,170 +16787,159 @@
       <c r="T224" s="7"/>
       <c r="U224" s="7"/>
     </row>
-    <row r="225" spans="1:26" s="21" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A225" s="28"/>
-      <c r="B225" s="28"/>
-      <c r="C225" s="7" t="s">
+    <row r="225" spans="1:26" s="65" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A225" s="66"/>
+      <c r="B225" s="66"/>
+      <c r="C225" s="64" t="s">
         <v>825</v>
       </c>
-      <c r="D225" s="10" t="s">
+      <c r="D225" s="62" t="s">
         <v>29</v>
       </c>
-      <c r="E225" s="10" t="s">
+      <c r="E225" s="62" t="s">
         <v>227</v>
       </c>
-      <c r="F225" s="10" t="s">
+      <c r="F225" s="62" t="s">
         <v>826</v>
       </c>
-      <c r="G225" s="10" t="s">
+      <c r="G225" s="62" t="s">
         <v>27</v>
       </c>
-      <c r="H225" s="72" t="s">
+      <c r="H225" s="60" t="s">
         <v>827</v>
       </c>
-      <c r="I225" s="27" t="s">
+      <c r="I225" s="74" t="s">
         <v>828</v>
       </c>
-      <c r="J225" s="3"/>
-      <c r="K225" s="7"/>
-      <c r="L225" s="7"/>
-      <c r="M225" s="7"/>
-      <c r="N225" s="7"/>
-      <c r="O225" s="7"/>
-      <c r="P225" s="7"/>
-      <c r="Q225" s="7"/>
-      <c r="R225" s="7"/>
-      <c r="S225" s="7"/>
-      <c r="T225" s="7"/>
-      <c r="U225" s="7"/>
-    </row>
-    <row r="226" spans="1:26" s="21" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A226" s="28"/>
-      <c r="B226" s="28"/>
-      <c r="C226" s="7" t="s">
+      <c r="J225" s="68"/>
+      <c r="K225" s="64"/>
+      <c r="L225" s="64"/>
+      <c r="M225" s="64"/>
+      <c r="N225" s="64"/>
+      <c r="O225" s="64"/>
+      <c r="P225" s="64"/>
+      <c r="Q225" s="64"/>
+      <c r="R225" s="64"/>
+      <c r="S225" s="64"/>
+      <c r="T225" s="64"/>
+      <c r="U225" s="64"/>
+    </row>
+    <row r="226" spans="1:26" s="65" customFormat="1" ht="13.8" customHeight="1">
+      <c r="A226" s="66"/>
+      <c r="B226" s="66"/>
+      <c r="C226" s="64" t="s">
         <v>832</v>
       </c>
-      <c r="D226" s="10" t="s">
+      <c r="D226" s="62" t="s">
         <v>29</v>
       </c>
-      <c r="E226" s="10" t="s">
+      <c r="E226" s="62" t="s">
         <v>95</v>
       </c>
-      <c r="F226" s="10" t="s">
+      <c r="F226" s="62" t="s">
         <v>65</v>
       </c>
-      <c r="G226" s="10" t="s">
+      <c r="G226" s="62" t="s">
         <v>27</v>
       </c>
-      <c r="H226" s="25" t="s">
+      <c r="H226" s="61" t="s">
         <v>833</v>
       </c>
-      <c r="I226" s="27" t="s">
+      <c r="I226" s="74" t="s">
         <v>834</v>
       </c>
-      <c r="J226" s="3"/>
-      <c r="K226" s="7"/>
-      <c r="L226" s="7"/>
-      <c r="M226" s="7"/>
-      <c r="N226" s="7"/>
-      <c r="O226" s="7"/>
-      <c r="P226" s="7"/>
-      <c r="Q226" s="7"/>
-      <c r="R226" s="7"/>
-      <c r="S226" s="7"/>
-      <c r="T226" s="7"/>
-      <c r="U226" s="7"/>
-    </row>
-    <row r="227" spans="1:26" ht="42.75" customHeight="1">
-      <c r="A227" s="6"/>
-      <c r="B227" s="6"/>
-      <c r="C227" s="18" t="s">
+      <c r="J226" s="68"/>
+      <c r="K226" s="64"/>
+      <c r="L226" s="64"/>
+      <c r="M226" s="64"/>
+      <c r="N226" s="64"/>
+      <c r="O226" s="64"/>
+      <c r="P226" s="64"/>
+      <c r="Q226" s="64"/>
+      <c r="R226" s="64"/>
+      <c r="S226" s="64"/>
+      <c r="T226" s="64"/>
+      <c r="U226" s="64"/>
+    </row>
+    <row r="227" spans="1:26" s="91" customFormat="1" ht="13.8" customHeight="1">
+      <c r="A227" s="96"/>
+      <c r="B227" s="96"/>
+      <c r="C227" s="97" t="s">
+        <v>990</v>
+      </c>
+      <c r="D227" s="99" t="s">
+        <v>109</v>
+      </c>
+      <c r="E227" s="99" t="s">
+        <v>173</v>
+      </c>
+      <c r="F227" s="99" t="s">
+        <v>826</v>
+      </c>
+      <c r="G227" s="99" t="s">
+        <v>27</v>
+      </c>
+      <c r="H227" s="77" t="s">
+        <v>991</v>
+      </c>
+      <c r="I227" s="98"/>
+      <c r="J227" s="84"/>
+      <c r="K227" s="97"/>
+      <c r="L227" s="97"/>
+      <c r="M227" s="97"/>
+      <c r="N227" s="97"/>
+      <c r="O227" s="97"/>
+      <c r="P227" s="97"/>
+      <c r="Q227" s="97"/>
+      <c r="R227" s="97"/>
+      <c r="S227" s="97"/>
+      <c r="T227" s="97"/>
+      <c r="U227" s="97"/>
+    </row>
+    <row r="228" spans="1:26" s="21" customFormat="1" ht="16.8" customHeight="1">
+      <c r="A228" s="28"/>
+      <c r="B228" s="28"/>
+      <c r="C228" s="21" t="s">
         <v>510</v>
       </c>
-      <c r="D227" s="10" t="s">
+      <c r="D228" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="E227" s="10" t="s">
+      <c r="E228" s="10" t="s">
         <v>511</v>
       </c>
-      <c r="F227" s="10" t="s">
+      <c r="F228" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="G227" s="10" t="s">
+      <c r="G228" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="H227" s="25" t="s">
+      <c r="H228" s="21" t="s">
         <v>729</v>
       </c>
-      <c r="I227" s="26" t="s">
+      <c r="I228" s="27" t="s">
         <v>815</v>
       </c>
-      <c r="J227" s="3"/>
-      <c r="K227" s="7"/>
-      <c r="L227" s="7"/>
-      <c r="M227" s="7"/>
-      <c r="N227" s="7"/>
-      <c r="O227" s="7"/>
-      <c r="P227" s="7"/>
-      <c r="Q227" s="7"/>
-      <c r="R227" s="7"/>
-      <c r="S227" s="7"/>
-      <c r="T227" s="7"/>
-      <c r="U227" s="7"/>
-    </row>
-    <row r="228" spans="1:26" ht="42.75" customHeight="1">
-      <c r="A228" s="6"/>
-      <c r="B228" s="6" t="s">
-        <v>160</v>
-      </c>
-      <c r="C228" s="7" t="s">
-        <v>730</v>
-      </c>
-      <c r="D228" s="8"/>
-      <c r="E228" s="8" t="s">
-        <v>731</v>
-      </c>
-      <c r="F228" s="10"/>
-      <c r="G228" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="H228" s="14" t="s">
-        <v>732</v>
-      </c>
-      <c r="I228" s="27" t="s">
-        <v>728</v>
-      </c>
-      <c r="J228" s="3"/>
-      <c r="K228" s="7"/>
-      <c r="L228" s="7"/>
-      <c r="M228" s="7"/>
-      <c r="N228" s="7"/>
-      <c r="O228" s="7"/>
-      <c r="P228" s="7"/>
-      <c r="Q228" s="7"/>
-      <c r="R228" s="7"/>
-      <c r="S228" s="7"/>
-      <c r="T228" s="7"/>
-      <c r="U228" s="7"/>
-    </row>
-    <row r="229" spans="1:26" ht="14.25" customHeight="1">
+      <c r="J228" s="23"/>
+    </row>
+    <row r="229" spans="1:26" ht="42.75" customHeight="1">
       <c r="A229" s="6"/>
       <c r="B229" s="6" t="s">
         <v>160</v>
       </c>
       <c r="C229" s="7" t="s">
-        <v>733</v>
+        <v>730</v>
       </c>
       <c r="D229" s="8"/>
       <c r="E229" s="8" t="s">
-        <v>70</v>
+        <v>731</v>
       </c>
       <c r="F229" s="10"/>
       <c r="G229" s="8" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="H229" s="14" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="I229" s="27" t="s">
         <v>728</v>
@@ -16927,10 +16960,10 @@
     <row r="230" spans="1:26" ht="14.25" customHeight="1">
       <c r="A230" s="6"/>
       <c r="B230" s="6" t="s">
-        <v>23</v>
+        <v>160</v>
       </c>
       <c r="C230" s="7" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="D230" s="8"/>
       <c r="E230" s="8" t="s">
@@ -16938,10 +16971,10 @@
       </c>
       <c r="F230" s="10"/>
       <c r="G230" s="8" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="H230" s="14" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="I230" s="27" t="s">
         <v>728</v>
@@ -16962,10 +16995,10 @@
     <row r="231" spans="1:26" ht="14.25" customHeight="1">
       <c r="A231" s="6"/>
       <c r="B231" s="6" t="s">
-        <v>160</v>
+        <v>23</v>
       </c>
       <c r="C231" s="7" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="D231" s="8"/>
       <c r="E231" s="8" t="s">
@@ -16973,12 +17006,14 @@
       </c>
       <c r="F231" s="10"/>
       <c r="G231" s="8" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="H231" s="14" t="s">
-        <v>738</v>
-      </c>
-      <c r="I231" s="27"/>
+        <v>736</v>
+      </c>
+      <c r="I231" s="27" t="s">
+        <v>728</v>
+      </c>
       <c r="J231" s="3"/>
       <c r="K231" s="7"/>
       <c r="L231" s="7"/>
@@ -16998,22 +17033,20 @@
         <v>160</v>
       </c>
       <c r="C232" s="7" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="D232" s="8"/>
       <c r="E232" s="8" t="s">
-        <v>227</v>
+        <v>70</v>
       </c>
       <c r="F232" s="10"/>
       <c r="G232" s="8" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="H232" s="14" t="s">
-        <v>740</v>
-      </c>
-      <c r="I232" s="27" t="s">
-        <v>728</v>
-      </c>
+        <v>738</v>
+      </c>
+      <c r="I232" s="27"/>
       <c r="J232" s="3"/>
       <c r="K232" s="7"/>
       <c r="L232" s="7"/>
@@ -17033,7 +17066,7 @@
         <v>160</v>
       </c>
       <c r="C233" s="7" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="D233" s="8"/>
       <c r="E233" s="8" t="s">
@@ -17044,7 +17077,7 @@
         <v>27</v>
       </c>
       <c r="H233" s="14" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="I233" s="27" t="s">
         <v>728</v>
@@ -17065,22 +17098,24 @@
     <row r="234" spans="1:26" ht="14.25" customHeight="1">
       <c r="A234" s="6"/>
       <c r="B234" s="6" t="s">
-        <v>23</v>
+        <v>160</v>
       </c>
       <c r="C234" s="7" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="D234" s="8"/>
-      <c r="E234" s="8"/>
+      <c r="E234" s="8" t="s">
+        <v>227</v>
+      </c>
       <c r="F234" s="10"/>
       <c r="G234" s="8" t="s">
         <v>27</v>
       </c>
       <c r="H234" s="14" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
       <c r="I234" s="27" t="s">
-        <v>114</v>
+        <v>728</v>
       </c>
       <c r="J234" s="3"/>
       <c r="K234" s="7"/>
@@ -17098,21 +17133,19 @@
     <row r="235" spans="1:26" ht="14.25" customHeight="1">
       <c r="A235" s="6"/>
       <c r="B235" s="6" t="s">
-        <v>160</v>
+        <v>23</v>
       </c>
       <c r="C235" s="7" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
       <c r="D235" s="8"/>
-      <c r="E235" s="8" t="s">
-        <v>746</v>
-      </c>
+      <c r="E235" s="8"/>
       <c r="F235" s="10"/>
       <c r="G235" s="8" t="s">
         <v>27</v>
       </c>
       <c r="H235" s="14" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="I235" s="27" t="s">
         <v>114</v>
@@ -17131,25 +17164,23 @@
       <c r="U235" s="7"/>
     </row>
     <row r="236" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A236" s="6" t="s">
-        <v>310</v>
-      </c>
+      <c r="A236" s="6"/>
       <c r="B236" s="6" t="s">
-        <v>23</v>
+        <v>160</v>
       </c>
       <c r="C236" s="7" t="s">
-        <v>748</v>
+        <v>745</v>
       </c>
       <c r="D236" s="8"/>
       <c r="E236" s="8" t="s">
-        <v>749</v>
+        <v>746</v>
       </c>
       <c r="F236" s="10"/>
       <c r="G236" s="8" t="s">
         <v>27</v>
       </c>
       <c r="H236" s="14" t="s">
-        <v>750</v>
+        <v>747</v>
       </c>
       <c r="I236" s="27" t="s">
         <v>114</v>
@@ -17168,31 +17199,31 @@
       <c r="U236" s="7"/>
     </row>
     <row r="237" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A237" s="6"/>
+      <c r="A237" s="6" t="s">
+        <v>310</v>
+      </c>
       <c r="B237" s="6" t="s">
-        <v>160</v>
+        <v>23</v>
       </c>
       <c r="C237" s="7" t="s">
-        <v>381</v>
+        <v>748</v>
       </c>
       <c r="D237" s="8"/>
       <c r="E237" s="8" t="s">
-        <v>197</v>
+        <v>749</v>
       </c>
       <c r="F237" s="10"/>
       <c r="G237" s="8" t="s">
         <v>27</v>
       </c>
       <c r="H237" s="14" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="I237" s="27" t="s">
         <v>114</v>
       </c>
       <c r="J237" s="3"/>
-      <c r="K237" s="3" t="s">
-        <v>190</v>
-      </c>
+      <c r="K237" s="7"/>
       <c r="L237" s="7"/>
       <c r="M237" s="7"/>
       <c r="N237" s="7"/>
@@ -17203,38 +17234,33 @@
       <c r="S237" s="7"/>
       <c r="T237" s="7"/>
       <c r="U237" s="7"/>
-      <c r="V237" s="7"/>
-      <c r="W237" s="7"/>
-      <c r="X237" s="7"/>
-      <c r="Y237" s="7"/>
-      <c r="Z237" s="7"/>
     </row>
     <row r="238" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A238" s="6" t="s">
-        <v>752</v>
-      </c>
+      <c r="A238" s="6"/>
       <c r="B238" s="6" t="s">
-        <v>23</v>
+        <v>160</v>
       </c>
       <c r="C238" s="7" t="s">
-        <v>753</v>
+        <v>381</v>
       </c>
       <c r="D238" s="8"/>
       <c r="E238" s="8" t="s">
-        <v>70</v>
+        <v>197</v>
       </c>
       <c r="F238" s="10"/>
       <c r="G238" s="8" t="s">
         <v>27</v>
       </c>
       <c r="H238" s="14" t="s">
-        <v>754</v>
+        <v>751</v>
       </c>
       <c r="I238" s="27" t="s">
         <v>114</v>
       </c>
       <c r="J238" s="3"/>
-      <c r="K238" s="7"/>
+      <c r="K238" s="3" t="s">
+        <v>190</v>
+      </c>
       <c r="L238" s="7"/>
       <c r="M238" s="7"/>
       <c r="N238" s="7"/>
@@ -17245,25 +17271,32 @@
       <c r="S238" s="7"/>
       <c r="T238" s="7"/>
       <c r="U238" s="7"/>
+      <c r="V238" s="7"/>
+      <c r="W238" s="7"/>
+      <c r="X238" s="7"/>
+      <c r="Y238" s="7"/>
+      <c r="Z238" s="7"/>
     </row>
     <row r="239" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A239" s="6"/>
+      <c r="A239" s="6" t="s">
+        <v>752</v>
+      </c>
       <c r="B239" s="6" t="s">
         <v>23</v>
       </c>
       <c r="C239" s="7" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
       <c r="D239" s="8"/>
       <c r="E239" s="8" t="s">
-        <v>756</v>
+        <v>70</v>
       </c>
       <c r="F239" s="10"/>
       <c r="G239" s="8" t="s">
         <v>27</v>
       </c>
       <c r="H239" s="14" t="s">
-        <v>757</v>
+        <v>754</v>
       </c>
       <c r="I239" s="27" t="s">
         <v>114</v>
@@ -17287,18 +17320,18 @@
         <v>23</v>
       </c>
       <c r="C240" s="7" t="s">
-        <v>758</v>
+        <v>755</v>
       </c>
       <c r="D240" s="8"/>
       <c r="E240" s="8" t="s">
-        <v>759</v>
+        <v>756</v>
       </c>
       <c r="F240" s="10"/>
       <c r="G240" s="8" t="s">
         <v>27</v>
       </c>
       <c r="H240" s="14" t="s">
-        <v>760</v>
+        <v>757</v>
       </c>
       <c r="I240" s="27" t="s">
         <v>114</v>
@@ -17317,23 +17350,23 @@
       <c r="U240" s="7"/>
     </row>
     <row r="241" spans="1:21" ht="14.25" customHeight="1">
-      <c r="A241" s="6" t="s">
-        <v>310</v>
-      </c>
+      <c r="A241" s="6"/>
       <c r="B241" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C241" s="8" t="s">
-        <v>761</v>
+      <c r="C241" s="7" t="s">
+        <v>758</v>
       </c>
       <c r="D241" s="8"/>
-      <c r="E241" s="8"/>
+      <c r="E241" s="8" t="s">
+        <v>759</v>
+      </c>
       <c r="F241" s="10"/>
       <c r="G241" s="8" t="s">
         <v>27</v>
       </c>
       <c r="H241" s="14" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
       <c r="I241" s="27" t="s">
         <v>114</v>
@@ -17358,8 +17391,8 @@
       <c r="B242" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C242" s="7" t="s">
-        <v>763</v>
+      <c r="C242" s="8" t="s">
+        <v>761</v>
       </c>
       <c r="D242" s="8"/>
       <c r="E242" s="8"/>
@@ -17394,7 +17427,7 @@
         <v>23</v>
       </c>
       <c r="C243" s="7" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="D243" s="8"/>
       <c r="E243" s="8"/>
@@ -17429,7 +17462,7 @@
         <v>23</v>
       </c>
       <c r="C244" s="7" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="D244" s="8"/>
       <c r="E244" s="8"/>
@@ -17464,7 +17497,7 @@
         <v>23</v>
       </c>
       <c r="C245" s="7" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="D245" s="8"/>
       <c r="E245" s="8"/>
@@ -17499,7 +17532,7 @@
         <v>23</v>
       </c>
       <c r="C246" s="7" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="D246" s="8"/>
       <c r="E246" s="8"/>
@@ -17534,7 +17567,7 @@
         <v>23</v>
       </c>
       <c r="C247" s="7" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="D247" s="8"/>
       <c r="E247" s="8"/>
@@ -17569,7 +17602,7 @@
         <v>23</v>
       </c>
       <c r="C248" s="7" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="D248" s="8"/>
       <c r="E248" s="8"/>
@@ -17604,7 +17637,7 @@
         <v>23</v>
       </c>
       <c r="C249" s="7" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="D249" s="8"/>
       <c r="E249" s="8"/>
@@ -17639,7 +17672,7 @@
         <v>23</v>
       </c>
       <c r="C250" s="7" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="D250" s="8"/>
       <c r="E250" s="8"/>
@@ -17674,7 +17707,7 @@
         <v>23</v>
       </c>
       <c r="C251" s="7" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="D251" s="8"/>
       <c r="E251" s="8"/>
@@ -17709,7 +17742,7 @@
         <v>23</v>
       </c>
       <c r="C252" s="7" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="D252" s="8"/>
       <c r="E252" s="8"/>
@@ -17744,7 +17777,7 @@
         <v>23</v>
       </c>
       <c r="C253" s="7" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="D253" s="8"/>
       <c r="E253" s="8"/>
@@ -17779,7 +17812,7 @@
         <v>23</v>
       </c>
       <c r="C254" s="7" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="D254" s="8"/>
       <c r="E254" s="8"/>
@@ -17814,7 +17847,7 @@
         <v>23</v>
       </c>
       <c r="C255" s="7" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="D255" s="8"/>
       <c r="E255" s="8"/>
@@ -17849,7 +17882,7 @@
         <v>23</v>
       </c>
       <c r="C256" s="7" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="D256" s="8"/>
       <c r="E256" s="8"/>
@@ -17884,7 +17917,7 @@
         <v>23</v>
       </c>
       <c r="C257" s="7" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="D257" s="8"/>
       <c r="E257" s="8"/>
@@ -17912,19 +17945,27 @@
       <c r="U257" s="7"/>
     </row>
     <row r="258" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A258" s="6"/>
+      <c r="A258" s="6" t="s">
+        <v>310</v>
+      </c>
       <c r="B258" s="6" t="s">
         <v>23</v>
       </c>
       <c r="C258" s="7" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="D258" s="8"/>
       <c r="E258" s="8"/>
       <c r="F258" s="10"/>
-      <c r="G258" s="8"/>
-      <c r="H258" s="14"/>
-      <c r="I258" s="27"/>
+      <c r="G258" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="H258" s="14" t="s">
+        <v>762</v>
+      </c>
+      <c r="I258" s="27" t="s">
+        <v>114</v>
+      </c>
       <c r="J258" s="3"/>
       <c r="K258" s="7"/>
       <c r="L258" s="7"/>
@@ -17941,22 +17982,16 @@
     <row r="259" spans="1:26" ht="14.25" customHeight="1">
       <c r="A259" s="6"/>
       <c r="B259" s="6" t="s">
-        <v>160</v>
+        <v>23</v>
       </c>
       <c r="C259" s="7" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="D259" s="8"/>
-      <c r="E259" s="8" t="s">
-        <v>158</v>
-      </c>
+      <c r="E259" s="8"/>
       <c r="F259" s="10"/>
-      <c r="G259" s="8" t="s">
-        <v>781</v>
-      </c>
-      <c r="H259" s="14" t="s">
-        <v>782</v>
-      </c>
+      <c r="G259" s="8"/>
+      <c r="H259" s="14"/>
       <c r="I259" s="27"/>
       <c r="J259" s="3"/>
       <c r="K259" s="7"/>
@@ -17977,7 +18012,7 @@
         <v>160</v>
       </c>
       <c r="C260" s="7" t="s">
-        <v>783</v>
+        <v>780</v>
       </c>
       <c r="D260" s="8"/>
       <c r="E260" s="8" t="s">
@@ -17988,7 +18023,7 @@
         <v>781</v>
       </c>
       <c r="H260" s="14" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="I260" s="27"/>
       <c r="J260" s="3"/>
@@ -18007,10 +18042,10 @@
     <row r="261" spans="1:26" ht="14.25" customHeight="1">
       <c r="A261" s="6"/>
       <c r="B261" s="6" t="s">
-        <v>23</v>
+        <v>160</v>
       </c>
       <c r="C261" s="7" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="D261" s="8"/>
       <c r="E261" s="8" t="s">
@@ -18021,7 +18056,7 @@
         <v>781</v>
       </c>
       <c r="H261" s="14" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="I261" s="27"/>
       <c r="J261" s="3"/>
@@ -18038,96 +18073,106 @@
       <c r="U261" s="7"/>
     </row>
     <row r="262" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A262" s="36" t="s">
+      <c r="A262" s="6"/>
+      <c r="B262" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C262" s="7" t="s">
+        <v>785</v>
+      </c>
+      <c r="D262" s="8"/>
+      <c r="E262" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="F262" s="10"/>
+      <c r="G262" s="8" t="s">
+        <v>781</v>
+      </c>
+      <c r="H262" s="14" t="s">
+        <v>786</v>
+      </c>
+      <c r="I262" s="27"/>
+      <c r="J262" s="3"/>
+      <c r="K262" s="7"/>
+      <c r="L262" s="7"/>
+      <c r="M262" s="7"/>
+      <c r="N262" s="7"/>
+      <c r="O262" s="7"/>
+      <c r="P262" s="7"/>
+      <c r="Q262" s="7"/>
+      <c r="R262" s="7"/>
+      <c r="S262" s="7"/>
+      <c r="T262" s="7"/>
+      <c r="U262" s="7"/>
+    </row>
+    <row r="263" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A263" s="36" t="s">
         <v>218</v>
       </c>
-      <c r="B262" s="29"/>
-      <c r="C262" s="37" t="s">
+      <c r="B263" s="29"/>
+      <c r="C263" s="37" t="s">
         <v>787</v>
       </c>
-      <c r="D262" s="38" t="s">
+      <c r="D263" s="38" t="s">
         <v>29</v>
       </c>
-      <c r="E262" s="38" t="s">
+      <c r="E263" s="38" t="s">
         <v>788</v>
       </c>
-      <c r="F262" s="38" t="s">
+      <c r="F263" s="38" t="s">
         <v>26</v>
       </c>
-      <c r="G262" s="38" t="s">
+      <c r="G263" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="H262" s="39" t="s">
+      <c r="H263" s="39" t="s">
         <v>789</v>
       </c>
-      <c r="I262" s="31"/>
-      <c r="J262" s="34"/>
-      <c r="K262" s="34"/>
-      <c r="L262" s="30"/>
-      <c r="M262" s="30"/>
-      <c r="N262" s="30"/>
-      <c r="O262" s="30"/>
-      <c r="P262" s="30"/>
-      <c r="Q262" s="30"/>
-      <c r="R262" s="30"/>
-      <c r="S262" s="30"/>
-      <c r="T262" s="30"/>
-      <c r="U262" s="30"/>
-      <c r="V262" s="35"/>
-      <c r="W262" s="35"/>
-      <c r="X262" s="35"/>
-      <c r="Y262" s="35"/>
-      <c r="Z262" s="35"/>
-    </row>
-    <row r="263" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A263" s="6" t="s">
+      <c r="I263" s="31"/>
+      <c r="J263" s="34"/>
+      <c r="K263" s="34"/>
+      <c r="L263" s="30"/>
+      <c r="M263" s="30"/>
+      <c r="N263" s="30"/>
+      <c r="O263" s="30"/>
+      <c r="P263" s="30"/>
+      <c r="Q263" s="30"/>
+      <c r="R263" s="30"/>
+      <c r="S263" s="30"/>
+      <c r="T263" s="30"/>
+      <c r="U263" s="30"/>
+      <c r="V263" s="35"/>
+      <c r="W263" s="35"/>
+      <c r="X263" s="35"/>
+      <c r="Y263" s="35"/>
+      <c r="Z263" s="35"/>
+    </row>
+    <row r="264" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A264" s="6" t="s">
         <v>790</v>
       </c>
-      <c r="B263" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C263" s="7" t="s">
+      <c r="B264" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C264" s="7" t="s">
         <v>229</v>
       </c>
-      <c r="D263" s="8"/>
-      <c r="E263" s="8" t="s">
+      <c r="D264" s="8"/>
+      <c r="E264" s="8" t="s">
         <v>197</v>
       </c>
-      <c r="F263" s="10"/>
-      <c r="G263" s="8" t="s">
+      <c r="F264" s="10"/>
+      <c r="G264" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="H263" s="14" t="s">
+      <c r="H264" s="14" t="s">
         <v>791</v>
       </c>
-      <c r="I263" s="8"/>
-      <c r="J263" s="3"/>
-      <c r="K263" s="3" t="s">
+      <c r="I264" s="8"/>
+      <c r="J264" s="3"/>
+      <c r="K264" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="L263" s="7"/>
-      <c r="M263" s="7"/>
-      <c r="N263" s="7"/>
-      <c r="O263" s="7"/>
-      <c r="P263" s="7"/>
-      <c r="Q263" s="7"/>
-      <c r="R263" s="7"/>
-      <c r="S263" s="7"/>
-      <c r="T263" s="7"/>
-      <c r="U263" s="7"/>
-    </row>
-    <row r="264" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A264" s="6"/>
-      <c r="B264" s="6"/>
-      <c r="C264" s="7"/>
-      <c r="D264" s="8"/>
-      <c r="E264" s="8"/>
-      <c r="F264" s="10"/>
-      <c r="G264" s="8"/>
-      <c r="H264" s="14"/>
-      <c r="I264" s="27"/>
-      <c r="J264" s="3"/>
-      <c r="K264" s="7"/>
       <c r="L264" s="7"/>
       <c r="M264" s="7"/>
       <c r="N264" s="7"/>
@@ -18148,8 +18193,8 @@
       <c r="F265" s="10"/>
       <c r="G265" s="8"/>
       <c r="H265" s="14"/>
-      <c r="I265" s="8"/>
-      <c r="J265" s="7"/>
+      <c r="I265" s="27"/>
+      <c r="J265" s="3"/>
       <c r="K265" s="7"/>
       <c r="L265" s="7"/>
       <c r="M265" s="7"/>
@@ -18376,8 +18421,8 @@
       <c r="D275" s="8"/>
       <c r="E275" s="8"/>
       <c r="F275" s="10"/>
-      <c r="G275" s="9"/>
-      <c r="H275" s="7"/>
+      <c r="G275" s="8"/>
+      <c r="H275" s="14"/>
       <c r="I275" s="8"/>
       <c r="J275" s="7"/>
       <c r="K275" s="7"/>
@@ -18392,14 +18437,14 @@
       <c r="T275" s="7"/>
       <c r="U275" s="7"/>
     </row>
-    <row r="276" spans="1:21" ht="14.4">
+    <row r="276" spans="1:21" ht="14.25" customHeight="1">
       <c r="A276" s="6"/>
       <c r="B276" s="6"/>
       <c r="C276" s="7"/>
       <c r="D276" s="8"/>
       <c r="E276" s="8"/>
       <c r="F276" s="10"/>
-      <c r="G276" s="8"/>
+      <c r="G276" s="9"/>
       <c r="H276" s="7"/>
       <c r="I276" s="8"/>
       <c r="J276" s="7"/>
@@ -18416,7 +18461,27 @@
       <c r="U276" s="7"/>
     </row>
     <row r="277" spans="1:21" ht="14.4">
-      <c r="B277" s="7"/>
+      <c r="A277" s="6"/>
+      <c r="B277" s="6"/>
+      <c r="C277" s="7"/>
+      <c r="D277" s="8"/>
+      <c r="E277" s="8"/>
+      <c r="F277" s="10"/>
+      <c r="G277" s="8"/>
+      <c r="H277" s="7"/>
+      <c r="I277" s="8"/>
+      <c r="J277" s="7"/>
+      <c r="K277" s="7"/>
+      <c r="L277" s="7"/>
+      <c r="M277" s="7"/>
+      <c r="N277" s="7"/>
+      <c r="O277" s="7"/>
+      <c r="P277" s="7"/>
+      <c r="Q277" s="7"/>
+      <c r="R277" s="7"/>
+      <c r="S277" s="7"/>
+      <c r="T277" s="7"/>
+      <c r="U277" s="7"/>
     </row>
     <row r="278" spans="1:21" ht="14.4">
       <c r="B278" s="7"/>
@@ -20727,6 +20792,9 @@
     </row>
     <row r="1047" spans="2:2" ht="14.4">
       <c r="B1047" s="7"/>
+    </row>
+    <row r="1048" spans="2:2" ht="14.4">
+      <c r="B1048" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -20739,11 +20807,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Z104"/>
+  <dimension ref="A1:Z107"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K57" sqref="K57"/>
+      <selection pane="bottomLeft" activeCell="K72" sqref="K72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -22085,90 +22153,101 @@
         <v>26</v>
       </c>
     </row>
-    <row r="53" spans="1:11" ht="14.4">
-      <c r="A53" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B53" s="15" t="s">
+    <row r="53" spans="1:11" s="21" customFormat="1" ht="14.4">
+      <c r="A53" s="20"/>
+      <c r="B53" s="20"/>
+      <c r="E53" s="7" t="s">
+        <v>993</v>
+      </c>
+      <c r="F53" s="7"/>
+      <c r="G53" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="H53" s="57" t="s">
+        <v>73</v>
+      </c>
+      <c r="I53" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="J53" s="57" t="s">
+        <v>30</v>
+      </c>
+      <c r="K53" s="57" t="s">
+        <v>994</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" ht="14.4">
+      <c r="A54" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B54" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="E53" s="7" t="s">
+      <c r="E54" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="F53" s="7">
+      <c r="F54" s="7">
         <v>0</v>
       </c>
-      <c r="G53" s="7"/>
-      <c r="H53" s="7"/>
-      <c r="K53" s="17" t="s">
+      <c r="G54" s="7"/>
+      <c r="H54" s="7"/>
+      <c r="K54" s="17" t="s">
         <v>91</v>
-      </c>
-    </row>
-    <row r="54" spans="1:11" s="21" customFormat="1" ht="14.4">
-      <c r="A54" s="20"/>
-      <c r="B54" s="20"/>
-      <c r="E54" s="7" t="s">
-        <v>859</v>
-      </c>
-      <c r="F54" s="7">
-        <v>0.08</v>
-      </c>
-      <c r="G54" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="H54" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="I54" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="J54" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="K54" s="23" t="s">
-        <v>860</v>
       </c>
     </row>
     <row r="55" spans="1:11" s="21" customFormat="1" ht="14.4">
       <c r="A55" s="20"/>
       <c r="B55" s="20"/>
-      <c r="E55" s="58" t="s">
-        <v>840</v>
-      </c>
-      <c r="F55" s="7"/>
+      <c r="E55" s="7" t="s">
+        <v>859</v>
+      </c>
+      <c r="F55" s="7">
+        <v>0.08</v>
+      </c>
       <c r="G55" s="7" t="s">
         <v>109</v>
       </c>
       <c r="H55" s="7" t="s">
-        <v>475</v>
+        <v>73</v>
       </c>
       <c r="I55" s="21" t="s">
-        <v>26</v>
+        <v>34</v>
+      </c>
+      <c r="J55" s="21" t="s">
+        <v>30</v>
       </c>
       <c r="K55" s="23" t="s">
-        <v>841</v>
+        <v>860</v>
       </c>
     </row>
     <row r="56" spans="1:11" s="21" customFormat="1" ht="14.4">
       <c r="A56" s="20"/>
       <c r="B56" s="20"/>
       <c r="E56" s="58" t="s">
-        <v>473</v>
+        <v>997</v>
       </c>
       <c r="F56" s="7"/>
-      <c r="G56" s="7"/>
+      <c r="G56" s="7" t="s">
+        <v>109</v>
+      </c>
       <c r="H56" s="7" t="s">
-        <v>475</v>
+        <v>995</v>
+      </c>
+      <c r="I56" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="J56" s="21" t="s">
+        <v>30</v>
       </c>
       <c r="K56" s="23" t="s">
-        <v>942</v>
+        <v>996</v>
       </c>
     </row>
     <row r="57" spans="1:11" s="21" customFormat="1" ht="14.4">
       <c r="A57" s="20"/>
       <c r="B57" s="20"/>
       <c r="E57" s="58" t="s">
-        <v>988</v>
+        <v>840</v>
       </c>
       <c r="F57" s="7"/>
       <c r="G57" s="7" t="s">
@@ -22180,38 +22259,30 @@
       <c r="I57" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="J57" s="21" t="s">
-        <v>27</v>
-      </c>
       <c r="K57" s="23" t="s">
-        <v>989</v>
+        <v>841</v>
       </c>
     </row>
     <row r="58" spans="1:11" s="21" customFormat="1" ht="14.4">
       <c r="A58" s="20"/>
       <c r="B58" s="20"/>
-      <c r="E58" s="7" t="s">
-        <v>839</v>
+      <c r="E58" s="58" t="s">
+        <v>473</v>
       </c>
       <c r="F58" s="7"/>
-      <c r="G58" s="7" t="s">
-        <v>109</v>
-      </c>
+      <c r="G58" s="7"/>
       <c r="H58" s="7" t="s">
         <v>475</v>
       </c>
-      <c r="I58" s="21" t="s">
-        <v>26</v>
-      </c>
       <c r="K58" s="23" t="s">
-        <v>853</v>
+        <v>942</v>
       </c>
     </row>
     <row r="59" spans="1:11" s="21" customFormat="1" ht="14.4">
       <c r="A59" s="20"/>
       <c r="B59" s="20"/>
-      <c r="E59" s="7" t="s">
-        <v>962</v>
+      <c r="E59" s="58" t="s">
+        <v>988</v>
       </c>
       <c r="F59" s="7"/>
       <c r="G59" s="7" t="s">
@@ -22221,95 +22292,86 @@
         <v>475</v>
       </c>
       <c r="I59" s="21" t="s">
-        <v>34</v>
+        <v>26</v>
+      </c>
+      <c r="J59" s="21" t="s">
+        <v>27</v>
       </c>
       <c r="K59" s="23" t="s">
-        <v>963</v>
-      </c>
-    </row>
-    <row r="60" spans="1:11" ht="14.4">
-      <c r="A60" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="B60" s="24" t="s">
-        <v>24</v>
-      </c>
-      <c r="C60" s="17" t="s">
-        <v>92</v>
-      </c>
-      <c r="D60" s="17" t="s">
-        <v>93</v>
-      </c>
-      <c r="E60" s="18" t="s">
-        <v>94</v>
+        <v>989</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" s="21" customFormat="1" ht="14.4">
+      <c r="A60" s="20"/>
+      <c r="B60" s="20"/>
+      <c r="E60" s="7" t="s">
+        <v>839</v>
       </c>
       <c r="F60" s="7"/>
-      <c r="G60" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="H60" s="18" t="s">
-        <v>95</v>
-      </c>
-      <c r="I60" s="17" t="s">
+      <c r="G60" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="H60" s="7" t="s">
+        <v>475</v>
+      </c>
+      <c r="I60" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="J60" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="K60" s="17" t="s">
-        <v>96</v>
+      <c r="K60" s="23" t="s">
+        <v>853</v>
       </c>
     </row>
     <row r="61" spans="1:11" s="21" customFormat="1" ht="14.4">
       <c r="A61" s="20"/>
-      <c r="B61" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="C61" s="22"/>
-      <c r="D61" s="22"/>
-      <c r="E61" s="21" t="s">
-        <v>916</v>
+      <c r="B61" s="20"/>
+      <c r="E61" s="7" t="s">
+        <v>962</v>
       </c>
       <c r="F61" s="7"/>
-      <c r="G61" s="21" t="s">
+      <c r="G61" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="H61" s="21" t="s">
-        <v>917</v>
-      </c>
-      <c r="I61" s="23" t="s">
+      <c r="H61" s="7" t="s">
+        <v>475</v>
+      </c>
+      <c r="I61" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="K61" s="23" t="s">
+        <v>963</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" ht="14.4">
+      <c r="A62" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B62" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="C62" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="D62" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="E62" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="F62" s="7"/>
+      <c r="G62" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="H62" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="I62" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="J61" s="23" t="s">
+      <c r="J62" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="K61" s="23" t="s">
-        <v>911</v>
-      </c>
-    </row>
-    <row r="62" spans="1:11" s="21" customFormat="1" ht="14.4">
-      <c r="A62" s="20"/>
-      <c r="B62" s="24"/>
-      <c r="C62" s="22"/>
-      <c r="D62" s="22"/>
-      <c r="E62" s="21" t="s">
-        <v>919</v>
-      </c>
-      <c r="F62" s="7"/>
-      <c r="G62" s="21" t="s">
-        <v>109</v>
-      </c>
-      <c r="H62" s="21" t="s">
-        <v>407</v>
-      </c>
-      <c r="I62" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="J62" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="K62" s="23" t="s">
-        <v>920</v>
+      <c r="K62" s="17" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="63" spans="1:11" s="21" customFormat="1" ht="14.4">
@@ -22320,14 +22382,14 @@
       <c r="C63" s="22"/>
       <c r="D63" s="22"/>
       <c r="E63" s="21" t="s">
-        <v>912</v>
+        <v>916</v>
       </c>
       <c r="F63" s="7"/>
       <c r="G63" s="21" t="s">
         <v>109</v>
       </c>
       <c r="H63" s="21" t="s">
-        <v>95</v>
+        <v>917</v>
       </c>
       <c r="I63" s="23" t="s">
         <v>26</v>
@@ -22336,229 +22398,240 @@
         <v>27</v>
       </c>
       <c r="K63" s="23" t="s">
-        <v>913</v>
-      </c>
-    </row>
-    <row r="64" spans="1:11" ht="43.2">
-      <c r="A64" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B64" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="E64" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="F64" s="18">
-        <v>1</v>
-      </c>
-      <c r="G64" s="18" t="s">
-        <v>98</v>
-      </c>
-      <c r="H64" s="18" t="s">
-        <v>99</v>
-      </c>
-      <c r="J64" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="K64" s="19" t="s">
-        <v>100</v>
+        <v>911</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" s="21" customFormat="1" ht="14.4">
+      <c r="A64" s="20"/>
+      <c r="B64" s="24"/>
+      <c r="C64" s="22"/>
+      <c r="D64" s="22"/>
+      <c r="E64" s="21" t="s">
+        <v>919</v>
+      </c>
+      <c r="F64" s="7"/>
+      <c r="G64" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="H64" s="21" t="s">
+        <v>407</v>
+      </c>
+      <c r="I64" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="J64" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="K64" s="23" t="s">
+        <v>920</v>
       </c>
     </row>
     <row r="65" spans="1:26" s="21" customFormat="1" ht="14.4">
       <c r="A65" s="20"/>
-      <c r="B65" s="20"/>
-      <c r="E65" s="7" t="s">
-        <v>921</v>
-      </c>
+      <c r="B65" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="C65" s="22"/>
+      <c r="D65" s="22"/>
+      <c r="E65" s="21" t="s">
+        <v>912</v>
+      </c>
+      <c r="F65" s="7"/>
       <c r="G65" s="21" t="s">
         <v>109</v>
       </c>
       <c r="H65" s="21" t="s">
-        <v>475</v>
+        <v>95</v>
       </c>
       <c r="I65" s="23" t="s">
         <v>26</v>
       </c>
       <c r="J65" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="K65" s="23" t="s">
+        <v>913</v>
+      </c>
+    </row>
+    <row r="66" spans="1:26" ht="43.2">
+      <c r="A66" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B66" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="E66" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="F66" s="18">
+        <v>1</v>
+      </c>
+      <c r="G66" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="H66" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="J66" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="K65" s="23" t="s">
+      <c r="K66" s="19" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="67" spans="1:26" s="21" customFormat="1" ht="14.4">
+      <c r="A67" s="20"/>
+      <c r="B67" s="20"/>
+      <c r="E67" s="7" t="s">
+        <v>921</v>
+      </c>
+      <c r="G67" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="H67" s="21" t="s">
+        <v>475</v>
+      </c>
+      <c r="I67" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="J67" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="K67" s="23" t="s">
         <v>922</v>
       </c>
     </row>
-    <row r="66" spans="1:26" s="25" customFormat="1" ht="86.4">
-      <c r="A66" s="81"/>
-      <c r="B66" s="81"/>
-      <c r="E66" s="25" t="s">
+    <row r="68" spans="1:26" s="25" customFormat="1" ht="86.4">
+      <c r="A68" s="81"/>
+      <c r="B68" s="81"/>
+      <c r="E68" s="25" t="s">
         <v>101</v>
       </c>
-      <c r="F66" s="25">
+      <c r="F68" s="25">
         <v>1</v>
       </c>
-      <c r="G66" s="25" t="s">
+      <c r="G68" s="25" t="s">
         <v>98</v>
       </c>
-      <c r="H66" s="25" t="s">
+      <c r="H68" s="25" t="s">
         <v>99</v>
       </c>
-      <c r="I66" s="19" t="s">
+      <c r="I68" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="J66" s="19" t="s">
+      <c r="J68" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="K66" s="80" t="s">
+      <c r="K68" s="80" t="s">
         <v>933</v>
       </c>
     </row>
-    <row r="67" spans="1:26" s="25" customFormat="1" ht="14.4">
-      <c r="A67" s="81"/>
-      <c r="B67" s="81"/>
-      <c r="E67" s="72" t="s">
+    <row r="69" spans="1:26" s="25" customFormat="1" ht="14.4">
+      <c r="A69" s="81"/>
+      <c r="B69" s="81"/>
+      <c r="E69" s="72" t="s">
         <v>923</v>
       </c>
-      <c r="G67" s="72" t="s">
+      <c r="G69" s="72" t="s">
         <v>109</v>
       </c>
-      <c r="H67" s="72" t="s">
+      <c r="H69" s="72" t="s">
         <v>475</v>
       </c>
-      <c r="I67" s="80" t="s">
+      <c r="I69" s="80" t="s">
         <v>26</v>
       </c>
-      <c r="J67" s="80" t="s">
+      <c r="J69" s="80" t="s">
         <v>27</v>
       </c>
-      <c r="K67" s="23" t="s">
+      <c r="K69" s="23" t="s">
         <v>924</v>
       </c>
     </row>
-    <row r="68" spans="1:26" s="25" customFormat="1" ht="28.8">
-      <c r="A68" s="81"/>
-      <c r="B68" s="81" t="s">
-        <v>23</v>
-      </c>
-      <c r="E68" s="25" t="s">
+    <row r="70" spans="1:26" s="25" customFormat="1" ht="28.8">
+      <c r="A70" s="81"/>
+      <c r="B70" s="81" t="s">
+        <v>23</v>
+      </c>
+      <c r="E70" s="25" t="s">
         <v>914</v>
       </c>
-      <c r="G68" s="25" t="s">
+      <c r="G70" s="25" t="s">
         <v>109</v>
       </c>
-      <c r="H68" s="25" t="s">
+      <c r="H70" s="25" t="s">
         <v>129</v>
       </c>
-      <c r="I68" s="80" t="s">
+      <c r="I70" s="80" t="s">
         <v>26</v>
       </c>
-      <c r="J68" s="19"/>
-      <c r="K68" s="80" t="s">
+      <c r="J70" s="19"/>
+      <c r="K70" s="80" t="s">
         <v>915</v>
       </c>
     </row>
-    <row r="69" spans="1:26" s="21" customFormat="1" ht="14.25" customHeight="1">
-      <c r="C69" s="28"/>
-      <c r="D69" s="28"/>
-      <c r="E69" s="7" t="s">
+    <row r="71" spans="1:26" s="21" customFormat="1" ht="14.25" customHeight="1">
+      <c r="C71" s="28"/>
+      <c r="D71" s="28"/>
+      <c r="E71" s="7" t="s">
         <v>812</v>
       </c>
-      <c r="F69" s="7"/>
-      <c r="G69" s="70" t="s">
+      <c r="F71" s="7"/>
+      <c r="G71" s="70" t="s">
         <v>29</v>
       </c>
-      <c r="H69" s="70" t="s">
+      <c r="H71" s="70" t="s">
         <v>227</v>
       </c>
-      <c r="I69" s="70" t="s">
+      <c r="I71" s="70" t="s">
         <v>34</v>
       </c>
-      <c r="J69" s="70" t="s">
+      <c r="J71" s="70" t="s">
         <v>27</v>
       </c>
-      <c r="K69" s="57" t="s">
+      <c r="K71" s="57" t="s">
         <v>813</v>
       </c>
-      <c r="L69" s="70" t="s">
+      <c r="L71" s="70" t="s">
         <v>814</v>
       </c>
-      <c r="M69" s="3"/>
-      <c r="N69" s="7"/>
-      <c r="O69" s="7"/>
-      <c r="P69" s="7"/>
-      <c r="Q69" s="7"/>
-      <c r="R69" s="7"/>
-      <c r="S69" s="7"/>
-      <c r="T69" s="7"/>
-      <c r="U69" s="7"/>
-      <c r="V69" s="7"/>
-      <c r="W69" s="7"/>
-      <c r="X69" s="7"/>
-    </row>
-    <row r="70" spans="1:26" ht="14.4">
-      <c r="A70" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B70" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="E70" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="F70" s="7">
-        <v>-1</v>
-      </c>
-      <c r="G70" s="7"/>
-      <c r="H70" s="7"/>
-    </row>
-    <row r="71" spans="1:26" s="21" customFormat="1" ht="14.4">
-      <c r="A71" s="20"/>
-      <c r="B71" s="20"/>
-      <c r="E71" s="25" t="s">
-        <v>982</v>
-      </c>
-      <c r="F71" s="7" t="s">
-        <v>983</v>
-      </c>
-      <c r="G71" s="25" t="s">
-        <v>70</v>
-      </c>
-      <c r="H71" s="7"/>
-      <c r="K71" s="21" t="s">
-        <v>984</v>
-      </c>
-    </row>
-    <row r="72" spans="1:26" ht="14.4">
-      <c r="A72" s="15"/>
-      <c r="B72" s="15"/>
-      <c r="C72" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="D72" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="E72" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="F72" s="7">
-        <v>0.6</v>
-      </c>
-      <c r="G72" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="H72" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="I72" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="J72" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="K72" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="L72" s="7"/>
-      <c r="M72" s="7"/>
+      <c r="M71" s="3"/>
+      <c r="N71" s="7"/>
+      <c r="O71" s="7"/>
+      <c r="P71" s="7"/>
+      <c r="Q71" s="7"/>
+      <c r="R71" s="7"/>
+      <c r="S71" s="7"/>
+      <c r="T71" s="7"/>
+      <c r="U71" s="7"/>
+      <c r="V71" s="7"/>
+      <c r="W71" s="7"/>
+      <c r="X71" s="7"/>
+    </row>
+    <row r="72" spans="1:26" s="21" customFormat="1" ht="14.25" customHeight="1">
+      <c r="C72" s="28"/>
+      <c r="D72" s="28"/>
+      <c r="E72" s="25" t="s">
+        <v>998</v>
+      </c>
+      <c r="F72" s="7"/>
+      <c r="G72" s="70" t="s">
+        <v>109</v>
+      </c>
+      <c r="H72" s="70" t="s">
+        <v>999</v>
+      </c>
+      <c r="I72" s="70" t="s">
+        <v>34</v>
+      </c>
+      <c r="J72" s="70" t="s">
+        <v>30</v>
+      </c>
+      <c r="K72" s="70" t="s">
+        <v>1000</v>
+      </c>
+      <c r="L72" s="70"/>
+      <c r="M72" s="3"/>
       <c r="N72" s="7"/>
       <c r="O72" s="7"/>
       <c r="P72" s="7"/>
@@ -22570,102 +22643,119 @@
       <c r="V72" s="7"/>
       <c r="W72" s="7"/>
       <c r="X72" s="7"/>
-      <c r="Y72" s="7"/>
-      <c r="Z72" s="7"/>
     </row>
     <row r="73" spans="1:26" ht="14.4">
       <c r="A73" s="15" t="s">
         <v>23</v>
       </c>
       <c r="B73" s="15" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E73" s="7" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="F73" s="7">
-        <v>1739.927555</v>
+        <v>-1</v>
       </c>
       <c r="G73" s="7"/>
-      <c r="H73" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="K73" s="3" t="s">
-        <v>113</v>
-      </c>
+      <c r="H73" s="7"/>
     </row>
     <row r="74" spans="1:26" s="21" customFormat="1" ht="14.4">
       <c r="A74" s="20"/>
       <c r="B74" s="20"/>
-      <c r="E74" s="7" t="s">
-        <v>959</v>
-      </c>
-      <c r="F74" s="7"/>
-      <c r="G74" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="H74" s="7" t="s">
+      <c r="E74" s="25" t="s">
+        <v>982</v>
+      </c>
+      <c r="F74" s="7" t="s">
+        <v>983</v>
+      </c>
+      <c r="G74" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="H74" s="7"/>
+      <c r="K74" s="21" t="s">
+        <v>984</v>
+      </c>
+    </row>
+    <row r="75" spans="1:26" ht="14.4">
+      <c r="A75" s="15"/>
+      <c r="B75" s="15"/>
+      <c r="C75" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="D75" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="E75" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="F75" s="7">
+        <v>0.6</v>
+      </c>
+      <c r="G75" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H75" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="I75" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="J75" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="K75" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="L75" s="7"/>
+      <c r="M75" s="7"/>
+      <c r="N75" s="7"/>
+      <c r="O75" s="7"/>
+      <c r="P75" s="7"/>
+      <c r="Q75" s="7"/>
+      <c r="R75" s="7"/>
+      <c r="S75" s="7"/>
+      <c r="T75" s="7"/>
+      <c r="U75" s="7"/>
+      <c r="V75" s="7"/>
+      <c r="W75" s="7"/>
+      <c r="X75" s="7"/>
+      <c r="Y75" s="7"/>
+      <c r="Z75" s="7"/>
+    </row>
+    <row r="76" spans="1:26" ht="14.4">
+      <c r="A76" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B76" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="E76" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="F76" s="7">
+        <v>1739.927555</v>
+      </c>
+      <c r="G76" s="7"/>
+      <c r="H76" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="I74" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="J74" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="K74" s="3"/>
-    </row>
-    <row r="75" spans="1:26" s="21" customFormat="1" ht="14.4">
-      <c r="A75" s="20"/>
-      <c r="B75" s="20"/>
-      <c r="E75" s="7" t="s">
-        <v>497</v>
-      </c>
-      <c r="F75" s="7"/>
-      <c r="G75" s="7"/>
-      <c r="H75" s="7"/>
-      <c r="K75" s="3" t="s">
-        <v>941</v>
-      </c>
-    </row>
-    <row r="76" spans="1:26" s="21" customFormat="1" ht="14.4">
-      <c r="A76" s="20"/>
-      <c r="B76" s="20"/>
-      <c r="E76" s="7" t="s">
-        <v>854</v>
-      </c>
-      <c r="F76" s="7"/>
-      <c r="G76" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="H76" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="I76" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="J76" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="K76" s="21" t="s">
-        <v>856</v>
-      </c>
-      <c r="L76" s="3" t="s">
-        <v>855</v>
+      <c r="K76" s="3" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="77" spans="1:26" s="21" customFormat="1" ht="14.4">
       <c r="A77" s="20"/>
       <c r="B77" s="20"/>
       <c r="E77" s="7" t="s">
-        <v>918</v>
+        <v>959</v>
       </c>
       <c r="F77" s="7"/>
       <c r="G77" s="7" t="s">
-        <v>29</v>
+        <v>109</v>
       </c>
       <c r="H77" s="7" t="s">
-        <v>129</v>
+        <v>84</v>
       </c>
       <c r="I77" s="21" t="s">
         <v>34</v>
@@ -22673,76 +22763,72 @@
       <c r="J77" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="K77" s="21" t="s">
+      <c r="K77" s="3"/>
+    </row>
+    <row r="78" spans="1:26" s="21" customFormat="1" ht="14.4">
+      <c r="A78" s="20"/>
+      <c r="B78" s="20"/>
+      <c r="E78" s="7" t="s">
+        <v>497</v>
+      </c>
+      <c r="F78" s="7"/>
+      <c r="G78" s="7"/>
+      <c r="H78" s="7"/>
+      <c r="K78" s="3" t="s">
+        <v>941</v>
+      </c>
+    </row>
+    <row r="79" spans="1:26" s="21" customFormat="1" ht="14.4">
+      <c r="A79" s="20"/>
+      <c r="B79" s="20"/>
+      <c r="E79" s="7" t="s">
+        <v>854</v>
+      </c>
+      <c r="F79" s="7"/>
+      <c r="G79" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H79" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="I79" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="J79" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="K79" s="21" t="s">
+        <v>856</v>
+      </c>
+      <c r="L79" s="3" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="80" spans="1:26" s="21" customFormat="1" ht="14.4">
+      <c r="A80" s="20"/>
+      <c r="B80" s="20"/>
+      <c r="E80" s="7" t="s">
+        <v>918</v>
+      </c>
+      <c r="F80" s="7"/>
+      <c r="G80" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H80" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="I80" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="J80" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="K80" s="21" t="s">
         <v>903</v>
       </c>
-      <c r="L77" s="3" t="s">
+      <c r="L80" s="3" t="s">
         <v>855</v>
       </c>
-    </row>
-    <row r="78" spans="1:26" ht="14.4">
-      <c r="A78" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B78" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="C78" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E78" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="F78" s="7">
-        <v>1</v>
-      </c>
-      <c r="G78" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="H78" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="I78" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="J78" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="K78" s="3" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="79" spans="1:26" ht="14.4">
-      <c r="A79" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B79" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="E79" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="F79" s="7">
-        <v>553659</v>
-      </c>
-      <c r="G79" s="7"/>
-      <c r="H79" s="7"/>
-    </row>
-    <row r="80" spans="1:26" ht="14.4">
-      <c r="A80" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B80" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="E80" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="F80" s="7">
-        <v>4891208</v>
-      </c>
-      <c r="G80" s="7"/>
-      <c r="H80" s="7"/>
     </row>
     <row r="81" spans="1:12" ht="14.4">
       <c r="A81" s="15" t="s">
@@ -22755,7 +22841,7 @@
         <v>24</v>
       </c>
       <c r="E81" s="7" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="F81" s="7">
         <v>1</v>
@@ -22764,7 +22850,7 @@
         <v>46</v>
       </c>
       <c r="H81" s="7" t="s">
-        <v>33</v>
+        <v>116</v>
       </c>
       <c r="I81" s="3" t="s">
         <v>34</v>
@@ -22773,66 +22859,40 @@
         <v>30</v>
       </c>
       <c r="K81" s="3" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="82" spans="1:12" s="21" customFormat="1" ht="14.4">
-      <c r="A82" s="20"/>
-      <c r="B82" s="20"/>
-      <c r="C82" s="3"/>
+        <v>117</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12" ht="14.4">
+      <c r="A82" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B82" s="15" t="s">
+        <v>24</v>
+      </c>
       <c r="E82" s="7" t="s">
-        <v>934</v>
-      </c>
-      <c r="F82" s="7"/>
+        <v>118</v>
+      </c>
+      <c r="F82" s="7">
+        <v>553659</v>
+      </c>
       <c r="G82" s="7"/>
-      <c r="H82" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="I82" s="3"/>
-      <c r="J82" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="K82" s="3" t="s">
-        <v>936</v>
-      </c>
-    </row>
-    <row r="83" spans="1:12" s="21" customFormat="1" ht="14.4">
-      <c r="A83" s="20" t="s">
-        <v>837</v>
-      </c>
-      <c r="B83" s="20" t="s">
+      <c r="H82" s="7"/>
+    </row>
+    <row r="83" spans="1:12" ht="14.4">
+      <c r="A83" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B83" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="C83" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="D83" s="21" t="s">
-        <v>65</v>
-      </c>
       <c r="E83" s="7" t="s">
-        <v>836</v>
+        <v>119</v>
       </c>
       <c r="F83" s="7">
-        <v>5</v>
-      </c>
-      <c r="G83" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="H83" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="I83" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="J83" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="K83" s="3" t="s">
-        <v>838</v>
-      </c>
-      <c r="L83" s="23" t="s">
-        <v>65</v>
-      </c>
+        <v>4891208</v>
+      </c>
+      <c r="G83" s="7"/>
+      <c r="H83" s="7"/>
     </row>
     <row r="84" spans="1:12" ht="14.4">
       <c r="A84" s="15" t="s">
@@ -22841,35 +22901,37 @@
       <c r="B84" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="D84" s="3" t="s">
-        <v>127</v>
+      <c r="C84" s="3" t="s">
+        <v>24</v>
       </c>
       <c r="E84" s="7" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="F84" s="7">
-        <v>0</v>
-      </c>
-      <c r="G84" s="7"/>
+        <v>1</v>
+      </c>
+      <c r="G84" s="7" t="s">
+        <v>46</v>
+      </c>
       <c r="H84" s="7" t="s">
-        <v>129</v>
+        <v>33</v>
       </c>
       <c r="I84" s="3" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="J84" s="3" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="K84" s="3" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
     </row>
     <row r="85" spans="1:12" s="21" customFormat="1" ht="14.4">
       <c r="A85" s="20"/>
       <c r="B85" s="20"/>
-      <c r="D85" s="3"/>
+      <c r="C85" s="3"/>
       <c r="E85" s="7" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="F85" s="7"/>
       <c r="G85" s="7"/>
@@ -22877,263 +22939,279 @@
         <v>129</v>
       </c>
       <c r="I85" s="3"/>
-      <c r="J85" s="3"/>
+      <c r="J85" s="3" t="s">
+        <v>27</v>
+      </c>
       <c r="K85" s="3" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
     </row>
     <row r="86" spans="1:12" s="21" customFormat="1" ht="14.4">
-      <c r="A86" s="20"/>
-      <c r="B86" s="20"/>
-      <c r="D86" s="3"/>
+      <c r="A86" s="20" t="s">
+        <v>837</v>
+      </c>
+      <c r="B86" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="C86" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D86" s="21" t="s">
+        <v>65</v>
+      </c>
       <c r="E86" s="7" t="s">
-        <v>938</v>
-      </c>
-      <c r="F86" s="7"/>
-      <c r="G86" s="7"/>
+        <v>836</v>
+      </c>
+      <c r="F86" s="7">
+        <v>5</v>
+      </c>
+      <c r="G86" s="7" t="s">
+        <v>109</v>
+      </c>
       <c r="H86" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="I86" s="3"/>
-      <c r="J86" s="3"/>
+      <c r="I86" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J86" s="3" t="s">
+        <v>27</v>
+      </c>
       <c r="K86" s="3" t="s">
-        <v>939</v>
+        <v>838</v>
+      </c>
+      <c r="L86" s="23" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="87" spans="1:12" ht="14.4">
       <c r="A87" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="B87" s="15"/>
+      <c r="B87" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D87" s="3" t="s">
+        <v>127</v>
+      </c>
       <c r="E87" s="7" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="F87" s="7">
-        <v>6772</v>
+        <v>0</v>
       </c>
       <c r="G87" s="7"/>
-      <c r="H87" s="7"/>
+      <c r="H87" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="I87" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J87" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K87" s="3" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="88" spans="1:12" s="21" customFormat="1" ht="14.4">
       <c r="A88" s="20"/>
       <c r="B88" s="20"/>
+      <c r="D88" s="3"/>
       <c r="E88" s="7" t="s">
-        <v>952</v>
-      </c>
-      <c r="F88" s="7">
-        <v>5</v>
-      </c>
-      <c r="G88" s="58" t="s">
-        <v>109</v>
-      </c>
+        <v>935</v>
+      </c>
+      <c r="F88" s="7"/>
+      <c r="G88" s="7"/>
       <c r="H88" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="I88" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="J88" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="K88" s="23" t="s">
-        <v>953</v>
+      <c r="I88" s="3"/>
+      <c r="J88" s="3"/>
+      <c r="K88" s="3" t="s">
+        <v>937</v>
       </c>
     </row>
     <row r="89" spans="1:12" s="21" customFormat="1" ht="14.4">
       <c r="A89" s="20"/>
       <c r="B89" s="20"/>
-      <c r="E89" s="58" t="s">
-        <v>954</v>
-      </c>
-      <c r="F89" s="7">
-        <v>5</v>
-      </c>
-      <c r="G89" s="58" t="s">
-        <v>109</v>
-      </c>
+      <c r="D89" s="3"/>
+      <c r="E89" s="7" t="s">
+        <v>938</v>
+      </c>
+      <c r="F89" s="7"/>
+      <c r="G89" s="7"/>
       <c r="H89" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="I89" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="J89" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="K89" s="23" t="s">
-        <v>955</v>
-      </c>
-    </row>
-    <row r="90" spans="1:12" s="21" customFormat="1" ht="14.4">
-      <c r="A90" s="20"/>
-      <c r="B90" s="20"/>
-      <c r="E90" s="58" t="s">
-        <v>956</v>
+      <c r="I89" s="3"/>
+      <c r="J89" s="3"/>
+      <c r="K89" s="3" t="s">
+        <v>939</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12" ht="14.4">
+      <c r="A90" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B90" s="15"/>
+      <c r="E90" s="7" t="s">
+        <v>131</v>
       </c>
       <c r="F90" s="7">
-        <v>5</v>
-      </c>
-      <c r="G90" s="58" t="s">
-        <v>109</v>
-      </c>
-      <c r="H90" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="I90" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="J90" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="K90" s="23" t="s">
-        <v>957</v>
-      </c>
+        <v>6772</v>
+      </c>
+      <c r="G90" s="7"/>
+      <c r="H90" s="7"/>
     </row>
     <row r="91" spans="1:12" s="21" customFormat="1" ht="14.4">
       <c r="A91" s="20"/>
       <c r="B91" s="20"/>
       <c r="E91" s="7" t="s">
-        <v>843</v>
+        <v>952</v>
       </c>
       <c r="F91" s="7">
-        <v>1</v>
-      </c>
-      <c r="G91" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G91" s="58" t="s">
         <v>109</v>
       </c>
       <c r="H91" s="7" t="s">
-        <v>844</v>
-      </c>
-      <c r="I91" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="J91" s="23" t="s">
-        <v>845</v>
+        <v>129</v>
+      </c>
+      <c r="I91" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="J91" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="K91" s="23" t="s">
+        <v>953</v>
       </c>
     </row>
     <row r="92" spans="1:12" s="21" customFormat="1" ht="14.4">
       <c r="A92" s="20"/>
       <c r="B92" s="20"/>
-      <c r="E92" s="7" t="s">
-        <v>978</v>
-      </c>
-      <c r="F92" s="7"/>
-      <c r="G92" s="7" t="s">
+      <c r="E92" s="58" t="s">
+        <v>954</v>
+      </c>
+      <c r="F92" s="7">
+        <v>5</v>
+      </c>
+      <c r="G92" s="58" t="s">
         <v>109</v>
       </c>
       <c r="H92" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="I92" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="J92" s="23" t="s">
-        <v>27</v>
+        <v>129</v>
+      </c>
+      <c r="I92" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="J92" s="21" t="s">
+        <v>30</v>
       </c>
       <c r="K92" s="23" t="s">
-        <v>979</v>
-      </c>
-      <c r="L92" s="23" t="s">
-        <v>977</v>
+        <v>955</v>
       </c>
     </row>
     <row r="93" spans="1:12" s="21" customFormat="1" ht="14.4">
       <c r="A93" s="20"/>
       <c r="B93" s="20"/>
-      <c r="E93" s="7" t="s">
-        <v>950</v>
-      </c>
-      <c r="F93" s="7"/>
-      <c r="G93" s="7" t="s">
+      <c r="E93" s="58" t="s">
+        <v>956</v>
+      </c>
+      <c r="F93" s="7">
+        <v>5</v>
+      </c>
+      <c r="G93" s="58" t="s">
         <v>109</v>
       </c>
       <c r="H93" s="7" t="s">
-        <v>626</v>
-      </c>
-      <c r="I93" s="23"/>
-      <c r="J93" s="23"/>
+        <v>129</v>
+      </c>
+      <c r="I93" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="J93" s="21" t="s">
+        <v>30</v>
+      </c>
       <c r="K93" s="23" t="s">
-        <v>980</v>
-      </c>
-      <c r="L93" s="23"/>
+        <v>957</v>
+      </c>
     </row>
     <row r="94" spans="1:12" s="21" customFormat="1" ht="14.4">
       <c r="A94" s="20"/>
       <c r="B94" s="20"/>
       <c r="E94" s="7" t="s">
-        <v>951</v>
-      </c>
-      <c r="F94" s="7"/>
+        <v>843</v>
+      </c>
+      <c r="F94" s="7">
+        <v>1</v>
+      </c>
       <c r="G94" s="7" t="s">
         <v>109</v>
       </c>
       <c r="H94" s="7" t="s">
-        <v>626</v>
-      </c>
-      <c r="I94" s="23"/>
-      <c r="J94" s="23"/>
-      <c r="K94" s="23" t="s">
-        <v>981</v>
-      </c>
-      <c r="L94" s="23"/>
+        <v>844</v>
+      </c>
+      <c r="I94" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="J94" s="23" t="s">
+        <v>845</v>
+      </c>
     </row>
     <row r="95" spans="1:12" s="21" customFormat="1" ht="14.4">
       <c r="A95" s="20"/>
       <c r="B95" s="20"/>
-      <c r="D95" s="57" t="s">
-        <v>944</v>
-      </c>
       <c r="E95" s="7" t="s">
-        <v>970</v>
+        <v>978</v>
       </c>
       <c r="F95" s="7"/>
-      <c r="G95" s="58" t="s">
+      <c r="G95" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="H95" s="58" t="s">
-        <v>84</v>
+      <c r="H95" s="7" t="s">
+        <v>63</v>
       </c>
       <c r="I95" s="23" t="s">
-        <v>947</v>
+        <v>26</v>
       </c>
       <c r="J95" s="23" t="s">
-        <v>947</v>
+        <v>27</v>
       </c>
       <c r="K95" s="23" t="s">
-        <v>971</v>
-      </c>
-      <c r="L95" s="23"/>
+        <v>979</v>
+      </c>
+      <c r="L95" s="23" t="s">
+        <v>977</v>
+      </c>
     </row>
     <row r="96" spans="1:12" s="21" customFormat="1" ht="14.4">
       <c r="A96" s="20"/>
       <c r="B96" s="20"/>
       <c r="E96" s="7" t="s">
-        <v>842</v>
-      </c>
-      <c r="F96" s="7">
-        <v>10</v>
-      </c>
+        <v>950</v>
+      </c>
+      <c r="F96" s="7"/>
       <c r="G96" s="7" t="s">
         <v>109</v>
       </c>
       <c r="H96" s="7" t="s">
         <v>626</v>
       </c>
-      <c r="I96" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="J96" s="23" t="s">
-        <v>27</v>
-      </c>
+      <c r="I96" s="23"/>
+      <c r="J96" s="23"/>
       <c r="K96" s="23" t="s">
-        <v>848</v>
-      </c>
+        <v>980</v>
+      </c>
+      <c r="L96" s="23"/>
     </row>
     <row r="97" spans="1:12" s="21" customFormat="1" ht="14.4">
       <c r="A97" s="20"/>
       <c r="B97" s="20"/>
       <c r="E97" s="7" t="s">
-        <v>960</v>
+        <v>951</v>
       </c>
       <c r="F97" s="7"/>
       <c r="G97" s="7" t="s">
@@ -23142,211 +23220,283 @@
       <c r="H97" s="7" t="s">
         <v>626</v>
       </c>
-      <c r="I97" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="J97" s="23" t="s">
-        <v>30</v>
-      </c>
+      <c r="I97" s="23"/>
+      <c r="J97" s="23"/>
       <c r="K97" s="23" t="s">
-        <v>961</v>
-      </c>
+        <v>981</v>
+      </c>
+      <c r="L97" s="23"/>
     </row>
     <row r="98" spans="1:12" s="21" customFormat="1" ht="14.4">
       <c r="A98" s="20"/>
       <c r="B98" s="20"/>
+      <c r="D98" s="57" t="s">
+        <v>944</v>
+      </c>
       <c r="E98" s="7" t="s">
-        <v>974</v>
+        <v>970</v>
       </c>
       <c r="F98" s="7"/>
-      <c r="G98" s="7" t="s">
+      <c r="G98" s="58" t="s">
         <v>109</v>
       </c>
-      <c r="H98" s="7" t="s">
-        <v>626</v>
-      </c>
-      <c r="I98" s="23"/>
+      <c r="H98" s="58" t="s">
+        <v>84</v>
+      </c>
+      <c r="I98" s="23" t="s">
+        <v>947</v>
+      </c>
       <c r="J98" s="23" t="s">
-        <v>27</v>
+        <v>947</v>
       </c>
       <c r="K98" s="23" t="s">
-        <v>975</v>
-      </c>
-      <c r="L98" s="23" t="s">
-        <v>976</v>
-      </c>
+        <v>971</v>
+      </c>
+      <c r="L98" s="23"/>
     </row>
     <row r="99" spans="1:12" s="21" customFormat="1" ht="14.4">
       <c r="A99" s="20"/>
       <c r="B99" s="20"/>
       <c r="E99" s="7" t="s">
-        <v>510</v>
-      </c>
-      <c r="F99" s="7"/>
-      <c r="G99" s="7"/>
+        <v>842</v>
+      </c>
+      <c r="F99" s="7">
+        <v>10</v>
+      </c>
+      <c r="G99" s="7" t="s">
+        <v>109</v>
+      </c>
       <c r="H99" s="7" t="s">
-        <v>511</v>
-      </c>
-      <c r="I99" s="23"/>
-      <c r="J99" s="23"/>
+        <v>626</v>
+      </c>
+      <c r="I99" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="J99" s="23" t="s">
+        <v>27</v>
+      </c>
       <c r="K99" s="23" t="s">
-        <v>943</v>
+        <v>848</v>
       </c>
     </row>
     <row r="100" spans="1:12" s="21" customFormat="1" ht="14.4">
       <c r="A100" s="20"/>
       <c r="B100" s="20"/>
-      <c r="D100" s="57" t="s">
-        <v>25</v>
-      </c>
       <c r="E100" s="7" t="s">
-        <v>796</v>
+        <v>960</v>
       </c>
       <c r="F100" s="7"/>
-      <c r="G100" s="58" t="s">
-        <v>29</v>
+      <c r="G100" s="7" t="s">
+        <v>109</v>
       </c>
       <c r="H100" s="7" t="s">
-        <v>73</v>
+        <v>626</v>
       </c>
       <c r="I100" s="23" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="J100" s="23" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="K100" s="23" t="s">
-        <v>797</v>
+        <v>961</v>
       </c>
     </row>
     <row r="101" spans="1:12" s="21" customFormat="1" ht="14.4">
-      <c r="A101" s="20" t="s">
-        <v>23</v>
-      </c>
+      <c r="A101" s="20"/>
       <c r="B101" s="20"/>
-      <c r="D101" s="57" t="s">
-        <v>25</v>
-      </c>
       <c r="E101" s="7" t="s">
-        <v>798</v>
+        <v>974</v>
       </c>
       <c r="F101" s="7"/>
-      <c r="G101" s="58" t="s">
-        <v>29</v>
+      <c r="G101" s="7" t="s">
+        <v>109</v>
       </c>
       <c r="H101" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="I101" s="23" t="s">
-        <v>26</v>
-      </c>
+        <v>626</v>
+      </c>
+      <c r="I101" s="23"/>
       <c r="J101" s="23" t="s">
         <v>27</v>
       </c>
       <c r="K101" s="23" t="s">
+        <v>975</v>
+      </c>
+      <c r="L101" s="23" t="s">
+        <v>976</v>
+      </c>
+    </row>
+    <row r="102" spans="1:12" s="21" customFormat="1" ht="14.4">
+      <c r="A102" s="20"/>
+      <c r="B102" s="20"/>
+      <c r="E102" s="7" t="s">
+        <v>510</v>
+      </c>
+      <c r="F102" s="7"/>
+      <c r="G102" s="7"/>
+      <c r="H102" s="7" t="s">
+        <v>511</v>
+      </c>
+      <c r="I102" s="23"/>
+      <c r="J102" s="23"/>
+      <c r="K102" s="23" t="s">
+        <v>943</v>
+      </c>
+    </row>
+    <row r="103" spans="1:12" s="21" customFormat="1" ht="14.4">
+      <c r="A103" s="20"/>
+      <c r="B103" s="20"/>
+      <c r="D103" s="57" t="s">
+        <v>25</v>
+      </c>
+      <c r="E103" s="7" t="s">
+        <v>796</v>
+      </c>
+      <c r="F103" s="7"/>
+      <c r="G103" s="58" t="s">
+        <v>29</v>
+      </c>
+      <c r="H103" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="I103" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="J103" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="K103" s="23" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="104" spans="1:12" s="21" customFormat="1" ht="14.4">
+      <c r="A104" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="B104" s="20"/>
+      <c r="D104" s="57" t="s">
+        <v>25</v>
+      </c>
+      <c r="E104" s="7" t="s">
+        <v>798</v>
+      </c>
+      <c r="F104" s="7"/>
+      <c r="G104" s="58" t="s">
+        <v>29</v>
+      </c>
+      <c r="H104" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="I104" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="J104" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="K104" s="23" t="s">
         <v>799</v>
       </c>
     </row>
-    <row r="102" spans="1:12" ht="14.4">
-      <c r="A102" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B102" s="16" t="s">
+    <row r="105" spans="1:12" ht="14.4">
+      <c r="A105" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B105" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="D102" s="17" t="s">
+      <c r="D105" s="17" t="s">
         <v>133</v>
       </c>
-      <c r="E102" s="18" t="s">
+      <c r="E105" s="18" t="s">
         <v>135</v>
       </c>
-      <c r="F102" s="18">
+      <c r="F105" s="18">
         <v>1500</v>
       </c>
-      <c r="G102" s="18" t="s">
+      <c r="G105" s="18" t="s">
         <v>109</v>
       </c>
-      <c r="H102" s="18" t="s">
+      <c r="H105" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="I102" s="17" t="s">
+      <c r="I105" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="J102" s="17" t="s">
+      <c r="J105" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="K102" s="17" t="s">
+      <c r="K105" s="17" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="103" spans="1:12" ht="14.4">
-      <c r="A103" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B103" s="16" t="s">
+    <row r="106" spans="1:12" ht="14.4">
+      <c r="A106" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B106" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="D103" s="17" t="s">
+      <c r="D106" s="17" t="s">
         <v>133</v>
       </c>
-      <c r="E103" s="17" t="s">
+      <c r="E106" s="17" t="s">
         <v>140</v>
       </c>
-      <c r="F103" s="17">
+      <c r="F106" s="17">
         <v>1500</v>
       </c>
-      <c r="G103" s="18" t="s">
+      <c r="G106" s="18" t="s">
         <v>109</v>
       </c>
-      <c r="H103" s="17" t="s">
+      <c r="H106" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="I103" s="17" t="s">
+      <c r="I106" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="J103" s="17" t="s">
+      <c r="J106" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="K103" s="17" t="s">
+      <c r="K106" s="17" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="104" spans="1:12" ht="14.4">
-      <c r="A104" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B104" s="16" t="s">
+    <row r="107" spans="1:12" ht="14.4">
+      <c r="A107" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B107" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="D104" s="17" t="s">
+      <c r="D107" s="17" t="s">
         <v>133</v>
       </c>
-      <c r="E104" s="17" t="s">
+      <c r="E107" s="17" t="s">
         <v>143</v>
       </c>
-      <c r="F104" s="17">
+      <c r="F107" s="17">
         <v>1500</v>
       </c>
-      <c r="G104" s="18" t="s">
+      <c r="G107" s="18" t="s">
         <v>109</v>
       </c>
-      <c r="H104" s="17" t="s">
+      <c r="H107" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="I104" s="17" t="s">
+      <c r="I107" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="J104" s="17" t="s">
+      <c r="J107" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="K104" s="17" t="s">
+      <c r="K107" s="17" t="s">
         <v>144</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B60:B63">
+  <conditionalFormatting sqref="B62:B65">
     <cfRule type="notContainsBlanks" dxfId="0" priority="1">
-      <formula>LEN(TRIM(B60))&gt;0</formula>
+      <formula>LEN(TRIM(B62))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Continue adding code for wetland model. EvapTrans.cpp - Recognize GM_WETLAND_ET method for calculating ET. Flow.h - #define WETL_CAP. HBV.cpp - Rewrite the logic for calculating WETL2Q from wetland IDUs in HRUs with standing water. Add the flux from standing water back to the stream.
</commit_message>
<xml_diff>
--- a/DataCW3M/CW3MdigitalHandbook/CW3MdataDictionary.xlsx
+++ b/DataCW3M/CW3MdigitalHandbook/CW3MdataDictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\CW3MdigitalHandbook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E562E4D1-141B-43CC-9EF5-BAC70937C645}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E40CC19-E537-49D1-A0F0-94A34DA5B9F1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-7425" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-7425" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Necessary input data" sheetId="7" r:id="rId1"/>
@@ -97,7 +97,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2996" uniqueCount="1009">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2996" uniqueCount="1007">
   <si>
     <t>LULC_A</t>
   </si>
@@ -2587,9 +2587,6 @@
     <t>WETL_CAP</t>
   </si>
   <si>
-    <t>constant?</t>
-  </si>
-  <si>
     <t>storage capacity of wetland</t>
   </si>
   <si>
@@ -3071,9 +3068,6 @@
   </si>
   <si>
     <t>&gt;0 =&gt; depth of inundation; &lt;0 =&gt; depth of water required to reach saturation</t>
-  </si>
-  <si>
-    <t>m3 H2O or maybe mm H2O</t>
   </si>
   <si>
     <t>Q_CAP</t>
@@ -9089,9 +9083,9 @@
   </sheetPr>
   <dimension ref="A1:Z1048"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A189" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E224" sqref="E224"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A196" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G225" sqref="G225"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -13315,18 +13309,18 @@
       <c r="A123" s="28"/>
       <c r="B123" s="28"/>
       <c r="C123" s="7" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="D123" s="10"/>
       <c r="E123" s="10" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="F123" s="10" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="G123" s="10"/>
       <c r="H123" s="25" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="I123" s="27" t="s">
         <v>113</v>
@@ -13348,18 +13342,18 @@
       <c r="A124" s="28"/>
       <c r="B124" s="28"/>
       <c r="C124" s="7" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="D124" s="10"/>
       <c r="E124" s="10" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="F124" s="10" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="G124" s="10"/>
       <c r="H124" s="25" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="I124" s="27" t="s">
         <v>113</v>
@@ -13381,18 +13375,18 @@
       <c r="A125" s="28"/>
       <c r="B125" s="28"/>
       <c r="C125" s="7" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="D125" s="10"/>
       <c r="E125" s="10" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="F125" s="10" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="G125" s="10"/>
       <c r="H125" s="25" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="I125" s="27" t="s">
         <v>113</v>
@@ -13414,18 +13408,18 @@
       <c r="A126" s="28"/>
       <c r="B126" s="28"/>
       <c r="C126" s="7" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="D126" s="10"/>
       <c r="E126" s="10" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="F126" s="10" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="G126" s="10"/>
       <c r="H126" s="25" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="I126" s="27" t="s">
         <v>113</v>
@@ -13485,22 +13479,22 @@
     <row r="128" spans="1:21" s="21" customFormat="1" ht="14.25" customHeight="1">
       <c r="B128" s="28"/>
       <c r="C128" s="21" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="D128" s="10" t="s">
         <v>29</v>
       </c>
       <c r="E128" s="10" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="F128" s="10" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="G128" s="10" t="s">
         <v>27</v>
       </c>
       <c r="H128" s="21" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="I128" s="27" t="s">
         <v>113</v>
@@ -13510,22 +13504,22 @@
     <row r="129" spans="1:26" s="21" customFormat="1" ht="14.25" customHeight="1">
       <c r="B129" s="28"/>
       <c r="C129" s="21" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="D129" s="10" t="s">
         <v>29</v>
       </c>
       <c r="E129" s="10" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="F129" s="10" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="G129" s="10" t="s">
         <v>27</v>
       </c>
       <c r="H129" s="21" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="I129" s="27" t="s">
         <v>113</v>
@@ -13535,22 +13529,22 @@
     <row r="130" spans="1:26" s="21" customFormat="1" ht="14.25" customHeight="1">
       <c r="B130" s="28"/>
       <c r="C130" s="21" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="D130" s="10" t="s">
         <v>29</v>
       </c>
       <c r="E130" s="10" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="F130" s="10" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="G130" s="10" t="s">
         <v>27</v>
       </c>
       <c r="H130" s="21" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="I130" s="27" t="s">
         <v>113</v>
@@ -13560,22 +13554,22 @@
     <row r="131" spans="1:26" s="21" customFormat="1" ht="14.25" customHeight="1">
       <c r="B131" s="28"/>
       <c r="C131" s="21" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="D131" s="10" t="s">
         <v>29</v>
       </c>
       <c r="E131" s="10" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="F131" s="10" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="G131" s="10" t="s">
         <v>27</v>
       </c>
       <c r="H131" s="21" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="I131" s="27" t="s">
         <v>113</v>
@@ -13586,18 +13580,18 @@
       <c r="A132" s="10"/>
       <c r="B132" s="28"/>
       <c r="C132" s="21" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="D132" s="10"/>
       <c r="E132" s="10" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="F132" s="10" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="G132" s="10"/>
       <c r="H132" s="21" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="I132" s="27" t="s">
         <v>113</v>
@@ -13608,18 +13602,18 @@
       <c r="A133" s="10"/>
       <c r="B133" s="28"/>
       <c r="C133" s="21" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="D133" s="10"/>
       <c r="E133" s="10" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="F133" s="10" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="G133" s="10"/>
       <c r="H133" s="21" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="I133" s="27" t="s">
         <v>113</v>
@@ -13704,7 +13698,7 @@
       </c>
       <c r="D136" s="8"/>
       <c r="E136" s="10" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="F136" s="10"/>
       <c r="G136" s="8" t="s">
@@ -13774,7 +13768,7 @@
       </c>
       <c r="D138" s="8"/>
       <c r="E138" s="10" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="F138" s="10"/>
       <c r="G138" s="8" t="s">
@@ -15938,7 +15932,7 @@
       <c r="A199" s="28"/>
       <c r="B199" s="28"/>
       <c r="C199" s="21" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="D199" s="10" t="s">
         <v>29</v>
@@ -15947,11 +15941,11 @@
         <v>128</v>
       </c>
       <c r="F199" s="10" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="G199" s="10"/>
       <c r="H199" s="25" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="I199" s="27"/>
       <c r="J199" s="3"/>
@@ -15969,7 +15963,7 @@
     <row r="200" spans="1:21" s="21" customFormat="1" ht="14.25" customHeight="1">
       <c r="B200" s="28"/>
       <c r="C200" s="21" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="D200" s="10" t="s">
         <v>29</v>
@@ -15978,13 +15972,13 @@
         <v>128</v>
       </c>
       <c r="F200" s="10" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="G200" s="10" t="s">
         <v>27</v>
       </c>
       <c r="H200" s="25" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="I200" s="27" t="s">
         <v>113</v>
@@ -16786,17 +16780,17 @@
         <v>828</v>
       </c>
       <c r="D224" s="10" t="s">
-        <v>29</v>
+        <v>108</v>
       </c>
       <c r="E224" s="70" t="s">
-        <v>991</v>
+        <v>406</v>
       </c>
       <c r="F224" s="10"/>
       <c r="G224" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H224" s="25" t="s">
         <v>829</v>
-      </c>
-      <c r="H224" s="25" t="s">
-        <v>830</v>
       </c>
       <c r="I224" s="27" t="s">
         <v>529</v>
@@ -16818,7 +16812,7 @@
       <c r="A225" s="66"/>
       <c r="B225" s="66"/>
       <c r="C225" s="64" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="D225" s="62" t="s">
         <v>29</v>
@@ -16833,10 +16827,10 @@
         <v>27</v>
       </c>
       <c r="H225" s="61" t="s">
+        <v>831</v>
+      </c>
+      <c r="I225" s="74" t="s">
         <v>832</v>
-      </c>
-      <c r="I225" s="74" t="s">
-        <v>833</v>
       </c>
       <c r="J225" s="68"/>
       <c r="K225" s="64"/>
@@ -16855,7 +16849,7 @@
       <c r="A226" s="96"/>
       <c r="B226" s="96"/>
       <c r="C226" s="97" t="s">
-        <v>1002</v>
+        <v>1000</v>
       </c>
       <c r="D226" s="100" t="s">
         <v>108</v>
@@ -16868,7 +16862,7 @@
         <v>27</v>
       </c>
       <c r="H226" s="91" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="I226" s="98"/>
       <c r="J226" s="84"/>
@@ -16888,7 +16882,7 @@
       <c r="A227" s="96"/>
       <c r="B227" s="96"/>
       <c r="C227" s="97" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
       <c r="D227" s="99" t="s">
         <v>108</v>
@@ -16903,7 +16897,7 @@
         <v>27</v>
       </c>
       <c r="H227" s="77" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
       <c r="I227" s="98"/>
       <c r="J227" s="84"/>
@@ -20832,9 +20826,9 @@
   </sheetPr>
   <dimension ref="A1:Z109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K46" sqref="K46"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A85" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E66" sqref="E66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -20881,7 +20875,7 @@
     </row>
     <row r="2" spans="1:26" s="57" customFormat="1" ht="14.25" customHeight="1">
       <c r="A2" s="70" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
       <c r="B2" s="69"/>
       <c r="C2" s="69"/>
@@ -20909,7 +20903,7 @@
     </row>
     <row r="3" spans="1:26" s="91" customFormat="1" ht="12.75" customHeight="1">
       <c r="A3" s="87" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="B3" s="88"/>
       <c r="C3" s="89"/>
@@ -20997,7 +20991,7 @@
       <c r="C5" s="13"/>
       <c r="D5" s="13"/>
       <c r="E5" s="72" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="F5" s="10"/>
       <c r="G5" s="70" t="s">
@@ -21013,7 +21007,7 @@
         <v>27</v>
       </c>
       <c r="K5" s="57" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="L5" s="9"/>
       <c r="M5" s="25"/>
@@ -21035,7 +21029,7 @@
       <c r="C6" s="13"/>
       <c r="D6" s="13"/>
       <c r="E6" s="72" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="F6" s="10"/>
       <c r="G6" s="70" t="s">
@@ -21051,7 +21045,7 @@
         <v>27</v>
       </c>
       <c r="K6" s="57" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="L6" s="9"/>
       <c r="M6" s="25"/>
@@ -21073,7 +21067,7 @@
       <c r="C7" s="13"/>
       <c r="D7" s="13"/>
       <c r="E7" s="72" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="F7" s="10"/>
       <c r="G7" s="70" t="s">
@@ -21089,7 +21083,7 @@
         <v>27</v>
       </c>
       <c r="K7" s="70" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="L7" s="9"/>
       <c r="M7" s="25"/>
@@ -21109,10 +21103,10 @@
       <c r="A8" s="82"/>
       <c r="B8" s="82"/>
       <c r="D8" s="84" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="E8" s="84" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="F8" s="84">
         <v>5.2</v>
@@ -21128,7 +21122,7 @@
         <v>27</v>
       </c>
       <c r="K8" s="83" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
     </row>
     <row r="9" spans="1:26" s="21" customFormat="1" ht="28.8">
@@ -21136,19 +21130,19 @@
       <c r="B9" s="20"/>
       <c r="C9" s="22"/>
       <c r="E9" s="21" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="G9" s="21" t="s">
         <v>46</v>
       </c>
       <c r="H9" s="21" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="J9" s="23" t="s">
         <v>30</v>
       </c>
       <c r="K9" s="80" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="L9" s="22"/>
     </row>
@@ -21157,19 +21151,19 @@
       <c r="B10" s="20"/>
       <c r="C10" s="22"/>
       <c r="E10" s="21" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="G10" s="21" t="s">
         <v>46</v>
       </c>
       <c r="H10" s="21" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="J10" s="23" t="s">
         <v>30</v>
       </c>
       <c r="K10" s="80" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="L10" s="22"/>
     </row>
@@ -21178,10 +21172,10 @@
       <c r="B11" s="92"/>
       <c r="C11" s="93"/>
       <c r="D11" s="76" t="s">
+        <v>942</v>
+      </c>
+      <c r="E11" s="76" t="s">
         <v>943</v>
-      </c>
-      <c r="E11" s="76" t="s">
-        <v>944</v>
       </c>
       <c r="F11" s="65">
         <v>36</v>
@@ -21193,16 +21187,16 @@
         <v>226</v>
       </c>
       <c r="I11" s="76" t="s">
+        <v>945</v>
+      </c>
+      <c r="J11" s="94" t="s">
+        <v>944</v>
+      </c>
+      <c r="K11" s="95" t="s">
         <v>946</v>
       </c>
-      <c r="J11" s="94" t="s">
-        <v>945</v>
-      </c>
-      <c r="K11" s="95" t="s">
+      <c r="L11" s="94" t="s">
         <v>947</v>
-      </c>
-      <c r="L11" s="94" t="s">
-        <v>948</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.4">
@@ -21361,7 +21355,7 @@
       <c r="B20" s="20"/>
       <c r="D20" s="3"/>
       <c r="E20" s="7" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="F20" s="7">
         <v>1</v>
@@ -21379,7 +21373,7 @@
         <v>27</v>
       </c>
       <c r="K20" s="21" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
     </row>
     <row r="21" spans="1:26" s="21" customFormat="1" ht="14.4">
@@ -21387,7 +21381,7 @@
       <c r="B21" s="20"/>
       <c r="D21" s="3"/>
       <c r="E21" s="7" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
       <c r="F21" s="7"/>
       <c r="G21" s="7" t="s">
@@ -21403,7 +21397,7 @@
         <v>27</v>
       </c>
       <c r="K21" s="21" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
     </row>
     <row r="22" spans="1:26" s="21" customFormat="1" ht="14.4">
@@ -21411,7 +21405,7 @@
       <c r="B22" s="20"/>
       <c r="D22" s="3"/>
       <c r="E22" s="7" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="F22" s="7">
         <v>90</v>
@@ -21420,13 +21414,13 @@
         <v>108</v>
       </c>
       <c r="H22" s="7" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="J22" s="21" t="s">
         <v>30</v>
       </c>
       <c r="K22" s="21" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
     </row>
     <row r="23" spans="1:26" ht="14.4">
@@ -21492,7 +21486,7 @@
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
       <c r="E25" s="7" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="F25" s="7">
         <v>4.2</v>
@@ -21510,7 +21504,7 @@
         <v>27</v>
       </c>
       <c r="K25" s="3" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="N25" s="3"/>
     </row>
@@ -21522,7 +21516,7 @@
         <v>24</v>
       </c>
       <c r="D26" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="E26" s="7" t="s">
         <v>50</v>
@@ -21531,11 +21525,11 @@
         <v>0</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="H26" s="7"/>
       <c r="K26" s="23" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
     </row>
     <row r="27" spans="1:26" ht="14.4">
@@ -21616,7 +21610,7 @@
         <v>30</v>
       </c>
       <c r="K30" s="80" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="L30" s="19"/>
       <c r="M30" s="19"/>
@@ -21720,7 +21714,7 @@
       <c r="B34" s="20"/>
       <c r="D34" s="22"/>
       <c r="E34" s="21" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="F34" s="7"/>
       <c r="G34" s="57" t="s">
@@ -21736,7 +21730,7 @@
         <v>27</v>
       </c>
       <c r="K34" s="23" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
     </row>
     <row r="35" spans="1:12" s="21" customFormat="1" ht="14.4">
@@ -21744,7 +21738,7 @@
       <c r="B35" s="20"/>
       <c r="D35" s="22"/>
       <c r="E35" s="21" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="F35" s="7"/>
       <c r="G35" s="57" t="s">
@@ -21760,7 +21754,7 @@
         <v>27</v>
       </c>
       <c r="K35" s="23" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
     </row>
     <row r="36" spans="1:12" ht="14.4">
@@ -21883,14 +21877,14 @@
       <c r="A41" s="20"/>
       <c r="B41" s="20"/>
       <c r="E41" s="7" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
       <c r="F41" s="7"/>
       <c r="G41" s="21" t="s">
         <v>108</v>
       </c>
       <c r="H41" s="21" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="I41" s="21" t="s">
         <v>26</v>
@@ -21899,7 +21893,7 @@
         <v>27</v>
       </c>
       <c r="K41" s="23" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
     </row>
     <row r="42" spans="1:12" s="21" customFormat="1" ht="14.4">
@@ -21915,7 +21909,7 @@
         <v>108</v>
       </c>
       <c r="H42" s="21" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
       <c r="I42" s="21" t="s">
         <v>26</v>
@@ -21924,21 +21918,21 @@
         <v>27</v>
       </c>
       <c r="K42" s="23" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
     </row>
     <row r="43" spans="1:12" s="21" customFormat="1" ht="14.4">
       <c r="A43" s="20"/>
       <c r="B43" s="20"/>
       <c r="E43" s="7" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="F43" s="7"/>
       <c r="G43" s="21" t="s">
         <v>108</v>
       </c>
       <c r="H43" s="21" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
       <c r="I43" s="21" t="s">
         <v>26</v>
@@ -21947,10 +21941,10 @@
         <v>27</v>
       </c>
       <c r="K43" s="23" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
       <c r="L43" s="21" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
     </row>
     <row r="44" spans="1:12" ht="14.4">
@@ -22007,18 +22001,18 @@
       <c r="B46" s="20"/>
       <c r="D46" s="3"/>
       <c r="E46" s="7" t="s">
-        <v>1006</v>
+        <v>1004</v>
       </c>
       <c r="F46" s="7"/>
       <c r="G46" s="7"/>
       <c r="H46" s="7" t="s">
-        <v>1007</v>
+        <v>1005</v>
       </c>
       <c r="I46" s="21" t="s">
         <v>26</v>
       </c>
       <c r="K46" s="23" t="s">
-        <v>1008</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="47" spans="1:12" ht="14.4">
@@ -22029,7 +22023,7 @@
         <v>24</v>
       </c>
       <c r="D47" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="E47" s="7" t="s">
         <v>87</v>
@@ -22038,11 +22032,11 @@
         <v>0</v>
       </c>
       <c r="G47" s="7" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="H47" s="7"/>
       <c r="K47" s="23" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
     </row>
     <row r="48" spans="1:12" ht="14.4">
@@ -22105,7 +22099,7 @@
         <v>803</v>
       </c>
       <c r="E50" s="7" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="F50" s="7"/>
       <c r="G50" s="7" t="s">
@@ -22121,7 +22115,7 @@
         <v>27</v>
       </c>
       <c r="K50" s="57" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
     </row>
     <row r="51" spans="1:11" s="21" customFormat="1" ht="14.4">
@@ -22169,7 +22163,7 @@
       <c r="I52" s="57"/>
       <c r="J52" s="57"/>
       <c r="K52" s="57" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
     </row>
     <row r="53" spans="1:11" ht="14.4">
@@ -22180,7 +22174,7 @@
         <v>24</v>
       </c>
       <c r="E53" s="7" t="s">
-        <v>1005</v>
+        <v>1003</v>
       </c>
       <c r="F53" s="7">
         <v>0</v>
@@ -22195,14 +22189,14 @@
         <v>26</v>
       </c>
       <c r="K53" s="57" t="s">
-        <v>1004</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="54" spans="1:11" s="21" customFormat="1" ht="14.4">
       <c r="A54" s="20"/>
       <c r="B54" s="20"/>
       <c r="E54" s="7" t="s">
-        <v>992</v>
+        <v>990</v>
       </c>
       <c r="F54" s="7"/>
       <c r="G54" s="21" t="s">
@@ -22218,7 +22212,7 @@
         <v>30</v>
       </c>
       <c r="K54" s="57" t="s">
-        <v>993</v>
+        <v>991</v>
       </c>
     </row>
     <row r="55" spans="1:11" ht="14.4">
@@ -22244,7 +22238,7 @@
       <c r="A56" s="20"/>
       <c r="B56" s="20"/>
       <c r="E56" s="7" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="F56" s="7">
         <v>0.08</v>
@@ -22262,21 +22256,21 @@
         <v>30</v>
       </c>
       <c r="K56" s="23" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
     </row>
     <row r="57" spans="1:11" s="21" customFormat="1" ht="14.4">
       <c r="A57" s="20"/>
       <c r="B57" s="20"/>
       <c r="E57" s="58" t="s">
-        <v>996</v>
+        <v>994</v>
       </c>
       <c r="F57" s="7"/>
       <c r="G57" s="7" t="s">
         <v>108</v>
       </c>
       <c r="H57" s="7" t="s">
-        <v>994</v>
+        <v>992</v>
       </c>
       <c r="I57" s="21" t="s">
         <v>34</v>
@@ -22285,14 +22279,14 @@
         <v>30</v>
       </c>
       <c r="K57" s="23" t="s">
-        <v>995</v>
+        <v>993</v>
       </c>
     </row>
     <row r="58" spans="1:11" s="21" customFormat="1" ht="14.4">
       <c r="A58" s="20"/>
       <c r="B58" s="20"/>
       <c r="E58" s="58" t="s">
-        <v>1000</v>
+        <v>998</v>
       </c>
       <c r="F58" s="7"/>
       <c r="G58" s="7" t="s">
@@ -22308,14 +22302,14 @@
         <v>27</v>
       </c>
       <c r="K58" s="23" t="s">
-        <v>1001</v>
+        <v>999</v>
       </c>
     </row>
     <row r="59" spans="1:11" s="21" customFormat="1" ht="14.4">
       <c r="A59" s="20"/>
       <c r="B59" s="20"/>
       <c r="E59" s="58" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="F59" s="7"/>
       <c r="G59" s="7" t="s">
@@ -22328,7 +22322,7 @@
         <v>26</v>
       </c>
       <c r="K59" s="23" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
     </row>
     <row r="60" spans="1:11" s="21" customFormat="1" ht="14.4">
@@ -22343,14 +22337,14 @@
         <v>474</v>
       </c>
       <c r="K60" s="23" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
     </row>
     <row r="61" spans="1:11" s="21" customFormat="1" ht="14.4">
       <c r="A61" s="20"/>
       <c r="B61" s="20"/>
       <c r="E61" s="58" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
       <c r="F61" s="7"/>
       <c r="G61" s="7" t="s">
@@ -22366,14 +22360,14 @@
         <v>27</v>
       </c>
       <c r="K61" s="23" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
     </row>
     <row r="62" spans="1:11" s="21" customFormat="1" ht="14.4">
       <c r="A62" s="20"/>
       <c r="B62" s="20"/>
       <c r="E62" s="7" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="F62" s="7"/>
       <c r="G62" s="7" t="s">
@@ -22386,14 +22380,14 @@
         <v>26</v>
       </c>
       <c r="K62" s="23" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
     </row>
     <row r="63" spans="1:11" s="21" customFormat="1" ht="14.4">
       <c r="A63" s="20"/>
       <c r="B63" s="20"/>
       <c r="E63" s="7" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="F63" s="7"/>
       <c r="G63" s="7" t="s">
@@ -22406,7 +22400,7 @@
         <v>34</v>
       </c>
       <c r="K63" s="23" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
     </row>
     <row r="64" spans="1:11" ht="14.4">
@@ -22450,14 +22444,14 @@
       <c r="C65" s="22"/>
       <c r="D65" s="22"/>
       <c r="E65" s="21" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="F65" s="7"/>
       <c r="G65" s="21" t="s">
         <v>108</v>
       </c>
       <c r="H65" s="21" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="I65" s="23" t="s">
         <v>26</v>
@@ -22466,7 +22460,7 @@
         <v>27</v>
       </c>
       <c r="K65" s="23" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
     </row>
     <row r="66" spans="1:26" s="21" customFormat="1" ht="14.4">
@@ -22475,7 +22469,7 @@
       <c r="C66" s="22"/>
       <c r="D66" s="22"/>
       <c r="E66" s="21" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="F66" s="7"/>
       <c r="G66" s="21" t="s">
@@ -22491,7 +22485,7 @@
         <v>27</v>
       </c>
       <c r="K66" s="23" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
     </row>
     <row r="67" spans="1:26" s="21" customFormat="1" ht="14.4">
@@ -22502,7 +22496,7 @@
       <c r="C67" s="22"/>
       <c r="D67" s="22"/>
       <c r="E67" s="21" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="F67" s="7"/>
       <c r="G67" s="21" t="s">
@@ -22518,7 +22512,7 @@
         <v>27</v>
       </c>
       <c r="K67" s="23" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
     </row>
     <row r="68" spans="1:26" ht="43.2">
@@ -22551,7 +22545,7 @@
       <c r="A69" s="20"/>
       <c r="B69" s="20"/>
       <c r="E69" s="7" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="G69" s="21" t="s">
         <v>108</v>
@@ -22566,7 +22560,7 @@
         <v>30</v>
       </c>
       <c r="K69" s="23" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
     </row>
     <row r="70" spans="1:26" s="25" customFormat="1" ht="86.4">
@@ -22591,14 +22585,14 @@
         <v>30</v>
       </c>
       <c r="K70" s="80" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
     </row>
     <row r="71" spans="1:26" s="25" customFormat="1" ht="14.4">
       <c r="A71" s="81"/>
       <c r="B71" s="81"/>
       <c r="E71" s="72" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="G71" s="72" t="s">
         <v>108</v>
@@ -22613,7 +22607,7 @@
         <v>27</v>
       </c>
       <c r="K71" s="23" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
     </row>
     <row r="72" spans="1:26" s="25" customFormat="1" ht="28.8">
@@ -22622,7 +22616,7 @@
         <v>23</v>
       </c>
       <c r="E72" s="25" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="G72" s="25" t="s">
         <v>108</v>
@@ -22635,7 +22629,7 @@
       </c>
       <c r="J72" s="19"/>
       <c r="K72" s="80" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
     </row>
     <row r="73" spans="1:26" s="21" customFormat="1" ht="14.25" customHeight="1">
@@ -22680,14 +22674,14 @@
       <c r="C74" s="28"/>
       <c r="D74" s="28"/>
       <c r="E74" s="25" t="s">
-        <v>997</v>
+        <v>995</v>
       </c>
       <c r="F74" s="7"/>
       <c r="G74" s="70" t="s">
         <v>108</v>
       </c>
       <c r="H74" s="70" t="s">
-        <v>998</v>
+        <v>996</v>
       </c>
       <c r="I74" s="70" t="s">
         <v>34</v>
@@ -22696,7 +22690,7 @@
         <v>30</v>
       </c>
       <c r="K74" s="70" t="s">
-        <v>999</v>
+        <v>997</v>
       </c>
       <c r="L74" s="70"/>
       <c r="M74" s="3"/>
@@ -22732,17 +22726,17 @@
       <c r="A76" s="20"/>
       <c r="B76" s="20"/>
       <c r="E76" s="25" t="s">
+        <v>980</v>
+      </c>
+      <c r="F76" s="7" t="s">
         <v>981</v>
-      </c>
-      <c r="F76" s="7" t="s">
-        <v>982</v>
       </c>
       <c r="G76" s="25" t="s">
         <v>70</v>
       </c>
       <c r="H76" s="7"/>
       <c r="K76" s="21" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
     </row>
     <row r="77" spans="1:26" ht="14.4">
@@ -22816,7 +22810,7 @@
       <c r="A79" s="20"/>
       <c r="B79" s="20"/>
       <c r="E79" s="7" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="F79" s="7"/>
       <c r="G79" s="7" t="s">
@@ -22843,14 +22837,14 @@
       <c r="G80" s="7"/>
       <c r="H80" s="7"/>
       <c r="K80" s="3" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
     </row>
     <row r="81" spans="1:12" s="21" customFormat="1" ht="14.4">
       <c r="A81" s="20"/>
       <c r="B81" s="20"/>
       <c r="E81" s="7" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="F81" s="7"/>
       <c r="G81" s="7" t="s">
@@ -22866,17 +22860,17 @@
         <v>30</v>
       </c>
       <c r="K81" s="21" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="L81" s="3" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
     </row>
     <row r="82" spans="1:12" s="21" customFormat="1" ht="14.4">
       <c r="A82" s="20"/>
       <c r="B82" s="20"/>
       <c r="E82" s="7" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="F82" s="7"/>
       <c r="G82" s="7" t="s">
@@ -22892,10 +22886,10 @@
         <v>30</v>
       </c>
       <c r="K82" s="21" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="L82" s="3" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
     </row>
     <row r="83" spans="1:12" ht="14.4">
@@ -22999,7 +22993,7 @@
       <c r="B87" s="20"/>
       <c r="C87" s="3"/>
       <c r="E87" s="7" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="F87" s="7"/>
       <c r="G87" s="7"/>
@@ -23011,12 +23005,12 @@
         <v>27</v>
       </c>
       <c r="K87" s="3" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
     </row>
     <row r="88" spans="1:12" s="21" customFormat="1" ht="14.4">
       <c r="A88" s="20" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="B88" s="20" t="s">
         <v>24</v>
@@ -23028,7 +23022,7 @@
         <v>65</v>
       </c>
       <c r="E88" s="7" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="F88" s="7">
         <v>5</v>
@@ -23046,7 +23040,7 @@
         <v>27</v>
       </c>
       <c r="K88" s="3" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="L88" s="23" t="s">
         <v>65</v>
@@ -23087,7 +23081,7 @@
       <c r="B90" s="20"/>
       <c r="D90" s="3"/>
       <c r="E90" s="7" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="F90" s="7"/>
       <c r="G90" s="7"/>
@@ -23097,7 +23091,7 @@
       <c r="I90" s="3"/>
       <c r="J90" s="3"/>
       <c r="K90" s="3" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
     </row>
     <row r="91" spans="1:12" s="21" customFormat="1" ht="14.4">
@@ -23105,7 +23099,7 @@
       <c r="B91" s="20"/>
       <c r="D91" s="3"/>
       <c r="E91" s="7" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="F91" s="7"/>
       <c r="G91" s="7"/>
@@ -23115,7 +23109,7 @@
       <c r="I91" s="3"/>
       <c r="J91" s="3"/>
       <c r="K91" s="3" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
     </row>
     <row r="92" spans="1:12" ht="14.4">
@@ -23136,7 +23130,7 @@
       <c r="A93" s="20"/>
       <c r="B93" s="20"/>
       <c r="E93" s="7" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="F93" s="7">
         <v>5</v>
@@ -23154,14 +23148,14 @@
         <v>30</v>
       </c>
       <c r="K93" s="23" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
     </row>
     <row r="94" spans="1:12" s="21" customFormat="1" ht="14.4">
       <c r="A94" s="20"/>
       <c r="B94" s="20"/>
       <c r="E94" s="58" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="F94" s="7">
         <v>5</v>
@@ -23179,14 +23173,14 @@
         <v>30</v>
       </c>
       <c r="K94" s="23" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
     </row>
     <row r="95" spans="1:12" s="21" customFormat="1" ht="14.4">
       <c r="A95" s="20"/>
       <c r="B95" s="20"/>
       <c r="E95" s="58" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="F95" s="7">
         <v>5</v>
@@ -23204,14 +23198,14 @@
         <v>30</v>
       </c>
       <c r="K95" s="23" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
     </row>
     <row r="96" spans="1:12" s="21" customFormat="1" ht="14.4">
       <c r="A96" s="20"/>
       <c r="B96" s="20"/>
       <c r="E96" s="7" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="F96" s="7">
         <v>1</v>
@@ -23220,20 +23214,20 @@
         <v>108</v>
       </c>
       <c r="H96" s="7" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="I96" s="23" t="s">
         <v>26</v>
       </c>
       <c r="J96" s="23" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
     </row>
     <row r="97" spans="1:12" s="21" customFormat="1" ht="14.4">
       <c r="A97" s="20"/>
       <c r="B97" s="20"/>
       <c r="E97" s="7" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="F97" s="7"/>
       <c r="G97" s="7" t="s">
@@ -23249,17 +23243,17 @@
         <v>27</v>
       </c>
       <c r="K97" s="23" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
       <c r="L97" s="23" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
     </row>
     <row r="98" spans="1:12" s="21" customFormat="1" ht="14.4">
       <c r="A98" s="20"/>
       <c r="B98" s="20"/>
       <c r="E98" s="7" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="F98" s="7"/>
       <c r="G98" s="7" t="s">
@@ -23271,7 +23265,7 @@
       <c r="I98" s="23"/>
       <c r="J98" s="23"/>
       <c r="K98" s="23" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
       <c r="L98" s="23"/>
     </row>
@@ -23279,7 +23273,7 @@
       <c r="A99" s="20"/>
       <c r="B99" s="20"/>
       <c r="E99" s="7" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="F99" s="7"/>
       <c r="G99" s="7" t="s">
@@ -23291,7 +23285,7 @@
       <c r="I99" s="23"/>
       <c r="J99" s="23"/>
       <c r="K99" s="23" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
       <c r="L99" s="23"/>
     </row>
@@ -23299,10 +23293,10 @@
       <c r="A100" s="20"/>
       <c r="B100" s="20"/>
       <c r="D100" s="57" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="E100" s="7" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
       <c r="F100" s="7"/>
       <c r="G100" s="58" t="s">
@@ -23312,13 +23306,13 @@
         <v>84</v>
       </c>
       <c r="I100" s="23" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="J100" s="23" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="K100" s="23" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="L100" s="23"/>
     </row>
@@ -23326,7 +23320,7 @@
       <c r="A101" s="20"/>
       <c r="B101" s="20"/>
       <c r="E101" s="7" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="F101" s="7">
         <v>10</v>
@@ -23344,14 +23338,14 @@
         <v>27</v>
       </c>
       <c r="K101" s="23" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
     </row>
     <row r="102" spans="1:12" s="21" customFormat="1" ht="14.4">
       <c r="A102" s="20"/>
       <c r="B102" s="20"/>
       <c r="E102" s="7" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="F102" s="7"/>
       <c r="G102" s="7" t="s">
@@ -23367,14 +23361,14 @@
         <v>30</v>
       </c>
       <c r="K102" s="23" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="103" spans="1:12" s="21" customFormat="1" ht="14.4">
       <c r="A103" s="20"/>
       <c r="B103" s="20"/>
       <c r="E103" s="7" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="F103" s="7"/>
       <c r="G103" s="7" t="s">
@@ -23388,10 +23382,10 @@
         <v>27</v>
       </c>
       <c r="K103" s="23" t="s">
+        <v>973</v>
+      </c>
+      <c r="L103" s="23" t="s">
         <v>974</v>
-      </c>
-      <c r="L103" s="23" t="s">
-        <v>975</v>
       </c>
     </row>
     <row r="104" spans="1:12" s="21" customFormat="1" ht="14.4">
@@ -23408,7 +23402,7 @@
       <c r="I104" s="23"/>
       <c r="J104" s="23"/>
       <c r="K104" s="23" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
     </row>
     <row r="105" spans="1:12" s="21" customFormat="1" ht="14.4">

</xml_diff>

<commit_message>
Continue developing the wetland model. Flow.cpp, .h - #define WETL_ID. Refine the Wetland class definition. Add AttInt() to FlowModel. Code up InitWetlands(). Refine QtoWetland(). Add a constructor for Wetland objects.  In the constructor for FlowModel, call RemoveAll() on m_scenarioArray, the array that holds pointers to the climate scenarios.
</commit_message>
<xml_diff>
--- a/DataCW3M/CW3MdigitalHandbook/CW3MdataDictionary.xlsx
+++ b/DataCW3M/CW3MdigitalHandbook/CW3MdataDictionary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\CW3MdigitalHandbook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E40CC19-E537-49D1-A0F0-94A34DA5B9F1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22362470-F3FC-4F58-8B76-9AF46BEABCEA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-7425" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -78,7 +78,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H264" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+    <comment ref="H265" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -97,7 +97,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2996" uniqueCount="1007">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3007" uniqueCount="1011">
   <si>
     <t>LULC_A</t>
   </si>
@@ -3119,6 +3119,18 @@
   </si>
   <si>
     <t>log10(Q_DISCHARG)</t>
+  </si>
+  <si>
+    <t>REACH_NDX</t>
+  </si>
+  <si>
+    <t>index into the internal C++ reach array for this reach; set by ReachInit() called by FlowModel::Init()</t>
+  </si>
+  <si>
+    <t>WETL_ID</t>
+  </si>
+  <si>
+    <t>wetland ID</t>
   </si>
 </sst>
 </file>
@@ -9081,11 +9093,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Z1048"/>
+  <dimension ref="A1:Z1049"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A196" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G225" sqref="G225"/>
+      <pane ySplit="3" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -10622,7 +10634,9 @@
       <c r="C44" s="7" t="s">
         <v>255</v>
       </c>
-      <c r="D44" s="8"/>
+      <c r="D44" s="8" t="s">
+        <v>29</v>
+      </c>
       <c r="E44" s="8" t="s">
         <v>84</v>
       </c>
@@ -16808,96 +16822,92 @@
       <c r="T224" s="7"/>
       <c r="U224" s="7"/>
     </row>
-    <row r="225" spans="1:26" s="65" customFormat="1" ht="13.95" customHeight="1">
-      <c r="A225" s="66"/>
-      <c r="B225" s="66"/>
-      <c r="C225" s="64" t="s">
+    <row r="225" spans="1:26" s="21" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A225" s="28"/>
+      <c r="B225" s="28"/>
+      <c r="C225" s="7" t="s">
+        <v>1009</v>
+      </c>
+      <c r="D225" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="E225" s="70"/>
+      <c r="F225" s="10"/>
+      <c r="G225" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H225" s="25" t="s">
+        <v>1010</v>
+      </c>
+      <c r="I225" s="27"/>
+      <c r="J225" s="3"/>
+      <c r="K225" s="7"/>
+      <c r="L225" s="7"/>
+      <c r="M225" s="7"/>
+      <c r="N225" s="7"/>
+      <c r="O225" s="7"/>
+      <c r="P225" s="7"/>
+      <c r="Q225" s="7"/>
+      <c r="R225" s="7"/>
+      <c r="S225" s="7"/>
+      <c r="T225" s="7"/>
+      <c r="U225" s="7"/>
+    </row>
+    <row r="226" spans="1:26" s="65" customFormat="1" ht="13.95" customHeight="1">
+      <c r="A226" s="66"/>
+      <c r="B226" s="66"/>
+      <c r="C226" s="64" t="s">
         <v>830</v>
       </c>
-      <c r="D225" s="62" t="s">
+      <c r="D226" s="62" t="s">
         <v>29</v>
       </c>
-      <c r="E225" s="62" t="s">
+      <c r="E226" s="62" t="s">
         <v>94</v>
       </c>
-      <c r="F225" s="62" t="s">
+      <c r="F226" s="62" t="s">
         <v>65</v>
       </c>
-      <c r="G225" s="62" t="s">
+      <c r="G226" s="62" t="s">
         <v>27</v>
       </c>
-      <c r="H225" s="61" t="s">
+      <c r="H226" s="61" t="s">
         <v>831</v>
       </c>
-      <c r="I225" s="74" t="s">
+      <c r="I226" s="74" t="s">
         <v>832</v>
       </c>
-      <c r="J225" s="68"/>
-      <c r="K225" s="64"/>
-      <c r="L225" s="64"/>
-      <c r="M225" s="64"/>
-      <c r="N225" s="64"/>
-      <c r="O225" s="64"/>
-      <c r="P225" s="64"/>
-      <c r="Q225" s="64"/>
-      <c r="R225" s="64"/>
-      <c r="S225" s="64"/>
-      <c r="T225" s="64"/>
-      <c r="U225" s="64"/>
-    </row>
-    <row r="226" spans="1:26" s="91" customFormat="1" ht="13.95" customHeight="1">
-      <c r="A226" s="96"/>
-      <c r="B226" s="96"/>
-      <c r="C226" s="97" t="s">
-        <v>1000</v>
-      </c>
-      <c r="D226" s="100" t="s">
-        <v>108</v>
-      </c>
-      <c r="E226" s="100" t="s">
-        <v>73</v>
-      </c>
-      <c r="F226" s="100"/>
-      <c r="G226" s="100" t="s">
-        <v>27</v>
-      </c>
-      <c r="H226" s="91" t="s">
-        <v>1001</v>
-      </c>
-      <c r="I226" s="98"/>
-      <c r="J226" s="84"/>
-      <c r="K226" s="97"/>
-      <c r="L226" s="97"/>
-      <c r="M226" s="97"/>
-      <c r="N226" s="97"/>
-      <c r="O226" s="97"/>
-      <c r="P226" s="97"/>
-      <c r="Q226" s="97"/>
-      <c r="R226" s="97"/>
-      <c r="S226" s="97"/>
-      <c r="T226" s="97"/>
-      <c r="U226" s="97"/>
+      <c r="J226" s="68"/>
+      <c r="K226" s="64"/>
+      <c r="L226" s="64"/>
+      <c r="M226" s="64"/>
+      <c r="N226" s="64"/>
+      <c r="O226" s="64"/>
+      <c r="P226" s="64"/>
+      <c r="Q226" s="64"/>
+      <c r="R226" s="64"/>
+      <c r="S226" s="64"/>
+      <c r="T226" s="64"/>
+      <c r="U226" s="64"/>
     </row>
     <row r="227" spans="1:26" s="91" customFormat="1" ht="13.95" customHeight="1">
       <c r="A227" s="96"/>
       <c r="B227" s="96"/>
       <c r="C227" s="97" t="s">
-        <v>988</v>
-      </c>
-      <c r="D227" s="99" t="s">
+        <v>1000</v>
+      </c>
+      <c r="D227" s="100" t="s">
         <v>108</v>
       </c>
-      <c r="E227" s="99" t="s">
-        <v>172</v>
-      </c>
-      <c r="F227" s="99" t="s">
-        <v>825</v>
-      </c>
-      <c r="G227" s="99" t="s">
+      <c r="E227" s="100" t="s">
+        <v>73</v>
+      </c>
+      <c r="F227" s="100"/>
+      <c r="G227" s="100" t="s">
         <v>27</v>
       </c>
-      <c r="H227" s="77" t="s">
-        <v>989</v>
+      <c r="H227" s="91" t="s">
+        <v>1001</v>
       </c>
       <c r="I227" s="98"/>
       <c r="J227" s="84"/>
@@ -16913,85 +16923,85 @@
       <c r="T227" s="97"/>
       <c r="U227" s="97"/>
     </row>
-    <row r="228" spans="1:26" s="21" customFormat="1" ht="16.95" customHeight="1">
-      <c r="A228" s="28"/>
-      <c r="B228" s="28"/>
-      <c r="C228" s="21" t="s">
+    <row r="228" spans="1:26" s="91" customFormat="1" ht="13.95" customHeight="1">
+      <c r="A228" s="96"/>
+      <c r="B228" s="96"/>
+      <c r="C228" s="97" t="s">
+        <v>988</v>
+      </c>
+      <c r="D228" s="99" t="s">
+        <v>108</v>
+      </c>
+      <c r="E228" s="99" t="s">
+        <v>172</v>
+      </c>
+      <c r="F228" s="99" t="s">
+        <v>825</v>
+      </c>
+      <c r="G228" s="99" t="s">
+        <v>27</v>
+      </c>
+      <c r="H228" s="77" t="s">
+        <v>989</v>
+      </c>
+      <c r="I228" s="98"/>
+      <c r="J228" s="84"/>
+      <c r="K228" s="97"/>
+      <c r="L228" s="97"/>
+      <c r="M228" s="97"/>
+      <c r="N228" s="97"/>
+      <c r="O228" s="97"/>
+      <c r="P228" s="97"/>
+      <c r="Q228" s="97"/>
+      <c r="R228" s="97"/>
+      <c r="S228" s="97"/>
+      <c r="T228" s="97"/>
+      <c r="U228" s="97"/>
+    </row>
+    <row r="229" spans="1:26" s="21" customFormat="1" ht="16.95" customHeight="1">
+      <c r="A229" s="28"/>
+      <c r="B229" s="28"/>
+      <c r="C229" s="21" t="s">
         <v>509</v>
       </c>
-      <c r="D228" s="10" t="s">
+      <c r="D229" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="E228" s="10" t="s">
+      <c r="E229" s="10" t="s">
         <v>510</v>
       </c>
-      <c r="F228" s="10" t="s">
+      <c r="F229" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="G228" s="10" t="s">
+      <c r="G229" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="H228" s="21" t="s">
+      <c r="H229" s="21" t="s">
         <v>728</v>
       </c>
-      <c r="I228" s="27" t="s">
+      <c r="I229" s="27" t="s">
         <v>814</v>
       </c>
-      <c r="J228" s="23"/>
-    </row>
-    <row r="229" spans="1:26" ht="42.75" customHeight="1">
-      <c r="A229" s="6"/>
-      <c r="B229" s="6" t="s">
-        <v>159</v>
-      </c>
-      <c r="C229" s="7" t="s">
-        <v>729</v>
-      </c>
-      <c r="D229" s="8"/>
-      <c r="E229" s="8" t="s">
-        <v>730</v>
-      </c>
-      <c r="F229" s="10"/>
-      <c r="G229" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="H229" s="14" t="s">
-        <v>731</v>
-      </c>
-      <c r="I229" s="27" t="s">
-        <v>727</v>
-      </c>
-      <c r="J229" s="3"/>
-      <c r="K229" s="7"/>
-      <c r="L229" s="7"/>
-      <c r="M229" s="7"/>
-      <c r="N229" s="7"/>
-      <c r="O229" s="7"/>
-      <c r="P229" s="7"/>
-      <c r="Q229" s="7"/>
-      <c r="R229" s="7"/>
-      <c r="S229" s="7"/>
-      <c r="T229" s="7"/>
-      <c r="U229" s="7"/>
-    </row>
-    <row r="230" spans="1:26" ht="14.25" customHeight="1">
+      <c r="J229" s="23"/>
+    </row>
+    <row r="230" spans="1:26" ht="42.75" customHeight="1">
       <c r="A230" s="6"/>
       <c r="B230" s="6" t="s">
         <v>159</v>
       </c>
       <c r="C230" s="7" t="s">
-        <v>732</v>
+        <v>729</v>
       </c>
       <c r="D230" s="8"/>
       <c r="E230" s="8" t="s">
-        <v>70</v>
+        <v>730</v>
       </c>
       <c r="F230" s="10"/>
       <c r="G230" s="8" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="H230" s="14" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="I230" s="27" t="s">
         <v>727</v>
@@ -17012,10 +17022,10 @@
     <row r="231" spans="1:26" ht="14.25" customHeight="1">
       <c r="A231" s="6"/>
       <c r="B231" s="6" t="s">
-        <v>23</v>
+        <v>159</v>
       </c>
       <c r="C231" s="7" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="D231" s="8"/>
       <c r="E231" s="8" t="s">
@@ -17023,10 +17033,10 @@
       </c>
       <c r="F231" s="10"/>
       <c r="G231" s="8" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="H231" s="14" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="I231" s="27" t="s">
         <v>727</v>
@@ -17047,10 +17057,10 @@
     <row r="232" spans="1:26" ht="14.25" customHeight="1">
       <c r="A232" s="6"/>
       <c r="B232" s="6" t="s">
-        <v>159</v>
+        <v>23</v>
       </c>
       <c r="C232" s="7" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="D232" s="8"/>
       <c r="E232" s="8" t="s">
@@ -17058,12 +17068,14 @@
       </c>
       <c r="F232" s="10"/>
       <c r="G232" s="8" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="H232" s="14" t="s">
-        <v>737</v>
-      </c>
-      <c r="I232" s="27"/>
+        <v>735</v>
+      </c>
+      <c r="I232" s="27" t="s">
+        <v>727</v>
+      </c>
       <c r="J232" s="3"/>
       <c r="K232" s="7"/>
       <c r="L232" s="7"/>
@@ -17083,22 +17095,20 @@
         <v>159</v>
       </c>
       <c r="C233" s="7" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="D233" s="8"/>
       <c r="E233" s="8" t="s">
-        <v>226</v>
+        <v>70</v>
       </c>
       <c r="F233" s="10"/>
       <c r="G233" s="8" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="H233" s="14" t="s">
-        <v>739</v>
-      </c>
-      <c r="I233" s="27" t="s">
-        <v>727</v>
-      </c>
+        <v>737</v>
+      </c>
+      <c r="I233" s="27"/>
       <c r="J233" s="3"/>
       <c r="K233" s="7"/>
       <c r="L233" s="7"/>
@@ -17118,7 +17128,7 @@
         <v>159</v>
       </c>
       <c r="C234" s="7" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="D234" s="8"/>
       <c r="E234" s="8" t="s">
@@ -17129,7 +17139,7 @@
         <v>27</v>
       </c>
       <c r="H234" s="14" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="I234" s="27" t="s">
         <v>727</v>
@@ -17150,22 +17160,24 @@
     <row r="235" spans="1:26" ht="14.25" customHeight="1">
       <c r="A235" s="6"/>
       <c r="B235" s="6" t="s">
-        <v>23</v>
+        <v>159</v>
       </c>
       <c r="C235" s="7" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="D235" s="8"/>
-      <c r="E235" s="8"/>
+      <c r="E235" s="8" t="s">
+        <v>226</v>
+      </c>
       <c r="F235" s="10"/>
       <c r="G235" s="8" t="s">
         <v>27</v>
       </c>
       <c r="H235" s="14" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="I235" s="27" t="s">
-        <v>113</v>
+        <v>727</v>
       </c>
       <c r="J235" s="3"/>
       <c r="K235" s="7"/>
@@ -17183,21 +17195,19 @@
     <row r="236" spans="1:26" ht="14.25" customHeight="1">
       <c r="A236" s="6"/>
       <c r="B236" s="6" t="s">
-        <v>159</v>
+        <v>23</v>
       </c>
       <c r="C236" s="7" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
       <c r="D236" s="8"/>
-      <c r="E236" s="8" t="s">
-        <v>745</v>
-      </c>
+      <c r="E236" s="8"/>
       <c r="F236" s="10"/>
       <c r="G236" s="8" t="s">
         <v>27</v>
       </c>
       <c r="H236" s="14" t="s">
-        <v>746</v>
+        <v>743</v>
       </c>
       <c r="I236" s="27" t="s">
         <v>113</v>
@@ -17216,25 +17226,23 @@
       <c r="U236" s="7"/>
     </row>
     <row r="237" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A237" s="6" t="s">
-        <v>309</v>
-      </c>
+      <c r="A237" s="6"/>
       <c r="B237" s="6" t="s">
-        <v>23</v>
+        <v>159</v>
       </c>
       <c r="C237" s="7" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
       <c r="D237" s="8"/>
       <c r="E237" s="8" t="s">
-        <v>748</v>
+        <v>745</v>
       </c>
       <c r="F237" s="10"/>
       <c r="G237" s="8" t="s">
         <v>27</v>
       </c>
       <c r="H237" s="14" t="s">
-        <v>749</v>
+        <v>746</v>
       </c>
       <c r="I237" s="27" t="s">
         <v>113</v>
@@ -17253,31 +17261,31 @@
       <c r="U237" s="7"/>
     </row>
     <row r="238" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A238" s="6"/>
+      <c r="A238" s="6" t="s">
+        <v>309</v>
+      </c>
       <c r="B238" s="6" t="s">
-        <v>159</v>
+        <v>23</v>
       </c>
       <c r="C238" s="7" t="s">
-        <v>380</v>
+        <v>747</v>
       </c>
       <c r="D238" s="8"/>
       <c r="E238" s="8" t="s">
-        <v>196</v>
+        <v>748</v>
       </c>
       <c r="F238" s="10"/>
       <c r="G238" s="8" t="s">
         <v>27</v>
       </c>
       <c r="H238" s="14" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="I238" s="27" t="s">
         <v>113</v>
       </c>
       <c r="J238" s="3"/>
-      <c r="K238" s="3" t="s">
-        <v>189</v>
-      </c>
+      <c r="K238" s="7"/>
       <c r="L238" s="7"/>
       <c r="M238" s="7"/>
       <c r="N238" s="7"/>
@@ -17288,38 +17296,33 @@
       <c r="S238" s="7"/>
       <c r="T238" s="7"/>
       <c r="U238" s="7"/>
-      <c r="V238" s="7"/>
-      <c r="W238" s="7"/>
-      <c r="X238" s="7"/>
-      <c r="Y238" s="7"/>
-      <c r="Z238" s="7"/>
     </row>
     <row r="239" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A239" s="6" t="s">
-        <v>751</v>
-      </c>
+      <c r="A239" s="6"/>
       <c r="B239" s="6" t="s">
-        <v>23</v>
+        <v>159</v>
       </c>
       <c r="C239" s="7" t="s">
-        <v>752</v>
+        <v>380</v>
       </c>
       <c r="D239" s="8"/>
       <c r="E239" s="8" t="s">
-        <v>70</v>
+        <v>196</v>
       </c>
       <c r="F239" s="10"/>
       <c r="G239" s="8" t="s">
         <v>27</v>
       </c>
       <c r="H239" s="14" t="s">
-        <v>753</v>
+        <v>750</v>
       </c>
       <c r="I239" s="27" t="s">
         <v>113</v>
       </c>
       <c r="J239" s="3"/>
-      <c r="K239" s="7"/>
+      <c r="K239" s="3" t="s">
+        <v>189</v>
+      </c>
       <c r="L239" s="7"/>
       <c r="M239" s="7"/>
       <c r="N239" s="7"/>
@@ -17330,25 +17333,32 @@
       <c r="S239" s="7"/>
       <c r="T239" s="7"/>
       <c r="U239" s="7"/>
+      <c r="V239" s="7"/>
+      <c r="W239" s="7"/>
+      <c r="X239" s="7"/>
+      <c r="Y239" s="7"/>
+      <c r="Z239" s="7"/>
     </row>
     <row r="240" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A240" s="6"/>
+      <c r="A240" s="6" t="s">
+        <v>751</v>
+      </c>
       <c r="B240" s="6" t="s">
         <v>23</v>
       </c>
       <c r="C240" s="7" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
       <c r="D240" s="8"/>
       <c r="E240" s="8" t="s">
-        <v>755</v>
+        <v>70</v>
       </c>
       <c r="F240" s="10"/>
       <c r="G240" s="8" t="s">
         <v>27</v>
       </c>
       <c r="H240" s="14" t="s">
-        <v>756</v>
+        <v>753</v>
       </c>
       <c r="I240" s="27" t="s">
         <v>113</v>
@@ -17372,18 +17382,18 @@
         <v>23</v>
       </c>
       <c r="C241" s="7" t="s">
-        <v>757</v>
+        <v>754</v>
       </c>
       <c r="D241" s="8"/>
       <c r="E241" s="8" t="s">
-        <v>758</v>
+        <v>755</v>
       </c>
       <c r="F241" s="10"/>
       <c r="G241" s="8" t="s">
         <v>27</v>
       </c>
       <c r="H241" s="14" t="s">
-        <v>759</v>
+        <v>756</v>
       </c>
       <c r="I241" s="27" t="s">
         <v>113</v>
@@ -17402,23 +17412,23 @@
       <c r="U241" s="7"/>
     </row>
     <row r="242" spans="1:21" ht="14.25" customHeight="1">
-      <c r="A242" s="6" t="s">
-        <v>309</v>
-      </c>
+      <c r="A242" s="6"/>
       <c r="B242" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C242" s="8" t="s">
-        <v>760</v>
+      <c r="C242" s="7" t="s">
+        <v>757</v>
       </c>
       <c r="D242" s="8"/>
-      <c r="E242" s="8"/>
+      <c r="E242" s="8" t="s">
+        <v>758</v>
+      </c>
       <c r="F242" s="10"/>
       <c r="G242" s="8" t="s">
         <v>27</v>
       </c>
       <c r="H242" s="14" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
       <c r="I242" s="27" t="s">
         <v>113</v>
@@ -17443,8 +17453,8 @@
       <c r="B243" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C243" s="7" t="s">
-        <v>762</v>
+      <c r="C243" s="8" t="s">
+        <v>760</v>
       </c>
       <c r="D243" s="8"/>
       <c r="E243" s="8"/>
@@ -17479,7 +17489,7 @@
         <v>23</v>
       </c>
       <c r="C244" s="7" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="D244" s="8"/>
       <c r="E244" s="8"/>
@@ -17514,7 +17524,7 @@
         <v>23</v>
       </c>
       <c r="C245" s="7" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="D245" s="8"/>
       <c r="E245" s="8"/>
@@ -17549,7 +17559,7 @@
         <v>23</v>
       </c>
       <c r="C246" s="7" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="D246" s="8"/>
       <c r="E246" s="8"/>
@@ -17584,7 +17594,7 @@
         <v>23</v>
       </c>
       <c r="C247" s="7" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="D247" s="8"/>
       <c r="E247" s="8"/>
@@ -17619,7 +17629,7 @@
         <v>23</v>
       </c>
       <c r="C248" s="7" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="D248" s="8"/>
       <c r="E248" s="8"/>
@@ -17654,7 +17664,7 @@
         <v>23</v>
       </c>
       <c r="C249" s="7" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="D249" s="8"/>
       <c r="E249" s="8"/>
@@ -17689,7 +17699,7 @@
         <v>23</v>
       </c>
       <c r="C250" s="7" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="D250" s="8"/>
       <c r="E250" s="8"/>
@@ -17724,7 +17734,7 @@
         <v>23</v>
       </c>
       <c r="C251" s="7" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="D251" s="8"/>
       <c r="E251" s="8"/>
@@ -17759,7 +17769,7 @@
         <v>23</v>
       </c>
       <c r="C252" s="7" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="D252" s="8"/>
       <c r="E252" s="8"/>
@@ -17794,7 +17804,7 @@
         <v>23</v>
       </c>
       <c r="C253" s="7" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="D253" s="8"/>
       <c r="E253" s="8"/>
@@ -17829,7 +17839,7 @@
         <v>23</v>
       </c>
       <c r="C254" s="7" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="D254" s="8"/>
       <c r="E254" s="8"/>
@@ -17864,7 +17874,7 @@
         <v>23</v>
       </c>
       <c r="C255" s="7" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="D255" s="8"/>
       <c r="E255" s="8"/>
@@ -17899,7 +17909,7 @@
         <v>23</v>
       </c>
       <c r="C256" s="7" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="D256" s="8"/>
       <c r="E256" s="8"/>
@@ -17934,7 +17944,7 @@
         <v>23</v>
       </c>
       <c r="C257" s="7" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="D257" s="8"/>
       <c r="E257" s="8"/>
@@ -17969,7 +17979,7 @@
         <v>23</v>
       </c>
       <c r="C258" s="7" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="D258" s="8"/>
       <c r="E258" s="8"/>
@@ -17997,19 +18007,27 @@
       <c r="U258" s="7"/>
     </row>
     <row r="259" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A259" s="6"/>
+      <c r="A259" s="6" t="s">
+        <v>309</v>
+      </c>
       <c r="B259" s="6" t="s">
         <v>23</v>
       </c>
       <c r="C259" s="7" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="D259" s="8"/>
       <c r="E259" s="8"/>
       <c r="F259" s="10"/>
-      <c r="G259" s="8"/>
-      <c r="H259" s="14"/>
-      <c r="I259" s="27"/>
+      <c r="G259" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="H259" s="14" t="s">
+        <v>761</v>
+      </c>
+      <c r="I259" s="27" t="s">
+        <v>113</v>
+      </c>
       <c r="J259" s="3"/>
       <c r="K259" s="7"/>
       <c r="L259" s="7"/>
@@ -18026,22 +18044,16 @@
     <row r="260" spans="1:26" ht="14.25" customHeight="1">
       <c r="A260" s="6"/>
       <c r="B260" s="6" t="s">
-        <v>159</v>
+        <v>23</v>
       </c>
       <c r="C260" s="7" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="D260" s="8"/>
-      <c r="E260" s="8" t="s">
-        <v>157</v>
-      </c>
+      <c r="E260" s="8"/>
       <c r="F260" s="10"/>
-      <c r="G260" s="8" t="s">
-        <v>780</v>
-      </c>
-      <c r="H260" s="14" t="s">
-        <v>781</v>
-      </c>
+      <c r="G260" s="8"/>
+      <c r="H260" s="14"/>
       <c r="I260" s="27"/>
       <c r="J260" s="3"/>
       <c r="K260" s="7"/>
@@ -18062,7 +18074,7 @@
         <v>159</v>
       </c>
       <c r="C261" s="7" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="D261" s="8"/>
       <c r="E261" s="8" t="s">
@@ -18073,7 +18085,7 @@
         <v>780</v>
       </c>
       <c r="H261" s="14" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
       <c r="I261" s="27"/>
       <c r="J261" s="3"/>
@@ -18092,10 +18104,10 @@
     <row r="262" spans="1:26" ht="14.25" customHeight="1">
       <c r="A262" s="6"/>
       <c r="B262" s="6" t="s">
-        <v>23</v>
+        <v>159</v>
       </c>
       <c r="C262" s="7" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="D262" s="8"/>
       <c r="E262" s="8" t="s">
@@ -18106,7 +18118,7 @@
         <v>780</v>
       </c>
       <c r="H262" s="14" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="I262" s="27"/>
       <c r="J262" s="3"/>
@@ -18123,96 +18135,106 @@
       <c r="U262" s="7"/>
     </row>
     <row r="263" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A263" s="36" t="s">
+      <c r="A263" s="6"/>
+      <c r="B263" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C263" s="7" t="s">
+        <v>784</v>
+      </c>
+      <c r="D263" s="8"/>
+      <c r="E263" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="F263" s="10"/>
+      <c r="G263" s="8" t="s">
+        <v>780</v>
+      </c>
+      <c r="H263" s="14" t="s">
+        <v>785</v>
+      </c>
+      <c r="I263" s="27"/>
+      <c r="J263" s="3"/>
+      <c r="K263" s="7"/>
+      <c r="L263" s="7"/>
+      <c r="M263" s="7"/>
+      <c r="N263" s="7"/>
+      <c r="O263" s="7"/>
+      <c r="P263" s="7"/>
+      <c r="Q263" s="7"/>
+      <c r="R263" s="7"/>
+      <c r="S263" s="7"/>
+      <c r="T263" s="7"/>
+      <c r="U263" s="7"/>
+    </row>
+    <row r="264" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A264" s="36" t="s">
         <v>217</v>
       </c>
-      <c r="B263" s="29"/>
-      <c r="C263" s="37" t="s">
+      <c r="B264" s="29"/>
+      <c r="C264" s="37" t="s">
         <v>786</v>
       </c>
-      <c r="D263" s="38" t="s">
+      <c r="D264" s="38" t="s">
         <v>29</v>
       </c>
-      <c r="E263" s="38" t="s">
+      <c r="E264" s="38" t="s">
         <v>787</v>
       </c>
-      <c r="F263" s="38" t="s">
+      <c r="F264" s="38" t="s">
         <v>26</v>
       </c>
-      <c r="G263" s="38" t="s">
+      <c r="G264" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="H263" s="39" t="s">
+      <c r="H264" s="39" t="s">
         <v>788</v>
       </c>
-      <c r="I263" s="31"/>
-      <c r="J263" s="34"/>
-      <c r="K263" s="34"/>
-      <c r="L263" s="30"/>
-      <c r="M263" s="30"/>
-      <c r="N263" s="30"/>
-      <c r="O263" s="30"/>
-      <c r="P263" s="30"/>
-      <c r="Q263" s="30"/>
-      <c r="R263" s="30"/>
-      <c r="S263" s="30"/>
-      <c r="T263" s="30"/>
-      <c r="U263" s="30"/>
-      <c r="V263" s="35"/>
-      <c r="W263" s="35"/>
-      <c r="X263" s="35"/>
-      <c r="Y263" s="35"/>
-      <c r="Z263" s="35"/>
-    </row>
-    <row r="264" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A264" s="6" t="s">
+      <c r="I264" s="31"/>
+      <c r="J264" s="34"/>
+      <c r="K264" s="34"/>
+      <c r="L264" s="30"/>
+      <c r="M264" s="30"/>
+      <c r="N264" s="30"/>
+      <c r="O264" s="30"/>
+      <c r="P264" s="30"/>
+      <c r="Q264" s="30"/>
+      <c r="R264" s="30"/>
+      <c r="S264" s="30"/>
+      <c r="T264" s="30"/>
+      <c r="U264" s="30"/>
+      <c r="V264" s="35"/>
+      <c r="W264" s="35"/>
+      <c r="X264" s="35"/>
+      <c r="Y264" s="35"/>
+      <c r="Z264" s="35"/>
+    </row>
+    <row r="265" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A265" s="6" t="s">
         <v>789</v>
       </c>
-      <c r="B264" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C264" s="7" t="s">
+      <c r="B265" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C265" s="7" t="s">
         <v>228</v>
       </c>
-      <c r="D264" s="8"/>
-      <c r="E264" s="8" t="s">
+      <c r="D265" s="8"/>
+      <c r="E265" s="8" t="s">
         <v>196</v>
       </c>
-      <c r="F264" s="10"/>
-      <c r="G264" s="8" t="s">
+      <c r="F265" s="10"/>
+      <c r="G265" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="H264" s="14" t="s">
+      <c r="H265" s="14" t="s">
         <v>790</v>
       </c>
-      <c r="I264" s="8"/>
-      <c r="J264" s="3"/>
-      <c r="K264" s="3" t="s">
+      <c r="I265" s="8"/>
+      <c r="J265" s="3"/>
+      <c r="K265" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="L264" s="7"/>
-      <c r="M264" s="7"/>
-      <c r="N264" s="7"/>
-      <c r="O264" s="7"/>
-      <c r="P264" s="7"/>
-      <c r="Q264" s="7"/>
-      <c r="R264" s="7"/>
-      <c r="S264" s="7"/>
-      <c r="T264" s="7"/>
-      <c r="U264" s="7"/>
-    </row>
-    <row r="265" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A265" s="6"/>
-      <c r="B265" s="6"/>
-      <c r="C265" s="7"/>
-      <c r="D265" s="8"/>
-      <c r="E265" s="8"/>
-      <c r="F265" s="10"/>
-      <c r="G265" s="8"/>
-      <c r="H265" s="14"/>
-      <c r="I265" s="27"/>
-      <c r="J265" s="3"/>
-      <c r="K265" s="7"/>
       <c r="L265" s="7"/>
       <c r="M265" s="7"/>
       <c r="N265" s="7"/>
@@ -18233,8 +18255,8 @@
       <c r="F266" s="10"/>
       <c r="G266" s="8"/>
       <c r="H266" s="14"/>
-      <c r="I266" s="8"/>
-      <c r="J266" s="7"/>
+      <c r="I266" s="27"/>
+      <c r="J266" s="3"/>
       <c r="K266" s="7"/>
       <c r="L266" s="7"/>
       <c r="M266" s="7"/>
@@ -18461,8 +18483,8 @@
       <c r="D276" s="8"/>
       <c r="E276" s="8"/>
       <c r="F276" s="10"/>
-      <c r="G276" s="9"/>
-      <c r="H276" s="7"/>
+      <c r="G276" s="8"/>
+      <c r="H276" s="14"/>
       <c r="I276" s="8"/>
       <c r="J276" s="7"/>
       <c r="K276" s="7"/>
@@ -18477,14 +18499,14 @@
       <c r="T276" s="7"/>
       <c r="U276" s="7"/>
     </row>
-    <row r="277" spans="1:21" ht="14.4">
+    <row r="277" spans="1:21" ht="14.25" customHeight="1">
       <c r="A277" s="6"/>
       <c r="B277" s="6"/>
       <c r="C277" s="7"/>
       <c r="D277" s="8"/>
       <c r="E277" s="8"/>
       <c r="F277" s="10"/>
-      <c r="G277" s="8"/>
+      <c r="G277" s="9"/>
       <c r="H277" s="7"/>
       <c r="I277" s="8"/>
       <c r="J277" s="7"/>
@@ -18501,7 +18523,27 @@
       <c r="U277" s="7"/>
     </row>
     <row r="278" spans="1:21" ht="14.4">
-      <c r="B278" s="7"/>
+      <c r="A278" s="6"/>
+      <c r="B278" s="6"/>
+      <c r="C278" s="7"/>
+      <c r="D278" s="8"/>
+      <c r="E278" s="8"/>
+      <c r="F278" s="10"/>
+      <c r="G278" s="8"/>
+      <c r="H278" s="7"/>
+      <c r="I278" s="8"/>
+      <c r="J278" s="7"/>
+      <c r="K278" s="7"/>
+      <c r="L278" s="7"/>
+      <c r="M278" s="7"/>
+      <c r="N278" s="7"/>
+      <c r="O278" s="7"/>
+      <c r="P278" s="7"/>
+      <c r="Q278" s="7"/>
+      <c r="R278" s="7"/>
+      <c r="S278" s="7"/>
+      <c r="T278" s="7"/>
+      <c r="U278" s="7"/>
     </row>
     <row r="279" spans="1:21" ht="14.4">
       <c r="B279" s="7"/>
@@ -20812,6 +20854,9 @@
     </row>
     <row r="1048" spans="2:2" ht="14.4">
       <c r="B1048" s="7"/>
+    </row>
+    <row r="1049" spans="2:2" ht="14.4">
+      <c r="B1049" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -20824,11 +20869,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Z109"/>
+  <dimension ref="A1:Z110"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A85" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E66" sqref="E66"/>
+      <pane ySplit="4" topLeftCell="A60" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K65" sqref="K65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -22438,45 +22483,45 @@
     </row>
     <row r="65" spans="1:26" s="21" customFormat="1" ht="14.4">
       <c r="A65" s="20"/>
-      <c r="B65" s="24" t="s">
-        <v>23</v>
-      </c>
+      <c r="B65" s="24"/>
       <c r="C65" s="22"/>
       <c r="D65" s="22"/>
       <c r="E65" s="21" t="s">
-        <v>914</v>
+        <v>1007</v>
       </c>
       <c r="F65" s="7"/>
       <c r="G65" s="21" t="s">
-        <v>108</v>
+        <v>46</v>
       </c>
       <c r="H65" s="21" t="s">
-        <v>915</v>
+        <v>57</v>
       </c>
       <c r="I65" s="23" t="s">
         <v>26</v>
       </c>
       <c r="J65" s="23" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="K65" s="23" t="s">
-        <v>909</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="66" spans="1:26" s="21" customFormat="1" ht="14.4">
       <c r="A66" s="20"/>
-      <c r="B66" s="24"/>
+      <c r="B66" s="24" t="s">
+        <v>23</v>
+      </c>
       <c r="C66" s="22"/>
       <c r="D66" s="22"/>
       <c r="E66" s="21" t="s">
-        <v>917</v>
+        <v>914</v>
       </c>
       <c r="F66" s="7"/>
       <c r="G66" s="21" t="s">
         <v>108</v>
       </c>
       <c r="H66" s="21" t="s">
-        <v>406</v>
+        <v>915</v>
       </c>
       <c r="I66" s="23" t="s">
         <v>26</v>
@@ -22485,25 +22530,23 @@
         <v>27</v>
       </c>
       <c r="K66" s="23" t="s">
-        <v>918</v>
+        <v>909</v>
       </c>
     </row>
     <row r="67" spans="1:26" s="21" customFormat="1" ht="14.4">
       <c r="A67" s="20"/>
-      <c r="B67" s="24" t="s">
-        <v>23</v>
-      </c>
+      <c r="B67" s="24"/>
       <c r="C67" s="22"/>
       <c r="D67" s="22"/>
       <c r="E67" s="21" t="s">
-        <v>910</v>
+        <v>917</v>
       </c>
       <c r="F67" s="7"/>
       <c r="G67" s="21" t="s">
         <v>108</v>
       </c>
       <c r="H67" s="21" t="s">
-        <v>94</v>
+        <v>406</v>
       </c>
       <c r="I67" s="23" t="s">
         <v>26</v>
@@ -22512,187 +22555,178 @@
         <v>27</v>
       </c>
       <c r="K67" s="23" t="s">
+        <v>918</v>
+      </c>
+    </row>
+    <row r="68" spans="1:26" s="21" customFormat="1" ht="14.4">
+      <c r="A68" s="20"/>
+      <c r="B68" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="C68" s="22"/>
+      <c r="D68" s="22"/>
+      <c r="E68" s="21" t="s">
+        <v>910</v>
+      </c>
+      <c r="F68" s="7"/>
+      <c r="G68" s="21" t="s">
+        <v>108</v>
+      </c>
+      <c r="H68" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="I68" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="J68" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="K68" s="23" t="s">
         <v>911</v>
       </c>
     </row>
-    <row r="68" spans="1:26" ht="43.2">
-      <c r="A68" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B68" s="15" t="s">
+    <row r="69" spans="1:26" ht="43.2">
+      <c r="A69" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B69" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="E68" s="7" t="s">
+      <c r="E69" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="F68" s="18">
+      <c r="F69" s="18">
         <v>1</v>
       </c>
-      <c r="G68" s="18" t="s">
+      <c r="G69" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="H68" s="18" t="s">
+      <c r="H69" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="J68" s="17" t="s">
+      <c r="J69" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="K68" s="19" t="s">
+      <c r="K69" s="19" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="69" spans="1:26" s="21" customFormat="1" ht="14.4">
-      <c r="A69" s="20"/>
-      <c r="B69" s="20"/>
-      <c r="E69" s="7" t="s">
+    <row r="70" spans="1:26" s="21" customFormat="1" ht="14.4">
+      <c r="A70" s="20"/>
+      <c r="B70" s="20"/>
+      <c r="E70" s="7" t="s">
         <v>919</v>
       </c>
-      <c r="G69" s="21" t="s">
+      <c r="G70" s="21" t="s">
         <v>108</v>
       </c>
-      <c r="H69" s="21" t="s">
+      <c r="H70" s="21" t="s">
         <v>474</v>
       </c>
-      <c r="I69" s="23" t="s">
+      <c r="I70" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="J69" s="23" t="s">
+      <c r="J70" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="K69" s="23" t="s">
+      <c r="K70" s="23" t="s">
         <v>920</v>
       </c>
     </row>
-    <row r="70" spans="1:26" s="25" customFormat="1" ht="86.4">
-      <c r="A70" s="81"/>
-      <c r="B70" s="81"/>
-      <c r="E70" s="25" t="s">
-        <v>100</v>
-      </c>
-      <c r="F70" s="25">
-        <v>1</v>
-      </c>
-      <c r="G70" s="25" t="s">
-        <v>97</v>
-      </c>
-      <c r="H70" s="25" t="s">
-        <v>98</v>
-      </c>
-      <c r="I70" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="J70" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="K70" s="80" t="s">
-        <v>931</v>
-      </c>
-    </row>
-    <row r="71" spans="1:26" s="25" customFormat="1" ht="14.4">
+    <row r="71" spans="1:26" s="25" customFormat="1" ht="86.4">
       <c r="A71" s="81"/>
       <c r="B71" s="81"/>
-      <c r="E71" s="72" t="s">
+      <c r="E71" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="F71" s="25">
+        <v>1</v>
+      </c>
+      <c r="G71" s="25" t="s">
+        <v>97</v>
+      </c>
+      <c r="H71" s="25" t="s">
+        <v>98</v>
+      </c>
+      <c r="I71" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="J71" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="K71" s="80" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="72" spans="1:26" s="25" customFormat="1" ht="14.4">
+      <c r="A72" s="81"/>
+      <c r="B72" s="81"/>
+      <c r="E72" s="72" t="s">
         <v>921</v>
       </c>
-      <c r="G71" s="72" t="s">
+      <c r="G72" s="72" t="s">
         <v>108</v>
       </c>
-      <c r="H71" s="72" t="s">
+      <c r="H72" s="72" t="s">
         <v>474</v>
-      </c>
-      <c r="I71" s="80" t="s">
-        <v>26</v>
-      </c>
-      <c r="J71" s="80" t="s">
-        <v>27</v>
-      </c>
-      <c r="K71" s="23" t="s">
-        <v>922</v>
-      </c>
-    </row>
-    <row r="72" spans="1:26" s="25" customFormat="1" ht="28.8">
-      <c r="A72" s="81"/>
-      <c r="B72" s="81" t="s">
-        <v>23</v>
-      </c>
-      <c r="E72" s="25" t="s">
-        <v>912</v>
-      </c>
-      <c r="G72" s="25" t="s">
-        <v>108</v>
-      </c>
-      <c r="H72" s="25" t="s">
-        <v>128</v>
       </c>
       <c r="I72" s="80" t="s">
         <v>26</v>
       </c>
-      <c r="J72" s="19"/>
-      <c r="K72" s="80" t="s">
+      <c r="J72" s="80" t="s">
+        <v>27</v>
+      </c>
+      <c r="K72" s="23" t="s">
+        <v>922</v>
+      </c>
+    </row>
+    <row r="73" spans="1:26" s="25" customFormat="1" ht="28.8">
+      <c r="A73" s="81"/>
+      <c r="B73" s="81" t="s">
+        <v>23</v>
+      </c>
+      <c r="E73" s="25" t="s">
+        <v>912</v>
+      </c>
+      <c r="G73" s="25" t="s">
+        <v>108</v>
+      </c>
+      <c r="H73" s="25" t="s">
+        <v>128</v>
+      </c>
+      <c r="I73" s="80" t="s">
+        <v>26</v>
+      </c>
+      <c r="J73" s="19"/>
+      <c r="K73" s="80" t="s">
         <v>913</v>
       </c>
-    </row>
-    <row r="73" spans="1:26" s="21" customFormat="1" ht="14.25" customHeight="1">
-      <c r="C73" s="28"/>
-      <c r="D73" s="28"/>
-      <c r="E73" s="7" t="s">
-        <v>811</v>
-      </c>
-      <c r="F73" s="7"/>
-      <c r="G73" s="70" t="s">
-        <v>29</v>
-      </c>
-      <c r="H73" s="70" t="s">
-        <v>226</v>
-      </c>
-      <c r="I73" s="70" t="s">
-        <v>34</v>
-      </c>
-      <c r="J73" s="70" t="s">
-        <v>27</v>
-      </c>
-      <c r="K73" s="57" t="s">
-        <v>812</v>
-      </c>
-      <c r="L73" s="70" t="s">
-        <v>813</v>
-      </c>
-      <c r="M73" s="3"/>
-      <c r="N73" s="7"/>
-      <c r="O73" s="7"/>
-      <c r="P73" s="7"/>
-      <c r="Q73" s="7"/>
-      <c r="R73" s="7"/>
-      <c r="S73" s="7"/>
-      <c r="T73" s="7"/>
-      <c r="U73" s="7"/>
-      <c r="V73" s="7"/>
-      <c r="W73" s="7"/>
-      <c r="X73" s="7"/>
     </row>
     <row r="74" spans="1:26" s="21" customFormat="1" ht="14.25" customHeight="1">
       <c r="C74" s="28"/>
       <c r="D74" s="28"/>
-      <c r="E74" s="25" t="s">
-        <v>995</v>
+      <c r="E74" s="7" t="s">
+        <v>811</v>
       </c>
       <c r="F74" s="7"/>
       <c r="G74" s="70" t="s">
-        <v>108</v>
+        <v>29</v>
       </c>
       <c r="H74" s="70" t="s">
-        <v>996</v>
+        <v>226</v>
       </c>
       <c r="I74" s="70" t="s">
         <v>34</v>
       </c>
       <c r="J74" s="70" t="s">
-        <v>30</v>
-      </c>
-      <c r="K74" s="70" t="s">
-        <v>997</v>
-      </c>
-      <c r="L74" s="70"/>
+        <v>27</v>
+      </c>
+      <c r="K74" s="57" t="s">
+        <v>812</v>
+      </c>
+      <c r="L74" s="70" t="s">
+        <v>813</v>
+      </c>
       <c r="M74" s="3"/>
       <c r="N74" s="7"/>
       <c r="O74" s="7"/>
@@ -22706,178 +22740,188 @@
       <c r="W74" s="7"/>
       <c r="X74" s="7"/>
     </row>
-    <row r="75" spans="1:26" ht="14.4">
-      <c r="A75" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B75" s="15" t="s">
+    <row r="75" spans="1:26" s="21" customFormat="1" ht="14.25" customHeight="1">
+      <c r="C75" s="28"/>
+      <c r="D75" s="28"/>
+      <c r="E75" s="25" t="s">
+        <v>995</v>
+      </c>
+      <c r="F75" s="7"/>
+      <c r="G75" s="70" t="s">
+        <v>108</v>
+      </c>
+      <c r="H75" s="70" t="s">
+        <v>996</v>
+      </c>
+      <c r="I75" s="70" t="s">
+        <v>34</v>
+      </c>
+      <c r="J75" s="70" t="s">
+        <v>30</v>
+      </c>
+      <c r="K75" s="70" t="s">
+        <v>997</v>
+      </c>
+      <c r="L75" s="70"/>
+      <c r="M75" s="3"/>
+      <c r="N75" s="7"/>
+      <c r="O75" s="7"/>
+      <c r="P75" s="7"/>
+      <c r="Q75" s="7"/>
+      <c r="R75" s="7"/>
+      <c r="S75" s="7"/>
+      <c r="T75" s="7"/>
+      <c r="U75" s="7"/>
+      <c r="V75" s="7"/>
+      <c r="W75" s="7"/>
+      <c r="X75" s="7"/>
+    </row>
+    <row r="76" spans="1:26" ht="14.4">
+      <c r="A76" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B76" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="E75" s="7" t="s">
+      <c r="E76" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="F75" s="7">
+      <c r="F76" s="7">
         <v>-1</v>
       </c>
-      <c r="G75" s="7"/>
-      <c r="H75" s="7"/>
-    </row>
-    <row r="76" spans="1:26" s="21" customFormat="1" ht="14.4">
-      <c r="A76" s="20"/>
-      <c r="B76" s="20"/>
-      <c r="E76" s="25" t="s">
+      <c r="G76" s="7"/>
+      <c r="H76" s="7"/>
+    </row>
+    <row r="77" spans="1:26" s="21" customFormat="1" ht="14.4">
+      <c r="A77" s="20"/>
+      <c r="B77" s="20"/>
+      <c r="E77" s="25" t="s">
         <v>980</v>
       </c>
-      <c r="F76" s="7" t="s">
+      <c r="F77" s="7" t="s">
         <v>981</v>
       </c>
-      <c r="G76" s="25" t="s">
+      <c r="G77" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="H76" s="7"/>
-      <c r="K76" s="21" t="s">
+      <c r="H77" s="7"/>
+      <c r="K77" s="21" t="s">
         <v>982</v>
       </c>
     </row>
-    <row r="77" spans="1:26" ht="14.4">
-      <c r="A77" s="15"/>
-      <c r="B77" s="15"/>
-      <c r="C77" s="7" t="s">
+    <row r="78" spans="1:26" ht="14.4">
+      <c r="A78" s="15"/>
+      <c r="B78" s="15"/>
+      <c r="C78" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="D77" s="7" t="s">
+      <c r="D78" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="E77" s="7" t="s">
+      <c r="E78" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="F77" s="7">
+      <c r="F78" s="7">
         <v>0.6</v>
       </c>
-      <c r="G77" s="7" t="s">
+      <c r="G78" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="H77" s="7" t="s">
+      <c r="H78" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="I77" s="7" t="s">
+      <c r="I78" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="J77" s="7" t="s">
+      <c r="J78" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="K77" s="7" t="s">
+      <c r="K78" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="L77" s="7"/>
-      <c r="M77" s="7"/>
-      <c r="N77" s="7"/>
-      <c r="O77" s="7"/>
-      <c r="P77" s="7"/>
-      <c r="Q77" s="7"/>
-      <c r="R77" s="7"/>
-      <c r="S77" s="7"/>
-      <c r="T77" s="7"/>
-      <c r="U77" s="7"/>
-      <c r="V77" s="7"/>
-      <c r="W77" s="7"/>
-      <c r="X77" s="7"/>
-      <c r="Y77" s="7"/>
-      <c r="Z77" s="7"/>
-    </row>
-    <row r="78" spans="1:26" ht="14.4">
-      <c r="A78" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B78" s="15" t="s">
+      <c r="L78" s="7"/>
+      <c r="M78" s="7"/>
+      <c r="N78" s="7"/>
+      <c r="O78" s="7"/>
+      <c r="P78" s="7"/>
+      <c r="Q78" s="7"/>
+      <c r="R78" s="7"/>
+      <c r="S78" s="7"/>
+      <c r="T78" s="7"/>
+      <c r="U78" s="7"/>
+      <c r="V78" s="7"/>
+      <c r="W78" s="7"/>
+      <c r="X78" s="7"/>
+      <c r="Y78" s="7"/>
+      <c r="Z78" s="7"/>
+    </row>
+    <row r="79" spans="1:26" ht="14.4">
+      <c r="A79" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B79" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="E78" s="7" t="s">
+      <c r="E79" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="F78" s="7">
+      <c r="F79" s="7">
         <v>1739.927555</v>
       </c>
-      <c r="G78" s="7"/>
-      <c r="H78" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="K78" s="3" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="79" spans="1:26" s="21" customFormat="1" ht="14.4">
-      <c r="A79" s="20"/>
-      <c r="B79" s="20"/>
-      <c r="E79" s="7" t="s">
-        <v>957</v>
-      </c>
-      <c r="F79" s="7"/>
-      <c r="G79" s="7" t="s">
-        <v>108</v>
-      </c>
+      <c r="G79" s="7"/>
       <c r="H79" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="I79" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="J79" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="K79" s="3"/>
+      <c r="K79" s="3" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="80" spans="1:26" s="21" customFormat="1" ht="14.4">
       <c r="A80" s="20"/>
       <c r="B80" s="20"/>
       <c r="E80" s="7" t="s">
-        <v>496</v>
+        <v>957</v>
       </c>
       <c r="F80" s="7"/>
-      <c r="G80" s="7"/>
-      <c r="H80" s="7"/>
-      <c r="K80" s="3" t="s">
-        <v>939</v>
-      </c>
+      <c r="G80" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="H80" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="I80" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="J80" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="K80" s="3"/>
     </row>
     <row r="81" spans="1:12" s="21" customFormat="1" ht="14.4">
       <c r="A81" s="20"/>
       <c r="B81" s="20"/>
       <c r="E81" s="7" t="s">
-        <v>852</v>
+        <v>496</v>
       </c>
       <c r="F81" s="7"/>
-      <c r="G81" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="H81" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="I81" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="J81" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="K81" s="21" t="s">
-        <v>854</v>
-      </c>
-      <c r="L81" s="3" t="s">
-        <v>853</v>
+      <c r="G81" s="7"/>
+      <c r="H81" s="7"/>
+      <c r="K81" s="3" t="s">
+        <v>939</v>
       </c>
     </row>
     <row r="82" spans="1:12" s="21" customFormat="1" ht="14.4">
       <c r="A82" s="20"/>
       <c r="B82" s="20"/>
       <c r="E82" s="7" t="s">
-        <v>916</v>
+        <v>852</v>
       </c>
       <c r="F82" s="7"/>
       <c r="G82" s="7" t="s">
         <v>29</v>
       </c>
       <c r="H82" s="7" t="s">
-        <v>128</v>
+        <v>73</v>
       </c>
       <c r="I82" s="21" t="s">
         <v>34</v>
@@ -22886,42 +22930,36 @@
         <v>30</v>
       </c>
       <c r="K82" s="21" t="s">
-        <v>901</v>
+        <v>854</v>
       </c>
       <c r="L82" s="3" t="s">
         <v>853</v>
       </c>
     </row>
-    <row r="83" spans="1:12" ht="14.4">
-      <c r="A83" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B83" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="C83" s="3" t="s">
-        <v>24</v>
-      </c>
+    <row r="83" spans="1:12" s="21" customFormat="1" ht="14.4">
+      <c r="A83" s="20"/>
+      <c r="B83" s="20"/>
       <c r="E83" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="F83" s="7">
-        <v>1</v>
-      </c>
+        <v>916</v>
+      </c>
+      <c r="F83" s="7"/>
       <c r="G83" s="7" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="H83" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="I83" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="I83" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="J83" s="3" t="s">
+      <c r="J83" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="K83" s="3" t="s">
-        <v>116</v>
+      <c r="K83" s="21" t="s">
+        <v>901</v>
+      </c>
+      <c r="L83" s="3" t="s">
+        <v>853</v>
       </c>
     </row>
     <row r="84" spans="1:12" ht="14.4">
@@ -22931,14 +22969,30 @@
       <c r="B84" s="15" t="s">
         <v>24</v>
       </c>
+      <c r="C84" s="3" t="s">
+        <v>24</v>
+      </c>
       <c r="E84" s="7" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="F84" s="7">
-        <v>553659</v>
-      </c>
-      <c r="G84" s="7"/>
-      <c r="H84" s="7"/>
+        <v>1</v>
+      </c>
+      <c r="G84" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="H84" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="I84" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="J84" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="K84" s="3" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="85" spans="1:12" ht="14.4">
       <c r="A85" s="15" t="s">
@@ -22948,10 +23002,10 @@
         <v>24</v>
       </c>
       <c r="E85" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F85" s="7">
-        <v>4891208</v>
+        <v>553659</v>
       </c>
       <c r="G85" s="7"/>
       <c r="H85" s="7"/>
@@ -22963,106 +23017,89 @@
       <c r="B86" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="C86" s="3" t="s">
+      <c r="E86" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="F86" s="7">
+        <v>4891208</v>
+      </c>
+      <c r="G86" s="7"/>
+      <c r="H86" s="7"/>
+    </row>
+    <row r="87" spans="1:12" ht="14.4">
+      <c r="A87" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B87" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="E86" s="7" t="s">
+      <c r="C87" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E87" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="F86" s="7">
+      <c r="F87" s="7">
         <v>1</v>
       </c>
-      <c r="G86" s="7" t="s">
+      <c r="G87" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="H86" s="7" t="s">
+      <c r="H87" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="I86" s="3" t="s">
+      <c r="I87" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="J86" s="3" t="s">
+      <c r="J87" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="K86" s="3" t="s">
+      <c r="K87" s="3" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="87" spans="1:12" s="21" customFormat="1" ht="14.4">
-      <c r="A87" s="20"/>
-      <c r="B87" s="20"/>
-      <c r="C87" s="3"/>
-      <c r="E87" s="7" t="s">
+    <row r="88" spans="1:12" s="21" customFormat="1" ht="14.4">
+      <c r="A88" s="20"/>
+      <c r="B88" s="20"/>
+      <c r="C88" s="3"/>
+      <c r="E88" s="7" t="s">
         <v>932</v>
       </c>
-      <c r="F87" s="7"/>
-      <c r="G87" s="7"/>
-      <c r="H87" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="I87" s="3"/>
-      <c r="J87" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="K87" s="3" t="s">
-        <v>934</v>
-      </c>
-    </row>
-    <row r="88" spans="1:12" s="21" customFormat="1" ht="14.4">
-      <c r="A88" s="20" t="s">
-        <v>835</v>
-      </c>
-      <c r="B88" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="C88" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="D88" s="21" t="s">
-        <v>65</v>
-      </c>
-      <c r="E88" s="7" t="s">
-        <v>834</v>
-      </c>
-      <c r="F88" s="7">
-        <v>5</v>
-      </c>
-      <c r="G88" s="7" t="s">
-        <v>108</v>
-      </c>
+      <c r="F88" s="7"/>
+      <c r="G88" s="7"/>
       <c r="H88" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="I88" s="3" t="s">
-        <v>26</v>
-      </c>
+      <c r="I88" s="3"/>
       <c r="J88" s="3" t="s">
         <v>27</v>
       </c>
       <c r="K88" s="3" t="s">
-        <v>836</v>
-      </c>
-      <c r="L88" s="23" t="s">
+        <v>934</v>
+      </c>
+    </row>
+    <row r="89" spans="1:12" s="21" customFormat="1" ht="14.4">
+      <c r="A89" s="20" t="s">
+        <v>835</v>
+      </c>
+      <c r="B89" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="C89" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D89" s="21" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="89" spans="1:12" ht="14.4">
-      <c r="A89" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B89" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="D89" s="3" t="s">
-        <v>126</v>
-      </c>
       <c r="E89" s="7" t="s">
-        <v>127</v>
+        <v>834</v>
       </c>
       <c r="F89" s="7">
-        <v>0</v>
-      </c>
-      <c r="G89" s="7"/>
+        <v>5</v>
+      </c>
+      <c r="G89" s="7" t="s">
+        <v>108</v>
+      </c>
       <c r="H89" s="7" t="s">
         <v>128</v>
       </c>
@@ -23073,25 +23110,40 @@
         <v>27</v>
       </c>
       <c r="K89" s="3" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="90" spans="1:12" s="21" customFormat="1" ht="14.4">
-      <c r="A90" s="20"/>
-      <c r="B90" s="20"/>
-      <c r="D90" s="3"/>
+        <v>836</v>
+      </c>
+      <c r="L89" s="23" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12" ht="14.4">
+      <c r="A90" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B90" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D90" s="3" t="s">
+        <v>126</v>
+      </c>
       <c r="E90" s="7" t="s">
-        <v>933</v>
-      </c>
-      <c r="F90" s="7"/>
+        <v>127</v>
+      </c>
+      <c r="F90" s="7">
+        <v>0</v>
+      </c>
       <c r="G90" s="7"/>
       <c r="H90" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="I90" s="3"/>
-      <c r="J90" s="3"/>
+      <c r="I90" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J90" s="3" t="s">
+        <v>27</v>
+      </c>
       <c r="K90" s="3" t="s">
-        <v>935</v>
+        <v>129</v>
       </c>
     </row>
     <row r="91" spans="1:12" s="21" customFormat="1" ht="14.4">
@@ -23099,7 +23151,7 @@
       <c r="B91" s="20"/>
       <c r="D91" s="3"/>
       <c r="E91" s="7" t="s">
-        <v>936</v>
+        <v>933</v>
       </c>
       <c r="F91" s="7"/>
       <c r="G91" s="7"/>
@@ -23109,53 +23161,46 @@
       <c r="I91" s="3"/>
       <c r="J91" s="3"/>
       <c r="K91" s="3" t="s">
+        <v>935</v>
+      </c>
+    </row>
+    <row r="92" spans="1:12" s="21" customFormat="1" ht="14.4">
+      <c r="A92" s="20"/>
+      <c r="B92" s="20"/>
+      <c r="D92" s="3"/>
+      <c r="E92" s="7" t="s">
+        <v>936</v>
+      </c>
+      <c r="F92" s="7"/>
+      <c r="G92" s="7"/>
+      <c r="H92" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="I92" s="3"/>
+      <c r="J92" s="3"/>
+      <c r="K92" s="3" t="s">
         <v>937</v>
       </c>
     </row>
-    <row r="92" spans="1:12" ht="14.4">
-      <c r="A92" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B92" s="15"/>
-      <c r="E92" s="7" t="s">
+    <row r="93" spans="1:12" ht="14.4">
+      <c r="A93" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B93" s="15"/>
+      <c r="E93" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="F92" s="7">
+      <c r="F93" s="7">
         <v>6772</v>
       </c>
-      <c r="G92" s="7"/>
-      <c r="H92" s="7"/>
-    </row>
-    <row r="93" spans="1:12" s="21" customFormat="1" ht="14.4">
-      <c r="A93" s="20"/>
-      <c r="B93" s="20"/>
-      <c r="E93" s="7" t="s">
-        <v>950</v>
-      </c>
-      <c r="F93" s="7">
-        <v>5</v>
-      </c>
-      <c r="G93" s="58" t="s">
-        <v>108</v>
-      </c>
-      <c r="H93" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="I93" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="J93" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="K93" s="23" t="s">
-        <v>951</v>
-      </c>
+      <c r="G93" s="7"/>
+      <c r="H93" s="7"/>
     </row>
     <row r="94" spans="1:12" s="21" customFormat="1" ht="14.4">
       <c r="A94" s="20"/>
       <c r="B94" s="20"/>
-      <c r="E94" s="58" t="s">
-        <v>952</v>
+      <c r="E94" s="7" t="s">
+        <v>950</v>
       </c>
       <c r="F94" s="7">
         <v>5</v>
@@ -23173,14 +23218,14 @@
         <v>30</v>
       </c>
       <c r="K94" s="23" t="s">
-        <v>953</v>
+        <v>951</v>
       </c>
     </row>
     <row r="95" spans="1:12" s="21" customFormat="1" ht="14.4">
       <c r="A95" s="20"/>
       <c r="B95" s="20"/>
       <c r="E95" s="58" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
       <c r="F95" s="7">
         <v>5</v>
@@ -23198,82 +23243,87 @@
         <v>30</v>
       </c>
       <c r="K95" s="23" t="s">
-        <v>955</v>
+        <v>953</v>
       </c>
     </row>
     <row r="96" spans="1:12" s="21" customFormat="1" ht="14.4">
       <c r="A96" s="20"/>
       <c r="B96" s="20"/>
-      <c r="E96" s="7" t="s">
-        <v>841</v>
+      <c r="E96" s="58" t="s">
+        <v>954</v>
       </c>
       <c r="F96" s="7">
-        <v>1</v>
-      </c>
-      <c r="G96" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G96" s="58" t="s">
         <v>108</v>
       </c>
       <c r="H96" s="7" t="s">
-        <v>842</v>
-      </c>
-      <c r="I96" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="J96" s="23" t="s">
-        <v>843</v>
+        <v>128</v>
+      </c>
+      <c r="I96" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="J96" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="K96" s="23" t="s">
+        <v>955</v>
       </c>
     </row>
     <row r="97" spans="1:12" s="21" customFormat="1" ht="14.4">
       <c r="A97" s="20"/>
       <c r="B97" s="20"/>
       <c r="E97" s="7" t="s">
-        <v>976</v>
-      </c>
-      <c r="F97" s="7"/>
+        <v>841</v>
+      </c>
+      <c r="F97" s="7">
+        <v>1</v>
+      </c>
       <c r="G97" s="7" t="s">
         <v>108</v>
       </c>
       <c r="H97" s="7" t="s">
-        <v>63</v>
+        <v>842</v>
       </c>
       <c r="I97" s="23" t="s">
         <v>26</v>
       </c>
       <c r="J97" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="K97" s="23" t="s">
-        <v>977</v>
-      </c>
-      <c r="L97" s="23" t="s">
-        <v>975</v>
+        <v>843</v>
       </c>
     </row>
     <row r="98" spans="1:12" s="21" customFormat="1" ht="14.4">
       <c r="A98" s="20"/>
       <c r="B98" s="20"/>
       <c r="E98" s="7" t="s">
-        <v>948</v>
+        <v>976</v>
       </c>
       <c r="F98" s="7"/>
       <c r="G98" s="7" t="s">
         <v>108</v>
       </c>
       <c r="H98" s="7" t="s">
-        <v>625</v>
-      </c>
-      <c r="I98" s="23"/>
-      <c r="J98" s="23"/>
+        <v>63</v>
+      </c>
+      <c r="I98" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="J98" s="23" t="s">
+        <v>27</v>
+      </c>
       <c r="K98" s="23" t="s">
-        <v>978</v>
-      </c>
-      <c r="L98" s="23"/>
+        <v>977</v>
+      </c>
+      <c r="L98" s="23" t="s">
+        <v>975</v>
+      </c>
     </row>
     <row r="99" spans="1:12" s="21" customFormat="1" ht="14.4">
       <c r="A99" s="20"/>
       <c r="B99" s="20"/>
       <c r="E99" s="7" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="F99" s="7"/>
       <c r="G99" s="7" t="s">
@@ -23285,69 +23335,66 @@
       <c r="I99" s="23"/>
       <c r="J99" s="23"/>
       <c r="K99" s="23" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
       <c r="L99" s="23"/>
     </row>
     <row r="100" spans="1:12" s="21" customFormat="1" ht="14.4">
       <c r="A100" s="20"/>
       <c r="B100" s="20"/>
-      <c r="D100" s="57" t="s">
-        <v>942</v>
-      </c>
       <c r="E100" s="7" t="s">
-        <v>968</v>
+        <v>949</v>
       </c>
       <c r="F100" s="7"/>
-      <c r="G100" s="58" t="s">
+      <c r="G100" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="H100" s="58" t="s">
-        <v>84</v>
-      </c>
-      <c r="I100" s="23" t="s">
-        <v>945</v>
-      </c>
-      <c r="J100" s="23" t="s">
-        <v>945</v>
-      </c>
+      <c r="H100" s="7" t="s">
+        <v>625</v>
+      </c>
+      <c r="I100" s="23"/>
+      <c r="J100" s="23"/>
       <c r="K100" s="23" t="s">
-        <v>969</v>
+        <v>979</v>
       </c>
       <c r="L100" s="23"/>
     </row>
     <row r="101" spans="1:12" s="21" customFormat="1" ht="14.4">
       <c r="A101" s="20"/>
       <c r="B101" s="20"/>
+      <c r="D101" s="57" t="s">
+        <v>942</v>
+      </c>
       <c r="E101" s="7" t="s">
-        <v>840</v>
-      </c>
-      <c r="F101" s="7">
-        <v>10</v>
-      </c>
-      <c r="G101" s="7" t="s">
+        <v>968</v>
+      </c>
+      <c r="F101" s="7"/>
+      <c r="G101" s="58" t="s">
         <v>108</v>
       </c>
-      <c r="H101" s="7" t="s">
-        <v>625</v>
+      <c r="H101" s="58" t="s">
+        <v>84</v>
       </c>
       <c r="I101" s="23" t="s">
-        <v>26</v>
+        <v>945</v>
       </c>
       <c r="J101" s="23" t="s">
-        <v>27</v>
+        <v>945</v>
       </c>
       <c r="K101" s="23" t="s">
-        <v>846</v>
-      </c>
+        <v>969</v>
+      </c>
+      <c r="L101" s="23"/>
     </row>
     <row r="102" spans="1:12" s="21" customFormat="1" ht="14.4">
       <c r="A102" s="20"/>
       <c r="B102" s="20"/>
       <c r="E102" s="7" t="s">
-        <v>958</v>
-      </c>
-      <c r="F102" s="7"/>
+        <v>840</v>
+      </c>
+      <c r="F102" s="7">
+        <v>10</v>
+      </c>
       <c r="G102" s="7" t="s">
         <v>108</v>
       </c>
@@ -23355,20 +23402,20 @@
         <v>625</v>
       </c>
       <c r="I102" s="23" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="J102" s="23" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="K102" s="23" t="s">
-        <v>959</v>
+        <v>846</v>
       </c>
     </row>
     <row r="103" spans="1:12" s="21" customFormat="1" ht="14.4">
       <c r="A103" s="20"/>
       <c r="B103" s="20"/>
       <c r="E103" s="7" t="s">
-        <v>972</v>
+        <v>958</v>
       </c>
       <c r="F103" s="7"/>
       <c r="G103" s="7" t="s">
@@ -23377,70 +23424,65 @@
       <c r="H103" s="7" t="s">
         <v>625</v>
       </c>
-      <c r="I103" s="23"/>
+      <c r="I103" s="23" t="s">
+        <v>34</v>
+      </c>
       <c r="J103" s="23" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="K103" s="23" t="s">
-        <v>973</v>
-      </c>
-      <c r="L103" s="23" t="s">
-        <v>974</v>
+        <v>959</v>
       </c>
     </row>
     <row r="104" spans="1:12" s="21" customFormat="1" ht="14.4">
       <c r="A104" s="20"/>
       <c r="B104" s="20"/>
       <c r="E104" s="7" t="s">
-        <v>509</v>
+        <v>972</v>
       </c>
       <c r="F104" s="7"/>
-      <c r="G104" s="7"/>
+      <c r="G104" s="7" t="s">
+        <v>108</v>
+      </c>
       <c r="H104" s="7" t="s">
-        <v>510</v>
+        <v>625</v>
       </c>
       <c r="I104" s="23"/>
-      <c r="J104" s="23"/>
+      <c r="J104" s="23" t="s">
+        <v>27</v>
+      </c>
       <c r="K104" s="23" t="s">
-        <v>941</v>
+        <v>973</v>
+      </c>
+      <c r="L104" s="23" t="s">
+        <v>974</v>
       </c>
     </row>
     <row r="105" spans="1:12" s="21" customFormat="1" ht="14.4">
       <c r="A105" s="20"/>
       <c r="B105" s="20"/>
-      <c r="D105" s="57" t="s">
-        <v>25</v>
-      </c>
       <c r="E105" s="7" t="s">
-        <v>795</v>
+        <v>509</v>
       </c>
       <c r="F105" s="7"/>
-      <c r="G105" s="58" t="s">
-        <v>29</v>
-      </c>
+      <c r="G105" s="7"/>
       <c r="H105" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="I105" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="J105" s="23" t="s">
-        <v>27</v>
-      </c>
+        <v>510</v>
+      </c>
+      <c r="I105" s="23"/>
+      <c r="J105" s="23"/>
       <c r="K105" s="23" t="s">
-        <v>796</v>
+        <v>941</v>
       </c>
     </row>
     <row r="106" spans="1:12" s="21" customFormat="1" ht="14.4">
-      <c r="A106" s="20" t="s">
-        <v>23</v>
-      </c>
+      <c r="A106" s="20"/>
       <c r="B106" s="20"/>
       <c r="D106" s="57" t="s">
         <v>25</v>
       </c>
       <c r="E106" s="7" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="F106" s="7"/>
       <c r="G106" s="58" t="s">
@@ -23456,39 +23498,35 @@
         <v>27</v>
       </c>
       <c r="K106" s="23" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="107" spans="1:12" s="21" customFormat="1" ht="14.4">
+      <c r="A107" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="B107" s="20"/>
+      <c r="D107" s="57" t="s">
+        <v>25</v>
+      </c>
+      <c r="E107" s="7" t="s">
+        <v>797</v>
+      </c>
+      <c r="F107" s="7"/>
+      <c r="G107" s="58" t="s">
+        <v>29</v>
+      </c>
+      <c r="H107" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="I107" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="J107" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="K107" s="23" t="s">
         <v>798</v>
-      </c>
-    </row>
-    <row r="107" spans="1:12" ht="14.4">
-      <c r="A107" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B107" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="D107" s="17" t="s">
-        <v>132</v>
-      </c>
-      <c r="E107" s="18" t="s">
-        <v>134</v>
-      </c>
-      <c r="F107" s="18">
-        <v>1500</v>
-      </c>
-      <c r="G107" s="18" t="s">
-        <v>108</v>
-      </c>
-      <c r="H107" s="18" t="s">
-        <v>84</v>
-      </c>
-      <c r="I107" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="J107" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="K107" s="17" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="108" spans="1:12" ht="14.4">
@@ -23501,16 +23539,16 @@
       <c r="D108" s="17" t="s">
         <v>132</v>
       </c>
-      <c r="E108" s="17" t="s">
-        <v>139</v>
-      </c>
-      <c r="F108" s="17">
+      <c r="E108" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="F108" s="18">
         <v>1500</v>
       </c>
       <c r="G108" s="18" t="s">
         <v>108</v>
       </c>
-      <c r="H108" s="17" t="s">
+      <c r="H108" s="18" t="s">
         <v>84</v>
       </c>
       <c r="I108" s="17" t="s">
@@ -23520,7 +23558,7 @@
         <v>30</v>
       </c>
       <c r="K108" s="17" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="109" spans="1:12" ht="14.4">
@@ -23534,7 +23572,7 @@
         <v>132</v>
       </c>
       <c r="E109" s="17" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="F109" s="17">
         <v>1500</v>
@@ -23552,11 +23590,43 @@
         <v>30</v>
       </c>
       <c r="K109" s="17" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="110" spans="1:12" ht="14.4">
+      <c r="A110" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B110" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="D110" s="17" t="s">
+        <v>132</v>
+      </c>
+      <c r="E110" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="F110" s="17">
+        <v>1500</v>
+      </c>
+      <c r="G110" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="H110" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="I110" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="J110" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="K110" s="17" t="s">
         <v>143</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B64:B67">
+  <conditionalFormatting sqref="B64:B68">
     <cfRule type="notContainsBlanks" dxfId="0" priority="1">
       <formula>LEN(TRIM(B64))&gt;0</formula>
     </cfRule>

</xml_diff>

<commit_message>
Save updates to CW3MdigitalHandbook.docx
</commit_message>
<xml_diff>
--- a/DataCW3M/CW3MdigitalHandbook/CW3MdataDictionary.xlsx
+++ b/DataCW3M/CW3MdigitalHandbook/CW3MdataDictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\CW3MdigitalHandbook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22362470-F3FC-4F58-8B76-9AF46BEABCEA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E27EF952-4DFF-4E68-8D2A-038A3E26DC90}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-7425" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-7425" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Necessary input data" sheetId="7" r:id="rId1"/>
@@ -3124,13 +3124,13 @@
     <t>REACH_NDX</t>
   </si>
   <si>
-    <t>index into the internal C++ reach array for this reach; set by ReachInit() called by FlowModel::Init()</t>
-  </si>
-  <si>
     <t>WETL_ID</t>
   </si>
   <si>
     <t>wetland ID</t>
+  </si>
+  <si>
+    <t>index into the internal C++ reach array for this reach; set by ReachInit() when ReachInit90 is called by FlowModel::Init()</t>
   </si>
 </sst>
 </file>
@@ -9095,8 +9095,8 @@
   </sheetPr>
   <dimension ref="A1:Z1049"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A132" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
@@ -16826,7 +16826,7 @@
       <c r="A225" s="28"/>
       <c r="B225" s="28"/>
       <c r="C225" s="7" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="D225" s="10" t="s">
         <v>46</v>
@@ -16837,7 +16837,7 @@
         <v>30</v>
       </c>
       <c r="H225" s="25" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="I225" s="27"/>
       <c r="J225" s="3"/>
@@ -20871,8 +20871,8 @@
   </sheetPr>
   <dimension ref="A1:Z110"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A60" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="K65" sqref="K65"/>
     </sheetView>
   </sheetViews>
@@ -22503,7 +22503,7 @@
         <v>30</v>
       </c>
       <c r="K65" s="23" t="s">
-        <v>1008</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="66" spans="1:26" s="21" customFormat="1" ht="14.4">

</xml_diff>

<commit_message>
WORK-IN-PROGRESS Flow.cpp, .h - Add m_snowpackFlag to class HRU. Add CheckHRUwaterBalance(). Add IDU attribute H2O_MELT. Extensive changes to InitHRULayers(), including adding initialization of IDU attributes SNOWPACK, WETNESS, and SM_DAY. HBV.cpp - Add a comment.
</commit_message>
<xml_diff>
--- a/DataCW3M/CW3MdigitalHandbook/CW3MdataDictionary.xlsx
+++ b/DataCW3M/CW3MdigitalHandbook/CW3MdataDictionary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\CW3MdigitalHandbook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CE2E32A-A27E-40CE-B282-583B227C10D4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{959D3744-8332-4D12-BBCA-5E1292BADB1B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-7425" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-7425" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Necessary input data" sheetId="7" r:id="rId1"/>
@@ -96,7 +96,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3052" uniqueCount="1026">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3054" uniqueCount="1026">
   <si>
     <t>LULC_A</t>
   </si>
@@ -9145,9 +9145,9 @@
   </sheetPr>
   <dimension ref="A1:Z1049"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A204" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E178" sqref="E178"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A132" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D164" sqref="D164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -9403,7 +9403,9 @@
       <c r="C8" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="D8" s="8"/>
+      <c r="D8" s="8" t="s">
+        <v>29</v>
+      </c>
       <c r="E8" s="8" t="s">
         <v>152</v>
       </c>
@@ -14790,7 +14792,9 @@
       <c r="C164" s="30" t="s">
         <v>602</v>
       </c>
-      <c r="D164" s="31"/>
+      <c r="D164" s="31" t="s">
+        <v>29</v>
+      </c>
       <c r="E164" s="31" t="s">
         <v>172</v>
       </c>
@@ -20923,7 +20927,7 @@
   </sheetPr>
   <dimension ref="A1:Z117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="H116" sqref="H116"/>
     </sheetView>

</xml_diff>

<commit_message>
This log entry applies to the previous version as well. Flow.cpp, .h - Add HRU attribute HBVCALIB. Add HRU::SetAttInt(), Reach::AttInt(), Reach::SetAttInt(). Make m_hruArray public in both FlowModel and Catchment classes. Make m_catchmentArray public in FlowModel. Add temporary code to populate the HRU attribute HBVCALIB in InitHRULayers(). Fix 2 typos in InitHRULayers(). Add the code in InitHRULayers() to handle the case where the IDU layer values are not usable. WaterRights.cpp - Add logic to PopulateHBVCALIB() to populate the new HruHBVCALIB attribute. Flow_PEST.xml - Comment out the NSantiam springs. HRU_McKenzie.dbf, IDU_McKenzie.dbf, Reach_McKenzie.dbf, McKenzie/flow2010.ic - versions from a new spinup
</commit_message>
<xml_diff>
--- a/DataCW3M/CW3MdigitalHandbook/CW3MdataDictionary.xlsx
+++ b/DataCW3M/CW3MdigitalHandbook/CW3MdataDictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\CW3MdigitalHandbook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D32E618-7C6C-477E-AEA0-E4E4848162FB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0C545FA-B27B-41B1-BAF0-6B60F83D349F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-7425" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-7425" windowWidth="29040" windowHeight="17640" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Necessary input data" sheetId="7" r:id="rId1"/>
@@ -96,7 +96,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3066" uniqueCount="1032">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3072" uniqueCount="1034">
   <si>
     <t>LULC_A</t>
   </si>
@@ -3193,6 +3193,12 @@
   </si>
   <si>
     <t>liquid water in snowpack</t>
+  </si>
+  <si>
+    <t>index to HBV parameters for this HRU</t>
+  </si>
+  <si>
+    <t>equal to the HBVCALIB value for the reach which drains this HRU</t>
   </si>
 </sst>
 </file>
@@ -9163,8 +9169,8 @@
   </sheetPr>
   <dimension ref="A1:Z1051"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A192" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C68" sqref="C68"/>
     </sheetView>
   </sheetViews>
@@ -23960,11 +23966,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Z41"/>
+  <dimension ref="A1:Z42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomLeft" activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -24449,29 +24455,29 @@
       <c r="U13" s="7"/>
       <c r="V13" s="7"/>
     </row>
-    <row r="14" spans="1:26" ht="14.4">
-      <c r="A14" s="6" t="s">
-        <v>159</v>
-      </c>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
+    <row r="14" spans="1:26" s="21" customFormat="1" ht="14.4">
+      <c r="A14" s="28"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
       <c r="E14" s="7" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="F14" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="G14" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="H14" s="8" t="s">
+      <c r="G14" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="H14" s="7" t="s">
         <v>30</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>346</v>
-      </c>
-      <c r="J14" s="8"/>
+        <v>1032</v>
+      </c>
+      <c r="J14" s="7" t="s">
+        <v>1033</v>
+      </c>
       <c r="K14" s="7"/>
       <c r="L14" s="7"/>
       <c r="M14" s="7"/>
@@ -24485,41 +24491,41 @@
       <c r="U14" s="7"/>
       <c r="V14" s="7"/>
     </row>
-    <row r="15" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A15" s="44"/>
-      <c r="B15" s="45"/>
-      <c r="C15" s="45"/>
-      <c r="D15" s="45"/>
-      <c r="E15" s="47" t="s">
-        <v>349</v>
-      </c>
-      <c r="F15" s="47" t="s">
-        <v>29</v>
-      </c>
-      <c r="G15" s="47" t="s">
-        <v>318</v>
-      </c>
-      <c r="H15" s="47" t="s">
-        <v>27</v>
-      </c>
-      <c r="I15" s="47" t="s">
-        <v>355</v>
-      </c>
-      <c r="J15" s="47" t="s">
-        <v>356</v>
-      </c>
-      <c r="K15" s="45"/>
-      <c r="L15" s="45"/>
-      <c r="M15" s="45"/>
-      <c r="N15" s="45"/>
-      <c r="O15" s="45"/>
-      <c r="P15" s="45"/>
-      <c r="Q15" s="45"/>
-      <c r="R15" s="45"/>
-      <c r="S15" s="45"/>
-      <c r="T15" s="45"/>
-      <c r="U15" s="45"/>
-      <c r="V15" s="45"/>
+    <row r="15" spans="1:26" ht="14.4">
+      <c r="A15" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H15" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="I15" s="7" t="s">
+        <v>346</v>
+      </c>
+      <c r="J15" s="8"/>
+      <c r="K15" s="7"/>
+      <c r="L15" s="7"/>
+      <c r="M15" s="7"/>
+      <c r="N15" s="7"/>
+      <c r="O15" s="7"/>
+      <c r="P15" s="7"/>
+      <c r="Q15" s="7"/>
+      <c r="R15" s="7"/>
+      <c r="S15" s="7"/>
+      <c r="T15" s="7"/>
+      <c r="U15" s="7"/>
+      <c r="V15" s="7"/>
     </row>
     <row r="16" spans="1:26" ht="12.75" customHeight="1">
       <c r="A16" s="44"/>
@@ -24527,7 +24533,7 @@
       <c r="C16" s="45"/>
       <c r="D16" s="45"/>
       <c r="E16" s="47" t="s">
-        <v>358</v>
+        <v>349</v>
       </c>
       <c r="F16" s="47" t="s">
         <v>29</v>
@@ -24539,7 +24545,7 @@
         <v>27</v>
       </c>
       <c r="I16" s="47" t="s">
-        <v>362</v>
+        <v>355</v>
       </c>
       <c r="J16" s="47" t="s">
         <v>356</v>
@@ -24563,19 +24569,23 @@
       <c r="C17" s="45"/>
       <c r="D17" s="45"/>
       <c r="E17" s="47" t="s">
-        <v>367</v>
-      </c>
-      <c r="F17" s="47"/>
+        <v>358</v>
+      </c>
+      <c r="F17" s="47" t="s">
+        <v>29</v>
+      </c>
       <c r="G17" s="47" t="s">
-        <v>29</v>
+        <v>318</v>
       </c>
       <c r="H17" s="47" t="s">
         <v>27</v>
       </c>
       <c r="I17" s="47" t="s">
-        <v>371</v>
-      </c>
-      <c r="J17" s="47"/>
+        <v>362</v>
+      </c>
+      <c r="J17" s="47" t="s">
+        <v>356</v>
+      </c>
       <c r="K17" s="45"/>
       <c r="L17" s="45"/>
       <c r="M17" s="45"/>
@@ -24595,23 +24605,19 @@
       <c r="C18" s="45"/>
       <c r="D18" s="45"/>
       <c r="E18" s="47" t="s">
-        <v>373</v>
-      </c>
-      <c r="F18" s="47" t="s">
+        <v>367</v>
+      </c>
+      <c r="F18" s="47"/>
+      <c r="G18" s="47" t="s">
         <v>29</v>
-      </c>
-      <c r="G18" s="47" t="s">
-        <v>172</v>
       </c>
       <c r="H18" s="47" t="s">
         <v>27</v>
       </c>
       <c r="I18" s="47" t="s">
-        <v>375</v>
-      </c>
-      <c r="J18" s="47" t="s">
-        <v>376</v>
-      </c>
+        <v>371</v>
+      </c>
+      <c r="J18" s="47"/>
       <c r="K18" s="45"/>
       <c r="L18" s="45"/>
       <c r="M18" s="45"/>
@@ -24631,22 +24637,22 @@
       <c r="C19" s="45"/>
       <c r="D19" s="45"/>
       <c r="E19" s="47" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
       <c r="F19" s="47" t="s">
         <v>29</v>
       </c>
       <c r="G19" s="47" t="s">
-        <v>318</v>
+        <v>172</v>
       </c>
       <c r="H19" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="I19" s="48" t="s">
-        <v>384</v>
+      <c r="I19" s="47" t="s">
+        <v>375</v>
       </c>
       <c r="J19" s="47" t="s">
-        <v>356</v>
+        <v>376</v>
       </c>
       <c r="K19" s="45"/>
       <c r="L19" s="45"/>
@@ -24667,21 +24673,23 @@
       <c r="C20" s="45"/>
       <c r="D20" s="45"/>
       <c r="E20" s="47" t="s">
-        <v>401</v>
+        <v>381</v>
       </c>
       <c r="F20" s="47" t="s">
         <v>29</v>
       </c>
       <c r="G20" s="47" t="s">
-        <v>172</v>
+        <v>318</v>
       </c>
       <c r="H20" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="I20" s="47" t="s">
-        <v>403</v>
-      </c>
-      <c r="J20" s="45"/>
+      <c r="I20" s="48" t="s">
+        <v>384</v>
+      </c>
+      <c r="J20" s="47" t="s">
+        <v>356</v>
+      </c>
       <c r="K20" s="45"/>
       <c r="L20" s="45"/>
       <c r="M20" s="45"/>
@@ -24696,24 +24704,24 @@
       <c r="V20" s="45"/>
     </row>
     <row r="21" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A21" s="44" t="s">
-        <v>159</v>
-      </c>
+      <c r="A21" s="44"/>
       <c r="B21" s="45"/>
       <c r="C21" s="45"/>
       <c r="D21" s="45"/>
-      <c r="E21" s="45" t="s">
-        <v>407</v>
-      </c>
-      <c r="F21" s="45" t="s">
-        <v>46</v>
-      </c>
-      <c r="G21" s="45"/>
-      <c r="H21" s="45" t="s">
-        <v>57</v>
-      </c>
-      <c r="I21" s="45" t="s">
-        <v>409</v>
+      <c r="E21" s="47" t="s">
+        <v>401</v>
+      </c>
+      <c r="F21" s="47" t="s">
+        <v>29</v>
+      </c>
+      <c r="G21" s="47" t="s">
+        <v>172</v>
+      </c>
+      <c r="H21" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="I21" s="47" t="s">
+        <v>403</v>
       </c>
       <c r="J21" s="45"/>
       <c r="K21" s="45"/>
@@ -24730,30 +24738,26 @@
       <c r="V21" s="45"/>
     </row>
     <row r="22" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A22" s="49" t="s">
-        <v>23</v>
+      <c r="A22" s="44" t="s">
+        <v>159</v>
       </c>
       <c r="B22" s="45"/>
       <c r="C22" s="45"/>
       <c r="D22" s="45"/>
-      <c r="E22" s="47" t="s">
-        <v>419</v>
-      </c>
-      <c r="F22" s="47" t="s">
-        <v>29</v>
-      </c>
-      <c r="G22" s="47" t="s">
-        <v>172</v>
-      </c>
-      <c r="H22" s="47" t="s">
-        <v>27</v>
-      </c>
-      <c r="I22" s="47" t="s">
-        <v>421</v>
-      </c>
-      <c r="J22" s="47" t="s">
-        <v>422</v>
-      </c>
+      <c r="E22" s="45" t="s">
+        <v>407</v>
+      </c>
+      <c r="F22" s="45" t="s">
+        <v>46</v>
+      </c>
+      <c r="G22" s="45"/>
+      <c r="H22" s="45" t="s">
+        <v>57</v>
+      </c>
+      <c r="I22" s="45" t="s">
+        <v>409</v>
+      </c>
+      <c r="J22" s="45"/>
       <c r="K22" s="45"/>
       <c r="L22" s="45"/>
       <c r="M22" s="45"/>
@@ -24766,31 +24770,31 @@
       <c r="T22" s="45"/>
       <c r="U22" s="45"/>
       <c r="V22" s="45"/>
-      <c r="W22" s="7"/>
-      <c r="X22" s="7"/>
-      <c r="Y22" s="7"/>
-      <c r="Z22" s="7"/>
     </row>
     <row r="23" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A23" s="49"/>
+      <c r="A23" s="49" t="s">
+        <v>23</v>
+      </c>
       <c r="B23" s="45"/>
       <c r="C23" s="45"/>
       <c r="D23" s="45"/>
       <c r="E23" s="47" t="s">
-        <v>426</v>
+        <v>419</v>
       </c>
       <c r="F23" s="47" t="s">
-        <v>46</v>
-      </c>
-      <c r="G23" s="17" t="s">
-        <v>70</v>
-      </c>
-      <c r="H23" s="47"/>
-      <c r="I23" s="48" t="s">
-        <v>428</v>
+        <v>29</v>
+      </c>
+      <c r="G23" s="47" t="s">
+        <v>172</v>
+      </c>
+      <c r="H23" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="I23" s="47" t="s">
+        <v>421</v>
       </c>
       <c r="J23" s="47" t="s">
-        <v>429</v>
+        <v>422</v>
       </c>
       <c r="K23" s="45"/>
       <c r="L23" s="45"/>
@@ -24810,50 +24814,42 @@
       <c r="Z23" s="7"/>
     </row>
     <row r="24" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A24" s="50" t="s">
-        <v>23</v>
-      </c>
-      <c r="B24" s="51" t="s">
-        <v>23</v>
-      </c>
-      <c r="C24" s="51" t="s">
-        <v>23</v>
-      </c>
-      <c r="D24" s="51" t="s">
-        <v>445</v>
-      </c>
-      <c r="E24" s="51" t="s">
-        <v>446</v>
-      </c>
-      <c r="F24" s="51" t="s">
-        <v>29</v>
-      </c>
-      <c r="G24" s="51" t="s">
-        <v>447</v>
-      </c>
-      <c r="H24" s="51" t="s">
-        <v>30</v>
-      </c>
-      <c r="I24" s="52" t="s">
-        <v>448</v>
-      </c>
-      <c r="J24" s="51"/>
-      <c r="K24" s="53"/>
-      <c r="L24" s="53"/>
-      <c r="M24" s="53"/>
-      <c r="N24" s="53"/>
-      <c r="O24" s="53"/>
-      <c r="P24" s="53"/>
-      <c r="Q24" s="53"/>
-      <c r="R24" s="53"/>
-      <c r="S24" s="53"/>
-      <c r="T24" s="53"/>
-      <c r="U24" s="53"/>
-      <c r="V24" s="53"/>
-      <c r="W24" s="30"/>
-      <c r="X24" s="30"/>
-      <c r="Y24" s="30"/>
-      <c r="Z24" s="30"/>
+      <c r="A24" s="49"/>
+      <c r="B24" s="45"/>
+      <c r="C24" s="45"/>
+      <c r="D24" s="45"/>
+      <c r="E24" s="47" t="s">
+        <v>426</v>
+      </c>
+      <c r="F24" s="47" t="s">
+        <v>46</v>
+      </c>
+      <c r="G24" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="H24" s="47"/>
+      <c r="I24" s="48" t="s">
+        <v>428</v>
+      </c>
+      <c r="J24" s="47" t="s">
+        <v>429</v>
+      </c>
+      <c r="K24" s="45"/>
+      <c r="L24" s="45"/>
+      <c r="M24" s="45"/>
+      <c r="N24" s="45"/>
+      <c r="O24" s="45"/>
+      <c r="P24" s="45"/>
+      <c r="Q24" s="45"/>
+      <c r="R24" s="45"/>
+      <c r="S24" s="45"/>
+      <c r="T24" s="45"/>
+      <c r="U24" s="45"/>
+      <c r="V24" s="45"/>
+      <c r="W24" s="7"/>
+      <c r="X24" s="7"/>
+      <c r="Y24" s="7"/>
+      <c r="Z24" s="7"/>
     </row>
     <row r="25" spans="1:26" ht="12.75" customHeight="1">
       <c r="A25" s="50" t="s">
@@ -24869,19 +24865,19 @@
         <v>445</v>
       </c>
       <c r="E25" s="51" t="s">
-        <v>454</v>
+        <v>446</v>
       </c>
       <c r="F25" s="51" t="s">
         <v>29</v>
       </c>
       <c r="G25" s="51" t="s">
-        <v>63</v>
+        <v>447</v>
       </c>
       <c r="H25" s="51" t="s">
         <v>30</v>
       </c>
       <c r="I25" s="52" t="s">
-        <v>458</v>
+        <v>448</v>
       </c>
       <c r="J25" s="51"/>
       <c r="K25" s="53"/>
@@ -24902,44 +24898,50 @@
       <c r="Z25" s="30"/>
     </row>
     <row r="26" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A26" s="49"/>
-      <c r="B26" s="45"/>
-      <c r="C26" s="45"/>
-      <c r="D26" s="45"/>
-      <c r="E26" s="47" t="s">
-        <v>460</v>
-      </c>
-      <c r="F26" s="47" t="s">
+      <c r="A26" s="50" t="s">
+        <v>23</v>
+      </c>
+      <c r="B26" s="51" t="s">
+        <v>23</v>
+      </c>
+      <c r="C26" s="51" t="s">
+        <v>23</v>
+      </c>
+      <c r="D26" s="51" t="s">
+        <v>445</v>
+      </c>
+      <c r="E26" s="51" t="s">
+        <v>454</v>
+      </c>
+      <c r="F26" s="51" t="s">
         <v>29</v>
       </c>
-      <c r="G26" s="47" t="s">
-        <v>318</v>
-      </c>
-      <c r="H26" s="47" t="s">
-        <v>27</v>
-      </c>
-      <c r="I26" s="48" t="s">
-        <v>463</v>
-      </c>
-      <c r="J26" s="47" t="s">
-        <v>464</v>
-      </c>
-      <c r="K26" s="45"/>
-      <c r="L26" s="45"/>
-      <c r="M26" s="45"/>
-      <c r="N26" s="45"/>
-      <c r="O26" s="45"/>
-      <c r="P26" s="45"/>
-      <c r="Q26" s="45"/>
-      <c r="R26" s="45"/>
-      <c r="S26" s="45"/>
-      <c r="T26" s="45"/>
-      <c r="U26" s="45"/>
-      <c r="V26" s="45"/>
-      <c r="W26" s="7"/>
-      <c r="X26" s="7"/>
-      <c r="Y26" s="7"/>
-      <c r="Z26" s="7"/>
+      <c r="G26" s="51" t="s">
+        <v>63</v>
+      </c>
+      <c r="H26" s="51" t="s">
+        <v>30</v>
+      </c>
+      <c r="I26" s="52" t="s">
+        <v>458</v>
+      </c>
+      <c r="J26" s="51"/>
+      <c r="K26" s="53"/>
+      <c r="L26" s="53"/>
+      <c r="M26" s="53"/>
+      <c r="N26" s="53"/>
+      <c r="O26" s="53"/>
+      <c r="P26" s="53"/>
+      <c r="Q26" s="53"/>
+      <c r="R26" s="53"/>
+      <c r="S26" s="53"/>
+      <c r="T26" s="53"/>
+      <c r="U26" s="53"/>
+      <c r="V26" s="53"/>
+      <c r="W26" s="30"/>
+      <c r="X26" s="30"/>
+      <c r="Y26" s="30"/>
+      <c r="Z26" s="30"/>
     </row>
     <row r="27" spans="1:26" ht="12.75" customHeight="1">
       <c r="A27" s="49"/>
@@ -24947,7 +24949,7 @@
       <c r="C27" s="45"/>
       <c r="D27" s="45"/>
       <c r="E27" s="47" t="s">
-        <v>468</v>
+        <v>460</v>
       </c>
       <c r="F27" s="47" t="s">
         <v>29</v>
@@ -24959,7 +24961,7 @@
         <v>27</v>
       </c>
       <c r="I27" s="48" t="s">
-        <v>469</v>
+        <v>463</v>
       </c>
       <c r="J27" s="47" t="s">
         <v>464</v>
@@ -24982,29 +24984,27 @@
       <c r="Z27" s="7"/>
     </row>
     <row r="28" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A28" s="49" t="s">
-        <v>23</v>
-      </c>
+      <c r="A28" s="49"/>
       <c r="B28" s="45"/>
       <c r="C28" s="45"/>
       <c r="D28" s="45"/>
       <c r="E28" s="47" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="F28" s="47" t="s">
         <v>29</v>
       </c>
       <c r="G28" s="47" t="s">
-        <v>474</v>
+        <v>318</v>
       </c>
       <c r="H28" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="I28" s="47" t="s">
-        <v>475</v>
+      <c r="I28" s="48" t="s">
+        <v>469</v>
       </c>
       <c r="J28" s="47" t="s">
-        <v>476</v>
+        <v>464</v>
       </c>
       <c r="K28" s="45"/>
       <c r="L28" s="45"/>
@@ -25023,115 +25023,136 @@
       <c r="Y28" s="7"/>
       <c r="Z28" s="7"/>
     </row>
-    <row r="29" spans="1:26" s="21" customFormat="1" ht="14.25" customHeight="1">
-      <c r="C29" s="28"/>
-      <c r="D29" s="28"/>
-      <c r="E29" s="7" t="s">
-        <v>811</v>
+    <row r="29" spans="1:26" ht="12.75" customHeight="1">
+      <c r="A29" s="49" t="s">
+        <v>23</v>
+      </c>
+      <c r="B29" s="45"/>
+      <c r="C29" s="45"/>
+      <c r="D29" s="45"/>
+      <c r="E29" s="47" t="s">
+        <v>472</v>
       </c>
       <c r="F29" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="G29" s="70" t="s">
-        <v>226</v>
-      </c>
-      <c r="H29" s="70" t="s">
+      <c r="G29" s="47" t="s">
+        <v>474</v>
+      </c>
+      <c r="H29" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="I29" s="70" t="s">
-        <v>812</v>
-      </c>
-      <c r="J29" s="70" t="s">
-        <v>813</v>
-      </c>
-      <c r="K29" s="57"/>
-      <c r="L29" s="70"/>
-      <c r="M29" s="3"/>
-      <c r="N29" s="7"/>
-      <c r="O29" s="7"/>
-      <c r="P29" s="7"/>
-      <c r="Q29" s="7"/>
-      <c r="R29" s="7"/>
-      <c r="S29" s="7"/>
-      <c r="T29" s="7"/>
-      <c r="U29" s="7"/>
-      <c r="V29" s="7"/>
+      <c r="I29" s="47" t="s">
+        <v>475</v>
+      </c>
+      <c r="J29" s="47" t="s">
+        <v>476</v>
+      </c>
+      <c r="K29" s="45"/>
+      <c r="L29" s="45"/>
+      <c r="M29" s="45"/>
+      <c r="N29" s="45"/>
+      <c r="O29" s="45"/>
+      <c r="P29" s="45"/>
+      <c r="Q29" s="45"/>
+      <c r="R29" s="45"/>
+      <c r="S29" s="45"/>
+      <c r="T29" s="45"/>
+      <c r="U29" s="45"/>
+      <c r="V29" s="45"/>
       <c r="W29" s="7"/>
       <c r="X29" s="7"/>
-    </row>
-    <row r="30" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A30" s="44" t="s">
-        <v>23</v>
-      </c>
-      <c r="B30" s="45"/>
-      <c r="C30" s="45"/>
-      <c r="D30" s="45"/>
-      <c r="E30" s="45" t="s">
-        <v>480</v>
-      </c>
-      <c r="F30" s="45"/>
-      <c r="G30" s="45"/>
-      <c r="H30" s="45"/>
-      <c r="I30" s="45"/>
-      <c r="J30" s="45"/>
-      <c r="K30" s="45"/>
-      <c r="L30" s="45"/>
-      <c r="M30" s="45"/>
-      <c r="N30" s="45"/>
-      <c r="O30" s="45"/>
-      <c r="P30" s="45"/>
-      <c r="Q30" s="45"/>
-      <c r="R30" s="45"/>
-      <c r="S30" s="45"/>
-      <c r="T30" s="45"/>
-      <c r="U30" s="45"/>
-      <c r="V30" s="45"/>
+      <c r="Y29" s="7"/>
+      <c r="Z29" s="7"/>
+    </row>
+    <row r="30" spans="1:26" s="21" customFormat="1" ht="14.25" customHeight="1">
+      <c r="C30" s="28"/>
+      <c r="D30" s="28"/>
+      <c r="E30" s="7" t="s">
+        <v>811</v>
+      </c>
+      <c r="F30" s="47" t="s">
+        <v>29</v>
+      </c>
+      <c r="G30" s="70" t="s">
+        <v>226</v>
+      </c>
+      <c r="H30" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="I30" s="70" t="s">
+        <v>812</v>
+      </c>
+      <c r="J30" s="70" t="s">
+        <v>813</v>
+      </c>
+      <c r="K30" s="57"/>
+      <c r="L30" s="70"/>
+      <c r="M30" s="3"/>
+      <c r="N30" s="7"/>
+      <c r="O30" s="7"/>
+      <c r="P30" s="7"/>
+      <c r="Q30" s="7"/>
+      <c r="R30" s="7"/>
+      <c r="S30" s="7"/>
+      <c r="T30" s="7"/>
+      <c r="U30" s="7"/>
+      <c r="V30" s="7"/>
       <c r="W30" s="7"/>
       <c r="X30" s="7"/>
-      <c r="Y30" s="7"/>
-      <c r="Z30" s="7"/>
-    </row>
-    <row r="31" spans="1:26" ht="14.4">
-      <c r="A31" s="6" t="s">
-        <v>23</v>
-      </c>
+    </row>
+    <row r="31" spans="1:26" ht="12.75" customHeight="1">
+      <c r="A31" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="B31" s="45"/>
+      <c r="C31" s="45"/>
+      <c r="D31" s="45"/>
       <c r="E31" s="45" t="s">
+        <v>480</v>
+      </c>
+      <c r="F31" s="45"/>
+      <c r="G31" s="45"/>
+      <c r="H31" s="45"/>
+      <c r="I31" s="45"/>
+      <c r="J31" s="45"/>
+      <c r="K31" s="45"/>
+      <c r="L31" s="45"/>
+      <c r="M31" s="45"/>
+      <c r="N31" s="45"/>
+      <c r="O31" s="45"/>
+      <c r="P31" s="45"/>
+      <c r="Q31" s="45"/>
+      <c r="R31" s="45"/>
+      <c r="S31" s="45"/>
+      <c r="T31" s="45"/>
+      <c r="U31" s="45"/>
+      <c r="V31" s="45"/>
+      <c r="W31" s="7"/>
+      <c r="X31" s="7"/>
+      <c r="Y31" s="7"/>
+      <c r="Z31" s="7"/>
+    </row>
+    <row r="32" spans="1:26" ht="14.4">
+      <c r="A32" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E32" s="45" t="s">
         <v>110</v>
       </c>
-      <c r="F31" s="45" t="s">
+      <c r="F32" s="45" t="s">
         <v>29</v>
       </c>
-      <c r="G31" s="7"/>
-      <c r="I31" s="7"/>
-      <c r="J31" s="7"/>
-    </row>
-    <row r="32" spans="1:26" ht="14.4">
-      <c r="A32" s="28" t="s">
-        <v>159</v>
-      </c>
-      <c r="E32" s="18" t="s">
-        <v>485</v>
-      </c>
-      <c r="F32" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="G32" s="18" t="s">
-        <v>172</v>
-      </c>
-      <c r="H32" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="I32" s="18" t="s">
-        <v>487</v>
-      </c>
-      <c r="J32" s="18"/>
+      <c r="G32" s="7"/>
+      <c r="I32" s="7"/>
+      <c r="J32" s="7"/>
     </row>
     <row r="33" spans="1:10" ht="14.4">
       <c r="A33" s="28" t="s">
         <v>159</v>
       </c>
       <c r="E33" s="18" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="F33" s="18" t="s">
         <v>29</v>
@@ -25143,7 +25164,7 @@
         <v>27</v>
       </c>
       <c r="I33" s="18" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="J33" s="18"/>
     </row>
@@ -25152,64 +25173,62 @@
         <v>159</v>
       </c>
       <c r="E34" s="18" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
       <c r="F34" s="18" t="s">
         <v>29</v>
       </c>
       <c r="G34" s="18" t="s">
-        <v>494</v>
+        <v>172</v>
       </c>
       <c r="H34" s="17" t="s">
         <v>27</v>
       </c>
       <c r="I34" s="18" t="s">
-        <v>495</v>
+        <v>490</v>
       </c>
       <c r="J34" s="18"/>
     </row>
     <row r="35" spans="1:10" ht="14.4">
       <c r="A35" s="28" t="s">
-        <v>23</v>
+        <v>159</v>
       </c>
       <c r="E35" s="18" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="F35" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="G35" s="18"/>
+      <c r="G35" s="18" t="s">
+        <v>494</v>
+      </c>
       <c r="H35" s="17" t="s">
         <v>27</v>
       </c>
       <c r="I35" s="18" t="s">
-        <v>497</v>
-      </c>
-      <c r="J35" s="18" t="s">
-        <v>498</v>
-      </c>
+        <v>495</v>
+      </c>
+      <c r="J35" s="18"/>
     </row>
     <row r="36" spans="1:10" ht="14.4">
       <c r="A36" s="28" t="s">
         <v>23</v>
       </c>
       <c r="E36" s="18" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="F36" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="G36" s="18" t="s">
-        <v>128</v>
-      </c>
+      <c r="G36" s="18"/>
       <c r="H36" s="17" t="s">
         <v>27</v>
       </c>
       <c r="I36" s="18" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="J36" s="18" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="14.4">
@@ -25217,7 +25236,7 @@
         <v>23</v>
       </c>
       <c r="E37" s="18" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
       <c r="F37" s="18" t="s">
         <v>29</v>
@@ -25229,10 +25248,10 @@
         <v>27</v>
       </c>
       <c r="I37" s="18" t="s">
-        <v>504</v>
+        <v>500</v>
       </c>
       <c r="J37" s="18" t="s">
-        <v>505</v>
+        <v>501</v>
       </c>
     </row>
     <row r="38" spans="1:10" ht="14.4">
@@ -25240,7 +25259,7 @@
         <v>23</v>
       </c>
       <c r="E38" s="18" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="F38" s="18" t="s">
         <v>29</v>
@@ -25252,10 +25271,10 @@
         <v>27</v>
       </c>
       <c r="I38" s="18" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="J38" s="18" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="14.4">
@@ -25263,31 +25282,46 @@
         <v>23</v>
       </c>
       <c r="E39" s="18" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="F39" s="18" t="s">
         <v>29</v>
       </c>
       <c r="G39" s="18" t="s">
-        <v>510</v>
+        <v>128</v>
       </c>
       <c r="H39" s="17" t="s">
         <v>27</v>
       </c>
       <c r="I39" s="18" t="s">
+        <v>507</v>
+      </c>
+      <c r="J39" s="18" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" ht="14.4">
+      <c r="A40" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="E40" s="18" t="s">
+        <v>509</v>
+      </c>
+      <c r="F40" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="G40" s="18" t="s">
+        <v>510</v>
+      </c>
+      <c r="H40" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="I40" s="18" t="s">
         <v>511</v>
       </c>
-      <c r="J39" s="18" t="s">
+      <c r="J40" s="18" t="s">
         <v>512</v>
       </c>
-    </row>
-    <row r="40" spans="1:10" ht="14.4">
-      <c r="A40" s="6"/>
-      <c r="E40" s="7"/>
-      <c r="F40" s="7"/>
-      <c r="G40" s="7"/>
-      <c r="I40" s="7"/>
-      <c r="J40" s="7"/>
     </row>
     <row r="41" spans="1:10" ht="14.4">
       <c r="A41" s="6"/>
@@ -25296,6 +25330,14 @@
       <c r="G41" s="7"/>
       <c r="I41" s="7"/>
       <c r="J41" s="7"/>
+    </row>
+    <row r="42" spans="1:10" ht="14.4">
+      <c r="A42" s="6"/>
+      <c r="E42" s="7"/>
+      <c r="F42" s="7"/>
+      <c r="G42" s="7"/>
+      <c r="I42" s="7"/>
+      <c r="J42" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Rename HruSNOWPACK as HruSNOW_BOX. Add HRU::m_snowpackArea_m2. Delete obsolete IDU attribute "SNOW", which has been replaced with "SNOWPACK", representing only the frozen water in the snowpack, not including the liquid water. Add logic to FlowModel::StartYear() to calculate HRU::m_wetlandArea_m2 and HRU::m_snowpackArea_m2 for all the HRUs. Adjust the close_enough() arguments in CheckHRUwaterBalance(). Add logic to FlowModel::WriteDataToMap() to write out the values of the IDU SNOWPACK attribute.
</commit_message>
<xml_diff>
--- a/DataCW3M/CW3MdigitalHandbook/CW3MdataDictionary.xlsx
+++ b/DataCW3M/CW3MdigitalHandbook/CW3MdataDictionary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\CW3MdigitalHandbook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44DF0A8E-73C4-4D38-968E-D33CDD92A4FA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43D64DCC-3C4A-4EE5-9C33-536B6BAB3A2F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-7425" windowWidth="29040" windowHeight="17640" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -96,7 +96,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3072" uniqueCount="1034">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3077" uniqueCount="1036">
   <si>
     <t>LULC_A</t>
   </si>
@@ -3199,6 +3199,12 @@
   </si>
   <si>
     <t>equal to the HBVCALIB value for the reach which drains this HRU</t>
+  </si>
+  <si>
+    <t>SNOW_BOX</t>
+  </si>
+  <si>
+    <t>volume in hru compartment 0 expressed as a depth over the entire HRU, not merely the area covered by snow (divide m_volumeWater by m_HRUltotArea_m2, not by m_snowpackArea_m2)</t>
   </si>
 </sst>
 </file>
@@ -9170,7 +9176,7 @@
   <dimension ref="A1:Z1051"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A192" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="3" topLeftCell="A152" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C68" sqref="C68"/>
     </sheetView>
   </sheetViews>
@@ -23966,11 +23972,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Z42"/>
+  <dimension ref="A1:Z43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A14" sqref="A14:XFD14"/>
+      <selection pane="bottomLeft" activeCell="I36" sqref="I36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -25189,46 +25195,42 @@
       </c>
       <c r="J34" s="18"/>
     </row>
-    <row r="35" spans="1:10" ht="14.4">
-      <c r="A35" s="28" t="s">
+    <row r="35" spans="1:10" s="21" customFormat="1" ht="14.4">
+      <c r="A35" s="28"/>
+      <c r="E35" s="21" t="s">
+        <v>1034</v>
+      </c>
+      <c r="F35" s="47" t="s">
+        <v>29</v>
+      </c>
+      <c r="G35" s="21" t="s">
+        <v>494</v>
+      </c>
+      <c r="H35" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="I35" s="21" t="s">
+        <v>1035</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" s="65" customFormat="1" ht="14.4">
+      <c r="A36" s="66" t="s">
         <v>159</v>
       </c>
-      <c r="E35" s="18" t="s">
+      <c r="E36" s="65" t="s">
         <v>492</v>
       </c>
-      <c r="F35" s="18" t="s">
+      <c r="F36" s="65" t="s">
         <v>29</v>
       </c>
-      <c r="G35" s="18" t="s">
+      <c r="G36" s="65" t="s">
         <v>494</v>
       </c>
-      <c r="H35" s="17" t="s">
+      <c r="H36" s="93" t="s">
         <v>27</v>
       </c>
-      <c r="I35" s="18" t="s">
+      <c r="I36" s="65" t="s">
         <v>495</v>
-      </c>
-      <c r="J35" s="18"/>
-    </row>
-    <row r="36" spans="1:10" ht="14.4">
-      <c r="A36" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="E36" s="18" t="s">
-        <v>496</v>
-      </c>
-      <c r="F36" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="G36" s="18"/>
-      <c r="H36" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="I36" s="18" t="s">
-        <v>497</v>
-      </c>
-      <c r="J36" s="18" t="s">
-        <v>498</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="14.4">
@@ -25236,22 +25238,20 @@
         <v>23</v>
       </c>
       <c r="E37" s="18" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="F37" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="G37" s="18" t="s">
-        <v>128</v>
-      </c>
+      <c r="G37" s="18"/>
       <c r="H37" s="17" t="s">
         <v>27</v>
       </c>
       <c r="I37" s="18" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="J37" s="18" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
     </row>
     <row r="38" spans="1:10" ht="14.4">
@@ -25259,7 +25259,7 @@
         <v>23</v>
       </c>
       <c r="E38" s="18" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
       <c r="F38" s="18" t="s">
         <v>29</v>
@@ -25271,10 +25271,10 @@
         <v>27</v>
       </c>
       <c r="I38" s="18" t="s">
-        <v>504</v>
+        <v>500</v>
       </c>
       <c r="J38" s="18" t="s">
-        <v>505</v>
+        <v>501</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="14.4">
@@ -25282,7 +25282,7 @@
         <v>23</v>
       </c>
       <c r="E39" s="18" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="F39" s="18" t="s">
         <v>29</v>
@@ -25294,10 +25294,10 @@
         <v>27</v>
       </c>
       <c r="I39" s="18" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="J39" s="18" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="14.4">
@@ -25305,31 +25305,46 @@
         <v>23</v>
       </c>
       <c r="E40" s="18" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="F40" s="18" t="s">
         <v>29</v>
       </c>
       <c r="G40" s="18" t="s">
-        <v>510</v>
+        <v>128</v>
       </c>
       <c r="H40" s="17" t="s">
         <v>27</v>
       </c>
       <c r="I40" s="18" t="s">
+        <v>507</v>
+      </c>
+      <c r="J40" s="18" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" ht="14.4">
+      <c r="A41" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="E41" s="18" t="s">
+        <v>509</v>
+      </c>
+      <c r="F41" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="G41" s="18" t="s">
+        <v>510</v>
+      </c>
+      <c r="H41" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="I41" s="18" t="s">
         <v>511</v>
       </c>
-      <c r="J40" s="18" t="s">
+      <c r="J41" s="18" t="s">
         <v>512</v>
       </c>
-    </row>
-    <row r="41" spans="1:10" ht="14.4">
-      <c r="A41" s="6"/>
-      <c r="E41" s="7"/>
-      <c r="F41" s="7"/>
-      <c r="G41" s="7"/>
-      <c r="I41" s="7"/>
-      <c r="J41" s="7"/>
     </row>
     <row r="42" spans="1:10" ht="14.4">
       <c r="A42" s="6"/>
@@ -25338,6 +25353,14 @@
       <c r="G42" s="7"/>
       <c r="I42" s="7"/>
       <c r="J42" s="7"/>
+    </row>
+    <row r="43" spans="1:10" ht="14.4">
+      <c r="A43" s="6"/>
+      <c r="E43" s="7"/>
+      <c r="F43" s="7"/>
+      <c r="G43" s="7"/>
+      <c r="I43" s="7"/>
+      <c r="J43" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Debugging spinup mode. Some debugging remains to do. CW3M_NSantiam.envx - Add "spinup='0'" to <settings>. CW3MdataDictionary.xlsx - Add HRU attribute FIELD_CAP. Flow.cpp, .h - Add attribute HruFIELD_CAP. In ReadState(), add logic to start spinup with wetlands at field capacity.
</commit_message>
<xml_diff>
--- a/DataCW3M/CW3MdigitalHandbook/CW3MdataDictionary.xlsx
+++ b/DataCW3M/CW3MdigitalHandbook/CW3MdataDictionary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\CW3MdigitalHandbook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43D64DCC-3C4A-4EE5-9C33-536B6BAB3A2F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B7ED2B9-424D-4CF6-9791-CFC61C984E6A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-7425" windowWidth="29040" windowHeight="17640" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -96,7 +96,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3077" uniqueCount="1036">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3083" uniqueCount="1039">
   <si>
     <t>LULC_A</t>
   </si>
@@ -3205,6 +3205,15 @@
   </si>
   <si>
     <t>volume in hru compartment 0 expressed as a depth over the entire HRU, not merely the area covered by snow (divide m_volumeWater by m_HRUltotArea_m2, not by m_snowpackArea_m2)</t>
+  </si>
+  <si>
+    <t>FIELD_CAP</t>
+  </si>
+  <si>
+    <t>field capacity of the soil in this HRU</t>
+  </si>
+  <si>
+    <t>from HBV.csv for the HRU's HBVCALIB value</t>
   </si>
 </sst>
 </file>
@@ -9176,7 +9185,7 @@
   <dimension ref="A1:Z1051"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A152" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="3" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C68" sqref="C68"/>
     </sheetView>
   </sheetViews>
@@ -21028,7 +21037,7 @@
   <dimension ref="A1:Z117"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="4" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="H116" sqref="H116"/>
     </sheetView>
   </sheetViews>
@@ -23972,11 +23981,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Z43"/>
+  <dimension ref="A1:Z44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I36" sqref="I36"/>
+      <selection pane="bottomLeft" activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -24356,29 +24365,27 @@
       <c r="V10" s="7"/>
     </row>
     <row r="11" spans="1:26" s="21" customFormat="1" ht="14.4">
-      <c r="A11" s="28" t="s">
-        <v>159</v>
-      </c>
+      <c r="A11" s="28"/>
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
-      <c r="E11" s="7" t="s">
-        <v>337</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="G11" s="10" t="s">
-        <v>339</v>
-      </c>
-      <c r="H11" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="I11" s="7" t="s">
-        <v>340</v>
-      </c>
-      <c r="J11" s="7" t="s">
-        <v>342</v>
+      <c r="E11" s="21" t="s">
+        <v>1036</v>
+      </c>
+      <c r="F11" s="57" t="s">
+        <v>29</v>
+      </c>
+      <c r="G11" s="70" t="s">
+        <v>1030</v>
+      </c>
+      <c r="H11" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="I11" s="21" t="s">
+        <v>1037</v>
+      </c>
+      <c r="J11" s="21" t="s">
+        <v>1038</v>
       </c>
       <c r="K11" s="7"/>
       <c r="L11" s="7"/>
@@ -24393,27 +24400,31 @@
       <c r="U11" s="7"/>
       <c r="V11" s="7"/>
     </row>
-    <row r="12" spans="1:26" ht="14.4">
-      <c r="A12" s="6"/>
+    <row r="12" spans="1:26" s="21" customFormat="1" ht="14.4">
+      <c r="A12" s="28" t="s">
+        <v>159</v>
+      </c>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
-      <c r="E12" s="18" t="s">
-        <v>325</v>
-      </c>
-      <c r="F12" s="18" t="s">
-        <v>29</v>
+      <c r="E12" s="7" t="s">
+        <v>337</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>108</v>
       </c>
       <c r="G12" s="10" t="s">
-        <v>172</v>
-      </c>
-      <c r="H12" s="18" t="s">
+        <v>339</v>
+      </c>
+      <c r="H12" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="I12" s="18" t="s">
-        <v>327</v>
-      </c>
-      <c r="J12" s="7"/>
+      <c r="I12" s="7" t="s">
+        <v>340</v>
+      </c>
+      <c r="J12" s="7" t="s">
+        <v>342</v>
+      </c>
       <c r="K12" s="7"/>
       <c r="L12" s="7"/>
       <c r="M12" s="7"/>
@@ -24433,7 +24444,7 @@
       <c r="C13" s="7"/>
       <c r="D13" s="7"/>
       <c r="E13" s="18" t="s">
-        <v>331</v>
+        <v>325</v>
       </c>
       <c r="F13" s="18" t="s">
         <v>29</v>
@@ -24445,7 +24456,7 @@
         <v>27</v>
       </c>
       <c r="I13" s="18" t="s">
-        <v>334</v>
+        <v>327</v>
       </c>
       <c r="J13" s="7"/>
       <c r="K13" s="7"/>
@@ -24461,29 +24472,27 @@
       <c r="U13" s="7"/>
       <c r="V13" s="7"/>
     </row>
-    <row r="14" spans="1:26" s="21" customFormat="1" ht="14.4">
-      <c r="A14" s="28"/>
+    <row r="14" spans="1:26" ht="14.4">
+      <c r="A14" s="6"/>
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
-      <c r="E14" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="F14" s="7" t="s">
-        <v>46</v>
+      <c r="E14" s="18" t="s">
+        <v>331</v>
+      </c>
+      <c r="F14" s="18" t="s">
+        <v>29</v>
       </c>
       <c r="G14" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="H14" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="I14" s="7" t="s">
-        <v>1032</v>
-      </c>
-      <c r="J14" s="7" t="s">
-        <v>1033</v>
-      </c>
+        <v>172</v>
+      </c>
+      <c r="H14" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="I14" s="18" t="s">
+        <v>334</v>
+      </c>
+      <c r="J14" s="7"/>
       <c r="K14" s="7"/>
       <c r="L14" s="7"/>
       <c r="M14" s="7"/>
@@ -24497,29 +24506,29 @@
       <c r="U14" s="7"/>
       <c r="V14" s="7"/>
     </row>
-    <row r="15" spans="1:26" ht="14.4">
-      <c r="A15" s="6" t="s">
-        <v>159</v>
-      </c>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
+    <row r="15" spans="1:26" s="21" customFormat="1" ht="14.4">
+      <c r="A15" s="28"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
       <c r="E15" s="7" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="F15" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="G15" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="H15" s="8" t="s">
+      <c r="G15" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="H15" s="7" t="s">
         <v>30</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>346</v>
-      </c>
-      <c r="J15" s="8"/>
+        <v>1032</v>
+      </c>
+      <c r="J15" s="7" t="s">
+        <v>1033</v>
+      </c>
       <c r="K15" s="7"/>
       <c r="L15" s="7"/>
       <c r="M15" s="7"/>
@@ -24533,41 +24542,41 @@
       <c r="U15" s="7"/>
       <c r="V15" s="7"/>
     </row>
-    <row r="16" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A16" s="44"/>
-      <c r="B16" s="45"/>
-      <c r="C16" s="45"/>
-      <c r="D16" s="45"/>
-      <c r="E16" s="47" t="s">
-        <v>349</v>
-      </c>
-      <c r="F16" s="47" t="s">
-        <v>29</v>
-      </c>
-      <c r="G16" s="47" t="s">
-        <v>318</v>
-      </c>
-      <c r="H16" s="47" t="s">
-        <v>27</v>
-      </c>
-      <c r="I16" s="47" t="s">
-        <v>355</v>
-      </c>
-      <c r="J16" s="47" t="s">
-        <v>356</v>
-      </c>
-      <c r="K16" s="45"/>
-      <c r="L16" s="45"/>
-      <c r="M16" s="45"/>
-      <c r="N16" s="45"/>
-      <c r="O16" s="45"/>
-      <c r="P16" s="45"/>
-      <c r="Q16" s="45"/>
-      <c r="R16" s="45"/>
-      <c r="S16" s="45"/>
-      <c r="T16" s="45"/>
-      <c r="U16" s="45"/>
-      <c r="V16" s="45"/>
+    <row r="16" spans="1:26" ht="14.4">
+      <c r="A16" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H16" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="I16" s="7" t="s">
+        <v>346</v>
+      </c>
+      <c r="J16" s="8"/>
+      <c r="K16" s="7"/>
+      <c r="L16" s="7"/>
+      <c r="M16" s="7"/>
+      <c r="N16" s="7"/>
+      <c r="O16" s="7"/>
+      <c r="P16" s="7"/>
+      <c r="Q16" s="7"/>
+      <c r="R16" s="7"/>
+      <c r="S16" s="7"/>
+      <c r="T16" s="7"/>
+      <c r="U16" s="7"/>
+      <c r="V16" s="7"/>
     </row>
     <row r="17" spans="1:26" ht="12.75" customHeight="1">
       <c r="A17" s="44"/>
@@ -24575,7 +24584,7 @@
       <c r="C17" s="45"/>
       <c r="D17" s="45"/>
       <c r="E17" s="47" t="s">
-        <v>358</v>
+        <v>349</v>
       </c>
       <c r="F17" s="47" t="s">
         <v>29</v>
@@ -24587,7 +24596,7 @@
         <v>27</v>
       </c>
       <c r="I17" s="47" t="s">
-        <v>362</v>
+        <v>355</v>
       </c>
       <c r="J17" s="47" t="s">
         <v>356</v>
@@ -24611,19 +24620,23 @@
       <c r="C18" s="45"/>
       <c r="D18" s="45"/>
       <c r="E18" s="47" t="s">
-        <v>367</v>
-      </c>
-      <c r="F18" s="47"/>
+        <v>358</v>
+      </c>
+      <c r="F18" s="47" t="s">
+        <v>29</v>
+      </c>
       <c r="G18" s="47" t="s">
-        <v>29</v>
+        <v>318</v>
       </c>
       <c r="H18" s="47" t="s">
         <v>27</v>
       </c>
       <c r="I18" s="47" t="s">
-        <v>371</v>
-      </c>
-      <c r="J18" s="47"/>
+        <v>362</v>
+      </c>
+      <c r="J18" s="47" t="s">
+        <v>356</v>
+      </c>
       <c r="K18" s="45"/>
       <c r="L18" s="45"/>
       <c r="M18" s="45"/>
@@ -24643,23 +24656,19 @@
       <c r="C19" s="45"/>
       <c r="D19" s="45"/>
       <c r="E19" s="47" t="s">
-        <v>373</v>
-      </c>
-      <c r="F19" s="47" t="s">
+        <v>367</v>
+      </c>
+      <c r="F19" s="47"/>
+      <c r="G19" s="47" t="s">
         <v>29</v>
-      </c>
-      <c r="G19" s="47" t="s">
-        <v>172</v>
       </c>
       <c r="H19" s="47" t="s">
         <v>27</v>
       </c>
       <c r="I19" s="47" t="s">
-        <v>375</v>
-      </c>
-      <c r="J19" s="47" t="s">
-        <v>376</v>
-      </c>
+        <v>371</v>
+      </c>
+      <c r="J19" s="47"/>
       <c r="K19" s="45"/>
       <c r="L19" s="45"/>
       <c r="M19" s="45"/>
@@ -24679,22 +24688,22 @@
       <c r="C20" s="45"/>
       <c r="D20" s="45"/>
       <c r="E20" s="47" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
       <c r="F20" s="47" t="s">
         <v>29</v>
       </c>
       <c r="G20" s="47" t="s">
-        <v>318</v>
+        <v>172</v>
       </c>
       <c r="H20" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="I20" s="48" t="s">
-        <v>384</v>
+      <c r="I20" s="47" t="s">
+        <v>375</v>
       </c>
       <c r="J20" s="47" t="s">
-        <v>356</v>
+        <v>376</v>
       </c>
       <c r="K20" s="45"/>
       <c r="L20" s="45"/>
@@ -24715,21 +24724,23 @@
       <c r="C21" s="45"/>
       <c r="D21" s="45"/>
       <c r="E21" s="47" t="s">
-        <v>401</v>
+        <v>381</v>
       </c>
       <c r="F21" s="47" t="s">
         <v>29</v>
       </c>
       <c r="G21" s="47" t="s">
-        <v>172</v>
+        <v>318</v>
       </c>
       <c r="H21" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="I21" s="47" t="s">
-        <v>403</v>
-      </c>
-      <c r="J21" s="45"/>
+      <c r="I21" s="48" t="s">
+        <v>384</v>
+      </c>
+      <c r="J21" s="47" t="s">
+        <v>356</v>
+      </c>
       <c r="K21" s="45"/>
       <c r="L21" s="45"/>
       <c r="M21" s="45"/>
@@ -24744,24 +24755,24 @@
       <c r="V21" s="45"/>
     </row>
     <row r="22" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A22" s="44" t="s">
-        <v>159</v>
-      </c>
+      <c r="A22" s="44"/>
       <c r="B22" s="45"/>
       <c r="C22" s="45"/>
       <c r="D22" s="45"/>
-      <c r="E22" s="45" t="s">
-        <v>407</v>
-      </c>
-      <c r="F22" s="45" t="s">
-        <v>46</v>
-      </c>
-      <c r="G22" s="45"/>
-      <c r="H22" s="45" t="s">
-        <v>57</v>
-      </c>
-      <c r="I22" s="45" t="s">
-        <v>409</v>
+      <c r="E22" s="47" t="s">
+        <v>401</v>
+      </c>
+      <c r="F22" s="47" t="s">
+        <v>29</v>
+      </c>
+      <c r="G22" s="47" t="s">
+        <v>172</v>
+      </c>
+      <c r="H22" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="I22" s="47" t="s">
+        <v>403</v>
       </c>
       <c r="J22" s="45"/>
       <c r="K22" s="45"/>
@@ -24778,30 +24789,26 @@
       <c r="V22" s="45"/>
     </row>
     <row r="23" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A23" s="49" t="s">
-        <v>23</v>
+      <c r="A23" s="44" t="s">
+        <v>159</v>
       </c>
       <c r="B23" s="45"/>
       <c r="C23" s="45"/>
       <c r="D23" s="45"/>
-      <c r="E23" s="47" t="s">
-        <v>419</v>
-      </c>
-      <c r="F23" s="47" t="s">
-        <v>29</v>
-      </c>
-      <c r="G23" s="47" t="s">
-        <v>172</v>
-      </c>
-      <c r="H23" s="47" t="s">
-        <v>27</v>
-      </c>
-      <c r="I23" s="47" t="s">
-        <v>421</v>
-      </c>
-      <c r="J23" s="47" t="s">
-        <v>422</v>
-      </c>
+      <c r="E23" s="45" t="s">
+        <v>407</v>
+      </c>
+      <c r="F23" s="45" t="s">
+        <v>46</v>
+      </c>
+      <c r="G23" s="45"/>
+      <c r="H23" s="45" t="s">
+        <v>57</v>
+      </c>
+      <c r="I23" s="45" t="s">
+        <v>409</v>
+      </c>
+      <c r="J23" s="45"/>
       <c r="K23" s="45"/>
       <c r="L23" s="45"/>
       <c r="M23" s="45"/>
@@ -24814,31 +24821,31 @@
       <c r="T23" s="45"/>
       <c r="U23" s="45"/>
       <c r="V23" s="45"/>
-      <c r="W23" s="7"/>
-      <c r="X23" s="7"/>
-      <c r="Y23" s="7"/>
-      <c r="Z23" s="7"/>
     </row>
     <row r="24" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A24" s="49"/>
+      <c r="A24" s="49" t="s">
+        <v>23</v>
+      </c>
       <c r="B24" s="45"/>
       <c r="C24" s="45"/>
       <c r="D24" s="45"/>
       <c r="E24" s="47" t="s">
-        <v>426</v>
+        <v>419</v>
       </c>
       <c r="F24" s="47" t="s">
-        <v>46</v>
-      </c>
-      <c r="G24" s="17" t="s">
-        <v>70</v>
-      </c>
-      <c r="H24" s="47"/>
-      <c r="I24" s="48" t="s">
-        <v>428</v>
+        <v>29</v>
+      </c>
+      <c r="G24" s="47" t="s">
+        <v>172</v>
+      </c>
+      <c r="H24" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="I24" s="47" t="s">
+        <v>421</v>
       </c>
       <c r="J24" s="47" t="s">
-        <v>429</v>
+        <v>422</v>
       </c>
       <c r="K24" s="45"/>
       <c r="L24" s="45"/>
@@ -24858,50 +24865,42 @@
       <c r="Z24" s="7"/>
     </row>
     <row r="25" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A25" s="50" t="s">
-        <v>23</v>
-      </c>
-      <c r="B25" s="51" t="s">
-        <v>23</v>
-      </c>
-      <c r="C25" s="51" t="s">
-        <v>23</v>
-      </c>
-      <c r="D25" s="51" t="s">
-        <v>445</v>
-      </c>
-      <c r="E25" s="51" t="s">
-        <v>446</v>
-      </c>
-      <c r="F25" s="51" t="s">
-        <v>29</v>
-      </c>
-      <c r="G25" s="51" t="s">
-        <v>447</v>
-      </c>
-      <c r="H25" s="51" t="s">
-        <v>30</v>
-      </c>
-      <c r="I25" s="52" t="s">
-        <v>448</v>
-      </c>
-      <c r="J25" s="51"/>
-      <c r="K25" s="53"/>
-      <c r="L25" s="53"/>
-      <c r="M25" s="53"/>
-      <c r="N25" s="53"/>
-      <c r="O25" s="53"/>
-      <c r="P25" s="53"/>
-      <c r="Q25" s="53"/>
-      <c r="R25" s="53"/>
-      <c r="S25" s="53"/>
-      <c r="T25" s="53"/>
-      <c r="U25" s="53"/>
-      <c r="V25" s="53"/>
-      <c r="W25" s="30"/>
-      <c r="X25" s="30"/>
-      <c r="Y25" s="30"/>
-      <c r="Z25" s="30"/>
+      <c r="A25" s="49"/>
+      <c r="B25" s="45"/>
+      <c r="C25" s="45"/>
+      <c r="D25" s="45"/>
+      <c r="E25" s="47" t="s">
+        <v>426</v>
+      </c>
+      <c r="F25" s="47" t="s">
+        <v>46</v>
+      </c>
+      <c r="G25" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="H25" s="47"/>
+      <c r="I25" s="48" t="s">
+        <v>428</v>
+      </c>
+      <c r="J25" s="47" t="s">
+        <v>429</v>
+      </c>
+      <c r="K25" s="45"/>
+      <c r="L25" s="45"/>
+      <c r="M25" s="45"/>
+      <c r="N25" s="45"/>
+      <c r="O25" s="45"/>
+      <c r="P25" s="45"/>
+      <c r="Q25" s="45"/>
+      <c r="R25" s="45"/>
+      <c r="S25" s="45"/>
+      <c r="T25" s="45"/>
+      <c r="U25" s="45"/>
+      <c r="V25" s="45"/>
+      <c r="W25" s="7"/>
+      <c r="X25" s="7"/>
+      <c r="Y25" s="7"/>
+      <c r="Z25" s="7"/>
     </row>
     <row r="26" spans="1:26" ht="12.75" customHeight="1">
       <c r="A26" s="50" t="s">
@@ -24917,19 +24916,19 @@
         <v>445</v>
       </c>
       <c r="E26" s="51" t="s">
-        <v>454</v>
+        <v>446</v>
       </c>
       <c r="F26" s="51" t="s">
         <v>29</v>
       </c>
       <c r="G26" s="51" t="s">
-        <v>63</v>
+        <v>447</v>
       </c>
       <c r="H26" s="51" t="s">
         <v>30</v>
       </c>
       <c r="I26" s="52" t="s">
-        <v>458</v>
+        <v>448</v>
       </c>
       <c r="J26" s="51"/>
       <c r="K26" s="53"/>
@@ -24950,44 +24949,50 @@
       <c r="Z26" s="30"/>
     </row>
     <row r="27" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A27" s="49"/>
-      <c r="B27" s="45"/>
-      <c r="C27" s="45"/>
-      <c r="D27" s="45"/>
-      <c r="E27" s="47" t="s">
-        <v>460</v>
-      </c>
-      <c r="F27" s="47" t="s">
+      <c r="A27" s="50" t="s">
+        <v>23</v>
+      </c>
+      <c r="B27" s="51" t="s">
+        <v>23</v>
+      </c>
+      <c r="C27" s="51" t="s">
+        <v>23</v>
+      </c>
+      <c r="D27" s="51" t="s">
+        <v>445</v>
+      </c>
+      <c r="E27" s="51" t="s">
+        <v>454</v>
+      </c>
+      <c r="F27" s="51" t="s">
         <v>29</v>
       </c>
-      <c r="G27" s="47" t="s">
-        <v>318</v>
-      </c>
-      <c r="H27" s="47" t="s">
-        <v>27</v>
-      </c>
-      <c r="I27" s="48" t="s">
-        <v>463</v>
-      </c>
-      <c r="J27" s="47" t="s">
-        <v>464</v>
-      </c>
-      <c r="K27" s="45"/>
-      <c r="L27" s="45"/>
-      <c r="M27" s="45"/>
-      <c r="N27" s="45"/>
-      <c r="O27" s="45"/>
-      <c r="P27" s="45"/>
-      <c r="Q27" s="45"/>
-      <c r="R27" s="45"/>
-      <c r="S27" s="45"/>
-      <c r="T27" s="45"/>
-      <c r="U27" s="45"/>
-      <c r="V27" s="45"/>
-      <c r="W27" s="7"/>
-      <c r="X27" s="7"/>
-      <c r="Y27" s="7"/>
-      <c r="Z27" s="7"/>
+      <c r="G27" s="51" t="s">
+        <v>63</v>
+      </c>
+      <c r="H27" s="51" t="s">
+        <v>30</v>
+      </c>
+      <c r="I27" s="52" t="s">
+        <v>458</v>
+      </c>
+      <c r="J27" s="51"/>
+      <c r="K27" s="53"/>
+      <c r="L27" s="53"/>
+      <c r="M27" s="53"/>
+      <c r="N27" s="53"/>
+      <c r="O27" s="53"/>
+      <c r="P27" s="53"/>
+      <c r="Q27" s="53"/>
+      <c r="R27" s="53"/>
+      <c r="S27" s="53"/>
+      <c r="T27" s="53"/>
+      <c r="U27" s="53"/>
+      <c r="V27" s="53"/>
+      <c r="W27" s="30"/>
+      <c r="X27" s="30"/>
+      <c r="Y27" s="30"/>
+      <c r="Z27" s="30"/>
     </row>
     <row r="28" spans="1:26" ht="12.75" customHeight="1">
       <c r="A28" s="49"/>
@@ -24995,7 +25000,7 @@
       <c r="C28" s="45"/>
       <c r="D28" s="45"/>
       <c r="E28" s="47" t="s">
-        <v>468</v>
+        <v>460</v>
       </c>
       <c r="F28" s="47" t="s">
         <v>29</v>
@@ -25007,7 +25012,7 @@
         <v>27</v>
       </c>
       <c r="I28" s="48" t="s">
-        <v>469</v>
+        <v>463</v>
       </c>
       <c r="J28" s="47" t="s">
         <v>464</v>
@@ -25030,29 +25035,27 @@
       <c r="Z28" s="7"/>
     </row>
     <row r="29" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A29" s="49" t="s">
-        <v>23</v>
-      </c>
+      <c r="A29" s="49"/>
       <c r="B29" s="45"/>
       <c r="C29" s="45"/>
       <c r="D29" s="45"/>
       <c r="E29" s="47" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="F29" s="47" t="s">
         <v>29</v>
       </c>
       <c r="G29" s="47" t="s">
-        <v>474</v>
+        <v>318</v>
       </c>
       <c r="H29" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="I29" s="47" t="s">
-        <v>475</v>
+      <c r="I29" s="48" t="s">
+        <v>469</v>
       </c>
       <c r="J29" s="47" t="s">
-        <v>476</v>
+        <v>464</v>
       </c>
       <c r="K29" s="45"/>
       <c r="L29" s="45"/>
@@ -25071,115 +25074,136 @@
       <c r="Y29" s="7"/>
       <c r="Z29" s="7"/>
     </row>
-    <row r="30" spans="1:26" s="21" customFormat="1" ht="14.25" customHeight="1">
-      <c r="C30" s="28"/>
-      <c r="D30" s="28"/>
-      <c r="E30" s="7" t="s">
-        <v>811</v>
+    <row r="30" spans="1:26" ht="12.75" customHeight="1">
+      <c r="A30" s="49" t="s">
+        <v>23</v>
+      </c>
+      <c r="B30" s="45"/>
+      <c r="C30" s="45"/>
+      <c r="D30" s="45"/>
+      <c r="E30" s="47" t="s">
+        <v>472</v>
       </c>
       <c r="F30" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="G30" s="70" t="s">
-        <v>226</v>
-      </c>
-      <c r="H30" s="70" t="s">
+      <c r="G30" s="47" t="s">
+        <v>474</v>
+      </c>
+      <c r="H30" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="I30" s="70" t="s">
-        <v>812</v>
-      </c>
-      <c r="J30" s="70" t="s">
-        <v>813</v>
-      </c>
-      <c r="K30" s="57"/>
-      <c r="L30" s="70"/>
-      <c r="M30" s="3"/>
-      <c r="N30" s="7"/>
-      <c r="O30" s="7"/>
-      <c r="P30" s="7"/>
-      <c r="Q30" s="7"/>
-      <c r="R30" s="7"/>
-      <c r="S30" s="7"/>
-      <c r="T30" s="7"/>
-      <c r="U30" s="7"/>
-      <c r="V30" s="7"/>
+      <c r="I30" s="47" t="s">
+        <v>475</v>
+      </c>
+      <c r="J30" s="47" t="s">
+        <v>476</v>
+      </c>
+      <c r="K30" s="45"/>
+      <c r="L30" s="45"/>
+      <c r="M30" s="45"/>
+      <c r="N30" s="45"/>
+      <c r="O30" s="45"/>
+      <c r="P30" s="45"/>
+      <c r="Q30" s="45"/>
+      <c r="R30" s="45"/>
+      <c r="S30" s="45"/>
+      <c r="T30" s="45"/>
+      <c r="U30" s="45"/>
+      <c r="V30" s="45"/>
       <c r="W30" s="7"/>
       <c r="X30" s="7"/>
-    </row>
-    <row r="31" spans="1:26" ht="12.75" customHeight="1">
-      <c r="A31" s="44" t="s">
-        <v>23</v>
-      </c>
-      <c r="B31" s="45"/>
-      <c r="C31" s="45"/>
-      <c r="D31" s="45"/>
-      <c r="E31" s="45" t="s">
-        <v>480</v>
-      </c>
-      <c r="F31" s="45"/>
-      <c r="G31" s="45"/>
-      <c r="H31" s="45"/>
-      <c r="I31" s="45"/>
-      <c r="J31" s="45"/>
-      <c r="K31" s="45"/>
-      <c r="L31" s="45"/>
-      <c r="M31" s="45"/>
-      <c r="N31" s="45"/>
-      <c r="O31" s="45"/>
-      <c r="P31" s="45"/>
-      <c r="Q31" s="45"/>
-      <c r="R31" s="45"/>
-      <c r="S31" s="45"/>
-      <c r="T31" s="45"/>
-      <c r="U31" s="45"/>
-      <c r="V31" s="45"/>
+      <c r="Y30" s="7"/>
+      <c r="Z30" s="7"/>
+    </row>
+    <row r="31" spans="1:26" s="21" customFormat="1" ht="14.25" customHeight="1">
+      <c r="C31" s="28"/>
+      <c r="D31" s="28"/>
+      <c r="E31" s="7" t="s">
+        <v>811</v>
+      </c>
+      <c r="F31" s="47" t="s">
+        <v>29</v>
+      </c>
+      <c r="G31" s="70" t="s">
+        <v>226</v>
+      </c>
+      <c r="H31" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="I31" s="70" t="s">
+        <v>812</v>
+      </c>
+      <c r="J31" s="70" t="s">
+        <v>813</v>
+      </c>
+      <c r="K31" s="57"/>
+      <c r="L31" s="70"/>
+      <c r="M31" s="3"/>
+      <c r="N31" s="7"/>
+      <c r="O31" s="7"/>
+      <c r="P31" s="7"/>
+      <c r="Q31" s="7"/>
+      <c r="R31" s="7"/>
+      <c r="S31" s="7"/>
+      <c r="T31" s="7"/>
+      <c r="U31" s="7"/>
+      <c r="V31" s="7"/>
       <c r="W31" s="7"/>
       <c r="X31" s="7"/>
-      <c r="Y31" s="7"/>
-      <c r="Z31" s="7"/>
-    </row>
-    <row r="32" spans="1:26" ht="14.4">
-      <c r="A32" s="6" t="s">
-        <v>23</v>
-      </c>
+    </row>
+    <row r="32" spans="1:26" ht="12.75" customHeight="1">
+      <c r="A32" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="B32" s="45"/>
+      <c r="C32" s="45"/>
+      <c r="D32" s="45"/>
       <c r="E32" s="45" t="s">
+        <v>480</v>
+      </c>
+      <c r="F32" s="45"/>
+      <c r="G32" s="45"/>
+      <c r="H32" s="45"/>
+      <c r="I32" s="45"/>
+      <c r="J32" s="45"/>
+      <c r="K32" s="45"/>
+      <c r="L32" s="45"/>
+      <c r="M32" s="45"/>
+      <c r="N32" s="45"/>
+      <c r="O32" s="45"/>
+      <c r="P32" s="45"/>
+      <c r="Q32" s="45"/>
+      <c r="R32" s="45"/>
+      <c r="S32" s="45"/>
+      <c r="T32" s="45"/>
+      <c r="U32" s="45"/>
+      <c r="V32" s="45"/>
+      <c r="W32" s="7"/>
+      <c r="X32" s="7"/>
+      <c r="Y32" s="7"/>
+      <c r="Z32" s="7"/>
+    </row>
+    <row r="33" spans="1:10" ht="14.4">
+      <c r="A33" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E33" s="45" t="s">
         <v>110</v>
       </c>
-      <c r="F32" s="45" t="s">
+      <c r="F33" s="45" t="s">
         <v>29</v>
       </c>
-      <c r="G32" s="7"/>
-      <c r="I32" s="7"/>
-      <c r="J32" s="7"/>
-    </row>
-    <row r="33" spans="1:10" ht="14.4">
-      <c r="A33" s="28" t="s">
-        <v>159</v>
-      </c>
-      <c r="E33" s="18" t="s">
-        <v>485</v>
-      </c>
-      <c r="F33" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="G33" s="18" t="s">
-        <v>172</v>
-      </c>
-      <c r="H33" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="I33" s="18" t="s">
-        <v>487</v>
-      </c>
-      <c r="J33" s="18"/>
+      <c r="G33" s="7"/>
+      <c r="I33" s="7"/>
+      <c r="J33" s="7"/>
     </row>
     <row r="34" spans="1:10" ht="14.4">
       <c r="A34" s="28" t="s">
         <v>159</v>
       </c>
       <c r="E34" s="18" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="F34" s="18" t="s">
         <v>29</v>
@@ -25191,67 +25215,67 @@
         <v>27</v>
       </c>
       <c r="I34" s="18" t="s">
+        <v>487</v>
+      </c>
+      <c r="J34" s="18"/>
+    </row>
+    <row r="35" spans="1:10" ht="14.4">
+      <c r="A35" s="28" t="s">
+        <v>159</v>
+      </c>
+      <c r="E35" s="18" t="s">
+        <v>488</v>
+      </c>
+      <c r="F35" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="G35" s="18" t="s">
+        <v>172</v>
+      </c>
+      <c r="H35" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="I35" s="18" t="s">
         <v>490</v>
       </c>
-      <c r="J34" s="18"/>
-    </row>
-    <row r="35" spans="1:10" s="21" customFormat="1" ht="14.4">
-      <c r="A35" s="28"/>
-      <c r="E35" s="21" t="s">
+      <c r="J35" s="18"/>
+    </row>
+    <row r="36" spans="1:10" s="21" customFormat="1" ht="14.4">
+      <c r="A36" s="28"/>
+      <c r="E36" s="21" t="s">
         <v>1034</v>
       </c>
-      <c r="F35" s="47" t="s">
+      <c r="F36" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="G35" s="21" t="s">
+      <c r="G36" s="21" t="s">
         <v>494</v>
       </c>
-      <c r="H35" s="23" t="s">
+      <c r="H36" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="I35" s="21" t="s">
+      <c r="I36" s="21" t="s">
         <v>1035</v>
       </c>
     </row>
-    <row r="36" spans="1:10" s="65" customFormat="1" ht="14.4">
-      <c r="A36" s="66" t="s">
+    <row r="37" spans="1:10" s="65" customFormat="1" ht="14.4">
+      <c r="A37" s="66" t="s">
         <v>159</v>
       </c>
-      <c r="E36" s="65" t="s">
+      <c r="E37" s="65" t="s">
         <v>492</v>
       </c>
-      <c r="F36" s="65" t="s">
+      <c r="F37" s="65" t="s">
         <v>29</v>
       </c>
-      <c r="G36" s="65" t="s">
+      <c r="G37" s="65" t="s">
         <v>494</v>
       </c>
-      <c r="H36" s="93" t="s">
+      <c r="H37" s="93" t="s">
         <v>27</v>
       </c>
-      <c r="I36" s="65" t="s">
+      <c r="I37" s="65" t="s">
         <v>495</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" ht="14.4">
-      <c r="A37" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="E37" s="18" t="s">
-        <v>496</v>
-      </c>
-      <c r="F37" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="G37" s="18"/>
-      <c r="H37" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="I37" s="18" t="s">
-        <v>497</v>
-      </c>
-      <c r="J37" s="18" t="s">
-        <v>498</v>
       </c>
     </row>
     <row r="38" spans="1:10" ht="14.4">
@@ -25259,22 +25283,20 @@
         <v>23</v>
       </c>
       <c r="E38" s="18" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="F38" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="G38" s="18" t="s">
-        <v>128</v>
-      </c>
+      <c r="G38" s="18"/>
       <c r="H38" s="17" t="s">
         <v>27</v>
       </c>
       <c r="I38" s="18" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="J38" s="18" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="14.4">
@@ -25282,7 +25304,7 @@
         <v>23</v>
       </c>
       <c r="E39" s="18" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
       <c r="F39" s="18" t="s">
         <v>29</v>
@@ -25294,10 +25316,10 @@
         <v>27</v>
       </c>
       <c r="I39" s="18" t="s">
-        <v>504</v>
+        <v>500</v>
       </c>
       <c r="J39" s="18" t="s">
-        <v>505</v>
+        <v>501</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="14.4">
@@ -25305,7 +25327,7 @@
         <v>23</v>
       </c>
       <c r="E40" s="18" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="F40" s="18" t="s">
         <v>29</v>
@@ -25317,10 +25339,10 @@
         <v>27</v>
       </c>
       <c r="I40" s="18" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="J40" s="18" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="14.4">
@@ -25328,31 +25350,46 @@
         <v>23</v>
       </c>
       <c r="E41" s="18" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="F41" s="18" t="s">
         <v>29</v>
       </c>
       <c r="G41" s="18" t="s">
-        <v>510</v>
+        <v>128</v>
       </c>
       <c r="H41" s="17" t="s">
         <v>27</v>
       </c>
       <c r="I41" s="18" t="s">
+        <v>507</v>
+      </c>
+      <c r="J41" s="18" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" ht="14.4">
+      <c r="A42" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="E42" s="18" t="s">
+        <v>509</v>
+      </c>
+      <c r="F42" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="G42" s="18" t="s">
+        <v>510</v>
+      </c>
+      <c r="H42" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="I42" s="18" t="s">
         <v>511</v>
       </c>
-      <c r="J41" s="18" t="s">
+      <c r="J42" s="18" t="s">
         <v>512</v>
       </c>
-    </row>
-    <row r="42" spans="1:10" ht="14.4">
-      <c r="A42" s="6"/>
-      <c r="E42" s="7"/>
-      <c r="F42" s="7"/>
-      <c r="G42" s="7"/>
-      <c r="I42" s="7"/>
-      <c r="J42" s="7"/>
     </row>
     <row r="43" spans="1:10" ht="14.4">
       <c r="A43" s="6"/>
@@ -25361,6 +25398,14 @@
       <c r="G43" s="7"/>
       <c r="I43" s="7"/>
       <c r="J43" s="7"/>
+    </row>
+    <row r="44" spans="1:10" ht="14.4">
+      <c r="A44" s="6"/>
+      <c r="E44" s="7"/>
+      <c r="F44" s="7"/>
+      <c r="G44" s="7"/>
+      <c r="I44" s="7"/>
+      <c r="J44" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Get MAXSNOW working. Get rid of the NaN in STORAGE_YR. FLOWreports_NSantiam.xml - Add "FLOW MAXSNOW analysis" report. Flow.cpp, .h - #define MAXSNOW and STORAGE_YR. Replace misnamed m_colHruMaxSWE with m_colMAXSNOW, and replace m_colStorage_yr with m_colSTORAGE_YR. In ReadState(), initialize pHRU->m_initStorage, pHRU->m_endingStorage, and IDU attribute STORAGE_YR in 2 places. In FlowModel::StartYear(), initialize MAXSNOW to 0. Rewrite GetMaxSnowPack(). In ResetCumulativeYearlyValues(), correct the calculation of pHRU->m_endingStorage. HBV.cpp - Add logic to calculate pHRU->m_snowpackFlag.
</commit_message>
<xml_diff>
--- a/DataCW3M/CW3MdigitalHandbook/CW3MdataDictionary.xlsx
+++ b/DataCW3M/CW3MdigitalHandbook/CW3MdataDictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\CW3MdigitalHandbook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B7ED2B9-424D-4CF6-9791-CFC61C984E6A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C62EEC5-8C73-4039-BDD5-B0CE3A3C75C3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-7425" windowWidth="29040" windowHeight="17640" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Necessary input data" sheetId="7" r:id="rId1"/>
@@ -96,7 +96,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3083" uniqueCount="1039">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3088" uniqueCount="1042">
   <si>
     <t>LULC_A</t>
   </si>
@@ -1947,9 +1947,6 @@
     <t>annual snow sublimation</t>
   </si>
   <si>
-    <t>daily snowpack mass as snow water equivalent</t>
-  </si>
-  <si>
     <t>used in MCfire</t>
   </si>
   <si>
@@ -3214,6 +3211,18 @@
   </si>
   <si>
     <t>from HBV.csv for the HRU's HBVCALIB value</t>
+  </si>
+  <si>
+    <t>mmSWE</t>
+  </si>
+  <si>
+    <t>GetMaxSnowPack()</t>
+  </si>
+  <si>
+    <t>SWE in this IDU (SNOW_BOX + MELT_BOX) on the day of the year on which the entire study area's snowpack is the largest</t>
+  </si>
+  <si>
+    <t>daily snowpack mass as snow water equivalent (BOX_SNOW only, not including BOX_MELT)</t>
   </si>
 </sst>
 </file>
@@ -3912,7 +3921,7 @@
   <sheetData>
     <row r="1" spans="1:21" ht="14.25" customHeight="1">
       <c r="A1" s="4" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="7"/>
@@ -5627,13 +5636,13 @@
         <v>159</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="D50" s="10" t="s">
         <v>29</v>
       </c>
       <c r="E50" s="10" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="F50" s="10" t="s">
         <v>34</v>
@@ -5642,7 +5651,7 @@
         <v>30</v>
       </c>
       <c r="H50" s="25" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="I50" s="27"/>
       <c r="J50" s="3"/>
@@ -5669,7 +5678,7 @@
         <v>23</v>
       </c>
       <c r="C51" s="7" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="D51" s="27"/>
       <c r="E51" s="27" t="s">
@@ -5677,15 +5686,15 @@
       </c>
       <c r="F51" s="27"/>
       <c r="G51" s="27" t="s">
+        <v>631</v>
+      </c>
+      <c r="H51" s="25" t="s">
         <v>632</v>
-      </c>
-      <c r="H51" s="25" t="s">
-        <v>633</v>
       </c>
       <c r="I51" s="10"/>
       <c r="J51" s="3"/>
       <c r="K51" s="7" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="L51" s="7"/>
       <c r="M51" s="7"/>
@@ -5704,14 +5713,14 @@
         <v>23</v>
       </c>
       <c r="C52" s="7" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="D52" s="10"/>
       <c r="E52" s="10"/>
       <c r="F52" s="10"/>
       <c r="G52" s="10"/>
       <c r="H52" s="25" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="I52" s="10"/>
       <c r="J52" s="3"/>
@@ -5737,14 +5746,14 @@
       </c>
       <c r="D53" s="10"/>
       <c r="E53" s="10" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="F53" s="10"/>
       <c r="G53" s="10" t="s">
         <v>30</v>
       </c>
       <c r="H53" s="25" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="I53" s="10"/>
       <c r="J53" s="3"/>
@@ -5768,18 +5777,18 @@
         <v>23</v>
       </c>
       <c r="C54" s="7" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="D54" s="10"/>
       <c r="E54" s="10" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="F54" s="10"/>
       <c r="G54" s="10" t="s">
         <v>30</v>
       </c>
       <c r="H54" s="25" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="I54" s="10"/>
       <c r="J54" s="3"/>
@@ -5803,7 +5812,7 @@
         <v>23</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="D55" s="10"/>
       <c r="E55" s="10"/>
@@ -5841,7 +5850,7 @@
         <v>27</v>
       </c>
       <c r="H56" s="25" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="I56" s="27"/>
       <c r="J56" s="3"/>
@@ -5865,7 +5874,7 @@
         <v>23</v>
       </c>
       <c r="C57" s="7" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="D57" s="10"/>
       <c r="E57" s="10" t="s">
@@ -5876,7 +5885,7 @@
         <v>30</v>
       </c>
       <c r="H57" s="25" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="I57" s="27"/>
       <c r="J57" s="3"/>
@@ -5898,7 +5907,7 @@
         <v>23</v>
       </c>
       <c r="C58" s="7" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="D58" s="10"/>
       <c r="E58" s="10" t="s">
@@ -5907,7 +5916,7 @@
       <c r="F58" s="10"/>
       <c r="G58" s="10"/>
       <c r="H58" s="25" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="I58" s="27"/>
       <c r="J58" s="3"/>
@@ -5940,7 +5949,7 @@
         <v>27</v>
       </c>
       <c r="H59" s="72" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="I59" s="27" t="s">
         <v>113</v>
@@ -5964,7 +5973,7 @@
       <c r="A60" s="28"/>
       <c r="B60" s="28"/>
       <c r="C60" s="7" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="D60" s="10" t="s">
         <v>29</v>
@@ -5973,16 +5982,16 @@
         <v>226</v>
       </c>
       <c r="F60" s="10" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="G60" s="10" t="s">
         <v>27</v>
       </c>
       <c r="H60" s="72" t="s">
+        <v>825</v>
+      </c>
+      <c r="I60" s="27" t="s">
         <v>826</v>
-      </c>
-      <c r="I60" s="27" t="s">
-        <v>827</v>
       </c>
       <c r="J60" s="3"/>
       <c r="K60" s="3"/>
@@ -5999,7 +6008,7 @@
     </row>
     <row r="61" spans="1:26" ht="14.25" customHeight="1">
       <c r="A61" s="28" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="B61" s="28" t="s">
         <v>23</v>
@@ -6016,7 +6025,7 @@
         <v>30</v>
       </c>
       <c r="H61" s="25" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="I61" s="10"/>
       <c r="J61" s="3"/>
@@ -9184,9 +9193,9 @@
   </sheetPr>
   <dimension ref="A1:Z1051"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C68" sqref="C68"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A160" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A173" sqref="A173:XFD173"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -9207,7 +9216,7 @@
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
       <c r="A1" s="2" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="7"/>
@@ -9821,7 +9830,7 @@
       </c>
       <c r="J18" s="68"/>
       <c r="K18" s="71" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="L18" s="64"/>
       <c r="M18" s="64"/>
@@ -10769,7 +10778,7 @@
       <c r="F45" s="10"/>
       <c r="G45" s="8"/>
       <c r="H45" s="72" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="I45" s="26" t="s">
         <v>260</v>
@@ -10915,7 +10924,7 @@
       <c r="A50" s="28"/>
       <c r="B50" s="28"/>
       <c r="C50" s="7" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="D50" s="10" t="s">
         <v>108</v>
@@ -10928,10 +10937,10 @@
         <v>30</v>
       </c>
       <c r="H50" s="25" t="s">
+        <v>1026</v>
+      </c>
+      <c r="I50" s="27" t="s">
         <v>1027</v>
-      </c>
-      <c r="I50" s="27" t="s">
-        <v>1028</v>
       </c>
       <c r="J50" s="3"/>
       <c r="K50" s="7"/>
@@ -11274,27 +11283,27 @@
       </c>
       <c r="B62" s="13"/>
       <c r="C62" s="25" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="D62" s="79" t="s">
         <v>46</v>
       </c>
       <c r="E62" s="79" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="F62" s="79" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="G62" s="79" t="s">
         <v>30</v>
       </c>
       <c r="H62" s="77" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="I62" s="46"/>
       <c r="J62" s="80"/>
       <c r="K62" s="72" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
     </row>
     <row r="63" spans="1:21" s="65" customFormat="1" ht="14.25" customHeight="1">
@@ -11323,7 +11332,7 @@
       </c>
       <c r="J63" s="68"/>
       <c r="K63" s="71" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="L63" s="64"/>
       <c r="M63" s="64"/>
@@ -11449,20 +11458,20 @@
       <c r="A67" s="28"/>
       <c r="B67" s="28"/>
       <c r="C67" s="7" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
       <c r="D67" s="10" t="s">
         <v>108</v>
       </c>
       <c r="E67" s="10" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="F67" s="10"/>
       <c r="G67" s="10" t="s">
         <v>27</v>
       </c>
       <c r="H67" s="25" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
       <c r="I67" s="27"/>
       <c r="J67" s="3"/>
@@ -12770,11 +12779,21 @@
       <c r="C104" s="7" t="s">
         <v>459</v>
       </c>
-      <c r="D104" s="8"/>
-      <c r="E104" s="8"/>
-      <c r="F104" s="10"/>
-      <c r="G104" s="8"/>
-      <c r="H104" s="14"/>
+      <c r="D104" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E104" s="8" t="s">
+        <v>1038</v>
+      </c>
+      <c r="F104" s="10" t="s">
+        <v>1039</v>
+      </c>
+      <c r="G104" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="H104" s="21" t="s">
+        <v>1040</v>
+      </c>
       <c r="I104" s="27"/>
       <c r="J104" s="3"/>
       <c r="K104" s="7"/>
@@ -13482,18 +13501,18 @@
       <c r="A125" s="28"/>
       <c r="B125" s="28"/>
       <c r="C125" s="7" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="D125" s="10"/>
       <c r="E125" s="10" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="F125" s="10" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="G125" s="10"/>
       <c r="H125" s="25" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="I125" s="27" t="s">
         <v>113</v>
@@ -13515,18 +13534,18 @@
       <c r="A126" s="28"/>
       <c r="B126" s="28"/>
       <c r="C126" s="7" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="D126" s="10"/>
       <c r="E126" s="10" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="F126" s="10" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="G126" s="10"/>
       <c r="H126" s="25" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="I126" s="27" t="s">
         <v>113</v>
@@ -13548,18 +13567,18 @@
       <c r="A127" s="28"/>
       <c r="B127" s="28"/>
       <c r="C127" s="7" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="D127" s="10"/>
       <c r="E127" s="10" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="F127" s="10" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="G127" s="10"/>
       <c r="H127" s="25" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="I127" s="27" t="s">
         <v>113</v>
@@ -13581,18 +13600,18 @@
       <c r="A128" s="28"/>
       <c r="B128" s="28"/>
       <c r="C128" s="7" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="D128" s="10"/>
       <c r="E128" s="10" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="F128" s="10" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="G128" s="10"/>
       <c r="H128" s="25" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="I128" s="27" t="s">
         <v>113</v>
@@ -13652,22 +13671,22 @@
     <row r="130" spans="1:26" s="21" customFormat="1" ht="14.25" customHeight="1">
       <c r="B130" s="28"/>
       <c r="C130" s="21" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="D130" s="10" t="s">
         <v>29</v>
       </c>
       <c r="E130" s="10" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="F130" s="10" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="G130" s="10" t="s">
         <v>27</v>
       </c>
       <c r="H130" s="21" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="I130" s="27" t="s">
         <v>113</v>
@@ -13677,22 +13696,22 @@
     <row r="131" spans="1:26" s="21" customFormat="1" ht="14.25" customHeight="1">
       <c r="B131" s="28"/>
       <c r="C131" s="21" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="D131" s="10" t="s">
         <v>29</v>
       </c>
       <c r="E131" s="10" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="F131" s="10" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="G131" s="10" t="s">
         <v>27</v>
       </c>
       <c r="H131" s="21" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="I131" s="27" t="s">
         <v>113</v>
@@ -13702,22 +13721,22 @@
     <row r="132" spans="1:26" s="21" customFormat="1" ht="14.25" customHeight="1">
       <c r="B132" s="28"/>
       <c r="C132" s="21" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="D132" s="10" t="s">
         <v>29</v>
       </c>
       <c r="E132" s="10" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="F132" s="10" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="G132" s="10" t="s">
         <v>27</v>
       </c>
       <c r="H132" s="21" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="I132" s="27" t="s">
         <v>113</v>
@@ -13727,22 +13746,22 @@
     <row r="133" spans="1:26" s="21" customFormat="1" ht="14.25" customHeight="1">
       <c r="B133" s="28"/>
       <c r="C133" s="21" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="D133" s="10" t="s">
         <v>29</v>
       </c>
       <c r="E133" s="10" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="F133" s="10" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="G133" s="10" t="s">
         <v>27</v>
       </c>
       <c r="H133" s="21" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="I133" s="27" t="s">
         <v>113</v>
@@ -13753,18 +13772,18 @@
       <c r="A134" s="10"/>
       <c r="B134" s="28"/>
       <c r="C134" s="21" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="D134" s="10"/>
       <c r="E134" s="10" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="F134" s="10" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="G134" s="10"/>
       <c r="H134" s="21" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="I134" s="27" t="s">
         <v>113</v>
@@ -13775,18 +13794,18 @@
       <c r="A135" s="10"/>
       <c r="B135" s="28"/>
       <c r="C135" s="21" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="D135" s="10"/>
       <c r="E135" s="10" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="F135" s="10" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="G135" s="10"/>
       <c r="H135" s="21" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="I135" s="27" t="s">
         <v>113</v>
@@ -13871,7 +13890,7 @@
       </c>
       <c r="D138" s="8"/>
       <c r="E138" s="10" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="F138" s="10"/>
       <c r="G138" s="8" t="s">
@@ -13941,7 +13960,7 @@
       </c>
       <c r="D140" s="8"/>
       <c r="E140" s="10" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="F140" s="10"/>
       <c r="G140" s="8" t="s">
@@ -14316,7 +14335,7 @@
       <c r="A150" s="28"/>
       <c r="B150" s="28"/>
       <c r="C150" s="7" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="D150" s="70" t="s">
         <v>29</v>
@@ -14331,10 +14350,10 @@
         <v>27</v>
       </c>
       <c r="H150" s="72" t="s">
+        <v>811</v>
+      </c>
+      <c r="I150" s="70" t="s">
         <v>812</v>
-      </c>
-      <c r="I150" s="70" t="s">
-        <v>813</v>
       </c>
       <c r="J150" s="3"/>
       <c r="K150" s="7"/>
@@ -15026,7 +15045,7 @@
         <v>27</v>
       </c>
       <c r="H169" s="76" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="I169" s="74" t="s">
         <v>113</v>
@@ -15106,7 +15125,7 @@
         <v>612</v>
       </c>
       <c r="I171" s="26" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="J171" s="3"/>
       <c r="K171" s="7"/>
@@ -15161,52 +15180,41 @@
       <c r="Y172" s="35"/>
       <c r="Z172" s="35"/>
     </row>
-    <row r="173" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A173" s="28"/>
-      <c r="B173" s="6"/>
-      <c r="C173" s="18" t="s">
+    <row r="173" spans="1:26" s="25" customFormat="1" ht="28.8">
+      <c r="A173" s="13"/>
+      <c r="B173" s="13"/>
+      <c r="C173" s="25" t="s">
         <v>492</v>
       </c>
-      <c r="D173" s="10" t="s">
+      <c r="D173" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="E173" s="10" t="s">
+      <c r="E173" s="9" t="s">
         <v>494</v>
       </c>
-      <c r="F173" s="10" t="s">
+      <c r="F173" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="G173" s="10" t="s">
+      <c r="G173" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="H173" s="25" t="s">
-        <v>616</v>
-      </c>
-      <c r="I173" s="27" t="s">
-        <v>815</v>
-      </c>
-      <c r="J173" s="3"/>
-      <c r="K173" s="7"/>
-      <c r="L173" s="7"/>
-      <c r="M173" s="7"/>
-      <c r="N173" s="7"/>
-      <c r="O173" s="7"/>
-      <c r="P173" s="7"/>
-      <c r="Q173" s="7"/>
-      <c r="R173" s="7"/>
-      <c r="S173" s="7"/>
-      <c r="T173" s="7"/>
-      <c r="U173" s="7"/>
+      <c r="H173" s="72" t="s">
+        <v>1041</v>
+      </c>
+      <c r="I173" s="46" t="s">
+        <v>814</v>
+      </c>
+      <c r="J173" s="80"/>
     </row>
     <row r="174" spans="1:26" ht="14.25" customHeight="1">
       <c r="A174" s="28" t="s">
+        <v>616</v>
+      </c>
+      <c r="B174" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C174" s="7" t="s">
         <v>617</v>
-      </c>
-      <c r="B174" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C174" s="7" t="s">
-        <v>618</v>
       </c>
       <c r="D174" s="8"/>
       <c r="E174" s="8"/>
@@ -15215,7 +15223,7 @@
         <v>27</v>
       </c>
       <c r="H174" s="14" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="I174" s="27" t="s">
         <v>113</v>
@@ -15239,7 +15247,7 @@
         <v>23</v>
       </c>
       <c r="C175" s="30" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="D175" s="31"/>
       <c r="E175" s="31"/>
@@ -15248,7 +15256,7 @@
         <v>27</v>
       </c>
       <c r="H175" s="32" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="I175" s="33" t="s">
         <v>113</v>
@@ -15275,7 +15283,7 @@
       <c r="A176" s="66"/>
       <c r="B176" s="66"/>
       <c r="C176" s="65" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="D176" s="62" t="s">
         <v>29</v>
@@ -15290,7 +15298,7 @@
         <v>27</v>
       </c>
       <c r="H176" s="61" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="I176" s="74"/>
       <c r="J176" s="68"/>
@@ -15316,13 +15324,13 @@
         <v>159</v>
       </c>
       <c r="C177" s="7" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="D177" s="8" t="s">
         <v>29</v>
       </c>
       <c r="E177" s="8" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="F177" s="10" t="s">
         <v>34</v>
@@ -15331,7 +15339,7 @@
         <v>30</v>
       </c>
       <c r="H177" s="14" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="I177" s="27"/>
       <c r="J177" s="3"/>
@@ -15358,7 +15366,7 @@
         <v>23</v>
       </c>
       <c r="C178" s="7" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="D178" s="8"/>
       <c r="E178" s="8" t="s">
@@ -15369,14 +15377,14 @@
         <v>27</v>
       </c>
       <c r="H178" s="14" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="I178" s="27" t="s">
         <v>113</v>
       </c>
       <c r="J178" s="3"/>
       <c r="K178" s="18" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="L178" s="7"/>
       <c r="M178" s="7"/>
@@ -15399,7 +15407,7 @@
         <v>29</v>
       </c>
       <c r="E179" s="27" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="F179" s="27" t="s">
         <v>34</v>
@@ -15408,7 +15416,7 @@
         <v>27</v>
       </c>
       <c r="H179" s="25" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="I179" s="10" t="s">
         <v>498</v>
@@ -15432,7 +15440,7 @@
         <v>23</v>
       </c>
       <c r="C180" s="7" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="D180" s="27"/>
       <c r="E180" s="27" t="s">
@@ -15440,15 +15448,15 @@
       </c>
       <c r="F180" s="27"/>
       <c r="G180" s="27" t="s">
+        <v>631</v>
+      </c>
+      <c r="H180" s="14" t="s">
         <v>632</v>
-      </c>
-      <c r="H180" s="14" t="s">
-        <v>633</v>
       </c>
       <c r="I180" s="8"/>
       <c r="J180" s="3"/>
       <c r="K180" s="7" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="L180" s="7"/>
       <c r="M180" s="7"/>
@@ -15467,19 +15475,19 @@
         <v>23</v>
       </c>
       <c r="C181" s="7" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="D181" s="8"/>
       <c r="E181" s="8"/>
       <c r="F181" s="10"/>
       <c r="G181" s="8"/>
       <c r="H181" s="14" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="I181" s="8"/>
       <c r="J181" s="3"/>
       <c r="K181" s="3" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="L181" s="7"/>
       <c r="M181" s="7"/>
@@ -15494,11 +15502,11 @@
     </row>
     <row r="182" spans="1:26" ht="14.25" customHeight="1">
       <c r="A182" s="12" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="B182" s="6"/>
       <c r="C182" s="18" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="D182" s="10" t="s">
         <v>46</v>
@@ -15511,10 +15519,10 @@
         <v>27</v>
       </c>
       <c r="H182" s="25" t="s">
+        <v>639</v>
+      </c>
+      <c r="I182" s="10" t="s">
         <v>640</v>
-      </c>
-      <c r="I182" s="10" t="s">
-        <v>641</v>
       </c>
       <c r="J182" s="3"/>
       <c r="K182" s="7"/>
@@ -15535,7 +15543,7 @@
         <v>23</v>
       </c>
       <c r="C183" s="7" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="D183" s="8"/>
       <c r="E183" s="8"/>
@@ -15562,14 +15570,14 @@
         <v>23</v>
       </c>
       <c r="C184" s="7" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="D184" s="8"/>
       <c r="E184" s="8"/>
       <c r="F184" s="10"/>
       <c r="G184" s="8"/>
       <c r="H184" s="14" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="I184" s="8"/>
       <c r="J184" s="3"/>
@@ -15591,14 +15599,14 @@
         <v>159</v>
       </c>
       <c r="C185" s="7" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="D185" s="8"/>
       <c r="E185" s="8"/>
       <c r="F185" s="10"/>
       <c r="G185" s="8"/>
       <c r="H185" s="14" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="I185" s="27" t="s">
         <v>113</v>
@@ -15629,7 +15637,7 @@
       <c r="F186" s="10"/>
       <c r="G186" s="8"/>
       <c r="H186" s="25" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="I186" s="8"/>
       <c r="J186" s="3"/>
@@ -15655,14 +15663,14 @@
       </c>
       <c r="D187" s="8"/>
       <c r="E187" s="8" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="F187" s="10"/>
       <c r="G187" s="8" t="s">
         <v>30</v>
       </c>
       <c r="H187" s="14" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="I187" s="8"/>
       <c r="J187" s="3"/>
@@ -15686,18 +15694,18 @@
         <v>23</v>
       </c>
       <c r="C188" s="7" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="D188" s="8"/>
       <c r="E188" s="8" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="F188" s="10"/>
       <c r="G188" s="8" t="s">
         <v>30</v>
       </c>
       <c r="H188" s="14" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="I188" s="8"/>
       <c r="J188" s="3"/>
@@ -15721,7 +15729,7 @@
         <v>23</v>
       </c>
       <c r="C189" s="7" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="D189" s="8"/>
       <c r="E189" s="8"/>
@@ -15746,7 +15754,7 @@
       <c r="A190" s="66"/>
       <c r="B190" s="66"/>
       <c r="C190" s="65" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="D190" s="62" t="s">
         <v>29</v>
@@ -15759,7 +15767,7 @@
         <v>27</v>
       </c>
       <c r="H190" s="61" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="I190" s="62" t="s">
         <v>113</v>
@@ -15781,7 +15789,7 @@
       <c r="A191" s="66"/>
       <c r="B191" s="66"/>
       <c r="C191" s="65" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="D191" s="62" t="s">
         <v>29</v>
@@ -15794,7 +15802,7 @@
         <v>27</v>
       </c>
       <c r="H191" s="61" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="I191" s="62" t="s">
         <v>113</v>
@@ -15818,7 +15826,7 @@
         <v>159</v>
       </c>
       <c r="C192" s="7" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="D192" s="8"/>
       <c r="E192" s="8" t="s">
@@ -15827,12 +15835,12 @@
       <c r="F192" s="10"/>
       <c r="G192" s="8"/>
       <c r="H192" s="14" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="I192" s="8"/>
       <c r="J192" s="3"/>
       <c r="K192" s="3" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="L192" s="7"/>
       <c r="M192" s="7"/>
@@ -15851,21 +15859,21 @@
         <v>159</v>
       </c>
       <c r="C193" s="7" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="D193" s="8"/>
       <c r="E193" s="8" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="F193" s="10"/>
       <c r="G193" s="8"/>
       <c r="H193" s="14" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="I193" s="8"/>
       <c r="J193" s="3"/>
       <c r="K193" s="3" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="L193" s="7"/>
       <c r="M193" s="7"/>
@@ -15884,7 +15892,7 @@
         <v>159</v>
       </c>
       <c r="C194" s="7" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="D194" s="8"/>
       <c r="E194" s="8" t="s">
@@ -15893,7 +15901,7 @@
       <c r="F194" s="10"/>
       <c r="G194" s="8"/>
       <c r="H194" s="14" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="I194" s="8"/>
       <c r="J194" s="3"/>
@@ -15915,7 +15923,7 @@
         <v>159</v>
       </c>
       <c r="C195" s="7" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="D195" s="8"/>
       <c r="E195" s="8" t="s">
@@ -15924,7 +15932,7 @@
       <c r="F195" s="10"/>
       <c r="G195" s="8"/>
       <c r="H195" s="14" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="I195" s="8"/>
       <c r="J195" s="3"/>
@@ -15957,7 +15965,7 @@
         <v>27</v>
       </c>
       <c r="H196" s="14" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="I196" s="8"/>
       <c r="J196" s="3"/>
@@ -15979,7 +15987,7 @@
         <v>23</v>
       </c>
       <c r="C197" s="7" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="D197" s="8"/>
       <c r="E197" s="8" t="s">
@@ -15990,10 +15998,10 @@
         <v>27</v>
       </c>
       <c r="H197" s="14" t="s">
+        <v>670</v>
+      </c>
+      <c r="I197" s="8" t="s">
         <v>671</v>
-      </c>
-      <c r="I197" s="8" t="s">
-        <v>672</v>
       </c>
       <c r="J197" s="3"/>
       <c r="K197" s="5"/>
@@ -16014,7 +16022,7 @@
         <v>23</v>
       </c>
       <c r="C198" s="7" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="D198" s="8"/>
       <c r="E198" s="8" t="s">
@@ -16025,7 +16033,7 @@
         <v>27</v>
       </c>
       <c r="H198" s="14" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="I198" s="27" t="s">
         <v>113</v>
@@ -16058,10 +16066,10 @@
         <v>27</v>
       </c>
       <c r="H199" s="25" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="I199" s="26" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="J199" s="3"/>
       <c r="L199" s="7"/>
@@ -16090,10 +16098,10 @@
         <v>27</v>
       </c>
       <c r="H200" s="25" t="s">
+        <v>679</v>
+      </c>
+      <c r="I200" s="26" t="s">
         <v>680</v>
-      </c>
-      <c r="I200" s="26" t="s">
-        <v>681</v>
       </c>
       <c r="J200" s="3"/>
       <c r="L200" s="7"/>
@@ -16111,7 +16119,7 @@
       <c r="A201" s="28"/>
       <c r="B201" s="28"/>
       <c r="C201" s="21" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="D201" s="10" t="s">
         <v>29</v>
@@ -16120,11 +16128,11 @@
         <v>128</v>
       </c>
       <c r="F201" s="10" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="G201" s="10"/>
       <c r="H201" s="25" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="I201" s="27"/>
       <c r="J201" s="3"/>
@@ -16142,7 +16150,7 @@
     <row r="202" spans="1:21" s="21" customFormat="1" ht="14.25" customHeight="1">
       <c r="B202" s="28"/>
       <c r="C202" s="21" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="D202" s="10" t="s">
         <v>29</v>
@@ -16151,13 +16159,13 @@
         <v>128</v>
       </c>
       <c r="F202" s="10" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="G202" s="10" t="s">
         <v>27</v>
       </c>
       <c r="H202" s="25" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="I202" s="27" t="s">
         <v>113</v>
@@ -16179,13 +16187,13 @@
       <c r="A203" s="101"/>
       <c r="B203" s="96"/>
       <c r="C203" s="91" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="D203" s="100" t="s">
         <v>29</v>
       </c>
       <c r="E203" s="100" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="F203" s="100" t="s">
         <v>217</v>
@@ -16194,7 +16202,7 @@
         <v>27</v>
       </c>
       <c r="H203" s="102" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="I203" s="98" t="s">
         <v>113</v>
@@ -16217,7 +16225,7 @@
         <v>23</v>
       </c>
       <c r="C204" s="7" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="D204" s="8"/>
       <c r="E204" s="8" t="s">
@@ -16228,7 +16236,7 @@
         <v>27</v>
       </c>
       <c r="H204" s="14" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="I204" s="27" t="s">
         <v>113</v>
@@ -16251,7 +16259,7 @@
         <v>159</v>
       </c>
       <c r="C205" s="7" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="D205" s="8"/>
       <c r="E205" s="8" t="s">
@@ -16262,14 +16270,14 @@
         <v>27</v>
       </c>
       <c r="H205" s="14" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="I205" s="27" t="s">
         <v>113</v>
       </c>
       <c r="J205" s="3"/>
       <c r="K205" s="3" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="L205" s="7"/>
       <c r="M205" s="7"/>
@@ -16288,7 +16296,7 @@
         <v>23</v>
       </c>
       <c r="C206" s="7" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="D206" s="8"/>
       <c r="E206" s="8" t="s">
@@ -16299,7 +16307,7 @@
         <v>30</v>
       </c>
       <c r="H206" s="14" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="I206" s="27"/>
       <c r="J206" s="3"/>
@@ -16321,7 +16329,7 @@
         <v>159</v>
       </c>
       <c r="C207" s="7" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="D207" s="8"/>
       <c r="E207" s="8" t="s">
@@ -16332,7 +16340,7 @@
         <v>30</v>
       </c>
       <c r="H207" s="14" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="I207" s="27"/>
       <c r="J207" s="3"/>
@@ -16365,7 +16373,7 @@
         <v>27</v>
       </c>
       <c r="H208" s="14" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="I208" s="27"/>
       <c r="J208" s="3"/>
@@ -16389,7 +16397,7 @@
         <v>23</v>
       </c>
       <c r="C209" s="7" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D209" s="8"/>
       <c r="E209" s="8"/>
@@ -16416,7 +16424,7 @@
         <v>23</v>
       </c>
       <c r="C210" s="7" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="D210" s="8"/>
       <c r="E210" s="8" t="s">
@@ -16427,7 +16435,7 @@
         <v>30</v>
       </c>
       <c r="H210" s="14" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="I210" s="27"/>
       <c r="J210" s="3"/>
@@ -16449,7 +16457,7 @@
         <v>23</v>
       </c>
       <c r="C211" s="7" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="D211" s="8"/>
       <c r="E211" s="8" t="s">
@@ -16458,7 +16466,7 @@
       <c r="F211" s="10"/>
       <c r="G211" s="8"/>
       <c r="H211" s="14" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="I211" s="27"/>
       <c r="J211" s="3"/>
@@ -16480,7 +16488,7 @@
         <v>159</v>
       </c>
       <c r="C212" s="7" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="D212" s="8"/>
       <c r="E212" s="8" t="s">
@@ -16491,7 +16499,7 @@
         <v>27</v>
       </c>
       <c r="H212" s="14" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="I212" s="27" t="s">
         <v>113</v>
@@ -16515,7 +16523,7 @@
         <v>159</v>
       </c>
       <c r="C213" s="7" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="D213" s="8"/>
       <c r="E213" s="8" t="s">
@@ -16526,7 +16534,7 @@
         <v>27</v>
       </c>
       <c r="H213" s="14" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="I213" s="27" t="s">
         <v>113</v>
@@ -16550,7 +16558,7 @@
         <v>159</v>
       </c>
       <c r="C214" s="7" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="D214" s="8"/>
       <c r="E214" s="8" t="s">
@@ -16561,7 +16569,7 @@
         <v>27</v>
       </c>
       <c r="H214" s="14" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="I214" s="27" t="s">
         <v>113</v>
@@ -16585,7 +16593,7 @@
         <v>159</v>
       </c>
       <c r="C215" s="7" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="D215" s="8"/>
       <c r="E215" s="8" t="s">
@@ -16596,7 +16604,7 @@
         <v>27</v>
       </c>
       <c r="H215" s="14" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="I215" s="27" t="s">
         <v>113</v>
@@ -16620,7 +16628,7 @@
         <v>159</v>
       </c>
       <c r="C216" s="7" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="D216" s="8"/>
       <c r="E216" s="8" t="s">
@@ -16631,7 +16639,7 @@
         <v>27</v>
       </c>
       <c r="H216" s="14" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="I216" s="27" t="s">
         <v>113</v>
@@ -16655,7 +16663,7 @@
         <v>159</v>
       </c>
       <c r="C217" s="7" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="D217" s="8"/>
       <c r="E217" s="8"/>
@@ -16678,13 +16686,13 @@
     </row>
     <row r="218" spans="1:21" ht="14.25" customHeight="1">
       <c r="A218" s="6" t="s">
+        <v>708</v>
+      </c>
+      <c r="B218" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C218" s="7" t="s">
         <v>709</v>
-      </c>
-      <c r="B218" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C218" s="7" t="s">
-        <v>710</v>
       </c>
       <c r="D218" s="8"/>
       <c r="E218" s="8" t="s">
@@ -16697,7 +16705,7 @@
         <v>27</v>
       </c>
       <c r="H218" s="14" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="I218" s="27" t="s">
         <v>113</v>
@@ -16732,7 +16740,7 @@
         <v>27</v>
       </c>
       <c r="H219" s="14" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="I219" s="27" t="s">
         <v>113</v>
@@ -16754,13 +16762,13 @@
     </row>
     <row r="220" spans="1:21" ht="14.25" customHeight="1">
       <c r="A220" s="28" t="s">
+        <v>712</v>
+      </c>
+      <c r="B220" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C220" s="7" t="s">
         <v>713</v>
-      </c>
-      <c r="B220" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C220" s="7" t="s">
-        <v>714</v>
       </c>
       <c r="D220" s="8"/>
       <c r="E220" s="8" t="s">
@@ -16771,7 +16779,7 @@
         <v>27</v>
       </c>
       <c r="H220" s="14" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="I220" s="27" t="s">
         <v>113</v>
@@ -16795,25 +16803,25 @@
         <v>23</v>
       </c>
       <c r="C221" s="7" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="D221" s="8"/>
       <c r="E221" s="8" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="F221" s="10"/>
       <c r="G221" s="8" t="s">
         <v>27</v>
       </c>
       <c r="H221" s="14" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="I221" s="27" t="s">
         <v>113</v>
       </c>
       <c r="J221" s="3"/>
       <c r="K221" s="3" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="L221" s="7"/>
       <c r="M221" s="7"/>
@@ -16832,7 +16840,7 @@
         <v>23</v>
       </c>
       <c r="C222" s="7" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="D222" s="8"/>
       <c r="E222" s="8" t="s">
@@ -16843,14 +16851,14 @@
         <v>27</v>
       </c>
       <c r="H222" s="14" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="I222" s="27" t="s">
         <v>113</v>
       </c>
       <c r="J222" s="3"/>
       <c r="K222" s="56" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="L222" s="7"/>
       <c r="M222" s="7"/>
@@ -16869,7 +16877,7 @@
         <v>159</v>
       </c>
       <c r="C223" s="7" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="D223" s="8"/>
       <c r="E223" s="8"/>
@@ -16896,7 +16904,7 @@
         <v>159</v>
       </c>
       <c r="C224" s="7" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="D224" s="8"/>
       <c r="E224" s="8"/>
@@ -16923,7 +16931,7 @@
         <v>159</v>
       </c>
       <c r="C225" s="7" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="D225" s="8"/>
       <c r="E225" s="8" t="s">
@@ -16934,10 +16942,10 @@
         <v>27</v>
       </c>
       <c r="H225" s="14" t="s">
+        <v>725</v>
+      </c>
+      <c r="I225" s="27" t="s">
         <v>726</v>
-      </c>
-      <c r="I225" s="27" t="s">
-        <v>727</v>
       </c>
       <c r="J225" s="3"/>
       <c r="K225" s="7"/>
@@ -16956,7 +16964,7 @@
       <c r="A226" s="28"/>
       <c r="B226" s="28"/>
       <c r="C226" s="7" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="D226" s="10" t="s">
         <v>108</v>
@@ -16969,7 +16977,7 @@
         <v>30</v>
       </c>
       <c r="H226" s="25" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="I226" s="27" t="s">
         <v>529</v>
@@ -16991,7 +16999,7 @@
       <c r="A227" s="28"/>
       <c r="B227" s="28"/>
       <c r="C227" s="7" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="D227" s="10" t="s">
         <v>46</v>
@@ -17002,7 +17010,7 @@
         <v>30</v>
       </c>
       <c r="H227" s="25" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="I227" s="27"/>
       <c r="J227" s="3"/>
@@ -17022,7 +17030,7 @@
       <c r="A228" s="66"/>
       <c r="B228" s="66"/>
       <c r="C228" s="64" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="D228" s="62" t="s">
         <v>29</v>
@@ -17037,10 +17045,10 @@
         <v>27</v>
       </c>
       <c r="H228" s="61" t="s">
+        <v>830</v>
+      </c>
+      <c r="I228" s="74" t="s">
         <v>831</v>
-      </c>
-      <c r="I228" s="74" t="s">
-        <v>832</v>
       </c>
       <c r="J228" s="68"/>
       <c r="K228" s="64"/>
@@ -17059,7 +17067,7 @@
       <c r="A229" s="96"/>
       <c r="B229" s="96"/>
       <c r="C229" s="97" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="D229" s="100" t="s">
         <v>108</v>
@@ -17072,7 +17080,7 @@
         <v>27</v>
       </c>
       <c r="H229" s="91" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="I229" s="98"/>
       <c r="J229" s="84"/>
@@ -17092,7 +17100,7 @@
       <c r="A230" s="96"/>
       <c r="B230" s="96"/>
       <c r="C230" s="97" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
       <c r="D230" s="99" t="s">
         <v>108</v>
@@ -17101,13 +17109,13 @@
         <v>172</v>
       </c>
       <c r="F230" s="99" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="G230" s="99" t="s">
         <v>27</v>
       </c>
       <c r="H230" s="77" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
       <c r="I230" s="98"/>
       <c r="J230" s="84"/>
@@ -17142,10 +17150,10 @@
         <v>27</v>
       </c>
       <c r="H231" s="21" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="I231" s="27" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="J231" s="23"/>
     </row>
@@ -17155,21 +17163,21 @@
         <v>159</v>
       </c>
       <c r="C232" s="7" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="D232" s="8"/>
       <c r="E232" s="8" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="F232" s="10"/>
       <c r="G232" s="8" t="s">
         <v>27</v>
       </c>
       <c r="H232" s="14" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="I232" s="27" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="J232" s="3"/>
       <c r="K232" s="7"/>
@@ -17190,7 +17198,7 @@
         <v>159</v>
       </c>
       <c r="C233" s="7" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="D233" s="8"/>
       <c r="E233" s="8" t="s">
@@ -17201,10 +17209,10 @@
         <v>30</v>
       </c>
       <c r="H233" s="14" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="I233" s="27" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="J233" s="3"/>
       <c r="K233" s="7"/>
@@ -17225,7 +17233,7 @@
         <v>23</v>
       </c>
       <c r="C234" s="7" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="D234" s="8"/>
       <c r="E234" s="8" t="s">
@@ -17236,10 +17244,10 @@
         <v>27</v>
       </c>
       <c r="H234" s="14" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="I234" s="27" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="J234" s="3"/>
       <c r="K234" s="7"/>
@@ -17260,7 +17268,7 @@
         <v>159</v>
       </c>
       <c r="C235" s="7" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="D235" s="8"/>
       <c r="E235" s="8" t="s">
@@ -17271,7 +17279,7 @@
         <v>30</v>
       </c>
       <c r="H235" s="14" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="I235" s="27"/>
       <c r="J235" s="3"/>
@@ -17293,7 +17301,7 @@
         <v>159</v>
       </c>
       <c r="C236" s="7" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="D236" s="8"/>
       <c r="E236" s="8" t="s">
@@ -17304,10 +17312,10 @@
         <v>27</v>
       </c>
       <c r="H236" s="14" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="I236" s="27" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="J236" s="3"/>
       <c r="K236" s="7"/>
@@ -17328,7 +17336,7 @@
         <v>159</v>
       </c>
       <c r="C237" s="7" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="D237" s="8"/>
       <c r="E237" s="8" t="s">
@@ -17339,10 +17347,10 @@
         <v>27</v>
       </c>
       <c r="H237" s="14" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="I237" s="27" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="J237" s="3"/>
       <c r="K237" s="7"/>
@@ -17363,7 +17371,7 @@
         <v>23</v>
       </c>
       <c r="C238" s="7" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="D238" s="8"/>
       <c r="E238" s="8"/>
@@ -17372,7 +17380,7 @@
         <v>27</v>
       </c>
       <c r="H238" s="14" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="I238" s="27" t="s">
         <v>113</v>
@@ -17396,18 +17404,18 @@
         <v>159</v>
       </c>
       <c r="C239" s="7" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="D239" s="8"/>
       <c r="E239" s="8" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="F239" s="10"/>
       <c r="G239" s="8" t="s">
         <v>27</v>
       </c>
       <c r="H239" s="14" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="I239" s="27" t="s">
         <v>113</v>
@@ -17433,18 +17441,18 @@
         <v>23</v>
       </c>
       <c r="C240" s="7" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="D240" s="8"/>
       <c r="E240" s="8" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="F240" s="10"/>
       <c r="G240" s="8" t="s">
         <v>27</v>
       </c>
       <c r="H240" s="14" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="I240" s="27" t="s">
         <v>113</v>
@@ -17479,7 +17487,7 @@
         <v>27</v>
       </c>
       <c r="H241" s="14" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="I241" s="27" t="s">
         <v>113</v>
@@ -17506,13 +17514,13 @@
     </row>
     <row r="242" spans="1:26" ht="14.25" customHeight="1">
       <c r="A242" s="6" t="s">
+        <v>750</v>
+      </c>
+      <c r="B242" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C242" s="7" t="s">
         <v>751</v>
-      </c>
-      <c r="B242" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C242" s="7" t="s">
-        <v>752</v>
       </c>
       <c r="D242" s="8"/>
       <c r="E242" s="8" t="s">
@@ -17523,7 +17531,7 @@
         <v>27</v>
       </c>
       <c r="H242" s="14" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="I242" s="27" t="s">
         <v>113</v>
@@ -17547,18 +17555,18 @@
         <v>23</v>
       </c>
       <c r="C243" s="7" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="D243" s="8"/>
       <c r="E243" s="8" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="F243" s="10"/>
       <c r="G243" s="8" t="s">
         <v>27</v>
       </c>
       <c r="H243" s="14" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="I243" s="27" t="s">
         <v>113</v>
@@ -17582,18 +17590,18 @@
         <v>23</v>
       </c>
       <c r="C244" s="7" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="D244" s="8"/>
       <c r="E244" s="8" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="F244" s="10"/>
       <c r="G244" s="8" t="s">
         <v>27</v>
       </c>
       <c r="H244" s="14" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="I244" s="27" t="s">
         <v>113</v>
@@ -17619,7 +17627,7 @@
         <v>23</v>
       </c>
       <c r="C245" s="8" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="D245" s="8"/>
       <c r="E245" s="8"/>
@@ -17628,7 +17636,7 @@
         <v>27</v>
       </c>
       <c r="H245" s="14" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="I245" s="27" t="s">
         <v>113</v>
@@ -17654,7 +17662,7 @@
         <v>23</v>
       </c>
       <c r="C246" s="7" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="D246" s="8"/>
       <c r="E246" s="8"/>
@@ -17663,7 +17671,7 @@
         <v>27</v>
       </c>
       <c r="H246" s="14" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="I246" s="27" t="s">
         <v>113</v>
@@ -17689,7 +17697,7 @@
         <v>23</v>
       </c>
       <c r="C247" s="7" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="D247" s="8"/>
       <c r="E247" s="8"/>
@@ -17698,7 +17706,7 @@
         <v>27</v>
       </c>
       <c r="H247" s="14" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="I247" s="27" t="s">
         <v>113</v>
@@ -17724,7 +17732,7 @@
         <v>23</v>
       </c>
       <c r="C248" s="7" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="D248" s="8"/>
       <c r="E248" s="8"/>
@@ -17733,7 +17741,7 @@
         <v>27</v>
       </c>
       <c r="H248" s="14" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="I248" s="27" t="s">
         <v>113</v>
@@ -17759,7 +17767,7 @@
         <v>23</v>
       </c>
       <c r="C249" s="7" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="D249" s="8"/>
       <c r="E249" s="8"/>
@@ -17768,7 +17776,7 @@
         <v>27</v>
       </c>
       <c r="H249" s="14" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="I249" s="27" t="s">
         <v>113</v>
@@ -17794,7 +17802,7 @@
         <v>23</v>
       </c>
       <c r="C250" s="7" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="D250" s="8"/>
       <c r="E250" s="8"/>
@@ -17803,7 +17811,7 @@
         <v>27</v>
       </c>
       <c r="H250" s="14" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="I250" s="27" t="s">
         <v>113</v>
@@ -17829,7 +17837,7 @@
         <v>23</v>
       </c>
       <c r="C251" s="7" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="D251" s="8"/>
       <c r="E251" s="8"/>
@@ -17838,7 +17846,7 @@
         <v>27</v>
       </c>
       <c r="H251" s="14" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="I251" s="27" t="s">
         <v>113</v>
@@ -17864,7 +17872,7 @@
         <v>23</v>
       </c>
       <c r="C252" s="7" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="D252" s="8"/>
       <c r="E252" s="8"/>
@@ -17873,7 +17881,7 @@
         <v>27</v>
       </c>
       <c r="H252" s="14" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="I252" s="27" t="s">
         <v>113</v>
@@ -17899,7 +17907,7 @@
         <v>23</v>
       </c>
       <c r="C253" s="7" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="D253" s="8"/>
       <c r="E253" s="8"/>
@@ -17908,7 +17916,7 @@
         <v>27</v>
       </c>
       <c r="H253" s="14" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="I253" s="27" t="s">
         <v>113</v>
@@ -17934,7 +17942,7 @@
         <v>23</v>
       </c>
       <c r="C254" s="7" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="D254" s="8"/>
       <c r="E254" s="8"/>
@@ -17943,7 +17951,7 @@
         <v>27</v>
       </c>
       <c r="H254" s="14" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="I254" s="27" t="s">
         <v>113</v>
@@ -17969,7 +17977,7 @@
         <v>23</v>
       </c>
       <c r="C255" s="7" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="D255" s="8"/>
       <c r="E255" s="8"/>
@@ -17978,7 +17986,7 @@
         <v>27</v>
       </c>
       <c r="H255" s="14" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="I255" s="27" t="s">
         <v>113</v>
@@ -18004,7 +18012,7 @@
         <v>23</v>
       </c>
       <c r="C256" s="7" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="D256" s="8"/>
       <c r="E256" s="8"/>
@@ -18013,7 +18021,7 @@
         <v>27</v>
       </c>
       <c r="H256" s="14" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="I256" s="27" t="s">
         <v>113</v>
@@ -18039,7 +18047,7 @@
         <v>23</v>
       </c>
       <c r="C257" s="7" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="D257" s="8"/>
       <c r="E257" s="8"/>
@@ -18048,7 +18056,7 @@
         <v>27</v>
       </c>
       <c r="H257" s="14" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="I257" s="27" t="s">
         <v>113</v>
@@ -18074,7 +18082,7 @@
         <v>23</v>
       </c>
       <c r="C258" s="7" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="D258" s="8"/>
       <c r="E258" s="8"/>
@@ -18083,7 +18091,7 @@
         <v>27</v>
       </c>
       <c r="H258" s="14" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="I258" s="27" t="s">
         <v>113</v>
@@ -18109,7 +18117,7 @@
         <v>23</v>
       </c>
       <c r="C259" s="7" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="D259" s="8"/>
       <c r="E259" s="8"/>
@@ -18118,7 +18126,7 @@
         <v>27</v>
       </c>
       <c r="H259" s="14" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="I259" s="27" t="s">
         <v>113</v>
@@ -18144,7 +18152,7 @@
         <v>23</v>
       </c>
       <c r="C260" s="7" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="D260" s="8"/>
       <c r="E260" s="8"/>
@@ -18153,7 +18161,7 @@
         <v>27</v>
       </c>
       <c r="H260" s="14" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="I260" s="27" t="s">
         <v>113</v>
@@ -18179,7 +18187,7 @@
         <v>23</v>
       </c>
       <c r="C261" s="7" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="D261" s="8"/>
       <c r="E261" s="8"/>
@@ -18188,7 +18196,7 @@
         <v>27</v>
       </c>
       <c r="H261" s="14" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="I261" s="27" t="s">
         <v>113</v>
@@ -18212,7 +18220,7 @@
         <v>23</v>
       </c>
       <c r="C262" s="7" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="D262" s="8"/>
       <c r="E262" s="8"/>
@@ -18239,7 +18247,7 @@
         <v>159</v>
       </c>
       <c r="C263" s="7" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="D263" s="8"/>
       <c r="E263" s="8" t="s">
@@ -18247,10 +18255,10 @@
       </c>
       <c r="F263" s="10"/>
       <c r="G263" s="8" t="s">
+        <v>779</v>
+      </c>
+      <c r="H263" s="14" t="s">
         <v>780</v>
-      </c>
-      <c r="H263" s="14" t="s">
-        <v>781</v>
       </c>
       <c r="I263" s="27"/>
       <c r="J263" s="3"/>
@@ -18272,7 +18280,7 @@
         <v>159</v>
       </c>
       <c r="C264" s="7" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="D264" s="8"/>
       <c r="E264" s="8" t="s">
@@ -18280,10 +18288,10 @@
       </c>
       <c r="F264" s="10"/>
       <c r="G264" s="8" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="H264" s="14" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="I264" s="27"/>
       <c r="J264" s="3"/>
@@ -18305,7 +18313,7 @@
         <v>23</v>
       </c>
       <c r="C265" s="7" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="D265" s="8"/>
       <c r="E265" s="8" t="s">
@@ -18313,10 +18321,10 @@
       </c>
       <c r="F265" s="10"/>
       <c r="G265" s="8" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="H265" s="14" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="I265" s="27"/>
       <c r="J265" s="3"/>
@@ -18338,13 +18346,13 @@
       </c>
       <c r="B266" s="29"/>
       <c r="C266" s="37" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="D266" s="38" t="s">
         <v>29</v>
       </c>
       <c r="E266" s="38" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="F266" s="38" t="s">
         <v>26</v>
@@ -18353,7 +18361,7 @@
         <v>27</v>
       </c>
       <c r="H266" s="39" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="I266" s="31"/>
       <c r="J266" s="34"/>
@@ -18376,7 +18384,7 @@
     </row>
     <row r="267" spans="1:26" ht="14.25" customHeight="1">
       <c r="A267" s="6" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="B267" s="6" t="s">
         <v>23</v>
@@ -18393,7 +18401,7 @@
         <v>30</v>
       </c>
       <c r="H267" s="14" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="I267" s="8"/>
       <c r="J267" s="3"/>
@@ -21025,7 +21033,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -21037,7 +21046,7 @@
   <dimension ref="A1:Z117"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="4" topLeftCell="A63" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="H116" sqref="H116"/>
     </sheetView>
   </sheetViews>
@@ -21057,7 +21066,7 @@
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
       <c r="A1" s="4" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -21085,7 +21094,7 @@
     </row>
     <row r="2" spans="1:26" s="57" customFormat="1" ht="14.25" customHeight="1">
       <c r="A2" s="70" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="B2" s="69"/>
       <c r="C2" s="69"/>
@@ -21113,7 +21122,7 @@
     </row>
     <row r="3" spans="1:26" s="91" customFormat="1" ht="12.75" customHeight="1">
       <c r="A3" s="87" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="B3" s="88"/>
       <c r="C3" s="89"/>
@@ -21201,7 +21210,7 @@
       <c r="C5" s="13"/>
       <c r="D5" s="13"/>
       <c r="E5" s="72" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="F5" s="10"/>
       <c r="G5" s="70" t="s">
@@ -21217,7 +21226,7 @@
         <v>27</v>
       </c>
       <c r="K5" s="57" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="L5" s="9"/>
       <c r="M5" s="25"/>
@@ -21239,7 +21248,7 @@
       <c r="C6" s="13"/>
       <c r="D6" s="13"/>
       <c r="E6" s="72" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="F6" s="10"/>
       <c r="G6" s="70" t="s">
@@ -21255,7 +21264,7 @@
         <v>27</v>
       </c>
       <c r="K6" s="57" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="L6" s="9"/>
       <c r="M6" s="25"/>
@@ -21277,7 +21286,7 @@
       <c r="C7" s="13"/>
       <c r="D7" s="13"/>
       <c r="E7" s="72" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F7" s="10"/>
       <c r="G7" s="70" t="s">
@@ -21293,7 +21302,7 @@
         <v>27</v>
       </c>
       <c r="K7" s="70" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="L7" s="9"/>
       <c r="M7" s="25"/>
@@ -21313,10 +21322,10 @@
       <c r="A8" s="82"/>
       <c r="B8" s="82"/>
       <c r="D8" s="84" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="E8" s="84" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="F8" s="84">
         <v>5.2</v>
@@ -21332,7 +21341,7 @@
         <v>27</v>
       </c>
       <c r="K8" s="83" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
     </row>
     <row r="9" spans="1:26" s="21" customFormat="1" ht="28.8">
@@ -21340,19 +21349,19 @@
       <c r="B9" s="20"/>
       <c r="C9" s="22"/>
       <c r="E9" s="21" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="G9" s="21" t="s">
         <v>46</v>
       </c>
       <c r="H9" s="21" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="J9" s="23" t="s">
         <v>30</v>
       </c>
       <c r="K9" s="80" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="L9" s="22"/>
     </row>
@@ -21361,19 +21370,19 @@
       <c r="B10" s="20"/>
       <c r="C10" s="22"/>
       <c r="E10" s="21" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="G10" s="21" t="s">
         <v>46</v>
       </c>
       <c r="H10" s="21" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="J10" s="23" t="s">
         <v>30</v>
       </c>
       <c r="K10" s="80" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
       <c r="L10" s="22"/>
     </row>
@@ -21382,10 +21391,10 @@
       <c r="B11" s="92"/>
       <c r="C11" s="93"/>
       <c r="D11" s="76" t="s">
+        <v>941</v>
+      </c>
+      <c r="E11" s="76" t="s">
         <v>942</v>
-      </c>
-      <c r="E11" s="76" t="s">
-        <v>943</v>
       </c>
       <c r="F11" s="65">
         <v>36</v>
@@ -21397,16 +21406,16 @@
         <v>226</v>
       </c>
       <c r="I11" s="76" t="s">
+        <v>944</v>
+      </c>
+      <c r="J11" s="94" t="s">
+        <v>943</v>
+      </c>
+      <c r="K11" s="95" t="s">
         <v>945</v>
       </c>
-      <c r="J11" s="94" t="s">
-        <v>944</v>
-      </c>
-      <c r="K11" s="95" t="s">
+      <c r="L11" s="94" t="s">
         <v>946</v>
-      </c>
-      <c r="L11" s="94" t="s">
-        <v>947</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.4">
@@ -21565,7 +21574,7 @@
       <c r="B20" s="20"/>
       <c r="D20" s="3"/>
       <c r="E20" s="7" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="F20" s="7">
         <v>1</v>
@@ -21574,7 +21583,7 @@
         <v>108</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="I20" s="21" t="s">
         <v>26</v>
@@ -21583,7 +21592,7 @@
         <v>27</v>
       </c>
       <c r="K20" s="21" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
     </row>
     <row r="21" spans="1:26" s="21" customFormat="1" ht="14.4">
@@ -21591,14 +21600,14 @@
       <c r="B21" s="20"/>
       <c r="D21" s="3"/>
       <c r="E21" s="7" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
       <c r="F21" s="7"/>
       <c r="G21" s="7" t="s">
         <v>108</v>
       </c>
       <c r="H21" s="7" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="I21" s="21" t="s">
         <v>26</v>
@@ -21607,7 +21616,7 @@
         <v>27</v>
       </c>
       <c r="K21" s="21" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
     </row>
     <row r="22" spans="1:26" s="21" customFormat="1" ht="14.4">
@@ -21615,7 +21624,7 @@
       <c r="B22" s="20"/>
       <c r="D22" s="3"/>
       <c r="E22" s="7" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="F22" s="7">
         <v>90</v>
@@ -21624,13 +21633,13 @@
         <v>108</v>
       </c>
       <c r="H22" s="7" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="J22" s="21" t="s">
         <v>30</v>
       </c>
       <c r="K22" s="21" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="23" spans="1:26" ht="14.4">
@@ -21696,7 +21705,7 @@
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
       <c r="E25" s="7" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="F25" s="7">
         <v>4.2</v>
@@ -21714,7 +21723,7 @@
         <v>27</v>
       </c>
       <c r="K25" s="3" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="N25" s="3"/>
     </row>
@@ -21726,7 +21735,7 @@
         <v>24</v>
       </c>
       <c r="D26" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="E26" s="7" t="s">
         <v>50</v>
@@ -21735,11 +21744,11 @@
         <v>0</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="H26" s="7"/>
       <c r="K26" s="23" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
     </row>
     <row r="27" spans="1:26" ht="14.4">
@@ -21820,7 +21829,7 @@
         <v>30</v>
       </c>
       <c r="K30" s="80" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="L30" s="19"/>
       <c r="M30" s="19"/>
@@ -21900,7 +21909,7 @@
       </c>
       <c r="D33" s="22"/>
       <c r="E33" s="21" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="F33" s="7"/>
       <c r="G33" s="57" t="s">
@@ -21916,7 +21925,7 @@
         <v>27</v>
       </c>
       <c r="K33" s="23" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
     </row>
     <row r="34" spans="1:12" s="21" customFormat="1" ht="14.4">
@@ -21924,7 +21933,7 @@
       <c r="B34" s="20"/>
       <c r="D34" s="22"/>
       <c r="E34" s="21" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="F34" s="7"/>
       <c r="G34" s="57" t="s">
@@ -21940,7 +21949,7 @@
         <v>27</v>
       </c>
       <c r="K34" s="23" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
     </row>
     <row r="35" spans="1:12" s="21" customFormat="1" ht="14.4">
@@ -21948,7 +21957,7 @@
       <c r="B35" s="20"/>
       <c r="D35" s="22"/>
       <c r="E35" s="21" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="F35" s="7"/>
       <c r="G35" s="57" t="s">
@@ -21964,7 +21973,7 @@
         <v>27</v>
       </c>
       <c r="K35" s="23" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
     </row>
     <row r="36" spans="1:12" ht="14.4">
@@ -22087,14 +22096,14 @@
       <c r="A41" s="20"/>
       <c r="B41" s="20"/>
       <c r="E41" s="7" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="F41" s="7"/>
       <c r="G41" s="21" t="s">
         <v>108</v>
       </c>
       <c r="H41" s="21" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
       <c r="I41" s="21" t="s">
         <v>26</v>
@@ -22103,7 +22112,7 @@
         <v>27</v>
       </c>
       <c r="K41" s="23" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
     </row>
     <row r="42" spans="1:12" s="21" customFormat="1" ht="14.4">
@@ -22119,7 +22128,7 @@
         <v>108</v>
       </c>
       <c r="H42" s="21" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
       <c r="I42" s="21" t="s">
         <v>26</v>
@@ -22128,21 +22137,21 @@
         <v>27</v>
       </c>
       <c r="K42" s="23" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
     </row>
     <row r="43" spans="1:12" s="21" customFormat="1" ht="14.4">
       <c r="A43" s="20"/>
       <c r="B43" s="20"/>
       <c r="E43" s="7" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="F43" s="7"/>
       <c r="G43" s="21" t="s">
         <v>108</v>
       </c>
       <c r="H43" s="21" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
       <c r="I43" s="21" t="s">
         <v>26</v>
@@ -22151,10 +22160,10 @@
         <v>27</v>
       </c>
       <c r="K43" s="23" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="L43" s="21" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
     </row>
     <row r="44" spans="1:12" ht="14.4">
@@ -22211,18 +22220,18 @@
       <c r="B46" s="20"/>
       <c r="D46" s="3"/>
       <c r="E46" s="7" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
       <c r="F46" s="7"/>
       <c r="G46" s="7"/>
       <c r="H46" s="7" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
       <c r="I46" s="21" t="s">
         <v>26</v>
       </c>
       <c r="K46" s="23" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="47" spans="1:12" ht="14.4">
@@ -22233,7 +22242,7 @@
         <v>24</v>
       </c>
       <c r="D47" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="E47" s="7" t="s">
         <v>87</v>
@@ -22242,11 +22251,11 @@
         <v>0</v>
       </c>
       <c r="G47" s="7" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="H47" s="7"/>
       <c r="K47" s="23" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
     </row>
     <row r="48" spans="1:12" ht="14.4">
@@ -22276,10 +22285,10 @@
         <v>24</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="E49" s="7" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="F49" s="7"/>
       <c r="G49" s="7" t="s">
@@ -22295,7 +22304,7 @@
         <v>27</v>
       </c>
       <c r="K49" s="57" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
     </row>
     <row r="50" spans="1:11" s="21" customFormat="1" ht="14.4">
@@ -22306,10 +22315,10 @@
         <v>24</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="E50" s="7" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="F50" s="7"/>
       <c r="G50" s="7" t="s">
@@ -22325,7 +22334,7 @@
         <v>27</v>
       </c>
       <c r="K50" s="57" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
     </row>
     <row r="51" spans="1:11" s="21" customFormat="1" ht="14.4">
@@ -22336,10 +22345,10 @@
         <v>24</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="E51" s="58" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="F51" s="7"/>
       <c r="G51" s="7" t="s">
@@ -22355,7 +22364,7 @@
         <v>27</v>
       </c>
       <c r="K51" s="57" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
     </row>
     <row r="52" spans="1:11" s="21" customFormat="1" ht="14.4">
@@ -22373,7 +22382,7 @@
       <c r="I52" s="57"/>
       <c r="J52" s="57"/>
       <c r="K52" s="57" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
     </row>
     <row r="53" spans="1:11" ht="14.4">
@@ -22384,7 +22393,7 @@
         <v>24</v>
       </c>
       <c r="E53" s="7" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="F53" s="7">
         <v>0</v>
@@ -22399,14 +22408,14 @@
         <v>26</v>
       </c>
       <c r="K53" s="57" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="54" spans="1:11" s="21" customFormat="1" ht="14.4">
       <c r="A54" s="20"/>
       <c r="B54" s="20"/>
       <c r="E54" s="7" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
       <c r="F54" s="7"/>
       <c r="G54" s="21" t="s">
@@ -22422,7 +22431,7 @@
         <v>30</v>
       </c>
       <c r="K54" s="57" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
     </row>
     <row r="55" spans="1:11" ht="14.4">
@@ -22448,7 +22457,7 @@
       <c r="A56" s="20"/>
       <c r="B56" s="20"/>
       <c r="E56" s="7" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="F56" s="7">
         <v>0.08</v>
@@ -22466,21 +22475,21 @@
         <v>30</v>
       </c>
       <c r="K56" s="23" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
     </row>
     <row r="57" spans="1:11" s="21" customFormat="1" ht="14.4">
       <c r="A57" s="20"/>
       <c r="B57" s="20"/>
       <c r="E57" s="58" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
       <c r="F57" s="7"/>
       <c r="G57" s="7" t="s">
         <v>108</v>
       </c>
       <c r="H57" s="7" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="I57" s="21" t="s">
         <v>34</v>
@@ -22489,14 +22498,14 @@
         <v>30</v>
       </c>
       <c r="K57" s="23" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
     </row>
     <row r="58" spans="1:11" s="21" customFormat="1" ht="14.4">
       <c r="A58" s="20"/>
       <c r="B58" s="20"/>
       <c r="E58" s="58" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="F58" s="7"/>
       <c r="G58" s="7" t="s">
@@ -22512,14 +22521,14 @@
         <v>27</v>
       </c>
       <c r="K58" s="23" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
     </row>
     <row r="59" spans="1:11" s="21" customFormat="1" ht="14.4">
       <c r="A59" s="20"/>
       <c r="B59" s="20"/>
       <c r="E59" s="58" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="F59" s="7"/>
       <c r="G59" s="7" t="s">
@@ -22532,7 +22541,7 @@
         <v>26</v>
       </c>
       <c r="K59" s="23" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
     </row>
     <row r="60" spans="1:11" s="21" customFormat="1" ht="14.4">
@@ -22547,14 +22556,14 @@
         <v>474</v>
       </c>
       <c r="K60" s="23" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
     </row>
     <row r="61" spans="1:11" s="21" customFormat="1" ht="14.4">
       <c r="A61" s="20"/>
       <c r="B61" s="20"/>
       <c r="E61" s="58" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="F61" s="7"/>
       <c r="G61" s="7" t="s">
@@ -22570,14 +22579,14 @@
         <v>27</v>
       </c>
       <c r="K61" s="23" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
     </row>
     <row r="62" spans="1:11" s="21" customFormat="1" ht="14.4">
       <c r="A62" s="20"/>
       <c r="B62" s="20"/>
       <c r="E62" s="7" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="F62" s="7"/>
       <c r="G62" s="7" t="s">
@@ -22590,14 +22599,14 @@
         <v>26</v>
       </c>
       <c r="K62" s="23" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
     </row>
     <row r="63" spans="1:11" s="21" customFormat="1" ht="14.4">
       <c r="A63" s="20"/>
       <c r="B63" s="20"/>
       <c r="E63" s="7" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="F63" s="7"/>
       <c r="G63" s="7" t="s">
@@ -22610,7 +22619,7 @@
         <v>34</v>
       </c>
       <c r="K63" s="23" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
     </row>
     <row r="64" spans="1:11" ht="14.4">
@@ -22652,7 +22661,7 @@
       <c r="C65" s="22"/>
       <c r="D65" s="22"/>
       <c r="E65" s="21" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="F65" s="7"/>
       <c r="G65" s="21" t="s">
@@ -22668,7 +22677,7 @@
         <v>30</v>
       </c>
       <c r="K65" s="23" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="66" spans="1:26" s="21" customFormat="1" ht="14.4">
@@ -22679,14 +22688,14 @@
       <c r="C66" s="22"/>
       <c r="D66" s="22"/>
       <c r="E66" s="21" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="F66" s="7"/>
       <c r="G66" s="21" t="s">
         <v>108</v>
       </c>
       <c r="H66" s="21" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="I66" s="23" t="s">
         <v>26</v>
@@ -22695,7 +22704,7 @@
         <v>27</v>
       </c>
       <c r="K66" s="23" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
     </row>
     <row r="67" spans="1:26" s="21" customFormat="1" ht="14.4">
@@ -22704,7 +22713,7 @@
       <c r="C67" s="22"/>
       <c r="D67" s="22"/>
       <c r="E67" s="21" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="F67" s="7"/>
       <c r="G67" s="21" t="s">
@@ -22720,7 +22729,7 @@
         <v>27</v>
       </c>
       <c r="K67" s="23" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
     </row>
     <row r="68" spans="1:26" s="21" customFormat="1" ht="14.4">
@@ -22731,7 +22740,7 @@
       <c r="C68" s="22"/>
       <c r="D68" s="22"/>
       <c r="E68" s="21" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="F68" s="7"/>
       <c r="G68" s="21" t="s">
@@ -22747,7 +22756,7 @@
         <v>27</v>
       </c>
       <c r="K68" s="23" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
     </row>
     <row r="69" spans="1:26" ht="43.2">
@@ -22780,7 +22789,7 @@
       <c r="A70" s="20"/>
       <c r="B70" s="20"/>
       <c r="E70" s="7" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="G70" s="21" t="s">
         <v>108</v>
@@ -22795,7 +22804,7 @@
         <v>30</v>
       </c>
       <c r="K70" s="23" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
     </row>
     <row r="71" spans="1:26" s="25" customFormat="1" ht="86.4">
@@ -22820,14 +22829,14 @@
         <v>30</v>
       </c>
       <c r="K71" s="80" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
     </row>
     <row r="72" spans="1:26" s="25" customFormat="1" ht="14.4">
       <c r="A72" s="81"/>
       <c r="B72" s="81"/>
       <c r="E72" s="72" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="G72" s="72" t="s">
         <v>108</v>
@@ -22842,7 +22851,7 @@
         <v>27</v>
       </c>
       <c r="K72" s="23" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
     </row>
     <row r="73" spans="1:26" s="25" customFormat="1" ht="28.8">
@@ -22851,7 +22860,7 @@
         <v>23</v>
       </c>
       <c r="E73" s="25" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="G73" s="25" t="s">
         <v>108</v>
@@ -22864,14 +22873,14 @@
       </c>
       <c r="J73" s="19"/>
       <c r="K73" s="80" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
     </row>
     <row r="74" spans="1:26" s="21" customFormat="1" ht="14.25" customHeight="1">
       <c r="C74" s="28"/>
       <c r="D74" s="28"/>
       <c r="E74" s="7" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="F74" s="7"/>
       <c r="G74" s="70" t="s">
@@ -22887,10 +22896,10 @@
         <v>27</v>
       </c>
       <c r="K74" s="57" t="s">
+        <v>811</v>
+      </c>
+      <c r="L74" s="70" t="s">
         <v>812</v>
-      </c>
-      <c r="L74" s="70" t="s">
-        <v>813</v>
       </c>
       <c r="M74" s="3"/>
       <c r="N74" s="7"/>
@@ -22909,14 +22918,14 @@
       <c r="C75" s="28"/>
       <c r="D75" s="28"/>
       <c r="E75" s="25" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="F75" s="7"/>
       <c r="G75" s="70" t="s">
         <v>108</v>
       </c>
       <c r="H75" s="70" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
       <c r="I75" s="70" t="s">
         <v>34</v>
@@ -22925,7 +22934,7 @@
         <v>30</v>
       </c>
       <c r="K75" s="70" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
       <c r="L75" s="70"/>
       <c r="M75" s="3"/>
@@ -22961,17 +22970,17 @@
       <c r="A77" s="20"/>
       <c r="B77" s="20"/>
       <c r="E77" s="25" t="s">
+        <v>979</v>
+      </c>
+      <c r="F77" s="7" t="s">
         <v>980</v>
-      </c>
-      <c r="F77" s="7" t="s">
-        <v>981</v>
       </c>
       <c r="G77" s="25" t="s">
         <v>70</v>
       </c>
       <c r="H77" s="7"/>
       <c r="K77" s="21" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
     </row>
     <row r="78" spans="1:26" ht="14.4">
@@ -23045,7 +23054,7 @@
       <c r="A80" s="20"/>
       <c r="B80" s="20"/>
       <c r="E80" s="7" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="F80" s="7"/>
       <c r="G80" s="7" t="s">
@@ -23072,14 +23081,14 @@
       <c r="G81" s="7"/>
       <c r="H81" s="7"/>
       <c r="K81" s="3" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
     </row>
     <row r="82" spans="1:12" s="21" customFormat="1" ht="14.4">
       <c r="A82" s="20"/>
       <c r="B82" s="20"/>
       <c r="E82" s="7" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="F82" s="7"/>
       <c r="G82" s="7" t="s">
@@ -23095,17 +23104,17 @@
         <v>30</v>
       </c>
       <c r="K82" s="21" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="L82" s="3" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
     </row>
     <row r="83" spans="1:12" s="21" customFormat="1" ht="14.4">
       <c r="A83" s="20"/>
       <c r="B83" s="20"/>
       <c r="E83" s="7" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="F83" s="7"/>
       <c r="G83" s="7" t="s">
@@ -23121,10 +23130,10 @@
         <v>30</v>
       </c>
       <c r="K83" s="21" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="L83" s="3" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
     </row>
     <row r="84" spans="1:12" ht="14.4">
@@ -23228,7 +23237,7 @@
       <c r="B88" s="20"/>
       <c r="C88" s="3"/>
       <c r="E88" s="7" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="F88" s="7"/>
       <c r="G88" s="7"/>
@@ -23240,12 +23249,12 @@
         <v>27</v>
       </c>
       <c r="K88" s="3" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
     </row>
     <row r="89" spans="1:12" s="21" customFormat="1" ht="14.4">
       <c r="A89" s="20" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="B89" s="20" t="s">
         <v>24</v>
@@ -23257,7 +23266,7 @@
         <v>65</v>
       </c>
       <c r="E89" s="7" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="F89" s="7">
         <v>5</v>
@@ -23275,7 +23284,7 @@
         <v>27</v>
       </c>
       <c r="K89" s="3" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="L89" s="23" t="s">
         <v>65</v>
@@ -23316,7 +23325,7 @@
       <c r="B91" s="20"/>
       <c r="D91" s="3"/>
       <c r="E91" s="7" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="F91" s="7"/>
       <c r="G91" s="7"/>
@@ -23326,7 +23335,7 @@
       <c r="I91" s="3"/>
       <c r="J91" s="3"/>
       <c r="K91" s="3" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
     </row>
     <row r="92" spans="1:12" s="21" customFormat="1" ht="14.4">
@@ -23334,7 +23343,7 @@
       <c r="B92" s="20"/>
       <c r="D92" s="3"/>
       <c r="E92" s="7" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="F92" s="7"/>
       <c r="G92" s="7"/>
@@ -23344,7 +23353,7 @@
       <c r="I92" s="3"/>
       <c r="J92" s="3"/>
       <c r="K92" s="3" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
     </row>
     <row r="93" spans="1:12" ht="14.4">
@@ -23365,7 +23374,7 @@
       <c r="A94" s="20"/>
       <c r="B94" s="20"/>
       <c r="E94" s="7" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="F94" s="7">
         <v>5</v>
@@ -23383,14 +23392,14 @@
         <v>30</v>
       </c>
       <c r="K94" s="23" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
     </row>
     <row r="95" spans="1:12" s="21" customFormat="1" ht="14.4">
       <c r="A95" s="20"/>
       <c r="B95" s="20"/>
       <c r="E95" s="58" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="F95" s="7">
         <v>5</v>
@@ -23408,14 +23417,14 @@
         <v>30</v>
       </c>
       <c r="K95" s="23" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
     </row>
     <row r="96" spans="1:12" s="21" customFormat="1" ht="14.4">
       <c r="A96" s="20"/>
       <c r="B96" s="20"/>
       <c r="E96" s="58" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="F96" s="7">
         <v>5</v>
@@ -23433,14 +23442,14 @@
         <v>30</v>
       </c>
       <c r="K96" s="23" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
     </row>
     <row r="97" spans="1:12" s="21" customFormat="1" ht="14.4">
       <c r="A97" s="20"/>
       <c r="B97" s="20"/>
       <c r="E97" s="7" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="F97" s="7">
         <v>1</v>
@@ -23449,23 +23458,23 @@
         <v>108</v>
       </c>
       <c r="H97" s="7" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="I97" s="23" t="s">
         <v>26</v>
       </c>
       <c r="J97" s="23" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
     </row>
     <row r="98" spans="1:12" s="65" customFormat="1" ht="14.4">
       <c r="A98" s="92"/>
       <c r="B98" s="92"/>
       <c r="C98" s="76" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="E98" s="64" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="F98" s="64"/>
       <c r="G98" s="64" t="s">
@@ -23482,26 +23491,26 @@
       </c>
       <c r="K98" s="94"/>
       <c r="L98" s="94" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
     </row>
     <row r="99" spans="1:12" s="21" customFormat="1" ht="14.4">
       <c r="A99" s="20"/>
       <c r="B99" s="20"/>
       <c r="E99" s="7" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="F99" s="7"/>
       <c r="G99" s="7" t="s">
         <v>108</v>
       </c>
       <c r="H99" s="7" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="I99" s="23"/>
       <c r="J99" s="23"/>
       <c r="K99" s="23" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
       <c r="L99" s="23"/>
     </row>
@@ -23509,19 +23518,19 @@
       <c r="A100" s="20"/>
       <c r="B100" s="20"/>
       <c r="E100" s="7" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="F100" s="7"/>
       <c r="G100" s="7" t="s">
         <v>108</v>
       </c>
       <c r="H100" s="7" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="I100" s="23"/>
       <c r="J100" s="23"/>
       <c r="K100" s="23" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
       <c r="L100" s="23"/>
     </row>
@@ -23529,14 +23538,14 @@
       <c r="A101" s="20"/>
       <c r="B101" s="20"/>
       <c r="E101" s="7" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="F101" s="7"/>
       <c r="G101" s="7" t="s">
         <v>108</v>
       </c>
       <c r="H101" s="7" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="I101" s="23" t="s">
         <v>26</v>
@@ -23545,7 +23554,7 @@
         <v>27</v>
       </c>
       <c r="K101" s="23" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="L101" s="23"/>
     </row>
@@ -23553,21 +23562,21 @@
       <c r="A102" s="20"/>
       <c r="B102" s="20"/>
       <c r="E102" s="7" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="F102" s="7"/>
       <c r="G102" s="7" t="s">
         <v>108</v>
       </c>
       <c r="H102" s="7" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="I102" s="23" t="s">
         <v>34</v>
       </c>
       <c r="J102" s="23"/>
       <c r="K102" s="23" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
       <c r="L102" s="23"/>
     </row>
@@ -23575,10 +23584,10 @@
       <c r="A103" s="20"/>
       <c r="B103" s="20"/>
       <c r="D103" s="57" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="E103" s="7" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
       <c r="F103" s="7"/>
       <c r="G103" s="58" t="s">
@@ -23588,13 +23597,13 @@
         <v>84</v>
       </c>
       <c r="I103" s="23" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="J103" s="23" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="K103" s="23" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
       <c r="L103" s="23"/>
     </row>
@@ -23603,7 +23612,7 @@
       <c r="B104" s="20"/>
       <c r="D104" s="57"/>
       <c r="E104" s="7" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="F104" s="7"/>
       <c r="G104" s="7" t="s">
@@ -23619,10 +23628,10 @@
         <v>27</v>
       </c>
       <c r="K104" s="23" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="L104" s="23" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="105" spans="1:12" s="21" customFormat="1" ht="14.4">
@@ -23630,7 +23639,7 @@
       <c r="B105" s="20"/>
       <c r="D105" s="57"/>
       <c r="E105" s="7" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
       <c r="F105" s="7"/>
       <c r="G105" s="7" t="s">
@@ -23646,10 +23655,10 @@
         <v>27</v>
       </c>
       <c r="K105" s="23" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="L105" s="23" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="106" spans="1:12" s="21" customFormat="1" ht="28.8">
@@ -23657,7 +23666,7 @@
       <c r="B106" s="20"/>
       <c r="D106" s="57"/>
       <c r="E106" s="25" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="F106" s="7"/>
       <c r="G106" s="7" t="s">
@@ -23673,17 +23682,17 @@
         <v>27</v>
       </c>
       <c r="K106" s="23" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="L106" s="23" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
     </row>
     <row r="107" spans="1:12" s="21" customFormat="1" ht="14.4">
       <c r="A107" s="20"/>
       <c r="B107" s="20"/>
       <c r="E107" s="7" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="F107" s="7">
         <v>10</v>
@@ -23692,7 +23701,7 @@
         <v>108</v>
       </c>
       <c r="H107" s="7" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="I107" s="23" t="s">
         <v>26</v>
@@ -23701,14 +23710,14 @@
         <v>27</v>
       </c>
       <c r="K107" s="23" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
     </row>
     <row r="108" spans="1:12" s="21" customFormat="1" ht="28.8">
       <c r="A108" s="20"/>
       <c r="B108" s="20"/>
       <c r="E108" s="72" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="F108" s="7">
         <v>10</v>
@@ -23717,7 +23726,7 @@
         <v>108</v>
       </c>
       <c r="H108" s="7" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="I108" s="23" t="s">
         <v>26</v>
@@ -23726,21 +23735,21 @@
         <v>27</v>
       </c>
       <c r="K108" s="23" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
     </row>
     <row r="109" spans="1:12" s="21" customFormat="1" ht="14.4">
       <c r="A109" s="20"/>
       <c r="B109" s="20"/>
       <c r="E109" s="72" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
       <c r="F109" s="7"/>
       <c r="G109" s="7" t="s">
         <v>108</v>
       </c>
       <c r="H109" s="7" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="I109" s="23" t="s">
         <v>26</v>
@@ -23749,21 +23758,21 @@
         <v>30</v>
       </c>
       <c r="K109" s="23" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="110" spans="1:12" s="21" customFormat="1" ht="14.4">
       <c r="A110" s="20"/>
       <c r="B110" s="20"/>
       <c r="E110" s="7" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="F110" s="7"/>
       <c r="G110" s="7" t="s">
         <v>108</v>
       </c>
       <c r="H110" s="7" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="I110" s="23" t="s">
         <v>34</v>
@@ -23772,31 +23781,31 @@
         <v>30</v>
       </c>
       <c r="K110" s="23" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
     </row>
     <row r="111" spans="1:12" s="21" customFormat="1" ht="14.4">
       <c r="A111" s="20"/>
       <c r="B111" s="20"/>
       <c r="E111" s="7" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="F111" s="7"/>
       <c r="G111" s="7" t="s">
         <v>108</v>
       </c>
       <c r="H111" s="7" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="I111" s="23"/>
       <c r="J111" s="23" t="s">
         <v>27</v>
       </c>
       <c r="K111" s="23" t="s">
+        <v>972</v>
+      </c>
+      <c r="L111" s="23" t="s">
         <v>973</v>
-      </c>
-      <c r="L111" s="23" t="s">
-        <v>974</v>
       </c>
     </row>
     <row r="112" spans="1:12" s="21" customFormat="1" ht="14.4">
@@ -23813,7 +23822,7 @@
       <c r="I112" s="23"/>
       <c r="J112" s="23"/>
       <c r="K112" s="23" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
     </row>
     <row r="113" spans="1:11" s="21" customFormat="1" ht="14.4">
@@ -23823,7 +23832,7 @@
         <v>25</v>
       </c>
       <c r="E113" s="7" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="F113" s="7"/>
       <c r="G113" s="58" t="s">
@@ -23839,7 +23848,7 @@
         <v>27</v>
       </c>
       <c r="K113" s="23" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
     </row>
     <row r="114" spans="1:11" s="21" customFormat="1" ht="14.4">
@@ -23851,7 +23860,7 @@
         <v>25</v>
       </c>
       <c r="E114" s="7" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="F114" s="7"/>
       <c r="G114" s="58" t="s">
@@ -23867,7 +23876,7 @@
         <v>27</v>
       </c>
       <c r="K114" s="23" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
     </row>
     <row r="115" spans="1:11" ht="14.4">
@@ -23890,7 +23899,7 @@
         <v>108</v>
       </c>
       <c r="H115" s="18" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="I115" s="17" t="s">
         <v>34</v>
@@ -23922,7 +23931,7 @@
         <v>108</v>
       </c>
       <c r="H116" s="23" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="I116" s="17" t="s">
         <v>34</v>
@@ -23954,7 +23963,7 @@
         <v>108</v>
       </c>
       <c r="H117" s="23" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="I117" s="17" t="s">
         <v>34</v>
@@ -23983,7 +23992,7 @@
   </sheetPr>
   <dimension ref="A1:Z44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F12" sqref="F12"/>
     </sheetView>
@@ -24004,7 +24013,7 @@
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
       <c r="A1" s="4" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -24082,7 +24091,7 @@
       <c r="C3" s="59"/>
       <c r="D3" s="59"/>
       <c r="E3" s="60" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="F3" s="61"/>
       <c r="G3" s="62"/>
@@ -24370,22 +24379,22 @@
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
       <c r="E11" s="21" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="F11" s="57" t="s">
         <v>29</v>
       </c>
       <c r="G11" s="70" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="H11" s="21" t="s">
         <v>30</v>
       </c>
       <c r="I11" s="21" t="s">
+        <v>1036</v>
+      </c>
+      <c r="J11" s="21" t="s">
         <v>1037</v>
-      </c>
-      <c r="J11" s="21" t="s">
-        <v>1038</v>
       </c>
       <c r="K11" s="7"/>
       <c r="L11" s="7"/>
@@ -24524,10 +24533,10 @@
         <v>30</v>
       </c>
       <c r="I15" s="7" t="s">
+        <v>1031</v>
+      </c>
+      <c r="J15" s="7" t="s">
         <v>1032</v>
-      </c>
-      <c r="J15" s="7" t="s">
-        <v>1033</v>
       </c>
       <c r="K15" s="7"/>
       <c r="L15" s="7"/>
@@ -25120,7 +25129,7 @@
       <c r="C31" s="28"/>
       <c r="D31" s="28"/>
       <c r="E31" s="7" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="F31" s="47" t="s">
         <v>29</v>
@@ -25132,10 +25141,10 @@
         <v>27</v>
       </c>
       <c r="I31" s="70" t="s">
+        <v>811</v>
+      </c>
+      <c r="J31" s="70" t="s">
         <v>812</v>
-      </c>
-      <c r="J31" s="70" t="s">
-        <v>813</v>
       </c>
       <c r="K31" s="57"/>
       <c r="L31" s="70"/>
@@ -25243,7 +25252,7 @@
     <row r="36" spans="1:10" s="21" customFormat="1" ht="14.4">
       <c r="A36" s="28"/>
       <c r="E36" s="21" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
       <c r="F36" s="47" t="s">
         <v>29</v>
@@ -25255,7 +25264,7 @@
         <v>27</v>
       </c>
       <c r="I36" s="21" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="37" spans="1:10" s="65" customFormat="1" ht="14.4">
@@ -25430,7 +25439,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
     </row>
     <row r="2" spans="1:1">
@@ -25438,17 +25447,17 @@
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="23" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Get MAXSNOW and the NSantiam stream temperatures working. CW3M_NSantiam.envx - Turn off spinup. HBV.csv - Populate W2A_SLP and W2A_INT for DET12, Mehama37, LowerNSantiam44, LittleNSantiam50, and Blowout51. Flow.cpp - Apply GetMaxSnowPack() to the entire calendar year instead of just the first half of the calendar year.
</commit_message>
<xml_diff>
--- a/DataCW3M/CW3MdigitalHandbook/CW3MdataDictionary.xlsx
+++ b/DataCW3M/CW3MdigitalHandbook/CW3MdataDictionary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\CW3MdigitalHandbook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C62EEC5-8C73-4039-BDD5-B0CE3A3C75C3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCBA0105-E285-40B0-8360-F05F83141A59}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3219,10 +3219,10 @@
     <t>GetMaxSnowPack()</t>
   </si>
   <si>
-    <t>SWE in this IDU (SNOW_BOX + MELT_BOX) on the day of the year on which the entire study area's snowpack is the largest</t>
-  </si>
-  <si>
     <t>daily snowpack mass as snow water equivalent (BOX_SNOW only, not including BOX_MELT)</t>
+  </si>
+  <si>
+    <t>SWE in this IDU (SNOW_BOX + MELT_BOX) on the day of the calendar year (not water year) on which the entire study area's snowpack is the largest</t>
   </si>
 </sst>
 </file>
@@ -9194,8 +9194,8 @@
   <dimension ref="A1:Z1051"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A160" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A173" sqref="A173:XFD173"/>
+      <pane ySplit="3" topLeftCell="A84" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H104" sqref="H104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -12791,8 +12791,8 @@
       <c r="G104" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="H104" s="21" t="s">
-        <v>1040</v>
+      <c r="H104" s="57" t="s">
+        <v>1041</v>
       </c>
       <c r="I104" s="27"/>
       <c r="J104" s="3"/>
@@ -15199,7 +15199,7 @@
         <v>27</v>
       </c>
       <c r="H173" s="72" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="I173" s="46" t="s">
         <v>814</v>
@@ -21046,7 +21046,7 @@
   <dimension ref="A1:Z117"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A63" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="4" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="H116" sqref="H116"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
New NSantiam spinup after extending DET12 down to the location of the Niagara gage. CW3M_NSantiam.envx - Turn on spinup. FLOWreports_NSantiam.xml - Adjust the gage area:HBVCALIB area factors. NSantiam/flow2010.ic, HRU_NSantiam.dbf, IDU_NSantiam.dbf, Reach_NSantiam.dbf - Results of spinup over 2000-09. WaterRights.cpp - Call PopulateHBVCALIB during FlowModel initialization whenever EnvContext.spinupFlag is set.
</commit_message>
<xml_diff>
--- a/DataCW3M/CW3MdigitalHandbook/CW3MdataDictionary.xlsx
+++ b/DataCW3M/CW3MdigitalHandbook/CW3MdataDictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\CW3MdigitalHandbook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCBA0105-E285-40B0-8360-F05F83141A59}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{AE125B5E-E388-4786-88E1-B2A120D8E714}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Necessary input data" sheetId="7" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="Conventions" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -96,7 +97,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3088" uniqueCount="1042">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3089" uniqueCount="1042">
   <si>
     <t>LULC_A</t>
   </si>
@@ -3333,7 +3334,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="103">
+  <cellXfs count="104">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -3568,6 +3569,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -9193,9 +9197,9 @@
   </sheetPr>
   <dimension ref="A1:Z1051"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A84" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H104" sqref="H104"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -10055,7 +10059,9 @@
       <c r="C25" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="D25" s="31"/>
+      <c r="D25" s="103" t="s">
+        <v>29</v>
+      </c>
       <c r="E25" s="31"/>
       <c r="F25" s="38"/>
       <c r="G25" s="31" t="s">
@@ -21045,9 +21051,9 @@
   </sheetPr>
   <dimension ref="A1:Z117"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H116" sqref="H116"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>

</xml_diff>

<commit_message>
Save an updated version of the Specification for Wetland Persistence Model.docx.
</commit_message>
<xml_diff>
--- a/DataCW3M/CW3MdigitalHandbook/CW3MdataDictionary.xlsx
+++ b/DataCW3M/CW3MdigitalHandbook/CW3MdataDictionary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\CW3MdigitalHandbook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AE125B5E-E388-4786-88E1-B2A120D8E714}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{463C8F75-A4EB-4846-8B66-367962766D33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-7425" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Necessary input data" sheetId="7" r:id="rId1"/>
@@ -2872,9 +2872,6 @@
     <t>ADDED_VOL</t>
   </si>
   <si>
-    <t>updated daily: amount added so far this year by the model to the volume of water in the reach by to avoid math problems (e.g. to prevent reaches from going dry)</t>
-  </si>
-  <si>
     <t>updated daily: the amount added so far this year to the reach discharge by the model to ensure that the discharge is &gt;= NOMINAL_LOW_FLOW_CMS</t>
   </si>
   <si>
@@ -3224,6 +3221,9 @@
   </si>
   <si>
     <t>SWE in this IDU (SNOW_BOX + MELT_BOX) on the day of the calendar year (not water year) on which the entire study area's snowpack is the largest</t>
+  </si>
+  <si>
+    <t>updated daily: amount added today by the model to the volume of water in the reach to avoid math problems (e.g. to prevent reaches from going dry)</t>
   </si>
 </sst>
 </file>
@@ -10930,7 +10930,7 @@
       <c r="A50" s="28"/>
       <c r="B50" s="28"/>
       <c r="C50" s="7" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="D50" s="10" t="s">
         <v>108</v>
@@ -10943,10 +10943,10 @@
         <v>30</v>
       </c>
       <c r="H50" s="25" t="s">
+        <v>1025</v>
+      </c>
+      <c r="I50" s="27" t="s">
         <v>1026</v>
-      </c>
-      <c r="I50" s="27" t="s">
-        <v>1027</v>
       </c>
       <c r="J50" s="3"/>
       <c r="K50" s="7"/>
@@ -11464,20 +11464,20 @@
       <c r="A67" s="28"/>
       <c r="B67" s="28"/>
       <c r="C67" s="7" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="D67" s="10" t="s">
         <v>108</v>
       </c>
       <c r="E67" s="10" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
       <c r="F67" s="10"/>
       <c r="G67" s="10" t="s">
         <v>27</v>
       </c>
       <c r="H67" s="25" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="I67" s="27"/>
       <c r="J67" s="3"/>
@@ -12789,16 +12789,16 @@
         <v>29</v>
       </c>
       <c r="E104" s="8" t="s">
+        <v>1037</v>
+      </c>
+      <c r="F104" s="10" t="s">
         <v>1038</v>
-      </c>
-      <c r="F104" s="10" t="s">
-        <v>1039</v>
       </c>
       <c r="G104" s="8" t="s">
         <v>27</v>
       </c>
       <c r="H104" s="57" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="I104" s="27"/>
       <c r="J104" s="3"/>
@@ -15205,7 +15205,7 @@
         <v>27</v>
       </c>
       <c r="H173" s="72" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="I173" s="46" t="s">
         <v>814</v>
@@ -15413,7 +15413,7 @@
         <v>29</v>
       </c>
       <c r="E179" s="27" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="F179" s="27" t="s">
         <v>34</v>
@@ -17005,7 +17005,7 @@
       <c r="A227" s="28"/>
       <c r="B227" s="28"/>
       <c r="C227" s="7" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="D227" s="10" t="s">
         <v>46</v>
@@ -17016,7 +17016,7 @@
         <v>30</v>
       </c>
       <c r="H227" s="25" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="I227" s="27"/>
       <c r="J227" s="3"/>
@@ -17073,7 +17073,7 @@
       <c r="A229" s="96"/>
       <c r="B229" s="96"/>
       <c r="C229" s="97" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="D229" s="100" t="s">
         <v>108</v>
@@ -17086,7 +17086,7 @@
         <v>27</v>
       </c>
       <c r="H229" s="91" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="I229" s="98"/>
       <c r="J229" s="84"/>
@@ -17106,7 +17106,7 @@
       <c r="A230" s="96"/>
       <c r="B230" s="96"/>
       <c r="C230" s="97" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
       <c r="D230" s="99" t="s">
         <v>108</v>
@@ -17121,7 +17121,7 @@
         <v>27</v>
       </c>
       <c r="H230" s="77" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
       <c r="I230" s="98"/>
       <c r="J230" s="84"/>
@@ -21053,7 +21053,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D19" sqref="D19"/>
+      <selection pane="bottomLeft" activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -21100,7 +21100,7 @@
     </row>
     <row r="2" spans="1:26" s="57" customFormat="1" ht="14.25" customHeight="1">
       <c r="A2" s="70" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="B2" s="69"/>
       <c r="C2" s="69"/>
@@ -21128,7 +21128,7 @@
     </row>
     <row r="3" spans="1:26" s="91" customFormat="1" ht="12.75" customHeight="1">
       <c r="A3" s="87" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="B3" s="88"/>
       <c r="C3" s="89"/>
@@ -21232,7 +21232,7 @@
         <v>27</v>
       </c>
       <c r="K5" s="57" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="L5" s="9"/>
       <c r="M5" s="25"/>
@@ -21270,7 +21270,7 @@
         <v>27</v>
       </c>
       <c r="K6" s="57" t="s">
-        <v>924</v>
+        <v>1041</v>
       </c>
       <c r="L6" s="9"/>
       <c r="M6" s="25"/>
@@ -21292,7 +21292,7 @@
       <c r="C7" s="13"/>
       <c r="D7" s="13"/>
       <c r="E7" s="72" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="F7" s="10"/>
       <c r="G7" s="70" t="s">
@@ -21308,7 +21308,7 @@
         <v>27</v>
       </c>
       <c r="K7" s="70" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="L7" s="9"/>
       <c r="M7" s="25"/>
@@ -21388,7 +21388,7 @@
         <v>30</v>
       </c>
       <c r="K10" s="80" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
       <c r="L10" s="22"/>
     </row>
@@ -21397,10 +21397,10 @@
       <c r="B11" s="92"/>
       <c r="C11" s="93"/>
       <c r="D11" s="76" t="s">
+        <v>940</v>
+      </c>
+      <c r="E11" s="76" t="s">
         <v>941</v>
-      </c>
-      <c r="E11" s="76" t="s">
-        <v>942</v>
       </c>
       <c r="F11" s="65">
         <v>36</v>
@@ -21412,16 +21412,16 @@
         <v>226</v>
       </c>
       <c r="I11" s="76" t="s">
+        <v>943</v>
+      </c>
+      <c r="J11" s="94" t="s">
+        <v>942</v>
+      </c>
+      <c r="K11" s="95" t="s">
         <v>944</v>
       </c>
-      <c r="J11" s="94" t="s">
-        <v>943</v>
-      </c>
-      <c r="K11" s="95" t="s">
+      <c r="L11" s="94" t="s">
         <v>945</v>
-      </c>
-      <c r="L11" s="94" t="s">
-        <v>946</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.4">
@@ -21606,7 +21606,7 @@
       <c r="B21" s="20"/>
       <c r="D21" s="3"/>
       <c r="E21" s="7" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="F21" s="7"/>
       <c r="G21" s="7" t="s">
@@ -21622,7 +21622,7 @@
         <v>27</v>
       </c>
       <c r="K21" s="21" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
     </row>
     <row r="22" spans="1:26" s="21" customFormat="1" ht="14.4">
@@ -22102,14 +22102,14 @@
       <c r="A41" s="20"/>
       <c r="B41" s="20"/>
       <c r="E41" s="7" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="F41" s="7"/>
       <c r="G41" s="21" t="s">
         <v>108</v>
       </c>
       <c r="H41" s="21" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
       <c r="I41" s="21" t="s">
         <v>26</v>
@@ -22118,7 +22118,7 @@
         <v>27</v>
       </c>
       <c r="K41" s="23" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
     </row>
     <row r="42" spans="1:12" s="21" customFormat="1" ht="14.4">
@@ -22134,7 +22134,7 @@
         <v>108</v>
       </c>
       <c r="H42" s="21" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="I42" s="21" t="s">
         <v>26</v>
@@ -22143,21 +22143,21 @@
         <v>27</v>
       </c>
       <c r="K42" s="23" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
     </row>
     <row r="43" spans="1:12" s="21" customFormat="1" ht="14.4">
       <c r="A43" s="20"/>
       <c r="B43" s="20"/>
       <c r="E43" s="7" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
       <c r="F43" s="7"/>
       <c r="G43" s="21" t="s">
         <v>108</v>
       </c>
       <c r="H43" s="21" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="I43" s="21" t="s">
         <v>26</v>
@@ -22166,10 +22166,10 @@
         <v>27</v>
       </c>
       <c r="K43" s="23" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
       <c r="L43" s="21" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
     </row>
     <row r="44" spans="1:12" ht="14.4">
@@ -22226,18 +22226,18 @@
       <c r="B46" s="20"/>
       <c r="D46" s="3"/>
       <c r="E46" s="7" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="F46" s="7"/>
       <c r="G46" s="7"/>
       <c r="H46" s="7" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
       <c r="I46" s="21" t="s">
         <v>26</v>
       </c>
       <c r="K46" s="23" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="47" spans="1:12" ht="14.4">
@@ -22324,7 +22324,7 @@
         <v>802</v>
       </c>
       <c r="E50" s="7" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="F50" s="7"/>
       <c r="G50" s="7" t="s">
@@ -22340,7 +22340,7 @@
         <v>27</v>
       </c>
       <c r="K50" s="57" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
     </row>
     <row r="51" spans="1:11" s="21" customFormat="1" ht="14.4">
@@ -22388,7 +22388,7 @@
       <c r="I52" s="57"/>
       <c r="J52" s="57"/>
       <c r="K52" s="57" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
     </row>
     <row r="53" spans="1:11" ht="14.4">
@@ -22399,7 +22399,7 @@
         <v>24</v>
       </c>
       <c r="E53" s="7" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="F53" s="7">
         <v>0</v>
@@ -22414,14 +22414,14 @@
         <v>26</v>
       </c>
       <c r="K53" s="57" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="54" spans="1:11" s="21" customFormat="1" ht="14.4">
       <c r="A54" s="20"/>
       <c r="B54" s="20"/>
       <c r="E54" s="7" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
       <c r="F54" s="7"/>
       <c r="G54" s="21" t="s">
@@ -22437,7 +22437,7 @@
         <v>30</v>
       </c>
       <c r="K54" s="57" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
     </row>
     <row r="55" spans="1:11" ht="14.4">
@@ -22488,14 +22488,14 @@
       <c r="A57" s="20"/>
       <c r="B57" s="20"/>
       <c r="E57" s="58" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="F57" s="7"/>
       <c r="G57" s="7" t="s">
         <v>108</v>
       </c>
       <c r="H57" s="7" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="I57" s="21" t="s">
         <v>34</v>
@@ -22504,14 +22504,14 @@
         <v>30</v>
       </c>
       <c r="K57" s="23" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
     </row>
     <row r="58" spans="1:11" s="21" customFormat="1" ht="14.4">
       <c r="A58" s="20"/>
       <c r="B58" s="20"/>
       <c r="E58" s="58" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
       <c r="F58" s="7"/>
       <c r="G58" s="7" t="s">
@@ -22527,7 +22527,7 @@
         <v>27</v>
       </c>
       <c r="K58" s="23" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
     </row>
     <row r="59" spans="1:11" s="21" customFormat="1" ht="14.4">
@@ -22562,14 +22562,14 @@
         <v>474</v>
       </c>
       <c r="K60" s="23" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
     </row>
     <row r="61" spans="1:11" s="21" customFormat="1" ht="14.4">
       <c r="A61" s="20"/>
       <c r="B61" s="20"/>
       <c r="E61" s="58" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
       <c r="F61" s="7"/>
       <c r="G61" s="7" t="s">
@@ -22585,7 +22585,7 @@
         <v>27</v>
       </c>
       <c r="K61" s="23" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
     </row>
     <row r="62" spans="1:11" s="21" customFormat="1" ht="14.4">
@@ -22612,7 +22612,7 @@
       <c r="A63" s="20"/>
       <c r="B63" s="20"/>
       <c r="E63" s="7" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="F63" s="7"/>
       <c r="G63" s="7" t="s">
@@ -22625,7 +22625,7 @@
         <v>34</v>
       </c>
       <c r="K63" s="23" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="64" spans="1:11" ht="14.4">
@@ -22667,7 +22667,7 @@
       <c r="C65" s="22"/>
       <c r="D65" s="22"/>
       <c r="E65" s="21" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
       <c r="F65" s="7"/>
       <c r="G65" s="21" t="s">
@@ -22683,7 +22683,7 @@
         <v>30</v>
       </c>
       <c r="K65" s="23" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="66" spans="1:26" s="21" customFormat="1" ht="14.4">
@@ -22835,7 +22835,7 @@
         <v>30</v>
       </c>
       <c r="K71" s="80" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
     </row>
     <row r="72" spans="1:26" s="25" customFormat="1" ht="14.4">
@@ -22924,14 +22924,14 @@
       <c r="C75" s="28"/>
       <c r="D75" s="28"/>
       <c r="E75" s="25" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
       <c r="F75" s="7"/>
       <c r="G75" s="70" t="s">
         <v>108</v>
       </c>
       <c r="H75" s="70" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="I75" s="70" t="s">
         <v>34</v>
@@ -22940,7 +22940,7 @@
         <v>30</v>
       </c>
       <c r="K75" s="70" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
       <c r="L75" s="70"/>
       <c r="M75" s="3"/>
@@ -22976,17 +22976,17 @@
       <c r="A77" s="20"/>
       <c r="B77" s="20"/>
       <c r="E77" s="25" t="s">
+        <v>978</v>
+      </c>
+      <c r="F77" s="7" t="s">
         <v>979</v>
-      </c>
-      <c r="F77" s="7" t="s">
-        <v>980</v>
       </c>
       <c r="G77" s="25" t="s">
         <v>70</v>
       </c>
       <c r="H77" s="7"/>
       <c r="K77" s="21" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
     </row>
     <row r="78" spans="1:26" ht="14.4">
@@ -23060,7 +23060,7 @@
       <c r="A80" s="20"/>
       <c r="B80" s="20"/>
       <c r="E80" s="7" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="F80" s="7"/>
       <c r="G80" s="7" t="s">
@@ -23087,7 +23087,7 @@
       <c r="G81" s="7"/>
       <c r="H81" s="7"/>
       <c r="K81" s="3" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
     </row>
     <row r="82" spans="1:12" s="21" customFormat="1" ht="14.4">
@@ -23243,7 +23243,7 @@
       <c r="B88" s="20"/>
       <c r="C88" s="3"/>
       <c r="E88" s="7" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="F88" s="7"/>
       <c r="G88" s="7"/>
@@ -23255,7 +23255,7 @@
         <v>27</v>
       </c>
       <c r="K88" s="3" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
     </row>
     <row r="89" spans="1:12" s="21" customFormat="1" ht="14.4">
@@ -23331,7 +23331,7 @@
       <c r="B91" s="20"/>
       <c r="D91" s="3"/>
       <c r="E91" s="7" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="F91" s="7"/>
       <c r="G91" s="7"/>
@@ -23341,7 +23341,7 @@
       <c r="I91" s="3"/>
       <c r="J91" s="3"/>
       <c r="K91" s="3" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
     </row>
     <row r="92" spans="1:12" s="21" customFormat="1" ht="14.4">
@@ -23349,7 +23349,7 @@
       <c r="B92" s="20"/>
       <c r="D92" s="3"/>
       <c r="E92" s="7" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="F92" s="7"/>
       <c r="G92" s="7"/>
@@ -23359,7 +23359,7 @@
       <c r="I92" s="3"/>
       <c r="J92" s="3"/>
       <c r="K92" s="3" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
     </row>
     <row r="93" spans="1:12" ht="14.4">
@@ -23380,7 +23380,7 @@
       <c r="A94" s="20"/>
       <c r="B94" s="20"/>
       <c r="E94" s="7" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="F94" s="7">
         <v>5</v>
@@ -23398,14 +23398,14 @@
         <v>30</v>
       </c>
       <c r="K94" s="23" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
     </row>
     <row r="95" spans="1:12" s="21" customFormat="1" ht="14.4">
       <c r="A95" s="20"/>
       <c r="B95" s="20"/>
       <c r="E95" s="58" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="F95" s="7">
         <v>5</v>
@@ -23423,14 +23423,14 @@
         <v>30</v>
       </c>
       <c r="K95" s="23" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
     </row>
     <row r="96" spans="1:12" s="21" customFormat="1" ht="14.4">
       <c r="A96" s="20"/>
       <c r="B96" s="20"/>
       <c r="E96" s="58" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="F96" s="7">
         <v>5</v>
@@ -23448,7 +23448,7 @@
         <v>30</v>
       </c>
       <c r="K96" s="23" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
     </row>
     <row r="97" spans="1:12" s="21" customFormat="1" ht="14.4">
@@ -23477,10 +23477,10 @@
       <c r="A98" s="92"/>
       <c r="B98" s="92"/>
       <c r="C98" s="76" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
       <c r="E98" s="64" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="F98" s="64"/>
       <c r="G98" s="64" t="s">
@@ -23497,14 +23497,14 @@
       </c>
       <c r="K98" s="94"/>
       <c r="L98" s="94" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
     </row>
     <row r="99" spans="1:12" s="21" customFormat="1" ht="14.4">
       <c r="A99" s="20"/>
       <c r="B99" s="20"/>
       <c r="E99" s="7" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
       <c r="F99" s="7"/>
       <c r="G99" s="7" t="s">
@@ -23516,7 +23516,7 @@
       <c r="I99" s="23"/>
       <c r="J99" s="23"/>
       <c r="K99" s="23" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="L99" s="23"/>
     </row>
@@ -23524,7 +23524,7 @@
       <c r="A100" s="20"/>
       <c r="B100" s="20"/>
       <c r="E100" s="7" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="F100" s="7"/>
       <c r="G100" s="7" t="s">
@@ -23536,7 +23536,7 @@
       <c r="I100" s="23"/>
       <c r="J100" s="23"/>
       <c r="K100" s="23" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
       <c r="L100" s="23"/>
     </row>
@@ -23544,7 +23544,7 @@
       <c r="A101" s="20"/>
       <c r="B101" s="20"/>
       <c r="E101" s="7" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="F101" s="7"/>
       <c r="G101" s="7" t="s">
@@ -23560,7 +23560,7 @@
         <v>27</v>
       </c>
       <c r="K101" s="23" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
       <c r="L101" s="23"/>
     </row>
@@ -23568,7 +23568,7 @@
       <c r="A102" s="20"/>
       <c r="B102" s="20"/>
       <c r="E102" s="7" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="F102" s="7"/>
       <c r="G102" s="7" t="s">
@@ -23582,7 +23582,7 @@
       </c>
       <c r="J102" s="23"/>
       <c r="K102" s="23" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="L102" s="23"/>
     </row>
@@ -23590,10 +23590,10 @@
       <c r="A103" s="20"/>
       <c r="B103" s="20"/>
       <c r="D103" s="57" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="E103" s="7" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
       <c r="F103" s="7"/>
       <c r="G103" s="58" t="s">
@@ -23603,13 +23603,13 @@
         <v>84</v>
       </c>
       <c r="I103" s="23" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="J103" s="23" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="K103" s="23" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
       <c r="L103" s="23"/>
     </row>
@@ -23618,7 +23618,7 @@
       <c r="B104" s="20"/>
       <c r="D104" s="57"/>
       <c r="E104" s="7" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="F104" s="7"/>
       <c r="G104" s="7" t="s">
@@ -23634,10 +23634,10 @@
         <v>27</v>
       </c>
       <c r="K104" s="23" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="L104" s="23" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="105" spans="1:12" s="21" customFormat="1" ht="14.4">
@@ -23645,7 +23645,7 @@
       <c r="B105" s="20"/>
       <c r="D105" s="57"/>
       <c r="E105" s="7" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="F105" s="7"/>
       <c r="G105" s="7" t="s">
@@ -23661,10 +23661,10 @@
         <v>27</v>
       </c>
       <c r="K105" s="23" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="L105" s="23" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="106" spans="1:12" s="21" customFormat="1" ht="28.8">
@@ -23672,7 +23672,7 @@
       <c r="B106" s="20"/>
       <c r="D106" s="57"/>
       <c r="E106" s="25" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
       <c r="F106" s="7"/>
       <c r="G106" s="7" t="s">
@@ -23688,10 +23688,10 @@
         <v>27</v>
       </c>
       <c r="K106" s="23" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="L106" s="23" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
     </row>
     <row r="107" spans="1:12" s="21" customFormat="1" ht="14.4">
@@ -23723,7 +23723,7 @@
       <c r="A108" s="20"/>
       <c r="B108" s="20"/>
       <c r="E108" s="72" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="F108" s="7">
         <v>10</v>
@@ -23748,7 +23748,7 @@
       <c r="A109" s="20"/>
       <c r="B109" s="20"/>
       <c r="E109" s="72" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="F109" s="7"/>
       <c r="G109" s="7" t="s">
@@ -23764,14 +23764,14 @@
         <v>30</v>
       </c>
       <c r="K109" s="23" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="110" spans="1:12" s="21" customFormat="1" ht="14.4">
       <c r="A110" s="20"/>
       <c r="B110" s="20"/>
       <c r="E110" s="7" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="F110" s="7"/>
       <c r="G110" s="7" t="s">
@@ -23787,14 +23787,14 @@
         <v>30</v>
       </c>
       <c r="K110" s="23" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
     </row>
     <row r="111" spans="1:12" s="21" customFormat="1" ht="14.4">
       <c r="A111" s="20"/>
       <c r="B111" s="20"/>
       <c r="E111" s="7" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="F111" s="7"/>
       <c r="G111" s="7" t="s">
@@ -23808,10 +23808,10 @@
         <v>27</v>
       </c>
       <c r="K111" s="23" t="s">
+        <v>971</v>
+      </c>
+      <c r="L111" s="23" t="s">
         <v>972</v>
-      </c>
-      <c r="L111" s="23" t="s">
-        <v>973</v>
       </c>
     </row>
     <row r="112" spans="1:12" s="21" customFormat="1" ht="14.4">
@@ -23828,7 +23828,7 @@
       <c r="I112" s="23"/>
       <c r="J112" s="23"/>
       <c r="K112" s="23" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
     </row>
     <row r="113" spans="1:11" s="21" customFormat="1" ht="14.4">
@@ -23905,7 +23905,7 @@
         <v>108</v>
       </c>
       <c r="H115" s="18" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="I115" s="17" t="s">
         <v>34</v>
@@ -23937,7 +23937,7 @@
         <v>108</v>
       </c>
       <c r="H116" s="23" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="I116" s="17" t="s">
         <v>34</v>
@@ -23969,7 +23969,7 @@
         <v>108</v>
       </c>
       <c r="H117" s="23" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="I117" s="17" t="s">
         <v>34</v>
@@ -24385,22 +24385,22 @@
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
       <c r="E11" s="21" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
       <c r="F11" s="57" t="s">
         <v>29</v>
       </c>
       <c r="G11" s="70" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
       <c r="H11" s="21" t="s">
         <v>30</v>
       </c>
       <c r="I11" s="21" t="s">
+        <v>1035</v>
+      </c>
+      <c r="J11" s="21" t="s">
         <v>1036</v>
-      </c>
-      <c r="J11" s="21" t="s">
-        <v>1037</v>
       </c>
       <c r="K11" s="7"/>
       <c r="L11" s="7"/>
@@ -24539,10 +24539,10 @@
         <v>30</v>
       </c>
       <c r="I15" s="7" t="s">
+        <v>1030</v>
+      </c>
+      <c r="J15" s="7" t="s">
         <v>1031</v>
-      </c>
-      <c r="J15" s="7" t="s">
-        <v>1032</v>
       </c>
       <c r="K15" s="7"/>
       <c r="L15" s="7"/>
@@ -25258,7 +25258,7 @@
     <row r="36" spans="1:10" s="21" customFormat="1" ht="14.4">
       <c r="A36" s="28"/>
       <c r="E36" s="21" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
       <c r="F36" s="47" t="s">
         <v>29</v>
@@ -25270,7 +25270,7 @@
         <v>27</v>
       </c>
       <c r="I36" s="21" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="37" spans="1:10" s="65" customFormat="1" ht="14.4">

</xml_diff>

<commit_message>
Continue implementation of the wetland submodel. HRU_NSantiam.dbf - Add 3 new HRU attributes. Flow.cpp, .h - #define IRRIGATION. Add FlowModel::SetAttInt(). Correct the calculation of HruBOXSURF_M3 in ReadState(), and add a call to FixHRUwaterBalance() in ReadState(). Extensively rewrite FixHRUwaterBalance(), including logic to lump the irrigated topsoil water into the natural topsoil water and turn off IRRIGATION for all IDUs. Begin to implement the convention that all snow falling on wetland IDUs melts immediately, even when there is no standing water on the wetland.
</commit_message>
<xml_diff>
--- a/DataCW3M/CW3MdigitalHandbook/CW3MdataDictionary.xlsx
+++ b/DataCW3M/CW3MdigitalHandbook/CW3MdataDictionary.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\CW3MdigitalHandbook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2F2C713-56CB-4208-82BE-9B4014FE2441}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0C2830F-166F-4DCA-9C0D-4618748F8BF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-7425" windowWidth="29040" windowHeight="17640" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -9255,7 +9255,7 @@
   <dimension ref="A1:Z1052"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A67" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="3" topLeftCell="A131" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A104" sqref="A104:XFD104"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Flow.cpp, .h - Replace HRU::m_percentIrrigated with m_fracIrrigated, and calculate it at the same time m_areaIrrigated is calculated, in FlowModel::StartYear(). Change m_areaIrrigated from a float to a double. Replace FlowModel::ResetFluxValuesForStep() with ResetHRUfluxes() and ResetReachFluxes(). Call ResetHRUfluxes() and ResetReachFluxes() from FlowModel::InitRun(). Call ResetHRUfluxes() near the end of GetCatchmentDerivatives(). Delete the IDU attribute confusingly named HRU_IRR_P as obsolete. Correct errors in the calculation of HruNAT_SOIL and HruIRRIG_SOIL. In CheckSurfaceH2O(), take the m_globalHandlerFluxValue into account for the surface water HRULayer. GlobalMethods.h, ReachRouting.cpp - Comment out GetLateralInflow(), not currently used. Add a call to ResetReachFluxes() at the end of SolveReachKinematicWave().
</commit_message>
<xml_diff>
--- a/DataCW3M/CW3MdigitalHandbook/CW3MdataDictionary.xlsx
+++ b/DataCW3M/CW3MdigitalHandbook/CW3MdataDictionary.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\CW3MdigitalHandbook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AF177FC-6D52-4FD5-8B35-B72571F0858E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6CED669-9D6E-4566-9614-268A875A6613}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24" yWindow="0" windowWidth="23016" windowHeight="12360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Necessary input data" sheetId="7" r:id="rId1"/>
     <sheet name="IDU attributes" sheetId="1" r:id="rId2"/>
     <sheet name="Reach attributes" sheetId="3" r:id="rId3"/>
     <sheet name="HRU attributes" sheetId="4" r:id="rId4"/>
-    <sheet name="Conventions" sheetId="6" r:id="rId5"/>
+    <sheet name="Deletions" sheetId="8" r:id="rId5"/>
+    <sheet name="Conventions" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -96,7 +97,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3110" uniqueCount="1051">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3128" uniqueCount="1053">
   <si>
     <t>LULC_A</t>
   </si>
@@ -3250,6 +3251,12 @@
   </si>
   <si>
     <t>snowpack, including the liquid water in the snowpack; 0 where there is standing water in wetlands.</t>
+  </si>
+  <si>
+    <t>SummarizeIDULULC()</t>
+  </si>
+  <si>
+    <t>Deleted from IDU layer</t>
   </si>
 </sst>
 </file>
@@ -3366,7 +3373,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="115">
+  <cellXfs count="117">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -3630,6 +3637,12 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -9254,9 +9267,9 @@
   </sheetPr>
   <dimension ref="A1:Z1052"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A163" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H173" sqref="H173"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -11749,7 +11762,9 @@
       <c r="E73" s="8" t="s">
         <v>225</v>
       </c>
-      <c r="F73" s="10"/>
+      <c r="F73" s="10" t="s">
+        <v>1051</v>
+      </c>
       <c r="G73" s="8" t="s">
         <v>26</v>
       </c>
@@ -21133,7 +21148,7 @@
   <dimension ref="A1:Z117"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A69" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
@@ -25599,6 +25614,95 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47342654-4E89-4C46-9D18-7FBA61993882}">
+  <dimension ref="A1:U2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="3" max="3" width="10.6640625" customWidth="1"/>
+    <col min="6" max="6" width="19.109375" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" s="21" customFormat="1" ht="59.25" customHeight="1">
+      <c r="A1" s="116" t="s">
+        <v>1052</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1" s="25"/>
+      <c r="M1" s="25"/>
+      <c r="N1" s="25"/>
+      <c r="O1" s="25"/>
+      <c r="P1" s="25"/>
+      <c r="Q1" s="25"/>
+      <c r="R1" s="25"/>
+      <c r="S1" s="25"/>
+      <c r="T1" s="25"/>
+      <c r="U1" s="25"/>
+    </row>
+    <row r="2" spans="1:21" s="21" customFormat="1">
+      <c r="A2" s="115">
+        <v>44441</v>
+      </c>
+      <c r="B2" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>353</v>
+      </c>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10" t="s">
+        <v>225</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>1051</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="H2" s="21" t="s">
+        <v>356</v>
+      </c>
+      <c r="I2" s="27" t="s">
+        <v>112</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>

</xml_diff>

<commit_message>
I think this is a usable version of CW3M, except for the McKenzie basin where I'm developing the wetland model. Flow.cpp - Comment out the log messages saying that CheckSurfaceH2O() has failed. This is temporary.
</commit_message>
<xml_diff>
--- a/DataCW3M/CW3MdigitalHandbook/CW3MdataDictionary.xlsx
+++ b/DataCW3M/CW3MdigitalHandbook/CW3MdataDictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\CW3MdigitalHandbook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6CED669-9D6E-4566-9614-268A875A6613}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F076E750-68F6-4F8E-BA50-08B31C8F7F0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Necessary input data" sheetId="7" r:id="rId1"/>
@@ -9268,8 +9268,8 @@
   <dimension ref="A1:Z1052"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3:XFD3"/>
+      <pane ySplit="3" topLeftCell="A216" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K160" sqref="K160"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -11750,42 +11750,42 @@
       <c r="T72" s="7"/>
       <c r="U72" s="7"/>
     </row>
-    <row r="73" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A73" s="6"/>
-      <c r="B73" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C73" s="7" t="s">
+    <row r="73" spans="1:26" s="65" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A73" s="66"/>
+      <c r="B73" s="66" t="s">
+        <v>22</v>
+      </c>
+      <c r="C73" s="64" t="s">
         <v>353</v>
       </c>
-      <c r="D73" s="8"/>
-      <c r="E73" s="8" t="s">
+      <c r="D73" s="62"/>
+      <c r="E73" s="62" t="s">
         <v>225</v>
       </c>
-      <c r="F73" s="10" t="s">
+      <c r="F73" s="62" t="s">
         <v>1051</v>
       </c>
-      <c r="G73" s="8" t="s">
+      <c r="G73" s="62" t="s">
         <v>26</v>
       </c>
-      <c r="H73" s="14" t="s">
+      <c r="H73" s="61" t="s">
         <v>356</v>
       </c>
-      <c r="I73" s="27" t="s">
+      <c r="I73" s="74" t="s">
         <v>112</v>
       </c>
-      <c r="J73" s="3"/>
-      <c r="K73" s="7"/>
-      <c r="L73" s="7"/>
-      <c r="M73" s="7"/>
-      <c r="N73" s="7"/>
-      <c r="O73" s="7"/>
-      <c r="P73" s="7"/>
-      <c r="Q73" s="7"/>
-      <c r="R73" s="7"/>
-      <c r="S73" s="7"/>
-      <c r="T73" s="7"/>
-      <c r="U73" s="7"/>
+      <c r="J73" s="68"/>
+      <c r="K73" s="64"/>
+      <c r="L73" s="64"/>
+      <c r="M73" s="64"/>
+      <c r="N73" s="64"/>
+      <c r="O73" s="64"/>
+      <c r="P73" s="64"/>
+      <c r="Q73" s="64"/>
+      <c r="R73" s="64"/>
+      <c r="S73" s="64"/>
+      <c r="T73" s="64"/>
+      <c r="U73" s="64"/>
     </row>
     <row r="74" spans="1:26" ht="14.25" customHeight="1">
       <c r="A74" s="6"/>
@@ -21148,7 +21148,7 @@
   <dimension ref="A1:Z117"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="4" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
@@ -24094,8 +24094,8 @@
   </sheetPr>
   <dimension ref="A1:Z47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
@@ -25617,7 +25617,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47342654-4E89-4C46-9D18-7FBA61993882}">
   <dimension ref="A1:U2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>

</xml_diff>

<commit_message>
Commit David Holman's new subbasin shapefiles to the repository.
</commit_message>
<xml_diff>
--- a/DataCW3M/CW3MdigitalHandbook/CW3MdataDictionary.xlsx
+++ b/DataCW3M/CW3MdigitalHandbook/CW3MdataDictionary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\CW3MdigitalHandbook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F076E750-68F6-4F8E-BA50-08B31C8F7F0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AAE678A-C111-4E09-8B63-4853C9E4E5C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24095,7 +24095,7 @@
   <dimension ref="A1:Z47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="2" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
lulc.xml - Add class 62221 PABFdrying
</commit_message>
<xml_diff>
--- a/DataCW3M/CW3MdigitalHandbook/CW3MdataDictionary.xlsx
+++ b/DataCW3M/CW3MdigitalHandbook/CW3MdataDictionary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CW3M.git\trunk\DataCW3M\CW3MdigitalHandbook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAF7C273-D490-419E-9893-35050E720825}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34520DB8-B06E-4A3B-A3AC-C3A447BC28A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1110" yWindow="870" windowWidth="23940" windowHeight="13845" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Necessary input data" sheetId="7" r:id="rId1"/>
@@ -9295,7 +9295,7 @@
   <dimension ref="A1:Z1056"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A90" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="3" topLeftCell="A214" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="H101" sqref="H101"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
WORK-IN-PROGRESS. Now at least it builds successfully. STMengine probably still won't run.
</commit_message>
<xml_diff>
--- a/DataCW3M/CW3MdigitalHandbook/CW3MdataDictionary.xlsx
+++ b/DataCW3M/CW3MdigitalHandbook/CW3MdataDictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\CW3MdigitalHandbook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37763671-031D-43C5-93C2-E4AA8327FCB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B89268C7-4323-4FE7-9F7F-71A9599C09F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1536" yWindow="2604" windowWidth="21120" windowHeight="9588" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1020" yWindow="852" windowWidth="21120" windowHeight="9588" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Necessary input data" sheetId="7" r:id="rId1"/>
@@ -78,7 +78,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H272" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+    <comment ref="H275" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -97,7 +97,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3153" uniqueCount="1062">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3168" uniqueCount="1069">
   <si>
     <t>LULC_A</t>
   </si>
@@ -3284,6 +3284,27 @@
   </si>
   <si>
     <t>calculated in VegSTM and STMengine</t>
+  </si>
+  <si>
+    <t>WET_FRAC</t>
+  </si>
+  <si>
+    <t>WETAVGDPTH</t>
+  </si>
+  <si>
+    <t>WETLONGEST</t>
+  </si>
+  <si>
+    <t>days</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the length of the longest sequence of consecutive days when WETNESS &gt;= 0 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">the fraction of days in the year when WETNESS &gt;= 0, i.e. the soil surface is saturated or covered by standing water </t>
+  </si>
+  <si>
+    <t xml:space="preserve">the average depth of the standing water on the days when the soil surface is saturated or covered by standing water, the average of all the WETNESS values greater than or equal to zero </t>
   </si>
 </sst>
 </file>
@@ -9292,11 +9313,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Z1056"/>
+  <dimension ref="A1:Z1059"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A90" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E96" sqref="E96"/>
+      <pane ySplit="3" topLeftCell="A226" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H232" sqref="H232"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -17235,24 +17256,22 @@
       <c r="A231" s="28"/>
       <c r="B231" s="28"/>
       <c r="C231" s="7" t="s">
-        <v>824</v>
+        <v>1062</v>
       </c>
       <c r="D231" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="E231" s="70" t="s">
-        <v>405</v>
+      <c r="E231" s="10" t="s">
+        <v>987</v>
       </c>
       <c r="F231" s="10"/>
       <c r="G231" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="H231" s="25" t="s">
-        <v>825</v>
-      </c>
-      <c r="I231" s="27" t="s">
-        <v>528</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="H231" s="57" t="s">
+        <v>1067</v>
+      </c>
+      <c r="I231" s="27"/>
       <c r="J231" s="3"/>
       <c r="K231" s="7"/>
       <c r="L231" s="7"/>
@@ -17270,18 +17289,20 @@
       <c r="A232" s="28"/>
       <c r="B232" s="28"/>
       <c r="C232" s="7" t="s">
-        <v>1003</v>
+        <v>1063</v>
       </c>
       <c r="D232" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="E232" s="70"/>
+        <v>107</v>
+      </c>
+      <c r="E232" s="10" t="s">
+        <v>1025</v>
+      </c>
       <c r="F232" s="10"/>
       <c r="G232" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="H232" s="25" t="s">
-        <v>1004</v>
+        <v>26</v>
+      </c>
+      <c r="H232" s="57" t="s">
+        <v>1068</v>
       </c>
       <c r="I232" s="27"/>
       <c r="J232" s="3"/>
@@ -17297,262 +17318,258 @@
       <c r="T232" s="7"/>
       <c r="U232" s="7"/>
     </row>
-    <row r="233" spans="1:21" s="65" customFormat="1" ht="13.95" customHeight="1">
-      <c r="A233" s="66"/>
-      <c r="B233" s="66"/>
-      <c r="C233" s="64" t="s">
+    <row r="233" spans="1:21" s="21" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A233" s="28"/>
+      <c r="B233" s="28"/>
+      <c r="C233" s="7" t="s">
+        <v>824</v>
+      </c>
+      <c r="D233" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="E233" s="70" t="s">
+        <v>405</v>
+      </c>
+      <c r="F233" s="10"/>
+      <c r="G233" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="H233" s="25" t="s">
+        <v>825</v>
+      </c>
+      <c r="I233" s="27" t="s">
+        <v>528</v>
+      </c>
+      <c r="J233" s="3"/>
+      <c r="K233" s="7"/>
+      <c r="L233" s="7"/>
+      <c r="M233" s="7"/>
+      <c r="N233" s="7"/>
+      <c r="O233" s="7"/>
+      <c r="P233" s="7"/>
+      <c r="Q233" s="7"/>
+      <c r="R233" s="7"/>
+      <c r="S233" s="7"/>
+      <c r="T233" s="7"/>
+      <c r="U233" s="7"/>
+    </row>
+    <row r="234" spans="1:21" s="21" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A234" s="28"/>
+      <c r="B234" s="28"/>
+      <c r="C234" s="7" t="s">
+        <v>1003</v>
+      </c>
+      <c r="D234" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="E234" s="70"/>
+      <c r="F234" s="10"/>
+      <c r="G234" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="H234" s="25" t="s">
+        <v>1004</v>
+      </c>
+      <c r="I234" s="27"/>
+      <c r="J234" s="3"/>
+      <c r="K234" s="7"/>
+      <c r="L234" s="7"/>
+      <c r="M234" s="7"/>
+      <c r="N234" s="7"/>
+      <c r="O234" s="7"/>
+      <c r="P234" s="7"/>
+      <c r="Q234" s="7"/>
+      <c r="R234" s="7"/>
+      <c r="S234" s="7"/>
+      <c r="T234" s="7"/>
+      <c r="U234" s="7"/>
+    </row>
+    <row r="235" spans="1:21" s="65" customFormat="1" ht="13.95" customHeight="1">
+      <c r="A235" s="66"/>
+      <c r="B235" s="66"/>
+      <c r="C235" s="64" t="s">
         <v>826</v>
       </c>
-      <c r="D233" s="62" t="s">
+      <c r="D235" s="62" t="s">
         <v>28</v>
       </c>
-      <c r="E233" s="62" t="s">
+      <c r="E235" s="62" t="s">
         <v>93</v>
       </c>
-      <c r="F233" s="62" t="s">
+      <c r="F235" s="62" t="s">
         <v>64</v>
       </c>
-      <c r="G233" s="62" t="s">
+      <c r="G235" s="62" t="s">
         <v>26</v>
       </c>
-      <c r="H233" s="61" t="s">
+      <c r="H235" s="61" t="s">
         <v>827</v>
       </c>
-      <c r="I233" s="74" t="s">
+      <c r="I235" s="74" t="s">
         <v>828</v>
       </c>
-      <c r="J233" s="68"/>
-      <c r="K233" s="64"/>
-      <c r="L233" s="64"/>
-      <c r="M233" s="64"/>
-      <c r="N233" s="64"/>
-      <c r="O233" s="64"/>
-      <c r="P233" s="64"/>
-      <c r="Q233" s="64"/>
-      <c r="R233" s="64"/>
-      <c r="S233" s="64"/>
-      <c r="T233" s="64"/>
-      <c r="U233" s="64"/>
-    </row>
-    <row r="234" spans="1:21" s="91" customFormat="1" ht="13.95" customHeight="1">
-      <c r="A234" s="96"/>
-      <c r="B234" s="96"/>
-      <c r="C234" s="97" t="s">
+      <c r="J235" s="68"/>
+      <c r="K235" s="64"/>
+      <c r="L235" s="64"/>
+      <c r="M235" s="64"/>
+      <c r="N235" s="64"/>
+      <c r="O235" s="64"/>
+      <c r="P235" s="64"/>
+      <c r="Q235" s="64"/>
+      <c r="R235" s="64"/>
+      <c r="S235" s="64"/>
+      <c r="T235" s="64"/>
+      <c r="U235" s="64"/>
+    </row>
+    <row r="236" spans="1:21" s="91" customFormat="1" ht="13.95" customHeight="1">
+      <c r="A236" s="96"/>
+      <c r="B236" s="96"/>
+      <c r="C236" s="97" t="s">
         <v>995</v>
       </c>
-      <c r="D234" s="100" t="s">
+      <c r="D236" s="100" t="s">
         <v>107</v>
       </c>
-      <c r="E234" s="100" t="s">
+      <c r="E236" s="100" t="s">
         <v>72</v>
       </c>
-      <c r="F234" s="100"/>
-      <c r="G234" s="100" t="s">
+      <c r="F236" s="100"/>
+      <c r="G236" s="100" t="s">
         <v>26</v>
       </c>
-      <c r="H234" s="91" t="s">
+      <c r="H236" s="91" t="s">
         <v>996</v>
       </c>
-      <c r="I234" s="98"/>
-      <c r="J234" s="84"/>
-      <c r="K234" s="97"/>
-      <c r="L234" s="97"/>
-      <c r="M234" s="97"/>
-      <c r="N234" s="97"/>
-      <c r="O234" s="97"/>
-      <c r="P234" s="97"/>
-      <c r="Q234" s="97"/>
-      <c r="R234" s="97"/>
-      <c r="S234" s="97"/>
-      <c r="T234" s="97"/>
-      <c r="U234" s="97"/>
-    </row>
-    <row r="235" spans="1:21" s="91" customFormat="1" ht="13.95" customHeight="1">
-      <c r="A235" s="96"/>
-      <c r="B235" s="96"/>
-      <c r="C235" s="97" t="s">
+      <c r="I236" s="98"/>
+      <c r="J236" s="84"/>
+      <c r="K236" s="97"/>
+      <c r="L236" s="97"/>
+      <c r="M236" s="97"/>
+      <c r="N236" s="97"/>
+      <c r="O236" s="97"/>
+      <c r="P236" s="97"/>
+      <c r="Q236" s="97"/>
+      <c r="R236" s="97"/>
+      <c r="S236" s="97"/>
+      <c r="T236" s="97"/>
+      <c r="U236" s="97"/>
+    </row>
+    <row r="237" spans="1:21" s="91" customFormat="1" ht="13.95" customHeight="1">
+      <c r="A237" s="96"/>
+      <c r="B237" s="96"/>
+      <c r="C237" s="97" t="s">
+        <v>1064</v>
+      </c>
+      <c r="D237" s="100" t="s">
+        <v>107</v>
+      </c>
+      <c r="E237" s="100" t="s">
+        <v>1065</v>
+      </c>
+      <c r="F237" s="100"/>
+      <c r="G237" s="100" t="s">
+        <v>26</v>
+      </c>
+      <c r="H237" s="57" t="s">
+        <v>1066</v>
+      </c>
+      <c r="I237" s="98"/>
+      <c r="J237" s="84"/>
+      <c r="K237" s="97"/>
+      <c r="L237" s="97"/>
+      <c r="M237" s="97"/>
+      <c r="N237" s="97"/>
+      <c r="O237" s="97"/>
+      <c r="P237" s="97"/>
+      <c r="Q237" s="97"/>
+      <c r="R237" s="97"/>
+      <c r="S237" s="97"/>
+      <c r="T237" s="97"/>
+      <c r="U237" s="97"/>
+    </row>
+    <row r="238" spans="1:21" s="91" customFormat="1" ht="13.95" customHeight="1">
+      <c r="A238" s="96"/>
+      <c r="B238" s="96"/>
+      <c r="C238" s="97" t="s">
         <v>983</v>
       </c>
-      <c r="D235" s="99" t="s">
+      <c r="D238" s="99" t="s">
         <v>107</v>
       </c>
-      <c r="E235" s="99" t="s">
+      <c r="E238" s="99" t="s">
         <v>171</v>
       </c>
-      <c r="F235" s="99" t="s">
+      <c r="F238" s="99" t="s">
         <v>821</v>
       </c>
-      <c r="G235" s="99" t="s">
+      <c r="G238" s="99" t="s">
         <v>26</v>
       </c>
-      <c r="H235" s="77" t="s">
+      <c r="H238" s="77" t="s">
         <v>984</v>
       </c>
-      <c r="I235" s="98"/>
-      <c r="J235" s="84"/>
-      <c r="K235" s="97"/>
-      <c r="L235" s="97"/>
-      <c r="M235" s="97"/>
-      <c r="N235" s="97"/>
-      <c r="O235" s="97"/>
-      <c r="P235" s="97"/>
-      <c r="Q235" s="97"/>
-      <c r="R235" s="97"/>
-      <c r="S235" s="97"/>
-      <c r="T235" s="97"/>
-      <c r="U235" s="97"/>
-    </row>
-    <row r="236" spans="1:21" s="21" customFormat="1" ht="16.95" customHeight="1">
-      <c r="A236" s="28"/>
-      <c r="B236" s="28"/>
-      <c r="C236" s="21" t="s">
+      <c r="I238" s="98"/>
+      <c r="J238" s="84"/>
+      <c r="K238" s="97"/>
+      <c r="L238" s="97"/>
+      <c r="M238" s="97"/>
+      <c r="N238" s="97"/>
+      <c r="O238" s="97"/>
+      <c r="P238" s="97"/>
+      <c r="Q238" s="97"/>
+      <c r="R238" s="97"/>
+      <c r="S238" s="97"/>
+      <c r="T238" s="97"/>
+      <c r="U238" s="97"/>
+    </row>
+    <row r="239" spans="1:21" s="21" customFormat="1" ht="16.95" customHeight="1">
+      <c r="A239" s="28"/>
+      <c r="B239" s="28"/>
+      <c r="C239" s="21" t="s">
         <v>508</v>
       </c>
-      <c r="D236" s="10" t="s">
+      <c r="D239" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="E236" s="10" t="s">
+      <c r="E239" s="10" t="s">
         <v>509</v>
       </c>
-      <c r="F236" s="10" t="s">
+      <c r="F239" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="G236" s="10" t="s">
+      <c r="G239" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="H236" s="21" t="s">
+      <c r="H239" s="21" t="s">
         <v>724</v>
       </c>
-      <c r="I236" s="27" t="s">
+      <c r="I239" s="27" t="s">
         <v>810</v>
       </c>
-      <c r="J236" s="23"/>
-    </row>
-    <row r="237" spans="1:21" ht="42.75" customHeight="1">
-      <c r="A237" s="6"/>
-      <c r="B237" s="6" t="s">
-        <v>158</v>
-      </c>
-      <c r="C237" s="7" t="s">
-        <v>725</v>
-      </c>
-      <c r="D237" s="8"/>
-      <c r="E237" s="8" t="s">
-        <v>726</v>
-      </c>
-      <c r="F237" s="10"/>
-      <c r="G237" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="H237" s="14" t="s">
-        <v>727</v>
-      </c>
-      <c r="I237" s="27" t="s">
-        <v>723</v>
-      </c>
-      <c r="J237" s="3"/>
-      <c r="K237" s="7"/>
-      <c r="L237" s="7"/>
-      <c r="M237" s="7"/>
-      <c r="N237" s="7"/>
-      <c r="O237" s="7"/>
-      <c r="P237" s="7"/>
-      <c r="Q237" s="7"/>
-      <c r="R237" s="7"/>
-      <c r="S237" s="7"/>
-      <c r="T237" s="7"/>
-      <c r="U237" s="7"/>
-    </row>
-    <row r="238" spans="1:21" ht="14.25" customHeight="1">
-      <c r="A238" s="6"/>
-      <c r="B238" s="6" t="s">
-        <v>158</v>
-      </c>
-      <c r="C238" s="7" t="s">
-        <v>728</v>
-      </c>
-      <c r="D238" s="8"/>
-      <c r="E238" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="F238" s="10"/>
-      <c r="G238" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="H238" s="14" t="s">
-        <v>729</v>
-      </c>
-      <c r="I238" s="27" t="s">
-        <v>723</v>
-      </c>
-      <c r="J238" s="3"/>
-      <c r="K238" s="7"/>
-      <c r="L238" s="7"/>
-      <c r="M238" s="7"/>
-      <c r="N238" s="7"/>
-      <c r="O238" s="7"/>
-      <c r="P238" s="7"/>
-      <c r="Q238" s="7"/>
-      <c r="R238" s="7"/>
-      <c r="S238" s="7"/>
-      <c r="T238" s="7"/>
-      <c r="U238" s="7"/>
-    </row>
-    <row r="239" spans="1:21" ht="14.25" customHeight="1">
-      <c r="A239" s="6"/>
-      <c r="B239" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C239" s="7" t="s">
-        <v>730</v>
-      </c>
-      <c r="D239" s="8"/>
-      <c r="E239" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="F239" s="10"/>
-      <c r="G239" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="H239" s="14" t="s">
-        <v>731</v>
-      </c>
-      <c r="I239" s="27" t="s">
-        <v>723</v>
-      </c>
-      <c r="J239" s="3"/>
-      <c r="K239" s="7"/>
-      <c r="L239" s="7"/>
-      <c r="M239" s="7"/>
-      <c r="N239" s="7"/>
-      <c r="O239" s="7"/>
-      <c r="P239" s="7"/>
-      <c r="Q239" s="7"/>
-      <c r="R239" s="7"/>
-      <c r="S239" s="7"/>
-      <c r="T239" s="7"/>
-      <c r="U239" s="7"/>
-    </row>
-    <row r="240" spans="1:21" ht="14.25" customHeight="1">
+      <c r="J239" s="23"/>
+    </row>
+    <row r="240" spans="1:21" ht="42.75" customHeight="1">
       <c r="A240" s="6"/>
       <c r="B240" s="6" t="s">
         <v>158</v>
       </c>
       <c r="C240" s="7" t="s">
-        <v>732</v>
+        <v>725</v>
       </c>
       <c r="D240" s="8"/>
       <c r="E240" s="8" t="s">
-        <v>69</v>
+        <v>726</v>
       </c>
       <c r="F240" s="10"/>
       <c r="G240" s="8" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="H240" s="14" t="s">
-        <v>733</v>
-      </c>
-      <c r="I240" s="27"/>
+        <v>727</v>
+      </c>
+      <c r="I240" s="27" t="s">
+        <v>723</v>
+      </c>
       <c r="J240" s="3"/>
       <c r="K240" s="7"/>
       <c r="L240" s="7"/>
@@ -17572,18 +17589,18 @@
         <v>158</v>
       </c>
       <c r="C241" s="7" t="s">
-        <v>734</v>
+        <v>728</v>
       </c>
       <c r="D241" s="8"/>
       <c r="E241" s="8" t="s">
-        <v>225</v>
+        <v>69</v>
       </c>
       <c r="F241" s="10"/>
       <c r="G241" s="8" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="H241" s="14" t="s">
-        <v>735</v>
+        <v>729</v>
       </c>
       <c r="I241" s="27" t="s">
         <v>723</v>
@@ -17604,21 +17621,21 @@
     <row r="242" spans="1:26" ht="14.25" customHeight="1">
       <c r="A242" s="6"/>
       <c r="B242" s="6" t="s">
-        <v>158</v>
+        <v>22</v>
       </c>
       <c r="C242" s="7" t="s">
-        <v>736</v>
+        <v>730</v>
       </c>
       <c r="D242" s="8"/>
       <c r="E242" s="8" t="s">
-        <v>225</v>
+        <v>69</v>
       </c>
       <c r="F242" s="10"/>
       <c r="G242" s="8" t="s">
         <v>26</v>
       </c>
       <c r="H242" s="14" t="s">
-        <v>737</v>
+        <v>731</v>
       </c>
       <c r="I242" s="27" t="s">
         <v>723</v>
@@ -17639,23 +17656,23 @@
     <row r="243" spans="1:26" ht="14.25" customHeight="1">
       <c r="A243" s="6"/>
       <c r="B243" s="6" t="s">
-        <v>22</v>
+        <v>158</v>
       </c>
       <c r="C243" s="7" t="s">
-        <v>738</v>
+        <v>732</v>
       </c>
       <c r="D243" s="8"/>
-      <c r="E243" s="8"/>
+      <c r="E243" s="8" t="s">
+        <v>69</v>
+      </c>
       <c r="F243" s="10"/>
       <c r="G243" s="8" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="H243" s="14" t="s">
-        <v>739</v>
-      </c>
-      <c r="I243" s="27" t="s">
-        <v>112</v>
-      </c>
+        <v>733</v>
+      </c>
+      <c r="I243" s="27"/>
       <c r="J243" s="3"/>
       <c r="K243" s="7"/>
       <c r="L243" s="7"/>
@@ -17675,21 +17692,21 @@
         <v>158</v>
       </c>
       <c r="C244" s="7" t="s">
-        <v>740</v>
+        <v>734</v>
       </c>
       <c r="D244" s="8"/>
       <c r="E244" s="8" t="s">
-        <v>741</v>
+        <v>225</v>
       </c>
       <c r="F244" s="10"/>
       <c r="G244" s="8" t="s">
         <v>26</v>
       </c>
       <c r="H244" s="14" t="s">
-        <v>742</v>
+        <v>735</v>
       </c>
       <c r="I244" s="27" t="s">
-        <v>112</v>
+        <v>723</v>
       </c>
       <c r="J244" s="3"/>
       <c r="K244" s="7"/>
@@ -17705,28 +17722,26 @@
       <c r="U244" s="7"/>
     </row>
     <row r="245" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A245" s="6" t="s">
-        <v>308</v>
-      </c>
+      <c r="A245" s="6"/>
       <c r="B245" s="6" t="s">
-        <v>22</v>
+        <v>158</v>
       </c>
       <c r="C245" s="7" t="s">
-        <v>743</v>
+        <v>736</v>
       </c>
       <c r="D245" s="8"/>
       <c r="E245" s="8" t="s">
-        <v>744</v>
+        <v>225</v>
       </c>
       <c r="F245" s="10"/>
       <c r="G245" s="8" t="s">
         <v>26</v>
       </c>
       <c r="H245" s="14" t="s">
-        <v>745</v>
+        <v>737</v>
       </c>
       <c r="I245" s="27" t="s">
-        <v>112</v>
+        <v>723</v>
       </c>
       <c r="J245" s="3"/>
       <c r="K245" s="7"/>
@@ -17744,29 +17759,25 @@
     <row r="246" spans="1:26" ht="14.25" customHeight="1">
       <c r="A246" s="6"/>
       <c r="B246" s="6" t="s">
-        <v>158</v>
+        <v>22</v>
       </c>
       <c r="C246" s="7" t="s">
-        <v>379</v>
+        <v>738</v>
       </c>
       <c r="D246" s="8"/>
-      <c r="E246" s="8" t="s">
-        <v>195</v>
-      </c>
+      <c r="E246" s="8"/>
       <c r="F246" s="10"/>
       <c r="G246" s="8" t="s">
         <v>26</v>
       </c>
       <c r="H246" s="14" t="s">
-        <v>746</v>
+        <v>739</v>
       </c>
       <c r="I246" s="27" t="s">
         <v>112</v>
       </c>
       <c r="J246" s="3"/>
-      <c r="K246" s="3" t="s">
-        <v>188</v>
-      </c>
+      <c r="K246" s="7"/>
       <c r="L246" s="7"/>
       <c r="M246" s="7"/>
       <c r="N246" s="7"/>
@@ -17777,32 +17788,25 @@
       <c r="S246" s="7"/>
       <c r="T246" s="7"/>
       <c r="U246" s="7"/>
-      <c r="V246" s="7"/>
-      <c r="W246" s="7"/>
-      <c r="X246" s="7"/>
-      <c r="Y246" s="7"/>
-      <c r="Z246" s="7"/>
     </row>
     <row r="247" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A247" s="6" t="s">
-        <v>747</v>
-      </c>
+      <c r="A247" s="6"/>
       <c r="B247" s="6" t="s">
-        <v>22</v>
+        <v>158</v>
       </c>
       <c r="C247" s="7" t="s">
-        <v>748</v>
+        <v>740</v>
       </c>
       <c r="D247" s="8"/>
       <c r="E247" s="8" t="s">
-        <v>69</v>
+        <v>741</v>
       </c>
       <c r="F247" s="10"/>
       <c r="G247" s="8" t="s">
         <v>26</v>
       </c>
       <c r="H247" s="14" t="s">
-        <v>749</v>
+        <v>742</v>
       </c>
       <c r="I247" s="27" t="s">
         <v>112</v>
@@ -17821,23 +17825,25 @@
       <c r="U247" s="7"/>
     </row>
     <row r="248" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A248" s="6"/>
+      <c r="A248" s="6" t="s">
+        <v>308</v>
+      </c>
       <c r="B248" s="6" t="s">
         <v>22</v>
       </c>
       <c r="C248" s="7" t="s">
-        <v>750</v>
+        <v>743</v>
       </c>
       <c r="D248" s="8"/>
       <c r="E248" s="8" t="s">
-        <v>751</v>
+        <v>744</v>
       </c>
       <c r="F248" s="10"/>
       <c r="G248" s="8" t="s">
         <v>26</v>
       </c>
       <c r="H248" s="14" t="s">
-        <v>752</v>
+        <v>745</v>
       </c>
       <c r="I248" s="27" t="s">
         <v>112</v>
@@ -17858,27 +17864,29 @@
     <row r="249" spans="1:26" ht="14.25" customHeight="1">
       <c r="A249" s="6"/>
       <c r="B249" s="6" t="s">
-        <v>22</v>
+        <v>158</v>
       </c>
       <c r="C249" s="7" t="s">
-        <v>753</v>
+        <v>379</v>
       </c>
       <c r="D249" s="8"/>
       <c r="E249" s="8" t="s">
-        <v>754</v>
+        <v>195</v>
       </c>
       <c r="F249" s="10"/>
       <c r="G249" s="8" t="s">
         <v>26</v>
       </c>
       <c r="H249" s="14" t="s">
-        <v>755</v>
+        <v>746</v>
       </c>
       <c r="I249" s="27" t="s">
         <v>112</v>
       </c>
       <c r="J249" s="3"/>
-      <c r="K249" s="7"/>
+      <c r="K249" s="3" t="s">
+        <v>188</v>
+      </c>
       <c r="L249" s="7"/>
       <c r="M249" s="7"/>
       <c r="N249" s="7"/>
@@ -17889,25 +17897,32 @@
       <c r="S249" s="7"/>
       <c r="T249" s="7"/>
       <c r="U249" s="7"/>
+      <c r="V249" s="7"/>
+      <c r="W249" s="7"/>
+      <c r="X249" s="7"/>
+      <c r="Y249" s="7"/>
+      <c r="Z249" s="7"/>
     </row>
     <row r="250" spans="1:26" ht="14.25" customHeight="1">
       <c r="A250" s="6" t="s">
-        <v>308</v>
+        <v>747</v>
       </c>
       <c r="B250" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C250" s="8" t="s">
-        <v>756</v>
+      <c r="C250" s="7" t="s">
+        <v>748</v>
       </c>
       <c r="D250" s="8"/>
-      <c r="E250" s="8"/>
+      <c r="E250" s="8" t="s">
+        <v>69</v>
+      </c>
       <c r="F250" s="10"/>
       <c r="G250" s="8" t="s">
         <v>26</v>
       </c>
       <c r="H250" s="14" t="s">
-        <v>757</v>
+        <v>749</v>
       </c>
       <c r="I250" s="27" t="s">
         <v>112</v>
@@ -17926,23 +17941,23 @@
       <c r="U250" s="7"/>
     </row>
     <row r="251" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A251" s="6" t="s">
-        <v>308</v>
-      </c>
+      <c r="A251" s="6"/>
       <c r="B251" s="6" t="s">
         <v>22</v>
       </c>
       <c r="C251" s="7" t="s">
-        <v>758</v>
+        <v>750</v>
       </c>
       <c r="D251" s="8"/>
-      <c r="E251" s="8"/>
+      <c r="E251" s="8" t="s">
+        <v>751</v>
+      </c>
       <c r="F251" s="10"/>
       <c r="G251" s="8" t="s">
         <v>26</v>
       </c>
       <c r="H251" s="14" t="s">
-        <v>757</v>
+        <v>752</v>
       </c>
       <c r="I251" s="27" t="s">
         <v>112</v>
@@ -17961,23 +17976,23 @@
       <c r="U251" s="7"/>
     </row>
     <row r="252" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A252" s="6" t="s">
-        <v>308</v>
-      </c>
+      <c r="A252" s="6"/>
       <c r="B252" s="6" t="s">
         <v>22</v>
       </c>
       <c r="C252" s="7" t="s">
-        <v>759</v>
+        <v>753</v>
       </c>
       <c r="D252" s="8"/>
-      <c r="E252" s="8"/>
+      <c r="E252" s="8" t="s">
+        <v>754</v>
+      </c>
       <c r="F252" s="10"/>
       <c r="G252" s="8" t="s">
         <v>26</v>
       </c>
       <c r="H252" s="14" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="I252" s="27" t="s">
         <v>112</v>
@@ -18002,8 +18017,8 @@
       <c r="B253" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C253" s="7" t="s">
-        <v>760</v>
+      <c r="C253" s="8" t="s">
+        <v>756</v>
       </c>
       <c r="D253" s="8"/>
       <c r="E253" s="8"/>
@@ -18038,7 +18053,7 @@
         <v>22</v>
       </c>
       <c r="C254" s="7" t="s">
-        <v>761</v>
+        <v>758</v>
       </c>
       <c r="D254" s="8"/>
       <c r="E254" s="8"/>
@@ -18073,7 +18088,7 @@
         <v>22</v>
       </c>
       <c r="C255" s="7" t="s">
-        <v>762</v>
+        <v>759</v>
       </c>
       <c r="D255" s="8"/>
       <c r="E255" s="8"/>
@@ -18108,7 +18123,7 @@
         <v>22</v>
       </c>
       <c r="C256" s="7" t="s">
-        <v>763</v>
+        <v>760</v>
       </c>
       <c r="D256" s="8"/>
       <c r="E256" s="8"/>
@@ -18135,7 +18150,7 @@
       <c r="T256" s="7"/>
       <c r="U256" s="7"/>
     </row>
-    <row r="257" spans="1:26" ht="14.25" customHeight="1">
+    <row r="257" spans="1:21" ht="14.25" customHeight="1">
       <c r="A257" s="6" t="s">
         <v>308</v>
       </c>
@@ -18143,7 +18158,7 @@
         <v>22</v>
       </c>
       <c r="C257" s="7" t="s">
-        <v>764</v>
+        <v>761</v>
       </c>
       <c r="D257" s="8"/>
       <c r="E257" s="8"/>
@@ -18170,7 +18185,7 @@
       <c r="T257" s="7"/>
       <c r="U257" s="7"/>
     </row>
-    <row r="258" spans="1:26" ht="14.25" customHeight="1">
+    <row r="258" spans="1:21" ht="14.25" customHeight="1">
       <c r="A258" s="6" t="s">
         <v>308</v>
       </c>
@@ -18178,7 +18193,7 @@
         <v>22</v>
       </c>
       <c r="C258" s="7" t="s">
-        <v>765</v>
+        <v>762</v>
       </c>
       <c r="D258" s="8"/>
       <c r="E258" s="8"/>
@@ -18205,7 +18220,7 @@
       <c r="T258" s="7"/>
       <c r="U258" s="7"/>
     </row>
-    <row r="259" spans="1:26" ht="14.25" customHeight="1">
+    <row r="259" spans="1:21" ht="14.25" customHeight="1">
       <c r="A259" s="6" t="s">
         <v>308</v>
       </c>
@@ -18213,7 +18228,7 @@
         <v>22</v>
       </c>
       <c r="C259" s="7" t="s">
-        <v>766</v>
+        <v>763</v>
       </c>
       <c r="D259" s="8"/>
       <c r="E259" s="8"/>
@@ -18240,7 +18255,7 @@
       <c r="T259" s="7"/>
       <c r="U259" s="7"/>
     </row>
-    <row r="260" spans="1:26" ht="14.25" customHeight="1">
+    <row r="260" spans="1:21" ht="14.25" customHeight="1">
       <c r="A260" s="6" t="s">
         <v>308</v>
       </c>
@@ -18248,7 +18263,7 @@
         <v>22</v>
       </c>
       <c r="C260" s="7" t="s">
-        <v>767</v>
+        <v>764</v>
       </c>
       <c r="D260" s="8"/>
       <c r="E260" s="8"/>
@@ -18275,7 +18290,7 @@
       <c r="T260" s="7"/>
       <c r="U260" s="7"/>
     </row>
-    <row r="261" spans="1:26" ht="14.25" customHeight="1">
+    <row r="261" spans="1:21" ht="14.25" customHeight="1">
       <c r="A261" s="6" t="s">
         <v>308</v>
       </c>
@@ -18283,7 +18298,7 @@
         <v>22</v>
       </c>
       <c r="C261" s="7" t="s">
-        <v>768</v>
+        <v>765</v>
       </c>
       <c r="D261" s="8"/>
       <c r="E261" s="8"/>
@@ -18310,7 +18325,7 @@
       <c r="T261" s="7"/>
       <c r="U261" s="7"/>
     </row>
-    <row r="262" spans="1:26" ht="14.25" customHeight="1">
+    <row r="262" spans="1:21" ht="14.25" customHeight="1">
       <c r="A262" s="6" t="s">
         <v>308</v>
       </c>
@@ -18318,7 +18333,7 @@
         <v>22</v>
       </c>
       <c r="C262" s="7" t="s">
-        <v>769</v>
+        <v>766</v>
       </c>
       <c r="D262" s="8"/>
       <c r="E262" s="8"/>
@@ -18345,7 +18360,7 @@
       <c r="T262" s="7"/>
       <c r="U262" s="7"/>
     </row>
-    <row r="263" spans="1:26" ht="14.25" customHeight="1">
+    <row r="263" spans="1:21" ht="14.25" customHeight="1">
       <c r="A263" s="6" t="s">
         <v>308</v>
       </c>
@@ -18353,7 +18368,7 @@
         <v>22</v>
       </c>
       <c r="C263" s="7" t="s">
-        <v>770</v>
+        <v>767</v>
       </c>
       <c r="D263" s="8"/>
       <c r="E263" s="8"/>
@@ -18380,7 +18395,7 @@
       <c r="T263" s="7"/>
       <c r="U263" s="7"/>
     </row>
-    <row r="264" spans="1:26" ht="14.25" customHeight="1">
+    <row r="264" spans="1:21" ht="14.25" customHeight="1">
       <c r="A264" s="6" t="s">
         <v>308</v>
       </c>
@@ -18388,7 +18403,7 @@
         <v>22</v>
       </c>
       <c r="C264" s="7" t="s">
-        <v>771</v>
+        <v>768</v>
       </c>
       <c r="D264" s="8"/>
       <c r="E264" s="8"/>
@@ -18415,7 +18430,7 @@
       <c r="T264" s="7"/>
       <c r="U264" s="7"/>
     </row>
-    <row r="265" spans="1:26" ht="14.25" customHeight="1">
+    <row r="265" spans="1:21" ht="14.25" customHeight="1">
       <c r="A265" s="6" t="s">
         <v>308</v>
       </c>
@@ -18423,7 +18438,7 @@
         <v>22</v>
       </c>
       <c r="C265" s="7" t="s">
-        <v>772</v>
+        <v>769</v>
       </c>
       <c r="D265" s="8"/>
       <c r="E265" s="8"/>
@@ -18450,7 +18465,7 @@
       <c r="T265" s="7"/>
       <c r="U265" s="7"/>
     </row>
-    <row r="266" spans="1:26" ht="14.25" customHeight="1">
+    <row r="266" spans="1:21" ht="14.25" customHeight="1">
       <c r="A266" s="6" t="s">
         <v>308</v>
       </c>
@@ -18458,7 +18473,7 @@
         <v>22</v>
       </c>
       <c r="C266" s="7" t="s">
-        <v>773</v>
+        <v>770</v>
       </c>
       <c r="D266" s="8"/>
       <c r="E266" s="8"/>
@@ -18485,20 +18500,28 @@
       <c r="T266" s="7"/>
       <c r="U266" s="7"/>
     </row>
-    <row r="267" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A267" s="6"/>
+    <row r="267" spans="1:21" ht="14.25" customHeight="1">
+      <c r="A267" s="6" t="s">
+        <v>308</v>
+      </c>
       <c r="B267" s="6" t="s">
         <v>22</v>
       </c>
       <c r="C267" s="7" t="s">
-        <v>774</v>
+        <v>771</v>
       </c>
       <c r="D267" s="8"/>
       <c r="E267" s="8"/>
       <c r="F267" s="10"/>
-      <c r="G267" s="8"/>
-      <c r="H267" s="14"/>
-      <c r="I267" s="27"/>
+      <c r="G267" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H267" s="14" t="s">
+        <v>757</v>
+      </c>
+      <c r="I267" s="27" t="s">
+        <v>112</v>
+      </c>
       <c r="J267" s="3"/>
       <c r="K267" s="7"/>
       <c r="L267" s="7"/>
@@ -18512,26 +18535,28 @@
       <c r="T267" s="7"/>
       <c r="U267" s="7"/>
     </row>
-    <row r="268" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A268" s="6"/>
+    <row r="268" spans="1:21" ht="14.25" customHeight="1">
+      <c r="A268" s="6" t="s">
+        <v>308</v>
+      </c>
       <c r="B268" s="6" t="s">
-        <v>158</v>
+        <v>22</v>
       </c>
       <c r="C268" s="7" t="s">
-        <v>775</v>
+        <v>772</v>
       </c>
       <c r="D268" s="8"/>
-      <c r="E268" s="8" t="s">
-        <v>156</v>
-      </c>
+      <c r="E268" s="8"/>
       <c r="F268" s="10"/>
       <c r="G268" s="8" t="s">
-        <v>776</v>
+        <v>26</v>
       </c>
       <c r="H268" s="14" t="s">
-        <v>777</v>
-      </c>
-      <c r="I268" s="27"/>
+        <v>757</v>
+      </c>
+      <c r="I268" s="27" t="s">
+        <v>112</v>
+      </c>
       <c r="J268" s="3"/>
       <c r="K268" s="7"/>
       <c r="L268" s="7"/>
@@ -18545,26 +18570,28 @@
       <c r="T268" s="7"/>
       <c r="U268" s="7"/>
     </row>
-    <row r="269" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A269" s="6"/>
+    <row r="269" spans="1:21" ht="14.25" customHeight="1">
+      <c r="A269" s="6" t="s">
+        <v>308</v>
+      </c>
       <c r="B269" s="6" t="s">
-        <v>158</v>
+        <v>22</v>
       </c>
       <c r="C269" s="7" t="s">
-        <v>778</v>
+        <v>773</v>
       </c>
       <c r="D269" s="8"/>
-      <c r="E269" s="8" t="s">
-        <v>156</v>
-      </c>
+      <c r="E269" s="8"/>
       <c r="F269" s="10"/>
       <c r="G269" s="8" t="s">
-        <v>776</v>
+        <v>26</v>
       </c>
       <c r="H269" s="14" t="s">
-        <v>779</v>
-      </c>
-      <c r="I269" s="27"/>
+        <v>757</v>
+      </c>
+      <c r="I269" s="27" t="s">
+        <v>112</v>
+      </c>
       <c r="J269" s="3"/>
       <c r="K269" s="7"/>
       <c r="L269" s="7"/>
@@ -18578,25 +18605,19 @@
       <c r="T269" s="7"/>
       <c r="U269" s="7"/>
     </row>
-    <row r="270" spans="1:26" ht="14.25" customHeight="1">
+    <row r="270" spans="1:21" ht="14.25" customHeight="1">
       <c r="A270" s="6"/>
       <c r="B270" s="6" t="s">
         <v>22</v>
       </c>
       <c r="C270" s="7" t="s">
-        <v>780</v>
+        <v>774</v>
       </c>
       <c r="D270" s="8"/>
-      <c r="E270" s="8" t="s">
-        <v>156</v>
-      </c>
+      <c r="E270" s="8"/>
       <c r="F270" s="10"/>
-      <c r="G270" s="8" t="s">
-        <v>776</v>
-      </c>
-      <c r="H270" s="14" t="s">
-        <v>781</v>
-      </c>
+      <c r="G270" s="8"/>
+      <c r="H270" s="14"/>
       <c r="I270" s="27"/>
       <c r="J270" s="3"/>
       <c r="K270" s="7"/>
@@ -18611,74 +18632,61 @@
       <c r="T270" s="7"/>
       <c r="U270" s="7"/>
     </row>
-    <row r="271" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A271" s="36" t="s">
-        <v>216</v>
-      </c>
-      <c r="B271" s="29"/>
-      <c r="C271" s="37" t="s">
-        <v>782</v>
-      </c>
-      <c r="D271" s="38" t="s">
-        <v>28</v>
-      </c>
-      <c r="E271" s="38" t="s">
-        <v>783</v>
-      </c>
-      <c r="F271" s="38" t="s">
-        <v>25</v>
-      </c>
-      <c r="G271" s="38" t="s">
-        <v>26</v>
-      </c>
-      <c r="H271" s="39" t="s">
-        <v>784</v>
-      </c>
-      <c r="I271" s="31"/>
-      <c r="J271" s="34"/>
-      <c r="K271" s="34"/>
-      <c r="L271" s="30"/>
-      <c r="M271" s="30"/>
-      <c r="N271" s="30"/>
-      <c r="O271" s="30"/>
-      <c r="P271" s="30"/>
-      <c r="Q271" s="30"/>
-      <c r="R271" s="30"/>
-      <c r="S271" s="30"/>
-      <c r="T271" s="30"/>
-      <c r="U271" s="30"/>
-      <c r="V271" s="35"/>
-      <c r="W271" s="35"/>
-      <c r="X271" s="35"/>
-      <c r="Y271" s="35"/>
-      <c r="Z271" s="35"/>
-    </row>
-    <row r="272" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A272" s="6" t="s">
-        <v>785</v>
-      </c>
+    <row r="271" spans="1:21" ht="14.25" customHeight="1">
+      <c r="A271" s="6"/>
+      <c r="B271" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="C271" s="7" t="s">
+        <v>775</v>
+      </c>
+      <c r="D271" s="8"/>
+      <c r="E271" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="F271" s="10"/>
+      <c r="G271" s="8" t="s">
+        <v>776</v>
+      </c>
+      <c r="H271" s="14" t="s">
+        <v>777</v>
+      </c>
+      <c r="I271" s="27"/>
+      <c r="J271" s="3"/>
+      <c r="K271" s="7"/>
+      <c r="L271" s="7"/>
+      <c r="M271" s="7"/>
+      <c r="N271" s="7"/>
+      <c r="O271" s="7"/>
+      <c r="P271" s="7"/>
+      <c r="Q271" s="7"/>
+      <c r="R271" s="7"/>
+      <c r="S271" s="7"/>
+      <c r="T271" s="7"/>
+      <c r="U271" s="7"/>
+    </row>
+    <row r="272" spans="1:21" ht="14.25" customHeight="1">
+      <c r="A272" s="6"/>
       <c r="B272" s="6" t="s">
-        <v>22</v>
+        <v>158</v>
       </c>
       <c r="C272" s="7" t="s">
-        <v>227</v>
+        <v>778</v>
       </c>
       <c r="D272" s="8"/>
       <c r="E272" s="8" t="s">
-        <v>195</v>
+        <v>156</v>
       </c>
       <c r="F272" s="10"/>
       <c r="G272" s="8" t="s">
-        <v>29</v>
+        <v>776</v>
       </c>
       <c r="H272" s="14" t="s">
-        <v>786</v>
-      </c>
-      <c r="I272" s="8"/>
+        <v>779</v>
+      </c>
+      <c r="I272" s="27"/>
       <c r="J272" s="3"/>
-      <c r="K272" s="3" t="s">
-        <v>188</v>
-      </c>
+      <c r="K272" s="7"/>
       <c r="L272" s="7"/>
       <c r="M272" s="7"/>
       <c r="N272" s="7"/>
@@ -18690,15 +18698,25 @@
       <c r="T272" s="7"/>
       <c r="U272" s="7"/>
     </row>
-    <row r="273" spans="1:21" ht="14.25" customHeight="1">
+    <row r="273" spans="1:26" ht="14.25" customHeight="1">
       <c r="A273" s="6"/>
-      <c r="B273" s="6"/>
-      <c r="C273" s="7"/>
+      <c r="B273" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C273" s="7" t="s">
+        <v>780</v>
+      </c>
       <c r="D273" s="8"/>
-      <c r="E273" s="8"/>
+      <c r="E273" s="8" t="s">
+        <v>156</v>
+      </c>
       <c r="F273" s="10"/>
-      <c r="G273" s="8"/>
-      <c r="H273" s="14"/>
+      <c r="G273" s="8" t="s">
+        <v>776</v>
+      </c>
+      <c r="H273" s="14" t="s">
+        <v>781</v>
+      </c>
       <c r="I273" s="27"/>
       <c r="J273" s="3"/>
       <c r="K273" s="7"/>
@@ -18713,41 +18731,74 @@
       <c r="T273" s="7"/>
       <c r="U273" s="7"/>
     </row>
-    <row r="274" spans="1:21" ht="14.25" customHeight="1">
-      <c r="A274" s="6"/>
-      <c r="B274" s="6"/>
-      <c r="C274" s="7"/>
-      <c r="D274" s="8"/>
-      <c r="E274" s="8"/>
-      <c r="F274" s="10"/>
-      <c r="G274" s="8"/>
-      <c r="H274" s="14"/>
-      <c r="I274" s="8"/>
-      <c r="J274" s="7"/>
-      <c r="K274" s="7"/>
-      <c r="L274" s="7"/>
-      <c r="M274" s="7"/>
-      <c r="N274" s="7"/>
-      <c r="O274" s="7"/>
-      <c r="P274" s="7"/>
-      <c r="Q274" s="7"/>
-      <c r="R274" s="7"/>
-      <c r="S274" s="7"/>
-      <c r="T274" s="7"/>
-      <c r="U274" s="7"/>
-    </row>
-    <row r="275" spans="1:21" ht="14.25" customHeight="1">
-      <c r="A275" s="6"/>
-      <c r="B275" s="6"/>
-      <c r="C275" s="7"/>
+    <row r="274" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A274" s="36" t="s">
+        <v>216</v>
+      </c>
+      <c r="B274" s="29"/>
+      <c r="C274" s="37" t="s">
+        <v>782</v>
+      </c>
+      <c r="D274" s="38" t="s">
+        <v>28</v>
+      </c>
+      <c r="E274" s="38" t="s">
+        <v>783</v>
+      </c>
+      <c r="F274" s="38" t="s">
+        <v>25</v>
+      </c>
+      <c r="G274" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="H274" s="39" t="s">
+        <v>784</v>
+      </c>
+      <c r="I274" s="31"/>
+      <c r="J274" s="34"/>
+      <c r="K274" s="34"/>
+      <c r="L274" s="30"/>
+      <c r="M274" s="30"/>
+      <c r="N274" s="30"/>
+      <c r="O274" s="30"/>
+      <c r="P274" s="30"/>
+      <c r="Q274" s="30"/>
+      <c r="R274" s="30"/>
+      <c r="S274" s="30"/>
+      <c r="T274" s="30"/>
+      <c r="U274" s="30"/>
+      <c r="V274" s="35"/>
+      <c r="W274" s="35"/>
+      <c r="X274" s="35"/>
+      <c r="Y274" s="35"/>
+      <c r="Z274" s="35"/>
+    </row>
+    <row r="275" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A275" s="6" t="s">
+        <v>785</v>
+      </c>
+      <c r="B275" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C275" s="7" t="s">
+        <v>227</v>
+      </c>
       <c r="D275" s="8"/>
-      <c r="E275" s="8"/>
+      <c r="E275" s="8" t="s">
+        <v>195</v>
+      </c>
       <c r="F275" s="10"/>
-      <c r="G275" s="8"/>
-      <c r="H275" s="14"/>
+      <c r="G275" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H275" s="14" t="s">
+        <v>786</v>
+      </c>
       <c r="I275" s="8"/>
-      <c r="J275" s="7"/>
-      <c r="K275" s="7"/>
+      <c r="J275" s="3"/>
+      <c r="K275" s="3" t="s">
+        <v>188</v>
+      </c>
       <c r="L275" s="7"/>
       <c r="M275" s="7"/>
       <c r="N275" s="7"/>
@@ -18759,7 +18810,7 @@
       <c r="T275" s="7"/>
       <c r="U275" s="7"/>
     </row>
-    <row r="276" spans="1:21" ht="14.25" customHeight="1">
+    <row r="276" spans="1:26" ht="14.25" customHeight="1">
       <c r="A276" s="6"/>
       <c r="B276" s="6"/>
       <c r="C276" s="7"/>
@@ -18768,8 +18819,8 @@
       <c r="F276" s="10"/>
       <c r="G276" s="8"/>
       <c r="H276" s="14"/>
-      <c r="I276" s="8"/>
-      <c r="J276" s="7"/>
+      <c r="I276" s="27"/>
+      <c r="J276" s="3"/>
       <c r="K276" s="7"/>
       <c r="L276" s="7"/>
       <c r="M276" s="7"/>
@@ -18782,7 +18833,7 @@
       <c r="T276" s="7"/>
       <c r="U276" s="7"/>
     </row>
-    <row r="277" spans="1:21" ht="14.25" customHeight="1">
+    <row r="277" spans="1:26" ht="14.25" customHeight="1">
       <c r="A277" s="6"/>
       <c r="B277" s="6"/>
       <c r="C277" s="7"/>
@@ -18805,7 +18856,7 @@
       <c r="T277" s="7"/>
       <c r="U277" s="7"/>
     </row>
-    <row r="278" spans="1:21" ht="14.25" customHeight="1">
+    <row r="278" spans="1:26" ht="14.25" customHeight="1">
       <c r="A278" s="6"/>
       <c r="B278" s="6"/>
       <c r="C278" s="7"/>
@@ -18828,7 +18879,7 @@
       <c r="T278" s="7"/>
       <c r="U278" s="7"/>
     </row>
-    <row r="279" spans="1:21" ht="14.25" customHeight="1">
+    <row r="279" spans="1:26" ht="14.25" customHeight="1">
       <c r="A279" s="6"/>
       <c r="B279" s="6"/>
       <c r="C279" s="7"/>
@@ -18851,7 +18902,7 @@
       <c r="T279" s="7"/>
       <c r="U279" s="7"/>
     </row>
-    <row r="280" spans="1:21" ht="14.25" customHeight="1">
+    <row r="280" spans="1:26" ht="14.25" customHeight="1">
       <c r="A280" s="6"/>
       <c r="B280" s="6"/>
       <c r="C280" s="7"/>
@@ -18874,7 +18925,7 @@
       <c r="T280" s="7"/>
       <c r="U280" s="7"/>
     </row>
-    <row r="281" spans="1:21" ht="14.25" customHeight="1">
+    <row r="281" spans="1:26" ht="14.25" customHeight="1">
       <c r="A281" s="6"/>
       <c r="B281" s="6"/>
       <c r="C281" s="7"/>
@@ -18897,7 +18948,7 @@
       <c r="T281" s="7"/>
       <c r="U281" s="7"/>
     </row>
-    <row r="282" spans="1:21" ht="14.25" customHeight="1">
+    <row r="282" spans="1:26" ht="14.25" customHeight="1">
       <c r="A282" s="6"/>
       <c r="B282" s="6"/>
       <c r="C282" s="7"/>
@@ -18920,7 +18971,7 @@
       <c r="T282" s="7"/>
       <c r="U282" s="7"/>
     </row>
-    <row r="283" spans="1:21" ht="14.25" customHeight="1">
+    <row r="283" spans="1:26" ht="14.25" customHeight="1">
       <c r="A283" s="6"/>
       <c r="B283" s="6"/>
       <c r="C283" s="7"/>
@@ -18943,15 +18994,15 @@
       <c r="T283" s="7"/>
       <c r="U283" s="7"/>
     </row>
-    <row r="284" spans="1:21" ht="14.25" customHeight="1">
+    <row r="284" spans="1:26" ht="14.25" customHeight="1">
       <c r="A284" s="6"/>
       <c r="B284" s="6"/>
       <c r="C284" s="7"/>
       <c r="D284" s="8"/>
       <c r="E284" s="8"/>
       <c r="F284" s="10"/>
-      <c r="G284" s="9"/>
-      <c r="H284" s="7"/>
+      <c r="G284" s="8"/>
+      <c r="H284" s="14"/>
       <c r="I284" s="8"/>
       <c r="J284" s="7"/>
       <c r="K284" s="7"/>
@@ -18966,7 +19017,7 @@
       <c r="T284" s="7"/>
       <c r="U284" s="7"/>
     </row>
-    <row r="285" spans="1:21" ht="14.4">
+    <row r="285" spans="1:26" ht="14.25" customHeight="1">
       <c r="A285" s="6"/>
       <c r="B285" s="6"/>
       <c r="C285" s="7"/>
@@ -18974,7 +19025,7 @@
       <c r="E285" s="8"/>
       <c r="F285" s="10"/>
       <c r="G285" s="8"/>
-      <c r="H285" s="7"/>
+      <c r="H285" s="14"/>
       <c r="I285" s="8"/>
       <c r="J285" s="7"/>
       <c r="K285" s="7"/>
@@ -18989,14 +19040,74 @@
       <c r="T285" s="7"/>
       <c r="U285" s="7"/>
     </row>
-    <row r="286" spans="1:21" ht="14.4">
-      <c r="B286" s="7"/>
-    </row>
-    <row r="287" spans="1:21" ht="14.4">
-      <c r="B287" s="7"/>
-    </row>
-    <row r="288" spans="1:21" ht="14.4">
-      <c r="B288" s="7"/>
+    <row r="286" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A286" s="6"/>
+      <c r="B286" s="6"/>
+      <c r="C286" s="7"/>
+      <c r="D286" s="8"/>
+      <c r="E286" s="8"/>
+      <c r="F286" s="10"/>
+      <c r="G286" s="8"/>
+      <c r="H286" s="14"/>
+      <c r="I286" s="8"/>
+      <c r="J286" s="7"/>
+      <c r="K286" s="7"/>
+      <c r="L286" s="7"/>
+      <c r="M286" s="7"/>
+      <c r="N286" s="7"/>
+      <c r="O286" s="7"/>
+      <c r="P286" s="7"/>
+      <c r="Q286" s="7"/>
+      <c r="R286" s="7"/>
+      <c r="S286" s="7"/>
+      <c r="T286" s="7"/>
+      <c r="U286" s="7"/>
+    </row>
+    <row r="287" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A287" s="6"/>
+      <c r="B287" s="6"/>
+      <c r="C287" s="7"/>
+      <c r="D287" s="8"/>
+      <c r="E287" s="8"/>
+      <c r="F287" s="10"/>
+      <c r="G287" s="9"/>
+      <c r="H287" s="7"/>
+      <c r="I287" s="8"/>
+      <c r="J287" s="7"/>
+      <c r="K287" s="7"/>
+      <c r="L287" s="7"/>
+      <c r="M287" s="7"/>
+      <c r="N287" s="7"/>
+      <c r="O287" s="7"/>
+      <c r="P287" s="7"/>
+      <c r="Q287" s="7"/>
+      <c r="R287" s="7"/>
+      <c r="S287" s="7"/>
+      <c r="T287" s="7"/>
+      <c r="U287" s="7"/>
+    </row>
+    <row r="288" spans="1:26" ht="14.4">
+      <c r="A288" s="6"/>
+      <c r="B288" s="6"/>
+      <c r="C288" s="7"/>
+      <c r="D288" s="8"/>
+      <c r="E288" s="8"/>
+      <c r="F288" s="10"/>
+      <c r="G288" s="8"/>
+      <c r="H288" s="7"/>
+      <c r="I288" s="8"/>
+      <c r="J288" s="7"/>
+      <c r="K288" s="7"/>
+      <c r="L288" s="7"/>
+      <c r="M288" s="7"/>
+      <c r="N288" s="7"/>
+      <c r="O288" s="7"/>
+      <c r="P288" s="7"/>
+      <c r="Q288" s="7"/>
+      <c r="R288" s="7"/>
+      <c r="S288" s="7"/>
+      <c r="T288" s="7"/>
+      <c r="U288" s="7"/>
     </row>
     <row r="289" spans="2:2" ht="14.4">
       <c r="B289" s="7"/>
@@ -21301,6 +21412,15 @@
     </row>
     <row r="1056" spans="2:2" ht="14.4">
       <c r="B1056" s="7"/>
+    </row>
+    <row r="1057" spans="2:2" ht="14.4">
+      <c r="B1057" s="7"/>
+    </row>
+    <row r="1058" spans="2:2" ht="14.4">
+      <c r="B1058" s="7"/>
+    </row>
+    <row r="1059" spans="2:2" ht="14.4">
+      <c r="B1059" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Stand up the PEST_WileyCreek55 simulation.
</commit_message>
<xml_diff>
--- a/DataCW3M/CW3MdigitalHandbook/CW3MdataDictionary.xlsx
+++ b/DataCW3M/CW3MdigitalHandbook/CW3MdataDictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\CW3MdigitalHandbook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6BF6417-76C8-41AD-9D57-AD6372C81208}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17D17E66-F37A-4938-B821-9B76CF59E93B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35265" yWindow="-3105" windowWidth="21120" windowHeight="9585" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Necessary input data" sheetId="7" r:id="rId1"/>
@@ -9324,7 +9324,7 @@
   </sheetPr>
   <dimension ref="A1:Z1060"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="3" topLeftCell="A226" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="H238" sqref="H238"/>
     </sheetView>
@@ -21480,8 +21480,8 @@
   </sheetPr>
   <dimension ref="A1:Z117"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A57" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Release CW3M_Installer_McKenzie_1.2.0.exe at Box CW3M/ReleasedPackages. At 214 MB, the file is too big to put on GitHub. prescribedLULCS.csv - Change a description. CW3M_McKenzie_Script.iss - Change the version from 1.1.0 to 1.2.0.
</commit_message>
<xml_diff>
--- a/DataCW3M/CW3MdigitalHandbook/CW3MdataDictionary.xlsx
+++ b/DataCW3M/CW3MdigitalHandbook/CW3MdataDictionary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\CW3MdigitalHandbook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17D17E66-F37A-4938-B821-9B76CF59E93B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1849FD59-3F06-4F5A-BDAF-27E33557869A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Necessary input data" sheetId="7" r:id="rId1"/>
@@ -97,7 +97,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3174" uniqueCount="1072">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3175" uniqueCount="1072">
   <si>
     <t>LULC_A</t>
   </si>
@@ -9324,9 +9324,9 @@
   </sheetPr>
   <dimension ref="A1:Z1060"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A226" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H238" sqref="H238"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A236" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F49" sqref="F49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -21480,7 +21480,7 @@
   </sheetPr>
   <dimension ref="A1:Z117"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="4" topLeftCell="A57" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="K7" sqref="K7"/>
     </sheetView>
@@ -24429,7 +24429,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I18" sqref="I18"/>
+      <selection pane="bottomLeft" activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -25192,9 +25192,11 @@
       <c r="E22" s="47" t="s">
         <v>366</v>
       </c>
-      <c r="F22" s="47"/>
+      <c r="F22" s="47" t="s">
+        <v>28</v>
+      </c>
       <c r="G22" s="47" t="s">
-        <v>28</v>
+        <v>171</v>
       </c>
       <c r="H22" s="47" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
Add reports for wetland 15.
</commit_message>
<xml_diff>
--- a/DataCW3M/CW3MdigitalHandbook/CW3MdataDictionary.xlsx
+++ b/DataCW3M/CW3MdigitalHandbook/CW3MdataDictionary.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\CW3MdigitalHandbook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1849FD59-3F06-4F5A-BDAF-27E33557869A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71BEEE47-0B11-41FA-92F1-97303E3E14D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -9325,8 +9325,8 @@
   <dimension ref="A1:Z1060"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A236" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F49" sqref="F49"/>
+      <pane ySplit="3" topLeftCell="A234" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -21480,8 +21480,8 @@
   </sheetPr>
   <dimension ref="A1:Z117"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A57" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A93" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add logic to Spring::Step() to use a water temperature based on the air temperature for springs for which the water temperature is not specified. Add reach attributes FLOOD_C and FLOOD_CMS. CW3MdataDictionary.xlsx - Add reach attributes FLOOD_C and FLOOD_CMS. FLOWreports_McKenzie.xml - Add columns for FLOOD_CMS and FLOOD_C to the "FLOW McKenzie Thermal Energy Budget for streams" report. Reach_McKenzie.dbf - Add reach attributes FLOOD_C and FLOOD_CMS. Flow.cpp, .h - Add reach attributes FLOOD_C and FLOOD_CMS. FluxExpr.cpp - Add logic to Spring::Step() to use a water temperature based on the air temperature for springs for which the water temperature is not specified. ReachRouting.cpp - Replace an assert with a warning message.
</commit_message>
<xml_diff>
--- a/DataCW3M/CW3MdigitalHandbook/CW3MdataDictionary.xlsx
+++ b/DataCW3M/CW3MdigitalHandbook/CW3MdataDictionary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\CW3MdigitalHandbook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE8C2DFF-6025-4ACE-9404-5F28C48D2E85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBB6889E-2C4E-40FD-8001-D44861D291CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-7425" windowWidth="29040" windowHeight="17520" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -97,7 +97,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3181" uniqueCount="1074">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3193" uniqueCount="1078">
   <si>
     <t>LULC_A</t>
   </si>
@@ -2656,9 +2656,6 @@
     <t>IN_RUNOFF</t>
   </si>
   <si>
-    <t>addition to reach as lateral flow in over and through the stream banks and stream bottom, from the precipitation-runoff model (HBV)</t>
-  </si>
-  <si>
     <t>Q_MIN</t>
   </si>
   <si>
@@ -3319,7 +3316,22 @@
     <t>withdrawals from reach as lateral flow; nets with IN_RUNOFF</t>
   </si>
   <si>
-    <t>2/2/21 - Added WIDTHGIVEN, RADSWGIVEN. 2/23/22 Added OUT_LATERL.</t>
+    <t>FLOOD_CMS</t>
+  </si>
+  <si>
+    <t>flow in Q2WETL returned immediately to the reach because the wetland itself is overflowing</t>
+  </si>
+  <si>
+    <t>FLOOD_C</t>
+  </si>
+  <si>
+    <t>temperature of FLOOD_CMS</t>
+  </si>
+  <si>
+    <t>2/2/21 - Added WIDTHGIVEN, RADSWGIVEN. 2/23/22 Added OUT_LATERL. 2/25 - Add FLOOD_C, FLOOD_CMS.</t>
+  </si>
+  <si>
+    <t>lateral flow into the reach over and through the stream banks and stream bottom, from the precipitation-runoff model (HBV), excluding water from springs and floodwater</t>
   </si>
 </sst>
 </file>
@@ -9331,7 +9343,7 @@
   <dimension ref="A1:Z1060"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A128" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="3" topLeftCell="A164" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A240" sqref="A240"/>
     </sheetView>
   </sheetViews>
@@ -11063,7 +11075,7 @@
       <c r="A50" s="28"/>
       <c r="B50" s="28"/>
       <c r="C50" s="7" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="D50" s="10" t="s">
         <v>107</v>
@@ -11076,10 +11088,10 @@
         <v>29</v>
       </c>
       <c r="H50" s="25" t="s">
+        <v>1020</v>
+      </c>
+      <c r="I50" s="27" t="s">
         <v>1021</v>
-      </c>
-      <c r="I50" s="27" t="s">
-        <v>1022</v>
       </c>
       <c r="J50" s="3"/>
       <c r="K50" s="7"/>
@@ -11597,20 +11609,20 @@
       <c r="A67" s="28"/>
       <c r="B67" s="28"/>
       <c r="C67" s="7" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="D67" s="10" t="s">
         <v>107</v>
       </c>
       <c r="E67" s="10" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="F67" s="10"/>
       <c r="G67" s="10" t="s">
         <v>26</v>
       </c>
       <c r="H67" s="25" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="I67" s="27"/>
       <c r="J67" s="3"/>
@@ -11671,7 +11683,7 @@
       </c>
       <c r="B69" s="28"/>
       <c r="C69" s="7" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
       <c r="D69" s="10" t="s">
         <v>107</v>
@@ -11682,7 +11694,7 @@
         <v>26</v>
       </c>
       <c r="H69" s="25" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="I69" s="27" t="s">
         <v>112</v>
@@ -11706,7 +11718,7 @@
       </c>
       <c r="B70" s="28"/>
       <c r="C70" s="7" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="D70" s="10" t="s">
         <v>107</v>
@@ -11717,7 +11729,7 @@
         <v>26</v>
       </c>
       <c r="H70" s="25" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
       <c r="I70" s="27" t="s">
         <v>112</v>
@@ -11896,7 +11908,7 @@
         <v>225</v>
       </c>
       <c r="F75" s="62" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
       <c r="G75" s="62" t="s">
         <v>26</v>
@@ -12772,11 +12784,11 @@
     </row>
     <row r="100" spans="1:26" s="21" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A100" s="28" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="B100" s="28"/>
       <c r="C100" s="7" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="D100" s="10" t="s">
         <v>28</v>
@@ -12787,7 +12799,7 @@
         <v>26</v>
       </c>
       <c r="H100" s="25" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
       <c r="I100" s="10" t="s">
         <v>112</v>
@@ -12996,16 +13008,16 @@
         <v>28</v>
       </c>
       <c r="E106" s="8" t="s">
+        <v>1032</v>
+      </c>
+      <c r="F106" s="10" t="s">
         <v>1033</v>
-      </c>
-      <c r="F106" s="10" t="s">
-        <v>1034</v>
       </c>
       <c r="G106" s="8" t="s">
         <v>26</v>
       </c>
       <c r="H106" s="57" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="I106" s="27"/>
       <c r="J106" s="3"/>
@@ -13714,18 +13726,18 @@
       <c r="A127" s="28"/>
       <c r="B127" s="28"/>
       <c r="C127" s="7" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="D127" s="10"/>
       <c r="E127" s="10" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="F127" s="10" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="G127" s="10"/>
       <c r="H127" s="25" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="I127" s="27" t="s">
         <v>112</v>
@@ -13747,18 +13759,18 @@
       <c r="A128" s="28"/>
       <c r="B128" s="28"/>
       <c r="C128" s="7" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="D128" s="10"/>
       <c r="E128" s="10" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="F128" s="10" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="G128" s="10"/>
       <c r="H128" s="25" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="I128" s="27" t="s">
         <v>112</v>
@@ -13780,18 +13792,18 @@
       <c r="A129" s="28"/>
       <c r="B129" s="28"/>
       <c r="C129" s="7" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="D129" s="10"/>
       <c r="E129" s="10" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="F129" s="10" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="G129" s="10"/>
       <c r="H129" s="25" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="I129" s="27" t="s">
         <v>112</v>
@@ -13813,18 +13825,18 @@
       <c r="A130" s="28"/>
       <c r="B130" s="28"/>
       <c r="C130" s="7" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="D130" s="10"/>
       <c r="E130" s="10" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="F130" s="10" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="G130" s="10"/>
       <c r="H130" s="25" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="I130" s="27" t="s">
         <v>112</v>
@@ -13884,22 +13896,22 @@
     <row r="132" spans="1:26" s="21" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B132" s="28"/>
       <c r="C132" s="21" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="D132" s="10" t="s">
         <v>28</v>
       </c>
       <c r="E132" s="10" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="F132" s="10" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="G132" s="10" t="s">
         <v>26</v>
       </c>
       <c r="H132" s="21" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="I132" s="27" t="s">
         <v>112</v>
@@ -13909,22 +13921,22 @@
     <row r="133" spans="1:26" s="21" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B133" s="28"/>
       <c r="C133" s="21" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="D133" s="10" t="s">
         <v>28</v>
       </c>
       <c r="E133" s="10" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="F133" s="10" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="G133" s="10" t="s">
         <v>26</v>
       </c>
       <c r="H133" s="21" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="I133" s="27" t="s">
         <v>112</v>
@@ -13934,22 +13946,22 @@
     <row r="134" spans="1:26" s="21" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B134" s="28"/>
       <c r="C134" s="21" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="D134" s="10" t="s">
         <v>28</v>
       </c>
       <c r="E134" s="10" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="F134" s="10" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="G134" s="10" t="s">
         <v>26</v>
       </c>
       <c r="H134" s="21" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="I134" s="27" t="s">
         <v>112</v>
@@ -13959,22 +13971,22 @@
     <row r="135" spans="1:26" s="21" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B135" s="28"/>
       <c r="C135" s="21" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="D135" s="10" t="s">
         <v>28</v>
       </c>
       <c r="E135" s="10" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="F135" s="10" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="G135" s="10" t="s">
         <v>26</v>
       </c>
       <c r="H135" s="21" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="I135" s="27" t="s">
         <v>112</v>
@@ -13985,18 +13997,18 @@
       <c r="A136" s="10"/>
       <c r="B136" s="28"/>
       <c r="C136" s="21" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="D136" s="10"/>
       <c r="E136" s="10" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="F136" s="10" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="G136" s="10"/>
       <c r="H136" s="21" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="I136" s="27" t="s">
         <v>112</v>
@@ -14007,18 +14019,18 @@
       <c r="A137" s="10"/>
       <c r="B137" s="28"/>
       <c r="C137" s="21" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="D137" s="10"/>
       <c r="E137" s="10" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="F137" s="10" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="G137" s="10"/>
       <c r="H137" s="21" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="I137" s="27" t="s">
         <v>112</v>
@@ -14103,7 +14115,7 @@
       </c>
       <c r="D140" s="8"/>
       <c r="E140" s="10" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="F140" s="10"/>
       <c r="G140" s="8" t="s">
@@ -14173,7 +14185,7 @@
       </c>
       <c r="D142" s="8"/>
       <c r="E142" s="10" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="F142" s="10"/>
       <c r="G142" s="8" t="s">
@@ -15412,7 +15424,7 @@
         <v>26</v>
       </c>
       <c r="H175" s="60" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
       <c r="I175" s="67" t="s">
         <v>811</v>
@@ -15423,7 +15435,7 @@
       <c r="A176" s="13"/>
       <c r="B176" s="13"/>
       <c r="C176" s="25" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="D176" s="9" t="s">
         <v>107</v>
@@ -15438,7 +15450,7 @@
         <v>26</v>
       </c>
       <c r="H176" s="72" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="I176" s="46" t="s">
         <v>811</v>
@@ -15646,7 +15658,7 @@
         <v>28</v>
       </c>
       <c r="E182" s="27" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="F182" s="27" t="s">
         <v>33</v>
@@ -15741,7 +15753,7 @@
     </row>
     <row r="185" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A185" s="13" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="B185" s="6"/>
       <c r="C185" s="18" t="s">
@@ -15761,7 +15773,7 @@
         <v>637</v>
       </c>
       <c r="I185" s="10" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="J185" s="3"/>
       <c r="K185" s="7"/>
@@ -16259,7 +16271,7 @@
       <c r="A201" s="28"/>
       <c r="B201" s="28"/>
       <c r="C201" s="7" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="D201" s="70" t="s">
         <v>107</v>
@@ -16272,7 +16284,7 @@
         <v>26</v>
       </c>
       <c r="H201" s="57" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
       <c r="I201" s="10"/>
       <c r="J201" s="3"/>
@@ -16391,7 +16403,7 @@
       <c r="A205" s="28"/>
       <c r="B205" s="28"/>
       <c r="C205" s="21" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="D205" s="10" t="s">
         <v>28</v>
@@ -16400,11 +16412,11 @@
         <v>127</v>
       </c>
       <c r="F205" s="10" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="G205" s="10"/>
       <c r="H205" s="25" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="I205" s="27"/>
       <c r="J205" s="3"/>
@@ -16422,7 +16434,7 @@
     <row r="206" spans="1:21" s="21" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B206" s="28"/>
       <c r="C206" s="21" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="D206" s="10" t="s">
         <v>28</v>
@@ -16431,13 +16443,13 @@
         <v>127</v>
       </c>
       <c r="F206" s="10" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="G206" s="10" t="s">
         <v>26</v>
       </c>
       <c r="H206" s="25" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="I206" s="27" t="s">
         <v>112</v>
@@ -16958,11 +16970,11 @@
     </row>
     <row r="222" spans="1:21" s="21" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A222" s="28" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="B222" s="28"/>
       <c r="C222" s="7" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="D222" s="10" t="s">
         <v>28</v>
@@ -16973,7 +16985,7 @@
         <v>26</v>
       </c>
       <c r="H222" s="25" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
       <c r="I222" s="27" t="s">
         <v>112</v>
@@ -17271,20 +17283,20 @@
       <c r="A231" s="28"/>
       <c r="B231" s="28"/>
       <c r="C231" s="7" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
       <c r="D231" s="10" t="s">
         <v>107</v>
       </c>
       <c r="E231" s="10" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="F231" s="10"/>
       <c r="G231" s="10" t="s">
         <v>26</v>
       </c>
       <c r="H231" s="57" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
       <c r="I231" s="27"/>
       <c r="J231" s="3"/>
@@ -17304,20 +17316,20 @@
       <c r="A232" s="28"/>
       <c r="B232" s="28"/>
       <c r="C232" s="7" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="D232" s="10" t="s">
         <v>107</v>
       </c>
       <c r="E232" s="10" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="F232" s="10"/>
       <c r="G232" s="10" t="s">
         <v>26</v>
       </c>
       <c r="H232" s="57" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
       <c r="I232" s="27"/>
       <c r="J232" s="3"/>
@@ -17372,7 +17384,7 @@
       <c r="A234" s="28"/>
       <c r="B234" s="28"/>
       <c r="C234" s="7" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="D234" s="10" t="s">
         <v>45</v>
@@ -17383,7 +17395,7 @@
         <v>29</v>
       </c>
       <c r="H234" s="25" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="I234" s="27"/>
       <c r="J234" s="3"/>
@@ -17440,7 +17452,7 @@
       <c r="A236" s="96"/>
       <c r="B236" s="96"/>
       <c r="C236" s="97" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
       <c r="D236" s="100" t="s">
         <v>107</v>
@@ -17453,7 +17465,7 @@
         <v>26</v>
       </c>
       <c r="H236" s="91" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="I236" s="98"/>
       <c r="J236" s="84"/>
@@ -17473,22 +17485,22 @@
       <c r="A237" s="96"/>
       <c r="B237" s="96"/>
       <c r="C237" s="97" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
       <c r="D237" s="99" t="s">
         <v>45</v>
       </c>
       <c r="E237" s="99" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
       <c r="F237" s="100" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
       <c r="G237" s="99" t="s">
         <v>26</v>
       </c>
       <c r="H237" s="99" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
       <c r="I237" s="98"/>
       <c r="J237" s="84"/>
@@ -17508,20 +17520,20 @@
       <c r="A238" s="96"/>
       <c r="B238" s="96"/>
       <c r="C238" s="97" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="D238" s="100" t="s">
         <v>107</v>
       </c>
       <c r="E238" s="100" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
       <c r="F238" s="100"/>
       <c r="G238" s="100" t="s">
         <v>26</v>
       </c>
       <c r="H238" s="57" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="I238" s="98"/>
       <c r="J238" s="84"/>
@@ -17541,7 +17553,7 @@
       <c r="A239" s="96"/>
       <c r="B239" s="96"/>
       <c r="C239" s="97" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="D239" s="99" t="s">
         <v>107</v>
@@ -17556,7 +17568,7 @@
         <v>26</v>
       </c>
       <c r="H239" s="77" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="I239" s="98"/>
       <c r="J239" s="84"/>
@@ -21484,11 +21496,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Z118"/>
+  <dimension ref="A1:Z120"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="K37" sqref="K37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -21535,7 +21547,7 @@
     </row>
     <row r="2" spans="1:26" s="57" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="70" t="s">
-        <v>1073</v>
+        <v>1076</v>
       </c>
       <c r="B2" s="69"/>
       <c r="C2" s="69"/>
@@ -21563,7 +21575,7 @@
     </row>
     <row r="3" spans="1:26" s="91" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="87" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="B3" s="88"/>
       <c r="C3" s="89"/>
@@ -21651,7 +21663,7 @@
       <c r="C5" s="13"/>
       <c r="D5" s="13"/>
       <c r="E5" s="72" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="F5" s="10"/>
       <c r="G5" s="70" t="s">
@@ -21667,7 +21679,7 @@
         <v>26</v>
       </c>
       <c r="K5" s="57" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="L5" s="9"/>
       <c r="M5" s="25"/>
@@ -21689,7 +21701,7 @@
       <c r="C6" s="13"/>
       <c r="D6" s="13"/>
       <c r="E6" s="72" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="F6" s="10"/>
       <c r="G6" s="70" t="s">
@@ -21705,7 +21717,7 @@
         <v>26</v>
       </c>
       <c r="K6" s="57" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="L6" s="9"/>
       <c r="M6" s="25"/>
@@ -21727,7 +21739,7 @@
       <c r="C7" s="13"/>
       <c r="D7" s="13"/>
       <c r="E7" s="72" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="F7" s="10"/>
       <c r="G7" s="70" t="s">
@@ -21743,7 +21755,7 @@
         <v>26</v>
       </c>
       <c r="K7" s="70" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="L7" s="9"/>
       <c r="M7" s="25"/>
@@ -21763,7 +21775,7 @@
       <c r="A8" s="82"/>
       <c r="B8" s="82"/>
       <c r="D8" s="84" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="E8" s="84" t="s">
         <v>844</v>
@@ -21790,19 +21802,19 @@
       <c r="B9" s="20"/>
       <c r="C9" s="22"/>
       <c r="E9" s="21" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="G9" s="21" t="s">
         <v>45</v>
       </c>
       <c r="H9" s="21" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="J9" s="23" t="s">
         <v>29</v>
       </c>
       <c r="K9" s="80" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="L9" s="22"/>
     </row>
@@ -21811,19 +21823,19 @@
       <c r="B10" s="20"/>
       <c r="C10" s="22"/>
       <c r="E10" s="21" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="G10" s="21" t="s">
         <v>45</v>
       </c>
       <c r="H10" s="21" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="J10" s="23" t="s">
         <v>29</v>
       </c>
       <c r="K10" s="80" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="L10" s="22"/>
     </row>
@@ -21832,10 +21844,10 @@
       <c r="B11" s="92"/>
       <c r="C11" s="93"/>
       <c r="D11" s="76" t="s">
+        <v>936</v>
+      </c>
+      <c r="E11" s="76" t="s">
         <v>937</v>
-      </c>
-      <c r="E11" s="76" t="s">
-        <v>938</v>
       </c>
       <c r="F11" s="65">
         <v>36</v>
@@ -21847,16 +21859,16 @@
         <v>225</v>
       </c>
       <c r="I11" s="76" t="s">
+        <v>939</v>
+      </c>
+      <c r="J11" s="94" t="s">
+        <v>938</v>
+      </c>
+      <c r="K11" s="95" t="s">
         <v>940</v>
       </c>
-      <c r="J11" s="94" t="s">
-        <v>939</v>
-      </c>
-      <c r="K11" s="95" t="s">
+      <c r="L11" s="94" t="s">
         <v>941</v>
-      </c>
-      <c r="L11" s="94" t="s">
-        <v>942</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
@@ -22041,7 +22053,7 @@
       <c r="B21" s="20"/>
       <c r="D21" s="3"/>
       <c r="E21" s="7" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="F21" s="7"/>
       <c r="G21" s="7" t="s">
@@ -22057,7 +22069,7 @@
         <v>26</v>
       </c>
       <c r="K21" s="21" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
     </row>
     <row r="22" spans="1:26" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
@@ -22065,7 +22077,7 @@
       <c r="B22" s="20"/>
       <c r="D22" s="3"/>
       <c r="E22" s="7" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="F22" s="7">
         <v>90</v>
@@ -22074,13 +22086,13 @@
         <v>107</v>
       </c>
       <c r="H22" s="7" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="J22" s="21" t="s">
         <v>29</v>
       </c>
       <c r="K22" s="21" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
     </row>
     <row r="23" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
@@ -22176,7 +22188,7 @@
         <v>23</v>
       </c>
       <c r="D26" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="E26" s="7" t="s">
         <v>49</v>
@@ -22185,227 +22197,225 @@
         <v>0</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="H26" s="7"/>
       <c r="K26" s="23" t="s">
-        <v>901</v>
-      </c>
-    </row>
-    <row r="27" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A27" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="B27" s="15"/>
+        <v>900</v>
+      </c>
+    </row>
+    <row r="27" spans="1:26" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A27" s="20"/>
+      <c r="B27" s="20"/>
       <c r="E27" s="7" t="s">
+        <v>1074</v>
+      </c>
+      <c r="F27" s="7"/>
+      <c r="G27" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="H27" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="I27" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="J27" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="K27" s="23" t="s">
+        <v>1075</v>
+      </c>
+    </row>
+    <row r="28" spans="1:26" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A28" s="20"/>
+      <c r="B28" s="20"/>
+      <c r="E28" s="7" t="s">
+        <v>1072</v>
+      </c>
+      <c r="F28" s="7"/>
+      <c r="G28" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="H28" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="I28" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="J28" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="K28" s="23" t="s">
+        <v>1073</v>
+      </c>
+    </row>
+    <row r="29" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A29" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B29" s="15"/>
+      <c r="E29" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="F27" s="7">
+      <c r="F29" s="7">
         <v>6713</v>
       </c>
-      <c r="G27" s="7"/>
-      <c r="H27" s="7"/>
-    </row>
-    <row r="28" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A28" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="B28" s="15"/>
-      <c r="E28" s="58" t="s">
+      <c r="G29" s="7"/>
+      <c r="H29" s="7"/>
+    </row>
+    <row r="30" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A30" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B30" s="15"/>
+      <c r="E30" s="58" t="s">
         <v>52</v>
       </c>
-      <c r="F28" s="7" t="s">
+      <c r="F30" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="G28" s="7"/>
-      <c r="H28" s="7"/>
-    </row>
-    <row r="29" spans="1:26" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="B29" s="15" t="s">
+      <c r="G30" s="7"/>
+      <c r="H30" s="7"/>
+    </row>
+    <row r="31" spans="1:26" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B31" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="C31" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="E29" s="7" t="s">
+      <c r="E31" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="F29" s="7">
+      <c r="F31" s="7">
         <v>34</v>
       </c>
-      <c r="G29" s="7" t="s">
+      <c r="G31" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="H29" s="7" t="s">
+      <c r="H31" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="K29" s="3" t="s">
+      <c r="K31" s="3" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="30" spans="1:26" s="25" customFormat="1" ht="72" x14ac:dyDescent="0.3">
-      <c r="A30" s="81"/>
-      <c r="B30" s="81"/>
-      <c r="C30" s="19"/>
-      <c r="D30" s="19" t="s">
+    <row r="32" spans="1:26" s="25" customFormat="1" ht="72" x14ac:dyDescent="0.3">
+      <c r="A32" s="81"/>
+      <c r="B32" s="81"/>
+      <c r="C32" s="19"/>
+      <c r="D32" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="E30" s="25" t="s">
+      <c r="E32" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="F30" s="85">
+      <c r="F32" s="85">
         <v>6737</v>
       </c>
-      <c r="G30" s="25" t="s">
+      <c r="G32" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="H30" s="86" t="s">
+      <c r="H32" s="86" t="s">
         <v>32</v>
       </c>
-      <c r="I30" s="19"/>
-      <c r="J30" s="19" t="s">
+      <c r="I32" s="19"/>
+      <c r="J32" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="K30" s="80" t="s">
+      <c r="K32" s="80" t="s">
         <v>829</v>
       </c>
-      <c r="L30" s="19"/>
-      <c r="M30" s="19"/>
-      <c r="N30" s="19"/>
-      <c r="O30" s="19"/>
-      <c r="P30" s="19"/>
-      <c r="Q30" s="19"/>
-      <c r="R30" s="19"/>
-      <c r="S30" s="19"/>
-      <c r="T30" s="19"/>
-      <c r="U30" s="19"/>
-      <c r="V30" s="19"/>
-      <c r="W30" s="19"/>
-      <c r="X30" s="19"/>
-      <c r="Y30" s="19"/>
-      <c r="Z30" s="19"/>
-    </row>
-    <row r="31" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A31" s="15"/>
-      <c r="B31" s="15"/>
-      <c r="D31" s="17" t="s">
+      <c r="L32" s="19"/>
+      <c r="M32" s="19"/>
+      <c r="N32" s="19"/>
+      <c r="O32" s="19"/>
+      <c r="P32" s="19"/>
+      <c r="Q32" s="19"/>
+      <c r="R32" s="19"/>
+      <c r="S32" s="19"/>
+      <c r="T32" s="19"/>
+      <c r="U32" s="19"/>
+      <c r="V32" s="19"/>
+      <c r="W32" s="19"/>
+      <c r="X32" s="19"/>
+      <c r="Y32" s="19"/>
+      <c r="Z32" s="19"/>
+    </row>
+    <row r="33" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A33" s="15"/>
+      <c r="B33" s="15"/>
+      <c r="D33" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="E31" s="18" t="s">
+      <c r="E33" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="F31" s="18">
+      <c r="F33" s="18">
         <v>1</v>
       </c>
-      <c r="G31" s="18" t="s">
+      <c r="G33" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="H31" s="18" t="s">
+      <c r="H33" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="J31" s="17" t="s">
+      <c r="J33" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="K31" s="17" t="s">
+      <c r="K33" s="17" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="32" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A32" s="15"/>
-      <c r="B32" s="16" t="s">
+    <row r="34" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A34" s="15"/>
+      <c r="B34" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="D32" s="17" t="s">
+      <c r="D34" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="E32" s="18" t="s">
+      <c r="E34" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="F32" s="7"/>
-      <c r="G32" s="18" t="s">
+      <c r="F34" s="7"/>
+      <c r="G34" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="H32" s="18" t="s">
+      <c r="H34" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="I32" s="17" t="s">
+      <c r="I34" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="J32" s="17" t="s">
+      <c r="J34" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="K32" s="23" t="s">
+      <c r="K34" s="23" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="33" spans="1:12" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A33" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="B33" s="20" t="s">
+    <row r="35" spans="1:12" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A35" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B35" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="D33" s="22"/>
-      <c r="E33" s="21" t="s">
-        <v>802</v>
-      </c>
-      <c r="F33" s="7"/>
-      <c r="G33" s="57" t="s">
-        <v>28</v>
-      </c>
-      <c r="H33" s="57" t="s">
-        <v>72</v>
-      </c>
-      <c r="I33" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="J33" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="K33" s="23" t="s">
-        <v>803</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A34" s="20"/>
-      <c r="B34" s="20"/>
-      <c r="D34" s="22"/>
-      <c r="E34" s="21" t="s">
-        <v>851</v>
-      </c>
-      <c r="F34" s="7"/>
-      <c r="G34" s="57" t="s">
-        <v>107</v>
-      </c>
-      <c r="H34" s="57" t="s">
-        <v>72</v>
-      </c>
-      <c r="I34" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="J34" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="K34" s="23" t="s">
-        <v>852</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A35" s="20"/>
-      <c r="B35" s="20"/>
       <c r="D35" s="22"/>
       <c r="E35" s="21" t="s">
-        <v>898</v>
+        <v>802</v>
       </c>
       <c r="F35" s="7"/>
       <c r="G35" s="57" t="s">
-        <v>107</v>
+        <v>28</v>
       </c>
       <c r="H35" s="57" t="s">
-        <v>127</v>
+        <v>72</v>
       </c>
       <c r="I35" s="23" t="s">
         <v>25</v>
@@ -22414,54 +22424,55 @@
         <v>26</v>
       </c>
       <c r="K35" s="23" t="s">
-        <v>899</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A36" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="B36" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="E36" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="F36" s="7">
-        <v>0</v>
-      </c>
-      <c r="G36" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="H36" s="7"/>
-      <c r="K36" s="3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A37" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="B37" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="E37" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="F37" s="7">
-        <v>0</v>
-      </c>
-      <c r="G37" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="H37" s="18" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A36" s="20"/>
+      <c r="B36" s="20"/>
+      <c r="D36" s="22"/>
+      <c r="E36" s="21" t="s">
+        <v>851</v>
+      </c>
+      <c r="F36" s="7"/>
+      <c r="G36" s="57" t="s">
+        <v>107</v>
+      </c>
+      <c r="H36" s="57" t="s">
         <v>72</v>
       </c>
-      <c r="K37" s="17" t="s">
-        <v>73</v>
+      <c r="I36" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="J36" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="K36" s="23" t="s">
+        <v>1077</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A37" s="20"/>
+      <c r="B37" s="20"/>
+      <c r="D37" s="22"/>
+      <c r="E37" s="21" t="s">
+        <v>897</v>
+      </c>
+      <c r="F37" s="7"/>
+      <c r="G37" s="57" t="s">
+        <v>107</v>
+      </c>
+      <c r="H37" s="57" t="s">
+        <v>127</v>
+      </c>
+      <c r="I37" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="J37" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="K37" s="23" t="s">
+        <v>898</v>
       </c>
     </row>
     <row r="38" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
@@ -22472,19 +22483,17 @@
         <v>23</v>
       </c>
       <c r="E38" s="7" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="F38" s="7">
         <v>0</v>
       </c>
-      <c r="G38" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="H38" s="18" t="s">
-        <v>75</v>
-      </c>
-      <c r="K38" s="17" t="s">
-        <v>76</v>
+      <c r="G38" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="H38" s="7"/>
+      <c r="K38" s="3" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="39" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
@@ -22494,8 +22503,11 @@
       <c r="B39" s="15" t="s">
         <v>23</v>
       </c>
+      <c r="D39" s="3" t="s">
+        <v>38</v>
+      </c>
       <c r="E39" s="7" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="F39" s="7">
         <v>0</v>
@@ -22507,7 +22519,7 @@
         <v>72</v>
       </c>
       <c r="K39" s="17" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
     <row r="40" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
@@ -22518,7 +22530,7 @@
         <v>23</v>
       </c>
       <c r="E40" s="7" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="F40" s="7">
         <v>0</v>
@@ -22527,72 +22539,70 @@
         <v>45</v>
       </c>
       <c r="H40" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="K40" s="17" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A41" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B41" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="E41" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="F41" s="7">
+        <v>0</v>
+      </c>
+      <c r="G41" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="H41" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="K41" s="17" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A42" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B42" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="E42" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="F42" s="7">
+        <v>0</v>
+      </c>
+      <c r="G42" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="H42" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="K40" s="17" t="s">
+      <c r="K42" s="17" t="s">
         <v>81</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A41" s="20"/>
-      <c r="B41" s="20"/>
-      <c r="E41" s="7" t="s">
-        <v>977</v>
-      </c>
-      <c r="F41" s="7"/>
-      <c r="G41" s="21" t="s">
-        <v>107</v>
-      </c>
-      <c r="H41" s="21" t="s">
-        <v>979</v>
-      </c>
-      <c r="I41" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="J41" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="K41" s="23" t="s">
-        <v>978</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A42" s="20"/>
-      <c r="B42" s="20"/>
-      <c r="E42" s="7" t="s">
-        <v>429</v>
-      </c>
-      <c r="F42" s="7">
-        <v>1.3</v>
-      </c>
-      <c r="G42" s="21" t="s">
-        <v>107</v>
-      </c>
-      <c r="H42" s="21" t="s">
-        <v>961</v>
-      </c>
-      <c r="I42" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="J42" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="K42" s="23" t="s">
-        <v>960</v>
       </c>
     </row>
     <row r="43" spans="1:12" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A43" s="20"/>
       <c r="B43" s="20"/>
       <c r="E43" s="7" t="s">
-        <v>964</v>
+        <v>976</v>
       </c>
       <c r="F43" s="7"/>
       <c r="G43" s="21" t="s">
         <v>107</v>
       </c>
       <c r="H43" s="21" t="s">
-        <v>961</v>
+        <v>978</v>
       </c>
       <c r="I43" s="21" t="s">
         <v>25</v>
@@ -22601,78 +22611,88 @@
         <v>26</v>
       </c>
       <c r="K43" s="23" t="s">
+        <v>977</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A44" s="20"/>
+      <c r="B44" s="20"/>
+      <c r="E44" s="7" t="s">
+        <v>429</v>
+      </c>
+      <c r="F44" s="7">
+        <v>1.3</v>
+      </c>
+      <c r="G44" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="H44" s="21" t="s">
         <v>960</v>
       </c>
-      <c r="L43" s="21" t="s">
-        <v>965</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A44" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="B44" s="15" t="s">
+      <c r="I44" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="J44" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="K44" s="23" t="s">
+        <v>959</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A45" s="20"/>
+      <c r="B45" s="20"/>
+      <c r="E45" s="7" t="s">
+        <v>963</v>
+      </c>
+      <c r="F45" s="7"/>
+      <c r="G45" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="H45" s="21" t="s">
+        <v>960</v>
+      </c>
+      <c r="I45" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="J45" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="K45" s="23" t="s">
+        <v>959</v>
+      </c>
+      <c r="L45" s="21" t="s">
+        <v>964</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A46" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B46" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="C44" s="3" t="s">
+      <c r="C46" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E44" s="7" t="s">
+      <c r="E46" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="F44" s="7">
+      <c r="F46" s="7">
         <v>1739.9274680000001</v>
       </c>
-      <c r="G44" s="7"/>
-      <c r="H44" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="I44" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="J44" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="K44" s="3" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A45" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="B45" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="D45" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="E45" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="F45" s="7">
-        <v>6699</v>
-      </c>
-      <c r="G45" s="7"/>
-      <c r="H45" s="7"/>
-    </row>
-    <row r="46" spans="1:12" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A46" s="20"/>
-      <c r="B46" s="20"/>
-      <c r="D46" s="3"/>
-      <c r="E46" s="7" t="s">
-        <v>998</v>
-      </c>
-      <c r="F46" s="7"/>
       <c r="G46" s="7"/>
       <c r="H46" s="7" t="s">
-        <v>999</v>
-      </c>
-      <c r="I46" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="K46" s="23" t="s">
-        <v>1000</v>
+        <v>83</v>
+      </c>
+      <c r="I46" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="J46" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="K46" s="3" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="47" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
@@ -22682,112 +22702,96 @@
       <c r="B47" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="D47" t="s">
+      <c r="D47" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E47" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="F47" s="7">
+        <v>6699</v>
+      </c>
+      <c r="G47" s="7"/>
+      <c r="H47" s="7"/>
+    </row>
+    <row r="48" spans="1:12" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A48" s="20"/>
+      <c r="B48" s="20"/>
+      <c r="D48" s="3"/>
+      <c r="E48" s="7" t="s">
+        <v>997</v>
+      </c>
+      <c r="F48" s="7"/>
+      <c r="G48" s="7"/>
+      <c r="H48" s="7" t="s">
+        <v>998</v>
+      </c>
+      <c r="I48" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="K48" s="23" t="s">
+        <v>999</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A49" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B49" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="D49" t="s">
+        <v>901</v>
+      </c>
+      <c r="E49" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="F49" s="7">
+        <v>0</v>
+      </c>
+      <c r="G49" s="7" t="s">
         <v>902</v>
       </c>
-      <c r="E47" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="F47" s="7">
-        <v>0</v>
-      </c>
-      <c r="G47" s="7" t="s">
+      <c r="H49" s="7"/>
+      <c r="K49" s="23" t="s">
         <v>903</v>
       </c>
-      <c r="H47" s="7"/>
-      <c r="K47" s="23" t="s">
-        <v>904</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A48" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="B48" s="15" t="s">
+    </row>
+    <row r="50" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A50" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B50" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="D48" s="3" t="s">
+      <c r="D50" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="E48" s="7" t="s">
+      <c r="E50" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="F48" s="7">
+      <c r="F50" s="7">
         <v>6758</v>
       </c>
-      <c r="G48" s="7"/>
-      <c r="H48" s="7"/>
-    </row>
-    <row r="49" spans="1:11" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A49" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="B49" s="20" t="s">
+      <c r="G50" s="7"/>
+      <c r="H50" s="7"/>
+    </row>
+    <row r="51" spans="1:11" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A51" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B51" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="D49" s="3" t="s">
+      <c r="D51" s="3" t="s">
         <v>799</v>
       </c>
-      <c r="E49" s="7" t="s">
+      <c r="E51" s="7" t="s">
         <v>796</v>
-      </c>
-      <c r="F49" s="7"/>
-      <c r="G49" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="H49" s="58" t="s">
-        <v>72</v>
-      </c>
-      <c r="I49" s="57" t="s">
-        <v>25</v>
-      </c>
-      <c r="J49" s="57" t="s">
-        <v>26</v>
-      </c>
-      <c r="K49" s="57" t="s">
-        <v>798</v>
-      </c>
-    </row>
-    <row r="50" spans="1:11" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A50" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="B50" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="D50" s="3" t="s">
-        <v>799</v>
-      </c>
-      <c r="E50" s="7" t="s">
-        <v>924</v>
-      </c>
-      <c r="F50" s="7"/>
-      <c r="G50" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="H50" s="58" t="s">
-        <v>127</v>
-      </c>
-      <c r="I50" s="57" t="s">
-        <v>25</v>
-      </c>
-      <c r="J50" s="57" t="s">
-        <v>26</v>
-      </c>
-      <c r="K50" s="57" t="s">
-        <v>925</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A51" s="20"/>
-      <c r="B51" s="20"/>
-      <c r="D51" s="3"/>
-      <c r="E51" s="7" t="s">
-        <v>1071</v>
       </c>
       <c r="F51" s="7"/>
       <c r="G51" s="7" t="s">
-        <v>107</v>
+        <v>28</v>
       </c>
       <c r="H51" s="58" t="s">
         <v>72</v>
@@ -22799,7 +22803,7 @@
         <v>26</v>
       </c>
       <c r="K51" s="57" t="s">
-        <v>1072</v>
+        <v>798</v>
       </c>
     </row>
     <row r="52" spans="1:11" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
@@ -22810,17 +22814,17 @@
         <v>23</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>800</v>
-      </c>
-      <c r="E52" s="58" t="s">
-        <v>797</v>
+        <v>799</v>
+      </c>
+      <c r="E52" s="7" t="s">
+        <v>923</v>
       </c>
       <c r="F52" s="7"/>
       <c r="G52" s="7" t="s">
-        <v>28</v>
+        <v>107</v>
       </c>
       <c r="H52" s="58" t="s">
-        <v>72</v>
+        <v>127</v>
       </c>
       <c r="I52" s="57" t="s">
         <v>25</v>
@@ -22829,74 +22833,79 @@
         <v>26</v>
       </c>
       <c r="K52" s="57" t="s">
-        <v>801</v>
+        <v>924</v>
       </c>
     </row>
     <row r="53" spans="1:11" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A53" s="20"/>
       <c r="B53" s="20"/>
       <c r="D53" s="3"/>
-      <c r="E53" s="58" t="s">
-        <v>418</v>
+      <c r="E53" s="7" t="s">
+        <v>1070</v>
       </c>
       <c r="F53" s="7"/>
-      <c r="G53" s="7"/>
+      <c r="G53" s="7" t="s">
+        <v>107</v>
+      </c>
       <c r="H53" s="58" t="s">
-        <v>171</v>
-      </c>
-      <c r="I53" s="57"/>
-      <c r="J53" s="57"/>
+        <v>72</v>
+      </c>
+      <c r="I53" s="57" t="s">
+        <v>25</v>
+      </c>
+      <c r="J53" s="57" t="s">
+        <v>26</v>
+      </c>
       <c r="K53" s="57" t="s">
-        <v>933</v>
-      </c>
-    </row>
-    <row r="54" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A54" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="B54" s="15" t="s">
+        <v>1071</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A54" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B54" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="E54" s="7" t="s">
-        <v>997</v>
-      </c>
-      <c r="F54" s="7">
-        <v>0</v>
-      </c>
-      <c r="G54" s="18" t="s">
+      <c r="D54" s="3" t="s">
+        <v>800</v>
+      </c>
+      <c r="E54" s="58" t="s">
+        <v>797</v>
+      </c>
+      <c r="F54" s="7"/>
+      <c r="G54" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="H54" s="57" t="s">
+      <c r="H54" s="58" t="s">
         <v>72</v>
       </c>
-      <c r="I54" s="17" t="s">
+      <c r="I54" s="57" t="s">
         <v>25</v>
       </c>
+      <c r="J54" s="57" t="s">
+        <v>26</v>
+      </c>
       <c r="K54" s="57" t="s">
-        <v>996</v>
+        <v>801</v>
       </c>
     </row>
     <row r="55" spans="1:11" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A55" s="20"/>
       <c r="B55" s="20"/>
-      <c r="E55" s="7" t="s">
-        <v>984</v>
+      <c r="D55" s="3"/>
+      <c r="E55" s="58" t="s">
+        <v>418</v>
       </c>
       <c r="F55" s="7"/>
-      <c r="G55" s="21" t="s">
-        <v>107</v>
-      </c>
-      <c r="H55" s="57" t="s">
-        <v>72</v>
-      </c>
-      <c r="I55" s="23" t="s">
-        <v>33</v>
-      </c>
-      <c r="J55" s="57" t="s">
-        <v>29</v>
-      </c>
+      <c r="G55" s="7"/>
+      <c r="H55" s="58" t="s">
+        <v>171</v>
+      </c>
+      <c r="I55" s="57"/>
+      <c r="J55" s="57"/>
       <c r="K55" s="57" t="s">
-        <v>985</v>
+        <v>932</v>
       </c>
     </row>
     <row r="56" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
@@ -22907,72 +22916,75 @@
         <v>23</v>
       </c>
       <c r="E56" s="7" t="s">
-        <v>88</v>
+        <v>996</v>
       </c>
       <c r="F56" s="7">
         <v>0</v>
       </c>
-      <c r="G56" s="7"/>
-      <c r="H56" s="7"/>
-      <c r="K56" s="17" t="s">
-        <v>89</v>
+      <c r="G56" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="H56" s="57" t="s">
+        <v>72</v>
+      </c>
+      <c r="I56" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="K56" s="57" t="s">
+        <v>995</v>
       </c>
     </row>
     <row r="57" spans="1:11" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A57" s="20"/>
       <c r="B57" s="20"/>
       <c r="E57" s="7" t="s">
-        <v>853</v>
-      </c>
-      <c r="F57" s="7">
-        <v>0.08</v>
-      </c>
-      <c r="G57" s="7" t="s">
+        <v>983</v>
+      </c>
+      <c r="F57" s="7"/>
+      <c r="G57" s="21" t="s">
         <v>107</v>
       </c>
-      <c r="H57" s="7" t="s">
+      <c r="H57" s="57" t="s">
         <v>72</v>
       </c>
-      <c r="I57" s="21" t="s">
+      <c r="I57" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="J57" s="21" t="s">
+      <c r="J57" s="57" t="s">
         <v>29</v>
       </c>
-      <c r="K57" s="23" t="s">
-        <v>854</v>
-      </c>
-    </row>
-    <row r="58" spans="1:11" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A58" s="20"/>
-      <c r="B58" s="20"/>
-      <c r="E58" s="58" t="s">
-        <v>988</v>
-      </c>
-      <c r="F58" s="7"/>
-      <c r="G58" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="H58" s="7" t="s">
-        <v>986</v>
-      </c>
-      <c r="I58" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="J58" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="K58" s="23" t="s">
-        <v>987</v>
+      <c r="K57" s="57" t="s">
+        <v>984</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A58" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B58" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="E58" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="F58" s="7">
+        <v>0</v>
+      </c>
+      <c r="G58" s="7"/>
+      <c r="H58" s="7"/>
+      <c r="K58" s="17" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="59" spans="1:11" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A59" s="20"/>
       <c r="B59" s="20"/>
-      <c r="E59" s="58" t="s">
-        <v>992</v>
-      </c>
-      <c r="F59" s="7"/>
+      <c r="E59" s="7" t="s">
+        <v>852</v>
+      </c>
+      <c r="F59" s="7">
+        <v>0.08</v>
+      </c>
       <c r="G59" s="7" t="s">
         <v>107</v>
       </c>
@@ -22980,55 +22992,66 @@
         <v>72</v>
       </c>
       <c r="I59" s="21" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="J59" s="21" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="K59" s="23" t="s">
-        <v>993</v>
+        <v>853</v>
       </c>
     </row>
     <row r="60" spans="1:11" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A60" s="20"/>
       <c r="B60" s="20"/>
       <c r="E60" s="58" t="s">
-        <v>834</v>
+        <v>987</v>
       </c>
       <c r="F60" s="7"/>
       <c r="G60" s="7" t="s">
         <v>107</v>
       </c>
       <c r="H60" s="7" t="s">
-        <v>473</v>
+        <v>985</v>
       </c>
       <c r="I60" s="21" t="s">
-        <v>25</v>
+        <v>33</v>
+      </c>
+      <c r="J60" s="21" t="s">
+        <v>29</v>
       </c>
       <c r="K60" s="23" t="s">
-        <v>835</v>
+        <v>986</v>
       </c>
     </row>
     <row r="61" spans="1:11" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A61" s="20"/>
       <c r="B61" s="20"/>
       <c r="E61" s="58" t="s">
-        <v>471</v>
+        <v>991</v>
       </c>
       <c r="F61" s="7"/>
-      <c r="G61" s="7"/>
+      <c r="G61" s="7" t="s">
+        <v>107</v>
+      </c>
       <c r="H61" s="7" t="s">
-        <v>473</v>
+        <v>72</v>
+      </c>
+      <c r="I61" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="J61" s="21" t="s">
+        <v>26</v>
       </c>
       <c r="K61" s="23" t="s">
-        <v>935</v>
+        <v>992</v>
       </c>
     </row>
     <row r="62" spans="1:11" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A62" s="20"/>
       <c r="B62" s="20"/>
       <c r="E62" s="58" t="s">
-        <v>980</v>
+        <v>834</v>
       </c>
       <c r="F62" s="7"/>
       <c r="G62" s="7" t="s">
@@ -23040,38 +23063,30 @@
       <c r="I62" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="J62" s="21" t="s">
-        <v>26</v>
-      </c>
       <c r="K62" s="23" t="s">
-        <v>981</v>
+        <v>835</v>
       </c>
     </row>
     <row r="63" spans="1:11" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A63" s="20"/>
       <c r="B63" s="20"/>
-      <c r="E63" s="7" t="s">
-        <v>833</v>
+      <c r="E63" s="58" t="s">
+        <v>471</v>
       </c>
       <c r="F63" s="7"/>
-      <c r="G63" s="7" t="s">
-        <v>107</v>
-      </c>
+      <c r="G63" s="7"/>
       <c r="H63" s="7" t="s">
         <v>473</v>
       </c>
-      <c r="I63" s="21" t="s">
-        <v>25</v>
-      </c>
       <c r="K63" s="23" t="s">
-        <v>847</v>
+        <v>934</v>
       </c>
     </row>
     <row r="64" spans="1:11" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A64" s="20"/>
       <c r="B64" s="20"/>
-      <c r="E64" s="7" t="s">
-        <v>955</v>
+      <c r="E64" s="58" t="s">
+        <v>979</v>
       </c>
       <c r="F64" s="7"/>
       <c r="G64" s="7" t="s">
@@ -23081,123 +23096,114 @@
         <v>473</v>
       </c>
       <c r="I64" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="J64" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="K64" s="23" t="s">
+        <v>980</v>
+      </c>
+    </row>
+    <row r="65" spans="1:24" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A65" s="20"/>
+      <c r="B65" s="20"/>
+      <c r="E65" s="7" t="s">
+        <v>833</v>
+      </c>
+      <c r="F65" s="7"/>
+      <c r="G65" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="H65" s="7" t="s">
+        <v>473</v>
+      </c>
+      <c r="I65" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="K65" s="23" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="66" spans="1:24" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A66" s="20"/>
+      <c r="B66" s="20"/>
+      <c r="E66" s="7" t="s">
+        <v>954</v>
+      </c>
+      <c r="F66" s="7"/>
+      <c r="G66" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="H66" s="7" t="s">
+        <v>473</v>
+      </c>
+      <c r="I66" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="K64" s="23" t="s">
-        <v>956</v>
-      </c>
-    </row>
-    <row r="65" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A65" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="B65" s="24" t="s">
+      <c r="K66" s="23" t="s">
+        <v>955</v>
+      </c>
+    </row>
+    <row r="67" spans="1:24" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A67" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B67" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="C65" s="17" t="s">
+      <c r="C67" s="17" t="s">
         <v>90</v>
       </c>
-      <c r="D65" s="17" t="s">
+      <c r="D67" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="E65" s="18" t="s">
+      <c r="E67" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="F65" s="7"/>
-      <c r="G65" s="18" t="s">
+      <c r="F67" s="7"/>
+      <c r="G67" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="H65" s="18" t="s">
+      <c r="H67" s="18" t="s">
         <v>93</v>
       </c>
-      <c r="I65" s="17" t="s">
+      <c r="I67" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="J65" s="17" t="s">
+      <c r="J67" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="K65" s="17" t="s">
+      <c r="K67" s="17" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="66" spans="1:26" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A66" s="20"/>
-      <c r="B66" s="24"/>
-      <c r="C66" s="22"/>
-      <c r="D66" s="22"/>
-      <c r="E66" s="21" t="s">
-        <v>1001</v>
-      </c>
-      <c r="F66" s="7"/>
-      <c r="G66" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="H66" s="21" t="s">
-        <v>56</v>
-      </c>
-      <c r="I66" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="J66" s="23" t="s">
-        <v>29</v>
-      </c>
-      <c r="K66" s="23" t="s">
-        <v>1004</v>
-      </c>
-    </row>
-    <row r="67" spans="1:26" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A67" s="20"/>
-      <c r="B67" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="C67" s="22"/>
-      <c r="D67" s="22"/>
-      <c r="E67" s="21" t="s">
-        <v>910</v>
-      </c>
-      <c r="F67" s="7"/>
-      <c r="G67" s="21" t="s">
-        <v>107</v>
-      </c>
-      <c r="H67" s="21" t="s">
-        <v>911</v>
-      </c>
-      <c r="I67" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="J67" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="K67" s="23" t="s">
-        <v>905</v>
-      </c>
-    </row>
-    <row r="68" spans="1:26" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:24" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A68" s="20"/>
       <c r="B68" s="24"/>
       <c r="C68" s="22"/>
       <c r="D68" s="22"/>
       <c r="E68" s="21" t="s">
-        <v>913</v>
+        <v>1000</v>
       </c>
       <c r="F68" s="7"/>
       <c r="G68" s="21" t="s">
-        <v>107</v>
+        <v>45</v>
       </c>
       <c r="H68" s="21" t="s">
-        <v>405</v>
+        <v>56</v>
       </c>
       <c r="I68" s="23" t="s">
         <v>25</v>
       </c>
       <c r="J68" s="23" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="K68" s="23" t="s">
-        <v>914</v>
-      </c>
-    </row>
-    <row r="69" spans="1:26" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+        <v>1003</v>
+      </c>
+    </row>
+    <row r="69" spans="1:24" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A69" s="20"/>
       <c r="B69" s="24" t="s">
         <v>22</v>
@@ -23205,14 +23211,14 @@
       <c r="C69" s="22"/>
       <c r="D69" s="22"/>
       <c r="E69" s="21" t="s">
-        <v>906</v>
+        <v>909</v>
       </c>
       <c r="F69" s="7"/>
       <c r="G69" s="21" t="s">
         <v>107</v>
       </c>
       <c r="H69" s="21" t="s">
-        <v>93</v>
+        <v>910</v>
       </c>
       <c r="I69" s="23" t="s">
         <v>25</v>
@@ -23221,346 +23227,364 @@
         <v>26</v>
       </c>
       <c r="K69" s="23" t="s">
-        <v>907</v>
-      </c>
-    </row>
-    <row r="70" spans="1:26" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A70" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="B70" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="E70" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="F70" s="18">
-        <v>1</v>
-      </c>
-      <c r="G70" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="H70" s="18" t="s">
-        <v>97</v>
-      </c>
-      <c r="J70" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="K70" s="19" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="71" spans="1:26" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+        <v>904</v>
+      </c>
+    </row>
+    <row r="70" spans="1:24" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A70" s="20"/>
+      <c r="B70" s="24"/>
+      <c r="C70" s="22"/>
+      <c r="D70" s="22"/>
+      <c r="E70" s="21" t="s">
+        <v>912</v>
+      </c>
+      <c r="F70" s="7"/>
+      <c r="G70" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="H70" s="21" t="s">
+        <v>405</v>
+      </c>
+      <c r="I70" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="J70" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="K70" s="23" t="s">
+        <v>913</v>
+      </c>
+    </row>
+    <row r="71" spans="1:24" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A71" s="20"/>
-      <c r="B71" s="20"/>
-      <c r="E71" s="7" t="s">
-        <v>915</v>
-      </c>
+      <c r="B71" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="C71" s="22"/>
+      <c r="D71" s="22"/>
+      <c r="E71" s="21" t="s">
+        <v>905</v>
+      </c>
+      <c r="F71" s="7"/>
       <c r="G71" s="21" t="s">
         <v>107</v>
       </c>
       <c r="H71" s="21" t="s">
-        <v>473</v>
+        <v>93</v>
       </c>
       <c r="I71" s="23" t="s">
         <v>25</v>
       </c>
       <c r="J71" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="K71" s="23" t="s">
+        <v>906</v>
+      </c>
+    </row>
+    <row r="72" spans="1:24" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A72" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B72" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="E72" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="F72" s="18">
+        <v>1</v>
+      </c>
+      <c r="G72" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="H72" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="J72" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="K71" s="23" t="s">
+      <c r="K72" s="19" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="73" spans="1:24" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A73" s="20"/>
+      <c r="B73" s="20"/>
+      <c r="E73" s="7" t="s">
+        <v>914</v>
+      </c>
+      <c r="G73" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="H73" s="21" t="s">
+        <v>473</v>
+      </c>
+      <c r="I73" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="J73" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="K73" s="23" t="s">
+        <v>915</v>
+      </c>
+    </row>
+    <row r="74" spans="1:24" s="25" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A74" s="81"/>
+      <c r="B74" s="81"/>
+      <c r="E74" s="25" t="s">
+        <v>99</v>
+      </c>
+      <c r="F74" s="25">
+        <v>1</v>
+      </c>
+      <c r="G74" s="25" t="s">
+        <v>96</v>
+      </c>
+      <c r="H74" s="25" t="s">
+        <v>97</v>
+      </c>
+      <c r="I74" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="J74" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="K74" s="80" t="s">
+        <v>925</v>
+      </c>
+    </row>
+    <row r="75" spans="1:24" s="25" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A75" s="81"/>
+      <c r="B75" s="81"/>
+      <c r="E75" s="72" t="s">
         <v>916</v>
       </c>
-    </row>
-    <row r="72" spans="1:26" s="25" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A72" s="81"/>
-      <c r="B72" s="81"/>
-      <c r="E72" s="25" t="s">
-        <v>99</v>
-      </c>
-      <c r="F72" s="25">
-        <v>1</v>
-      </c>
-      <c r="G72" s="25" t="s">
-        <v>96</v>
-      </c>
-      <c r="H72" s="25" t="s">
-        <v>97</v>
-      </c>
-      <c r="I72" s="19" t="s">
+      <c r="G75" s="72" t="s">
+        <v>107</v>
+      </c>
+      <c r="H75" s="72" t="s">
+        <v>473</v>
+      </c>
+      <c r="I75" s="80" t="s">
         <v>25</v>
       </c>
-      <c r="J72" s="19" t="s">
+      <c r="J75" s="80" t="s">
+        <v>26</v>
+      </c>
+      <c r="K75" s="23" t="s">
+        <v>917</v>
+      </c>
+    </row>
+    <row r="76" spans="1:24" s="25" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A76" s="81"/>
+      <c r="B76" s="81" t="s">
+        <v>22</v>
+      </c>
+      <c r="E76" s="25" t="s">
+        <v>907</v>
+      </c>
+      <c r="G76" s="25" t="s">
+        <v>107</v>
+      </c>
+      <c r="H76" s="25" t="s">
+        <v>127</v>
+      </c>
+      <c r="I76" s="80" t="s">
+        <v>25</v>
+      </c>
+      <c r="J76" s="19"/>
+      <c r="K76" s="80" t="s">
+        <v>908</v>
+      </c>
+    </row>
+    <row r="77" spans="1:24" s="21" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C77" s="28"/>
+      <c r="D77" s="28"/>
+      <c r="E77" s="7" t="s">
+        <v>807</v>
+      </c>
+      <c r="F77" s="7"/>
+      <c r="G77" s="70" t="s">
+        <v>28</v>
+      </c>
+      <c r="H77" s="70" t="s">
+        <v>225</v>
+      </c>
+      <c r="I77" s="70" t="s">
+        <v>33</v>
+      </c>
+      <c r="J77" s="70" t="s">
+        <v>26</v>
+      </c>
+      <c r="K77" s="57" t="s">
+        <v>808</v>
+      </c>
+      <c r="L77" s="70" t="s">
+        <v>809</v>
+      </c>
+      <c r="M77" s="3"/>
+      <c r="N77" s="7"/>
+      <c r="O77" s="7"/>
+      <c r="P77" s="7"/>
+      <c r="Q77" s="7"/>
+      <c r="R77" s="7"/>
+      <c r="S77" s="7"/>
+      <c r="T77" s="7"/>
+      <c r="U77" s="7"/>
+      <c r="V77" s="7"/>
+      <c r="W77" s="7"/>
+      <c r="X77" s="7"/>
+    </row>
+    <row r="78" spans="1:24" s="21" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C78" s="28"/>
+      <c r="D78" s="28"/>
+      <c r="E78" s="25" t="s">
+        <v>988</v>
+      </c>
+      <c r="F78" s="7"/>
+      <c r="G78" s="70" t="s">
+        <v>107</v>
+      </c>
+      <c r="H78" s="70" t="s">
+        <v>989</v>
+      </c>
+      <c r="I78" s="70" t="s">
+        <v>33</v>
+      </c>
+      <c r="J78" s="70" t="s">
         <v>29</v>
       </c>
-      <c r="K72" s="80" t="s">
-        <v>926</v>
-      </c>
-    </row>
-    <row r="73" spans="1:26" s="25" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A73" s="81"/>
-      <c r="B73" s="81"/>
-      <c r="E73" s="72" t="s">
-        <v>917</v>
-      </c>
-      <c r="G73" s="72" t="s">
-        <v>107</v>
-      </c>
-      <c r="H73" s="72" t="s">
-        <v>473</v>
-      </c>
-      <c r="I73" s="80" t="s">
+      <c r="K78" s="70" t="s">
+        <v>990</v>
+      </c>
+      <c r="L78" s="70"/>
+      <c r="M78" s="3"/>
+      <c r="N78" s="7"/>
+      <c r="O78" s="7"/>
+      <c r="P78" s="7"/>
+      <c r="Q78" s="7"/>
+      <c r="R78" s="7"/>
+      <c r="S78" s="7"/>
+      <c r="T78" s="7"/>
+      <c r="U78" s="7"/>
+      <c r="V78" s="7"/>
+      <c r="W78" s="7"/>
+      <c r="X78" s="7"/>
+    </row>
+    <row r="79" spans="1:24" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A79" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B79" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="E79" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="F79" s="7">
+        <v>-1</v>
+      </c>
+      <c r="G79" s="7"/>
+      <c r="H79" s="7"/>
+    </row>
+    <row r="80" spans="1:24" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A80" s="20"/>
+      <c r="B80" s="20"/>
+      <c r="E80" s="25" t="s">
+        <v>973</v>
+      </c>
+      <c r="F80" s="7" t="s">
+        <v>974</v>
+      </c>
+      <c r="G80" s="25" t="s">
+        <v>69</v>
+      </c>
+      <c r="H80" s="7"/>
+      <c r="K80" s="21" t="s">
+        <v>975</v>
+      </c>
+    </row>
+    <row r="81" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A81" s="15"/>
+      <c r="B81" s="15"/>
+      <c r="C81" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="D81" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="E81" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="F81" s="7">
+        <v>0.6</v>
+      </c>
+      <c r="G81" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="H81" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="I81" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="J73" s="80" t="s">
+      <c r="J81" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="K73" s="23" t="s">
-        <v>918</v>
-      </c>
-    </row>
-    <row r="74" spans="1:26" s="25" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A74" s="81"/>
-      <c r="B74" s="81" t="s">
-        <v>22</v>
-      </c>
-      <c r="E74" s="25" t="s">
-        <v>908</v>
-      </c>
-      <c r="G74" s="25" t="s">
-        <v>107</v>
-      </c>
-      <c r="H74" s="25" t="s">
-        <v>127</v>
-      </c>
-      <c r="I74" s="80" t="s">
-        <v>25</v>
-      </c>
-      <c r="J74" s="19"/>
-      <c r="K74" s="80" t="s">
-        <v>909</v>
-      </c>
-    </row>
-    <row r="75" spans="1:26" s="21" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C75" s="28"/>
-      <c r="D75" s="28"/>
-      <c r="E75" s="7" t="s">
-        <v>807</v>
-      </c>
-      <c r="F75" s="7"/>
-      <c r="G75" s="70" t="s">
-        <v>28</v>
-      </c>
-      <c r="H75" s="70" t="s">
-        <v>225</v>
-      </c>
-      <c r="I75" s="70" t="s">
-        <v>33</v>
-      </c>
-      <c r="J75" s="70" t="s">
-        <v>26</v>
-      </c>
-      <c r="K75" s="57" t="s">
-        <v>808</v>
-      </c>
-      <c r="L75" s="70" t="s">
-        <v>809</v>
-      </c>
-      <c r="M75" s="3"/>
-      <c r="N75" s="7"/>
-      <c r="O75" s="7"/>
-      <c r="P75" s="7"/>
-      <c r="Q75" s="7"/>
-      <c r="R75" s="7"/>
-      <c r="S75" s="7"/>
-      <c r="T75" s="7"/>
-      <c r="U75" s="7"/>
-      <c r="V75" s="7"/>
-      <c r="W75" s="7"/>
-      <c r="X75" s="7"/>
-    </row>
-    <row r="76" spans="1:26" s="21" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C76" s="28"/>
-      <c r="D76" s="28"/>
-      <c r="E76" s="25" t="s">
-        <v>989</v>
-      </c>
-      <c r="F76" s="7"/>
-      <c r="G76" s="70" t="s">
-        <v>107</v>
-      </c>
-      <c r="H76" s="70" t="s">
-        <v>990</v>
-      </c>
-      <c r="I76" s="70" t="s">
-        <v>33</v>
-      </c>
-      <c r="J76" s="70" t="s">
-        <v>29</v>
-      </c>
-      <c r="K76" s="70" t="s">
-        <v>991</v>
-      </c>
-      <c r="L76" s="70"/>
-      <c r="M76" s="3"/>
-      <c r="N76" s="7"/>
-      <c r="O76" s="7"/>
-      <c r="P76" s="7"/>
-      <c r="Q76" s="7"/>
-      <c r="R76" s="7"/>
-      <c r="S76" s="7"/>
-      <c r="T76" s="7"/>
-      <c r="U76" s="7"/>
-      <c r="V76" s="7"/>
-      <c r="W76" s="7"/>
-      <c r="X76" s="7"/>
-    </row>
-    <row r="77" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A77" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="B77" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="E77" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="F77" s="7">
-        <v>-1</v>
-      </c>
-      <c r="G77" s="7"/>
-      <c r="H77" s="7"/>
-    </row>
-    <row r="78" spans="1:26" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A78" s="20"/>
-      <c r="B78" s="20"/>
-      <c r="E78" s="25" t="s">
-        <v>974</v>
-      </c>
-      <c r="F78" s="7" t="s">
-        <v>975</v>
-      </c>
-      <c r="G78" s="25" t="s">
-        <v>69</v>
-      </c>
-      <c r="H78" s="7"/>
-      <c r="K78" s="21" t="s">
-        <v>976</v>
-      </c>
-    </row>
-    <row r="79" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A79" s="15"/>
-      <c r="B79" s="15"/>
-      <c r="C79" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="D79" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="E79" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="F79" s="7">
-        <v>0.6</v>
-      </c>
-      <c r="G79" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="H79" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="I79" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="J79" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="K79" s="7" t="s">
+      <c r="K81" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="L79" s="7"/>
-      <c r="M79" s="7"/>
-      <c r="N79" s="7"/>
-      <c r="O79" s="7"/>
-      <c r="P79" s="7"/>
-      <c r="Q79" s="7"/>
-      <c r="R79" s="7"/>
-      <c r="S79" s="7"/>
-      <c r="T79" s="7"/>
-      <c r="U79" s="7"/>
-      <c r="V79" s="7"/>
-      <c r="W79" s="7"/>
-      <c r="X79" s="7"/>
-      <c r="Y79" s="7"/>
-      <c r="Z79" s="7"/>
-    </row>
-    <row r="80" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A80" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="B80" s="15" t="s">
+      <c r="L81" s="7"/>
+      <c r="M81" s="7"/>
+      <c r="N81" s="7"/>
+      <c r="O81" s="7"/>
+      <c r="P81" s="7"/>
+      <c r="Q81" s="7"/>
+      <c r="R81" s="7"/>
+      <c r="S81" s="7"/>
+      <c r="T81" s="7"/>
+      <c r="U81" s="7"/>
+      <c r="V81" s="7"/>
+      <c r="W81" s="7"/>
+      <c r="X81" s="7"/>
+      <c r="Y81" s="7"/>
+      <c r="Z81" s="7"/>
+    </row>
+    <row r="82" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A82" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B82" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="E80" s="7" t="s">
+      <c r="E82" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="F80" s="7">
+      <c r="F82" s="7">
         <v>1739.927555</v>
       </c>
-      <c r="G80" s="7"/>
-      <c r="H80" s="7" t="s">
+      <c r="G82" s="7"/>
+      <c r="H82" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="K80" s="3" t="s">
+      <c r="K82" s="3" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="81" spans="1:12" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A81" s="20"/>
-      <c r="B81" s="20"/>
-      <c r="E81" s="7" t="s">
-        <v>952</v>
-      </c>
-      <c r="F81" s="7"/>
-      <c r="G81" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="H81" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="I81" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="J81" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="K81" s="3"/>
-    </row>
-    <row r="82" spans="1:12" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A82" s="20"/>
-      <c r="B82" s="20"/>
-      <c r="E82" s="7" t="s">
-        <v>495</v>
-      </c>
-      <c r="F82" s="7"/>
-      <c r="G82" s="7"/>
-      <c r="H82" s="7"/>
-      <c r="K82" s="3" t="s">
-        <v>934</v>
-      </c>
-    </row>
-    <row r="83" spans="1:12" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:26" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A83" s="20"/>
       <c r="B83" s="20"/>
       <c r="E83" s="7" t="s">
-        <v>848</v>
+        <v>951</v>
       </c>
       <c r="F83" s="7"/>
       <c r="G83" s="7" t="s">
-        <v>28</v>
+        <v>107</v>
       </c>
       <c r="H83" s="7" t="s">
-        <v>72</v>
+        <v>83</v>
       </c>
       <c r="I83" s="21" t="s">
         <v>33</v>
@@ -23568,328 +23592,312 @@
       <c r="J83" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="K83" s="21" t="s">
-        <v>850</v>
-      </c>
-      <c r="L83" s="3" t="s">
-        <v>849</v>
-      </c>
-    </row>
-    <row r="84" spans="1:12" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="K83" s="3"/>
+    </row>
+    <row r="84" spans="1:26" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A84" s="20"/>
       <c r="B84" s="20"/>
       <c r="E84" s="7" t="s">
-        <v>912</v>
+        <v>495</v>
       </c>
       <c r="F84" s="7"/>
-      <c r="G84" s="7" t="s">
+      <c r="G84" s="7"/>
+      <c r="H84" s="7"/>
+      <c r="K84" s="3" t="s">
+        <v>933</v>
+      </c>
+    </row>
+    <row r="85" spans="1:26" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A85" s="20"/>
+      <c r="B85" s="20"/>
+      <c r="E85" s="7" t="s">
+        <v>848</v>
+      </c>
+      <c r="F85" s="7"/>
+      <c r="G85" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="H84" s="7" t="s">
+      <c r="H85" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="I85" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="J85" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="K85" s="21" t="s">
+        <v>850</v>
+      </c>
+      <c r="L85" s="3" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="86" spans="1:26" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A86" s="20"/>
+      <c r="B86" s="20"/>
+      <c r="E86" s="7" t="s">
+        <v>911</v>
+      </c>
+      <c r="F86" s="7"/>
+      <c r="G86" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="H86" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="I84" s="21" t="s">
+      <c r="I86" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="J84" s="21" t="s">
+      <c r="J86" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="K84" s="21" t="s">
-        <v>897</v>
-      </c>
-      <c r="L84" s="3" t="s">
+      <c r="K86" s="21" t="s">
+        <v>896</v>
+      </c>
+      <c r="L86" s="3" t="s">
         <v>849</v>
       </c>
     </row>
-    <row r="85" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A85" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="B85" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="C85" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E85" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="F85" s="7">
-        <v>1</v>
-      </c>
-      <c r="G85" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="H85" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="I85" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="J85" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="K85" s="3" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="86" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A86" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="B86" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="E86" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="F86" s="7">
-        <v>553659</v>
-      </c>
-      <c r="G86" s="7"/>
-      <c r="H86" s="7"/>
-    </row>
-    <row r="87" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A87" s="15" t="s">
         <v>22</v>
       </c>
       <c r="B87" s="15" t="s">
         <v>23</v>
       </c>
+      <c r="C87" s="3" t="s">
+        <v>23</v>
+      </c>
       <c r="E87" s="7" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="F87" s="7">
-        <v>4891208</v>
-      </c>
-      <c r="G87" s="7"/>
-      <c r="H87" s="7"/>
-    </row>
-    <row r="88" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="G87" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="H87" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="I87" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="J87" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="K87" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="88" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A88" s="15" t="s">
         <v>22</v>
       </c>
       <c r="B88" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="C88" s="3" t="s">
+      <c r="E88" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="F88" s="7">
+        <v>553659</v>
+      </c>
+      <c r="G88" s="7"/>
+      <c r="H88" s="7"/>
+    </row>
+    <row r="89" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A89" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B89" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="E88" s="7" t="s">
+      <c r="E89" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="F89" s="7">
+        <v>4891208</v>
+      </c>
+      <c r="G89" s="7"/>
+      <c r="H89" s="7"/>
+    </row>
+    <row r="90" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A90" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B90" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C90" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E90" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="F88" s="7">
+      <c r="F90" s="7">
         <v>1</v>
       </c>
-      <c r="G88" s="7" t="s">
+      <c r="G90" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="H88" s="7" t="s">
+      <c r="H90" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="I88" s="3" t="s">
+      <c r="I90" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="J88" s="3" t="s">
+      <c r="J90" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="K88" s="3" t="s">
+      <c r="K90" s="3" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="89" spans="1:12" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A89" s="20"/>
-      <c r="B89" s="20"/>
-      <c r="C89" s="3"/>
-      <c r="E89" s="7" t="s">
-        <v>927</v>
-      </c>
-      <c r="F89" s="7"/>
-      <c r="G89" s="7"/>
-      <c r="H89" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="I89" s="3"/>
-      <c r="J89" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="K89" s="3" t="s">
-        <v>929</v>
-      </c>
-    </row>
-    <row r="90" spans="1:12" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A90" s="20" t="s">
-        <v>831</v>
-      </c>
-      <c r="B90" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="C90" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="D90" s="21" t="s">
-        <v>64</v>
-      </c>
-      <c r="E90" s="7" t="s">
-        <v>830</v>
-      </c>
-      <c r="F90" s="7">
-        <v>5</v>
-      </c>
-      <c r="G90" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="H90" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="I90" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="J90" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="K90" s="3" t="s">
-        <v>832</v>
-      </c>
-      <c r="L90" s="23" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="91" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A91" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="B91" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="D91" s="3" t="s">
-        <v>125</v>
-      </c>
+    <row r="91" spans="1:26" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A91" s="20"/>
+      <c r="B91" s="20"/>
+      <c r="C91" s="3"/>
       <c r="E91" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="F91" s="7">
-        <v>0</v>
-      </c>
+        <v>926</v>
+      </c>
+      <c r="F91" s="7"/>
       <c r="G91" s="7"/>
       <c r="H91" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="I91" s="3" t="s">
-        <v>25</v>
-      </c>
+      <c r="I91" s="3"/>
       <c r="J91" s="3" t="s">
         <v>26</v>
       </c>
       <c r="K91" s="3" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="92" spans="1:12" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A92" s="20"/>
-      <c r="B92" s="20"/>
-      <c r="D92" s="3"/>
+        <v>928</v>
+      </c>
+    </row>
+    <row r="92" spans="1:26" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A92" s="20" t="s">
+        <v>831</v>
+      </c>
+      <c r="B92" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="C92" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D92" s="21" t="s">
+        <v>64</v>
+      </c>
       <c r="E92" s="7" t="s">
-        <v>928</v>
-      </c>
-      <c r="F92" s="7"/>
-      <c r="G92" s="7"/>
+        <v>830</v>
+      </c>
+      <c r="F92" s="7">
+        <v>5</v>
+      </c>
+      <c r="G92" s="7" t="s">
+        <v>107</v>
+      </c>
       <c r="H92" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="I92" s="3"/>
-      <c r="J92" s="3"/>
+      <c r="I92" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="J92" s="3" t="s">
+        <v>26</v>
+      </c>
       <c r="K92" s="3" t="s">
-        <v>930</v>
-      </c>
-    </row>
-    <row r="93" spans="1:12" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A93" s="20"/>
-      <c r="B93" s="20"/>
-      <c r="D93" s="3"/>
+        <v>832</v>
+      </c>
+      <c r="L92" s="23" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="93" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A93" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B93" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="D93" s="3" t="s">
+        <v>125</v>
+      </c>
       <c r="E93" s="7" t="s">
-        <v>931</v>
-      </c>
-      <c r="F93" s="7"/>
+        <v>126</v>
+      </c>
+      <c r="F93" s="7">
+        <v>0</v>
+      </c>
       <c r="G93" s="7"/>
       <c r="H93" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="I93" s="3"/>
-      <c r="J93" s="3"/>
+      <c r="I93" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="J93" s="3" t="s">
+        <v>26</v>
+      </c>
       <c r="K93" s="3" t="s">
-        <v>932</v>
-      </c>
-    </row>
-    <row r="94" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A94" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="B94" s="15"/>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="94" spans="1:26" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A94" s="20"/>
+      <c r="B94" s="20"/>
+      <c r="D94" s="3"/>
       <c r="E94" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="F94" s="7">
-        <v>6772</v>
-      </c>
+        <v>927</v>
+      </c>
+      <c r="F94" s="7"/>
       <c r="G94" s="7"/>
-      <c r="H94" s="7"/>
-    </row>
-    <row r="95" spans="1:12" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="H94" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="I94" s="3"/>
+      <c r="J94" s="3"/>
+      <c r="K94" s="3" t="s">
+        <v>929</v>
+      </c>
+    </row>
+    <row r="95" spans="1:26" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A95" s="20"/>
       <c r="B95" s="20"/>
+      <c r="D95" s="3"/>
       <c r="E95" s="7" t="s">
-        <v>945</v>
-      </c>
-      <c r="F95" s="7">
-        <v>5</v>
-      </c>
-      <c r="G95" s="58" t="s">
-        <v>107</v>
-      </c>
+        <v>930</v>
+      </c>
+      <c r="F95" s="7"/>
+      <c r="G95" s="7"/>
       <c r="H95" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="I95" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="J95" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="K95" s="23" t="s">
-        <v>946</v>
-      </c>
-    </row>
-    <row r="96" spans="1:12" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A96" s="20"/>
-      <c r="B96" s="20"/>
-      <c r="E96" s="58" t="s">
-        <v>947</v>
+      <c r="I95" s="3"/>
+      <c r="J95" s="3"/>
+      <c r="K95" s="3" t="s">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="96" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A96" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B96" s="15"/>
+      <c r="E96" s="7" t="s">
+        <v>129</v>
       </c>
       <c r="F96" s="7">
-        <v>5</v>
-      </c>
-      <c r="G96" s="58" t="s">
-        <v>107</v>
-      </c>
-      <c r="H96" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="I96" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="J96" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="K96" s="23" t="s">
-        <v>948</v>
-      </c>
+        <v>6772</v>
+      </c>
+      <c r="G96" s="7"/>
+      <c r="H96" s="7"/>
     </row>
     <row r="97" spans="1:12" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A97" s="20"/>
       <c r="B97" s="20"/>
-      <c r="E97" s="58" t="s">
-        <v>949</v>
+      <c r="E97" s="7" t="s">
+        <v>944</v>
       </c>
       <c r="F97" s="7">
         <v>5</v>
@@ -23907,103 +23915,113 @@
         <v>29</v>
       </c>
       <c r="K97" s="23" t="s">
-        <v>950</v>
+        <v>945</v>
       </c>
     </row>
     <row r="98" spans="1:12" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A98" s="20"/>
       <c r="B98" s="20"/>
-      <c r="E98" s="7" t="s">
-        <v>837</v>
+      <c r="E98" s="58" t="s">
+        <v>946</v>
       </c>
       <c r="F98" s="7">
-        <v>1</v>
-      </c>
-      <c r="G98" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G98" s="58" t="s">
         <v>107</v>
       </c>
       <c r="H98" s="7" t="s">
-        <v>838</v>
-      </c>
-      <c r="I98" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="J98" s="23" t="s">
-        <v>839</v>
-      </c>
-    </row>
-    <row r="99" spans="1:12" s="65" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A99" s="92"/>
-      <c r="B99" s="92"/>
-      <c r="C99" s="76" t="s">
-        <v>1017</v>
-      </c>
-      <c r="E99" s="64" t="s">
-        <v>970</v>
-      </c>
-      <c r="F99" s="64"/>
-      <c r="G99" s="64" t="s">
+        <v>127</v>
+      </c>
+      <c r="I98" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="J98" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="K98" s="23" t="s">
+        <v>947</v>
+      </c>
+    </row>
+    <row r="99" spans="1:12" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A99" s="20"/>
+      <c r="B99" s="20"/>
+      <c r="E99" s="58" t="s">
+        <v>948</v>
+      </c>
+      <c r="F99" s="7">
+        <v>5</v>
+      </c>
+      <c r="G99" s="58" t="s">
         <v>107</v>
       </c>
-      <c r="H99" s="64" t="s">
-        <v>62</v>
-      </c>
-      <c r="I99" s="94" t="s">
-        <v>25</v>
-      </c>
-      <c r="J99" s="94" t="s">
-        <v>26</v>
-      </c>
-      <c r="K99" s="94"/>
-      <c r="L99" s="94" t="s">
-        <v>969</v>
+      <c r="H99" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="I99" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="J99" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="K99" s="23" t="s">
+        <v>949</v>
       </c>
     </row>
     <row r="100" spans="1:12" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A100" s="20"/>
       <c r="B100" s="20"/>
       <c r="E100" s="7" t="s">
-        <v>943</v>
-      </c>
-      <c r="F100" s="7"/>
+        <v>837</v>
+      </c>
+      <c r="F100" s="7">
+        <v>1</v>
+      </c>
       <c r="G100" s="7" t="s">
         <v>107</v>
       </c>
       <c r="H100" s="7" t="s">
-        <v>623</v>
-      </c>
-      <c r="I100" s="23"/>
-      <c r="J100" s="23"/>
-      <c r="K100" s="23" t="s">
-        <v>972</v>
-      </c>
-      <c r="L100" s="23"/>
-    </row>
-    <row r="101" spans="1:12" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A101" s="20"/>
-      <c r="B101" s="20"/>
-      <c r="E101" s="7" t="s">
-        <v>944</v>
-      </c>
-      <c r="F101" s="7"/>
-      <c r="G101" s="7" t="s">
+        <v>838</v>
+      </c>
+      <c r="I100" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="J100" s="23" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="101" spans="1:12" s="65" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A101" s="92"/>
+      <c r="B101" s="92"/>
+      <c r="C101" s="76" t="s">
+        <v>1016</v>
+      </c>
+      <c r="E101" s="64" t="s">
+        <v>969</v>
+      </c>
+      <c r="F101" s="64"/>
+      <c r="G101" s="64" t="s">
         <v>107</v>
       </c>
-      <c r="H101" s="7" t="s">
-        <v>623</v>
-      </c>
-      <c r="I101" s="23"/>
-      <c r="J101" s="23"/>
-      <c r="K101" s="23" t="s">
-        <v>973</v>
-      </c>
-      <c r="L101" s="23"/>
+      <c r="H101" s="64" t="s">
+        <v>62</v>
+      </c>
+      <c r="I101" s="94" t="s">
+        <v>25</v>
+      </c>
+      <c r="J101" s="94" t="s">
+        <v>26</v>
+      </c>
+      <c r="K101" s="94"/>
+      <c r="L101" s="94" t="s">
+        <v>968</v>
+      </c>
     </row>
     <row r="102" spans="1:12" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A102" s="20"/>
       <c r="B102" s="20"/>
       <c r="E102" s="7" t="s">
-        <v>1006</v>
+        <v>942</v>
       </c>
       <c r="F102" s="7"/>
       <c r="G102" s="7" t="s">
@@ -24012,14 +24030,10 @@
       <c r="H102" s="7" t="s">
         <v>623</v>
       </c>
-      <c r="I102" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="J102" s="23" t="s">
-        <v>26</v>
-      </c>
+      <c r="I102" s="23"/>
+      <c r="J102" s="23"/>
       <c r="K102" s="23" t="s">
-        <v>1009</v>
+        <v>971</v>
       </c>
       <c r="L102" s="23"/>
     </row>
@@ -24027,7 +24041,7 @@
       <c r="A103" s="20"/>
       <c r="B103" s="20"/>
       <c r="E103" s="7" t="s">
-        <v>1007</v>
+        <v>943</v>
       </c>
       <c r="F103" s="7"/>
       <c r="G103" s="7" t="s">
@@ -24036,102 +24050,92 @@
       <c r="H103" s="7" t="s">
         <v>623</v>
       </c>
-      <c r="I103" s="23" t="s">
-        <v>33</v>
-      </c>
+      <c r="I103" s="23"/>
       <c r="J103" s="23"/>
       <c r="K103" s="23" t="s">
-        <v>1008</v>
+        <v>972</v>
       </c>
       <c r="L103" s="23"/>
     </row>
     <row r="104" spans="1:12" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A104" s="20"/>
       <c r="B104" s="20"/>
-      <c r="D104" s="57" t="s">
-        <v>937</v>
-      </c>
       <c r="E104" s="7" t="s">
-        <v>962</v>
+        <v>1005</v>
       </c>
       <c r="F104" s="7"/>
-      <c r="G104" s="58" t="s">
+      <c r="G104" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="H104" s="58" t="s">
-        <v>83</v>
+      <c r="H104" s="7" t="s">
+        <v>623</v>
       </c>
       <c r="I104" s="23" t="s">
-        <v>940</v>
+        <v>25</v>
       </c>
       <c r="J104" s="23" t="s">
-        <v>940</v>
+        <v>26</v>
       </c>
       <c r="K104" s="23" t="s">
-        <v>963</v>
+        <v>1008</v>
       </c>
       <c r="L104" s="23"/>
     </row>
     <row r="105" spans="1:12" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A105" s="20"/>
       <c r="B105" s="20"/>
-      <c r="D105" s="57"/>
       <c r="E105" s="7" t="s">
-        <v>1012</v>
+        <v>1006</v>
       </c>
       <c r="F105" s="7"/>
       <c r="G105" s="7" t="s">
         <v>107</v>
       </c>
       <c r="H105" s="7" t="s">
-        <v>62</v>
+        <v>623</v>
       </c>
       <c r="I105" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="J105" s="23" t="s">
-        <v>26</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="J105" s="23"/>
       <c r="K105" s="23" t="s">
-        <v>971</v>
-      </c>
-      <c r="L105" s="23" t="s">
-        <v>1015</v>
-      </c>
+        <v>1007</v>
+      </c>
+      <c r="L105" s="23"/>
     </row>
     <row r="106" spans="1:12" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A106" s="20"/>
       <c r="B106" s="20"/>
-      <c r="D106" s="57"/>
+      <c r="D106" s="57" t="s">
+        <v>936</v>
+      </c>
       <c r="E106" s="7" t="s">
-        <v>1013</v>
+        <v>961</v>
       </c>
       <c r="F106" s="7"/>
-      <c r="G106" s="7" t="s">
+      <c r="G106" s="58" t="s">
         <v>107</v>
       </c>
-      <c r="H106" s="7" t="s">
-        <v>62</v>
+      <c r="H106" s="58" t="s">
+        <v>83</v>
       </c>
       <c r="I106" s="23" t="s">
-        <v>25</v>
+        <v>939</v>
       </c>
       <c r="J106" s="23" t="s">
-        <v>26</v>
+        <v>939</v>
       </c>
       <c r="K106" s="23" t="s">
-        <v>971</v>
-      </c>
-      <c r="L106" s="23" t="s">
-        <v>1016</v>
-      </c>
-    </row>
-    <row r="107" spans="1:12" s="21" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+        <v>962</v>
+      </c>
+      <c r="L106" s="23"/>
+    </row>
+    <row r="107" spans="1:12" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A107" s="20"/>
       <c r="B107" s="20"/>
       <c r="D107" s="57"/>
-      <c r="E107" s="25" t="s">
-        <v>1014</v>
+      <c r="E107" s="7" t="s">
+        <v>1011</v>
       </c>
       <c r="F107" s="7"/>
       <c r="G107" s="7" t="s">
@@ -24147,26 +24151,25 @@
         <v>26</v>
       </c>
       <c r="K107" s="23" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="L107" s="23" t="s">
-        <v>969</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="108" spans="1:12" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A108" s="20"/>
       <c r="B108" s="20"/>
+      <c r="D108" s="57"/>
       <c r="E108" s="7" t="s">
-        <v>836</v>
-      </c>
-      <c r="F108" s="7">
-        <v>10</v>
-      </c>
+        <v>1012</v>
+      </c>
+      <c r="F108" s="7"/>
       <c r="G108" s="7" t="s">
         <v>107</v>
       </c>
       <c r="H108" s="7" t="s">
-        <v>623</v>
+        <v>62</v>
       </c>
       <c r="I108" s="23" t="s">
         <v>25</v>
@@ -24175,23 +24178,25 @@
         <v>26</v>
       </c>
       <c r="K108" s="23" t="s">
-        <v>842</v>
+        <v>970</v>
+      </c>
+      <c r="L108" s="23" t="s">
+        <v>1015</v>
       </c>
     </row>
     <row r="109" spans="1:12" s="21" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A109" s="20"/>
       <c r="B109" s="20"/>
-      <c r="E109" s="72" t="s">
-        <v>1005</v>
-      </c>
-      <c r="F109" s="7">
-        <v>10</v>
-      </c>
+      <c r="D109" s="57"/>
+      <c r="E109" s="25" t="s">
+        <v>1013</v>
+      </c>
+      <c r="F109" s="7"/>
       <c r="G109" s="7" t="s">
         <v>107</v>
       </c>
       <c r="H109" s="7" t="s">
-        <v>623</v>
+        <v>62</v>
       </c>
       <c r="I109" s="23" t="s">
         <v>25</v>
@@ -24200,16 +24205,21 @@
         <v>26</v>
       </c>
       <c r="K109" s="23" t="s">
-        <v>842</v>
+        <v>970</v>
+      </c>
+      <c r="L109" s="23" t="s">
+        <v>968</v>
       </c>
     </row>
     <row r="110" spans="1:12" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A110" s="20"/>
       <c r="B110" s="20"/>
-      <c r="E110" s="72" t="s">
-        <v>1010</v>
-      </c>
-      <c r="F110" s="7"/>
+      <c r="E110" s="7" t="s">
+        <v>836</v>
+      </c>
+      <c r="F110" s="7">
+        <v>10</v>
+      </c>
       <c r="G110" s="7" t="s">
         <v>107</v>
       </c>
@@ -24220,19 +24230,21 @@
         <v>25</v>
       </c>
       <c r="J110" s="23" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="K110" s="23" t="s">
-        <v>1011</v>
-      </c>
-    </row>
-    <row r="111" spans="1:12" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+        <v>842</v>
+      </c>
+    </row>
+    <row r="111" spans="1:12" s="21" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A111" s="20"/>
       <c r="B111" s="20"/>
-      <c r="E111" s="7" t="s">
-        <v>953</v>
-      </c>
-      <c r="F111" s="7"/>
+      <c r="E111" s="72" t="s">
+        <v>1004</v>
+      </c>
+      <c r="F111" s="7">
+        <v>10</v>
+      </c>
       <c r="G111" s="7" t="s">
         <v>107</v>
       </c>
@@ -24240,20 +24252,20 @@
         <v>623</v>
       </c>
       <c r="I111" s="23" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="J111" s="23" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="K111" s="23" t="s">
-        <v>954</v>
+        <v>842</v>
       </c>
     </row>
     <row r="112" spans="1:12" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A112" s="20"/>
       <c r="B112" s="20"/>
-      <c r="E112" s="7" t="s">
-        <v>966</v>
+      <c r="E112" s="72" t="s">
+        <v>1009</v>
       </c>
       <c r="F112" s="7"/>
       <c r="G112" s="7" t="s">
@@ -24262,153 +24274,135 @@
       <c r="H112" s="7" t="s">
         <v>623</v>
       </c>
-      <c r="I112" s="23"/>
+      <c r="I112" s="23" t="s">
+        <v>25</v>
+      </c>
       <c r="J112" s="23" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="K112" s="23" t="s">
-        <v>967</v>
-      </c>
-      <c r="L112" s="23" t="s">
-        <v>968</v>
-      </c>
-    </row>
-    <row r="113" spans="1:11" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+        <v>1010</v>
+      </c>
+    </row>
+    <row r="113" spans="1:12" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A113" s="20"/>
       <c r="B113" s="20"/>
       <c r="E113" s="7" t="s">
-        <v>508</v>
+        <v>952</v>
       </c>
       <c r="F113" s="7"/>
-      <c r="G113" s="7"/>
+      <c r="G113" s="7" t="s">
+        <v>107</v>
+      </c>
       <c r="H113" s="7" t="s">
-        <v>509</v>
-      </c>
-      <c r="I113" s="23"/>
-      <c r="J113" s="23"/>
+        <v>623</v>
+      </c>
+      <c r="I113" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="J113" s="23" t="s">
+        <v>29</v>
+      </c>
       <c r="K113" s="23" t="s">
-        <v>936</v>
-      </c>
-    </row>
-    <row r="114" spans="1:11" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+        <v>953</v>
+      </c>
+    </row>
+    <row r="114" spans="1:12" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A114" s="20"/>
       <c r="B114" s="20"/>
-      <c r="D114" s="57" t="s">
-        <v>24</v>
-      </c>
       <c r="E114" s="7" t="s">
-        <v>791</v>
+        <v>965</v>
       </c>
       <c r="F114" s="7"/>
-      <c r="G114" s="58" t="s">
-        <v>28</v>
+      <c r="G114" s="7" t="s">
+        <v>107</v>
       </c>
       <c r="H114" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="I114" s="23" t="s">
-        <v>25</v>
-      </c>
+        <v>623</v>
+      </c>
+      <c r="I114" s="23"/>
       <c r="J114" s="23" t="s">
         <v>26</v>
       </c>
       <c r="K114" s="23" t="s">
+        <v>966</v>
+      </c>
+      <c r="L114" s="23" t="s">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="115" spans="1:12" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A115" s="20"/>
+      <c r="B115" s="20"/>
+      <c r="E115" s="7" t="s">
+        <v>508</v>
+      </c>
+      <c r="F115" s="7"/>
+      <c r="G115" s="7"/>
+      <c r="H115" s="7" t="s">
+        <v>509</v>
+      </c>
+      <c r="I115" s="23"/>
+      <c r="J115" s="23"/>
+      <c r="K115" s="23" t="s">
+        <v>935</v>
+      </c>
+    </row>
+    <row r="116" spans="1:12" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A116" s="20"/>
+      <c r="B116" s="20"/>
+      <c r="D116" s="57" t="s">
+        <v>24</v>
+      </c>
+      <c r="E116" s="7" t="s">
+        <v>791</v>
+      </c>
+      <c r="F116" s="7"/>
+      <c r="G116" s="58" t="s">
+        <v>28</v>
+      </c>
+      <c r="H116" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="I116" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="J116" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="K116" s="23" t="s">
         <v>792</v>
       </c>
     </row>
-    <row r="115" spans="1:11" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A115" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="B115" s="20"/>
-      <c r="D115" s="57" t="s">
+    <row r="117" spans="1:12" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A117" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B117" s="20"/>
+      <c r="D117" s="57" t="s">
         <v>24</v>
       </c>
-      <c r="E115" s="7" t="s">
+      <c r="E117" s="7" t="s">
         <v>793</v>
       </c>
-      <c r="F115" s="7"/>
-      <c r="G115" s="58" t="s">
+      <c r="F117" s="7"/>
+      <c r="G117" s="58" t="s">
         <v>28</v>
       </c>
-      <c r="H115" s="7" t="s">
+      <c r="H117" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="I115" s="23" t="s">
+      <c r="I117" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="J115" s="23" t="s">
+      <c r="J117" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="K115" s="23" t="s">
+      <c r="K117" s="23" t="s">
         <v>794</v>
       </c>
     </row>
-    <row r="116" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A116" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="B116" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="D116" s="17" t="s">
-        <v>131</v>
-      </c>
-      <c r="E116" s="18" t="s">
-        <v>133</v>
-      </c>
-      <c r="F116" s="18">
-        <v>1500</v>
-      </c>
-      <c r="G116" s="18" t="s">
-        <v>107</v>
-      </c>
-      <c r="H116" s="18" t="s">
-        <v>1019</v>
-      </c>
-      <c r="I116" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="J116" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="K116" s="17" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="117" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A117" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="B117" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="D117" s="17" t="s">
-        <v>131</v>
-      </c>
-      <c r="E117" s="17" t="s">
-        <v>138</v>
-      </c>
-      <c r="F117" s="17">
-        <v>1500</v>
-      </c>
-      <c r="G117" s="18" t="s">
-        <v>107</v>
-      </c>
-      <c r="H117" s="23" t="s">
-        <v>1019</v>
-      </c>
-      <c r="I117" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="J117" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="K117" s="17" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="118" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A118" s="15" t="s">
         <v>22</v>
       </c>
@@ -24418,17 +24412,17 @@
       <c r="D118" s="17" t="s">
         <v>131</v>
       </c>
-      <c r="E118" s="17" t="s">
-        <v>141</v>
-      </c>
-      <c r="F118" s="17">
+      <c r="E118" s="18" t="s">
+        <v>133</v>
+      </c>
+      <c r="F118" s="18">
         <v>1500</v>
       </c>
       <c r="G118" s="18" t="s">
         <v>107</v>
       </c>
-      <c r="H118" s="23" t="s">
-        <v>1019</v>
+      <c r="H118" s="18" t="s">
+        <v>1018</v>
       </c>
       <c r="I118" s="17" t="s">
         <v>33</v>
@@ -24437,13 +24431,77 @@
         <v>29</v>
       </c>
       <c r="K118" s="17" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="119" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A119" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B119" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="D119" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="E119" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="F119" s="17">
+        <v>1500</v>
+      </c>
+      <c r="G119" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="H119" s="23" t="s">
+        <v>1018</v>
+      </c>
+      <c r="I119" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="J119" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="K119" s="17" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="120" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A120" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B120" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="D120" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="E120" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="F120" s="17">
+        <v>1500</v>
+      </c>
+      <c r="G120" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="H120" s="23" t="s">
+        <v>1018</v>
+      </c>
+      <c r="I120" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="J120" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="K120" s="17" t="s">
         <v>142</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B65:B69">
+  <conditionalFormatting sqref="B67:B71">
     <cfRule type="notContainsBlanks" dxfId="0" priority="1">
-      <formula>LEN(TRIM(B65))&gt;0</formula>
+      <formula>LEN(TRIM(B67))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -24698,7 +24756,7 @@
       <c r="C7" s="107"/>
       <c r="D7" s="107"/>
       <c r="E7" s="108" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="F7" s="108" t="s">
         <v>107</v>
@@ -24710,7 +24768,7 @@
         <v>26</v>
       </c>
       <c r="I7" s="110" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
       <c r="J7" s="109"/>
     </row>
@@ -24866,22 +24924,22 @@
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
       <c r="E12" s="21" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="F12" s="57" t="s">
         <v>28</v>
       </c>
       <c r="G12" s="70" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="H12" s="21" t="s">
         <v>29</v>
       </c>
       <c r="I12" s="21" t="s">
+        <v>1030</v>
+      </c>
+      <c r="J12" s="21" t="s">
         <v>1031</v>
-      </c>
-      <c r="J12" s="21" t="s">
-        <v>1032</v>
       </c>
       <c r="K12" s="7"/>
       <c r="L12" s="7"/>
@@ -25020,10 +25078,10 @@
         <v>29</v>
       </c>
       <c r="I16" s="7" t="s">
+        <v>1025</v>
+      </c>
+      <c r="J16" s="7" t="s">
         <v>1026</v>
-      </c>
-      <c r="J16" s="7" t="s">
-        <v>1027</v>
       </c>
       <c r="K16" s="7"/>
       <c r="L16" s="7"/>
@@ -25080,7 +25138,7 @@
       <c r="C18" s="111"/>
       <c r="D18" s="111"/>
       <c r="E18" s="112" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
       <c r="F18" s="112" t="s">
         <v>107</v>
@@ -25092,7 +25150,7 @@
         <v>26</v>
       </c>
       <c r="I18" s="112" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
       <c r="J18" s="113"/>
       <c r="K18" s="112"/>
@@ -25114,7 +25172,7 @@
       <c r="C19" s="111"/>
       <c r="D19" s="111"/>
       <c r="E19" s="112" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="F19" s="112" t="s">
         <v>107</v>
@@ -25126,7 +25184,7 @@
         <v>26</v>
       </c>
       <c r="I19" s="112" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="J19" s="113"/>
       <c r="K19" s="112"/>
@@ -25809,7 +25867,7 @@
     <row r="39" spans="1:26" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A39" s="28"/>
       <c r="E39" s="21" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="F39" s="47" t="s">
         <v>28</v>
@@ -25821,7 +25879,7 @@
         <v>26</v>
       </c>
       <c r="I39" s="21" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="40" spans="1:26" s="65" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
@@ -25993,7 +26051,7 @@
   <sheetData>
     <row r="1" spans="1:21" s="21" customFormat="1" ht="59.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="116" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="25" t="s">
@@ -26049,7 +26107,7 @@
         <v>225</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
       <c r="G2" s="10" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
CW3MdataDictionary.xlsx - Add WETL_VOL, the volume of standing water in a wetland IDU. FLOWreports_McKenzie.xml - Add 6 summary columns at the beginning of the Thermal Energy Budget report. Add WETL_VOL and Wetland ET_DAY at the end. IDU_McKenzie.dbf - Add WETL_VOL. Flow.cpp, .h - Change FlowModel::CalcTotH2OinReaches() and ...inReservoirs() to return WaterParcels instead of doubles. In FlowModel::Init(), during a coldstart initialize WETL_VOL to zero. In FlowModel::InitRun(), ...ReadState(), and ...StartYear(), write out temperatures as well as volumes for total water in reaches and reservoirs. In FlowModel::EndStep() calculate and store WETL_VOL based on WETNESS. In FlowModel::WriteDataToMap(), add logic to handle error returns from Evaporate(). WaterRights.cpp - Adjust for CalcTotH2OinReaches()'s new calling sequence. MapLayer.h - Add WETL_VOL.
</commit_message>
<xml_diff>
--- a/DataCW3M/CW3MdigitalHandbook/CW3MdataDictionary.xlsx
+++ b/DataCW3M/CW3MdigitalHandbook/CW3MdataDictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\CW3MdigitalHandbook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBB6889E-2C4E-40FD-8001-D44861D291CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{828968D3-0326-4268-BEC9-3C91C4CFAFD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-7425" windowWidth="29040" windowHeight="17520" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-7425" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Necessary input data" sheetId="7" r:id="rId1"/>
@@ -97,7 +97,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3193" uniqueCount="1078">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3193" uniqueCount="1079">
   <si>
     <t>LULC_A</t>
   </si>
@@ -2581,12 +2581,6 @@
     <t>WETL_VOL</t>
   </si>
   <si>
-    <t>current volume of water stored in the wetland</t>
-  </si>
-  <si>
-    <t>calculated in Flow?</t>
-  </si>
-  <si>
     <t>HRU_ID of HRU associated with this reach; reaches are assigned to HRUs in FlowModel::AssignReachesToHRUs().  Every reach should be assigned to a single HRU.  See also HRU_FRAC.</t>
   </si>
   <si>
@@ -3332,6 +3326,15 @@
   </si>
   <si>
     <t>lateral flow into the reach over and through the stream banks and stream bottom, from the precipitation-runoff model (HBV), excluding water from springs and floodwater</t>
+  </si>
+  <si>
+    <t>FlowModel::EndStep()</t>
+  </si>
+  <si>
+    <t>calculated in FlowModel::EndStep() from WETNESS.</t>
+  </si>
+  <si>
+    <t>current volume of standing water in a wetland</t>
   </si>
 </sst>
 </file>
@@ -3448,7 +3451,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="117">
+  <cellXfs count="118">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -3717,6 +3720,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -9342,9 +9348,9 @@
   </sheetPr>
   <dimension ref="A1:Z1060"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A164" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A240" sqref="A240"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A204" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H236" sqref="H236"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -11075,7 +11081,7 @@
       <c r="A50" s="28"/>
       <c r="B50" s="28"/>
       <c r="C50" s="7" t="s">
-        <v>1019</v>
+        <v>1017</v>
       </c>
       <c r="D50" s="10" t="s">
         <v>107</v>
@@ -11088,10 +11094,10 @@
         <v>29</v>
       </c>
       <c r="H50" s="25" t="s">
-        <v>1020</v>
+        <v>1018</v>
       </c>
       <c r="I50" s="27" t="s">
-        <v>1021</v>
+        <v>1019</v>
       </c>
       <c r="J50" s="3"/>
       <c r="K50" s="7"/>
@@ -11609,20 +11615,20 @@
       <c r="A67" s="28"/>
       <c r="B67" s="28"/>
       <c r="C67" s="7" t="s">
-        <v>1022</v>
+        <v>1020</v>
       </c>
       <c r="D67" s="10" t="s">
         <v>107</v>
       </c>
       <c r="E67" s="10" t="s">
-        <v>1023</v>
+        <v>1021</v>
       </c>
       <c r="F67" s="10"/>
       <c r="G67" s="10" t="s">
         <v>26</v>
       </c>
       <c r="H67" s="25" t="s">
-        <v>1024</v>
+        <v>1022</v>
       </c>
       <c r="I67" s="27"/>
       <c r="J67" s="3"/>
@@ -11683,7 +11689,7 @@
       </c>
       <c r="B69" s="28"/>
       <c r="C69" s="7" t="s">
-        <v>1049</v>
+        <v>1047</v>
       </c>
       <c r="D69" s="10" t="s">
         <v>107</v>
@@ -11694,7 +11700,7 @@
         <v>26</v>
       </c>
       <c r="H69" s="25" t="s">
-        <v>1050</v>
+        <v>1048</v>
       </c>
       <c r="I69" s="27" t="s">
         <v>112</v>
@@ -11718,7 +11724,7 @@
       </c>
       <c r="B70" s="28"/>
       <c r="C70" s="7" t="s">
-        <v>1051</v>
+        <v>1049</v>
       </c>
       <c r="D70" s="10" t="s">
         <v>107</v>
@@ -11729,7 +11735,7 @@
         <v>26</v>
       </c>
       <c r="H70" s="25" t="s">
-        <v>1052</v>
+        <v>1050</v>
       </c>
       <c r="I70" s="27" t="s">
         <v>112</v>
@@ -11908,7 +11914,7 @@
         <v>225</v>
       </c>
       <c r="F75" s="62" t="s">
-        <v>1047</v>
+        <v>1045</v>
       </c>
       <c r="G75" s="62" t="s">
         <v>26</v>
@@ -12784,11 +12790,11 @@
     </row>
     <row r="100" spans="1:26" s="21" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A100" s="28" t="s">
-        <v>1053</v>
+        <v>1051</v>
       </c>
       <c r="B100" s="28"/>
       <c r="C100" s="7" t="s">
-        <v>1054</v>
+        <v>1052</v>
       </c>
       <c r="D100" s="10" t="s">
         <v>28</v>
@@ -12799,7 +12805,7 @@
         <v>26</v>
       </c>
       <c r="H100" s="25" t="s">
-        <v>1057</v>
+        <v>1055</v>
       </c>
       <c r="I100" s="10" t="s">
         <v>112</v>
@@ -13008,16 +13014,16 @@
         <v>28</v>
       </c>
       <c r="E106" s="8" t="s">
-        <v>1032</v>
+        <v>1030</v>
       </c>
       <c r="F106" s="10" t="s">
-        <v>1033</v>
+        <v>1031</v>
       </c>
       <c r="G106" s="8" t="s">
         <v>26</v>
       </c>
       <c r="H106" s="57" t="s">
-        <v>1035</v>
+        <v>1033</v>
       </c>
       <c r="I106" s="27"/>
       <c r="J106" s="3"/>
@@ -13726,18 +13732,18 @@
       <c r="A127" s="28"/>
       <c r="B127" s="28"/>
       <c r="C127" s="7" t="s">
-        <v>870</v>
+        <v>868</v>
       </c>
       <c r="D127" s="10"/>
       <c r="E127" s="10" t="s">
-        <v>866</v>
+        <v>864</v>
       </c>
       <c r="F127" s="10" t="s">
-        <v>873</v>
+        <v>871</v>
       </c>
       <c r="G127" s="10"/>
       <c r="H127" s="25" t="s">
-        <v>883</v>
+        <v>881</v>
       </c>
       <c r="I127" s="27" t="s">
         <v>112</v>
@@ -13759,18 +13765,18 @@
       <c r="A128" s="28"/>
       <c r="B128" s="28"/>
       <c r="C128" s="7" t="s">
-        <v>865</v>
+        <v>863</v>
       </c>
       <c r="D128" s="10"/>
       <c r="E128" s="10" t="s">
-        <v>867</v>
+        <v>865</v>
       </c>
       <c r="F128" s="10" t="s">
-        <v>873</v>
+        <v>871</v>
       </c>
       <c r="G128" s="10"/>
       <c r="H128" s="25" t="s">
-        <v>886</v>
+        <v>884</v>
       </c>
       <c r="I128" s="27" t="s">
         <v>112</v>
@@ -13792,18 +13798,18 @@
       <c r="A129" s="28"/>
       <c r="B129" s="28"/>
       <c r="C129" s="7" t="s">
-        <v>871</v>
+        <v>869</v>
       </c>
       <c r="D129" s="10"/>
       <c r="E129" s="10" t="s">
-        <v>868</v>
+        <v>866</v>
       </c>
       <c r="F129" s="10" t="s">
-        <v>873</v>
+        <v>871</v>
       </c>
       <c r="G129" s="10"/>
       <c r="H129" s="25" t="s">
-        <v>885</v>
+        <v>883</v>
       </c>
       <c r="I129" s="27" t="s">
         <v>112</v>
@@ -13825,18 +13831,18 @@
       <c r="A130" s="28"/>
       <c r="B130" s="28"/>
       <c r="C130" s="7" t="s">
-        <v>872</v>
+        <v>870</v>
       </c>
       <c r="D130" s="10"/>
       <c r="E130" s="10" t="s">
-        <v>869</v>
+        <v>867</v>
       </c>
       <c r="F130" s="10" t="s">
-        <v>873</v>
+        <v>871</v>
       </c>
       <c r="G130" s="10"/>
       <c r="H130" s="25" t="s">
-        <v>884</v>
+        <v>882</v>
       </c>
       <c r="I130" s="27" t="s">
         <v>112</v>
@@ -13896,22 +13902,22 @@
     <row r="132" spans="1:26" s="21" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B132" s="28"/>
       <c r="C132" s="21" t="s">
-        <v>854</v>
+        <v>852</v>
       </c>
       <c r="D132" s="10" t="s">
         <v>28</v>
       </c>
       <c r="E132" s="10" t="s">
-        <v>866</v>
+        <v>864</v>
       </c>
       <c r="F132" s="10" t="s">
-        <v>858</v>
+        <v>856</v>
       </c>
       <c r="G132" s="10" t="s">
         <v>26</v>
       </c>
       <c r="H132" s="21" t="s">
-        <v>860</v>
+        <v>858</v>
       </c>
       <c r="I132" s="27" t="s">
         <v>112</v>
@@ -13921,22 +13927,22 @@
     <row r="133" spans="1:26" s="21" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B133" s="28"/>
       <c r="C133" s="21" t="s">
-        <v>855</v>
+        <v>853</v>
       </c>
       <c r="D133" s="10" t="s">
         <v>28</v>
       </c>
       <c r="E133" s="10" t="s">
-        <v>867</v>
+        <v>865</v>
       </c>
       <c r="F133" s="10" t="s">
-        <v>858</v>
+        <v>856</v>
       </c>
       <c r="G133" s="10" t="s">
         <v>26</v>
       </c>
       <c r="H133" s="21" t="s">
-        <v>874</v>
+        <v>872</v>
       </c>
       <c r="I133" s="27" t="s">
         <v>112</v>
@@ -13946,22 +13952,22 @@
     <row r="134" spans="1:26" s="21" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B134" s="28"/>
       <c r="C134" s="21" t="s">
-        <v>857</v>
+        <v>855</v>
       </c>
       <c r="D134" s="10" t="s">
         <v>28</v>
       </c>
       <c r="E134" s="10" t="s">
-        <v>868</v>
+        <v>866</v>
       </c>
       <c r="F134" s="10" t="s">
-        <v>858</v>
+        <v>856</v>
       </c>
       <c r="G134" s="10" t="s">
         <v>26</v>
       </c>
       <c r="H134" s="21" t="s">
-        <v>862</v>
+        <v>860</v>
       </c>
       <c r="I134" s="27" t="s">
         <v>112</v>
@@ -13971,22 +13977,22 @@
     <row r="135" spans="1:26" s="21" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B135" s="28"/>
       <c r="C135" s="21" t="s">
-        <v>856</v>
+        <v>854</v>
       </c>
       <c r="D135" s="10" t="s">
         <v>28</v>
       </c>
       <c r="E135" s="10" t="s">
-        <v>869</v>
+        <v>867</v>
       </c>
       <c r="F135" s="10" t="s">
-        <v>858</v>
+        <v>856</v>
       </c>
       <c r="G135" s="10" t="s">
         <v>26</v>
       </c>
       <c r="H135" s="21" t="s">
-        <v>861</v>
+        <v>859</v>
       </c>
       <c r="I135" s="27" t="s">
         <v>112</v>
@@ -13997,18 +14003,18 @@
       <c r="A136" s="10"/>
       <c r="B136" s="28"/>
       <c r="C136" s="21" t="s">
-        <v>863</v>
+        <v>861</v>
       </c>
       <c r="D136" s="10"/>
       <c r="E136" s="10" t="s">
-        <v>877</v>
+        <v>875</v>
       </c>
       <c r="F136" s="10" t="s">
-        <v>858</v>
+        <v>856</v>
       </c>
       <c r="G136" s="10"/>
       <c r="H136" s="21" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
       <c r="I136" s="27" t="s">
         <v>112</v>
@@ -14019,18 +14025,18 @@
       <c r="A137" s="10"/>
       <c r="B137" s="28"/>
       <c r="C137" s="21" t="s">
-        <v>864</v>
+        <v>862</v>
       </c>
       <c r="D137" s="10"/>
       <c r="E137" s="10" t="s">
-        <v>878</v>
+        <v>876</v>
       </c>
       <c r="F137" s="10" t="s">
-        <v>858</v>
+        <v>856</v>
       </c>
       <c r="G137" s="10"/>
       <c r="H137" s="21" t="s">
-        <v>876</v>
+        <v>874</v>
       </c>
       <c r="I137" s="27" t="s">
         <v>112</v>
@@ -14115,7 +14121,7 @@
       </c>
       <c r="D140" s="8"/>
       <c r="E140" s="10" t="s">
-        <v>879</v>
+        <v>877</v>
       </c>
       <c r="F140" s="10"/>
       <c r="G140" s="8" t="s">
@@ -14185,7 +14191,7 @@
       </c>
       <c r="D142" s="8"/>
       <c r="E142" s="10" t="s">
-        <v>880</v>
+        <v>878</v>
       </c>
       <c r="F142" s="10"/>
       <c r="G142" s="8" t="s">
@@ -15424,7 +15430,7 @@
         <v>26</v>
       </c>
       <c r="H175" s="60" t="s">
-        <v>1034</v>
+        <v>1032</v>
       </c>
       <c r="I175" s="67" t="s">
         <v>811</v>
@@ -15435,7 +15441,7 @@
       <c r="A176" s="13"/>
       <c r="B176" s="13"/>
       <c r="C176" s="25" t="s">
-        <v>1039</v>
+        <v>1037</v>
       </c>
       <c r="D176" s="9" t="s">
         <v>107</v>
@@ -15450,7 +15456,7 @@
         <v>26</v>
       </c>
       <c r="H176" s="72" t="s">
-        <v>1046</v>
+        <v>1044</v>
       </c>
       <c r="I176" s="46" t="s">
         <v>811</v>
@@ -15658,7 +15664,7 @@
         <v>28</v>
       </c>
       <c r="E182" s="27" t="s">
-        <v>1017</v>
+        <v>1015</v>
       </c>
       <c r="F182" s="27" t="s">
         <v>33</v>
@@ -15753,7 +15759,7 @@
     </row>
     <row r="185" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A185" s="13" t="s">
-        <v>1058</v>
+        <v>1056</v>
       </c>
       <c r="B185" s="6"/>
       <c r="C185" s="18" t="s">
@@ -15773,7 +15779,7 @@
         <v>637</v>
       </c>
       <c r="I185" s="10" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="J185" s="3"/>
       <c r="K185" s="7"/>
@@ -16271,7 +16277,7 @@
       <c r="A201" s="28"/>
       <c r="B201" s="28"/>
       <c r="C201" s="7" t="s">
-        <v>1037</v>
+        <v>1035</v>
       </c>
       <c r="D201" s="70" t="s">
         <v>107</v>
@@ -16284,7 +16290,7 @@
         <v>26</v>
       </c>
       <c r="H201" s="57" t="s">
-        <v>1038</v>
+        <v>1036</v>
       </c>
       <c r="I201" s="10"/>
       <c r="J201" s="3"/>
@@ -16403,7 +16409,7 @@
       <c r="A205" s="28"/>
       <c r="B205" s="28"/>
       <c r="C205" s="21" t="s">
-        <v>882</v>
+        <v>880</v>
       </c>
       <c r="D205" s="10" t="s">
         <v>28</v>
@@ -16412,11 +16418,11 @@
         <v>127</v>
       </c>
       <c r="F205" s="10" t="s">
-        <v>873</v>
+        <v>871</v>
       </c>
       <c r="G205" s="10"/>
       <c r="H205" s="25" t="s">
-        <v>887</v>
+        <v>885</v>
       </c>
       <c r="I205" s="27"/>
       <c r="J205" s="3"/>
@@ -16434,7 +16440,7 @@
     <row r="206" spans="1:21" s="21" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B206" s="28"/>
       <c r="C206" s="21" t="s">
-        <v>859</v>
+        <v>857</v>
       </c>
       <c r="D206" s="10" t="s">
         <v>28</v>
@@ -16443,13 +16449,13 @@
         <v>127</v>
       </c>
       <c r="F206" s="10" t="s">
-        <v>858</v>
+        <v>856</v>
       </c>
       <c r="G206" s="10" t="s">
         <v>26</v>
       </c>
       <c r="H206" s="25" t="s">
-        <v>881</v>
+        <v>879</v>
       </c>
       <c r="I206" s="27" t="s">
         <v>112</v>
@@ -16970,11 +16976,11 @@
     </row>
     <row r="222" spans="1:21" s="21" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A222" s="28" t="s">
-        <v>1053</v>
+        <v>1051</v>
       </c>
       <c r="B222" s="28"/>
       <c r="C222" s="7" t="s">
-        <v>1055</v>
+        <v>1053</v>
       </c>
       <c r="D222" s="10" t="s">
         <v>28</v>
@@ -16985,7 +16991,7 @@
         <v>26</v>
       </c>
       <c r="H222" s="25" t="s">
-        <v>1056</v>
+        <v>1054</v>
       </c>
       <c r="I222" s="27" t="s">
         <v>112</v>
@@ -17283,20 +17289,20 @@
       <c r="A231" s="28"/>
       <c r="B231" s="28"/>
       <c r="C231" s="7" t="s">
-        <v>1060</v>
+        <v>1058</v>
       </c>
       <c r="D231" s="10" t="s">
         <v>107</v>
       </c>
       <c r="E231" s="10" t="s">
-        <v>985</v>
+        <v>983</v>
       </c>
       <c r="F231" s="10"/>
       <c r="G231" s="10" t="s">
         <v>26</v>
       </c>
       <c r="H231" s="57" t="s">
-        <v>1064</v>
+        <v>1062</v>
       </c>
       <c r="I231" s="27"/>
       <c r="J231" s="3"/>
@@ -17316,20 +17322,20 @@
       <c r="A232" s="28"/>
       <c r="B232" s="28"/>
       <c r="C232" s="7" t="s">
-        <v>1061</v>
+        <v>1059</v>
       </c>
       <c r="D232" s="10" t="s">
         <v>107</v>
       </c>
       <c r="E232" s="10" t="s">
-        <v>1023</v>
+        <v>1021</v>
       </c>
       <c r="F232" s="10"/>
       <c r="G232" s="10" t="s">
         <v>26</v>
       </c>
       <c r="H232" s="57" t="s">
-        <v>1065</v>
+        <v>1063</v>
       </c>
       <c r="I232" s="27"/>
       <c r="J232" s="3"/>
@@ -17384,7 +17390,7 @@
       <c r="A234" s="28"/>
       <c r="B234" s="28"/>
       <c r="C234" s="7" t="s">
-        <v>1001</v>
+        <v>999</v>
       </c>
       <c r="D234" s="10" t="s">
         <v>45</v>
@@ -17395,7 +17401,7 @@
         <v>29</v>
       </c>
       <c r="H234" s="25" t="s">
-        <v>1002</v>
+        <v>1000</v>
       </c>
       <c r="I234" s="27"/>
       <c r="J234" s="3"/>
@@ -17411,48 +17417,48 @@
       <c r="T234" s="7"/>
       <c r="U234" s="7"/>
     </row>
-    <row r="235" spans="1:21" s="65" customFormat="1" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A235" s="66"/>
-      <c r="B235" s="66"/>
-      <c r="C235" s="64" t="s">
+    <row r="235" spans="1:21" s="91" customFormat="1" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A235" s="96"/>
+      <c r="B235" s="96"/>
+      <c r="C235" s="97" t="s">
         <v>826</v>
       </c>
-      <c r="D235" s="62" t="s">
+      <c r="D235" s="100" t="s">
         <v>28</v>
       </c>
-      <c r="E235" s="62" t="s">
+      <c r="E235" s="100" t="s">
         <v>93</v>
       </c>
-      <c r="F235" s="62" t="s">
-        <v>64</v>
-      </c>
-      <c r="G235" s="62" t="s">
+      <c r="F235" s="99" t="s">
+        <v>1076</v>
+      </c>
+      <c r="G235" s="100" t="s">
         <v>26</v>
       </c>
-      <c r="H235" s="61" t="s">
-        <v>827</v>
-      </c>
-      <c r="I235" s="74" t="s">
-        <v>828</v>
-      </c>
-      <c r="J235" s="68"/>
-      <c r="K235" s="64"/>
-      <c r="L235" s="64"/>
-      <c r="M235" s="64"/>
-      <c r="N235" s="64"/>
-      <c r="O235" s="64"/>
-      <c r="P235" s="64"/>
-      <c r="Q235" s="64"/>
-      <c r="R235" s="64"/>
-      <c r="S235" s="64"/>
-      <c r="T235" s="64"/>
-      <c r="U235" s="64"/>
+      <c r="H235" s="117" t="s">
+        <v>1078</v>
+      </c>
+      <c r="I235" s="98" t="s">
+        <v>1077</v>
+      </c>
+      <c r="J235" s="84"/>
+      <c r="K235" s="97"/>
+      <c r="L235" s="97"/>
+      <c r="M235" s="97"/>
+      <c r="N235" s="97"/>
+      <c r="O235" s="97"/>
+      <c r="P235" s="97"/>
+      <c r="Q235" s="97"/>
+      <c r="R235" s="97"/>
+      <c r="S235" s="97"/>
+      <c r="T235" s="97"/>
+      <c r="U235" s="97"/>
     </row>
     <row r="236" spans="1:21" s="91" customFormat="1" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A236" s="96"/>
       <c r="B236" s="96"/>
       <c r="C236" s="97" t="s">
-        <v>993</v>
+        <v>991</v>
       </c>
       <c r="D236" s="100" t="s">
         <v>107</v>
@@ -17465,7 +17471,7 @@
         <v>26</v>
       </c>
       <c r="H236" s="91" t="s">
-        <v>994</v>
+        <v>992</v>
       </c>
       <c r="I236" s="98"/>
       <c r="J236" s="84"/>
@@ -17485,22 +17491,22 @@
       <c r="A237" s="96"/>
       <c r="B237" s="96"/>
       <c r="C237" s="97" t="s">
-        <v>1066</v>
+        <v>1064</v>
       </c>
       <c r="D237" s="99" t="s">
         <v>45</v>
       </c>
       <c r="E237" s="99" t="s">
-        <v>1063</v>
+        <v>1061</v>
       </c>
       <c r="F237" s="100" t="s">
-        <v>1067</v>
+        <v>1065</v>
       </c>
       <c r="G237" s="99" t="s">
         <v>26</v>
       </c>
       <c r="H237" s="99" t="s">
-        <v>1068</v>
+        <v>1066</v>
       </c>
       <c r="I237" s="98"/>
       <c r="J237" s="84"/>
@@ -17520,20 +17526,20 @@
       <c r="A238" s="96"/>
       <c r="B238" s="96"/>
       <c r="C238" s="97" t="s">
-        <v>1062</v>
+        <v>1060</v>
       </c>
       <c r="D238" s="100" t="s">
         <v>107</v>
       </c>
       <c r="E238" s="100" t="s">
-        <v>1063</v>
+        <v>1061</v>
       </c>
       <c r="F238" s="100"/>
       <c r="G238" s="100" t="s">
         <v>26</v>
       </c>
       <c r="H238" s="57" t="s">
-        <v>1069</v>
+        <v>1067</v>
       </c>
       <c r="I238" s="98"/>
       <c r="J238" s="84"/>
@@ -17553,7 +17559,7 @@
       <c r="A239" s="96"/>
       <c r="B239" s="96"/>
       <c r="C239" s="97" t="s">
-        <v>981</v>
+        <v>979</v>
       </c>
       <c r="D239" s="99" t="s">
         <v>107</v>
@@ -17568,7 +17574,7 @@
         <v>26</v>
       </c>
       <c r="H239" s="77" t="s">
-        <v>982</v>
+        <v>980</v>
       </c>
       <c r="I239" s="98"/>
       <c r="J239" s="84"/>
@@ -21498,8 +21504,8 @@
   </sheetPr>
   <dimension ref="A1:Z120"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="K37" sqref="K37"/>
     </sheetView>
   </sheetViews>
@@ -21547,7 +21553,7 @@
     </row>
     <row r="2" spans="1:26" s="57" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="70" t="s">
-        <v>1076</v>
+        <v>1074</v>
       </c>
       <c r="B2" s="69"/>
       <c r="C2" s="69"/>
@@ -21575,7 +21581,7 @@
     </row>
     <row r="3" spans="1:26" s="91" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="87" t="s">
-        <v>950</v>
+        <v>948</v>
       </c>
       <c r="B3" s="88"/>
       <c r="C3" s="89"/>
@@ -21663,7 +21669,7 @@
       <c r="C5" s="13"/>
       <c r="D5" s="13"/>
       <c r="E5" s="72" t="s">
-        <v>918</v>
+        <v>916</v>
       </c>
       <c r="F5" s="10"/>
       <c r="G5" s="70" t="s">
@@ -21679,7 +21685,7 @@
         <v>26</v>
       </c>
       <c r="K5" s="57" t="s">
-        <v>920</v>
+        <v>918</v>
       </c>
       <c r="L5" s="9"/>
       <c r="M5" s="25"/>
@@ -21701,7 +21707,7 @@
       <c r="C6" s="13"/>
       <c r="D6" s="13"/>
       <c r="E6" s="72" t="s">
-        <v>919</v>
+        <v>917</v>
       </c>
       <c r="F6" s="10"/>
       <c r="G6" s="70" t="s">
@@ -21717,7 +21723,7 @@
         <v>26</v>
       </c>
       <c r="K6" s="57" t="s">
-        <v>1036</v>
+        <v>1034</v>
       </c>
       <c r="L6" s="9"/>
       <c r="M6" s="25"/>
@@ -21739,7 +21745,7 @@
       <c r="C7" s="13"/>
       <c r="D7" s="13"/>
       <c r="E7" s="72" t="s">
-        <v>921</v>
+        <v>919</v>
       </c>
       <c r="F7" s="10"/>
       <c r="G7" s="70" t="s">
@@ -21755,7 +21761,7 @@
         <v>26</v>
       </c>
       <c r="K7" s="70" t="s">
-        <v>922</v>
+        <v>920</v>
       </c>
       <c r="L7" s="9"/>
       <c r="M7" s="25"/>
@@ -21775,10 +21781,10 @@
       <c r="A8" s="82"/>
       <c r="B8" s="82"/>
       <c r="D8" s="84" t="s">
-        <v>890</v>
+        <v>888</v>
       </c>
       <c r="E8" s="84" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
       <c r="F8" s="84">
         <v>5.2</v>
@@ -21794,7 +21800,7 @@
         <v>26</v>
       </c>
       <c r="K8" s="83" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
     </row>
     <row r="9" spans="1:26" s="21" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -21802,19 +21808,19 @@
       <c r="B9" s="20"/>
       <c r="C9" s="22"/>
       <c r="E9" s="21" t="s">
-        <v>888</v>
+        <v>886</v>
       </c>
       <c r="G9" s="21" t="s">
         <v>45</v>
       </c>
       <c r="H9" s="21" t="s">
-        <v>891</v>
+        <v>889</v>
       </c>
       <c r="J9" s="23" t="s">
         <v>29</v>
       </c>
       <c r="K9" s="80" t="s">
-        <v>892</v>
+        <v>890</v>
       </c>
       <c r="L9" s="22"/>
     </row>
@@ -21823,19 +21829,19 @@
       <c r="B10" s="20"/>
       <c r="C10" s="22"/>
       <c r="E10" s="21" t="s">
-        <v>889</v>
+        <v>887</v>
       </c>
       <c r="G10" s="21" t="s">
         <v>45</v>
       </c>
       <c r="H10" s="21" t="s">
-        <v>891</v>
+        <v>889</v>
       </c>
       <c r="J10" s="23" t="s">
         <v>29</v>
       </c>
       <c r="K10" s="80" t="s">
-        <v>958</v>
+        <v>956</v>
       </c>
       <c r="L10" s="22"/>
     </row>
@@ -21844,10 +21850,10 @@
       <c r="B11" s="92"/>
       <c r="C11" s="93"/>
       <c r="D11" s="76" t="s">
-        <v>936</v>
+        <v>934</v>
       </c>
       <c r="E11" s="76" t="s">
-        <v>937</v>
+        <v>935</v>
       </c>
       <c r="F11" s="65">
         <v>36</v>
@@ -21859,16 +21865,16 @@
         <v>225</v>
       </c>
       <c r="I11" s="76" t="s">
+        <v>937</v>
+      </c>
+      <c r="J11" s="94" t="s">
+        <v>936</v>
+      </c>
+      <c r="K11" s="95" t="s">
+        <v>938</v>
+      </c>
+      <c r="L11" s="94" t="s">
         <v>939</v>
-      </c>
-      <c r="J11" s="94" t="s">
-        <v>938</v>
-      </c>
-      <c r="K11" s="95" t="s">
-        <v>940</v>
-      </c>
-      <c r="L11" s="94" t="s">
-        <v>941</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
@@ -22027,7 +22033,7 @@
       <c r="B20" s="20"/>
       <c r="D20" s="3"/>
       <c r="E20" s="7" t="s">
-        <v>840</v>
+        <v>838</v>
       </c>
       <c r="F20" s="7">
         <v>1</v>
@@ -22045,7 +22051,7 @@
         <v>26</v>
       </c>
       <c r="K20" s="21" t="s">
-        <v>841</v>
+        <v>839</v>
       </c>
     </row>
     <row r="21" spans="1:26" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
@@ -22053,7 +22059,7 @@
       <c r="B21" s="20"/>
       <c r="D21" s="3"/>
       <c r="E21" s="7" t="s">
-        <v>956</v>
+        <v>954</v>
       </c>
       <c r="F21" s="7"/>
       <c r="G21" s="7" t="s">
@@ -22069,7 +22075,7 @@
         <v>26</v>
       </c>
       <c r="K21" s="21" t="s">
-        <v>957</v>
+        <v>955</v>
       </c>
     </row>
     <row r="22" spans="1:26" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
@@ -22077,7 +22083,7 @@
       <c r="B22" s="20"/>
       <c r="D22" s="3"/>
       <c r="E22" s="7" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
       <c r="F22" s="7">
         <v>90</v>
@@ -22086,13 +22092,13 @@
         <v>107</v>
       </c>
       <c r="H22" s="7" t="s">
-        <v>894</v>
+        <v>892</v>
       </c>
       <c r="J22" s="21" t="s">
         <v>29</v>
       </c>
       <c r="K22" s="21" t="s">
-        <v>895</v>
+        <v>893</v>
       </c>
     </row>
     <row r="23" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
@@ -22158,7 +22164,7 @@
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
       <c r="E25" s="7" t="s">
-        <v>846</v>
+        <v>844</v>
       </c>
       <c r="F25" s="7">
         <v>4.2</v>
@@ -22176,7 +22182,7 @@
         <v>26</v>
       </c>
       <c r="K25" s="3" t="s">
-        <v>845</v>
+        <v>843</v>
       </c>
       <c r="N25" s="3"/>
     </row>
@@ -22188,7 +22194,7 @@
         <v>23</v>
       </c>
       <c r="D26" t="s">
-        <v>901</v>
+        <v>899</v>
       </c>
       <c r="E26" s="7" t="s">
         <v>49</v>
@@ -22197,18 +22203,18 @@
         <v>0</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
       <c r="H26" s="7"/>
       <c r="K26" s="23" t="s">
-        <v>900</v>
+        <v>898</v>
       </c>
     </row>
     <row r="27" spans="1:26" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A27" s="20"/>
       <c r="B27" s="20"/>
       <c r="E27" s="7" t="s">
-        <v>1074</v>
+        <v>1072</v>
       </c>
       <c r="F27" s="7"/>
       <c r="G27" s="7" t="s">
@@ -22224,14 +22230,14 @@
         <v>26</v>
       </c>
       <c r="K27" s="23" t="s">
-        <v>1075</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="28" spans="1:26" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A28" s="20"/>
       <c r="B28" s="20"/>
       <c r="E28" s="7" t="s">
-        <v>1072</v>
+        <v>1070</v>
       </c>
       <c r="F28" s="7"/>
       <c r="G28" s="7" t="s">
@@ -22247,7 +22253,7 @@
         <v>26</v>
       </c>
       <c r="K28" s="23" t="s">
-        <v>1073</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="29" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
@@ -22328,7 +22334,7 @@
         <v>29</v>
       </c>
       <c r="K32" s="80" t="s">
-        <v>829</v>
+        <v>827</v>
       </c>
       <c r="L32" s="19"/>
       <c r="M32" s="19"/>
@@ -22432,7 +22438,7 @@
       <c r="B36" s="20"/>
       <c r="D36" s="22"/>
       <c r="E36" s="21" t="s">
-        <v>851</v>
+        <v>849</v>
       </c>
       <c r="F36" s="7"/>
       <c r="G36" s="57" t="s">
@@ -22448,7 +22454,7 @@
         <v>26</v>
       </c>
       <c r="K36" s="23" t="s">
-        <v>1077</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="37" spans="1:12" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
@@ -22456,7 +22462,7 @@
       <c r="B37" s="20"/>
       <c r="D37" s="22"/>
       <c r="E37" s="21" t="s">
-        <v>897</v>
+        <v>895</v>
       </c>
       <c r="F37" s="7"/>
       <c r="G37" s="57" t="s">
@@ -22472,7 +22478,7 @@
         <v>26</v>
       </c>
       <c r="K37" s="23" t="s">
-        <v>898</v>
+        <v>896</v>
       </c>
     </row>
     <row r="38" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
@@ -22595,14 +22601,14 @@
       <c r="A43" s="20"/>
       <c r="B43" s="20"/>
       <c r="E43" s="7" t="s">
-        <v>976</v>
+        <v>974</v>
       </c>
       <c r="F43" s="7"/>
       <c r="G43" s="21" t="s">
         <v>107</v>
       </c>
       <c r="H43" s="21" t="s">
-        <v>978</v>
+        <v>976</v>
       </c>
       <c r="I43" s="21" t="s">
         <v>25</v>
@@ -22611,7 +22617,7 @@
         <v>26</v>
       </c>
       <c r="K43" s="23" t="s">
-        <v>977</v>
+        <v>975</v>
       </c>
     </row>
     <row r="44" spans="1:12" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
@@ -22627,7 +22633,7 @@
         <v>107</v>
       </c>
       <c r="H44" s="21" t="s">
-        <v>960</v>
+        <v>958</v>
       </c>
       <c r="I44" s="21" t="s">
         <v>25</v>
@@ -22636,21 +22642,21 @@
         <v>26</v>
       </c>
       <c r="K44" s="23" t="s">
-        <v>959</v>
+        <v>957</v>
       </c>
     </row>
     <row r="45" spans="1:12" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A45" s="20"/>
       <c r="B45" s="20"/>
       <c r="E45" s="7" t="s">
-        <v>963</v>
+        <v>961</v>
       </c>
       <c r="F45" s="7"/>
       <c r="G45" s="21" t="s">
         <v>107</v>
       </c>
       <c r="H45" s="21" t="s">
-        <v>960</v>
+        <v>958</v>
       </c>
       <c r="I45" s="21" t="s">
         <v>25</v>
@@ -22659,10 +22665,10 @@
         <v>26</v>
       </c>
       <c r="K45" s="23" t="s">
-        <v>959</v>
+        <v>957</v>
       </c>
       <c r="L45" s="21" t="s">
-        <v>964</v>
+        <v>962</v>
       </c>
     </row>
     <row r="46" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
@@ -22719,18 +22725,18 @@
       <c r="B48" s="20"/>
       <c r="D48" s="3"/>
       <c r="E48" s="7" t="s">
-        <v>997</v>
+        <v>995</v>
       </c>
       <c r="F48" s="7"/>
       <c r="G48" s="7"/>
       <c r="H48" s="7" t="s">
-        <v>998</v>
+        <v>996</v>
       </c>
       <c r="I48" s="21" t="s">
         <v>25</v>
       </c>
       <c r="K48" s="23" t="s">
-        <v>999</v>
+        <v>997</v>
       </c>
     </row>
     <row r="49" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
@@ -22741,7 +22747,7 @@
         <v>23</v>
       </c>
       <c r="D49" t="s">
-        <v>901</v>
+        <v>899</v>
       </c>
       <c r="E49" s="7" t="s">
         <v>86</v>
@@ -22750,11 +22756,11 @@
         <v>0</v>
       </c>
       <c r="G49" s="7" t="s">
-        <v>902</v>
+        <v>900</v>
       </c>
       <c r="H49" s="7"/>
       <c r="K49" s="23" t="s">
-        <v>903</v>
+        <v>901</v>
       </c>
     </row>
     <row r="50" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
@@ -22817,7 +22823,7 @@
         <v>799</v>
       </c>
       <c r="E52" s="7" t="s">
-        <v>923</v>
+        <v>921</v>
       </c>
       <c r="F52" s="7"/>
       <c r="G52" s="7" t="s">
@@ -22833,7 +22839,7 @@
         <v>26</v>
       </c>
       <c r="K52" s="57" t="s">
-        <v>924</v>
+        <v>922</v>
       </c>
     </row>
     <row r="53" spans="1:11" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
@@ -22841,7 +22847,7 @@
       <c r="B53" s="20"/>
       <c r="D53" s="3"/>
       <c r="E53" s="7" t="s">
-        <v>1070</v>
+        <v>1068</v>
       </c>
       <c r="F53" s="7"/>
       <c r="G53" s="7" t="s">
@@ -22857,7 +22863,7 @@
         <v>26</v>
       </c>
       <c r="K53" s="57" t="s">
-        <v>1071</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="54" spans="1:11" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
@@ -22905,7 +22911,7 @@
       <c r="I55" s="57"/>
       <c r="J55" s="57"/>
       <c r="K55" s="57" t="s">
-        <v>932</v>
+        <v>930</v>
       </c>
     </row>
     <row r="56" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
@@ -22916,7 +22922,7 @@
         <v>23</v>
       </c>
       <c r="E56" s="7" t="s">
-        <v>996</v>
+        <v>994</v>
       </c>
       <c r="F56" s="7">
         <v>0</v>
@@ -22931,14 +22937,14 @@
         <v>25</v>
       </c>
       <c r="K56" s="57" t="s">
-        <v>995</v>
+        <v>993</v>
       </c>
     </row>
     <row r="57" spans="1:11" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A57" s="20"/>
       <c r="B57" s="20"/>
       <c r="E57" s="7" t="s">
-        <v>983</v>
+        <v>981</v>
       </c>
       <c r="F57" s="7"/>
       <c r="G57" s="21" t="s">
@@ -22954,7 +22960,7 @@
         <v>29</v>
       </c>
       <c r="K57" s="57" t="s">
-        <v>984</v>
+        <v>982</v>
       </c>
     </row>
     <row r="58" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
@@ -22980,7 +22986,7 @@
       <c r="A59" s="20"/>
       <c r="B59" s="20"/>
       <c r="E59" s="7" t="s">
-        <v>852</v>
+        <v>850</v>
       </c>
       <c r="F59" s="7">
         <v>0.08</v>
@@ -22998,21 +23004,21 @@
         <v>29</v>
       </c>
       <c r="K59" s="23" t="s">
-        <v>853</v>
+        <v>851</v>
       </c>
     </row>
     <row r="60" spans="1:11" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A60" s="20"/>
       <c r="B60" s="20"/>
       <c r="E60" s="58" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
       <c r="F60" s="7"/>
       <c r="G60" s="7" t="s">
         <v>107</v>
       </c>
       <c r="H60" s="7" t="s">
-        <v>985</v>
+        <v>983</v>
       </c>
       <c r="I60" s="21" t="s">
         <v>33</v>
@@ -23021,14 +23027,14 @@
         <v>29</v>
       </c>
       <c r="K60" s="23" t="s">
-        <v>986</v>
+        <v>984</v>
       </c>
     </row>
     <row r="61" spans="1:11" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A61" s="20"/>
       <c r="B61" s="20"/>
       <c r="E61" s="58" t="s">
-        <v>991</v>
+        <v>989</v>
       </c>
       <c r="F61" s="7"/>
       <c r="G61" s="7" t="s">
@@ -23044,14 +23050,14 @@
         <v>26</v>
       </c>
       <c r="K61" s="23" t="s">
-        <v>992</v>
+        <v>990</v>
       </c>
     </row>
     <row r="62" spans="1:11" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A62" s="20"/>
       <c r="B62" s="20"/>
       <c r="E62" s="58" t="s">
-        <v>834</v>
+        <v>832</v>
       </c>
       <c r="F62" s="7"/>
       <c r="G62" s="7" t="s">
@@ -23064,7 +23070,7 @@
         <v>25</v>
       </c>
       <c r="K62" s="23" t="s">
-        <v>835</v>
+        <v>833</v>
       </c>
     </row>
     <row r="63" spans="1:11" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
@@ -23079,14 +23085,14 @@
         <v>473</v>
       </c>
       <c r="K63" s="23" t="s">
-        <v>934</v>
+        <v>932</v>
       </c>
     </row>
     <row r="64" spans="1:11" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A64" s="20"/>
       <c r="B64" s="20"/>
       <c r="E64" s="58" t="s">
-        <v>979</v>
+        <v>977</v>
       </c>
       <c r="F64" s="7"/>
       <c r="G64" s="7" t="s">
@@ -23102,14 +23108,14 @@
         <v>26</v>
       </c>
       <c r="K64" s="23" t="s">
-        <v>980</v>
+        <v>978</v>
       </c>
     </row>
     <row r="65" spans="1:24" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A65" s="20"/>
       <c r="B65" s="20"/>
       <c r="E65" s="7" t="s">
-        <v>833</v>
+        <v>831</v>
       </c>
       <c r="F65" s="7"/>
       <c r="G65" s="7" t="s">
@@ -23122,14 +23128,14 @@
         <v>25</v>
       </c>
       <c r="K65" s="23" t="s">
-        <v>847</v>
+        <v>845</v>
       </c>
     </row>
     <row r="66" spans="1:24" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A66" s="20"/>
       <c r="B66" s="20"/>
       <c r="E66" s="7" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
       <c r="F66" s="7"/>
       <c r="G66" s="7" t="s">
@@ -23142,7 +23148,7 @@
         <v>33</v>
       </c>
       <c r="K66" s="23" t="s">
-        <v>955</v>
+        <v>953</v>
       </c>
     </row>
     <row r="67" spans="1:24" ht="14.4" x14ac:dyDescent="0.3">
@@ -23184,7 +23190,7 @@
       <c r="C68" s="22"/>
       <c r="D68" s="22"/>
       <c r="E68" s="21" t="s">
-        <v>1000</v>
+        <v>998</v>
       </c>
       <c r="F68" s="7"/>
       <c r="G68" s="21" t="s">
@@ -23200,7 +23206,7 @@
         <v>29</v>
       </c>
       <c r="K68" s="23" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="69" spans="1:24" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
@@ -23211,14 +23217,14 @@
       <c r="C69" s="22"/>
       <c r="D69" s="22"/>
       <c r="E69" s="21" t="s">
-        <v>909</v>
+        <v>907</v>
       </c>
       <c r="F69" s="7"/>
       <c r="G69" s="21" t="s">
         <v>107</v>
       </c>
       <c r="H69" s="21" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="I69" s="23" t="s">
         <v>25</v>
@@ -23227,7 +23233,7 @@
         <v>26</v>
       </c>
       <c r="K69" s="23" t="s">
-        <v>904</v>
+        <v>902</v>
       </c>
     </row>
     <row r="70" spans="1:24" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
@@ -23236,7 +23242,7 @@
       <c r="C70" s="22"/>
       <c r="D70" s="22"/>
       <c r="E70" s="21" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
       <c r="F70" s="7"/>
       <c r="G70" s="21" t="s">
@@ -23252,7 +23258,7 @@
         <v>26</v>
       </c>
       <c r="K70" s="23" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
     </row>
     <row r="71" spans="1:24" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
@@ -23263,7 +23269,7 @@
       <c r="C71" s="22"/>
       <c r="D71" s="22"/>
       <c r="E71" s="21" t="s">
-        <v>905</v>
+        <v>903</v>
       </c>
       <c r="F71" s="7"/>
       <c r="G71" s="21" t="s">
@@ -23279,7 +23285,7 @@
         <v>26</v>
       </c>
       <c r="K71" s="23" t="s">
-        <v>906</v>
+        <v>904</v>
       </c>
     </row>
     <row r="72" spans="1:24" ht="43.2" x14ac:dyDescent="0.3">
@@ -23312,7 +23318,7 @@
       <c r="A73" s="20"/>
       <c r="B73" s="20"/>
       <c r="E73" s="7" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="G73" s="21" t="s">
         <v>107</v>
@@ -23327,7 +23333,7 @@
         <v>29</v>
       </c>
       <c r="K73" s="23" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
     </row>
     <row r="74" spans="1:24" s="25" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
@@ -23352,14 +23358,14 @@
         <v>29</v>
       </c>
       <c r="K74" s="80" t="s">
-        <v>925</v>
+        <v>923</v>
       </c>
     </row>
     <row r="75" spans="1:24" s="25" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A75" s="81"/>
       <c r="B75" s="81"/>
       <c r="E75" s="72" t="s">
-        <v>916</v>
+        <v>914</v>
       </c>
       <c r="G75" s="72" t="s">
         <v>107</v>
@@ -23374,7 +23380,7 @@
         <v>26</v>
       </c>
       <c r="K75" s="23" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
     </row>
     <row r="76" spans="1:24" s="25" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -23383,7 +23389,7 @@
         <v>22</v>
       </c>
       <c r="E76" s="25" t="s">
-        <v>907</v>
+        <v>905</v>
       </c>
       <c r="G76" s="25" t="s">
         <v>107</v>
@@ -23396,7 +23402,7 @@
       </c>
       <c r="J76" s="19"/>
       <c r="K76" s="80" t="s">
-        <v>908</v>
+        <v>906</v>
       </c>
     </row>
     <row r="77" spans="1:24" s="21" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -23441,14 +23447,14 @@
       <c r="C78" s="28"/>
       <c r="D78" s="28"/>
       <c r="E78" s="25" t="s">
-        <v>988</v>
+        <v>986</v>
       </c>
       <c r="F78" s="7"/>
       <c r="G78" s="70" t="s">
         <v>107</v>
       </c>
       <c r="H78" s="70" t="s">
-        <v>989</v>
+        <v>987</v>
       </c>
       <c r="I78" s="70" t="s">
         <v>33</v>
@@ -23457,7 +23463,7 @@
         <v>29</v>
       </c>
       <c r="K78" s="70" t="s">
-        <v>990</v>
+        <v>988</v>
       </c>
       <c r="L78" s="70"/>
       <c r="M78" s="3"/>
@@ -23493,17 +23499,17 @@
       <c r="A80" s="20"/>
       <c r="B80" s="20"/>
       <c r="E80" s="25" t="s">
-        <v>973</v>
+        <v>971</v>
       </c>
       <c r="F80" s="7" t="s">
-        <v>974</v>
+        <v>972</v>
       </c>
       <c r="G80" s="25" t="s">
         <v>69</v>
       </c>
       <c r="H80" s="7"/>
       <c r="K80" s="21" t="s">
-        <v>975</v>
+        <v>973</v>
       </c>
     </row>
     <row r="81" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
@@ -23577,7 +23583,7 @@
       <c r="A83" s="20"/>
       <c r="B83" s="20"/>
       <c r="E83" s="7" t="s">
-        <v>951</v>
+        <v>949</v>
       </c>
       <c r="F83" s="7"/>
       <c r="G83" s="7" t="s">
@@ -23604,14 +23610,14 @@
       <c r="G84" s="7"/>
       <c r="H84" s="7"/>
       <c r="K84" s="3" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
     </row>
     <row r="85" spans="1:26" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A85" s="20"/>
       <c r="B85" s="20"/>
       <c r="E85" s="7" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
       <c r="F85" s="7"/>
       <c r="G85" s="7" t="s">
@@ -23627,17 +23633,17 @@
         <v>29</v>
       </c>
       <c r="K85" s="21" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
       <c r="L85" s="3" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
     </row>
     <row r="86" spans="1:26" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A86" s="20"/>
       <c r="B86" s="20"/>
       <c r="E86" s="7" t="s">
-        <v>911</v>
+        <v>909</v>
       </c>
       <c r="F86" s="7"/>
       <c r="G86" s="7" t="s">
@@ -23653,10 +23659,10 @@
         <v>29</v>
       </c>
       <c r="K86" s="21" t="s">
-        <v>896</v>
+        <v>894</v>
       </c>
       <c r="L86" s="3" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
     </row>
     <row r="87" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
@@ -23760,7 +23766,7 @@
       <c r="B91" s="20"/>
       <c r="C91" s="3"/>
       <c r="E91" s="7" t="s">
-        <v>926</v>
+        <v>924</v>
       </c>
       <c r="F91" s="7"/>
       <c r="G91" s="7"/>
@@ -23772,12 +23778,12 @@
         <v>26</v>
       </c>
       <c r="K91" s="3" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
     </row>
     <row r="92" spans="1:26" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A92" s="20" t="s">
-        <v>831</v>
+        <v>829</v>
       </c>
       <c r="B92" s="20" t="s">
         <v>23</v>
@@ -23789,7 +23795,7 @@
         <v>64</v>
       </c>
       <c r="E92" s="7" t="s">
-        <v>830</v>
+        <v>828</v>
       </c>
       <c r="F92" s="7">
         <v>5</v>
@@ -23807,7 +23813,7 @@
         <v>26</v>
       </c>
       <c r="K92" s="3" t="s">
-        <v>832</v>
+        <v>830</v>
       </c>
       <c r="L92" s="23" t="s">
         <v>64</v>
@@ -23848,7 +23854,7 @@
       <c r="B94" s="20"/>
       <c r="D94" s="3"/>
       <c r="E94" s="7" t="s">
-        <v>927</v>
+        <v>925</v>
       </c>
       <c r="F94" s="7"/>
       <c r="G94" s="7"/>
@@ -23858,7 +23864,7 @@
       <c r="I94" s="3"/>
       <c r="J94" s="3"/>
       <c r="K94" s="3" t="s">
-        <v>929</v>
+        <v>927</v>
       </c>
     </row>
     <row r="95" spans="1:26" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
@@ -23866,7 +23872,7 @@
       <c r="B95" s="20"/>
       <c r="D95" s="3"/>
       <c r="E95" s="7" t="s">
-        <v>930</v>
+        <v>928</v>
       </c>
       <c r="F95" s="7"/>
       <c r="G95" s="7"/>
@@ -23876,7 +23882,7 @@
       <c r="I95" s="3"/>
       <c r="J95" s="3"/>
       <c r="K95" s="3" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
     </row>
     <row r="96" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
@@ -23897,7 +23903,7 @@
       <c r="A97" s="20"/>
       <c r="B97" s="20"/>
       <c r="E97" s="7" t="s">
-        <v>944</v>
+        <v>942</v>
       </c>
       <c r="F97" s="7">
         <v>5</v>
@@ -23915,14 +23921,14 @@
         <v>29</v>
       </c>
       <c r="K97" s="23" t="s">
-        <v>945</v>
+        <v>943</v>
       </c>
     </row>
     <row r="98" spans="1:12" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A98" s="20"/>
       <c r="B98" s="20"/>
       <c r="E98" s="58" t="s">
-        <v>946</v>
+        <v>944</v>
       </c>
       <c r="F98" s="7">
         <v>5</v>
@@ -23940,14 +23946,14 @@
         <v>29</v>
       </c>
       <c r="K98" s="23" t="s">
-        <v>947</v>
+        <v>945</v>
       </c>
     </row>
     <row r="99" spans="1:12" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A99" s="20"/>
       <c r="B99" s="20"/>
       <c r="E99" s="58" t="s">
-        <v>948</v>
+        <v>946</v>
       </c>
       <c r="F99" s="7">
         <v>5</v>
@@ -23965,14 +23971,14 @@
         <v>29</v>
       </c>
       <c r="K99" s="23" t="s">
-        <v>949</v>
+        <v>947</v>
       </c>
     </row>
     <row r="100" spans="1:12" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A100" s="20"/>
       <c r="B100" s="20"/>
       <c r="E100" s="7" t="s">
-        <v>837</v>
+        <v>835</v>
       </c>
       <c r="F100" s="7">
         <v>1</v>
@@ -23981,23 +23987,23 @@
         <v>107</v>
       </c>
       <c r="H100" s="7" t="s">
-        <v>838</v>
+        <v>836</v>
       </c>
       <c r="I100" s="23" t="s">
         <v>25</v>
       </c>
       <c r="J100" s="23" t="s">
-        <v>839</v>
+        <v>837</v>
       </c>
     </row>
     <row r="101" spans="1:12" s="65" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A101" s="92"/>
       <c r="B101" s="92"/>
       <c r="C101" s="76" t="s">
-        <v>1016</v>
+        <v>1014</v>
       </c>
       <c r="E101" s="64" t="s">
-        <v>969</v>
+        <v>967</v>
       </c>
       <c r="F101" s="64"/>
       <c r="G101" s="64" t="s">
@@ -24014,14 +24020,14 @@
       </c>
       <c r="K101" s="94"/>
       <c r="L101" s="94" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
     </row>
     <row r="102" spans="1:12" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A102" s="20"/>
       <c r="B102" s="20"/>
       <c r="E102" s="7" t="s">
-        <v>942</v>
+        <v>940</v>
       </c>
       <c r="F102" s="7"/>
       <c r="G102" s="7" t="s">
@@ -24033,7 +24039,7 @@
       <c r="I102" s="23"/>
       <c r="J102" s="23"/>
       <c r="K102" s="23" t="s">
-        <v>971</v>
+        <v>969</v>
       </c>
       <c r="L102" s="23"/>
     </row>
@@ -24041,7 +24047,7 @@
       <c r="A103" s="20"/>
       <c r="B103" s="20"/>
       <c r="E103" s="7" t="s">
-        <v>943</v>
+        <v>941</v>
       </c>
       <c r="F103" s="7"/>
       <c r="G103" s="7" t="s">
@@ -24053,7 +24059,7 @@
       <c r="I103" s="23"/>
       <c r="J103" s="23"/>
       <c r="K103" s="23" t="s">
-        <v>972</v>
+        <v>970</v>
       </c>
       <c r="L103" s="23"/>
     </row>
@@ -24061,7 +24067,7 @@
       <c r="A104" s="20"/>
       <c r="B104" s="20"/>
       <c r="E104" s="7" t="s">
-        <v>1005</v>
+        <v>1003</v>
       </c>
       <c r="F104" s="7"/>
       <c r="G104" s="7" t="s">
@@ -24077,7 +24083,7 @@
         <v>26</v>
       </c>
       <c r="K104" s="23" t="s">
-        <v>1008</v>
+        <v>1006</v>
       </c>
       <c r="L104" s="23"/>
     </row>
@@ -24085,7 +24091,7 @@
       <c r="A105" s="20"/>
       <c r="B105" s="20"/>
       <c r="E105" s="7" t="s">
-        <v>1006</v>
+        <v>1004</v>
       </c>
       <c r="F105" s="7"/>
       <c r="G105" s="7" t="s">
@@ -24099,7 +24105,7 @@
       </c>
       <c r="J105" s="23"/>
       <c r="K105" s="23" t="s">
-        <v>1007</v>
+        <v>1005</v>
       </c>
       <c r="L105" s="23"/>
     </row>
@@ -24107,10 +24113,10 @@
       <c r="A106" s="20"/>
       <c r="B106" s="20"/>
       <c r="D106" s="57" t="s">
-        <v>936</v>
+        <v>934</v>
       </c>
       <c r="E106" s="7" t="s">
-        <v>961</v>
+        <v>959</v>
       </c>
       <c r="F106" s="7"/>
       <c r="G106" s="58" t="s">
@@ -24120,13 +24126,13 @@
         <v>83</v>
       </c>
       <c r="I106" s="23" t="s">
-        <v>939</v>
+        <v>937</v>
       </c>
       <c r="J106" s="23" t="s">
-        <v>939</v>
+        <v>937</v>
       </c>
       <c r="K106" s="23" t="s">
-        <v>962</v>
+        <v>960</v>
       </c>
       <c r="L106" s="23"/>
     </row>
@@ -24135,7 +24141,7 @@
       <c r="B107" s="20"/>
       <c r="D107" s="57"/>
       <c r="E107" s="7" t="s">
-        <v>1011</v>
+        <v>1009</v>
       </c>
       <c r="F107" s="7"/>
       <c r="G107" s="7" t="s">
@@ -24151,10 +24157,10 @@
         <v>26</v>
       </c>
       <c r="K107" s="23" t="s">
-        <v>970</v>
+        <v>968</v>
       </c>
       <c r="L107" s="23" t="s">
-        <v>1014</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="108" spans="1:12" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
@@ -24162,7 +24168,7 @@
       <c r="B108" s="20"/>
       <c r="D108" s="57"/>
       <c r="E108" s="7" t="s">
-        <v>1012</v>
+        <v>1010</v>
       </c>
       <c r="F108" s="7"/>
       <c r="G108" s="7" t="s">
@@ -24178,10 +24184,10 @@
         <v>26</v>
       </c>
       <c r="K108" s="23" t="s">
-        <v>970</v>
+        <v>968</v>
       </c>
       <c r="L108" s="23" t="s">
-        <v>1015</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="109" spans="1:12" s="21" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -24189,7 +24195,7 @@
       <c r="B109" s="20"/>
       <c r="D109" s="57"/>
       <c r="E109" s="25" t="s">
-        <v>1013</v>
+        <v>1011</v>
       </c>
       <c r="F109" s="7"/>
       <c r="G109" s="7" t="s">
@@ -24205,17 +24211,17 @@
         <v>26</v>
       </c>
       <c r="K109" s="23" t="s">
-        <v>970</v>
+        <v>968</v>
       </c>
       <c r="L109" s="23" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
     </row>
     <row r="110" spans="1:12" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A110" s="20"/>
       <c r="B110" s="20"/>
       <c r="E110" s="7" t="s">
-        <v>836</v>
+        <v>834</v>
       </c>
       <c r="F110" s="7">
         <v>10</v>
@@ -24233,14 +24239,14 @@
         <v>26</v>
       </c>
       <c r="K110" s="23" t="s">
-        <v>842</v>
+        <v>840</v>
       </c>
     </row>
     <row r="111" spans="1:12" s="21" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A111" s="20"/>
       <c r="B111" s="20"/>
       <c r="E111" s="72" t="s">
-        <v>1004</v>
+        <v>1002</v>
       </c>
       <c r="F111" s="7">
         <v>10</v>
@@ -24258,14 +24264,14 @@
         <v>26</v>
       </c>
       <c r="K111" s="23" t="s">
-        <v>842</v>
+        <v>840</v>
       </c>
     </row>
     <row r="112" spans="1:12" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A112" s="20"/>
       <c r="B112" s="20"/>
       <c r="E112" s="72" t="s">
-        <v>1009</v>
+        <v>1007</v>
       </c>
       <c r="F112" s="7"/>
       <c r="G112" s="7" t="s">
@@ -24281,14 +24287,14 @@
         <v>29</v>
       </c>
       <c r="K112" s="23" t="s">
-        <v>1010</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="113" spans="1:12" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A113" s="20"/>
       <c r="B113" s="20"/>
       <c r="E113" s="7" t="s">
-        <v>952</v>
+        <v>950</v>
       </c>
       <c r="F113" s="7"/>
       <c r="G113" s="7" t="s">
@@ -24304,14 +24310,14 @@
         <v>29</v>
       </c>
       <c r="K113" s="23" t="s">
-        <v>953</v>
+        <v>951</v>
       </c>
     </row>
     <row r="114" spans="1:12" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A114" s="20"/>
       <c r="B114" s="20"/>
       <c r="E114" s="7" t="s">
-        <v>965</v>
+        <v>963</v>
       </c>
       <c r="F114" s="7"/>
       <c r="G114" s="7" t="s">
@@ -24325,10 +24331,10 @@
         <v>26</v>
       </c>
       <c r="K114" s="23" t="s">
-        <v>966</v>
+        <v>964</v>
       </c>
       <c r="L114" s="23" t="s">
-        <v>967</v>
+        <v>965</v>
       </c>
     </row>
     <row r="115" spans="1:12" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
@@ -24345,7 +24351,7 @@
       <c r="I115" s="23"/>
       <c r="J115" s="23"/>
       <c r="K115" s="23" t="s">
-        <v>935</v>
+        <v>933</v>
       </c>
     </row>
     <row r="116" spans="1:12" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
@@ -24422,7 +24428,7 @@
         <v>107</v>
       </c>
       <c r="H118" s="18" t="s">
-        <v>1018</v>
+        <v>1016</v>
       </c>
       <c r="I118" s="17" t="s">
         <v>33</v>
@@ -24454,7 +24460,7 @@
         <v>107</v>
       </c>
       <c r="H119" s="23" t="s">
-        <v>1018</v>
+        <v>1016</v>
       </c>
       <c r="I119" s="17" t="s">
         <v>33</v>
@@ -24486,7 +24492,7 @@
         <v>107</v>
       </c>
       <c r="H120" s="23" t="s">
-        <v>1018</v>
+        <v>1016</v>
       </c>
       <c r="I120" s="17" t="s">
         <v>33</v>
@@ -24756,7 +24762,7 @@
       <c r="C7" s="107"/>
       <c r="D7" s="107"/>
       <c r="E7" s="108" t="s">
-        <v>1040</v>
+        <v>1038</v>
       </c>
       <c r="F7" s="108" t="s">
         <v>107</v>
@@ -24768,7 +24774,7 @@
         <v>26</v>
       </c>
       <c r="I7" s="110" t="s">
-        <v>1041</v>
+        <v>1039</v>
       </c>
       <c r="J7" s="109"/>
     </row>
@@ -24924,22 +24930,22 @@
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
       <c r="E12" s="21" t="s">
-        <v>1029</v>
+        <v>1027</v>
       </c>
       <c r="F12" s="57" t="s">
         <v>28</v>
       </c>
       <c r="G12" s="70" t="s">
-        <v>1023</v>
+        <v>1021</v>
       </c>
       <c r="H12" s="21" t="s">
         <v>29</v>
       </c>
       <c r="I12" s="21" t="s">
-        <v>1030</v>
+        <v>1028</v>
       </c>
       <c r="J12" s="21" t="s">
-        <v>1031</v>
+        <v>1029</v>
       </c>
       <c r="K12" s="7"/>
       <c r="L12" s="7"/>
@@ -25078,10 +25084,10 @@
         <v>29</v>
       </c>
       <c r="I16" s="7" t="s">
-        <v>1025</v>
+        <v>1023</v>
       </c>
       <c r="J16" s="7" t="s">
-        <v>1026</v>
+        <v>1024</v>
       </c>
       <c r="K16" s="7"/>
       <c r="L16" s="7"/>
@@ -25138,7 +25144,7 @@
       <c r="C18" s="111"/>
       <c r="D18" s="111"/>
       <c r="E18" s="112" t="s">
-        <v>1042</v>
+        <v>1040</v>
       </c>
       <c r="F18" s="112" t="s">
         <v>107</v>
@@ -25150,7 +25156,7 @@
         <v>26</v>
       </c>
       <c r="I18" s="112" t="s">
-        <v>1045</v>
+        <v>1043</v>
       </c>
       <c r="J18" s="113"/>
       <c r="K18" s="112"/>
@@ -25172,7 +25178,7 @@
       <c r="C19" s="111"/>
       <c r="D19" s="111"/>
       <c r="E19" s="112" t="s">
-        <v>1043</v>
+        <v>1041</v>
       </c>
       <c r="F19" s="112" t="s">
         <v>107</v>
@@ -25184,7 +25190,7 @@
         <v>26</v>
       </c>
       <c r="I19" s="112" t="s">
-        <v>1044</v>
+        <v>1042</v>
       </c>
       <c r="J19" s="113"/>
       <c r="K19" s="112"/>
@@ -25867,7 +25873,7 @@
     <row r="39" spans="1:26" s="21" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A39" s="28"/>
       <c r="E39" s="21" t="s">
-        <v>1027</v>
+        <v>1025</v>
       </c>
       <c r="F39" s="47" t="s">
         <v>28</v>
@@ -25879,7 +25885,7 @@
         <v>26</v>
       </c>
       <c r="I39" s="21" t="s">
-        <v>1028</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="40" spans="1:26" s="65" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
@@ -26051,7 +26057,7 @@
   <sheetData>
     <row r="1" spans="1:21" s="21" customFormat="1" ht="59.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="116" t="s">
-        <v>1048</v>
+        <v>1046</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="25" t="s">
@@ -26107,7 +26113,7 @@
         <v>225</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>1047</v>
+        <v>1045</v>
       </c>
       <c r="G2" s="10" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
Fix a bug associated with converting IDUs with snow to wetlands. Correct a comment about the sign of m_globalHandlerFluxValue. APs.cpp - Correct the sign of the flux associated with changes to the surface water compartment when an IDU is added to a wetland. Flow.cpp - Begin to address an assert in FlowModel::Run(). Flow.h - Correct a comment about the sign of m_globalHandlerFluxValue. HBV.cpp - In HBV::HBVdailyProcess(), allow for the possibility that the flux value for BOX_SNOWPACK is already non-zero on entry.  This can happen on Jan 1 as a result of an IDU with snow being added to a wetland.  The snow is converted to surface water in the PrescribedLulcs autonomous process.
</commit_message>
<xml_diff>
--- a/DataCW3M/CW3MdigitalHandbook/CW3MdataDictionary.xlsx
+++ b/DataCW3M/CW3MdigitalHandbook/CW3MdataDictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\CW3MdigitalHandbook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E80B66C-9879-48A1-9941-9417303CCB38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27824BFE-DA54-4F43-B7EC-5E877C873CC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-7425" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Necessary input data" sheetId="7" r:id="rId1"/>
@@ -9348,9 +9348,9 @@
   </sheetPr>
   <dimension ref="A1:Z1060"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A88" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A78" sqref="A78:XFD78"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A76" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A163" sqref="A163:XFD163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -24521,8 +24521,8 @@
   </sheetPr>
   <dimension ref="A1:Z47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Save new working version, with initial runs in McKenzie and NSantiam. Note new IDU_McKenzie.dbf and IDU_NSantiam.dbf files will go to Box, because they are too big for GitHub's new, lowered file size limit of 25MB. CW3M_McKenzie.envx - Turn off spinup. McKenzie/flow2010.ic, HRU_McKenzie.dbf, Reach_McKenzie.dbf - Save spinup data from C787. IDU_NSantiam.dbf - Add attributes FLOODDEPTH, Q2WETL_MM, WETL_VOL, and WETL2Q_CMS. Reach_NSantiam.dbf - Add ReachOUT_LATERL, ReachFLOOD_CMS, and ReachFLOOD_C.
</commit_message>
<xml_diff>
--- a/DataCW3M/CW3MdigitalHandbook/CW3MdataDictionary.xlsx
+++ b/DataCW3M/CW3MdigitalHandbook/CW3MdataDictionary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\CW3MdigitalHandbook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20B9004E-21E2-42C2-898E-969CEAF890EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3D92E0F0-ECD9-4C2A-91CB-B0CBC30F64F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-7425" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,6 +21,7 @@
     <sheet name="Conventions" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -9395,8 +9396,8 @@
   <dimension ref="A1:Y1064"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J1" sqref="J1:J1048576"/>
+      <pane ySplit="4" topLeftCell="A69" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C90" sqref="C90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>

</xml_diff>

<commit_message>
This is the repository version for CW3M_Installer_1.2.3.exe (322 MB).  The previous release (1.2.2) was from version 744 on 2/17/22.  Since that release, the logic for wetland flooding has been overhauled as part of an effort to close the thermal energy budget, which now closes to within 1% for the McKenzie basin in the years 2010-18.  Some refinements have also been made to the McKenzie water rights file to improve the simulation of municipal water use.
</commit_message>
<xml_diff>
--- a/DataCW3M/CW3MdigitalHandbook/CW3MdataDictionary.xlsx
+++ b/DataCW3M/CW3MdigitalHandbook/CW3MdataDictionary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\CW3MdigitalHandbook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3D92E0F0-ECD9-4C2A-91CB-B0CBC30F64F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87D1AE09-2F6F-4931-8054-49731022C9A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-7425" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,6 @@
     <sheet name="Conventions" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -9396,7 +9395,7 @@
   <dimension ref="A1:Y1064"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A69" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="4" topLeftCell="A217" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C90" sqref="C90"/>
     </sheetView>
   </sheetViews>

</xml_diff>